<commit_message>
chg: Added info about tankers in freq master list
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="579">
   <si>
     <t>AWACS</t>
   </si>
@@ -1026,141 +1026,6 @@
     <t>VIPER 1</t>
   </si>
   <si>
-    <t>VENOM 2</t>
-  </si>
-  <si>
-    <t>VM21</t>
-  </si>
-  <si>
-    <t>00035</t>
-  </si>
-  <si>
-    <t>00036</t>
-  </si>
-  <si>
-    <t>00037</t>
-  </si>
-  <si>
-    <t>00040</t>
-  </si>
-  <si>
-    <t>LOBO 3</t>
-  </si>
-  <si>
-    <t>LO31</t>
-  </si>
-  <si>
-    <t>00055</t>
-  </si>
-  <si>
-    <t>00056</t>
-  </si>
-  <si>
-    <t>00057</t>
-  </si>
-  <si>
-    <t>00060</t>
-  </si>
-  <si>
-    <t>VM22</t>
-  </si>
-  <si>
-    <t>VM23</t>
-  </si>
-  <si>
-    <t>VM24</t>
-  </si>
-  <si>
-    <t>LO32</t>
-  </si>
-  <si>
-    <t>LO33</t>
-  </si>
-  <si>
-    <t>LO34</t>
-  </si>
-  <si>
-    <t>COWBOY 4</t>
-  </si>
-  <si>
-    <t>CY41</t>
-  </si>
-  <si>
-    <t>00065</t>
-  </si>
-  <si>
-    <t>00066</t>
-  </si>
-  <si>
-    <t>00067</t>
-  </si>
-  <si>
-    <t>00070</t>
-  </si>
-  <si>
-    <t>CY42</t>
-  </si>
-  <si>
-    <t>CY43</t>
-  </si>
-  <si>
-    <t>CY44</t>
-  </si>
-  <si>
-    <t>PYTHON 5</t>
-  </si>
-  <si>
-    <t>PN51</t>
-  </si>
-  <si>
-    <t>00011</t>
-  </si>
-  <si>
-    <t>00012</t>
-  </si>
-  <si>
-    <t>00013</t>
-  </si>
-  <si>
-    <t>00014</t>
-  </si>
-  <si>
-    <t>PN52</t>
-  </si>
-  <si>
-    <t>PN53</t>
-  </si>
-  <si>
-    <t>PN54</t>
-  </si>
-  <si>
-    <t>RATTLER 6</t>
-  </si>
-  <si>
-    <t>RR61</t>
-  </si>
-  <si>
-    <t>00025</t>
-  </si>
-  <si>
-    <t>00026</t>
-  </si>
-  <si>
-    <t>00027</t>
-  </si>
-  <si>
-    <t>00030</t>
-  </si>
-  <si>
-    <t>RR62</t>
-  </si>
-  <si>
-    <t>RR63</t>
-  </si>
-  <si>
-    <t>RR64</t>
-  </si>
-  <si>
     <t>F-16C presets  (TRMA) V1.0</t>
   </si>
   <si>
@@ -1657,6 +1522,243 @@
   </si>
   <si>
     <t>F-15 presets  (TRMA) V1.0</t>
+  </si>
+  <si>
+    <t>Gunslinger 1</t>
+  </si>
+  <si>
+    <t>Hammerhead 1</t>
+  </si>
+  <si>
+    <t>OH-58</t>
+  </si>
+  <si>
+    <t>SABER 1</t>
+  </si>
+  <si>
+    <t>OUTCAST 1</t>
+  </si>
+  <si>
+    <t>Lobo</t>
+  </si>
+  <si>
+    <t>Roman</t>
+  </si>
+  <si>
+    <t>Hawg</t>
+  </si>
+  <si>
+    <t>Jedi</t>
+  </si>
+  <si>
+    <t>Hornet</t>
+  </si>
+  <si>
+    <t>Tusk</t>
+  </si>
+  <si>
+    <t>Chevy</t>
+  </si>
+  <si>
+    <t>Squid</t>
+  </si>
+  <si>
+    <t>VENOM</t>
+  </si>
+  <si>
+    <t>DEVIL</t>
+  </si>
+  <si>
+    <t>PONTIAC</t>
+  </si>
+  <si>
+    <t>AR201 #IFF:5201FR</t>
+  </si>
+  <si>
+    <t>ARCO 1</t>
+  </si>
+  <si>
+    <t>280.000</t>
+  </si>
+  <si>
+    <t>281.000</t>
+  </si>
+  <si>
+    <t>282.000</t>
+  </si>
+  <si>
+    <t>283.000</t>
+  </si>
+  <si>
+    <t>284.000</t>
+  </si>
+  <si>
+    <t>285.000</t>
+  </si>
+  <si>
+    <t>286.000</t>
+  </si>
+  <si>
+    <t>287.000</t>
+  </si>
+  <si>
+    <t>288.000</t>
+  </si>
+  <si>
+    <t>289.000</t>
+  </si>
+  <si>
+    <t>280.5</t>
+  </si>
+  <si>
+    <t>281.5</t>
+  </si>
+  <si>
+    <t>282.5</t>
+  </si>
+  <si>
+    <t>283.5</t>
+  </si>
+  <si>
+    <t>GRAY 12</t>
+  </si>
+  <si>
+    <t>AR301 #IFF:5301FR</t>
+  </si>
+  <si>
+    <t>SHELL 1</t>
+  </si>
+  <si>
+    <t>PINK 12</t>
+  </si>
+  <si>
+    <t>45X</t>
+  </si>
+  <si>
+    <t>AR201 #IFF:5101FR</t>
+  </si>
+  <si>
+    <t>TEXACO 1</t>
+  </si>
+  <si>
+    <t>37Y</t>
+  </si>
+  <si>
+    <t>38Y</t>
+  </si>
+  <si>
+    <t>39Y</t>
+  </si>
+  <si>
+    <t>40Y</t>
+  </si>
+  <si>
+    <t>41Y</t>
+  </si>
+  <si>
+    <t>42Y</t>
+  </si>
+  <si>
+    <t>43Y</t>
+  </si>
+  <si>
+    <t>44Y</t>
+  </si>
+  <si>
+    <t>64Y</t>
+  </si>
+  <si>
+    <t>46Y</t>
+  </si>
+  <si>
+    <t>47Y</t>
+  </si>
+  <si>
+    <t>48Y</t>
+  </si>
+  <si>
+    <t>49Y</t>
+  </si>
+  <si>
+    <t>65Y</t>
+  </si>
+  <si>
+    <t>GREEN 12</t>
+  </si>
+  <si>
+    <t>ARCO 2</t>
+  </si>
+  <si>
+    <t>INDIGO 12</t>
+  </si>
+  <si>
+    <t>ARCO 3</t>
+  </si>
+  <si>
+    <t>ARCO 4</t>
+  </si>
+  <si>
+    <t>ARCO 5</t>
+  </si>
+  <si>
+    <t>AR203 #IFF:5203FR</t>
+  </si>
+  <si>
+    <t>AR202 #IFF:5202FR</t>
+  </si>
+  <si>
+    <t>ORANGE 12</t>
+  </si>
+  <si>
+    <t>AR302 #IFF:5302FR</t>
+  </si>
+  <si>
+    <t>SHELL 2</t>
+  </si>
+  <si>
+    <t>AR303 #IFF:5303FR</t>
+  </si>
+  <si>
+    <t>SHELL 3</t>
+  </si>
+  <si>
+    <t>OLIVE 12</t>
+  </si>
+  <si>
+    <t>OCHRE 12</t>
+  </si>
+  <si>
+    <t>SHELL 4</t>
+  </si>
+  <si>
+    <t>AR304 #IFF:5304FR</t>
+  </si>
+  <si>
+    <t>LEMON 12</t>
+  </si>
+  <si>
+    <t>AR401 #IFF:5401FR</t>
+  </si>
+  <si>
+    <t>LIME 12</t>
+  </si>
+  <si>
+    <t>AR501 #IFF:5501FR</t>
+  </si>
+  <si>
+    <t>SHELL 5</t>
+  </si>
+  <si>
+    <t>SHELL 6</t>
+  </si>
+  <si>
+    <t>AR502 #IFF:5502FR</t>
+  </si>
+  <si>
+    <t>MAROON 12</t>
+  </si>
+  <si>
+    <t>PURPLE 12</t>
   </si>
 </sst>
 </file>
@@ -1666,7 +1768,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1812,6 +1914,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="18">
     <fill>
@@ -2443,7 +2552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="201">
+  <cellXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2778,6 +2887,26 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2805,21 +2934,6 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2967,6 +3081,10 @@
     <xf numFmtId="0" fontId="16" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3333,10 +3451,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Ark1"/>
-  <dimension ref="A1:AK53"/>
+  <dimension ref="A1:AP53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AJ34" sqref="AJ34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -3356,9 +3474,11 @@
     <col min="32" max="32" width="16" customWidth="1"/>
     <col min="33" max="33" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="18.28515625" customWidth="1"/>
+    <col min="36" max="36" width="23" customWidth="1"/>
+    <col min="39" max="39" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:42">
       <c r="A1" s="129"/>
       <c r="B1" s="129">
         <v>1</v>
@@ -3403,9 +3523,9 @@
       <c r="T1" s="12"/>
       <c r="Z1" s="12"/>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:42">
       <c r="A2" s="129" t="s">
-        <v>386</v>
+        <v>341</v>
       </c>
       <c r="B2" s="130" t="s">
         <v>111</v>
@@ -3426,7 +3546,7 @@
         <v>116</v>
       </c>
       <c r="H2" s="130" t="s">
-        <v>412</v>
+        <v>367</v>
       </c>
       <c r="I2" s="130" t="s">
         <v>117</v>
@@ -3441,34 +3561,34 @@
         <v>120</v>
       </c>
       <c r="M2" s="130" t="s">
-        <v>413</v>
+        <v>368</v>
       </c>
       <c r="N2" s="129" t="s">
-        <v>386</v>
+        <v>341</v>
       </c>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
       <c r="T2" s="12"/>
-      <c r="V2" s="147" t="s">
+      <c r="V2" s="141" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="147"/>
-      <c r="X2" s="147"/>
-      <c r="Y2" s="147"/>
-      <c r="Z2" s="147"/>
+      <c r="W2" s="141"/>
+      <c r="X2" s="141"/>
+      <c r="Y2" s="141"/>
+      <c r="Z2" s="141"/>
       <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
       <c r="AC2" s="12"/>
       <c r="AD2" s="12"/>
       <c r="AE2" s="12"/>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:42">
       <c r="A3" s="129" t="s">
-        <v>387</v>
+        <v>342</v>
       </c>
       <c r="B3" s="130" t="s">
-        <v>414</v>
+        <v>369</v>
       </c>
       <c r="C3" s="130" t="s">
         <v>121</v>
@@ -3498,24 +3618,24 @@
         <v>129</v>
       </c>
       <c r="L3" s="130" t="s">
-        <v>415</v>
+        <v>370</v>
       </c>
       <c r="M3" s="130" t="s">
-        <v>416</v>
+        <v>371</v>
       </c>
       <c r="N3" s="129" t="s">
-        <v>387</v>
+        <v>342</v>
       </c>
       <c r="O3" s="133"/>
       <c r="P3" t="s">
-        <v>482</v>
+        <v>437</v>
       </c>
       <c r="Q3" s="12"/>
-      <c r="R3" s="151"/>
-      <c r="S3" s="151"/>
-      <c r="T3" s="151"/>
+      <c r="R3" s="145"/>
+      <c r="S3" s="145"/>
+      <c r="T3" s="145"/>
       <c r="V3" s="122" t="s">
-        <v>384</v>
+        <v>339</v>
       </c>
       <c r="W3" s="115" t="s">
         <v>224</v>
@@ -3535,9 +3655,9 @@
       <c r="AD3" s="37"/>
       <c r="AE3" s="37"/>
     </row>
-    <row r="4" spans="1:34" ht="15.75">
+    <row r="4" spans="1:42" ht="15.75">
       <c r="A4" s="129" t="s">
-        <v>388</v>
+        <v>343</v>
       </c>
       <c r="B4" s="131" t="s">
         <v>234</v>
@@ -3573,10 +3693,10 @@
         <v>238</v>
       </c>
       <c r="M4" s="130" t="s">
-        <v>417</v>
+        <v>372</v>
       </c>
       <c r="N4" s="129" t="s">
-        <v>388</v>
+        <v>343</v>
       </c>
       <c r="O4" s="13"/>
       <c r="Q4" s="12"/>
@@ -3590,24 +3710,33 @@
         <v>12</v>
       </c>
       <c r="X4" s="10" t="s">
-        <v>536</v>
+        <v>491</v>
       </c>
       <c r="Y4" s="10"/>
       <c r="Z4" s="10"/>
       <c r="AA4" s="36"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="36"/>
-      <c r="AD4" s="147" t="s">
-        <v>485</v>
-      </c>
-      <c r="AE4" s="147"/>
-      <c r="AF4" s="147"/>
-      <c r="AG4" s="147"/>
-      <c r="AH4" s="147"/>
-    </row>
-    <row r="5" spans="1:34" ht="15.75">
+      <c r="AD4" s="141" t="s">
+        <v>440</v>
+      </c>
+      <c r="AE4" s="141"/>
+      <c r="AF4" s="141"/>
+      <c r="AG4" s="141"/>
+      <c r="AH4" s="141"/>
+      <c r="AJ4" s="141" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="141"/>
+      <c r="AL4" s="141"/>
+      <c r="AM4" s="141"/>
+      <c r="AN4" s="141"/>
+      <c r="AO4" s="141"/>
+      <c r="AP4" s="141"/>
+    </row>
+    <row r="5" spans="1:42" ht="15.75">
       <c r="A5" s="129" t="s">
-        <v>389</v>
+        <v>344</v>
       </c>
       <c r="B5" s="130" t="s">
         <v>10</v>
@@ -3622,7 +3751,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="130" t="s">
-        <v>418</v>
+        <v>373</v>
       </c>
       <c r="G5" s="130" t="s">
         <v>14</v>
@@ -3637,16 +3766,16 @@
         <v>17</v>
       </c>
       <c r="K5" s="130" t="s">
-        <v>419</v>
+        <v>374</v>
       </c>
       <c r="L5" s="130" t="s">
         <v>18</v>
       </c>
       <c r="M5" s="130" t="s">
-        <v>420</v>
+        <v>375</v>
       </c>
       <c r="N5" s="129" t="s">
-        <v>389</v>
+        <v>344</v>
       </c>
       <c r="O5" s="13"/>
       <c r="Q5" s="12"/>
@@ -3657,10 +3786,10 @@
         <v>3</v>
       </c>
       <c r="W5" s="14" t="s">
-        <v>462</v>
+        <v>417</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>537</v>
+        <v>492</v>
       </c>
       <c r="Y5" s="1" t="s">
         <v>73</v>
@@ -3686,39 +3815,60 @@
       <c r="AH5" s="115" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="6" spans="1:34" ht="15.75">
+      <c r="AJ5" s="115" t="s">
+        <v>218</v>
+      </c>
+      <c r="AK5" s="115" t="s">
+        <v>219</v>
+      </c>
+      <c r="AL5" s="115" t="s">
+        <v>224</v>
+      </c>
+      <c r="AM5" s="115" t="s">
+        <v>227</v>
+      </c>
+      <c r="AN5" s="115" t="s">
+        <v>220</v>
+      </c>
+      <c r="AO5" s="115" t="s">
+        <v>284</v>
+      </c>
+      <c r="AP5" s="115" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" ht="15.75">
       <c r="A6" s="129" t="s">
-        <v>390</v>
+        <v>345</v>
       </c>
       <c r="B6" s="131" t="s">
-        <v>421</v>
+        <v>376</v>
       </c>
       <c r="C6" s="130"/>
       <c r="D6" s="127" t="s">
-        <v>422</v>
+        <v>377</v>
       </c>
       <c r="E6" s="131" t="s">
-        <v>423</v>
+        <v>378</v>
       </c>
       <c r="F6" s="130"/>
       <c r="G6" s="131" t="s">
-        <v>424</v>
+        <v>379</v>
       </c>
       <c r="H6" s="127" t="s">
-        <v>425</v>
+        <v>380</v>
       </c>
       <c r="I6" s="131" t="s">
-        <v>426</v>
+        <v>381</v>
       </c>
       <c r="J6" s="130"/>
       <c r="K6" s="130"/>
       <c r="L6" s="130"/>
       <c r="M6" s="130" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="N6" s="129" t="s">
-        <v>390</v>
+        <v>345</v>
       </c>
       <c r="O6" s="14"/>
       <c r="P6" s="2" t="s">
@@ -3743,7 +3893,7 @@
       <c r="AB6" s="12"/>
       <c r="AC6" s="12"/>
       <c r="AD6" s="3" t="s">
-        <v>486</v>
+        <v>441</v>
       </c>
       <c r="AE6" s="127" t="s">
         <v>23</v>
@@ -3752,15 +3902,30 @@
         <v>240</v>
       </c>
       <c r="AG6" s="127" t="s">
-        <v>432</v>
+        <v>387</v>
       </c>
       <c r="AH6" s="3" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" ht="15.75">
+        <v>472</v>
+      </c>
+      <c r="AJ6" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>538</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>539</v>
+      </c>
+      <c r="AO6">
+        <v>5101</v>
+      </c>
+      <c r="AP6">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" ht="15.75">
       <c r="A7" s="129" t="s">
-        <v>391</v>
+        <v>346</v>
       </c>
       <c r="B7" s="130" t="s">
         <v>92</v>
@@ -3772,7 +3937,7 @@
         <v>94</v>
       </c>
       <c r="E7" s="130" t="s">
-        <v>428</v>
+        <v>383</v>
       </c>
       <c r="F7" s="130" t="s">
         <v>95</v>
@@ -3797,7 +3962,7 @@
       </c>
       <c r="M7" s="130"/>
       <c r="N7" s="129" t="s">
-        <v>391</v>
+        <v>346</v>
       </c>
       <c r="O7" s="134"/>
       <c r="P7" s="2" t="s">
@@ -3822,13 +3987,13 @@
       <c r="AB7" s="12"/>
       <c r="AC7" s="12"/>
       <c r="AD7" s="3" t="s">
-        <v>487</v>
+        <v>442</v>
       </c>
       <c r="AE7" s="127" t="s">
         <v>114</v>
       </c>
       <c r="AF7" s="10" t="s">
-        <v>505</v>
+        <v>460</v>
       </c>
       <c r="AG7" s="127" t="s">
         <v>26</v>
@@ -3836,22 +4001,25 @@
       <c r="AH7" s="3" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" ht="15.75">
+      <c r="AN7" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" ht="15.75">
       <c r="A8" s="129" t="s">
-        <v>392</v>
+        <v>347</v>
       </c>
       <c r="B8" s="132" t="s">
         <v>130</v>
       </c>
       <c r="C8" s="130" t="s">
-        <v>429</v>
+        <v>384</v>
       </c>
       <c r="D8" s="127" t="s">
         <v>131</v>
       </c>
       <c r="E8" s="130" t="s">
-        <v>430</v>
+        <v>385</v>
       </c>
       <c r="F8" s="132" t="s">
         <v>132</v>
@@ -3876,7 +4044,7 @@
       </c>
       <c r="M8" s="130"/>
       <c r="N8" s="129" t="s">
-        <v>392</v>
+        <v>347</v>
       </c>
       <c r="O8" s="132"/>
       <c r="P8" s="2" t="s">
@@ -3893,60 +4061,63 @@
         <v>171</v>
       </c>
       <c r="X8" s="10" t="s">
-        <v>502</v>
+        <v>457</v>
       </c>
       <c r="Y8" s="10"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="12"/>
       <c r="AB8" s="12"/>
       <c r="AD8" s="3" t="s">
-        <v>488</v>
+        <v>443</v>
       </c>
       <c r="AE8" s="127" t="s">
         <v>97</v>
       </c>
       <c r="AF8" s="10" t="s">
-        <v>506</v>
+        <v>461</v>
       </c>
       <c r="AG8" s="127" t="s">
         <v>50</v>
       </c>
       <c r="AH8" s="3" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" ht="15.75">
+        <v>475</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" ht="15.75">
       <c r="A9" s="129" t="s">
-        <v>393</v>
+        <v>348</v>
       </c>
       <c r="B9" s="127" t="s">
-        <v>431</v>
+        <v>386</v>
       </c>
       <c r="C9" s="127" t="s">
-        <v>432</v>
+        <v>387</v>
       </c>
       <c r="D9" s="130"/>
       <c r="E9" s="130" t="s">
-        <v>433</v>
+        <v>388</v>
       </c>
       <c r="F9" s="131" t="s">
-        <v>434</v>
+        <v>389</v>
       </c>
       <c r="G9" s="131" t="s">
-        <v>435</v>
+        <v>390</v>
       </c>
       <c r="H9" s="130"/>
       <c r="I9" s="130"/>
       <c r="J9" s="131" t="s">
-        <v>436</v>
+        <v>391</v>
       </c>
       <c r="K9" s="127" t="s">
-        <v>437</v>
+        <v>392</v>
       </c>
       <c r="L9" s="130"/>
       <c r="M9" s="130"/>
       <c r="N9" s="129" t="s">
-        <v>393</v>
+        <v>348</v>
       </c>
       <c r="O9" s="135"/>
       <c r="P9" s="2" t="s">
@@ -3963,18 +4134,18 @@
         <v>53</v>
       </c>
       <c r="X9" s="10" t="s">
-        <v>503</v>
+        <v>458</v>
       </c>
       <c r="Y9" s="10"/>
       <c r="Z9" s="3"/>
       <c r="AD9" s="3" t="s">
-        <v>489</v>
+        <v>444</v>
       </c>
       <c r="AE9" s="127" t="s">
         <v>38</v>
       </c>
       <c r="AF9" s="10" t="s">
-        <v>507</v>
+        <v>462</v>
       </c>
       <c r="AG9" s="127" t="s">
         <v>106</v>
@@ -3982,16 +4153,37 @@
       <c r="AH9" s="3" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="10" spans="1:34" ht="15.75">
+      <c r="AJ9" s="11" t="s">
+        <v>516</v>
+      </c>
+      <c r="AK9" s="11" t="s">
+        <v>517</v>
+      </c>
+      <c r="AL9" s="135" t="s">
+        <v>518</v>
+      </c>
+      <c r="AM9" s="11" t="s">
+        <v>532</v>
+      </c>
+      <c r="AN9" s="10" t="s">
+        <v>542</v>
+      </c>
+      <c r="AO9" s="10">
+        <v>5201</v>
+      </c>
+      <c r="AP9" s="10">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" ht="15.75">
       <c r="A10" s="129" t="s">
-        <v>394</v>
+        <v>349</v>
       </c>
       <c r="B10" s="130" t="s">
         <v>148</v>
       </c>
       <c r="C10" s="130" t="s">
-        <v>438</v>
+        <v>393</v>
       </c>
       <c r="D10" s="127" t="s">
         <v>149</v>
@@ -4006,7 +4198,7 @@
         <v>152</v>
       </c>
       <c r="H10" s="130" t="s">
-        <v>439</v>
+        <v>394</v>
       </c>
       <c r="I10" s="130" t="s">
         <v>153</v>
@@ -4022,7 +4214,7 @@
       </c>
       <c r="M10" s="130"/>
       <c r="N10" s="129" t="s">
-        <v>394</v>
+        <v>349</v>
       </c>
       <c r="O10" s="136"/>
       <c r="P10" s="2" t="s">
@@ -4039,12 +4231,12 @@
         <v>189</v>
       </c>
       <c r="X10" s="10" t="s">
-        <v>504</v>
+        <v>459</v>
       </c>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AD10" s="3" t="s">
-        <v>490</v>
+        <v>445</v>
       </c>
       <c r="AE10" s="127" t="s">
         <v>101</v>
@@ -4056,12 +4248,33 @@
         <v>200</v>
       </c>
       <c r="AH10" s="3" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" ht="15.75">
+        <v>476</v>
+      </c>
+      <c r="AJ10" s="11" t="s">
+        <v>560</v>
+      </c>
+      <c r="AK10" s="11" t="s">
+        <v>554</v>
+      </c>
+      <c r="AL10" s="135" t="s">
+        <v>519</v>
+      </c>
+      <c r="AM10" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="AN10" s="10" t="s">
+        <v>543</v>
+      </c>
+      <c r="AO10" s="3">
+        <v>5202</v>
+      </c>
+      <c r="AP10" s="3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" ht="15.75">
       <c r="A11" s="129" t="s">
-        <v>395</v>
+        <v>350</v>
       </c>
       <c r="B11" s="130" t="s">
         <v>139</v>
@@ -4076,7 +4289,7 @@
         <v>142</v>
       </c>
       <c r="F11" s="130" t="s">
-        <v>440</v>
+        <v>395</v>
       </c>
       <c r="G11" s="131" t="s">
         <v>143</v>
@@ -4091,14 +4304,14 @@
         <v>146</v>
       </c>
       <c r="K11" s="130" t="s">
-        <v>441</v>
+        <v>396</v>
       </c>
       <c r="L11" s="131" t="s">
         <v>147</v>
       </c>
       <c r="M11" s="130"/>
       <c r="N11" s="129" t="s">
-        <v>395</v>
+        <v>350</v>
       </c>
       <c r="O11" s="137"/>
       <c r="P11" s="2" t="s">
@@ -4125,22 +4338,43 @@
       <c r="AB11" s="36"/>
       <c r="AC11" s="36"/>
       <c r="AD11" s="3" t="s">
-        <v>490</v>
+        <v>445</v>
       </c>
       <c r="AE11" s="127" t="s">
         <v>135</v>
       </c>
       <c r="AF11" s="10" t="s">
-        <v>509</v>
+        <v>464</v>
       </c>
       <c r="AG11" s="127" t="s">
         <v>129</v>
       </c>
       <c r="AH11" s="3" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" ht="15.75">
+        <v>479</v>
+      </c>
+      <c r="AJ11" s="11" t="s">
+        <v>559</v>
+      </c>
+      <c r="AK11" s="11" t="s">
+        <v>556</v>
+      </c>
+      <c r="AL11" s="135" t="s">
+        <v>520</v>
+      </c>
+      <c r="AM11" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="AN11" s="10" t="s">
+        <v>544</v>
+      </c>
+      <c r="AO11" s="10">
+        <v>5203</v>
+      </c>
+      <c r="AP11" s="10">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" ht="15.75">
       <c r="A12" s="129"/>
       <c r="B12" s="129">
         <v>1</v>
@@ -4196,27 +4430,48 @@
       <c r="Z12" s="10"/>
       <c r="AA12" s="36"/>
       <c r="AD12" s="3" t="s">
-        <v>491</v>
+        <v>446</v>
       </c>
       <c r="AE12" s="127" t="s">
         <v>193</v>
       </c>
       <c r="AF12" s="10" t="s">
-        <v>510</v>
+        <v>465</v>
       </c>
       <c r="AG12" s="127" t="s">
         <v>194</v>
       </c>
       <c r="AH12" s="3" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" ht="15.75">
+        <v>480</v>
+      </c>
+      <c r="AJ12" s="204" t="s">
+        <v>571</v>
+      </c>
+      <c r="AK12" s="11" t="s">
+        <v>557</v>
+      </c>
+      <c r="AL12" s="135" t="s">
+        <v>521</v>
+      </c>
+      <c r="AM12" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="AN12" s="10" t="s">
+        <v>545</v>
+      </c>
+      <c r="AO12" s="3">
+        <v>5204</v>
+      </c>
+      <c r="AP12" s="3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" ht="15.75">
       <c r="A13" s="129" t="s">
-        <v>396</v>
+        <v>351</v>
       </c>
       <c r="B13" s="130" t="s">
-        <v>442</v>
+        <v>397</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>74</v>
@@ -4246,15 +4501,17 @@
         <v>82</v>
       </c>
       <c r="L13" s="130" t="s">
-        <v>443</v>
-      </c>
-      <c r="M13" s="130"/>
+        <v>398</v>
+      </c>
+      <c r="M13" s="135" t="s">
+        <v>518</v>
+      </c>
       <c r="N13" s="129" t="s">
-        <v>396</v>
+        <v>351</v>
       </c>
       <c r="O13" s="127"/>
       <c r="P13" s="2" t="s">
-        <v>500</v>
+        <v>455</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="119"/>
@@ -4269,30 +4526,51 @@
       <c r="Z13" s="10"/>
       <c r="AA13" s="12"/>
       <c r="AD13" s="3" t="s">
-        <v>492</v>
+        <v>447</v>
       </c>
       <c r="AE13" s="127" t="s">
         <v>36</v>
       </c>
       <c r="AF13" s="10" t="s">
-        <v>508</v>
+        <v>463</v>
       </c>
       <c r="AG13" s="127" t="s">
         <v>149</v>
       </c>
       <c r="AH13" s="3" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" ht="15.75">
+        <v>481</v>
+      </c>
+      <c r="AJ13" s="204" t="s">
+        <v>571</v>
+      </c>
+      <c r="AK13" s="11" t="s">
+        <v>558</v>
+      </c>
+      <c r="AL13" s="135" t="s">
+        <v>522</v>
+      </c>
+      <c r="AM13" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="AN13" s="10" t="s">
+        <v>546</v>
+      </c>
+      <c r="AO13" s="10">
+        <v>5205</v>
+      </c>
+      <c r="AP13" s="10">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" ht="15.75">
       <c r="A14" s="129" t="s">
-        <v>397</v>
+        <v>352</v>
       </c>
       <c r="B14" s="130" t="s">
-        <v>444</v>
+        <v>399</v>
       </c>
       <c r="C14" s="130" t="s">
-        <v>445</v>
+        <v>400</v>
       </c>
       <c r="D14" s="130" t="s">
         <v>19</v>
@@ -4310,7 +4588,7 @@
         <v>23</v>
       </c>
       <c r="I14" s="130" t="s">
-        <v>446</v>
+        <v>401</v>
       </c>
       <c r="J14" s="130" t="s">
         <v>24</v>
@@ -4319,15 +4597,17 @@
         <v>25</v>
       </c>
       <c r="L14" s="130" t="s">
-        <v>447</v>
-      </c>
-      <c r="M14" s="130"/>
+        <v>402</v>
+      </c>
+      <c r="M14" s="135" t="s">
+        <v>519</v>
+      </c>
       <c r="N14" s="129" t="s">
-        <v>397</v>
+        <v>352</v>
       </c>
       <c r="O14" s="128"/>
       <c r="P14" s="2" t="s">
-        <v>539</v>
+        <v>494</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="121"/>
@@ -4346,10 +4626,11 @@
       <c r="AF14" s="45"/>
       <c r="AG14" s="45"/>
       <c r="AH14" s="45"/>
-    </row>
-    <row r="15" spans="1:34" ht="15.75">
+      <c r="AN14" s="12"/>
+    </row>
+    <row r="15" spans="1:42" ht="15.75">
       <c r="A15" s="129" t="s">
-        <v>398</v>
+        <v>353</v>
       </c>
       <c r="B15" s="130" t="s">
         <v>157</v>
@@ -4384,9 +4665,11 @@
       <c r="L15" s="127" t="s">
         <v>167</v>
       </c>
-      <c r="M15" s="130"/>
+      <c r="M15" s="135" t="s">
+        <v>520</v>
+      </c>
       <c r="N15" s="129" t="s">
-        <v>398</v>
+        <v>353</v>
       </c>
       <c r="O15" s="35"/>
       <c r="P15" s="2"/>
@@ -4398,30 +4681,30 @@
       <c r="Z15" s="12"/>
       <c r="AA15" s="12"/>
       <c r="AD15" s="3" t="s">
-        <v>493</v>
+        <v>448</v>
       </c>
       <c r="AE15" s="127" t="s">
         <v>166</v>
       </c>
       <c r="AF15" s="10" t="s">
-        <v>511</v>
+        <v>466</v>
       </c>
       <c r="AG15" s="127" t="s">
-        <v>437</v>
+        <v>392</v>
       </c>
       <c r="AH15" s="3" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" ht="15.75">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" ht="15.75">
       <c r="A16" s="129" t="s">
-        <v>399</v>
+        <v>354</v>
       </c>
       <c r="B16" s="130" t="s">
-        <v>448</v>
+        <v>403</v>
       </c>
       <c r="C16" s="130" t="s">
-        <v>449</v>
+        <v>404</v>
       </c>
       <c r="D16" s="127" t="s">
         <v>168</v>
@@ -4430,7 +4713,7 @@
         <v>169</v>
       </c>
       <c r="F16" s="130" t="s">
-        <v>450</v>
+        <v>405</v>
       </c>
       <c r="G16" s="130" t="s">
         <v>170</v>
@@ -4439,7 +4722,7 @@
         <v>171</v>
       </c>
       <c r="I16" s="130" t="s">
-        <v>451</v>
+        <v>406</v>
       </c>
       <c r="J16" s="131" t="s">
         <v>172</v>
@@ -4448,11 +4731,13 @@
         <v>173</v>
       </c>
       <c r="L16" s="130" t="s">
-        <v>452</v>
-      </c>
-      <c r="M16" s="130"/>
+        <v>407</v>
+      </c>
+      <c r="M16" s="135" t="s">
+        <v>521</v>
+      </c>
       <c r="N16" s="129" t="s">
-        <v>399</v>
+        <v>354</v>
       </c>
       <c r="O16" s="35"/>
       <c r="P16" s="2"/>
@@ -4460,23 +4745,14 @@
       <c r="R16" s="121"/>
       <c r="S16" s="120"/>
       <c r="T16" s="12"/>
-      <c r="V16" s="147" t="s">
-        <v>1</v>
-      </c>
-      <c r="W16" s="147"/>
-      <c r="X16" s="147"/>
-      <c r="Y16" s="147"/>
-      <c r="Z16" s="147"/>
-      <c r="AA16" s="147"/>
-      <c r="AB16" s="147"/>
       <c r="AD16" s="3" t="s">
-        <v>494</v>
+        <v>449</v>
       </c>
       <c r="AE16" s="127" t="s">
         <v>49</v>
       </c>
       <c r="AF16" s="10" t="s">
-        <v>513</v>
+        <v>468</v>
       </c>
       <c r="AG16" s="127" t="s">
         <v>71</v>
@@ -4485,9 +4761,9 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="15.75">
+    <row r="17" spans="1:42" ht="15.75">
       <c r="A17" s="129" t="s">
-        <v>400</v>
+        <v>355</v>
       </c>
       <c r="B17" s="131" t="s">
         <v>174</v>
@@ -4505,7 +4781,7 @@
         <v>178</v>
       </c>
       <c r="G17" s="130" t="s">
-        <v>453</v>
+        <v>408</v>
       </c>
       <c r="H17" s="130" t="s">
         <v>179</v>
@@ -4514,7 +4790,7 @@
         <v>180</v>
       </c>
       <c r="J17" s="130" t="s">
-        <v>454</v>
+        <v>409</v>
       </c>
       <c r="K17" s="130" t="s">
         <v>181</v>
@@ -4522,9 +4798,11 @@
       <c r="L17" s="130" t="s">
         <v>182</v>
       </c>
-      <c r="M17" s="130"/>
+      <c r="M17" s="135" t="s">
+        <v>522</v>
+      </c>
       <c r="N17" s="129" t="s">
-        <v>400</v>
+        <v>355</v>
       </c>
       <c r="O17" s="35"/>
       <c r="P17" s="2"/>
@@ -4532,52 +4810,40 @@
       <c r="R17" s="12"/>
       <c r="S17" s="120"/>
       <c r="T17" s="12"/>
-      <c r="V17" s="115" t="s">
-        <v>218</v>
-      </c>
-      <c r="W17" s="115" t="s">
-        <v>219</v>
-      </c>
-      <c r="X17" s="115" t="s">
-        <v>224</v>
-      </c>
-      <c r="Y17" s="115" t="s">
-        <v>227</v>
-      </c>
-      <c r="Z17" s="115" t="s">
-        <v>220</v>
-      </c>
-      <c r="AA17" s="115" t="s">
-        <v>284</v>
-      </c>
-      <c r="AB17" s="115" t="s">
-        <v>280</v>
-      </c>
       <c r="AD17" s="10" t="s">
-        <v>495</v>
+        <v>450</v>
       </c>
       <c r="AE17" s="127" t="s">
         <v>131</v>
       </c>
       <c r="AF17" s="10" t="s">
-        <v>514</v>
+        <v>469</v>
       </c>
       <c r="AG17" s="127" t="s">
-        <v>425</v>
+        <v>380</v>
       </c>
       <c r="AH17" s="3" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="18" spans="1:34" ht="15.75">
+        <v>478</v>
+      </c>
+      <c r="AJ17" s="141" t="s">
+        <v>277</v>
+      </c>
+      <c r="AK17" s="141"/>
+      <c r="AL17" s="141"/>
+      <c r="AM17" s="141"/>
+      <c r="AN17" s="141"/>
+      <c r="AO17" s="141"/>
+      <c r="AP17" s="141"/>
+    </row>
+    <row r="18" spans="1:42" ht="15.75">
       <c r="A18" s="129" t="s">
-        <v>401</v>
+        <v>356</v>
       </c>
       <c r="B18" s="131" t="s">
         <v>183</v>
       </c>
       <c r="C18" s="130" t="s">
-        <v>455</v>
+        <v>410</v>
       </c>
       <c r="D18" s="130" t="s">
         <v>184</v>
@@ -4586,10 +4852,10 @@
         <v>185</v>
       </c>
       <c r="F18" s="130" t="s">
-        <v>456</v>
+        <v>411</v>
       </c>
       <c r="G18" s="130" t="s">
-        <v>457</v>
+        <v>412</v>
       </c>
       <c r="H18" s="130" t="s">
         <v>186</v>
@@ -4598,7 +4864,7 @@
         <v>187</v>
       </c>
       <c r="J18" s="130" t="s">
-        <v>458</v>
+        <v>413</v>
       </c>
       <c r="K18" s="130" t="s">
         <v>188</v>
@@ -4606,9 +4872,11 @@
       <c r="L18" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="M18" s="130"/>
+      <c r="M18" s="135" t="s">
+        <v>523</v>
+      </c>
       <c r="N18" s="129" t="s">
-        <v>401</v>
+        <v>356</v>
       </c>
       <c r="O18" s="35"/>
       <c r="P18" s="2"/>
@@ -4617,32 +4885,46 @@
       <c r="S18" s="120"/>
       <c r="T18" s="37"/>
       <c r="U18" s="12"/>
-      <c r="V18" s="11"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="10"/>
-      <c r="AA18" s="10"/>
-      <c r="AB18" s="10"/>
       <c r="AD18" s="10" t="s">
-        <v>496</v>
+        <v>451</v>
       </c>
       <c r="AE18" s="127" t="s">
         <v>96</v>
       </c>
       <c r="AF18" s="10" t="s">
-        <v>515</v>
+        <v>470</v>
       </c>
       <c r="AG18" s="127" t="s">
         <v>168</v>
       </c>
       <c r="AH18" s="3" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="19" spans="1:34" ht="15.75">
+        <v>483</v>
+      </c>
+      <c r="AJ18" s="114" t="s">
+        <v>218</v>
+      </c>
+      <c r="AK18" s="114" t="s">
+        <v>219</v>
+      </c>
+      <c r="AL18" s="114" t="s">
+        <v>224</v>
+      </c>
+      <c r="AM18" s="114" t="s">
+        <v>227</v>
+      </c>
+      <c r="AN18" s="114" t="s">
+        <v>220</v>
+      </c>
+      <c r="AO18" s="114" t="s">
+        <v>284</v>
+      </c>
+      <c r="AP18" s="114" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" ht="15.75">
       <c r="A19" s="129" t="s">
-        <v>402</v>
+        <v>357</v>
       </c>
       <c r="B19" s="130" t="s">
         <v>190</v>
@@ -4660,10 +4942,10 @@
         <v>194</v>
       </c>
       <c r="G19" s="130" t="s">
-        <v>459</v>
+        <v>414</v>
       </c>
       <c r="H19" s="130" t="s">
-        <v>460</v>
+        <v>415</v>
       </c>
       <c r="I19" s="131" t="s">
         <v>195</v>
@@ -4675,11 +4957,13 @@
         <v>197</v>
       </c>
       <c r="L19" s="130" t="s">
-        <v>461</v>
-      </c>
-      <c r="M19" s="130"/>
+        <v>416</v>
+      </c>
+      <c r="M19" s="135" t="s">
+        <v>524</v>
+      </c>
       <c r="N19" s="129" t="s">
-        <v>402</v>
+        <v>357</v>
       </c>
       <c r="O19" s="35"/>
       <c r="P19" s="2"/>
@@ -4700,10 +4984,31 @@
       <c r="AF19" s="45"/>
       <c r="AG19" s="45"/>
       <c r="AH19" s="45"/>
-    </row>
-    <row r="20" spans="1:34">
+      <c r="AJ19" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="AK19" s="11" t="s">
+        <v>534</v>
+      </c>
+      <c r="AL19" s="135" t="s">
+        <v>527</v>
+      </c>
+      <c r="AM19" s="11" t="s">
+        <v>535</v>
+      </c>
+      <c r="AN19" s="10" t="s">
+        <v>548</v>
+      </c>
+      <c r="AO19" s="10">
+        <v>5301</v>
+      </c>
+      <c r="AP19" s="10">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42">
       <c r="A20" s="129" t="s">
-        <v>403</v>
+        <v>358</v>
       </c>
       <c r="B20" s="130" t="s">
         <v>198</v>
@@ -4734,18 +5039,20 @@
         <v>205</v>
       </c>
       <c r="L20" s="14" t="s">
-        <v>462</v>
-      </c>
-      <c r="M20" s="130"/>
+        <v>417</v>
+      </c>
+      <c r="M20" s="135" t="s">
+        <v>525</v>
+      </c>
       <c r="N20" s="129" t="s">
-        <v>403</v>
+        <v>358</v>
       </c>
       <c r="O20" s="35"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="151"/>
-      <c r="S20" s="151"/>
-      <c r="T20" s="151"/>
+      <c r="R20" s="145"/>
+      <c r="S20" s="145"/>
+      <c r="T20" s="145"/>
       <c r="U20" s="2"/>
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
@@ -4755,24 +5062,45 @@
       <c r="AA20" s="12"/>
       <c r="AB20" s="12"/>
       <c r="AD20" s="10" t="s">
-        <v>497</v>
+        <v>452</v>
       </c>
       <c r="AE20" s="127" t="s">
         <v>167</v>
       </c>
       <c r="AF20" s="10" t="s">
-        <v>512</v>
+        <v>467</v>
       </c>
       <c r="AG20" s="127" t="s">
-        <v>431</v>
+        <v>386</v>
       </c>
       <c r="AH20" s="3" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="21" spans="1:34">
+        <v>473</v>
+      </c>
+      <c r="AJ20" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="AK20" s="11" t="s">
+        <v>563</v>
+      </c>
+      <c r="AL20" s="135" t="s">
+        <v>526</v>
+      </c>
+      <c r="AM20" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="AN20" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="AO20" s="3">
+        <v>5302</v>
+      </c>
+      <c r="AP20" s="3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42">
       <c r="A21" s="129" t="s">
-        <v>404</v>
+        <v>359</v>
       </c>
       <c r="B21" s="130" t="s">
         <v>43</v>
@@ -4796,7 +5124,7 @@
         <v>49</v>
       </c>
       <c r="I21" s="130" t="s">
-        <v>463</v>
+        <v>418</v>
       </c>
       <c r="J21" s="127" t="s">
         <v>50</v>
@@ -4807,9 +5135,11 @@
       <c r="L21" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="M21" s="130"/>
+      <c r="M21" s="135" t="s">
+        <v>526</v>
+      </c>
       <c r="N21" s="129" t="s">
-        <v>404</v>
+        <v>359</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
@@ -4826,24 +5156,45 @@
       <c r="AA21" s="12"/>
       <c r="AB21" s="12"/>
       <c r="AD21" s="10" t="s">
-        <v>498</v>
+        <v>453</v>
       </c>
       <c r="AE21" s="127" t="s">
         <v>196</v>
       </c>
       <c r="AF21" s="3" t="s">
-        <v>516</v>
+        <v>471</v>
       </c>
       <c r="AG21" s="127" t="s">
-        <v>422</v>
+        <v>377</v>
       </c>
       <c r="AH21" s="3" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="22" spans="1:34">
+        <v>477</v>
+      </c>
+      <c r="AJ21" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="AK21" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="AL21" s="135" t="s">
+        <v>525</v>
+      </c>
+      <c r="AM21" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="AN21" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="AO21" s="10">
+        <v>5303</v>
+      </c>
+      <c r="AP21" s="10">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42">
       <c r="A22" s="129" t="s">
-        <v>405</v>
+        <v>360</v>
       </c>
       <c r="B22" s="131" t="s">
         <v>83</v>
@@ -4861,13 +5212,13 @@
         <v>87</v>
       </c>
       <c r="G22" s="130" t="s">
-        <v>464</v>
+        <v>419</v>
       </c>
       <c r="H22" s="130" t="s">
         <v>88</v>
       </c>
       <c r="I22" s="130" t="s">
-        <v>465</v>
+        <v>420</v>
       </c>
       <c r="J22" s="131" t="s">
         <v>89</v>
@@ -4878,9 +5229,11 @@
       <c r="L22" s="131" t="s">
         <v>91</v>
       </c>
-      <c r="M22" s="130"/>
+      <c r="M22" s="135" t="s">
+        <v>527</v>
+      </c>
       <c r="N22" s="129" t="s">
-        <v>405</v>
+        <v>360</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
@@ -4888,17 +5241,8 @@
       <c r="R22" s="12"/>
       <c r="S22" s="12"/>
       <c r="T22" s="12"/>
-      <c r="V22" s="147" t="s">
-        <v>277</v>
-      </c>
-      <c r="W22" s="147"/>
-      <c r="X22" s="147"/>
-      <c r="Y22" s="147"/>
-      <c r="Z22" s="147"/>
-      <c r="AA22" s="147"/>
-      <c r="AB22" s="147"/>
       <c r="AD22" s="10" t="s">
-        <v>499</v>
+        <v>454</v>
       </c>
       <c r="AE22" s="127" t="s">
         <v>112</v>
@@ -4910,10 +5254,31 @@
         <v>151</v>
       </c>
       <c r="AH22" s="3" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="23" spans="1:34">
+        <v>482</v>
+      </c>
+      <c r="AJ22" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="AK22" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="AL22" s="135" t="s">
+        <v>524</v>
+      </c>
+      <c r="AM22" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="AN22" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="AO22" s="3">
+        <v>5304</v>
+      </c>
+      <c r="AP22" s="3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42">
       <c r="A23" s="129"/>
       <c r="B23" s="129">
         <v>1</v>
@@ -4957,31 +5322,31 @@
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
       <c r="T23" s="12"/>
-      <c r="V23" s="114" t="s">
-        <v>218</v>
-      </c>
-      <c r="W23" s="114" t="s">
-        <v>219</v>
-      </c>
-      <c r="X23" s="114" t="s">
-        <v>224</v>
-      </c>
-      <c r="Y23" s="114" t="s">
-        <v>227</v>
-      </c>
-      <c r="Z23" s="114" t="s">
-        <v>220</v>
-      </c>
-      <c r="AA23" s="114" t="s">
-        <v>284</v>
-      </c>
-      <c r="AB23" s="114" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="24" spans="1:34">
+      <c r="AJ23" s="205" t="s">
+        <v>573</v>
+      </c>
+      <c r="AK23" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="AL23" s="135" t="s">
+        <v>523</v>
+      </c>
+      <c r="AM23" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="AN23" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="AO23" s="10">
+        <v>5305</v>
+      </c>
+      <c r="AP23" s="10">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42">
       <c r="A24" s="129" t="s">
-        <v>406</v>
+        <v>361</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>53</v>
@@ -4996,7 +5361,7 @@
         <v>56</v>
       </c>
       <c r="F24" s="130" t="s">
-        <v>466</v>
+        <v>421</v>
       </c>
       <c r="G24" s="130" t="s">
         <v>57</v>
@@ -5016,42 +5381,58 @@
       <c r="L24" s="131" t="s">
         <v>62</v>
       </c>
-      <c r="M24" s="130"/>
+      <c r="M24" s="135" t="s">
+        <v>528</v>
+      </c>
       <c r="N24" s="129" t="s">
-        <v>406</v>
+        <v>361</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="11"/>
-      <c r="Z24" s="10"/>
-      <c r="AA24" s="10"/>
-      <c r="AB24" s="10"/>
-      <c r="AD24" s="147" t="s">
-        <v>542</v>
-      </c>
-      <c r="AE24" s="147"/>
-      <c r="AF24" s="147"/>
-      <c r="AG24" s="147"/>
-      <c r="AH24" s="147"/>
-    </row>
-    <row r="25" spans="1:34">
+      <c r="AD24" s="141" t="s">
+        <v>497</v>
+      </c>
+      <c r="AE24" s="141"/>
+      <c r="AF24" s="141"/>
+      <c r="AG24" s="141"/>
+      <c r="AH24" s="141"/>
+      <c r="AJ24" s="205" t="s">
+        <v>576</v>
+      </c>
+      <c r="AK24" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="AL24" s="135" t="s">
+        <v>528</v>
+      </c>
+      <c r="AM24" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="AN24" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="AO24" s="3">
+        <v>5306</v>
+      </c>
+      <c r="AP24" s="3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="25" spans="1:42">
       <c r="A25" s="129" t="s">
-        <v>407</v>
+        <v>362</v>
       </c>
       <c r="B25" s="127" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="130" t="s">
-        <v>467</v>
+        <v>422</v>
       </c>
       <c r="D25" s="130" t="s">
-        <v>468</v>
+        <v>423</v>
       </c>
       <c r="E25" s="130" t="s">
         <v>27</v>
@@ -5060,7 +5441,7 @@
         <v>28</v>
       </c>
       <c r="G25" s="130" t="s">
-        <v>469</v>
+        <v>424</v>
       </c>
       <c r="H25" s="131" t="s">
         <v>29</v>
@@ -5077,9 +5458,11 @@
       <c r="L25" s="130" t="s">
         <v>33</v>
       </c>
-      <c r="M25" s="130"/>
+      <c r="M25" s="130" t="s">
+        <v>529</v>
+      </c>
       <c r="N25" s="129" t="s">
-        <v>407</v>
+        <v>362</v>
       </c>
       <c r="R25" s="37"/>
       <c r="S25" s="37"/>
@@ -5108,38 +5491,40 @@
         <v>227</v>
       </c>
     </row>
-    <row r="26" spans="1:34">
+    <row r="26" spans="1:42">
       <c r="A26" s="129" t="s">
-        <v>408</v>
+        <v>363</v>
       </c>
       <c r="B26" s="131" t="s">
-        <v>470</v>
+        <v>425</v>
       </c>
       <c r="C26" s="131" t="s">
-        <v>471</v>
+        <v>426</v>
       </c>
       <c r="D26" s="130" t="s">
-        <v>472</v>
+        <v>427</v>
       </c>
       <c r="E26" s="131" t="s">
-        <v>473</v>
+        <v>428</v>
       </c>
       <c r="F26" s="130"/>
       <c r="G26" s="130"/>
       <c r="H26" s="131" t="s">
-        <v>474</v>
+        <v>429</v>
       </c>
       <c r="I26" s="130"/>
       <c r="J26" s="130" t="s">
-        <v>475</v>
+        <v>430</v>
       </c>
       <c r="K26" s="131" t="s">
-        <v>476</v>
+        <v>431</v>
       </c>
       <c r="L26" s="130"/>
-      <c r="M26" s="130"/>
+      <c r="M26" s="130" t="s">
+        <v>530</v>
+      </c>
       <c r="N26" s="129" t="s">
-        <v>408</v>
+        <v>363</v>
       </c>
       <c r="O26" s="13"/>
       <c r="P26" s="2"/>
@@ -5155,24 +5540,24 @@
       <c r="AA26" s="12"/>
       <c r="AB26" s="12"/>
       <c r="AD26" s="3" t="s">
-        <v>538</v>
+        <v>493</v>
       </c>
       <c r="AE26" s="128" t="s">
         <v>78</v>
       </c>
       <c r="AF26" s="3" t="s">
-        <v>540</v>
+        <v>495</v>
       </c>
       <c r="AG26" s="128" t="s">
         <v>25</v>
       </c>
       <c r="AH26" s="3" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="27" spans="1:34">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="27" spans="1:42">
       <c r="A27" s="129" t="s">
-        <v>409</v>
+        <v>364</v>
       </c>
       <c r="B27" s="127" t="s">
         <v>101</v>
@@ -5190,7 +5575,7 @@
         <v>105</v>
       </c>
       <c r="G27" s="130" t="s">
-        <v>477</v>
+        <v>432</v>
       </c>
       <c r="H27" s="127" t="s">
         <v>106</v>
@@ -5207,9 +5592,11 @@
       <c r="L27" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="M27" s="130"/>
+      <c r="M27" s="130" t="s">
+        <v>531</v>
+      </c>
       <c r="N27" s="129" t="s">
-        <v>409</v>
+        <v>364</v>
       </c>
       <c r="O27" s="13"/>
       <c r="R27" s="12"/>
@@ -5224,9 +5611,9 @@
       <c r="AA27" s="12"/>
       <c r="AB27" s="12"/>
     </row>
-    <row r="28" spans="1:34">
+    <row r="28" spans="1:42">
       <c r="A28" s="129" t="s">
-        <v>410</v>
+        <v>365</v>
       </c>
       <c r="B28" s="130" t="s">
         <v>63</v>
@@ -5262,19 +5649,19 @@
         <v>73</v>
       </c>
       <c r="M28" s="131" t="s">
-        <v>478</v>
+        <v>433</v>
       </c>
       <c r="N28" s="129" t="s">
-        <v>410</v>
+        <v>365</v>
       </c>
       <c r="R28" s="12"/>
       <c r="S28" s="12"/>
       <c r="T28" s="12"/>
       <c r="U28" s="12"/>
     </row>
-    <row r="29" spans="1:34">
+    <row r="29" spans="1:42">
       <c r="A29" s="129" t="s">
-        <v>411</v>
+        <v>366</v>
       </c>
       <c r="B29" s="131" t="s">
         <v>34</v>
@@ -5286,7 +5673,7 @@
         <v>36</v>
       </c>
       <c r="E29" s="130" t="s">
-        <v>479</v>
+        <v>434</v>
       </c>
       <c r="F29" s="131" t="s">
         <v>37</v>
@@ -5301,7 +5688,7 @@
         <v>40</v>
       </c>
       <c r="J29" s="130" t="s">
-        <v>480</v>
+        <v>435</v>
       </c>
       <c r="K29" s="130" t="s">
         <v>41</v>
@@ -5310,10 +5697,10 @@
         <v>42</v>
       </c>
       <c r="M29" s="131" t="s">
-        <v>481</v>
+        <v>436</v>
       </c>
       <c r="N29" s="129" t="s">
-        <v>411</v>
+        <v>366</v>
       </c>
       <c r="O29" s="12"/>
       <c r="P29" s="12"/>
@@ -5321,17 +5708,17 @@
       <c r="S29" s="35"/>
       <c r="T29" s="35"/>
       <c r="U29" s="35"/>
-      <c r="V29" s="147" t="s">
+      <c r="V29" s="141" t="s">
         <v>212</v>
       </c>
-      <c r="W29" s="147"/>
-      <c r="X29" s="147"/>
-      <c r="Y29" s="147"/>
-      <c r="Z29" s="147"/>
-      <c r="AA29" s="147"/>
-      <c r="AB29" s="147"/>
-    </row>
-    <row r="30" spans="1:34">
+      <c r="W29" s="141"/>
+      <c r="X29" s="141"/>
+      <c r="Y29" s="141"/>
+      <c r="Z29" s="141"/>
+      <c r="AA29" s="141"/>
+      <c r="AB29" s="141"/>
+    </row>
+    <row r="30" spans="1:42">
       <c r="A30" s="129"/>
       <c r="B30" s="129">
         <v>1</v>
@@ -5392,7 +5779,7 @@
       <c r="AA30" s="114"/>
       <c r="AB30" s="114"/>
     </row>
-    <row r="31" spans="1:34">
+    <row r="31" spans="1:42">
       <c r="A31" s="12"/>
       <c r="B31" s="37"/>
       <c r="C31" s="37"/>
@@ -5419,13 +5806,13 @@
       <c r="Y31" s="37"/>
       <c r="Z31" s="37"/>
       <c r="AA31" s="12"/>
-      <c r="AD31" s="148" t="s">
+      <c r="AD31" s="142" t="s">
         <v>263</v>
       </c>
-      <c r="AE31" s="149"/>
-      <c r="AF31" s="150"/>
-    </row>
-    <row r="32" spans="1:34">
+      <c r="AE31" s="143"/>
+      <c r="AF31" s="144"/>
+    </row>
+    <row r="32" spans="1:42">
       <c r="S32" s="12"/>
       <c r="T32" s="117"/>
       <c r="U32" s="117"/>
@@ -5528,15 +5915,15 @@
       <c r="S37" s="12"/>
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
-      <c r="V37" s="147" t="s">
+      <c r="V37" s="141" t="s">
         <v>9</v>
       </c>
-      <c r="W37" s="147"/>
-      <c r="X37" s="147"/>
-      <c r="Y37" s="147"/>
-      <c r="Z37" s="147"/>
-      <c r="AA37" s="147"/>
-      <c r="AB37" s="147"/>
+      <c r="W37" s="141"/>
+      <c r="X37" s="141"/>
+      <c r="Y37" s="141"/>
+      <c r="Z37" s="141"/>
+      <c r="AA37" s="141"/>
+      <c r="AB37" s="141"/>
       <c r="AD37" s="3" t="s">
         <v>259</v>
       </c>
@@ -5585,7 +5972,7 @@
       <c r="T39" s="12"/>
       <c r="U39" s="12"/>
       <c r="V39" s="10" t="s">
-        <v>385</v>
+        <v>340</v>
       </c>
       <c r="W39" s="10"/>
       <c r="X39" s="10"/>
@@ -5635,15 +6022,15 @@
       <c r="S42" s="12"/>
       <c r="T42" s="12"/>
       <c r="U42" s="12"/>
-      <c r="V42" s="147" t="s">
+      <c r="V42" s="141" t="s">
         <v>247</v>
       </c>
-      <c r="W42" s="147"/>
-      <c r="X42" s="147"/>
-      <c r="Y42" s="147"/>
-      <c r="Z42" s="147"/>
-      <c r="AA42" s="147"/>
-      <c r="AB42" s="147"/>
+      <c r="W42" s="141"/>
+      <c r="X42" s="141"/>
+      <c r="Y42" s="141"/>
+      <c r="Z42" s="141"/>
+      <c r="AA42" s="141"/>
+      <c r="AB42" s="141"/>
       <c r="AD42" s="3" t="s">
         <v>265</v>
       </c>
@@ -5655,7 +6042,7 @@
       <c r="T43" s="12"/>
       <c r="U43" s="12"/>
       <c r="V43" s="115" t="s">
-        <v>484</v>
+        <v>439</v>
       </c>
       <c r="W43" s="115" t="s">
         <v>218</v>
@@ -5664,7 +6051,7 @@
         <v>224</v>
       </c>
       <c r="Y43" s="115" t="s">
-        <v>483</v>
+        <v>438</v>
       </c>
       <c r="Z43" s="115" t="s">
         <v>278</v>
@@ -5748,15 +6135,15 @@
       <c r="S48" s="12"/>
       <c r="T48" s="12"/>
       <c r="U48" s="12"/>
-      <c r="V48" s="148" t="s">
-        <v>529</v>
-      </c>
-      <c r="W48" s="149"/>
-      <c r="X48" s="149"/>
-      <c r="Y48" s="149"/>
-      <c r="Z48" s="149"/>
-      <c r="AA48" s="149"/>
-      <c r="AB48" s="150"/>
+      <c r="V48" s="142" t="s">
+        <v>484</v>
+      </c>
+      <c r="W48" s="143"/>
+      <c r="X48" s="143"/>
+      <c r="Y48" s="143"/>
+      <c r="Z48" s="143"/>
+      <c r="AA48" s="143"/>
+      <c r="AB48" s="144"/>
     </row>
     <row r="49" spans="19:28">
       <c r="S49" s="12"/>
@@ -5766,16 +6153,18 @@
         <v>281</v>
       </c>
       <c r="W49" s="115" t="s">
-        <v>384</v>
+        <v>339</v>
       </c>
       <c r="X49" s="115" t="s">
-        <v>530</v>
+        <v>485</v>
       </c>
       <c r="Y49" s="115" t="s">
         <v>227</v>
       </c>
       <c r="Z49" s="115"/>
-      <c r="AA49" s="115"/>
+      <c r="AA49" s="138" t="s">
+        <v>220</v>
+      </c>
       <c r="AB49" s="115"/>
     </row>
     <row r="50" spans="19:28">
@@ -5783,30 +6172,32 @@
       <c r="T50" s="12"/>
       <c r="U50" s="12"/>
       <c r="V50" s="10" t="s">
-        <v>531</v>
+        <v>486</v>
       </c>
       <c r="W50" s="10" t="s">
         <v>271</v>
       </c>
       <c r="X50" s="10" t="s">
-        <v>532</v>
+        <v>487</v>
       </c>
       <c r="Y50" s="12"/>
       <c r="Z50" s="12"/>
-      <c r="AA50" s="12"/>
+      <c r="AA50" s="12" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="51" spans="19:28">
       <c r="S51" s="12"/>
       <c r="T51" s="12"/>
       <c r="U51" s="12"/>
       <c r="V51" s="10" t="s">
-        <v>531</v>
+        <v>486</v>
       </c>
       <c r="W51" s="10" t="s">
         <v>252</v>
       </c>
       <c r="X51" s="10" t="s">
-        <v>533</v>
+        <v>488</v>
       </c>
       <c r="Y51" s="12"/>
       <c r="Z51" s="12"/>
@@ -5817,13 +6208,13 @@
       <c r="T52" s="12"/>
       <c r="U52" s="12"/>
       <c r="V52" s="10" t="s">
-        <v>531</v>
+        <v>486</v>
       </c>
       <c r="W52" s="10" t="s">
-        <v>534</v>
+        <v>489</v>
       </c>
       <c r="X52" s="10" t="s">
-        <v>535</v>
+        <v>490</v>
       </c>
       <c r="Y52" s="12"/>
       <c r="Z52" s="12"/>
@@ -5844,8 +6235,8 @@
   <mergeCells count="12">
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
-    <mergeCell ref="V16:AB16"/>
-    <mergeCell ref="V22:AB22"/>
+    <mergeCell ref="AJ4:AP4"/>
+    <mergeCell ref="AJ17:AP17"/>
     <mergeCell ref="AD31:AF31"/>
     <mergeCell ref="V29:AB29"/>
     <mergeCell ref="AD24:AH24"/>
@@ -5862,10 +6253,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:AD32"/>
+  <dimension ref="B2:AJ32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -5879,44 +6270,51 @@
     <col min="25" max="25" width="1.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:30">
-      <c r="B2" s="147" t="s">
+    <row r="2" spans="2:36">
+      <c r="B2" s="141" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="H2" s="147" t="s">
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="141"/>
+      <c r="H2" s="141" t="s">
         <v>231</v>
       </c>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="147"/>
-      <c r="L2" s="147"/>
-      <c r="N2" s="147" t="s">
+      <c r="I2" s="141"/>
+      <c r="J2" s="141"/>
+      <c r="K2" s="141"/>
+      <c r="L2" s="141"/>
+      <c r="N2" s="141" t="s">
         <v>239</v>
       </c>
-      <c r="O2" s="147"/>
-      <c r="P2" s="147"/>
-      <c r="Q2" s="147"/>
-      <c r="R2" s="147"/>
-      <c r="T2" s="147" t="s">
+      <c r="O2" s="141"/>
+      <c r="P2" s="141"/>
+      <c r="Q2" s="141"/>
+      <c r="R2" s="141"/>
+      <c r="T2" s="141" t="s">
         <v>249</v>
       </c>
-      <c r="U2" s="147"/>
-      <c r="V2" s="147"/>
-      <c r="W2" s="147"/>
-      <c r="X2" s="147"/>
-      <c r="Z2" s="147" t="s">
+      <c r="U2" s="141"/>
+      <c r="V2" s="141"/>
+      <c r="W2" s="141"/>
+      <c r="X2" s="141"/>
+      <c r="Z2" s="141" t="s">
         <v>321</v>
       </c>
-      <c r="AA2" s="147"/>
-      <c r="AB2" s="147"/>
-      <c r="AC2" s="147"/>
-      <c r="AD2" s="147"/>
-    </row>
-    <row r="3" spans="2:30">
+      <c r="AA2" s="141"/>
+      <c r="AB2" s="141"/>
+      <c r="AC2" s="141"/>
+      <c r="AD2" s="141"/>
+      <c r="AF2" s="141" t="s">
+        <v>502</v>
+      </c>
+      <c r="AG2" s="141"/>
+      <c r="AH2" s="141"/>
+      <c r="AI2" s="141"/>
+      <c r="AJ2" s="141"/>
+    </row>
+    <row r="3" spans="2:36">
       <c r="B3" s="124" t="s">
         <v>218</v>
       </c>
@@ -5924,7 +6322,7 @@
         <v>281</v>
       </c>
       <c r="D3" s="125" t="s">
-        <v>501</v>
+        <v>456</v>
       </c>
       <c r="E3" s="124" t="s">
         <v>282</v>
@@ -5939,7 +6337,7 @@
         <v>281</v>
       </c>
       <c r="J3" s="125" t="s">
-        <v>501</v>
+        <v>456</v>
       </c>
       <c r="K3" s="124" t="s">
         <v>282</v>
@@ -5954,7 +6352,7 @@
         <v>281</v>
       </c>
       <c r="P3" s="125" t="s">
-        <v>501</v>
+        <v>456</v>
       </c>
       <c r="Q3" s="124" t="s">
         <v>282</v>
@@ -5969,7 +6367,7 @@
         <v>281</v>
       </c>
       <c r="V3" s="125" t="s">
-        <v>501</v>
+        <v>456</v>
       </c>
       <c r="W3" s="124" t="s">
         <v>282</v>
@@ -5984,7 +6382,7 @@
         <v>281</v>
       </c>
       <c r="AB3" s="125" t="s">
-        <v>501</v>
+        <v>456</v>
       </c>
       <c r="AC3" s="124" t="s">
         <v>282</v>
@@ -5992,8 +6390,23 @@
       <c r="AD3" s="125" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="4" spans="2:30">
+      <c r="AF3" s="124" t="s">
+        <v>218</v>
+      </c>
+      <c r="AG3" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="AH3" s="125" t="s">
+        <v>456</v>
+      </c>
+      <c r="AI3" s="124" t="s">
+        <v>282</v>
+      </c>
+      <c r="AJ3" s="125" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="4" spans="2:36">
       <c r="B4" s="3" t="s">
         <v>333</v>
       </c>
@@ -6005,8 +6418,29 @@
       <c r="F4" s="126" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="5" spans="2:30">
+      <c r="H4" t="s">
+        <v>506</v>
+      </c>
+      <c r="N4" t="s">
+        <v>507</v>
+      </c>
+      <c r="T4" t="s">
+        <v>511</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>500</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>486</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>503</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="5" spans="2:36">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="126"/>
@@ -6017,7 +6451,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="6" spans="2:30">
+    <row r="6" spans="2:36">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="126"/>
@@ -6027,8 +6461,14 @@
       <c r="F6" s="126" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="7" spans="2:30">
+      <c r="H6" t="s">
+        <v>509</v>
+      </c>
+      <c r="N6" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="7" spans="2:36">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="126"/>
@@ -6039,273 +6479,217 @@
         <v>329</v>
       </c>
     </row>
-    <row r="8" spans="2:30">
+    <row r="8" spans="2:36">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="126"/>
       <c r="E8" s="3"/>
       <c r="F8" s="126"/>
-    </row>
-    <row r="9" spans="2:30">
-      <c r="B9" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="126"/>
-      <c r="E9" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="F9" s="126" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="10" spans="2:30">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="126"/>
-      <c r="E10" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="F10" s="126" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="11" spans="2:30">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="126"/>
-      <c r="E11" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="F11" s="126" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="12" spans="2:30">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="126"/>
-      <c r="E12" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="F12" s="126" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="13" spans="2:30">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="126"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="126"/>
-    </row>
-    <row r="14" spans="2:30">
-      <c r="B14" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="126"/>
-      <c r="E14" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="F14" s="126" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="15" spans="2:30">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="126"/>
-      <c r="E15" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="F15" s="126" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="16" spans="2:30">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="126"/>
-      <c r="E16" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="F16" s="126" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="126"/>
-      <c r="E17" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="F17" s="126" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="126"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="126"/>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="B19" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="126"/>
-      <c r="E19" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="F19" s="126" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="F20" s="126" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="126"/>
-      <c r="E21" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="F21" s="126" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="126"/>
-      <c r="E22" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="F22" s="126" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="126"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="126"/>
-    </row>
-    <row r="24" spans="2:6">
-      <c r="B24" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="126"/>
-      <c r="E24" s="3" t="s">
+      <c r="Z8" t="s">
+        <v>501</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>486</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>504</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="9" spans="2:36">
+      <c r="B9" t="s">
+        <v>505</v>
+      </c>
+      <c r="D9" s="74"/>
+      <c r="H9" t="s">
+        <v>512</v>
+      </c>
+      <c r="J9"/>
+    </row>
+    <row r="10" spans="2:36">
+      <c r="B10" s="139"/>
+      <c r="C10" s="139"/>
+      <c r="D10" s="140"/>
+      <c r="E10" s="139"/>
+      <c r="F10" s="140"/>
+    </row>
+    <row r="11" spans="2:36">
+      <c r="B11" s="139" t="s">
+        <v>508</v>
+      </c>
+      <c r="C11" s="139"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="139"/>
+      <c r="F11" s="140"/>
+    </row>
+    <row r="12" spans="2:36">
+      <c r="B12" s="139"/>
+      <c r="C12" s="139"/>
+      <c r="D12" s="140"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="140"/>
+    </row>
+    <row r="13" spans="2:36">
+      <c r="B13" s="139"/>
+      <c r="C13" s="139"/>
+      <c r="D13" s="140"/>
+      <c r="E13" s="139"/>
+      <c r="F13" s="140"/>
+    </row>
+    <row r="14" spans="2:36">
+      <c r="B14" s="139"/>
+      <c r="C14" s="139"/>
+      <c r="D14" s="140"/>
+      <c r="E14" s="139"/>
+      <c r="F14" s="140"/>
+    </row>
+    <row r="15" spans="2:36">
+      <c r="B15" s="139"/>
+      <c r="C15" s="139"/>
+      <c r="D15" s="140"/>
+      <c r="E15" s="139"/>
+      <c r="F15" s="140"/>
+    </row>
+    <row r="16" spans="2:36">
+      <c r="B16" s="139"/>
+      <c r="C16" s="139"/>
+      <c r="D16" s="140"/>
+      <c r="E16" s="139"/>
+      <c r="F16" s="140"/>
+    </row>
+    <row r="17" spans="2:20">
+      <c r="B17" s="139"/>
+      <c r="C17" s="139"/>
+      <c r="D17" s="140"/>
+      <c r="E17" s="139"/>
+      <c r="F17" s="140"/>
+    </row>
+    <row r="18" spans="2:20">
+      <c r="B18" s="139"/>
+      <c r="C18" s="139"/>
+      <c r="D18" s="140"/>
+      <c r="E18" s="139"/>
+      <c r="F18" s="140"/>
+    </row>
+    <row r="19" spans="2:20">
+      <c r="B19" s="139"/>
+      <c r="C19" s="139"/>
+      <c r="D19" s="140"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="140"/>
+      <c r="H19" t="s">
         <v>362</v>
       </c>
-      <c r="F24" s="126" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="126"/>
-      <c r="E25" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="F25" s="126" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="126"/>
-      <c r="E26" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="F26" s="126" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="126"/>
-      <c r="E27" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="F27" s="126" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6">
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="126"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="126"/>
-    </row>
-    <row r="29" spans="2:6">
-      <c r="B29" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="126"/>
-      <c r="E29" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="F29" s="126" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6">
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="126"/>
-      <c r="E30" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="F30" s="126" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6">
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="126"/>
-      <c r="E31" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="F31" s="126" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6">
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="126"/>
-      <c r="E32" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="F32" s="126" t="s">
-        <v>375</v>
-      </c>
+      <c r="T19" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20">
+      <c r="B20" s="139" t="s">
+        <v>362</v>
+      </c>
+      <c r="C20" s="139"/>
+      <c r="D20" s="140"/>
+      <c r="E20" s="139"/>
+      <c r="F20" s="140"/>
+      <c r="H20" t="s">
+        <v>514</v>
+      </c>
+      <c r="T20" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20">
+      <c r="B21" s="139" t="s">
+        <v>513</v>
+      </c>
+      <c r="C21" s="139"/>
+      <c r="D21" s="140"/>
+      <c r="E21" s="139"/>
+      <c r="F21" s="140"/>
+    </row>
+    <row r="22" spans="2:20">
+      <c r="B22" s="139"/>
+      <c r="C22" s="139"/>
+      <c r="D22" s="140"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="140"/>
+    </row>
+    <row r="23" spans="2:20">
+      <c r="B23" s="139"/>
+      <c r="C23" s="139"/>
+      <c r="D23" s="140"/>
+      <c r="E23" s="139"/>
+      <c r="F23" s="140"/>
+    </row>
+    <row r="24" spans="2:20">
+      <c r="B24" s="139"/>
+      <c r="C24" s="139"/>
+      <c r="D24" s="140"/>
+      <c r="E24" s="139"/>
+      <c r="F24" s="140"/>
+    </row>
+    <row r="25" spans="2:20">
+      <c r="B25" s="139"/>
+      <c r="C25" s="139"/>
+      <c r="D25" s="140"/>
+      <c r="E25" s="139"/>
+      <c r="F25" s="140"/>
+    </row>
+    <row r="26" spans="2:20">
+      <c r="B26" s="139"/>
+      <c r="C26" s="139"/>
+      <c r="D26" s="140"/>
+      <c r="E26" s="139"/>
+      <c r="F26" s="140"/>
+    </row>
+    <row r="27" spans="2:20">
+      <c r="B27" s="139"/>
+      <c r="C27" s="139"/>
+      <c r="D27" s="140"/>
+      <c r="E27" s="139"/>
+      <c r="F27" s="140"/>
+    </row>
+    <row r="28" spans="2:20">
+      <c r="B28" s="139"/>
+      <c r="C28" s="139"/>
+      <c r="D28" s="140"/>
+      <c r="E28" s="139"/>
+      <c r="F28" s="140"/>
+    </row>
+    <row r="29" spans="2:20">
+      <c r="B29" s="139"/>
+      <c r="C29" s="139"/>
+      <c r="D29" s="140"/>
+      <c r="E29" s="139"/>
+      <c r="F29" s="140"/>
+    </row>
+    <row r="30" spans="2:20">
+      <c r="B30" s="139"/>
+      <c r="C30" s="139"/>
+      <c r="D30" s="140"/>
+      <c r="E30" s="139"/>
+      <c r="F30" s="140"/>
+    </row>
+    <row r="31" spans="2:20">
+      <c r="B31" s="139"/>
+      <c r="C31" s="139"/>
+      <c r="D31" s="140"/>
+      <c r="E31" s="139"/>
+      <c r="F31" s="140"/>
+    </row>
+    <row r="32" spans="2:20">
+      <c r="B32" s="139"/>
+      <c r="C32" s="139"/>
+      <c r="D32" s="140"/>
+      <c r="E32" s="139"/>
+      <c r="F32" s="140"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="AF2:AJ2"/>
     <mergeCell ref="Z2:AD2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="H2:L2"/>
@@ -6339,40 +6723,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="138" t="s">
-        <v>379</v>
-      </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="140"/>
+      <c r="A1" s="146" t="s">
+        <v>334</v>
+      </c>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="148"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="141"/>
-      <c r="B2" s="142"/>
-      <c r="C2" s="142"/>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="143"/>
+      <c r="A2" s="149"/>
+      <c r="B2" s="150"/>
+      <c r="C2" s="150"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="151"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="144" t="s">
+      <c r="A3" s="152" t="s">
         <v>253</v>
       </c>
-      <c r="B3" s="145"/>
-      <c r="C3" s="145"/>
-      <c r="D3" s="145"/>
-      <c r="E3" s="145" t="s">
+      <c r="B3" s="153"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153" t="s">
         <v>254</v>
       </c>
-      <c r="F3" s="145"/>
-      <c r="G3" s="145"/>
-      <c r="H3" s="146"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="154"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="20">
@@ -6977,28 +7361,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="155" t="s">
-        <v>380</v>
-      </c>
-      <c r="B1" s="155"/>
-      <c r="C1" s="155"/>
-      <c r="D1" s="155"/>
-      <c r="E1" s="155"/>
-      <c r="F1" s="155"/>
-      <c r="G1" s="155"/>
-      <c r="H1" s="155"/>
+      <c r="A1" s="158" t="s">
+        <v>335</v>
+      </c>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="158"/>
+      <c r="H1" s="158"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="152" t="s">
+      <c r="A2" s="155" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="153"/>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
-      <c r="G2" s="153"/>
-      <c r="H2" s="154"/>
+      <c r="B2" s="156"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="157"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="5"/>
@@ -7177,16 +7561,16 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="152" t="s">
+      <c r="A15" s="155" t="s">
         <v>225</v>
       </c>
-      <c r="B15" s="153"/>
-      <c r="C15" s="153"/>
-      <c r="D15" s="153"/>
-      <c r="E15" s="153"/>
-      <c r="F15" s="153"/>
-      <c r="G15" s="153"/>
-      <c r="H15" s="154"/>
+      <c r="B15" s="156"/>
+      <c r="C15" s="156"/>
+      <c r="D15" s="156"/>
+      <c r="E15" s="156"/>
+      <c r="F15" s="156"/>
+      <c r="G15" s="156"/>
+      <c r="H15" s="157"/>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="9"/>
@@ -7362,16 +7746,16 @@
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:11" ht="15.75">
-      <c r="A28" s="152" t="s">
+      <c r="A28" s="155" t="s">
         <v>226</v>
       </c>
-      <c r="B28" s="153"/>
-      <c r="C28" s="153"/>
-      <c r="D28" s="153"/>
-      <c r="E28" s="153"/>
-      <c r="F28" s="153"/>
-      <c r="G28" s="153"/>
-      <c r="H28" s="154"/>
+      <c r="B28" s="156"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="157"/>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="5"/>
@@ -7571,40 +7955,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="156" t="s">
-        <v>381</v>
-      </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157"/>
-      <c r="F1" s="157"/>
-      <c r="G1" s="157"/>
-      <c r="H1" s="158"/>
+      <c r="A1" s="159" t="s">
+        <v>336</v>
+      </c>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="161"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="159"/>
-      <c r="B2" s="160"/>
-      <c r="C2" s="160"/>
-      <c r="D2" s="160"/>
-      <c r="E2" s="160"/>
-      <c r="F2" s="160"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="161"/>
+      <c r="A2" s="162"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="163"/>
+      <c r="H2" s="164"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="162" t="s">
+      <c r="A3" s="165" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="163"/>
-      <c r="C3" s="164"/>
-      <c r="D3" s="165"/>
-      <c r="E3" s="162" t="s">
+      <c r="B3" s="166"/>
+      <c r="C3" s="167"/>
+      <c r="D3" s="168"/>
+      <c r="E3" s="165" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="163"/>
-      <c r="G3" s="164"/>
-      <c r="H3" s="165"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="167"/>
+      <c r="H3" s="168"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="16">
@@ -8043,40 +8427,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="166" t="s">
-        <v>382</v>
-      </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
+      <c r="A1" s="169" t="s">
+        <v>337</v>
+      </c>
+      <c r="B1" s="169"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="169"/>
+      <c r="H1" s="169"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="167"/>
-      <c r="B2" s="167"/>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-      <c r="F2" s="167"/>
-      <c r="G2" s="167"/>
-      <c r="H2" s="167"/>
+      <c r="A2" s="170"/>
+      <c r="B2" s="170"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="170"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="171" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="169"/>
-      <c r="C3" s="170"/>
-      <c r="D3" s="171"/>
-      <c r="E3" s="168" t="s">
+      <c r="B3" s="172"/>
+      <c r="C3" s="173"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="171" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="169"/>
-      <c r="G3" s="170"/>
-      <c r="H3" s="171"/>
+      <c r="F3" s="172"/>
+      <c r="G3" s="173"/>
+      <c r="H3" s="174"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="46">
@@ -8369,114 +8753,114 @@
       <c r="H24" s="74"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="168" t="s">
+      <c r="A25" s="171" t="s">
         <v>293</v>
       </c>
-      <c r="B25" s="169"/>
-      <c r="C25" s="170"/>
-      <c r="D25" s="171"/>
-      <c r="E25" s="168" t="s">
+      <c r="B25" s="172"/>
+      <c r="C25" s="173"/>
+      <c r="D25" s="174"/>
+      <c r="E25" s="171" t="s">
         <v>294</v>
       </c>
-      <c r="F25" s="169"/>
-      <c r="G25" s="170"/>
-      <c r="H25" s="171"/>
+      <c r="F25" s="172"/>
+      <c r="G25" s="173"/>
+      <c r="H25" s="174"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="50" t="s">
         <v>295</v>
       </c>
-      <c r="B26" s="172"/>
-      <c r="C26" s="173"/>
-      <c r="D26" s="174"/>
+      <c r="B26" s="175"/>
+      <c r="C26" s="176"/>
+      <c r="D26" s="177"/>
       <c r="E26" s="46" t="s">
         <v>296</v>
       </c>
-      <c r="F26" s="175"/>
-      <c r="G26" s="176"/>
-      <c r="H26" s="177"/>
+      <c r="F26" s="178"/>
+      <c r="G26" s="179"/>
+      <c r="H26" s="180"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="B27" s="178"/>
-      <c r="C27" s="179"/>
-      <c r="D27" s="180"/>
+      <c r="B27" s="181"/>
+      <c r="C27" s="182"/>
+      <c r="D27" s="183"/>
       <c r="E27" s="50" t="s">
         <v>298</v>
       </c>
-      <c r="F27" s="172"/>
-      <c r="G27" s="173"/>
-      <c r="H27" s="181"/>
+      <c r="F27" s="175"/>
+      <c r="G27" s="176"/>
+      <c r="H27" s="184"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="50" t="s">
         <v>299</v>
       </c>
-      <c r="B28" s="172"/>
-      <c r="C28" s="173"/>
-      <c r="D28" s="174"/>
+      <c r="B28" s="175"/>
+      <c r="C28" s="176"/>
+      <c r="D28" s="177"/>
       <c r="E28" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="F28" s="178"/>
-      <c r="G28" s="179"/>
-      <c r="H28" s="182"/>
+      <c r="F28" s="181"/>
+      <c r="G28" s="182"/>
+      <c r="H28" s="185"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="58" t="s">
         <v>301</v>
       </c>
-      <c r="B29" s="178"/>
-      <c r="C29" s="179"/>
-      <c r="D29" s="180"/>
+      <c r="B29" s="181"/>
+      <c r="C29" s="182"/>
+      <c r="D29" s="183"/>
       <c r="E29" s="50" t="s">
         <v>302</v>
       </c>
-      <c r="F29" s="172"/>
-      <c r="G29" s="173"/>
-      <c r="H29" s="181"/>
+      <c r="F29" s="175"/>
+      <c r="G29" s="176"/>
+      <c r="H29" s="184"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="50" t="s">
         <v>303</v>
       </c>
-      <c r="B30" s="172"/>
-      <c r="C30" s="173"/>
-      <c r="D30" s="174"/>
+      <c r="B30" s="175"/>
+      <c r="C30" s="176"/>
+      <c r="D30" s="177"/>
       <c r="E30" s="58" t="s">
         <v>304</v>
       </c>
-      <c r="F30" s="178"/>
-      <c r="G30" s="179"/>
-      <c r="H30" s="182"/>
+      <c r="F30" s="181"/>
+      <c r="G30" s="182"/>
+      <c r="H30" s="185"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="B31" s="178"/>
-      <c r="C31" s="179"/>
-      <c r="D31" s="180"/>
+      <c r="B31" s="181"/>
+      <c r="C31" s="182"/>
+      <c r="D31" s="183"/>
       <c r="E31" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="F31" s="172"/>
-      <c r="G31" s="173"/>
-      <c r="H31" s="181"/>
+      <c r="F31" s="175"/>
+      <c r="G31" s="176"/>
+      <c r="H31" s="184"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="50" t="s">
         <v>307</v>
       </c>
-      <c r="B32" s="172"/>
-      <c r="C32" s="173"/>
-      <c r="D32" s="174"/>
+      <c r="B32" s="175"/>
+      <c r="C32" s="176"/>
+      <c r="D32" s="177"/>
       <c r="E32" s="58"/>
-      <c r="F32" s="178"/>
-      <c r="G32" s="179"/>
-      <c r="H32" s="182" t="s">
+      <c r="F32" s="181"/>
+      <c r="G32" s="182"/>
+      <c r="H32" s="185" t="s">
         <v>245</v>
       </c>
     </row>
@@ -8484,13 +8868,13 @@
       <c r="A33" s="58" t="s">
         <v>308</v>
       </c>
-      <c r="B33" s="178"/>
-      <c r="C33" s="179"/>
-      <c r="D33" s="180"/>
+      <c r="B33" s="181"/>
+      <c r="C33" s="182"/>
+      <c r="D33" s="183"/>
       <c r="E33" s="50"/>
-      <c r="F33" s="172"/>
-      <c r="G33" s="173"/>
-      <c r="H33" s="181" t="s">
+      <c r="F33" s="175"/>
+      <c r="G33" s="176"/>
+      <c r="H33" s="184" t="s">
         <v>288</v>
       </c>
     </row>
@@ -8498,13 +8882,13 @@
       <c r="A34" s="50" t="s">
         <v>309</v>
       </c>
-      <c r="B34" s="172"/>
-      <c r="C34" s="173"/>
-      <c r="D34" s="174"/>
+      <c r="B34" s="175"/>
+      <c r="C34" s="176"/>
+      <c r="D34" s="177"/>
       <c r="E34" s="58"/>
-      <c r="F34" s="178"/>
-      <c r="G34" s="179"/>
-      <c r="H34" s="182" t="s">
+      <c r="F34" s="181"/>
+      <c r="G34" s="182"/>
+      <c r="H34" s="185" t="s">
         <v>289</v>
       </c>
     </row>
@@ -8512,13 +8896,13 @@
       <c r="A35" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="B35" s="178"/>
-      <c r="C35" s="179"/>
-      <c r="D35" s="180"/>
+      <c r="B35" s="181"/>
+      <c r="C35" s="182"/>
+      <c r="D35" s="183"/>
       <c r="E35" s="50"/>
-      <c r="F35" s="172"/>
-      <c r="G35" s="173"/>
-      <c r="H35" s="181" t="s">
+      <c r="F35" s="175"/>
+      <c r="G35" s="176"/>
+      <c r="H35" s="184" t="s">
         <v>290</v>
       </c>
     </row>
@@ -8526,13 +8910,13 @@
       <c r="A36" s="50" t="s">
         <v>311</v>
       </c>
-      <c r="B36" s="172"/>
-      <c r="C36" s="173"/>
-      <c r="D36" s="174"/>
+      <c r="B36" s="175"/>
+      <c r="C36" s="176"/>
+      <c r="D36" s="177"/>
       <c r="E36" s="58"/>
-      <c r="F36" s="178"/>
-      <c r="G36" s="179"/>
-      <c r="H36" s="182" t="s">
+      <c r="F36" s="181"/>
+      <c r="G36" s="182"/>
+      <c r="H36" s="185" t="s">
         <v>291</v>
       </c>
     </row>
@@ -8540,13 +8924,13 @@
       <c r="A37" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="B37" s="178"/>
-      <c r="C37" s="179"/>
-      <c r="D37" s="180"/>
+      <c r="B37" s="181"/>
+      <c r="C37" s="182"/>
+      <c r="D37" s="183"/>
       <c r="E37" s="50"/>
-      <c r="F37" s="172"/>
-      <c r="G37" s="173"/>
-      <c r="H37" s="181" t="s">
+      <c r="F37" s="175"/>
+      <c r="G37" s="176"/>
+      <c r="H37" s="184" t="s">
         <v>292</v>
       </c>
     </row>
@@ -8554,13 +8938,13 @@
       <c r="A38" s="50" t="s">
         <v>313</v>
       </c>
-      <c r="B38" s="172"/>
-      <c r="C38" s="173"/>
-      <c r="D38" s="174"/>
+      <c r="B38" s="175"/>
+      <c r="C38" s="176"/>
+      <c r="D38" s="177"/>
       <c r="E38" s="58"/>
-      <c r="F38" s="178"/>
-      <c r="G38" s="179"/>
-      <c r="H38" s="182" t="s">
+      <c r="F38" s="181"/>
+      <c r="G38" s="182"/>
+      <c r="H38" s="185" t="s">
         <v>244</v>
       </c>
     </row>
@@ -8568,13 +8952,13 @@
       <c r="A39" s="58" t="s">
         <v>314</v>
       </c>
-      <c r="B39" s="178"/>
-      <c r="C39" s="179"/>
-      <c r="D39" s="180"/>
+      <c r="B39" s="181"/>
+      <c r="C39" s="182"/>
+      <c r="D39" s="183"/>
       <c r="E39" s="50"/>
-      <c r="F39" s="172"/>
-      <c r="G39" s="173"/>
-      <c r="H39" s="181" t="s">
+      <c r="F39" s="175"/>
+      <c r="G39" s="176"/>
+      <c r="H39" s="184" t="s">
         <v>245</v>
       </c>
     </row>
@@ -8582,25 +8966,25 @@
       <c r="A40" s="50" t="s">
         <v>315</v>
       </c>
-      <c r="B40" s="172"/>
-      <c r="C40" s="173"/>
-      <c r="D40" s="174"/>
+      <c r="B40" s="175"/>
+      <c r="C40" s="176"/>
+      <c r="D40" s="177"/>
       <c r="E40" s="58"/>
-      <c r="F40" s="178"/>
-      <c r="G40" s="179"/>
-      <c r="H40" s="182"/>
+      <c r="F40" s="181"/>
+      <c r="G40" s="182"/>
+      <c r="H40" s="185"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="70" t="s">
         <v>316</v>
       </c>
-      <c r="B41" s="183"/>
-      <c r="C41" s="184"/>
-      <c r="D41" s="185"/>
+      <c r="B41" s="186"/>
+      <c r="C41" s="187"/>
+      <c r="D41" s="188"/>
       <c r="E41" s="75"/>
-      <c r="F41" s="186"/>
-      <c r="G41" s="187"/>
-      <c r="H41" s="188"/>
+      <c r="F41" s="189"/>
+      <c r="G41" s="190"/>
+      <c r="H41" s="191"/>
     </row>
   </sheetData>
   <mergeCells count="37">
@@ -8669,40 +9053,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="195" t="s">
-        <v>383</v>
-      </c>
-      <c r="B1" s="196"/>
-      <c r="C1" s="196"/>
-      <c r="D1" s="196"/>
-      <c r="E1" s="196"/>
-      <c r="F1" s="196"/>
-      <c r="G1" s="196"/>
-      <c r="H1" s="197"/>
+      <c r="A1" s="198" t="s">
+        <v>338</v>
+      </c>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
+      <c r="F1" s="199"/>
+      <c r="G1" s="199"/>
+      <c r="H1" s="200"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="198"/>
-      <c r="B2" s="199"/>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="200"/>
+      <c r="A2" s="201"/>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="202"/>
+      <c r="F2" s="202"/>
+      <c r="G2" s="202"/>
+      <c r="H2" s="203"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="192" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="190"/>
-      <c r="C3" s="190"/>
-      <c r="D3" s="191"/>
-      <c r="E3" s="189" t="s">
+      <c r="B3" s="193"/>
+      <c r="C3" s="193"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="192" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="190"/>
-      <c r="G3" s="190"/>
-      <c r="H3" s="191"/>
+      <c r="F3" s="193"/>
+      <c r="G3" s="193"/>
+      <c r="H3" s="194"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="93">
@@ -8919,18 +9303,18 @@
       <c r="H21" s="85"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="192" t="s">
+      <c r="A22" s="195" t="s">
         <v>319</v>
       </c>
-      <c r="B22" s="193"/>
-      <c r="C22" s="193"/>
-      <c r="D22" s="194"/>
-      <c r="E22" s="192" t="s">
+      <c r="B22" s="196"/>
+      <c r="C22" s="196"/>
+      <c r="D22" s="197"/>
+      <c r="E22" s="195" t="s">
         <v>320</v>
       </c>
-      <c r="F22" s="193"/>
-      <c r="G22" s="193"/>
-      <c r="H22" s="194"/>
+      <c r="F22" s="196"/>
+      <c r="G22" s="196"/>
+      <c r="H22" s="197"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="78">
@@ -9207,40 +9591,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="195" t="s">
-        <v>543</v>
-      </c>
-      <c r="B1" s="196"/>
-      <c r="C1" s="196"/>
-      <c r="D1" s="196"/>
-      <c r="E1" s="196"/>
-      <c r="F1" s="196"/>
-      <c r="G1" s="196"/>
-      <c r="H1" s="197"/>
+      <c r="A1" s="198" t="s">
+        <v>498</v>
+      </c>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
+      <c r="F1" s="199"/>
+      <c r="G1" s="199"/>
+      <c r="H1" s="200"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="198"/>
-      <c r="B2" s="199"/>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="200"/>
+      <c r="A2" s="201"/>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="202"/>
+      <c r="F2" s="202"/>
+      <c r="G2" s="202"/>
+      <c r="H2" s="203"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="192" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="190"/>
-      <c r="C3" s="190"/>
-      <c r="D3" s="191"/>
-      <c r="E3" s="189" t="s">
+      <c r="B3" s="193"/>
+      <c r="C3" s="193"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="192" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="190"/>
-      <c r="G3" s="190"/>
-      <c r="H3" s="191"/>
+      <c r="F3" s="193"/>
+      <c r="G3" s="193"/>
+      <c r="H3" s="194"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="93">
@@ -9457,18 +9841,18 @@
       <c r="H21" s="85"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="192" t="s">
+      <c r="A22" s="195" t="s">
         <v>319</v>
       </c>
-      <c r="B22" s="193"/>
-      <c r="C22" s="193"/>
-      <c r="D22" s="194"/>
-      <c r="E22" s="192" t="s">
+      <c r="B22" s="196"/>
+      <c r="C22" s="196"/>
+      <c r="D22" s="197"/>
+      <c r="E22" s="195" t="s">
         <v>320</v>
       </c>
-      <c r="F22" s="193"/>
-      <c r="G22" s="193"/>
-      <c r="H22" s="194"/>
+      <c r="F22" s="196"/>
+      <c r="G22" s="196"/>
+      <c r="H22" s="197"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="78">
@@ -9745,40 +10129,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="138" t="s">
-        <v>544</v>
-      </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="140"/>
+      <c r="A1" s="146" t="s">
+        <v>499</v>
+      </c>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="148"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="141"/>
-      <c r="B2" s="142"/>
-      <c r="C2" s="142"/>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="143"/>
+      <c r="A2" s="149"/>
+      <c r="B2" s="150"/>
+      <c r="C2" s="150"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="151"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="144" t="s">
+      <c r="A3" s="152" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="145"/>
-      <c r="C3" s="145"/>
-      <c r="D3" s="145"/>
-      <c r="E3" s="145" t="s">
+      <c r="B3" s="153"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153" t="s">
         <v>322</v>
       </c>
-      <c r="F3" s="145"/>
-      <c r="G3" s="145"/>
-      <c r="H3" s="146"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="154"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="20">

</xml_diff>

<commit_message>
chg: Added range 15 info
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="580">
   <si>
     <t>AWACS</t>
   </si>
@@ -1759,6 +1759,9 @@
   </si>
   <si>
     <t>PURPLE 12</t>
+  </si>
+  <si>
+    <t>Range 16</t>
   </si>
 </sst>
 </file>
@@ -2892,6 +2895,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2904,9 +2914,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2976,6 +2983,57 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2994,57 +3052,6 @@
     <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3081,10 +3088,6 @@
     <xf numFmtId="0" fontId="16" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3127,7 +3130,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3454,7 +3457,7 @@
   <dimension ref="A1:AP53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AJ34" sqref="AJ34"/>
+      <selection activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -3570,13 +3573,13 @@
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
       <c r="T2" s="12"/>
-      <c r="V2" s="141" t="s">
+      <c r="V2" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="141"/>
-      <c r="X2" s="141"/>
-      <c r="Y2" s="141"/>
-      <c r="Z2" s="141"/>
+      <c r="W2" s="144"/>
+      <c r="X2" s="144"/>
+      <c r="Y2" s="144"/>
+      <c r="Z2" s="144"/>
       <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
       <c r="AC2" s="12"/>
@@ -3631,9 +3634,9 @@
         <v>437</v>
       </c>
       <c r="Q3" s="12"/>
-      <c r="R3" s="145"/>
-      <c r="S3" s="145"/>
-      <c r="T3" s="145"/>
+      <c r="R3" s="143"/>
+      <c r="S3" s="143"/>
+      <c r="T3" s="143"/>
       <c r="V3" s="122" t="s">
         <v>339</v>
       </c>
@@ -3717,22 +3720,22 @@
       <c r="AA4" s="36"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="36"/>
-      <c r="AD4" s="141" t="s">
+      <c r="AD4" s="144" t="s">
         <v>440</v>
       </c>
-      <c r="AE4" s="141"/>
-      <c r="AF4" s="141"/>
-      <c r="AG4" s="141"/>
-      <c r="AH4" s="141"/>
-      <c r="AJ4" s="141" t="s">
+      <c r="AE4" s="144"/>
+      <c r="AF4" s="144"/>
+      <c r="AG4" s="144"/>
+      <c r="AH4" s="144"/>
+      <c r="AJ4" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="AK4" s="141"/>
-      <c r="AL4" s="141"/>
-      <c r="AM4" s="141"/>
-      <c r="AN4" s="141"/>
-      <c r="AO4" s="141"/>
-      <c r="AP4" s="141"/>
+      <c r="AK4" s="144"/>
+      <c r="AL4" s="144"/>
+      <c r="AM4" s="144"/>
+      <c r="AN4" s="144"/>
+      <c r="AO4" s="144"/>
+      <c r="AP4" s="144"/>
     </row>
     <row r="5" spans="1:42" ht="15.75">
       <c r="A5" s="129" t="s">
@@ -4338,7 +4341,7 @@
       <c r="AB11" s="36"/>
       <c r="AC11" s="36"/>
       <c r="AD11" s="3" t="s">
-        <v>445</v>
+        <v>579</v>
       </c>
       <c r="AE11" s="127" t="s">
         <v>135</v>
@@ -4444,7 +4447,7 @@
       <c r="AH12" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="AJ12" s="204" t="s">
+      <c r="AJ12" s="141" t="s">
         <v>571</v>
       </c>
       <c r="AK12" s="11" t="s">
@@ -4540,7 +4543,7 @@
       <c r="AH13" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="AJ13" s="204" t="s">
+      <c r="AJ13" s="141" t="s">
         <v>571</v>
       </c>
       <c r="AK13" s="11" t="s">
@@ -4825,15 +4828,15 @@
       <c r="AH17" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="AJ17" s="141" t="s">
+      <c r="AJ17" s="144" t="s">
         <v>277</v>
       </c>
-      <c r="AK17" s="141"/>
-      <c r="AL17" s="141"/>
-      <c r="AM17" s="141"/>
-      <c r="AN17" s="141"/>
-      <c r="AO17" s="141"/>
-      <c r="AP17" s="141"/>
+      <c r="AK17" s="144"/>
+      <c r="AL17" s="144"/>
+      <c r="AM17" s="144"/>
+      <c r="AN17" s="144"/>
+      <c r="AO17" s="144"/>
+      <c r="AP17" s="144"/>
     </row>
     <row r="18" spans="1:42" ht="15.75">
       <c r="A18" s="129" t="s">
@@ -5050,9 +5053,9 @@
       <c r="O20" s="35"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="145"/>
-      <c r="S20" s="145"/>
-      <c r="T20" s="145"/>
+      <c r="R20" s="143"/>
+      <c r="S20" s="143"/>
+      <c r="T20" s="143"/>
       <c r="U20" s="2"/>
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
@@ -5322,7 +5325,7 @@
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
       <c r="T23" s="12"/>
-      <c r="AJ23" s="205" t="s">
+      <c r="AJ23" s="142" t="s">
         <v>573</v>
       </c>
       <c r="AK23" s="3" t="s">
@@ -5392,14 +5395,14 @@
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
-      <c r="AD24" s="141" t="s">
+      <c r="AD24" s="144" t="s">
         <v>497</v>
       </c>
-      <c r="AE24" s="141"/>
-      <c r="AF24" s="141"/>
-      <c r="AG24" s="141"/>
-      <c r="AH24" s="141"/>
-      <c r="AJ24" s="205" t="s">
+      <c r="AE24" s="144"/>
+      <c r="AF24" s="144"/>
+      <c r="AG24" s="144"/>
+      <c r="AH24" s="144"/>
+      <c r="AJ24" s="142" t="s">
         <v>576</v>
       </c>
       <c r="AK24" s="3" t="s">
@@ -5708,15 +5711,15 @@
       <c r="S29" s="35"/>
       <c r="T29" s="35"/>
       <c r="U29" s="35"/>
-      <c r="V29" s="141" t="s">
+      <c r="V29" s="144" t="s">
         <v>212</v>
       </c>
-      <c r="W29" s="141"/>
-      <c r="X29" s="141"/>
-      <c r="Y29" s="141"/>
-      <c r="Z29" s="141"/>
-      <c r="AA29" s="141"/>
-      <c r="AB29" s="141"/>
+      <c r="W29" s="144"/>
+      <c r="X29" s="144"/>
+      <c r="Y29" s="144"/>
+      <c r="Z29" s="144"/>
+      <c r="AA29" s="144"/>
+      <c r="AB29" s="144"/>
     </row>
     <row r="30" spans="1:42">
       <c r="A30" s="129"/>
@@ -5806,11 +5809,11 @@
       <c r="Y31" s="37"/>
       <c r="Z31" s="37"/>
       <c r="AA31" s="12"/>
-      <c r="AD31" s="142" t="s">
+      <c r="AD31" s="145" t="s">
         <v>263</v>
       </c>
-      <c r="AE31" s="143"/>
-      <c r="AF31" s="144"/>
+      <c r="AE31" s="146"/>
+      <c r="AF31" s="147"/>
     </row>
     <row r="32" spans="1:42">
       <c r="S32" s="12"/>
@@ -5915,15 +5918,15 @@
       <c r="S37" s="12"/>
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
-      <c r="V37" s="141" t="s">
+      <c r="V37" s="144" t="s">
         <v>9</v>
       </c>
-      <c r="W37" s="141"/>
-      <c r="X37" s="141"/>
-      <c r="Y37" s="141"/>
-      <c r="Z37" s="141"/>
-      <c r="AA37" s="141"/>
-      <c r="AB37" s="141"/>
+      <c r="W37" s="144"/>
+      <c r="X37" s="144"/>
+      <c r="Y37" s="144"/>
+      <c r="Z37" s="144"/>
+      <c r="AA37" s="144"/>
+      <c r="AB37" s="144"/>
       <c r="AD37" s="3" t="s">
         <v>259</v>
       </c>
@@ -6022,15 +6025,15 @@
       <c r="S42" s="12"/>
       <c r="T42" s="12"/>
       <c r="U42" s="12"/>
-      <c r="V42" s="141" t="s">
+      <c r="V42" s="144" t="s">
         <v>247</v>
       </c>
-      <c r="W42" s="141"/>
-      <c r="X42" s="141"/>
-      <c r="Y42" s="141"/>
-      <c r="Z42" s="141"/>
-      <c r="AA42" s="141"/>
-      <c r="AB42" s="141"/>
+      <c r="W42" s="144"/>
+      <c r="X42" s="144"/>
+      <c r="Y42" s="144"/>
+      <c r="Z42" s="144"/>
+      <c r="AA42" s="144"/>
+      <c r="AB42" s="144"/>
       <c r="AD42" s="3" t="s">
         <v>265</v>
       </c>
@@ -6135,15 +6138,15 @@
       <c r="S48" s="12"/>
       <c r="T48" s="12"/>
       <c r="U48" s="12"/>
-      <c r="V48" s="142" t="s">
+      <c r="V48" s="145" t="s">
         <v>484</v>
       </c>
-      <c r="W48" s="143"/>
-      <c r="X48" s="143"/>
-      <c r="Y48" s="143"/>
-      <c r="Z48" s="143"/>
-      <c r="AA48" s="143"/>
-      <c r="AB48" s="144"/>
+      <c r="W48" s="146"/>
+      <c r="X48" s="146"/>
+      <c r="Y48" s="146"/>
+      <c r="Z48" s="146"/>
+      <c r="AA48" s="146"/>
+      <c r="AB48" s="147"/>
     </row>
     <row r="49" spans="19:28">
       <c r="S49" s="12"/>
@@ -6233,6 +6236,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="V42:AB42"/>
+    <mergeCell ref="AD4:AH4"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="V48:AB48"/>
+    <mergeCell ref="V37:AB37"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="AJ4:AP4"/>
@@ -6240,11 +6248,6 @@
     <mergeCell ref="AD31:AF31"/>
     <mergeCell ref="V29:AB29"/>
     <mergeCell ref="AD24:AH24"/>
-    <mergeCell ref="V42:AB42"/>
-    <mergeCell ref="AD4:AH4"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="V48:AB48"/>
-    <mergeCell ref="V37:AB37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6271,48 +6274,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:36">
-      <c r="B2" s="141" t="s">
+      <c r="B2" s="144" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
-      <c r="E2" s="141"/>
-      <c r="F2" s="141"/>
-      <c r="H2" s="141" t="s">
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="H2" s="144" t="s">
         <v>231</v>
       </c>
-      <c r="I2" s="141"/>
-      <c r="J2" s="141"/>
-      <c r="K2" s="141"/>
-      <c r="L2" s="141"/>
-      <c r="N2" s="141" t="s">
+      <c r="I2" s="144"/>
+      <c r="J2" s="144"/>
+      <c r="K2" s="144"/>
+      <c r="L2" s="144"/>
+      <c r="N2" s="144" t="s">
         <v>239</v>
       </c>
-      <c r="O2" s="141"/>
-      <c r="P2" s="141"/>
-      <c r="Q2" s="141"/>
-      <c r="R2" s="141"/>
-      <c r="T2" s="141" t="s">
+      <c r="O2" s="144"/>
+      <c r="P2" s="144"/>
+      <c r="Q2" s="144"/>
+      <c r="R2" s="144"/>
+      <c r="T2" s="144" t="s">
         <v>249</v>
       </c>
-      <c r="U2" s="141"/>
-      <c r="V2" s="141"/>
-      <c r="W2" s="141"/>
-      <c r="X2" s="141"/>
-      <c r="Z2" s="141" t="s">
+      <c r="U2" s="144"/>
+      <c r="V2" s="144"/>
+      <c r="W2" s="144"/>
+      <c r="X2" s="144"/>
+      <c r="Z2" s="144" t="s">
         <v>321</v>
       </c>
-      <c r="AA2" s="141"/>
-      <c r="AB2" s="141"/>
-      <c r="AC2" s="141"/>
-      <c r="AD2" s="141"/>
-      <c r="AF2" s="141" t="s">
+      <c r="AA2" s="144"/>
+      <c r="AB2" s="144"/>
+      <c r="AC2" s="144"/>
+      <c r="AD2" s="144"/>
+      <c r="AF2" s="144" t="s">
         <v>502</v>
       </c>
-      <c r="AG2" s="141"/>
-      <c r="AH2" s="141"/>
-      <c r="AI2" s="141"/>
-      <c r="AJ2" s="141"/>
+      <c r="AG2" s="144"/>
+      <c r="AH2" s="144"/>
+      <c r="AI2" s="144"/>
+      <c r="AJ2" s="144"/>
     </row>
     <row r="3" spans="2:36">
       <c r="B3" s="124" t="s">
@@ -6723,40 +6726,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="148" t="s">
         <v>334</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="148"/>
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="150"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="149"/>
-      <c r="B2" s="150"/>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
-      <c r="H2" s="151"/>
+      <c r="A2" s="151"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="153"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="152" t="s">
+      <c r="A3" s="154" t="s">
         <v>253</v>
       </c>
-      <c r="B3" s="153"/>
-      <c r="C3" s="153"/>
-      <c r="D3" s="153"/>
-      <c r="E3" s="153" t="s">
+      <c r="B3" s="155"/>
+      <c r="C3" s="155"/>
+      <c r="D3" s="155"/>
+      <c r="E3" s="155" t="s">
         <v>254</v>
       </c>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="154"/>
+      <c r="F3" s="155"/>
+      <c r="G3" s="155"/>
+      <c r="H3" s="156"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="20">
@@ -7361,28 +7364,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="160" t="s">
         <v>335</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
-      <c r="H1" s="158"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="157" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="156"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="157"/>
+      <c r="B2" s="158"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="159"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="5"/>
@@ -7561,16 +7564,16 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="155" t="s">
+      <c r="A15" s="157" t="s">
         <v>225</v>
       </c>
-      <c r="B15" s="156"/>
-      <c r="C15" s="156"/>
-      <c r="D15" s="156"/>
-      <c r="E15" s="156"/>
-      <c r="F15" s="156"/>
-      <c r="G15" s="156"/>
-      <c r="H15" s="157"/>
+      <c r="B15" s="158"/>
+      <c r="C15" s="158"/>
+      <c r="D15" s="158"/>
+      <c r="E15" s="158"/>
+      <c r="F15" s="158"/>
+      <c r="G15" s="158"/>
+      <c r="H15" s="159"/>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="9"/>
@@ -7746,16 +7749,16 @@
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:11" ht="15.75">
-      <c r="A28" s="155" t="s">
+      <c r="A28" s="157" t="s">
         <v>226</v>
       </c>
-      <c r="B28" s="156"/>
-      <c r="C28" s="156"/>
-      <c r="D28" s="156"/>
-      <c r="E28" s="156"/>
-      <c r="F28" s="156"/>
-      <c r="G28" s="156"/>
-      <c r="H28" s="157"/>
+      <c r="B28" s="158"/>
+      <c r="C28" s="158"/>
+      <c r="D28" s="158"/>
+      <c r="E28" s="158"/>
+      <c r="F28" s="158"/>
+      <c r="G28" s="158"/>
+      <c r="H28" s="159"/>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="5"/>
@@ -7955,40 +7958,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="161" t="s">
         <v>336</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
-      <c r="H1" s="161"/>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
+      <c r="H1" s="163"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="162"/>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="164"/>
+      <c r="A2" s="164"/>
+      <c r="B2" s="165"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="166"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="167" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="167"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="165" t="s">
+      <c r="B3" s="168"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="167" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="166"/>
-      <c r="G3" s="167"/>
-      <c r="H3" s="168"/>
+      <c r="F3" s="168"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="170"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="16">
@@ -8427,40 +8430,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="188" t="s">
         <v>337</v>
       </c>
-      <c r="B1" s="169"/>
-      <c r="C1" s="169"/>
-      <c r="D1" s="169"/>
-      <c r="E1" s="169"/>
-      <c r="F1" s="169"/>
-      <c r="G1" s="169"/>
-      <c r="H1" s="169"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="170"/>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
+      <c r="A2" s="189"/>
+      <c r="B2" s="189"/>
+      <c r="C2" s="189"/>
+      <c r="D2" s="189"/>
+      <c r="E2" s="189"/>
+      <c r="F2" s="189"/>
+      <c r="G2" s="189"/>
+      <c r="H2" s="189"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="171" t="s">
+      <c r="A3" s="190" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="172"/>
-      <c r="C3" s="173"/>
-      <c r="D3" s="174"/>
-      <c r="E3" s="171" t="s">
+      <c r="B3" s="191"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="193"/>
+      <c r="E3" s="190" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="172"/>
-      <c r="G3" s="173"/>
-      <c r="H3" s="174"/>
+      <c r="F3" s="191"/>
+      <c r="G3" s="192"/>
+      <c r="H3" s="193"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="46">
@@ -8753,114 +8756,114 @@
       <c r="H24" s="74"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="171" t="s">
+      <c r="A25" s="190" t="s">
         <v>293</v>
       </c>
-      <c r="B25" s="172"/>
-      <c r="C25" s="173"/>
-      <c r="D25" s="174"/>
-      <c r="E25" s="171" t="s">
+      <c r="B25" s="191"/>
+      <c r="C25" s="192"/>
+      <c r="D25" s="193"/>
+      <c r="E25" s="190" t="s">
         <v>294</v>
       </c>
-      <c r="F25" s="172"/>
-      <c r="G25" s="173"/>
-      <c r="H25" s="174"/>
+      <c r="F25" s="191"/>
+      <c r="G25" s="192"/>
+      <c r="H25" s="193"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="50" t="s">
         <v>295</v>
       </c>
-      <c r="B26" s="175"/>
-      <c r="C26" s="176"/>
-      <c r="D26" s="177"/>
+      <c r="B26" s="177"/>
+      <c r="C26" s="178"/>
+      <c r="D26" s="179"/>
       <c r="E26" s="46" t="s">
         <v>296</v>
       </c>
-      <c r="F26" s="178"/>
-      <c r="G26" s="179"/>
-      <c r="H26" s="180"/>
+      <c r="F26" s="185"/>
+      <c r="G26" s="186"/>
+      <c r="H26" s="187"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="B27" s="181"/>
-      <c r="C27" s="182"/>
+      <c r="B27" s="180"/>
+      <c r="C27" s="181"/>
       <c r="D27" s="183"/>
       <c r="E27" s="50" t="s">
         <v>298</v>
       </c>
-      <c r="F27" s="175"/>
-      <c r="G27" s="176"/>
+      <c r="F27" s="177"/>
+      <c r="G27" s="178"/>
       <c r="H27" s="184"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="50" t="s">
         <v>299</v>
       </c>
-      <c r="B28" s="175"/>
-      <c r="C28" s="176"/>
-      <c r="D28" s="177"/>
+      <c r="B28" s="177"/>
+      <c r="C28" s="178"/>
+      <c r="D28" s="179"/>
       <c r="E28" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="F28" s="181"/>
-      <c r="G28" s="182"/>
-      <c r="H28" s="185"/>
+      <c r="F28" s="180"/>
+      <c r="G28" s="181"/>
+      <c r="H28" s="182"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="58" t="s">
         <v>301</v>
       </c>
-      <c r="B29" s="181"/>
-      <c r="C29" s="182"/>
+      <c r="B29" s="180"/>
+      <c r="C29" s="181"/>
       <c r="D29" s="183"/>
       <c r="E29" s="50" t="s">
         <v>302</v>
       </c>
-      <c r="F29" s="175"/>
-      <c r="G29" s="176"/>
+      <c r="F29" s="177"/>
+      <c r="G29" s="178"/>
       <c r="H29" s="184"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="50" t="s">
         <v>303</v>
       </c>
-      <c r="B30" s="175"/>
-      <c r="C30" s="176"/>
-      <c r="D30" s="177"/>
+      <c r="B30" s="177"/>
+      <c r="C30" s="178"/>
+      <c r="D30" s="179"/>
       <c r="E30" s="58" t="s">
         <v>304</v>
       </c>
-      <c r="F30" s="181"/>
-      <c r="G30" s="182"/>
-      <c r="H30" s="185"/>
+      <c r="F30" s="180"/>
+      <c r="G30" s="181"/>
+      <c r="H30" s="182"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="B31" s="181"/>
-      <c r="C31" s="182"/>
+      <c r="B31" s="180"/>
+      <c r="C31" s="181"/>
       <c r="D31" s="183"/>
       <c r="E31" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="F31" s="175"/>
-      <c r="G31" s="176"/>
+      <c r="F31" s="177"/>
+      <c r="G31" s="178"/>
       <c r="H31" s="184"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="50" t="s">
         <v>307</v>
       </c>
-      <c r="B32" s="175"/>
-      <c r="C32" s="176"/>
-      <c r="D32" s="177"/>
+      <c r="B32" s="177"/>
+      <c r="C32" s="178"/>
+      <c r="D32" s="179"/>
       <c r="E32" s="58"/>
-      <c r="F32" s="181"/>
-      <c r="G32" s="182"/>
-      <c r="H32" s="185" t="s">
+      <c r="F32" s="180"/>
+      <c r="G32" s="181"/>
+      <c r="H32" s="182" t="s">
         <v>245</v>
       </c>
     </row>
@@ -8868,12 +8871,12 @@
       <c r="A33" s="58" t="s">
         <v>308</v>
       </c>
-      <c r="B33" s="181"/>
-      <c r="C33" s="182"/>
+      <c r="B33" s="180"/>
+      <c r="C33" s="181"/>
       <c r="D33" s="183"/>
       <c r="E33" s="50"/>
-      <c r="F33" s="175"/>
-      <c r="G33" s="176"/>
+      <c r="F33" s="177"/>
+      <c r="G33" s="178"/>
       <c r="H33" s="184" t="s">
         <v>288</v>
       </c>
@@ -8882,13 +8885,13 @@
       <c r="A34" s="50" t="s">
         <v>309</v>
       </c>
-      <c r="B34" s="175"/>
-      <c r="C34" s="176"/>
-      <c r="D34" s="177"/>
+      <c r="B34" s="177"/>
+      <c r="C34" s="178"/>
+      <c r="D34" s="179"/>
       <c r="E34" s="58"/>
-      <c r="F34" s="181"/>
-      <c r="G34" s="182"/>
-      <c r="H34" s="185" t="s">
+      <c r="F34" s="180"/>
+      <c r="G34" s="181"/>
+      <c r="H34" s="182" t="s">
         <v>289</v>
       </c>
     </row>
@@ -8896,12 +8899,12 @@
       <c r="A35" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="B35" s="181"/>
-      <c r="C35" s="182"/>
+      <c r="B35" s="180"/>
+      <c r="C35" s="181"/>
       <c r="D35" s="183"/>
       <c r="E35" s="50"/>
-      <c r="F35" s="175"/>
-      <c r="G35" s="176"/>
+      <c r="F35" s="177"/>
+      <c r="G35" s="178"/>
       <c r="H35" s="184" t="s">
         <v>290</v>
       </c>
@@ -8910,13 +8913,13 @@
       <c r="A36" s="50" t="s">
         <v>311</v>
       </c>
-      <c r="B36" s="175"/>
-      <c r="C36" s="176"/>
-      <c r="D36" s="177"/>
+      <c r="B36" s="177"/>
+      <c r="C36" s="178"/>
+      <c r="D36" s="179"/>
       <c r="E36" s="58"/>
-      <c r="F36" s="181"/>
-      <c r="G36" s="182"/>
-      <c r="H36" s="185" t="s">
+      <c r="F36" s="180"/>
+      <c r="G36" s="181"/>
+      <c r="H36" s="182" t="s">
         <v>291</v>
       </c>
     </row>
@@ -8924,12 +8927,12 @@
       <c r="A37" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="B37" s="181"/>
-      <c r="C37" s="182"/>
+      <c r="B37" s="180"/>
+      <c r="C37" s="181"/>
       <c r="D37" s="183"/>
       <c r="E37" s="50"/>
-      <c r="F37" s="175"/>
-      <c r="G37" s="176"/>
+      <c r="F37" s="177"/>
+      <c r="G37" s="178"/>
       <c r="H37" s="184" t="s">
         <v>292</v>
       </c>
@@ -8938,13 +8941,13 @@
       <c r="A38" s="50" t="s">
         <v>313</v>
       </c>
-      <c r="B38" s="175"/>
-      <c r="C38" s="176"/>
-      <c r="D38" s="177"/>
+      <c r="B38" s="177"/>
+      <c r="C38" s="178"/>
+      <c r="D38" s="179"/>
       <c r="E38" s="58"/>
-      <c r="F38" s="181"/>
-      <c r="G38" s="182"/>
-      <c r="H38" s="185" t="s">
+      <c r="F38" s="180"/>
+      <c r="G38" s="181"/>
+      <c r="H38" s="182" t="s">
         <v>244</v>
       </c>
     </row>
@@ -8952,12 +8955,12 @@
       <c r="A39" s="58" t="s">
         <v>314</v>
       </c>
-      <c r="B39" s="181"/>
-      <c r="C39" s="182"/>
+      <c r="B39" s="180"/>
+      <c r="C39" s="181"/>
       <c r="D39" s="183"/>
       <c r="E39" s="50"/>
-      <c r="F39" s="175"/>
-      <c r="G39" s="176"/>
+      <c r="F39" s="177"/>
+      <c r="G39" s="178"/>
       <c r="H39" s="184" t="s">
         <v>245</v>
       </c>
@@ -8966,28 +8969,57 @@
       <c r="A40" s="50" t="s">
         <v>315</v>
       </c>
-      <c r="B40" s="175"/>
-      <c r="C40" s="176"/>
-      <c r="D40" s="177"/>
+      <c r="B40" s="177"/>
+      <c r="C40" s="178"/>
+      <c r="D40" s="179"/>
       <c r="E40" s="58"/>
-      <c r="F40" s="181"/>
-      <c r="G40" s="182"/>
-      <c r="H40" s="185"/>
+      <c r="F40" s="180"/>
+      <c r="G40" s="181"/>
+      <c r="H40" s="182"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="70" t="s">
         <v>316</v>
       </c>
-      <c r="B41" s="186"/>
-      <c r="C41" s="187"/>
-      <c r="D41" s="188"/>
+      <c r="B41" s="171"/>
+      <c r="C41" s="172"/>
+      <c r="D41" s="173"/>
       <c r="E41" s="75"/>
-      <c r="F41" s="189"/>
-      <c r="G41" s="190"/>
-      <c r="H41" s="191"/>
+      <c r="F41" s="174"/>
+      <c r="G41" s="175"/>
+      <c r="H41" s="176"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -8996,35 +9028,6 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9053,40 +9056,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="200" t="s">
         <v>338</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="200"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="202"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="201"/>
-      <c r="B2" s="202"/>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="203"/>
+      <c r="A2" s="203"/>
+      <c r="B2" s="204"/>
+      <c r="C2" s="204"/>
+      <c r="D2" s="204"/>
+      <c r="E2" s="204"/>
+      <c r="F2" s="204"/>
+      <c r="G2" s="204"/>
+      <c r="H2" s="205"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="192" t="s">
+      <c r="A3" s="194" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="193"/>
-      <c r="C3" s="193"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="192" t="s">
+      <c r="B3" s="195"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="196"/>
+      <c r="E3" s="194" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="193"/>
-      <c r="G3" s="193"/>
-      <c r="H3" s="194"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="196"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="93">
@@ -9303,18 +9306,18 @@
       <c r="H21" s="85"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="195" t="s">
+      <c r="A22" s="197" t="s">
         <v>319</v>
       </c>
-      <c r="B22" s="196"/>
-      <c r="C22" s="196"/>
-      <c r="D22" s="197"/>
-      <c r="E22" s="195" t="s">
+      <c r="B22" s="198"/>
+      <c r="C22" s="198"/>
+      <c r="D22" s="199"/>
+      <c r="E22" s="197" t="s">
         <v>320</v>
       </c>
-      <c r="F22" s="196"/>
-      <c r="G22" s="196"/>
-      <c r="H22" s="197"/>
+      <c r="F22" s="198"/>
+      <c r="G22" s="198"/>
+      <c r="H22" s="199"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="78">
@@ -9591,40 +9594,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="200" t="s">
         <v>498</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="200"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="202"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="201"/>
-      <c r="B2" s="202"/>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="203"/>
+      <c r="A2" s="203"/>
+      <c r="B2" s="204"/>
+      <c r="C2" s="204"/>
+      <c r="D2" s="204"/>
+      <c r="E2" s="204"/>
+      <c r="F2" s="204"/>
+      <c r="G2" s="204"/>
+      <c r="H2" s="205"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="192" t="s">
+      <c r="A3" s="194" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="193"/>
-      <c r="C3" s="193"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="192" t="s">
+      <c r="B3" s="195"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="196"/>
+      <c r="E3" s="194" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="193"/>
-      <c r="G3" s="193"/>
-      <c r="H3" s="194"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="196"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="93">
@@ -9841,18 +9844,18 @@
       <c r="H21" s="85"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="195" t="s">
+      <c r="A22" s="197" t="s">
         <v>319</v>
       </c>
-      <c r="B22" s="196"/>
-      <c r="C22" s="196"/>
-      <c r="D22" s="197"/>
-      <c r="E22" s="195" t="s">
+      <c r="B22" s="198"/>
+      <c r="C22" s="198"/>
+      <c r="D22" s="199"/>
+      <c r="E22" s="197" t="s">
         <v>320</v>
       </c>
-      <c r="F22" s="196"/>
-      <c r="G22" s="196"/>
-      <c r="H22" s="197"/>
+      <c r="F22" s="198"/>
+      <c r="G22" s="198"/>
+      <c r="H22" s="199"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="78">
@@ -10129,40 +10132,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="148" t="s">
         <v>499</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="148"/>
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="150"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="149"/>
-      <c r="B2" s="150"/>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
-      <c r="H2" s="151"/>
+      <c r="A2" s="151"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="153"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="152" t="s">
+      <c r="A3" s="154" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="153"/>
-      <c r="C3" s="153"/>
-      <c r="D3" s="153"/>
-      <c r="E3" s="153" t="s">
+      <c r="B3" s="155"/>
+      <c r="C3" s="155"/>
+      <c r="D3" s="155"/>
+      <c r="E3" s="155" t="s">
         <v>322</v>
       </c>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="154"/>
+      <c r="F3" s="155"/>
+      <c r="G3" s="155"/>
+      <c r="H3" s="156"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="20">

</xml_diff>

<commit_message>
chg: Added tanker information
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="581">
   <si>
     <t>AWACS</t>
   </si>
@@ -1762,6 +1762,9 @@
   </si>
   <si>
     <t>Range 16</t>
+  </si>
+  <si>
+    <t>AR402 #IFF:5402FR</t>
   </si>
 </sst>
 </file>
@@ -2899,21 +2902,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2983,6 +2986,57 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3000,57 +3054,6 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3130,7 +3133,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3456,8 +3459,8 @@
   <sheetPr codeName="Ark1"/>
   <dimension ref="A1:AP53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD16" sqref="AD16"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AJ13" sqref="AJ13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -3573,13 +3576,13 @@
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
       <c r="T2" s="12"/>
-      <c r="V2" s="144" t="s">
+      <c r="V2" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="144"/>
-      <c r="X2" s="144"/>
-      <c r="Y2" s="144"/>
-      <c r="Z2" s="144"/>
+      <c r="W2" s="143"/>
+      <c r="X2" s="143"/>
+      <c r="Y2" s="143"/>
+      <c r="Z2" s="143"/>
       <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
       <c r="AC2" s="12"/>
@@ -3634,9 +3637,9 @@
         <v>437</v>
       </c>
       <c r="Q3" s="12"/>
-      <c r="R3" s="143"/>
-      <c r="S3" s="143"/>
-      <c r="T3" s="143"/>
+      <c r="R3" s="147"/>
+      <c r="S3" s="147"/>
+      <c r="T3" s="147"/>
       <c r="V3" s="122" t="s">
         <v>339</v>
       </c>
@@ -3720,22 +3723,22 @@
       <c r="AA4" s="36"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="36"/>
-      <c r="AD4" s="144" t="s">
+      <c r="AD4" s="143" t="s">
         <v>440</v>
       </c>
-      <c r="AE4" s="144"/>
-      <c r="AF4" s="144"/>
-      <c r="AG4" s="144"/>
-      <c r="AH4" s="144"/>
-      <c r="AJ4" s="144" t="s">
+      <c r="AE4" s="143"/>
+      <c r="AF4" s="143"/>
+      <c r="AG4" s="143"/>
+      <c r="AH4" s="143"/>
+      <c r="AJ4" s="143" t="s">
         <v>1</v>
       </c>
-      <c r="AK4" s="144"/>
-      <c r="AL4" s="144"/>
-      <c r="AM4" s="144"/>
-      <c r="AN4" s="144"/>
-      <c r="AO4" s="144"/>
-      <c r="AP4" s="144"/>
+      <c r="AK4" s="143"/>
+      <c r="AL4" s="143"/>
+      <c r="AM4" s="143"/>
+      <c r="AN4" s="143"/>
+      <c r="AO4" s="143"/>
+      <c r="AP4" s="143"/>
     </row>
     <row r="5" spans="1:42" ht="15.75">
       <c r="A5" s="129" t="s">
@@ -4544,7 +4547,7 @@
         <v>481</v>
       </c>
       <c r="AJ13" s="141" t="s">
-        <v>571</v>
+        <v>580</v>
       </c>
       <c r="AK13" s="11" t="s">
         <v>558</v>
@@ -4828,15 +4831,15 @@
       <c r="AH17" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="AJ17" s="144" t="s">
+      <c r="AJ17" s="143" t="s">
         <v>277</v>
       </c>
-      <c r="AK17" s="144"/>
-      <c r="AL17" s="144"/>
-      <c r="AM17" s="144"/>
-      <c r="AN17" s="144"/>
-      <c r="AO17" s="144"/>
-      <c r="AP17" s="144"/>
+      <c r="AK17" s="143"/>
+      <c r="AL17" s="143"/>
+      <c r="AM17" s="143"/>
+      <c r="AN17" s="143"/>
+      <c r="AO17" s="143"/>
+      <c r="AP17" s="143"/>
     </row>
     <row r="18" spans="1:42" ht="15.75">
       <c r="A18" s="129" t="s">
@@ -5053,9 +5056,9 @@
       <c r="O20" s="35"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="143"/>
-      <c r="S20" s="143"/>
-      <c r="T20" s="143"/>
+      <c r="R20" s="147"/>
+      <c r="S20" s="147"/>
+      <c r="T20" s="147"/>
       <c r="U20" s="2"/>
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
@@ -5395,13 +5398,13 @@
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
-      <c r="AD24" s="144" t="s">
+      <c r="AD24" s="143" t="s">
         <v>497</v>
       </c>
-      <c r="AE24" s="144"/>
-      <c r="AF24" s="144"/>
-      <c r="AG24" s="144"/>
-      <c r="AH24" s="144"/>
+      <c r="AE24" s="143"/>
+      <c r="AF24" s="143"/>
+      <c r="AG24" s="143"/>
+      <c r="AH24" s="143"/>
       <c r="AJ24" s="142" t="s">
         <v>576</v>
       </c>
@@ -5711,15 +5714,15 @@
       <c r="S29" s="35"/>
       <c r="T29" s="35"/>
       <c r="U29" s="35"/>
-      <c r="V29" s="144" t="s">
+      <c r="V29" s="143" t="s">
         <v>212</v>
       </c>
-      <c r="W29" s="144"/>
-      <c r="X29" s="144"/>
-      <c r="Y29" s="144"/>
-      <c r="Z29" s="144"/>
-      <c r="AA29" s="144"/>
-      <c r="AB29" s="144"/>
+      <c r="W29" s="143"/>
+      <c r="X29" s="143"/>
+      <c r="Y29" s="143"/>
+      <c r="Z29" s="143"/>
+      <c r="AA29" s="143"/>
+      <c r="AB29" s="143"/>
     </row>
     <row r="30" spans="1:42">
       <c r="A30" s="129"/>
@@ -5809,11 +5812,11 @@
       <c r="Y31" s="37"/>
       <c r="Z31" s="37"/>
       <c r="AA31" s="12"/>
-      <c r="AD31" s="145" t="s">
+      <c r="AD31" s="144" t="s">
         <v>263</v>
       </c>
-      <c r="AE31" s="146"/>
-      <c r="AF31" s="147"/>
+      <c r="AE31" s="145"/>
+      <c r="AF31" s="146"/>
     </row>
     <row r="32" spans="1:42">
       <c r="S32" s="12"/>
@@ -5918,15 +5921,15 @@
       <c r="S37" s="12"/>
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
-      <c r="V37" s="144" t="s">
+      <c r="V37" s="143" t="s">
         <v>9</v>
       </c>
-      <c r="W37" s="144"/>
-      <c r="X37" s="144"/>
-      <c r="Y37" s="144"/>
-      <c r="Z37" s="144"/>
-      <c r="AA37" s="144"/>
-      <c r="AB37" s="144"/>
+      <c r="W37" s="143"/>
+      <c r="X37" s="143"/>
+      <c r="Y37" s="143"/>
+      <c r="Z37" s="143"/>
+      <c r="AA37" s="143"/>
+      <c r="AB37" s="143"/>
       <c r="AD37" s="3" t="s">
         <v>259</v>
       </c>
@@ -6025,15 +6028,15 @@
       <c r="S42" s="12"/>
       <c r="T42" s="12"/>
       <c r="U42" s="12"/>
-      <c r="V42" s="144" t="s">
+      <c r="V42" s="143" t="s">
         <v>247</v>
       </c>
-      <c r="W42" s="144"/>
-      <c r="X42" s="144"/>
-      <c r="Y42" s="144"/>
-      <c r="Z42" s="144"/>
-      <c r="AA42" s="144"/>
-      <c r="AB42" s="144"/>
+      <c r="W42" s="143"/>
+      <c r="X42" s="143"/>
+      <c r="Y42" s="143"/>
+      <c r="Z42" s="143"/>
+      <c r="AA42" s="143"/>
+      <c r="AB42" s="143"/>
       <c r="AD42" s="3" t="s">
         <v>265</v>
       </c>
@@ -6138,15 +6141,15 @@
       <c r="S48" s="12"/>
       <c r="T48" s="12"/>
       <c r="U48" s="12"/>
-      <c r="V48" s="145" t="s">
+      <c r="V48" s="144" t="s">
         <v>484</v>
       </c>
-      <c r="W48" s="146"/>
-      <c r="X48" s="146"/>
-      <c r="Y48" s="146"/>
-      <c r="Z48" s="146"/>
-      <c r="AA48" s="146"/>
-      <c r="AB48" s="147"/>
+      <c r="W48" s="145"/>
+      <c r="X48" s="145"/>
+      <c r="Y48" s="145"/>
+      <c r="Z48" s="145"/>
+      <c r="AA48" s="145"/>
+      <c r="AB48" s="146"/>
     </row>
     <row r="49" spans="19:28">
       <c r="S49" s="12"/>
@@ -6236,11 +6239,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="V42:AB42"/>
-    <mergeCell ref="AD4:AH4"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="V48:AB48"/>
-    <mergeCell ref="V37:AB37"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="AJ4:AP4"/>
@@ -6248,6 +6246,11 @@
     <mergeCell ref="AD31:AF31"/>
     <mergeCell ref="V29:AB29"/>
     <mergeCell ref="AD24:AH24"/>
+    <mergeCell ref="V42:AB42"/>
+    <mergeCell ref="AD4:AH4"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="V48:AB48"/>
+    <mergeCell ref="V37:AB37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6274,48 +6277,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:36">
-      <c r="B2" s="144" t="s">
+      <c r="B2" s="143" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="144"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="144"/>
-      <c r="H2" s="144" t="s">
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="H2" s="143" t="s">
         <v>231</v>
       </c>
-      <c r="I2" s="144"/>
-      <c r="J2" s="144"/>
-      <c r="K2" s="144"/>
-      <c r="L2" s="144"/>
-      <c r="N2" s="144" t="s">
+      <c r="I2" s="143"/>
+      <c r="J2" s="143"/>
+      <c r="K2" s="143"/>
+      <c r="L2" s="143"/>
+      <c r="N2" s="143" t="s">
         <v>239</v>
       </c>
-      <c r="O2" s="144"/>
-      <c r="P2" s="144"/>
-      <c r="Q2" s="144"/>
-      <c r="R2" s="144"/>
-      <c r="T2" s="144" t="s">
+      <c r="O2" s="143"/>
+      <c r="P2" s="143"/>
+      <c r="Q2" s="143"/>
+      <c r="R2" s="143"/>
+      <c r="T2" s="143" t="s">
         <v>249</v>
       </c>
-      <c r="U2" s="144"/>
-      <c r="V2" s="144"/>
-      <c r="W2" s="144"/>
-      <c r="X2" s="144"/>
-      <c r="Z2" s="144" t="s">
+      <c r="U2" s="143"/>
+      <c r="V2" s="143"/>
+      <c r="W2" s="143"/>
+      <c r="X2" s="143"/>
+      <c r="Z2" s="143" t="s">
         <v>321</v>
       </c>
-      <c r="AA2" s="144"/>
-      <c r="AB2" s="144"/>
-      <c r="AC2" s="144"/>
-      <c r="AD2" s="144"/>
-      <c r="AF2" s="144" t="s">
+      <c r="AA2" s="143"/>
+      <c r="AB2" s="143"/>
+      <c r="AC2" s="143"/>
+      <c r="AD2" s="143"/>
+      <c r="AF2" s="143" t="s">
         <v>502</v>
       </c>
-      <c r="AG2" s="144"/>
-      <c r="AH2" s="144"/>
-      <c r="AI2" s="144"/>
-      <c r="AJ2" s="144"/>
+      <c r="AG2" s="143"/>
+      <c r="AH2" s="143"/>
+      <c r="AI2" s="143"/>
+      <c r="AJ2" s="143"/>
     </row>
     <row r="3" spans="2:36">
       <c r="B3" s="124" t="s">
@@ -8430,40 +8433,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="171" t="s">
         <v>337</v>
       </c>
-      <c r="B1" s="188"/>
-      <c r="C1" s="188"/>
-      <c r="D1" s="188"/>
-      <c r="E1" s="188"/>
-      <c r="F1" s="188"/>
-      <c r="G1" s="188"/>
-      <c r="H1" s="188"/>
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
+      <c r="G1" s="171"/>
+      <c r="H1" s="171"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="189"/>
-      <c r="B2" s="189"/>
-      <c r="C2" s="189"/>
-      <c r="D2" s="189"/>
-      <c r="E2" s="189"/>
-      <c r="F2" s="189"/>
-      <c r="G2" s="189"/>
-      <c r="H2" s="189"/>
+      <c r="A2" s="172"/>
+      <c r="B2" s="172"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="172"/>
+      <c r="F2" s="172"/>
+      <c r="G2" s="172"/>
+      <c r="H2" s="172"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="190" t="s">
+      <c r="A3" s="173" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="191"/>
-      <c r="C3" s="192"/>
-      <c r="D3" s="193"/>
-      <c r="E3" s="190" t="s">
+      <c r="B3" s="174"/>
+      <c r="C3" s="175"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="173" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="191"/>
-      <c r="G3" s="192"/>
-      <c r="H3" s="193"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="175"/>
+      <c r="H3" s="176"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="46">
@@ -8756,18 +8759,18 @@
       <c r="H24" s="74"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="190" t="s">
+      <c r="A25" s="173" t="s">
         <v>293</v>
       </c>
-      <c r="B25" s="191"/>
-      <c r="C25" s="192"/>
-      <c r="D25" s="193"/>
-      <c r="E25" s="190" t="s">
+      <c r="B25" s="174"/>
+      <c r="C25" s="175"/>
+      <c r="D25" s="176"/>
+      <c r="E25" s="173" t="s">
         <v>294</v>
       </c>
-      <c r="F25" s="191"/>
-      <c r="G25" s="192"/>
-      <c r="H25" s="193"/>
+      <c r="F25" s="174"/>
+      <c r="G25" s="175"/>
+      <c r="H25" s="176"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="50" t="s">
@@ -8779,23 +8782,23 @@
       <c r="E26" s="46" t="s">
         <v>296</v>
       </c>
-      <c r="F26" s="185"/>
-      <c r="G26" s="186"/>
-      <c r="H26" s="187"/>
+      <c r="F26" s="180"/>
+      <c r="G26" s="181"/>
+      <c r="H26" s="182"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="B27" s="180"/>
-      <c r="C27" s="181"/>
-      <c r="D27" s="183"/>
+      <c r="B27" s="183"/>
+      <c r="C27" s="184"/>
+      <c r="D27" s="185"/>
       <c r="E27" s="50" t="s">
         <v>298</v>
       </c>
       <c r="F27" s="177"/>
       <c r="G27" s="178"/>
-      <c r="H27" s="184"/>
+      <c r="H27" s="186"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="50" t="s">
@@ -8807,23 +8810,23 @@
       <c r="E28" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="F28" s="180"/>
-      <c r="G28" s="181"/>
-      <c r="H28" s="182"/>
+      <c r="F28" s="183"/>
+      <c r="G28" s="184"/>
+      <c r="H28" s="187"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="58" t="s">
         <v>301</v>
       </c>
-      <c r="B29" s="180"/>
-      <c r="C29" s="181"/>
-      <c r="D29" s="183"/>
+      <c r="B29" s="183"/>
+      <c r="C29" s="184"/>
+      <c r="D29" s="185"/>
       <c r="E29" s="50" t="s">
         <v>302</v>
       </c>
       <c r="F29" s="177"/>
       <c r="G29" s="178"/>
-      <c r="H29" s="184"/>
+      <c r="H29" s="186"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="50" t="s">
@@ -8835,23 +8838,23 @@
       <c r="E30" s="58" t="s">
         <v>304</v>
       </c>
-      <c r="F30" s="180"/>
-      <c r="G30" s="181"/>
-      <c r="H30" s="182"/>
+      <c r="F30" s="183"/>
+      <c r="G30" s="184"/>
+      <c r="H30" s="187"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="B31" s="180"/>
-      <c r="C31" s="181"/>
-      <c r="D31" s="183"/>
+      <c r="B31" s="183"/>
+      <c r="C31" s="184"/>
+      <c r="D31" s="185"/>
       <c r="E31" s="50" t="s">
         <v>306</v>
       </c>
       <c r="F31" s="177"/>
       <c r="G31" s="178"/>
-      <c r="H31" s="184"/>
+      <c r="H31" s="186"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="50" t="s">
@@ -8861,9 +8864,9 @@
       <c r="C32" s="178"/>
       <c r="D32" s="179"/>
       <c r="E32" s="58"/>
-      <c r="F32" s="180"/>
-      <c r="G32" s="181"/>
-      <c r="H32" s="182" t="s">
+      <c r="F32" s="183"/>
+      <c r="G32" s="184"/>
+      <c r="H32" s="187" t="s">
         <v>245</v>
       </c>
     </row>
@@ -8871,13 +8874,13 @@
       <c r="A33" s="58" t="s">
         <v>308</v>
       </c>
-      <c r="B33" s="180"/>
-      <c r="C33" s="181"/>
-      <c r="D33" s="183"/>
+      <c r="B33" s="183"/>
+      <c r="C33" s="184"/>
+      <c r="D33" s="185"/>
       <c r="E33" s="50"/>
       <c r="F33" s="177"/>
       <c r="G33" s="178"/>
-      <c r="H33" s="184" t="s">
+      <c r="H33" s="186" t="s">
         <v>288</v>
       </c>
     </row>
@@ -8889,9 +8892,9 @@
       <c r="C34" s="178"/>
       <c r="D34" s="179"/>
       <c r="E34" s="58"/>
-      <c r="F34" s="180"/>
-      <c r="G34" s="181"/>
-      <c r="H34" s="182" t="s">
+      <c r="F34" s="183"/>
+      <c r="G34" s="184"/>
+      <c r="H34" s="187" t="s">
         <v>289</v>
       </c>
     </row>
@@ -8899,13 +8902,13 @@
       <c r="A35" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="B35" s="180"/>
-      <c r="C35" s="181"/>
-      <c r="D35" s="183"/>
+      <c r="B35" s="183"/>
+      <c r="C35" s="184"/>
+      <c r="D35" s="185"/>
       <c r="E35" s="50"/>
       <c r="F35" s="177"/>
       <c r="G35" s="178"/>
-      <c r="H35" s="184" t="s">
+      <c r="H35" s="186" t="s">
         <v>290</v>
       </c>
     </row>
@@ -8917,9 +8920,9 @@
       <c r="C36" s="178"/>
       <c r="D36" s="179"/>
       <c r="E36" s="58"/>
-      <c r="F36" s="180"/>
-      <c r="G36" s="181"/>
-      <c r="H36" s="182" t="s">
+      <c r="F36" s="183"/>
+      <c r="G36" s="184"/>
+      <c r="H36" s="187" t="s">
         <v>291</v>
       </c>
     </row>
@@ -8927,13 +8930,13 @@
       <c r="A37" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="B37" s="180"/>
-      <c r="C37" s="181"/>
-      <c r="D37" s="183"/>
+      <c r="B37" s="183"/>
+      <c r="C37" s="184"/>
+      <c r="D37" s="185"/>
       <c r="E37" s="50"/>
       <c r="F37" s="177"/>
       <c r="G37" s="178"/>
-      <c r="H37" s="184" t="s">
+      <c r="H37" s="186" t="s">
         <v>292</v>
       </c>
     </row>
@@ -8945,9 +8948,9 @@
       <c r="C38" s="178"/>
       <c r="D38" s="179"/>
       <c r="E38" s="58"/>
-      <c r="F38" s="180"/>
-      <c r="G38" s="181"/>
-      <c r="H38" s="182" t="s">
+      <c r="F38" s="183"/>
+      <c r="G38" s="184"/>
+      <c r="H38" s="187" t="s">
         <v>244</v>
       </c>
     </row>
@@ -8955,13 +8958,13 @@
       <c r="A39" s="58" t="s">
         <v>314</v>
       </c>
-      <c r="B39" s="180"/>
-      <c r="C39" s="181"/>
-      <c r="D39" s="183"/>
+      <c r="B39" s="183"/>
+      <c r="C39" s="184"/>
+      <c r="D39" s="185"/>
       <c r="E39" s="50"/>
       <c r="F39" s="177"/>
       <c r="G39" s="178"/>
-      <c r="H39" s="184" t="s">
+      <c r="H39" s="186" t="s">
         <v>245</v>
       </c>
     </row>
@@ -8973,53 +8976,24 @@
       <c r="C40" s="178"/>
       <c r="D40" s="179"/>
       <c r="E40" s="58"/>
-      <c r="F40" s="180"/>
-      <c r="G40" s="181"/>
-      <c r="H40" s="182"/>
+      <c r="F40" s="183"/>
+      <c r="G40" s="184"/>
+      <c r="H40" s="187"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="70" t="s">
         <v>316</v>
       </c>
-      <c r="B41" s="171"/>
-      <c r="C41" s="172"/>
-      <c r="D41" s="173"/>
+      <c r="B41" s="188"/>
+      <c r="C41" s="189"/>
+      <c r="D41" s="190"/>
       <c r="E41" s="75"/>
-      <c r="F41" s="174"/>
-      <c r="G41" s="175"/>
-      <c r="H41" s="176"/>
+      <c r="F41" s="191"/>
+      <c r="G41" s="192"/>
+      <c r="H41" s="193"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -9028,6 +9002,35 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chg: Updated flight callsigns
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="584">
   <si>
     <t>AWACS</t>
   </si>
@@ -1765,6 +1765,15 @@
   </si>
   <si>
     <t>AR402 #IFF:5402FR</t>
+  </si>
+  <si>
+    <t>JURY</t>
+  </si>
+  <si>
+    <t>BOAR</t>
+  </si>
+  <si>
+    <t>SNAKE</t>
   </si>
 </sst>
 </file>
@@ -2902,6 +2911,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2914,9 +2926,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2986,6 +2995,57 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3003,57 +3063,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3133,7 +3142,7 @@
         <xdr:cNvPr id="2050" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3459,7 +3468,7 @@
   <sheetPr codeName="Ark1"/>
   <dimension ref="A1:AP53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="Z1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AJ13" sqref="AJ13"/>
     </sheetView>
   </sheetViews>
@@ -3576,13 +3585,13 @@
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
       <c r="T2" s="12"/>
-      <c r="V2" s="143" t="s">
+      <c r="V2" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="143"/>
-      <c r="X2" s="143"/>
-      <c r="Y2" s="143"/>
-      <c r="Z2" s="143"/>
+      <c r="W2" s="144"/>
+      <c r="X2" s="144"/>
+      <c r="Y2" s="144"/>
+      <c r="Z2" s="144"/>
       <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
       <c r="AC2" s="12"/>
@@ -3637,9 +3646,9 @@
         <v>437</v>
       </c>
       <c r="Q3" s="12"/>
-      <c r="R3" s="147"/>
-      <c r="S3" s="147"/>
-      <c r="T3" s="147"/>
+      <c r="R3" s="143"/>
+      <c r="S3" s="143"/>
+      <c r="T3" s="143"/>
       <c r="V3" s="122" t="s">
         <v>339</v>
       </c>
@@ -3723,22 +3732,22 @@
       <c r="AA4" s="36"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="36"/>
-      <c r="AD4" s="143" t="s">
+      <c r="AD4" s="144" t="s">
         <v>440</v>
       </c>
-      <c r="AE4" s="143"/>
-      <c r="AF4" s="143"/>
-      <c r="AG4" s="143"/>
-      <c r="AH4" s="143"/>
-      <c r="AJ4" s="143" t="s">
+      <c r="AE4" s="144"/>
+      <c r="AF4" s="144"/>
+      <c r="AG4" s="144"/>
+      <c r="AH4" s="144"/>
+      <c r="AJ4" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="AK4" s="143"/>
-      <c r="AL4" s="143"/>
-      <c r="AM4" s="143"/>
-      <c r="AN4" s="143"/>
-      <c r="AO4" s="143"/>
-      <c r="AP4" s="143"/>
+      <c r="AK4" s="144"/>
+      <c r="AL4" s="144"/>
+      <c r="AM4" s="144"/>
+      <c r="AN4" s="144"/>
+      <c r="AO4" s="144"/>
+      <c r="AP4" s="144"/>
     </row>
     <row r="5" spans="1:42" ht="15.75">
       <c r="A5" s="129" t="s">
@@ -4831,15 +4840,15 @@
       <c r="AH17" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="AJ17" s="143" t="s">
+      <c r="AJ17" s="144" t="s">
         <v>277</v>
       </c>
-      <c r="AK17" s="143"/>
-      <c r="AL17" s="143"/>
-      <c r="AM17" s="143"/>
-      <c r="AN17" s="143"/>
-      <c r="AO17" s="143"/>
-      <c r="AP17" s="143"/>
+      <c r="AK17" s="144"/>
+      <c r="AL17" s="144"/>
+      <c r="AM17" s="144"/>
+      <c r="AN17" s="144"/>
+      <c r="AO17" s="144"/>
+      <c r="AP17" s="144"/>
     </row>
     <row r="18" spans="1:42" ht="15.75">
       <c r="A18" s="129" t="s">
@@ -5056,9 +5065,9 @@
       <c r="O20" s="35"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="147"/>
-      <c r="S20" s="147"/>
-      <c r="T20" s="147"/>
+      <c r="R20" s="143"/>
+      <c r="S20" s="143"/>
+      <c r="T20" s="143"/>
       <c r="U20" s="2"/>
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
@@ -5398,13 +5407,13 @@
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
-      <c r="AD24" s="143" t="s">
+      <c r="AD24" s="144" t="s">
         <v>497</v>
       </c>
-      <c r="AE24" s="143"/>
-      <c r="AF24" s="143"/>
-      <c r="AG24" s="143"/>
-      <c r="AH24" s="143"/>
+      <c r="AE24" s="144"/>
+      <c r="AF24" s="144"/>
+      <c r="AG24" s="144"/>
+      <c r="AH24" s="144"/>
       <c r="AJ24" s="142" t="s">
         <v>576</v>
       </c>
@@ -5714,15 +5723,15 @@
       <c r="S29" s="35"/>
       <c r="T29" s="35"/>
       <c r="U29" s="35"/>
-      <c r="V29" s="143" t="s">
+      <c r="V29" s="144" t="s">
         <v>212</v>
       </c>
-      <c r="W29" s="143"/>
-      <c r="X29" s="143"/>
-      <c r="Y29" s="143"/>
-      <c r="Z29" s="143"/>
-      <c r="AA29" s="143"/>
-      <c r="AB29" s="143"/>
+      <c r="W29" s="144"/>
+      <c r="X29" s="144"/>
+      <c r="Y29" s="144"/>
+      <c r="Z29" s="144"/>
+      <c r="AA29" s="144"/>
+      <c r="AB29" s="144"/>
     </row>
     <row r="30" spans="1:42">
       <c r="A30" s="129"/>
@@ -5812,11 +5821,11 @@
       <c r="Y31" s="37"/>
       <c r="Z31" s="37"/>
       <c r="AA31" s="12"/>
-      <c r="AD31" s="144" t="s">
+      <c r="AD31" s="145" t="s">
         <v>263</v>
       </c>
-      <c r="AE31" s="145"/>
-      <c r="AF31" s="146"/>
+      <c r="AE31" s="146"/>
+      <c r="AF31" s="147"/>
     </row>
     <row r="32" spans="1:42">
       <c r="S32" s="12"/>
@@ -5921,15 +5930,15 @@
       <c r="S37" s="12"/>
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
-      <c r="V37" s="143" t="s">
+      <c r="V37" s="144" t="s">
         <v>9</v>
       </c>
-      <c r="W37" s="143"/>
-      <c r="X37" s="143"/>
-      <c r="Y37" s="143"/>
-      <c r="Z37" s="143"/>
-      <c r="AA37" s="143"/>
-      <c r="AB37" s="143"/>
+      <c r="W37" s="144"/>
+      <c r="X37" s="144"/>
+      <c r="Y37" s="144"/>
+      <c r="Z37" s="144"/>
+      <c r="AA37" s="144"/>
+      <c r="AB37" s="144"/>
       <c r="AD37" s="3" t="s">
         <v>259</v>
       </c>
@@ -6028,15 +6037,15 @@
       <c r="S42" s="12"/>
       <c r="T42" s="12"/>
       <c r="U42" s="12"/>
-      <c r="V42" s="143" t="s">
+      <c r="V42" s="144" t="s">
         <v>247</v>
       </c>
-      <c r="W42" s="143"/>
-      <c r="X42" s="143"/>
-      <c r="Y42" s="143"/>
-      <c r="Z42" s="143"/>
-      <c r="AA42" s="143"/>
-      <c r="AB42" s="143"/>
+      <c r="W42" s="144"/>
+      <c r="X42" s="144"/>
+      <c r="Y42" s="144"/>
+      <c r="Z42" s="144"/>
+      <c r="AA42" s="144"/>
+      <c r="AB42" s="144"/>
       <c r="AD42" s="3" t="s">
         <v>265</v>
       </c>
@@ -6141,15 +6150,15 @@
       <c r="S48" s="12"/>
       <c r="T48" s="12"/>
       <c r="U48" s="12"/>
-      <c r="V48" s="144" t="s">
+      <c r="V48" s="145" t="s">
         <v>484</v>
       </c>
-      <c r="W48" s="145"/>
-      <c r="X48" s="145"/>
-      <c r="Y48" s="145"/>
-      <c r="Z48" s="145"/>
-      <c r="AA48" s="145"/>
-      <c r="AB48" s="146"/>
+      <c r="W48" s="146"/>
+      <c r="X48" s="146"/>
+      <c r="Y48" s="146"/>
+      <c r="Z48" s="146"/>
+      <c r="AA48" s="146"/>
+      <c r="AB48" s="147"/>
     </row>
     <row r="49" spans="19:28">
       <c r="S49" s="12"/>
@@ -6239,6 +6248,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="V42:AB42"/>
+    <mergeCell ref="AD4:AH4"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="V48:AB48"/>
+    <mergeCell ref="V37:AB37"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="AJ4:AP4"/>
@@ -6246,11 +6260,6 @@
     <mergeCell ref="AD31:AF31"/>
     <mergeCell ref="V29:AB29"/>
     <mergeCell ref="AD24:AH24"/>
-    <mergeCell ref="V42:AB42"/>
-    <mergeCell ref="AD4:AH4"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="V48:AB48"/>
-    <mergeCell ref="V37:AB37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6261,8 +6270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AJ32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -6277,48 +6286,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:36">
-      <c r="B2" s="143" t="s">
+      <c r="B2" s="144" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="H2" s="143" t="s">
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="H2" s="144" t="s">
         <v>231</v>
       </c>
-      <c r="I2" s="143"/>
-      <c r="J2" s="143"/>
-      <c r="K2" s="143"/>
-      <c r="L2" s="143"/>
-      <c r="N2" s="143" t="s">
+      <c r="I2" s="144"/>
+      <c r="J2" s="144"/>
+      <c r="K2" s="144"/>
+      <c r="L2" s="144"/>
+      <c r="N2" s="144" t="s">
         <v>239</v>
       </c>
-      <c r="O2" s="143"/>
-      <c r="P2" s="143"/>
-      <c r="Q2" s="143"/>
-      <c r="R2" s="143"/>
-      <c r="T2" s="143" t="s">
+      <c r="O2" s="144"/>
+      <c r="P2" s="144"/>
+      <c r="Q2" s="144"/>
+      <c r="R2" s="144"/>
+      <c r="T2" s="144" t="s">
         <v>249</v>
       </c>
-      <c r="U2" s="143"/>
-      <c r="V2" s="143"/>
-      <c r="W2" s="143"/>
-      <c r="X2" s="143"/>
-      <c r="Z2" s="143" t="s">
+      <c r="U2" s="144"/>
+      <c r="V2" s="144"/>
+      <c r="W2" s="144"/>
+      <c r="X2" s="144"/>
+      <c r="Z2" s="144" t="s">
         <v>321</v>
       </c>
-      <c r="AA2" s="143"/>
-      <c r="AB2" s="143"/>
-      <c r="AC2" s="143"/>
-      <c r="AD2" s="143"/>
-      <c r="AF2" s="143" t="s">
+      <c r="AA2" s="144"/>
+      <c r="AB2" s="144"/>
+      <c r="AC2" s="144"/>
+      <c r="AD2" s="144"/>
+      <c r="AF2" s="144" t="s">
         <v>502</v>
       </c>
-      <c r="AG2" s="143"/>
-      <c r="AH2" s="143"/>
-      <c r="AI2" s="143"/>
-      <c r="AJ2" s="143"/>
+      <c r="AG2" s="144"/>
+      <c r="AH2" s="144"/>
+      <c r="AI2" s="144"/>
+      <c r="AJ2" s="144"/>
     </row>
     <row r="3" spans="2:36">
       <c r="B3" s="124" t="s">
@@ -6513,6 +6522,9 @@
         <v>512</v>
       </c>
       <c r="J9"/>
+      <c r="N9" t="s">
+        <v>582</v>
+      </c>
     </row>
     <row r="10" spans="2:36">
       <c r="B10" s="139"/>
@@ -6543,6 +6555,9 @@
       <c r="D13" s="140"/>
       <c r="E13" s="139"/>
       <c r="F13" s="140"/>
+      <c r="H13" t="s">
+        <v>581</v>
+      </c>
     </row>
     <row r="14" spans="2:36">
       <c r="B14" s="139"/>
@@ -6564,6 +6579,9 @@
       <c r="D16" s="140"/>
       <c r="E16" s="139"/>
       <c r="F16" s="140"/>
+      <c r="H16" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="17" spans="2:20">
       <c r="B17" s="139"/>
@@ -8433,40 +8451,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="171" t="s">
+      <c r="A1" s="188" t="s">
         <v>337</v>
       </c>
-      <c r="B1" s="171"/>
-      <c r="C1" s="171"/>
-      <c r="D1" s="171"/>
-      <c r="E1" s="171"/>
-      <c r="F1" s="171"/>
-      <c r="G1" s="171"/>
-      <c r="H1" s="171"/>
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="172"/>
-      <c r="B2" s="172"/>
-      <c r="C2" s="172"/>
-      <c r="D2" s="172"/>
-      <c r="E2" s="172"/>
-      <c r="F2" s="172"/>
-      <c r="G2" s="172"/>
-      <c r="H2" s="172"/>
+      <c r="A2" s="189"/>
+      <c r="B2" s="189"/>
+      <c r="C2" s="189"/>
+      <c r="D2" s="189"/>
+      <c r="E2" s="189"/>
+      <c r="F2" s="189"/>
+      <c r="G2" s="189"/>
+      <c r="H2" s="189"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="173" t="s">
+      <c r="A3" s="190" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="174"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="173" t="s">
+      <c r="B3" s="191"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="193"/>
+      <c r="E3" s="190" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="174"/>
-      <c r="G3" s="175"/>
-      <c r="H3" s="176"/>
+      <c r="F3" s="191"/>
+      <c r="G3" s="192"/>
+      <c r="H3" s="193"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="46">
@@ -8759,18 +8777,18 @@
       <c r="H24" s="74"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="173" t="s">
+      <c r="A25" s="190" t="s">
         <v>293</v>
       </c>
-      <c r="B25" s="174"/>
-      <c r="C25" s="175"/>
-      <c r="D25" s="176"/>
-      <c r="E25" s="173" t="s">
+      <c r="B25" s="191"/>
+      <c r="C25" s="192"/>
+      <c r="D25" s="193"/>
+      <c r="E25" s="190" t="s">
         <v>294</v>
       </c>
-      <c r="F25" s="174"/>
-      <c r="G25" s="175"/>
-      <c r="H25" s="176"/>
+      <c r="F25" s="191"/>
+      <c r="G25" s="192"/>
+      <c r="H25" s="193"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="50" t="s">
@@ -8782,23 +8800,23 @@
       <c r="E26" s="46" t="s">
         <v>296</v>
       </c>
-      <c r="F26" s="180"/>
-      <c r="G26" s="181"/>
-      <c r="H26" s="182"/>
+      <c r="F26" s="185"/>
+      <c r="G26" s="186"/>
+      <c r="H26" s="187"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="B27" s="183"/>
-      <c r="C27" s="184"/>
-      <c r="D27" s="185"/>
+      <c r="B27" s="180"/>
+      <c r="C27" s="181"/>
+      <c r="D27" s="183"/>
       <c r="E27" s="50" t="s">
         <v>298</v>
       </c>
       <c r="F27" s="177"/>
       <c r="G27" s="178"/>
-      <c r="H27" s="186"/>
+      <c r="H27" s="184"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="50" t="s">
@@ -8810,23 +8828,23 @@
       <c r="E28" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="F28" s="183"/>
-      <c r="G28" s="184"/>
-      <c r="H28" s="187"/>
+      <c r="F28" s="180"/>
+      <c r="G28" s="181"/>
+      <c r="H28" s="182"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="58" t="s">
         <v>301</v>
       </c>
-      <c r="B29" s="183"/>
-      <c r="C29" s="184"/>
-      <c r="D29" s="185"/>
+      <c r="B29" s="180"/>
+      <c r="C29" s="181"/>
+      <c r="D29" s="183"/>
       <c r="E29" s="50" t="s">
         <v>302</v>
       </c>
       <c r="F29" s="177"/>
       <c r="G29" s="178"/>
-      <c r="H29" s="186"/>
+      <c r="H29" s="184"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="50" t="s">
@@ -8838,23 +8856,23 @@
       <c r="E30" s="58" t="s">
         <v>304</v>
       </c>
-      <c r="F30" s="183"/>
-      <c r="G30" s="184"/>
-      <c r="H30" s="187"/>
+      <c r="F30" s="180"/>
+      <c r="G30" s="181"/>
+      <c r="H30" s="182"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="B31" s="183"/>
-      <c r="C31" s="184"/>
-      <c r="D31" s="185"/>
+      <c r="B31" s="180"/>
+      <c r="C31" s="181"/>
+      <c r="D31" s="183"/>
       <c r="E31" s="50" t="s">
         <v>306</v>
       </c>
       <c r="F31" s="177"/>
       <c r="G31" s="178"/>
-      <c r="H31" s="186"/>
+      <c r="H31" s="184"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="50" t="s">
@@ -8864,9 +8882,9 @@
       <c r="C32" s="178"/>
       <c r="D32" s="179"/>
       <c r="E32" s="58"/>
-      <c r="F32" s="183"/>
-      <c r="G32" s="184"/>
-      <c r="H32" s="187" t="s">
+      <c r="F32" s="180"/>
+      <c r="G32" s="181"/>
+      <c r="H32" s="182" t="s">
         <v>245</v>
       </c>
     </row>
@@ -8874,13 +8892,13 @@
       <c r="A33" s="58" t="s">
         <v>308</v>
       </c>
-      <c r="B33" s="183"/>
-      <c r="C33" s="184"/>
-      <c r="D33" s="185"/>
+      <c r="B33" s="180"/>
+      <c r="C33" s="181"/>
+      <c r="D33" s="183"/>
       <c r="E33" s="50"/>
       <c r="F33" s="177"/>
       <c r="G33" s="178"/>
-      <c r="H33" s="186" t="s">
+      <c r="H33" s="184" t="s">
         <v>288</v>
       </c>
     </row>
@@ -8892,9 +8910,9 @@
       <c r="C34" s="178"/>
       <c r="D34" s="179"/>
       <c r="E34" s="58"/>
-      <c r="F34" s="183"/>
-      <c r="G34" s="184"/>
-      <c r="H34" s="187" t="s">
+      <c r="F34" s="180"/>
+      <c r="G34" s="181"/>
+      <c r="H34" s="182" t="s">
         <v>289</v>
       </c>
     </row>
@@ -8902,13 +8920,13 @@
       <c r="A35" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="B35" s="183"/>
-      <c r="C35" s="184"/>
-      <c r="D35" s="185"/>
+      <c r="B35" s="180"/>
+      <c r="C35" s="181"/>
+      <c r="D35" s="183"/>
       <c r="E35" s="50"/>
       <c r="F35" s="177"/>
       <c r="G35" s="178"/>
-      <c r="H35" s="186" t="s">
+      <c r="H35" s="184" t="s">
         <v>290</v>
       </c>
     </row>
@@ -8920,9 +8938,9 @@
       <c r="C36" s="178"/>
       <c r="D36" s="179"/>
       <c r="E36" s="58"/>
-      <c r="F36" s="183"/>
-      <c r="G36" s="184"/>
-      <c r="H36" s="187" t="s">
+      <c r="F36" s="180"/>
+      <c r="G36" s="181"/>
+      <c r="H36" s="182" t="s">
         <v>291</v>
       </c>
     </row>
@@ -8930,13 +8948,13 @@
       <c r="A37" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="B37" s="183"/>
-      <c r="C37" s="184"/>
-      <c r="D37" s="185"/>
+      <c r="B37" s="180"/>
+      <c r="C37" s="181"/>
+      <c r="D37" s="183"/>
       <c r="E37" s="50"/>
       <c r="F37" s="177"/>
       <c r="G37" s="178"/>
-      <c r="H37" s="186" t="s">
+      <c r="H37" s="184" t="s">
         <v>292</v>
       </c>
     </row>
@@ -8948,9 +8966,9 @@
       <c r="C38" s="178"/>
       <c r="D38" s="179"/>
       <c r="E38" s="58"/>
-      <c r="F38" s="183"/>
-      <c r="G38" s="184"/>
-      <c r="H38" s="187" t="s">
+      <c r="F38" s="180"/>
+      <c r="G38" s="181"/>
+      <c r="H38" s="182" t="s">
         <v>244</v>
       </c>
     </row>
@@ -8958,13 +8976,13 @@
       <c r="A39" s="58" t="s">
         <v>314</v>
       </c>
-      <c r="B39" s="183"/>
-      <c r="C39" s="184"/>
-      <c r="D39" s="185"/>
+      <c r="B39" s="180"/>
+      <c r="C39" s="181"/>
+      <c r="D39" s="183"/>
       <c r="E39" s="50"/>
       <c r="F39" s="177"/>
       <c r="G39" s="178"/>
-      <c r="H39" s="186" t="s">
+      <c r="H39" s="184" t="s">
         <v>245</v>
       </c>
     </row>
@@ -8976,24 +8994,53 @@
       <c r="C40" s="178"/>
       <c r="D40" s="179"/>
       <c r="E40" s="58"/>
-      <c r="F40" s="183"/>
-      <c r="G40" s="184"/>
-      <c r="H40" s="187"/>
+      <c r="F40" s="180"/>
+      <c r="G40" s="181"/>
+      <c r="H40" s="182"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="70" t="s">
         <v>316</v>
       </c>
-      <c r="B41" s="188"/>
-      <c r="C41" s="189"/>
-      <c r="D41" s="190"/>
+      <c r="B41" s="171"/>
+      <c r="C41" s="172"/>
+      <c r="D41" s="173"/>
       <c r="E41" s="75"/>
-      <c r="F41" s="191"/>
-      <c r="G41" s="192"/>
-      <c r="H41" s="193"/>
+      <c r="F41" s="174"/>
+      <c r="G41" s="175"/>
+      <c r="H41" s="176"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -9002,35 +9049,6 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chg: Added strike bridge tasking in range 23
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="626">
   <si>
     <t>AWACS</t>
   </si>
@@ -1774,6 +1774,132 @@
   </si>
   <si>
     <t>SNAKE</t>
+  </si>
+  <si>
+    <t>AWACS VHF Backup</t>
+  </si>
+  <si>
+    <t>Bodø TWR</t>
+  </si>
+  <si>
+    <t>AWACS Check-in</t>
+  </si>
+  <si>
+    <t>Bodø APP</t>
+  </si>
+  <si>
+    <t>Bodø ATIS</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>AR201</t>
+  </si>
+  <si>
+    <t>AR202</t>
+  </si>
+  <si>
+    <t>AR203</t>
+  </si>
+  <si>
+    <t>In Flight Report</t>
+  </si>
+  <si>
+    <t>Alert Freq</t>
+  </si>
+  <si>
+    <t>Admin Freq</t>
+  </si>
+  <si>
+    <t>Air Request Secondary</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R11 Secondary</t>
+  </si>
+  <si>
+    <t>R12 Secondary</t>
+  </si>
+  <si>
+    <t>R15 Secondary</t>
+  </si>
+  <si>
+    <t>R16 Secondary</t>
+  </si>
+  <si>
+    <t>R17 Secondary</t>
+  </si>
+  <si>
+    <t>R18 Secondary</t>
+  </si>
+  <si>
+    <t>R21 Secondary</t>
+  </si>
+  <si>
+    <t>R22Secondary</t>
+  </si>
+  <si>
+    <t>R24 Secondary</t>
+  </si>
+  <si>
+    <t>R23 Secondary</t>
+  </si>
+  <si>
+    <t>R31 Secondary</t>
+  </si>
+  <si>
+    <t>R32 Secondary</t>
+  </si>
+  <si>
+    <t>R33 Secondary</t>
+  </si>
+  <si>
+    <t>MOA 1 Secondary</t>
+  </si>
+  <si>
+    <t>Bodø Airbase AI (for lights)</t>
   </si>
 </sst>
 </file>
@@ -2567,7 +2693,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="206">
+  <cellXfs count="210">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2911,6 +3037,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2925,6 +3060,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3120,64 +3258,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2050" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="133350" y="7277100"/>
-          <a:ext cx="3467100" cy="3419475"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="1">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3468,8 +3548,8 @@
   <sheetPr codeName="Ark1"/>
   <dimension ref="A1:AP53"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AJ13" sqref="AJ13"/>
+    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AI3" sqref="AI3:AP25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -3585,13 +3665,13 @@
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
       <c r="T2" s="12"/>
-      <c r="V2" s="144" t="s">
+      <c r="V2" s="147" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="144"/>
-      <c r="X2" s="144"/>
-      <c r="Y2" s="144"/>
-      <c r="Z2" s="144"/>
+      <c r="W2" s="147"/>
+      <c r="X2" s="147"/>
+      <c r="Y2" s="147"/>
+      <c r="Z2" s="147"/>
       <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
       <c r="AC2" s="12"/>
@@ -3646,9 +3726,9 @@
         <v>437</v>
       </c>
       <c r="Q3" s="12"/>
-      <c r="R3" s="143"/>
-      <c r="S3" s="143"/>
-      <c r="T3" s="143"/>
+      <c r="R3" s="146"/>
+      <c r="S3" s="146"/>
+      <c r="T3" s="146"/>
       <c r="V3" s="122" t="s">
         <v>339</v>
       </c>
@@ -3732,22 +3812,22 @@
       <c r="AA4" s="36"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="36"/>
-      <c r="AD4" s="144" t="s">
+      <c r="AD4" s="147" t="s">
         <v>440</v>
       </c>
-      <c r="AE4" s="144"/>
-      <c r="AF4" s="144"/>
-      <c r="AG4" s="144"/>
-      <c r="AH4" s="144"/>
-      <c r="AJ4" s="144" t="s">
+      <c r="AE4" s="147"/>
+      <c r="AF4" s="147"/>
+      <c r="AG4" s="147"/>
+      <c r="AH4" s="147"/>
+      <c r="AJ4" s="147" t="s">
         <v>1</v>
       </c>
-      <c r="AK4" s="144"/>
-      <c r="AL4" s="144"/>
-      <c r="AM4" s="144"/>
-      <c r="AN4" s="144"/>
-      <c r="AO4" s="144"/>
-      <c r="AP4" s="144"/>
+      <c r="AK4" s="147"/>
+      <c r="AL4" s="147"/>
+      <c r="AM4" s="147"/>
+      <c r="AN4" s="147"/>
+      <c r="AO4" s="147"/>
+      <c r="AP4" s="147"/>
     </row>
     <row r="5" spans="1:42" ht="15.75">
       <c r="A5" s="129" t="s">
@@ -4840,15 +4920,15 @@
       <c r="AH17" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="AJ17" s="144" t="s">
+      <c r="AJ17" s="147" t="s">
         <v>277</v>
       </c>
-      <c r="AK17" s="144"/>
-      <c r="AL17" s="144"/>
-      <c r="AM17" s="144"/>
-      <c r="AN17" s="144"/>
-      <c r="AO17" s="144"/>
-      <c r="AP17" s="144"/>
+      <c r="AK17" s="147"/>
+      <c r="AL17" s="147"/>
+      <c r="AM17" s="147"/>
+      <c r="AN17" s="147"/>
+      <c r="AO17" s="147"/>
+      <c r="AP17" s="147"/>
     </row>
     <row r="18" spans="1:42" ht="15.75">
       <c r="A18" s="129" t="s">
@@ -5065,9 +5145,9 @@
       <c r="O20" s="35"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="143"/>
-      <c r="S20" s="143"/>
-      <c r="T20" s="143"/>
+      <c r="R20" s="146"/>
+      <c r="S20" s="146"/>
+      <c r="T20" s="146"/>
       <c r="U20" s="2"/>
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
@@ -5407,13 +5487,13 @@
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
-      <c r="AD24" s="144" t="s">
+      <c r="AD24" s="147" t="s">
         <v>497</v>
       </c>
-      <c r="AE24" s="144"/>
-      <c r="AF24" s="144"/>
-      <c r="AG24" s="144"/>
-      <c r="AH24" s="144"/>
+      <c r="AE24" s="147"/>
+      <c r="AF24" s="147"/>
+      <c r="AG24" s="147"/>
+      <c r="AH24" s="147"/>
       <c r="AJ24" s="142" t="s">
         <v>576</v>
       </c>
@@ -5723,15 +5803,15 @@
       <c r="S29" s="35"/>
       <c r="T29" s="35"/>
       <c r="U29" s="35"/>
-      <c r="V29" s="144" t="s">
+      <c r="V29" s="147" t="s">
         <v>212</v>
       </c>
-      <c r="W29" s="144"/>
-      <c r="X29" s="144"/>
-      <c r="Y29" s="144"/>
-      <c r="Z29" s="144"/>
-      <c r="AA29" s="144"/>
-      <c r="AB29" s="144"/>
+      <c r="W29" s="147"/>
+      <c r="X29" s="147"/>
+      <c r="Y29" s="147"/>
+      <c r="Z29" s="147"/>
+      <c r="AA29" s="147"/>
+      <c r="AB29" s="147"/>
     </row>
     <row r="30" spans="1:42">
       <c r="A30" s="129"/>
@@ -5821,11 +5901,11 @@
       <c r="Y31" s="37"/>
       <c r="Z31" s="37"/>
       <c r="AA31" s="12"/>
-      <c r="AD31" s="145" t="s">
+      <c r="AD31" s="148" t="s">
         <v>263</v>
       </c>
-      <c r="AE31" s="146"/>
-      <c r="AF31" s="147"/>
+      <c r="AE31" s="149"/>
+      <c r="AF31" s="150"/>
     </row>
     <row r="32" spans="1:42">
       <c r="S32" s="12"/>
@@ -5930,15 +6010,15 @@
       <c r="S37" s="12"/>
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
-      <c r="V37" s="144" t="s">
+      <c r="V37" s="147" t="s">
         <v>9</v>
       </c>
-      <c r="W37" s="144"/>
-      <c r="X37" s="144"/>
-      <c r="Y37" s="144"/>
-      <c r="Z37" s="144"/>
-      <c r="AA37" s="144"/>
-      <c r="AB37" s="144"/>
+      <c r="W37" s="147"/>
+      <c r="X37" s="147"/>
+      <c r="Y37" s="147"/>
+      <c r="Z37" s="147"/>
+      <c r="AA37" s="147"/>
+      <c r="AB37" s="147"/>
       <c r="AD37" s="3" t="s">
         <v>259</v>
       </c>
@@ -6037,15 +6117,15 @@
       <c r="S42" s="12"/>
       <c r="T42" s="12"/>
       <c r="U42" s="12"/>
-      <c r="V42" s="144" t="s">
+      <c r="V42" s="147" t="s">
         <v>247</v>
       </c>
-      <c r="W42" s="144"/>
-      <c r="X42" s="144"/>
-      <c r="Y42" s="144"/>
-      <c r="Z42" s="144"/>
-      <c r="AA42" s="144"/>
-      <c r="AB42" s="144"/>
+      <c r="W42" s="147"/>
+      <c r="X42" s="147"/>
+      <c r="Y42" s="147"/>
+      <c r="Z42" s="147"/>
+      <c r="AA42" s="147"/>
+      <c r="AB42" s="147"/>
       <c r="AD42" s="3" t="s">
         <v>265</v>
       </c>
@@ -6150,15 +6230,15 @@
       <c r="S48" s="12"/>
       <c r="T48" s="12"/>
       <c r="U48" s="12"/>
-      <c r="V48" s="145" t="s">
+      <c r="V48" s="148" t="s">
         <v>484</v>
       </c>
-      <c r="W48" s="146"/>
-      <c r="X48" s="146"/>
-      <c r="Y48" s="146"/>
-      <c r="Z48" s="146"/>
-      <c r="AA48" s="146"/>
-      <c r="AB48" s="147"/>
+      <c r="W48" s="149"/>
+      <c r="X48" s="149"/>
+      <c r="Y48" s="149"/>
+      <c r="Z48" s="149"/>
+      <c r="AA48" s="149"/>
+      <c r="AB48" s="150"/>
     </row>
     <row r="49" spans="19:28">
       <c r="S49" s="12"/>
@@ -6270,7 +6350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AJ32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -6286,48 +6366,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:36">
-      <c r="B2" s="144" t="s">
+      <c r="B2" s="147" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="144"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="144"/>
-      <c r="H2" s="144" t="s">
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="147"/>
+      <c r="H2" s="147" t="s">
         <v>231</v>
       </c>
-      <c r="I2" s="144"/>
-      <c r="J2" s="144"/>
-      <c r="K2" s="144"/>
-      <c r="L2" s="144"/>
-      <c r="N2" s="144" t="s">
+      <c r="I2" s="147"/>
+      <c r="J2" s="147"/>
+      <c r="K2" s="147"/>
+      <c r="L2" s="147"/>
+      <c r="N2" s="147" t="s">
         <v>239</v>
       </c>
-      <c r="O2" s="144"/>
-      <c r="P2" s="144"/>
-      <c r="Q2" s="144"/>
-      <c r="R2" s="144"/>
-      <c r="T2" s="144" t="s">
+      <c r="O2" s="147"/>
+      <c r="P2" s="147"/>
+      <c r="Q2" s="147"/>
+      <c r="R2" s="147"/>
+      <c r="T2" s="147" t="s">
         <v>249</v>
       </c>
-      <c r="U2" s="144"/>
-      <c r="V2" s="144"/>
-      <c r="W2" s="144"/>
-      <c r="X2" s="144"/>
-      <c r="Z2" s="144" t="s">
+      <c r="U2" s="147"/>
+      <c r="V2" s="147"/>
+      <c r="W2" s="147"/>
+      <c r="X2" s="147"/>
+      <c r="Z2" s="147" t="s">
         <v>321</v>
       </c>
-      <c r="AA2" s="144"/>
-      <c r="AB2" s="144"/>
-      <c r="AC2" s="144"/>
-      <c r="AD2" s="144"/>
-      <c r="AF2" s="144" t="s">
+      <c r="AA2" s="147"/>
+      <c r="AB2" s="147"/>
+      <c r="AC2" s="147"/>
+      <c r="AD2" s="147"/>
+      <c r="AF2" s="147" t="s">
         <v>502</v>
       </c>
-      <c r="AG2" s="144"/>
-      <c r="AH2" s="144"/>
-      <c r="AI2" s="144"/>
-      <c r="AJ2" s="144"/>
+      <c r="AG2" s="147"/>
+      <c r="AH2" s="147"/>
+      <c r="AI2" s="147"/>
+      <c r="AJ2" s="147"/>
     </row>
     <row r="3" spans="2:36">
       <c r="B3" s="124" t="s">
@@ -6729,8 +6809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8:M9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -6741,46 +6821,49 @@
     <col min="5" max="5" width="3.5703125" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" customWidth="1"/>
+    <col min="18" max="18" width="1.140625" customWidth="1"/>
+    <col min="19" max="19" width="3.42578125" customWidth="1"/>
     <col min="20" max="20" width="19.7109375" customWidth="1"/>
     <col min="21" max="21" width="14.7109375" customWidth="1"/>
     <col min="22" max="22" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="152" t="s">
         <v>334</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="150"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="154"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="151"/>
-      <c r="B2" s="152"/>
-      <c r="C2" s="152"/>
-      <c r="D2" s="152"/>
-      <c r="E2" s="152"/>
-      <c r="F2" s="152"/>
-      <c r="G2" s="152"/>
-      <c r="H2" s="153"/>
+      <c r="A2" s="155"/>
+      <c r="B2" s="156"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="157"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="158" t="s">
         <v>253</v>
       </c>
-      <c r="B3" s="155"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="155"/>
-      <c r="E3" s="155" t="s">
+      <c r="B3" s="159"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159" t="s">
         <v>254</v>
       </c>
-      <c r="F3" s="155"/>
-      <c r="G3" s="155"/>
-      <c r="H3" s="156"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="160"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="20">
@@ -6806,13 +6889,17 @@
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="23"/>
-      <c r="D5" s="30"/>
+      <c r="D5" s="30" t="s">
+        <v>588</v>
+      </c>
       <c r="E5" s="21">
         <v>2</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="23"/>
-      <c r="H5" s="22"/>
+      <c r="H5" s="22" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="18.75" thickBot="1">
       <c r="A6" s="20">
@@ -6820,7 +6907,9 @@
       </c>
       <c r="B6" s="22"/>
       <c r="C6" s="23"/>
-      <c r="D6" s="30"/>
+      <c r="D6" s="30" t="s">
+        <v>585</v>
+      </c>
       <c r="E6" s="21">
         <v>3</v>
       </c>
@@ -6834,7 +6923,9 @@
       </c>
       <c r="B7" s="22"/>
       <c r="C7" s="23"/>
-      <c r="D7" s="30"/>
+      <c r="D7" s="30" t="s">
+        <v>587</v>
+      </c>
       <c r="E7" s="21">
         <v>4</v>
       </c>
@@ -6848,7 +6939,9 @@
       </c>
       <c r="B8" s="22"/>
       <c r="C8" s="23"/>
-      <c r="D8" s="30"/>
+      <c r="D8" s="30" t="s">
+        <v>586</v>
+      </c>
       <c r="E8" s="21">
         <v>5</v>
       </c>
@@ -6862,7 +6955,9 @@
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="23"/>
-      <c r="D9" s="30"/>
+      <c r="D9" s="30" t="s">
+        <v>602</v>
+      </c>
       <c r="E9" s="21">
         <v>6</v>
       </c>
@@ -6876,13 +6971,17 @@
       </c>
       <c r="B10" s="22"/>
       <c r="C10" s="23"/>
-      <c r="D10" s="30"/>
+      <c r="D10" s="30" t="s">
+        <v>603</v>
+      </c>
       <c r="E10" s="21">
         <v>7</v>
       </c>
       <c r="F10" s="22"/>
       <c r="G10" s="23"/>
-      <c r="H10" s="22"/>
+      <c r="H10" s="22" t="s">
+        <v>624</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="18.75" thickBot="1">
       <c r="A11" s="20">
@@ -6890,13 +6989,17 @@
       </c>
       <c r="B11" s="22"/>
       <c r="C11" s="23"/>
-      <c r="D11" s="30"/>
+      <c r="D11" s="30" t="s">
+        <v>589</v>
+      </c>
       <c r="E11" s="21">
         <v>8</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="41"/>
-      <c r="H11" s="22"/>
+      <c r="H11" s="22" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="18.75" thickBot="1">
       <c r="A12" s="20">
@@ -6904,13 +7007,17 @@
       </c>
       <c r="B12" s="22"/>
       <c r="C12" s="23"/>
-      <c r="D12" s="30"/>
+      <c r="D12" s="30" t="s">
+        <v>590</v>
+      </c>
       <c r="E12" s="21">
         <v>9</v>
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="23"/>
-      <c r="H12" s="22"/>
+      <c r="H12" s="22" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="18.75" thickBot="1">
       <c r="A13" s="20">
@@ -6918,13 +7025,17 @@
       </c>
       <c r="B13" s="22"/>
       <c r="C13" s="23"/>
-      <c r="D13" s="30"/>
+      <c r="D13" s="30" t="s">
+        <v>591</v>
+      </c>
       <c r="E13" s="21">
         <v>10</v>
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="23"/>
-      <c r="H13" s="22"/>
+      <c r="H13" s="22" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="18.75" thickBot="1">
       <c r="A14" s="20">
@@ -6932,13 +7043,17 @@
       </c>
       <c r="B14" s="22"/>
       <c r="C14" s="23"/>
-      <c r="D14" s="30"/>
+      <c r="D14" s="30" t="s">
+        <v>592</v>
+      </c>
       <c r="E14" s="21">
         <v>11</v>
       </c>
       <c r="F14" s="22"/>
       <c r="G14" s="23"/>
-      <c r="H14" s="22"/>
+      <c r="H14" s="22" t="s">
+        <v>614</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="18.75" thickBot="1">
       <c r="A15" s="20">
@@ -6946,13 +7061,17 @@
       </c>
       <c r="B15" s="22"/>
       <c r="C15" s="23"/>
-      <c r="D15" s="30"/>
+      <c r="D15" s="30" t="s">
+        <v>593</v>
+      </c>
       <c r="E15" s="21">
         <v>12</v>
       </c>
       <c r="F15" s="22"/>
       <c r="G15" s="41"/>
-      <c r="H15" s="22"/>
+      <c r="H15" s="22" t="s">
+        <v>615</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="18.75" thickBot="1">
       <c r="A16" s="20">
@@ -6960,13 +7079,17 @@
       </c>
       <c r="B16" s="22"/>
       <c r="C16" s="23"/>
-      <c r="D16" s="30"/>
+      <c r="D16" s="30" t="s">
+        <v>594</v>
+      </c>
       <c r="E16" s="21">
         <v>13</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="23"/>
-      <c r="H16" s="22"/>
+      <c r="H16" s="22" t="s">
+        <v>616</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="18.75" thickBot="1">
       <c r="A17" s="20">
@@ -6974,13 +7097,17 @@
       </c>
       <c r="B17" s="22"/>
       <c r="C17" s="23"/>
-      <c r="D17" s="30"/>
+      <c r="D17" s="30" t="s">
+        <v>595</v>
+      </c>
       <c r="E17" s="21">
         <v>14</v>
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="41"/>
-      <c r="H17" s="22"/>
+      <c r="H17" s="22" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="18.75" thickBot="1">
       <c r="A18" s="20">
@@ -6988,13 +7115,17 @@
       </c>
       <c r="B18" s="22"/>
       <c r="C18" s="23"/>
-      <c r="D18" s="39"/>
+      <c r="D18" s="30" t="s">
+        <v>596</v>
+      </c>
       <c r="E18" s="21">
         <v>15</v>
       </c>
       <c r="F18" s="22"/>
       <c r="G18" s="40"/>
-      <c r="H18" s="22"/>
+      <c r="H18" s="22" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="18.75" thickBot="1">
       <c r="A19" s="20">
@@ -7002,13 +7133,17 @@
       </c>
       <c r="B19" s="22"/>
       <c r="C19" s="23"/>
-      <c r="D19" s="39"/>
+      <c r="D19" s="30" t="s">
+        <v>597</v>
+      </c>
       <c r="E19" s="21">
         <v>16</v>
       </c>
       <c r="F19" s="22"/>
       <c r="G19" s="40"/>
-      <c r="H19" s="22"/>
+      <c r="H19" s="22" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="18.75" thickBot="1">
       <c r="A20" s="20">
@@ -7016,13 +7151,17 @@
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="23"/>
-      <c r="D20" s="39"/>
+      <c r="D20" s="30" t="s">
+        <v>598</v>
+      </c>
       <c r="E20" s="21">
         <v>17</v>
       </c>
       <c r="F20" s="22"/>
       <c r="G20" s="41"/>
-      <c r="H20" s="22"/>
+      <c r="H20" s="22" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="18.75" thickBot="1">
       <c r="A21" s="20">
@@ -7030,13 +7169,17 @@
       </c>
       <c r="B21" s="22"/>
       <c r="C21" s="23"/>
-      <c r="D21" s="30"/>
+      <c r="D21" s="30" t="s">
+        <v>599</v>
+      </c>
       <c r="E21" s="21">
         <v>18</v>
       </c>
       <c r="F21" s="22"/>
       <c r="G21" s="23"/>
-      <c r="H21" s="22"/>
+      <c r="H21" s="22" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="18.75" thickBot="1">
       <c r="A22" s="20">
@@ -7044,13 +7187,17 @@
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="23"/>
-      <c r="D22" s="30"/>
+      <c r="D22" s="30" t="s">
+        <v>600</v>
+      </c>
       <c r="E22" s="21">
         <v>19</v>
       </c>
       <c r="F22" s="22"/>
       <c r="G22" s="23"/>
-      <c r="H22" s="22"/>
+      <c r="H22" s="22" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="23" spans="1:8" ht="18.75" thickBot="1">
       <c r="A23" s="20">
@@ -7058,13 +7205,17 @@
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="23"/>
-      <c r="D23" s="30"/>
+      <c r="D23" s="30" t="s">
+        <v>601</v>
+      </c>
       <c r="E23" s="21">
         <v>20</v>
       </c>
       <c r="F23" s="22"/>
       <c r="G23" s="23"/>
-      <c r="H23" s="22"/>
+      <c r="H23" s="22" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="24"/>
@@ -7086,103 +7237,121 @@
       <c r="G25" s="25"/>
       <c r="H25" s="26"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" ht="18">
       <c r="A26" s="24"/>
       <c r="B26" s="25"/>
       <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
+      <c r="D26" s="143"/>
       <c r="E26" s="25"/>
       <c r="F26" s="25"/>
       <c r="G26" s="25"/>
       <c r="H26" s="26"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" ht="18">
       <c r="A27" s="24"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
+      <c r="B27" s="144"/>
+      <c r="C27" s="145"/>
+      <c r="D27" s="151" t="s">
+        <v>604</v>
+      </c>
+      <c r="E27" s="151"/>
+      <c r="F27" s="151"/>
       <c r="G27" s="25"/>
       <c r="H27" s="26"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" ht="18">
       <c r="A28" s="24"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
+      <c r="B28" s="145"/>
+      <c r="C28" s="145"/>
+      <c r="D28" s="151" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="151"/>
+      <c r="F28" s="151"/>
       <c r="G28" s="25"/>
       <c r="H28" s="26"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" ht="18">
       <c r="A29" s="24"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
+      <c r="B29" s="145"/>
+      <c r="C29" s="145"/>
+      <c r="D29" s="151" t="s">
+        <v>605</v>
+      </c>
+      <c r="E29" s="151"/>
+      <c r="F29" s="151"/>
       <c r="G29" s="25"/>
       <c r="H29" s="26"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" ht="18">
       <c r="A30" s="24"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
+      <c r="B30" s="145"/>
+      <c r="C30" s="145"/>
+      <c r="D30" s="151" t="s">
+        <v>606</v>
+      </c>
+      <c r="E30" s="151"/>
+      <c r="F30" s="151"/>
       <c r="G30" s="25"/>
       <c r="H30" s="26"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" ht="18">
       <c r="A31" s="24"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
+      <c r="B31" s="145"/>
+      <c r="C31" s="145"/>
+      <c r="D31" s="151" t="s">
+        <v>607</v>
+      </c>
+      <c r="E31" s="151"/>
+      <c r="F31" s="151"/>
       <c r="G31" s="25"/>
       <c r="H31" s="26"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" ht="18">
       <c r="A32" s="24"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
+      <c r="B32" s="145"/>
+      <c r="C32" s="145"/>
+      <c r="D32" s="151" t="s">
+        <v>608</v>
+      </c>
+      <c r="E32" s="151"/>
+      <c r="F32" s="151"/>
       <c r="G32" s="25"/>
       <c r="H32" s="26"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" ht="18">
       <c r="A33" s="24"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
+      <c r="B33" s="145"/>
+      <c r="C33" s="145"/>
+      <c r="D33" s="151" t="s">
+        <v>493</v>
+      </c>
+      <c r="E33" s="151"/>
+      <c r="F33" s="151"/>
       <c r="G33" s="25"/>
       <c r="H33" s="26"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" ht="18">
       <c r="A34" s="24"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
+      <c r="B34" s="145"/>
+      <c r="C34" s="145"/>
+      <c r="D34" s="151" t="s">
+        <v>609</v>
+      </c>
+      <c r="E34" s="151"/>
+      <c r="F34" s="151"/>
       <c r="G34" s="25"/>
       <c r="H34" s="26"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" ht="18">
       <c r="A35" s="24"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
+      <c r="B35" s="145"/>
+      <c r="C35" s="145"/>
+      <c r="D35" s="151" t="s">
+        <v>610</v>
+      </c>
+      <c r="E35" s="151"/>
+      <c r="F35" s="151"/>
       <c r="G35" s="25"/>
       <c r="H35" s="26"/>
     </row>
@@ -7190,7 +7359,9 @@
       <c r="A36" s="24"/>
       <c r="B36" s="25"/>
       <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
+      <c r="D36" s="25" t="s">
+        <v>625</v>
+      </c>
       <c r="E36" s="25"/>
       <c r="F36" s="25"/>
       <c r="G36" s="25"/>
@@ -7357,14 +7528,22 @@
       <c r="H52" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="12">
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:H3"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7372,7 +7551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F30" sqref="F30:H39"/>
     </sheetView>
   </sheetViews>
@@ -7385,28 +7564,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="164" t="s">
         <v>335</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
-      <c r="H1" s="160"/>
+      <c r="B1" s="164"/>
+      <c r="C1" s="164"/>
+      <c r="D1" s="164"/>
+      <c r="E1" s="164"/>
+      <c r="F1" s="164"/>
+      <c r="G1" s="164"/>
+      <c r="H1" s="164"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="157" t="s">
+      <c r="A2" s="161" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="158"/>
-      <c r="C2" s="158"/>
-      <c r="D2" s="158"/>
-      <c r="E2" s="158"/>
-      <c r="F2" s="158"/>
-      <c r="G2" s="158"/>
-      <c r="H2" s="159"/>
+      <c r="B2" s="162"/>
+      <c r="C2" s="162"/>
+      <c r="D2" s="162"/>
+      <c r="E2" s="162"/>
+      <c r="F2" s="162"/>
+      <c r="G2" s="162"/>
+      <c r="H2" s="163"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="5"/>
@@ -7585,16 +7764,16 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="157" t="s">
+      <c r="A15" s="161" t="s">
         <v>225</v>
       </c>
-      <c r="B15" s="158"/>
-      <c r="C15" s="158"/>
-      <c r="D15" s="158"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="158"/>
-      <c r="H15" s="159"/>
+      <c r="B15" s="162"/>
+      <c r="C15" s="162"/>
+      <c r="D15" s="162"/>
+      <c r="E15" s="162"/>
+      <c r="F15" s="162"/>
+      <c r="G15" s="162"/>
+      <c r="H15" s="163"/>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="9"/>
@@ -7770,16 +7949,16 @@
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:11" ht="15.75">
-      <c r="A28" s="157" t="s">
+      <c r="A28" s="161" t="s">
         <v>226</v>
       </c>
-      <c r="B28" s="158"/>
-      <c r="C28" s="158"/>
-      <c r="D28" s="158"/>
-      <c r="E28" s="158"/>
-      <c r="F28" s="158"/>
-      <c r="G28" s="158"/>
-      <c r="H28" s="159"/>
+      <c r="B28" s="162"/>
+      <c r="C28" s="162"/>
+      <c r="D28" s="162"/>
+      <c r="E28" s="162"/>
+      <c r="F28" s="162"/>
+      <c r="G28" s="162"/>
+      <c r="H28" s="163"/>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="5"/>
@@ -7979,40 +8158,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="165" t="s">
         <v>336</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
-      <c r="G1" s="162"/>
-      <c r="H1" s="163"/>
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="167"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="164"/>
-      <c r="B2" s="165"/>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="166"/>
+      <c r="A2" s="168"/>
+      <c r="B2" s="169"/>
+      <c r="C2" s="169"/>
+      <c r="D2" s="169"/>
+      <c r="E2" s="169"/>
+      <c r="F2" s="169"/>
+      <c r="G2" s="169"/>
+      <c r="H2" s="170"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="167" t="s">
+      <c r="A3" s="171" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="168"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="167" t="s">
+      <c r="B3" s="172"/>
+      <c r="C3" s="173"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="171" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="168"/>
-      <c r="G3" s="169"/>
-      <c r="H3" s="170"/>
+      <c r="F3" s="172"/>
+      <c r="G3" s="173"/>
+      <c r="H3" s="174"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="16">
@@ -8451,40 +8630,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="192" t="s">
         <v>337</v>
       </c>
-      <c r="B1" s="188"/>
-      <c r="C1" s="188"/>
-      <c r="D1" s="188"/>
-      <c r="E1" s="188"/>
-      <c r="F1" s="188"/>
-      <c r="G1" s="188"/>
-      <c r="H1" s="188"/>
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
+      <c r="F1" s="192"/>
+      <c r="G1" s="192"/>
+      <c r="H1" s="192"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="189"/>
-      <c r="B2" s="189"/>
-      <c r="C2" s="189"/>
-      <c r="D2" s="189"/>
-      <c r="E2" s="189"/>
-      <c r="F2" s="189"/>
-      <c r="G2" s="189"/>
-      <c r="H2" s="189"/>
+      <c r="A2" s="193"/>
+      <c r="B2" s="193"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="190" t="s">
+      <c r="A3" s="194" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="191"/>
-      <c r="C3" s="192"/>
-      <c r="D3" s="193"/>
-      <c r="E3" s="190" t="s">
+      <c r="B3" s="195"/>
+      <c r="C3" s="196"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="194" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="191"/>
-      <c r="G3" s="192"/>
-      <c r="H3" s="193"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="196"/>
+      <c r="H3" s="197"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="46">
@@ -8777,114 +8956,114 @@
       <c r="H24" s="74"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="190" t="s">
+      <c r="A25" s="194" t="s">
         <v>293</v>
       </c>
-      <c r="B25" s="191"/>
-      <c r="C25" s="192"/>
-      <c r="D25" s="193"/>
-      <c r="E25" s="190" t="s">
+      <c r="B25" s="195"/>
+      <c r="C25" s="196"/>
+      <c r="D25" s="197"/>
+      <c r="E25" s="194" t="s">
         <v>294</v>
       </c>
-      <c r="F25" s="191"/>
-      <c r="G25" s="192"/>
-      <c r="H25" s="193"/>
+      <c r="F25" s="195"/>
+      <c r="G25" s="196"/>
+      <c r="H25" s="197"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="50" t="s">
         <v>295</v>
       </c>
-      <c r="B26" s="177"/>
-      <c r="C26" s="178"/>
-      <c r="D26" s="179"/>
+      <c r="B26" s="181"/>
+      <c r="C26" s="182"/>
+      <c r="D26" s="183"/>
       <c r="E26" s="46" t="s">
         <v>296</v>
       </c>
-      <c r="F26" s="185"/>
-      <c r="G26" s="186"/>
-      <c r="H26" s="187"/>
+      <c r="F26" s="189"/>
+      <c r="G26" s="190"/>
+      <c r="H26" s="191"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="B27" s="180"/>
-      <c r="C27" s="181"/>
-      <c r="D27" s="183"/>
+      <c r="B27" s="184"/>
+      <c r="C27" s="185"/>
+      <c r="D27" s="187"/>
       <c r="E27" s="50" t="s">
         <v>298</v>
       </c>
-      <c r="F27" s="177"/>
-      <c r="G27" s="178"/>
-      <c r="H27" s="184"/>
+      <c r="F27" s="181"/>
+      <c r="G27" s="182"/>
+      <c r="H27" s="188"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="50" t="s">
         <v>299</v>
       </c>
-      <c r="B28" s="177"/>
-      <c r="C28" s="178"/>
-      <c r="D28" s="179"/>
+      <c r="B28" s="181"/>
+      <c r="C28" s="182"/>
+      <c r="D28" s="183"/>
       <c r="E28" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="F28" s="180"/>
-      <c r="G28" s="181"/>
-      <c r="H28" s="182"/>
+      <c r="F28" s="184"/>
+      <c r="G28" s="185"/>
+      <c r="H28" s="186"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="58" t="s">
         <v>301</v>
       </c>
-      <c r="B29" s="180"/>
-      <c r="C29" s="181"/>
-      <c r="D29" s="183"/>
+      <c r="B29" s="184"/>
+      <c r="C29" s="185"/>
+      <c r="D29" s="187"/>
       <c r="E29" s="50" t="s">
         <v>302</v>
       </c>
-      <c r="F29" s="177"/>
-      <c r="G29" s="178"/>
-      <c r="H29" s="184"/>
+      <c r="F29" s="181"/>
+      <c r="G29" s="182"/>
+      <c r="H29" s="188"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="50" t="s">
         <v>303</v>
       </c>
-      <c r="B30" s="177"/>
-      <c r="C30" s="178"/>
-      <c r="D30" s="179"/>
+      <c r="B30" s="181"/>
+      <c r="C30" s="182"/>
+      <c r="D30" s="183"/>
       <c r="E30" s="58" t="s">
         <v>304</v>
       </c>
-      <c r="F30" s="180"/>
-      <c r="G30" s="181"/>
-      <c r="H30" s="182"/>
+      <c r="F30" s="184"/>
+      <c r="G30" s="185"/>
+      <c r="H30" s="186"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="B31" s="180"/>
-      <c r="C31" s="181"/>
-      <c r="D31" s="183"/>
+      <c r="B31" s="184"/>
+      <c r="C31" s="185"/>
+      <c r="D31" s="187"/>
       <c r="E31" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="F31" s="177"/>
-      <c r="G31" s="178"/>
-      <c r="H31" s="184"/>
+      <c r="F31" s="181"/>
+      <c r="G31" s="182"/>
+      <c r="H31" s="188"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="50" t="s">
         <v>307</v>
       </c>
-      <c r="B32" s="177"/>
-      <c r="C32" s="178"/>
-      <c r="D32" s="179"/>
+      <c r="B32" s="181"/>
+      <c r="C32" s="182"/>
+      <c r="D32" s="183"/>
       <c r="E32" s="58"/>
-      <c r="F32" s="180"/>
-      <c r="G32" s="181"/>
-      <c r="H32" s="182" t="s">
+      <c r="F32" s="184"/>
+      <c r="G32" s="185"/>
+      <c r="H32" s="186" t="s">
         <v>245</v>
       </c>
     </row>
@@ -8892,13 +9071,13 @@
       <c r="A33" s="58" t="s">
         <v>308</v>
       </c>
-      <c r="B33" s="180"/>
-      <c r="C33" s="181"/>
-      <c r="D33" s="183"/>
+      <c r="B33" s="184"/>
+      <c r="C33" s="185"/>
+      <c r="D33" s="187"/>
       <c r="E33" s="50"/>
-      <c r="F33" s="177"/>
-      <c r="G33" s="178"/>
-      <c r="H33" s="184" t="s">
+      <c r="F33" s="181"/>
+      <c r="G33" s="182"/>
+      <c r="H33" s="188" t="s">
         <v>288</v>
       </c>
     </row>
@@ -8906,13 +9085,13 @@
       <c r="A34" s="50" t="s">
         <v>309</v>
       </c>
-      <c r="B34" s="177"/>
-      <c r="C34" s="178"/>
-      <c r="D34" s="179"/>
+      <c r="B34" s="181"/>
+      <c r="C34" s="182"/>
+      <c r="D34" s="183"/>
       <c r="E34" s="58"/>
-      <c r="F34" s="180"/>
-      <c r="G34" s="181"/>
-      <c r="H34" s="182" t="s">
+      <c r="F34" s="184"/>
+      <c r="G34" s="185"/>
+      <c r="H34" s="186" t="s">
         <v>289</v>
       </c>
     </row>
@@ -8920,13 +9099,13 @@
       <c r="A35" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="B35" s="180"/>
-      <c r="C35" s="181"/>
-      <c r="D35" s="183"/>
+      <c r="B35" s="184"/>
+      <c r="C35" s="185"/>
+      <c r="D35" s="187"/>
       <c r="E35" s="50"/>
-      <c r="F35" s="177"/>
-      <c r="G35" s="178"/>
-      <c r="H35" s="184" t="s">
+      <c r="F35" s="181"/>
+      <c r="G35" s="182"/>
+      <c r="H35" s="188" t="s">
         <v>290</v>
       </c>
     </row>
@@ -8934,13 +9113,13 @@
       <c r="A36" s="50" t="s">
         <v>311</v>
       </c>
-      <c r="B36" s="177"/>
-      <c r="C36" s="178"/>
-      <c r="D36" s="179"/>
+      <c r="B36" s="181"/>
+      <c r="C36" s="182"/>
+      <c r="D36" s="183"/>
       <c r="E36" s="58"/>
-      <c r="F36" s="180"/>
-      <c r="G36" s="181"/>
-      <c r="H36" s="182" t="s">
+      <c r="F36" s="184"/>
+      <c r="G36" s="185"/>
+      <c r="H36" s="186" t="s">
         <v>291</v>
       </c>
     </row>
@@ -8948,13 +9127,13 @@
       <c r="A37" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="B37" s="180"/>
-      <c r="C37" s="181"/>
-      <c r="D37" s="183"/>
+      <c r="B37" s="184"/>
+      <c r="C37" s="185"/>
+      <c r="D37" s="187"/>
       <c r="E37" s="50"/>
-      <c r="F37" s="177"/>
-      <c r="G37" s="178"/>
-      <c r="H37" s="184" t="s">
+      <c r="F37" s="181"/>
+      <c r="G37" s="182"/>
+      <c r="H37" s="188" t="s">
         <v>292</v>
       </c>
     </row>
@@ -8962,13 +9141,13 @@
       <c r="A38" s="50" t="s">
         <v>313</v>
       </c>
-      <c r="B38" s="177"/>
-      <c r="C38" s="178"/>
-      <c r="D38" s="179"/>
+      <c r="B38" s="181"/>
+      <c r="C38" s="182"/>
+      <c r="D38" s="183"/>
       <c r="E38" s="58"/>
-      <c r="F38" s="180"/>
-      <c r="G38" s="181"/>
-      <c r="H38" s="182" t="s">
+      <c r="F38" s="184"/>
+      <c r="G38" s="185"/>
+      <c r="H38" s="186" t="s">
         <v>244</v>
       </c>
     </row>
@@ -8976,13 +9155,13 @@
       <c r="A39" s="58" t="s">
         <v>314</v>
       </c>
-      <c r="B39" s="180"/>
-      <c r="C39" s="181"/>
-      <c r="D39" s="183"/>
+      <c r="B39" s="184"/>
+      <c r="C39" s="185"/>
+      <c r="D39" s="187"/>
       <c r="E39" s="50"/>
-      <c r="F39" s="177"/>
-      <c r="G39" s="178"/>
-      <c r="H39" s="184" t="s">
+      <c r="F39" s="181"/>
+      <c r="G39" s="182"/>
+      <c r="H39" s="188" t="s">
         <v>245</v>
       </c>
     </row>
@@ -8990,25 +9169,25 @@
       <c r="A40" s="50" t="s">
         <v>315</v>
       </c>
-      <c r="B40" s="177"/>
-      <c r="C40" s="178"/>
-      <c r="D40" s="179"/>
+      <c r="B40" s="181"/>
+      <c r="C40" s="182"/>
+      <c r="D40" s="183"/>
       <c r="E40" s="58"/>
-      <c r="F40" s="180"/>
-      <c r="G40" s="181"/>
-      <c r="H40" s="182"/>
+      <c r="F40" s="184"/>
+      <c r="G40" s="185"/>
+      <c r="H40" s="186"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="70" t="s">
         <v>316</v>
       </c>
-      <c r="B41" s="171"/>
-      <c r="C41" s="172"/>
-      <c r="D41" s="173"/>
+      <c r="B41" s="175"/>
+      <c r="C41" s="176"/>
+      <c r="D41" s="177"/>
       <c r="E41" s="75"/>
-      <c r="F41" s="174"/>
-      <c r="G41" s="175"/>
-      <c r="H41" s="176"/>
+      <c r="F41" s="178"/>
+      <c r="G41" s="179"/>
+      <c r="H41" s="180"/>
     </row>
   </sheetData>
   <mergeCells count="37">
@@ -9077,40 +9256,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="204" t="s">
         <v>338</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="202"/>
+      <c r="B1" s="205"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
+      <c r="E1" s="205"/>
+      <c r="F1" s="205"/>
+      <c r="G1" s="205"/>
+      <c r="H1" s="206"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="203"/>
-      <c r="B2" s="204"/>
-      <c r="C2" s="204"/>
-      <c r="D2" s="204"/>
-      <c r="E2" s="204"/>
-      <c r="F2" s="204"/>
-      <c r="G2" s="204"/>
-      <c r="H2" s="205"/>
+      <c r="A2" s="207"/>
+      <c r="B2" s="208"/>
+      <c r="C2" s="208"/>
+      <c r="D2" s="208"/>
+      <c r="E2" s="208"/>
+      <c r="F2" s="208"/>
+      <c r="G2" s="208"/>
+      <c r="H2" s="209"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="194" t="s">
+      <c r="A3" s="198" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="195"/>
-      <c r="C3" s="195"/>
-      <c r="D3" s="196"/>
-      <c r="E3" s="194" t="s">
+      <c r="B3" s="199"/>
+      <c r="C3" s="199"/>
+      <c r="D3" s="200"/>
+      <c r="E3" s="198" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="195"/>
-      <c r="G3" s="195"/>
-      <c r="H3" s="196"/>
+      <c r="F3" s="199"/>
+      <c r="G3" s="199"/>
+      <c r="H3" s="200"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="93">
@@ -9327,18 +9506,18 @@
       <c r="H21" s="85"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="197" t="s">
+      <c r="A22" s="201" t="s">
         <v>319</v>
       </c>
-      <c r="B22" s="198"/>
-      <c r="C22" s="198"/>
-      <c r="D22" s="199"/>
-      <c r="E22" s="197" t="s">
+      <c r="B22" s="202"/>
+      <c r="C22" s="202"/>
+      <c r="D22" s="203"/>
+      <c r="E22" s="201" t="s">
         <v>320</v>
       </c>
-      <c r="F22" s="198"/>
-      <c r="G22" s="198"/>
-      <c r="H22" s="199"/>
+      <c r="F22" s="202"/>
+      <c r="G22" s="202"/>
+      <c r="H22" s="203"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="78">
@@ -9615,40 +9794,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="204" t="s">
         <v>498</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="202"/>
+      <c r="B1" s="205"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
+      <c r="E1" s="205"/>
+      <c r="F1" s="205"/>
+      <c r="G1" s="205"/>
+      <c r="H1" s="206"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="203"/>
-      <c r="B2" s="204"/>
-      <c r="C2" s="204"/>
-      <c r="D2" s="204"/>
-      <c r="E2" s="204"/>
-      <c r="F2" s="204"/>
-      <c r="G2" s="204"/>
-      <c r="H2" s="205"/>
+      <c r="A2" s="207"/>
+      <c r="B2" s="208"/>
+      <c r="C2" s="208"/>
+      <c r="D2" s="208"/>
+      <c r="E2" s="208"/>
+      <c r="F2" s="208"/>
+      <c r="G2" s="208"/>
+      <c r="H2" s="209"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="194" t="s">
+      <c r="A3" s="198" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="195"/>
-      <c r="C3" s="195"/>
-      <c r="D3" s="196"/>
-      <c r="E3" s="194" t="s">
+      <c r="B3" s="199"/>
+      <c r="C3" s="199"/>
+      <c r="D3" s="200"/>
+      <c r="E3" s="198" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="195"/>
-      <c r="G3" s="195"/>
-      <c r="H3" s="196"/>
+      <c r="F3" s="199"/>
+      <c r="G3" s="199"/>
+      <c r="H3" s="200"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="93">
@@ -9865,18 +10044,18 @@
       <c r="H21" s="85"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="197" t="s">
+      <c r="A22" s="201" t="s">
         <v>319</v>
       </c>
-      <c r="B22" s="198"/>
-      <c r="C22" s="198"/>
-      <c r="D22" s="199"/>
-      <c r="E22" s="197" t="s">
+      <c r="B22" s="202"/>
+      <c r="C22" s="202"/>
+      <c r="D22" s="203"/>
+      <c r="E22" s="201" t="s">
         <v>320</v>
       </c>
-      <c r="F22" s="198"/>
-      <c r="G22" s="198"/>
-      <c r="H22" s="199"/>
+      <c r="F22" s="202"/>
+      <c r="G22" s="202"/>
+      <c r="H22" s="203"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="78">
@@ -10135,7 +10314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
@@ -10153,40 +10332,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="152" t="s">
         <v>499</v>
       </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="150"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="154"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="151"/>
-      <c r="B2" s="152"/>
-      <c r="C2" s="152"/>
-      <c r="D2" s="152"/>
-      <c r="E2" s="152"/>
-      <c r="F2" s="152"/>
-      <c r="G2" s="152"/>
-      <c r="H2" s="153"/>
+      <c r="A2" s="155"/>
+      <c r="B2" s="156"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="157"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="154" t="s">
+      <c r="A3" s="158" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="155"/>
-      <c r="C3" s="155"/>
-      <c r="D3" s="155"/>
-      <c r="E3" s="155" t="s">
+      <c r="B3" s="159"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159" t="s">
         <v>322</v>
       </c>
-      <c r="F3" s="155"/>
-      <c r="G3" s="155"/>
-      <c r="H3" s="156"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="160"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="20">

</xml_diff>

<commit_message>
chg: Added F-16 presets
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="679">
   <si>
     <t>AWACS</t>
   </si>
@@ -1791,45 +1791,6 @@
     <t>Bodø ATIS</t>
   </si>
   <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>R17</t>
-  </si>
-  <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>R21</t>
-  </si>
-  <si>
-    <t>R22</t>
-  </si>
-  <si>
-    <t>R23</t>
-  </si>
-  <si>
-    <t>R24</t>
-  </si>
-  <si>
-    <t>R31</t>
-  </si>
-  <si>
-    <t>R32</t>
-  </si>
-  <si>
-    <t>R33</t>
-  </si>
-  <si>
     <t>AR201</t>
   </si>
   <si>
@@ -1900,6 +1861,204 @@
   </si>
   <si>
     <t>Bodø Airbase AI (for lights)</t>
+  </si>
+  <si>
+    <t>280.0</t>
+  </si>
+  <si>
+    <t>281.0</t>
+  </si>
+  <si>
+    <t>282.0</t>
+  </si>
+  <si>
+    <t>237.0</t>
+  </si>
+  <si>
+    <t>140.0</t>
+  </si>
+  <si>
+    <t>MAROON11</t>
+  </si>
+  <si>
+    <t>248.0</t>
+  </si>
+  <si>
+    <t>229.0</t>
+  </si>
+  <si>
+    <t>236.5</t>
+  </si>
+  <si>
+    <t>248.5</t>
+  </si>
+  <si>
+    <t>235.0</t>
+  </si>
+  <si>
+    <t>231.5</t>
+  </si>
+  <si>
+    <t>235.75</t>
+  </si>
+  <si>
+    <t>240.0</t>
+  </si>
+  <si>
+    <t>243.75</t>
+  </si>
+  <si>
+    <t>242.5</t>
+  </si>
+  <si>
+    <t>237.75</t>
+  </si>
+  <si>
+    <t>225.85</t>
+  </si>
+  <si>
+    <t>246.25</t>
+  </si>
+  <si>
+    <t>242.0</t>
+  </si>
+  <si>
+    <t>233.5</t>
+  </si>
+  <si>
+    <t>230.5</t>
+  </si>
+  <si>
+    <t>234.0</t>
+  </si>
+  <si>
+    <t>238.75</t>
+  </si>
+  <si>
+    <t>235.25</t>
+  </si>
+  <si>
+    <t>231.75</t>
+  </si>
+  <si>
+    <t>230.0</t>
+  </si>
+  <si>
+    <t>R13 Secondary</t>
+  </si>
+  <si>
+    <t>R14 Secondary</t>
+  </si>
+  <si>
+    <t>119.5</t>
+  </si>
+  <si>
+    <t>130.75</t>
+  </si>
+  <si>
+    <t>123.75</t>
+  </si>
+  <si>
+    <t>134.7</t>
+  </si>
+  <si>
+    <t>140.25</t>
+  </si>
+  <si>
+    <t>141.0</t>
+  </si>
+  <si>
+    <t>139.75</t>
+  </si>
+  <si>
+    <t>120.25</t>
+  </si>
+  <si>
+    <t>138.25</t>
+  </si>
+  <si>
+    <t>133.7</t>
+  </si>
+  <si>
+    <t>120.5</t>
+  </si>
+  <si>
+    <t>132.7</t>
+  </si>
+  <si>
+    <t>132.75</t>
+  </si>
+  <si>
+    <t>137.7</t>
+  </si>
+  <si>
+    <t>130.7</t>
+  </si>
+  <si>
+    <t>134.75</t>
+  </si>
+  <si>
+    <t>398.15</t>
+  </si>
+  <si>
+    <t>398.65</t>
+  </si>
+  <si>
+    <t>277.3</t>
+  </si>
+  <si>
+    <t>RANGE 11</t>
+  </si>
+  <si>
+    <t>RANGE 12</t>
+  </si>
+  <si>
+    <t>RANGE 15</t>
+  </si>
+  <si>
+    <t>RANGE 16</t>
+  </si>
+  <si>
+    <t>RANGE 17</t>
+  </si>
+  <si>
+    <t>RANGE 18</t>
+  </si>
+  <si>
+    <t>RANGE 21</t>
+  </si>
+  <si>
+    <t>RANGE 22</t>
+  </si>
+  <si>
+    <t>RANGE 23</t>
+  </si>
+  <si>
+    <t>RANGE 24</t>
+  </si>
+  <si>
+    <t>RANGE 31</t>
+  </si>
+  <si>
+    <t>RANGE 32</t>
+  </si>
+  <si>
+    <t>RANGE 33</t>
+  </si>
+  <si>
+    <t>250.6</t>
+  </si>
+  <si>
+    <t>Kiruna Airbase AI (for lights)</t>
+  </si>
+  <si>
+    <t>250.1</t>
+  </si>
+  <si>
+    <t>250.5</t>
+  </si>
+  <si>
+    <t>Jokkmokk roadbase AI (for lights)</t>
   </si>
 </sst>
 </file>
@@ -2693,7 +2852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="210">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3040,30 +3199,24 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3133,6 +3286,57 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3151,57 +3355,6 @@
     <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3238,6 +3391,22 @@
     <xf numFmtId="0" fontId="16" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3549,7 +3718,7 @@
   <dimension ref="A1:AP53"/>
   <sheetViews>
     <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AI3" sqref="AI3:AP25"/>
+      <selection activeCell="V50" sqref="V50:X52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -3665,13 +3834,13 @@
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
       <c r="T2" s="12"/>
-      <c r="V2" s="147" t="s">
+      <c r="V2" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="147"/>
-      <c r="X2" s="147"/>
-      <c r="Y2" s="147"/>
-      <c r="Z2" s="147"/>
+      <c r="W2" s="144"/>
+      <c r="X2" s="144"/>
+      <c r="Y2" s="144"/>
+      <c r="Z2" s="144"/>
       <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
       <c r="AC2" s="12"/>
@@ -3726,9 +3895,9 @@
         <v>437</v>
       </c>
       <c r="Q3" s="12"/>
-      <c r="R3" s="146"/>
-      <c r="S3" s="146"/>
-      <c r="T3" s="146"/>
+      <c r="R3" s="148"/>
+      <c r="S3" s="148"/>
+      <c r="T3" s="148"/>
       <c r="V3" s="122" t="s">
         <v>339</v>
       </c>
@@ -3812,22 +3981,22 @@
       <c r="AA4" s="36"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="36"/>
-      <c r="AD4" s="147" t="s">
+      <c r="AD4" s="144" t="s">
         <v>440</v>
       </c>
-      <c r="AE4" s="147"/>
-      <c r="AF4" s="147"/>
-      <c r="AG4" s="147"/>
-      <c r="AH4" s="147"/>
-      <c r="AJ4" s="147" t="s">
+      <c r="AE4" s="144"/>
+      <c r="AF4" s="144"/>
+      <c r="AG4" s="144"/>
+      <c r="AH4" s="144"/>
+      <c r="AJ4" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="AK4" s="147"/>
-      <c r="AL4" s="147"/>
-      <c r="AM4" s="147"/>
-      <c r="AN4" s="147"/>
-      <c r="AO4" s="147"/>
-      <c r="AP4" s="147"/>
+      <c r="AK4" s="144"/>
+      <c r="AL4" s="144"/>
+      <c r="AM4" s="144"/>
+      <c r="AN4" s="144"/>
+      <c r="AO4" s="144"/>
+      <c r="AP4" s="144"/>
     </row>
     <row r="5" spans="1:42" ht="15.75">
       <c r="A5" s="129" t="s">
@@ -4920,15 +5089,15 @@
       <c r="AH17" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="AJ17" s="147" t="s">
+      <c r="AJ17" s="144" t="s">
         <v>277</v>
       </c>
-      <c r="AK17" s="147"/>
-      <c r="AL17" s="147"/>
-      <c r="AM17" s="147"/>
-      <c r="AN17" s="147"/>
-      <c r="AO17" s="147"/>
-      <c r="AP17" s="147"/>
+      <c r="AK17" s="144"/>
+      <c r="AL17" s="144"/>
+      <c r="AM17" s="144"/>
+      <c r="AN17" s="144"/>
+      <c r="AO17" s="144"/>
+      <c r="AP17" s="144"/>
     </row>
     <row r="18" spans="1:42" ht="15.75">
       <c r="A18" s="129" t="s">
@@ -5145,9 +5314,9 @@
       <c r="O20" s="35"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="146"/>
-      <c r="S20" s="146"/>
-      <c r="T20" s="146"/>
+      <c r="R20" s="148"/>
+      <c r="S20" s="148"/>
+      <c r="T20" s="148"/>
       <c r="U20" s="2"/>
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
@@ -5487,13 +5656,13 @@
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
-      <c r="AD24" s="147" t="s">
+      <c r="AD24" s="144" t="s">
         <v>497</v>
       </c>
-      <c r="AE24" s="147"/>
-      <c r="AF24" s="147"/>
-      <c r="AG24" s="147"/>
-      <c r="AH24" s="147"/>
+      <c r="AE24" s="144"/>
+      <c r="AF24" s="144"/>
+      <c r="AG24" s="144"/>
+      <c r="AH24" s="144"/>
       <c r="AJ24" s="142" t="s">
         <v>576</v>
       </c>
@@ -5803,15 +5972,15 @@
       <c r="S29" s="35"/>
       <c r="T29" s="35"/>
       <c r="U29" s="35"/>
-      <c r="V29" s="147" t="s">
+      <c r="V29" s="144" t="s">
         <v>212</v>
       </c>
-      <c r="W29" s="147"/>
-      <c r="X29" s="147"/>
-      <c r="Y29" s="147"/>
-      <c r="Z29" s="147"/>
-      <c r="AA29" s="147"/>
-      <c r="AB29" s="147"/>
+      <c r="W29" s="144"/>
+      <c r="X29" s="144"/>
+      <c r="Y29" s="144"/>
+      <c r="Z29" s="144"/>
+      <c r="AA29" s="144"/>
+      <c r="AB29" s="144"/>
     </row>
     <row r="30" spans="1:42">
       <c r="A30" s="129"/>
@@ -5901,11 +6070,11 @@
       <c r="Y31" s="37"/>
       <c r="Z31" s="37"/>
       <c r="AA31" s="12"/>
-      <c r="AD31" s="148" t="s">
+      <c r="AD31" s="145" t="s">
         <v>263</v>
       </c>
-      <c r="AE31" s="149"/>
-      <c r="AF31" s="150"/>
+      <c r="AE31" s="146"/>
+      <c r="AF31" s="147"/>
     </row>
     <row r="32" spans="1:42">
       <c r="S32" s="12"/>
@@ -6010,15 +6179,15 @@
       <c r="S37" s="12"/>
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
-      <c r="V37" s="147" t="s">
+      <c r="V37" s="144" t="s">
         <v>9</v>
       </c>
-      <c r="W37" s="147"/>
-      <c r="X37" s="147"/>
-      <c r="Y37" s="147"/>
-      <c r="Z37" s="147"/>
-      <c r="AA37" s="147"/>
-      <c r="AB37" s="147"/>
+      <c r="W37" s="144"/>
+      <c r="X37" s="144"/>
+      <c r="Y37" s="144"/>
+      <c r="Z37" s="144"/>
+      <c r="AA37" s="144"/>
+      <c r="AB37" s="144"/>
       <c r="AD37" s="3" t="s">
         <v>259</v>
       </c>
@@ -6117,15 +6286,15 @@
       <c r="S42" s="12"/>
       <c r="T42" s="12"/>
       <c r="U42" s="12"/>
-      <c r="V42" s="147" t="s">
+      <c r="V42" s="144" t="s">
         <v>247</v>
       </c>
-      <c r="W42" s="147"/>
-      <c r="X42" s="147"/>
-      <c r="Y42" s="147"/>
-      <c r="Z42" s="147"/>
-      <c r="AA42" s="147"/>
-      <c r="AB42" s="147"/>
+      <c r="W42" s="144"/>
+      <c r="X42" s="144"/>
+      <c r="Y42" s="144"/>
+      <c r="Z42" s="144"/>
+      <c r="AA42" s="144"/>
+      <c r="AB42" s="144"/>
       <c r="AD42" s="3" t="s">
         <v>265</v>
       </c>
@@ -6230,15 +6399,15 @@
       <c r="S48" s="12"/>
       <c r="T48" s="12"/>
       <c r="U48" s="12"/>
-      <c r="V48" s="148" t="s">
+      <c r="V48" s="145" t="s">
         <v>484</v>
       </c>
-      <c r="W48" s="149"/>
-      <c r="X48" s="149"/>
-      <c r="Y48" s="149"/>
-      <c r="Z48" s="149"/>
-      <c r="AA48" s="149"/>
-      <c r="AB48" s="150"/>
+      <c r="W48" s="146"/>
+      <c r="X48" s="146"/>
+      <c r="Y48" s="146"/>
+      <c r="Z48" s="146"/>
+      <c r="AA48" s="146"/>
+      <c r="AB48" s="147"/>
     </row>
     <row r="49" spans="19:28">
       <c r="S49" s="12"/>
@@ -6328,11 +6497,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="V42:AB42"/>
-    <mergeCell ref="AD4:AH4"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="V48:AB48"/>
-    <mergeCell ref="V37:AB37"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="AJ4:AP4"/>
@@ -6340,6 +6504,11 @@
     <mergeCell ref="AD31:AF31"/>
     <mergeCell ref="V29:AB29"/>
     <mergeCell ref="AD24:AH24"/>
+    <mergeCell ref="V42:AB42"/>
+    <mergeCell ref="AD4:AH4"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="V48:AB48"/>
+    <mergeCell ref="V37:AB37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6366,48 +6535,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:36">
-      <c r="B2" s="147" t="s">
+      <c r="B2" s="144" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="H2" s="147" t="s">
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="H2" s="144" t="s">
         <v>231</v>
       </c>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="147"/>
-      <c r="L2" s="147"/>
-      <c r="N2" s="147" t="s">
+      <c r="I2" s="144"/>
+      <c r="J2" s="144"/>
+      <c r="K2" s="144"/>
+      <c r="L2" s="144"/>
+      <c r="N2" s="144" t="s">
         <v>239</v>
       </c>
-      <c r="O2" s="147"/>
-      <c r="P2" s="147"/>
-      <c r="Q2" s="147"/>
-      <c r="R2" s="147"/>
-      <c r="T2" s="147" t="s">
+      <c r="O2" s="144"/>
+      <c r="P2" s="144"/>
+      <c r="Q2" s="144"/>
+      <c r="R2" s="144"/>
+      <c r="T2" s="144" t="s">
         <v>249</v>
       </c>
-      <c r="U2" s="147"/>
-      <c r="V2" s="147"/>
-      <c r="W2" s="147"/>
-      <c r="X2" s="147"/>
-      <c r="Z2" s="147" t="s">
+      <c r="U2" s="144"/>
+      <c r="V2" s="144"/>
+      <c r="W2" s="144"/>
+      <c r="X2" s="144"/>
+      <c r="Z2" s="144" t="s">
         <v>321</v>
       </c>
-      <c r="AA2" s="147"/>
-      <c r="AB2" s="147"/>
-      <c r="AC2" s="147"/>
-      <c r="AD2" s="147"/>
-      <c r="AF2" s="147" t="s">
+      <c r="AA2" s="144"/>
+      <c r="AB2" s="144"/>
+      <c r="AC2" s="144"/>
+      <c r="AD2" s="144"/>
+      <c r="AF2" s="144" t="s">
         <v>502</v>
       </c>
-      <c r="AG2" s="147"/>
-      <c r="AH2" s="147"/>
-      <c r="AI2" s="147"/>
-      <c r="AJ2" s="147"/>
+      <c r="AG2" s="144"/>
+      <c r="AH2" s="144"/>
+      <c r="AI2" s="144"/>
+      <c r="AJ2" s="144"/>
     </row>
     <row r="3" spans="2:36">
       <c r="B3" s="124" t="s">
@@ -6807,63 +6976,59 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
     <col min="5" max="5" width="3.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="17" max="17" width="4.7109375" customWidth="1"/>
-    <col min="18" max="18" width="1.140625" customWidth="1"/>
-    <col min="19" max="19" width="3.42578125" customWidth="1"/>
-    <col min="20" max="20" width="19.7109375" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="152" t="s">
+      <c r="A1" s="150" t="s">
         <v>334</v>
       </c>
-      <c r="B1" s="153"/>
-      <c r="C1" s="153"/>
-      <c r="D1" s="153"/>
-      <c r="E1" s="153"/>
-      <c r="F1" s="153"/>
-      <c r="G1" s="153"/>
-      <c r="H1" s="154"/>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="152"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="155"/>
-      <c r="B2" s="156"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="157"/>
+      <c r="A2" s="153"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="155"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="158" t="s">
+      <c r="A3" s="156" t="s">
         <v>253</v>
       </c>
-      <c r="B3" s="159"/>
-      <c r="C3" s="159"/>
-      <c r="D3" s="159"/>
-      <c r="E3" s="159" t="s">
+      <c r="B3" s="157"/>
+      <c r="C3" s="157"/>
+      <c r="D3" s="157"/>
+      <c r="E3" s="157" t="s">
         <v>254</v>
       </c>
-      <c r="F3" s="159"/>
-      <c r="G3" s="159"/>
-      <c r="H3" s="160"/>
+      <c r="F3" s="157"/>
+      <c r="G3" s="157"/>
+      <c r="H3" s="158"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="20">
@@ -6888,15 +7053,21 @@
         <v>2</v>
       </c>
       <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
+      <c r="C5" s="22" t="s">
+        <v>658</v>
+      </c>
       <c r="D5" s="30" t="s">
         <v>588</v>
       </c>
       <c r="E5" s="21">
         <v>2</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23"/>
+      <c r="F5" s="23" t="s">
+        <v>618</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>617</v>
+      </c>
       <c r="H5" s="22" t="s">
         <v>584</v>
       </c>
@@ -6906,7 +7077,9 @@
         <v>3</v>
       </c>
       <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
+      <c r="C6" s="22" t="s">
+        <v>659</v>
+      </c>
       <c r="D6" s="30" t="s">
         <v>585</v>
       </c>
@@ -6922,7 +7095,9 @@
         <v>4</v>
       </c>
       <c r="B7" s="22"/>
-      <c r="C7" s="23"/>
+      <c r="C7" s="22" t="s">
+        <v>660</v>
+      </c>
       <c r="D7" s="30" t="s">
         <v>587</v>
       </c>
@@ -6937,284 +7112,416 @@
       <c r="A8" s="20">
         <v>5</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="23"/>
+      <c r="B8" s="23" t="s">
+        <v>491</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>616</v>
+      </c>
       <c r="D8" s="30" t="s">
         <v>586</v>
       </c>
       <c r="E8" s="21">
         <v>5</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="22"/>
+      <c r="F8" s="23" t="s">
+        <v>475</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>640</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="18.75" thickBot="1">
       <c r="A9" s="20">
         <v>6</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
+      <c r="B9" s="23" t="s">
+        <v>532</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>613</v>
+      </c>
       <c r="D9" s="30" t="s">
-        <v>602</v>
+        <v>589</v>
       </c>
       <c r="E9" s="21">
         <v>6</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="22"/>
+      <c r="F9" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>641</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="18.75" thickBot="1">
       <c r="A10" s="20">
         <v>7</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
+      <c r="B10" s="23" t="s">
+        <v>553</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>614</v>
+      </c>
       <c r="D10" s="30" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="E10" s="21">
         <v>7</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
+      <c r="F10" s="23" t="s">
+        <v>496</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>644</v>
+      </c>
       <c r="H10" s="22" t="s">
-        <v>624</v>
+        <v>611</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18.75" thickBot="1">
       <c r="A11" s="20">
         <v>8</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
+      <c r="B11" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>624</v>
+      </c>
       <c r="D11" s="30" t="s">
-        <v>589</v>
+        <v>661</v>
       </c>
       <c r="E11" s="21">
         <v>8</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="41"/>
+      <c r="F11" s="23" t="s">
+        <v>472</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>645</v>
+      </c>
       <c r="H11" s="22" t="s">
-        <v>611</v>
+        <v>598</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18.75" thickBot="1">
       <c r="A12" s="20">
         <v>9</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
+      <c r="B12" s="23" t="s">
+        <v>460</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>625</v>
+      </c>
       <c r="D12" s="30" t="s">
-        <v>590</v>
+        <v>662</v>
       </c>
       <c r="E12" s="21">
         <v>9</v>
       </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
+      <c r="F12" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>646</v>
+      </c>
       <c r="H12" s="22" t="s">
-        <v>612</v>
+        <v>599</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18.75" thickBot="1">
       <c r="A13" s="20">
         <v>10</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
+      <c r="B13" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>626</v>
+      </c>
       <c r="D13" s="30" t="s">
-        <v>591</v>
+        <v>663</v>
       </c>
       <c r="E13" s="21">
         <v>10</v>
       </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23"/>
+      <c r="F13" s="23" t="s">
+        <v>476</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>647</v>
+      </c>
       <c r="H13" s="22" t="s">
-        <v>613</v>
+        <v>600</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="18.75" thickBot="1">
       <c r="A14" s="20">
         <v>11</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
+      <c r="B14" s="23" t="s">
+        <v>464</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>627</v>
+      </c>
       <c r="D14" s="30" t="s">
-        <v>592</v>
+        <v>664</v>
       </c>
       <c r="E14" s="21">
         <v>11</v>
       </c>
-      <c r="F14" s="22"/>
-      <c r="G14" s="23"/>
+      <c r="F14" s="23" t="s">
+        <v>479</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>648</v>
+      </c>
       <c r="H14" s="22" t="s">
-        <v>614</v>
+        <v>601</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18.75" thickBot="1">
       <c r="A15" s="20">
         <v>12</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
+      <c r="B15" s="23" t="s">
+        <v>465</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>628</v>
+      </c>
       <c r="D15" s="30" t="s">
-        <v>593</v>
+        <v>665</v>
       </c>
       <c r="E15" s="21">
         <v>12</v>
       </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="41"/>
+      <c r="F15" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>649</v>
+      </c>
       <c r="H15" s="22" t="s">
-        <v>615</v>
+        <v>602</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18.75" thickBot="1">
       <c r="A16" s="20">
         <v>13</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
+      <c r="B16" s="23" t="s">
+        <v>463</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>629</v>
+      </c>
       <c r="D16" s="30" t="s">
-        <v>594</v>
+        <v>666</v>
       </c>
       <c r="E16" s="21">
         <v>13</v>
       </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="23"/>
+      <c r="F16" s="23" t="s">
+        <v>481</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>650</v>
+      </c>
       <c r="H16" s="22" t="s">
-        <v>616</v>
+        <v>603</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18.75" thickBot="1">
       <c r="A17" s="20">
         <v>14</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
+      <c r="B17" s="23" t="s">
+        <v>466</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>630</v>
+      </c>
       <c r="D17" s="30" t="s">
-        <v>595</v>
+        <v>667</v>
       </c>
       <c r="E17" s="21">
         <v>14</v>
       </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="41"/>
+      <c r="F17" s="23" t="s">
+        <v>474</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>651</v>
+      </c>
       <c r="H17" s="22" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18.75" thickBot="1">
       <c r="A18" s="20">
         <v>15</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
+      <c r="B18" s="23" t="s">
+        <v>468</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>631</v>
+      </c>
       <c r="D18" s="30" t="s">
-        <v>596</v>
+        <v>668</v>
       </c>
       <c r="E18" s="21">
         <v>15</v>
       </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="40"/>
+      <c r="F18" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>652</v>
+      </c>
       <c r="H18" s="22" t="s">
-        <v>618</v>
+        <v>605</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18.75" thickBot="1">
       <c r="A19" s="20">
         <v>16</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="23"/>
+      <c r="B19" s="23" t="s">
+        <v>469</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>632</v>
+      </c>
       <c r="D19" s="30" t="s">
-        <v>597</v>
+        <v>669</v>
       </c>
       <c r="E19" s="21">
         <v>16</v>
       </c>
-      <c r="F19" s="22"/>
-      <c r="G19" s="40"/>
+      <c r="F19" s="23" t="s">
+        <v>478</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>653</v>
+      </c>
       <c r="H19" s="22" t="s">
-        <v>620</v>
+        <v>607</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18.75" thickBot="1">
       <c r="A20" s="20">
         <v>17</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="23"/>
+      <c r="B20" s="23" t="s">
+        <v>470</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>633</v>
+      </c>
       <c r="D20" s="30" t="s">
-        <v>598</v>
+        <v>670</v>
       </c>
       <c r="E20" s="21">
         <v>17</v>
       </c>
-      <c r="F20" s="22"/>
-      <c r="G20" s="41"/>
+      <c r="F20" s="23" t="s">
+        <v>483</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>654</v>
+      </c>
       <c r="H20" s="22" t="s">
-        <v>619</v>
+        <v>606</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="18.75" thickBot="1">
       <c r="A21" s="20">
         <v>18</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="23"/>
+      <c r="B21" s="23" t="s">
+        <v>467</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>634</v>
+      </c>
       <c r="D21" s="30" t="s">
-        <v>599</v>
+        <v>671</v>
       </c>
       <c r="E21" s="21">
         <v>18</v>
       </c>
-      <c r="F21" s="22"/>
-      <c r="G21" s="23"/>
+      <c r="F21" s="23" t="s">
+        <v>474</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>655</v>
+      </c>
       <c r="H21" s="22" t="s">
-        <v>621</v>
+        <v>608</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="18.75" thickBot="1">
       <c r="A22" s="20">
         <v>19</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="23"/>
+      <c r="B22" s="23" t="s">
+        <v>471</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>635</v>
+      </c>
       <c r="D22" s="30" t="s">
-        <v>600</v>
+        <v>672</v>
       </c>
       <c r="E22" s="21">
         <v>19</v>
       </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="23"/>
+      <c r="F22" s="23" t="s">
+        <v>477</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>656</v>
+      </c>
       <c r="H22" s="22" t="s">
-        <v>622</v>
+        <v>609</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18.75" thickBot="1">
       <c r="A23" s="20">
         <v>20</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="23"/>
+      <c r="B23" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>636</v>
+      </c>
       <c r="D23" s="30" t="s">
-        <v>601</v>
+        <v>673</v>
       </c>
       <c r="E23" s="21">
         <v>20</v>
       </c>
-      <c r="F23" s="22"/>
-      <c r="G23" s="23"/>
+      <c r="F23" s="23" t="s">
+        <v>482</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>657</v>
+      </c>
       <c r="H23" s="22" t="s">
-        <v>623</v>
+        <v>610</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -7249,151 +7556,197 @@
     </row>
     <row r="27" spans="1:8" ht="18">
       <c r="A27" s="24"/>
-      <c r="B27" s="144"/>
-      <c r="C27" s="145"/>
-      <c r="D27" s="151" t="s">
-        <v>604</v>
-      </c>
-      <c r="E27" s="151"/>
-      <c r="F27" s="151"/>
+      <c r="B27" s="212" t="s">
+        <v>555</v>
+      </c>
+      <c r="C27" s="208" t="s">
+        <v>615</v>
+      </c>
+      <c r="D27" s="149" t="s">
+        <v>591</v>
+      </c>
+      <c r="E27" s="149"/>
+      <c r="F27" s="149"/>
       <c r="G27" s="25"/>
       <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:8" ht="18">
       <c r="A28" s="24"/>
-      <c r="B28" s="145"/>
-      <c r="C28" s="145"/>
-      <c r="D28" s="151" t="s">
+      <c r="B28" s="212" t="s">
+        <v>241</v>
+      </c>
+      <c r="C28" s="208" t="s">
+        <v>619</v>
+      </c>
+      <c r="D28" s="149" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="151"/>
-      <c r="F28" s="151"/>
+      <c r="E28" s="149"/>
+      <c r="F28" s="149"/>
       <c r="G28" s="25"/>
       <c r="H28" s="26"/>
     </row>
     <row r="29" spans="1:8" ht="18">
       <c r="A29" s="24"/>
-      <c r="B29" s="145"/>
-      <c r="C29" s="145"/>
-      <c r="D29" s="151" t="s">
-        <v>605</v>
-      </c>
-      <c r="E29" s="151"/>
-      <c r="F29" s="151"/>
+      <c r="B29" s="212" t="s">
+        <v>242</v>
+      </c>
+      <c r="C29" s="208" t="s">
+        <v>620</v>
+      </c>
+      <c r="D29" s="149" t="s">
+        <v>592</v>
+      </c>
+      <c r="E29" s="149"/>
+      <c r="F29" s="149"/>
       <c r="G29" s="25"/>
       <c r="H29" s="26"/>
     </row>
     <row r="30" spans="1:8" ht="18">
       <c r="A30" s="24"/>
-      <c r="B30" s="145"/>
-      <c r="C30" s="145"/>
-      <c r="D30" s="151" t="s">
-        <v>606</v>
-      </c>
-      <c r="E30" s="151"/>
-      <c r="F30" s="151"/>
+      <c r="B30" s="212" t="s">
+        <v>457</v>
+      </c>
+      <c r="C30" s="208" t="s">
+        <v>621</v>
+      </c>
+      <c r="D30" s="149" t="s">
+        <v>593</v>
+      </c>
+      <c r="E30" s="149"/>
+      <c r="F30" s="149"/>
       <c r="G30" s="25"/>
       <c r="H30" s="26"/>
     </row>
     <row r="31" spans="1:8" ht="18">
       <c r="A31" s="24"/>
-      <c r="B31" s="145"/>
-      <c r="C31" s="145"/>
-      <c r="D31" s="151" t="s">
-        <v>607</v>
-      </c>
-      <c r="E31" s="151"/>
-      <c r="F31" s="151"/>
+      <c r="B31" s="212" t="s">
+        <v>458</v>
+      </c>
+      <c r="C31" s="208" t="s">
+        <v>622</v>
+      </c>
+      <c r="D31" s="149" t="s">
+        <v>594</v>
+      </c>
+      <c r="E31" s="149"/>
+      <c r="F31" s="149"/>
       <c r="G31" s="25"/>
       <c r="H31" s="26"/>
     </row>
     <row r="32" spans="1:8" ht="18">
       <c r="A32" s="24"/>
-      <c r="B32" s="145"/>
-      <c r="C32" s="145"/>
-      <c r="D32" s="151" t="s">
-        <v>608</v>
-      </c>
-      <c r="E32" s="151"/>
-      <c r="F32" s="151"/>
+      <c r="B32" s="212" t="s">
+        <v>246</v>
+      </c>
+      <c r="C32" s="208" t="s">
+        <v>623</v>
+      </c>
+      <c r="D32" s="149" t="s">
+        <v>595</v>
+      </c>
+      <c r="E32" s="149"/>
+      <c r="F32" s="149"/>
       <c r="G32" s="25"/>
       <c r="H32" s="26"/>
     </row>
     <row r="33" spans="1:8" ht="18">
       <c r="A33" s="24"/>
-      <c r="B33" s="145"/>
-      <c r="C33" s="145"/>
-      <c r="D33" s="151" t="s">
+      <c r="B33" s="212" t="s">
+        <v>495</v>
+      </c>
+      <c r="C33" s="208" t="s">
+        <v>637</v>
+      </c>
+      <c r="D33" s="149" t="s">
         <v>493</v>
       </c>
-      <c r="E33" s="151"/>
-      <c r="F33" s="151"/>
+      <c r="E33" s="149"/>
+      <c r="F33" s="149"/>
       <c r="G33" s="25"/>
       <c r="H33" s="26"/>
     </row>
     <row r="34" spans="1:8" ht="18">
       <c r="A34" s="24"/>
-      <c r="B34" s="145"/>
-      <c r="C34" s="145"/>
-      <c r="D34" s="151" t="s">
-        <v>609</v>
-      </c>
-      <c r="E34" s="151"/>
-      <c r="F34" s="151"/>
+      <c r="B34" s="212" t="s">
+        <v>461</v>
+      </c>
+      <c r="C34" s="208" t="s">
+        <v>638</v>
+      </c>
+      <c r="D34" s="149" t="s">
+        <v>596</v>
+      </c>
+      <c r="E34" s="149"/>
+      <c r="F34" s="149"/>
       <c r="G34" s="25"/>
       <c r="H34" s="26"/>
     </row>
     <row r="35" spans="1:8" ht="18">
       <c r="A35" s="24"/>
-      <c r="B35" s="145"/>
-      <c r="C35" s="145"/>
-      <c r="D35" s="151" t="s">
-        <v>610</v>
-      </c>
-      <c r="E35" s="151"/>
-      <c r="F35" s="151"/>
+      <c r="B35" s="212" t="s">
+        <v>462</v>
+      </c>
+      <c r="C35" s="208" t="s">
+        <v>639</v>
+      </c>
+      <c r="D35" s="149" t="s">
+        <v>597</v>
+      </c>
+      <c r="E35" s="149"/>
+      <c r="F35" s="149"/>
       <c r="G35" s="25"/>
       <c r="H35" s="26"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" ht="18">
       <c r="A36" s="24"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25" t="s">
-        <v>625</v>
-      </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="B36" s="208"/>
+      <c r="C36" s="208" t="s">
+        <v>674</v>
+      </c>
+      <c r="D36" s="209" t="s">
+        <v>612</v>
+      </c>
+      <c r="E36" s="210"/>
+      <c r="F36" s="211"/>
       <c r="G36" s="25"/>
       <c r="H36" s="26"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" ht="18">
       <c r="A37" s="24"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
+      <c r="B37" s="213"/>
+      <c r="C37" s="208" t="s">
+        <v>677</v>
+      </c>
+      <c r="D37" s="209" t="s">
+        <v>675</v>
+      </c>
+      <c r="E37" s="210"/>
+      <c r="F37" s="211"/>
       <c r="G37" s="25"/>
       <c r="H37" s="26"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" ht="18">
       <c r="A38" s="24"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
+      <c r="B38" s="213"/>
+      <c r="C38" s="208" t="s">
+        <v>676</v>
+      </c>
+      <c r="D38" s="209" t="s">
+        <v>678</v>
+      </c>
+      <c r="E38" s="210"/>
+      <c r="F38" s="211"/>
       <c r="G38" s="25"/>
       <c r="H38" s="26"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" ht="18">
       <c r="A39" s="24"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
+      <c r="B39" s="213"/>
+      <c r="C39" s="208"/>
+      <c r="D39" s="209"/>
+      <c r="E39" s="210"/>
+      <c r="F39" s="211"/>
       <c r="G39" s="25"/>
       <c r="H39" s="26"/>
     </row>
@@ -7477,58 +7830,24 @@
       <c r="G47" s="25"/>
       <c r="H47" s="26"/>
     </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="24"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="26"/>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="24"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="26"/>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="24"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
-      <c r="H50" s="26"/>
-    </row>
-    <row r="51" spans="1:8" ht="10.5" customHeight="1">
-      <c r="A51" s="24"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="25"/>
-      <c r="H51" s="26"/>
-    </row>
-    <row r="52" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A52" s="27"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="28"/>
-      <c r="H52" s="29"/>
-    </row>
+    <row r="48" spans="1:8" ht="41.25" customHeight="1" thickBot="1">
+      <c r="A48" s="27"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="28"/>
+      <c r="H48" s="29"/>
+    </row>
+    <row r="51" ht="10.5" customHeight="1"/>
+    <row r="52" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
     <mergeCell ref="D33:F33"/>
     <mergeCell ref="D34:F34"/>
     <mergeCell ref="D35:F35"/>
@@ -7564,28 +7883,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="164" t="s">
+      <c r="A1" s="162" t="s">
         <v>335</v>
       </c>
-      <c r="B1" s="164"/>
-      <c r="C1" s="164"/>
-      <c r="D1" s="164"/>
-      <c r="E1" s="164"/>
-      <c r="F1" s="164"/>
-      <c r="G1" s="164"/>
-      <c r="H1" s="164"/>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
+      <c r="H1" s="162"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="161" t="s">
+      <c r="A2" s="159" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="162"/>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="162"/>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="163"/>
+      <c r="B2" s="160"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="F2" s="160"/>
+      <c r="G2" s="160"/>
+      <c r="H2" s="161"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="5"/>
@@ -7764,16 +8083,16 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="161" t="s">
+      <c r="A15" s="159" t="s">
         <v>225</v>
       </c>
-      <c r="B15" s="162"/>
-      <c r="C15" s="162"/>
-      <c r="D15" s="162"/>
-      <c r="E15" s="162"/>
-      <c r="F15" s="162"/>
-      <c r="G15" s="162"/>
-      <c r="H15" s="163"/>
+      <c r="B15" s="160"/>
+      <c r="C15" s="160"/>
+      <c r="D15" s="160"/>
+      <c r="E15" s="160"/>
+      <c r="F15" s="160"/>
+      <c r="G15" s="160"/>
+      <c r="H15" s="161"/>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="9"/>
@@ -7949,16 +8268,16 @@
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:11" ht="15.75">
-      <c r="A28" s="161" t="s">
+      <c r="A28" s="159" t="s">
         <v>226</v>
       </c>
-      <c r="B28" s="162"/>
-      <c r="C28" s="162"/>
-      <c r="D28" s="162"/>
-      <c r="E28" s="162"/>
-      <c r="F28" s="162"/>
-      <c r="G28" s="162"/>
-      <c r="H28" s="163"/>
+      <c r="B28" s="160"/>
+      <c r="C28" s="160"/>
+      <c r="D28" s="160"/>
+      <c r="E28" s="160"/>
+      <c r="F28" s="160"/>
+      <c r="G28" s="160"/>
+      <c r="H28" s="161"/>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="5"/>
@@ -8158,40 +8477,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="163" t="s">
         <v>336</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="167"/>
+      <c r="B1" s="164"/>
+      <c r="C1" s="164"/>
+      <c r="D1" s="164"/>
+      <c r="E1" s="164"/>
+      <c r="F1" s="164"/>
+      <c r="G1" s="164"/>
+      <c r="H1" s="165"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="168"/>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="170"/>
+      <c r="A2" s="166"/>
+      <c r="B2" s="167"/>
+      <c r="C2" s="167"/>
+      <c r="D2" s="167"/>
+      <c r="E2" s="167"/>
+      <c r="F2" s="167"/>
+      <c r="G2" s="167"/>
+      <c r="H2" s="168"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="171" t="s">
+      <c r="A3" s="169" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="172"/>
-      <c r="C3" s="173"/>
-      <c r="D3" s="174"/>
-      <c r="E3" s="171" t="s">
+      <c r="B3" s="170"/>
+      <c r="C3" s="171"/>
+      <c r="D3" s="172"/>
+      <c r="E3" s="169" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="172"/>
-      <c r="G3" s="173"/>
-      <c r="H3" s="174"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="171"/>
+      <c r="H3" s="172"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="16">
@@ -8630,40 +8949,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="192" t="s">
+      <c r="A1" s="173" t="s">
         <v>337</v>
       </c>
-      <c r="B1" s="192"/>
-      <c r="C1" s="192"/>
-      <c r="D1" s="192"/>
-      <c r="E1" s="192"/>
-      <c r="F1" s="192"/>
-      <c r="G1" s="192"/>
-      <c r="H1" s="192"/>
+      <c r="B1" s="173"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="173"/>
+      <c r="G1" s="173"/>
+      <c r="H1" s="173"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="193"/>
-      <c r="B2" s="193"/>
-      <c r="C2" s="193"/>
-      <c r="D2" s="193"/>
-      <c r="E2" s="193"/>
-      <c r="F2" s="193"/>
-      <c r="G2" s="193"/>
-      <c r="H2" s="193"/>
+      <c r="A2" s="174"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="194" t="s">
+      <c r="A3" s="175" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="195"/>
-      <c r="C3" s="196"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="194" t="s">
+      <c r="B3" s="176"/>
+      <c r="C3" s="177"/>
+      <c r="D3" s="178"/>
+      <c r="E3" s="175" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="195"/>
-      <c r="G3" s="196"/>
-      <c r="H3" s="197"/>
+      <c r="F3" s="176"/>
+      <c r="G3" s="177"/>
+      <c r="H3" s="178"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="46">
@@ -8956,114 +9275,114 @@
       <c r="H24" s="74"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="194" t="s">
+      <c r="A25" s="175" t="s">
         <v>293</v>
       </c>
-      <c r="B25" s="195"/>
-      <c r="C25" s="196"/>
-      <c r="D25" s="197"/>
-      <c r="E25" s="194" t="s">
+      <c r="B25" s="176"/>
+      <c r="C25" s="177"/>
+      <c r="D25" s="178"/>
+      <c r="E25" s="175" t="s">
         <v>294</v>
       </c>
-      <c r="F25" s="195"/>
-      <c r="G25" s="196"/>
-      <c r="H25" s="197"/>
+      <c r="F25" s="176"/>
+      <c r="G25" s="177"/>
+      <c r="H25" s="178"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="50" t="s">
         <v>295</v>
       </c>
-      <c r="B26" s="181"/>
-      <c r="C26" s="182"/>
-      <c r="D26" s="183"/>
+      <c r="B26" s="179"/>
+      <c r="C26" s="180"/>
+      <c r="D26" s="181"/>
       <c r="E26" s="46" t="s">
         <v>296</v>
       </c>
-      <c r="F26" s="189"/>
-      <c r="G26" s="190"/>
-      <c r="H26" s="191"/>
+      <c r="F26" s="182"/>
+      <c r="G26" s="183"/>
+      <c r="H26" s="184"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="B27" s="184"/>
-      <c r="C27" s="185"/>
+      <c r="B27" s="185"/>
+      <c r="C27" s="186"/>
       <c r="D27" s="187"/>
       <c r="E27" s="50" t="s">
         <v>298</v>
       </c>
-      <c r="F27" s="181"/>
-      <c r="G27" s="182"/>
+      <c r="F27" s="179"/>
+      <c r="G27" s="180"/>
       <c r="H27" s="188"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="50" t="s">
         <v>299</v>
       </c>
-      <c r="B28" s="181"/>
-      <c r="C28" s="182"/>
-      <c r="D28" s="183"/>
+      <c r="B28" s="179"/>
+      <c r="C28" s="180"/>
+      <c r="D28" s="181"/>
       <c r="E28" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="F28" s="184"/>
-      <c r="G28" s="185"/>
-      <c r="H28" s="186"/>
+      <c r="F28" s="185"/>
+      <c r="G28" s="186"/>
+      <c r="H28" s="189"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="58" t="s">
         <v>301</v>
       </c>
-      <c r="B29" s="184"/>
-      <c r="C29" s="185"/>
+      <c r="B29" s="185"/>
+      <c r="C29" s="186"/>
       <c r="D29" s="187"/>
       <c r="E29" s="50" t="s">
         <v>302</v>
       </c>
-      <c r="F29" s="181"/>
-      <c r="G29" s="182"/>
+      <c r="F29" s="179"/>
+      <c r="G29" s="180"/>
       <c r="H29" s="188"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="50" t="s">
         <v>303</v>
       </c>
-      <c r="B30" s="181"/>
-      <c r="C30" s="182"/>
-      <c r="D30" s="183"/>
+      <c r="B30" s="179"/>
+      <c r="C30" s="180"/>
+      <c r="D30" s="181"/>
       <c r="E30" s="58" t="s">
         <v>304</v>
       </c>
-      <c r="F30" s="184"/>
-      <c r="G30" s="185"/>
-      <c r="H30" s="186"/>
+      <c r="F30" s="185"/>
+      <c r="G30" s="186"/>
+      <c r="H30" s="189"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="B31" s="184"/>
-      <c r="C31" s="185"/>
+      <c r="B31" s="185"/>
+      <c r="C31" s="186"/>
       <c r="D31" s="187"/>
       <c r="E31" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="F31" s="181"/>
-      <c r="G31" s="182"/>
+      <c r="F31" s="179"/>
+      <c r="G31" s="180"/>
       <c r="H31" s="188"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="50" t="s">
         <v>307</v>
       </c>
-      <c r="B32" s="181"/>
-      <c r="C32" s="182"/>
-      <c r="D32" s="183"/>
+      <c r="B32" s="179"/>
+      <c r="C32" s="180"/>
+      <c r="D32" s="181"/>
       <c r="E32" s="58"/>
-      <c r="F32" s="184"/>
-      <c r="G32" s="185"/>
-      <c r="H32" s="186" t="s">
+      <c r="F32" s="185"/>
+      <c r="G32" s="186"/>
+      <c r="H32" s="189" t="s">
         <v>245</v>
       </c>
     </row>
@@ -9071,12 +9390,12 @@
       <c r="A33" s="58" t="s">
         <v>308</v>
       </c>
-      <c r="B33" s="184"/>
-      <c r="C33" s="185"/>
+      <c r="B33" s="185"/>
+      <c r="C33" s="186"/>
       <c r="D33" s="187"/>
       <c r="E33" s="50"/>
-      <c r="F33" s="181"/>
-      <c r="G33" s="182"/>
+      <c r="F33" s="179"/>
+      <c r="G33" s="180"/>
       <c r="H33" s="188" t="s">
         <v>288</v>
       </c>
@@ -9085,13 +9404,13 @@
       <c r="A34" s="50" t="s">
         <v>309</v>
       </c>
-      <c r="B34" s="181"/>
-      <c r="C34" s="182"/>
-      <c r="D34" s="183"/>
+      <c r="B34" s="179"/>
+      <c r="C34" s="180"/>
+      <c r="D34" s="181"/>
       <c r="E34" s="58"/>
-      <c r="F34" s="184"/>
-      <c r="G34" s="185"/>
-      <c r="H34" s="186" t="s">
+      <c r="F34" s="185"/>
+      <c r="G34" s="186"/>
+      <c r="H34" s="189" t="s">
         <v>289</v>
       </c>
     </row>
@@ -9099,12 +9418,12 @@
       <c r="A35" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="B35" s="184"/>
-      <c r="C35" s="185"/>
+      <c r="B35" s="185"/>
+      <c r="C35" s="186"/>
       <c r="D35" s="187"/>
       <c r="E35" s="50"/>
-      <c r="F35" s="181"/>
-      <c r="G35" s="182"/>
+      <c r="F35" s="179"/>
+      <c r="G35" s="180"/>
       <c r="H35" s="188" t="s">
         <v>290</v>
       </c>
@@ -9113,13 +9432,13 @@
       <c r="A36" s="50" t="s">
         <v>311</v>
       </c>
-      <c r="B36" s="181"/>
-      <c r="C36" s="182"/>
-      <c r="D36" s="183"/>
+      <c r="B36" s="179"/>
+      <c r="C36" s="180"/>
+      <c r="D36" s="181"/>
       <c r="E36" s="58"/>
-      <c r="F36" s="184"/>
-      <c r="G36" s="185"/>
-      <c r="H36" s="186" t="s">
+      <c r="F36" s="185"/>
+      <c r="G36" s="186"/>
+      <c r="H36" s="189" t="s">
         <v>291</v>
       </c>
     </row>
@@ -9127,12 +9446,12 @@
       <c r="A37" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="B37" s="184"/>
-      <c r="C37" s="185"/>
+      <c r="B37" s="185"/>
+      <c r="C37" s="186"/>
       <c r="D37" s="187"/>
       <c r="E37" s="50"/>
-      <c r="F37" s="181"/>
-      <c r="G37" s="182"/>
+      <c r="F37" s="179"/>
+      <c r="G37" s="180"/>
       <c r="H37" s="188" t="s">
         <v>292</v>
       </c>
@@ -9141,13 +9460,13 @@
       <c r="A38" s="50" t="s">
         <v>313</v>
       </c>
-      <c r="B38" s="181"/>
-      <c r="C38" s="182"/>
-      <c r="D38" s="183"/>
+      <c r="B38" s="179"/>
+      <c r="C38" s="180"/>
+      <c r="D38" s="181"/>
       <c r="E38" s="58"/>
-      <c r="F38" s="184"/>
-      <c r="G38" s="185"/>
-      <c r="H38" s="186" t="s">
+      <c r="F38" s="185"/>
+      <c r="G38" s="186"/>
+      <c r="H38" s="189" t="s">
         <v>244</v>
       </c>
     </row>
@@ -9155,12 +9474,12 @@
       <c r="A39" s="58" t="s">
         <v>314</v>
       </c>
-      <c r="B39" s="184"/>
-      <c r="C39" s="185"/>
+      <c r="B39" s="185"/>
+      <c r="C39" s="186"/>
       <c r="D39" s="187"/>
       <c r="E39" s="50"/>
-      <c r="F39" s="181"/>
-      <c r="G39" s="182"/>
+      <c r="F39" s="179"/>
+      <c r="G39" s="180"/>
       <c r="H39" s="188" t="s">
         <v>245</v>
       </c>
@@ -9169,57 +9488,28 @@
       <c r="A40" s="50" t="s">
         <v>315</v>
       </c>
-      <c r="B40" s="181"/>
-      <c r="C40" s="182"/>
-      <c r="D40" s="183"/>
+      <c r="B40" s="179"/>
+      <c r="C40" s="180"/>
+      <c r="D40" s="181"/>
       <c r="E40" s="58"/>
-      <c r="F40" s="184"/>
-      <c r="G40" s="185"/>
-      <c r="H40" s="186"/>
+      <c r="F40" s="185"/>
+      <c r="G40" s="186"/>
+      <c r="H40" s="189"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="70" t="s">
         <v>316</v>
       </c>
-      <c r="B41" s="175"/>
-      <c r="C41" s="176"/>
-      <c r="D41" s="177"/>
+      <c r="B41" s="190"/>
+      <c r="C41" s="191"/>
+      <c r="D41" s="192"/>
       <c r="E41" s="75"/>
-      <c r="F41" s="178"/>
-      <c r="G41" s="179"/>
-      <c r="H41" s="180"/>
+      <c r="F41" s="193"/>
+      <c r="G41" s="194"/>
+      <c r="H41" s="195"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -9228,6 +9518,35 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9256,40 +9575,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="202" t="s">
         <v>338</v>
       </c>
-      <c r="B1" s="205"/>
-      <c r="C1" s="205"/>
-      <c r="D1" s="205"/>
-      <c r="E1" s="205"/>
-      <c r="F1" s="205"/>
-      <c r="G1" s="205"/>
-      <c r="H1" s="206"/>
+      <c r="B1" s="203"/>
+      <c r="C1" s="203"/>
+      <c r="D1" s="203"/>
+      <c r="E1" s="203"/>
+      <c r="F1" s="203"/>
+      <c r="G1" s="203"/>
+      <c r="H1" s="204"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="207"/>
-      <c r="B2" s="208"/>
-      <c r="C2" s="208"/>
-      <c r="D2" s="208"/>
-      <c r="E2" s="208"/>
-      <c r="F2" s="208"/>
-      <c r="G2" s="208"/>
-      <c r="H2" s="209"/>
+      <c r="A2" s="205"/>
+      <c r="B2" s="206"/>
+      <c r="C2" s="206"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="206"/>
+      <c r="F2" s="206"/>
+      <c r="G2" s="206"/>
+      <c r="H2" s="207"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="198" t="s">
+      <c r="A3" s="196" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="199"/>
-      <c r="C3" s="199"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="198" t="s">
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="196" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="199"/>
-      <c r="G3" s="199"/>
-      <c r="H3" s="200"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="198"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="93">
@@ -9506,18 +9825,18 @@
       <c r="H21" s="85"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="201" t="s">
+      <c r="A22" s="199" t="s">
         <v>319</v>
       </c>
-      <c r="B22" s="202"/>
-      <c r="C22" s="202"/>
-      <c r="D22" s="203"/>
-      <c r="E22" s="201" t="s">
+      <c r="B22" s="200"/>
+      <c r="C22" s="200"/>
+      <c r="D22" s="201"/>
+      <c r="E22" s="199" t="s">
         <v>320</v>
       </c>
-      <c r="F22" s="202"/>
-      <c r="G22" s="202"/>
-      <c r="H22" s="203"/>
+      <c r="F22" s="200"/>
+      <c r="G22" s="200"/>
+      <c r="H22" s="201"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="78">
@@ -9794,40 +10113,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="202" t="s">
         <v>498</v>
       </c>
-      <c r="B1" s="205"/>
-      <c r="C1" s="205"/>
-      <c r="D1" s="205"/>
-      <c r="E1" s="205"/>
-      <c r="F1" s="205"/>
-      <c r="G1" s="205"/>
-      <c r="H1" s="206"/>
+      <c r="B1" s="203"/>
+      <c r="C1" s="203"/>
+      <c r="D1" s="203"/>
+      <c r="E1" s="203"/>
+      <c r="F1" s="203"/>
+      <c r="G1" s="203"/>
+      <c r="H1" s="204"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="207"/>
-      <c r="B2" s="208"/>
-      <c r="C2" s="208"/>
-      <c r="D2" s="208"/>
-      <c r="E2" s="208"/>
-      <c r="F2" s="208"/>
-      <c r="G2" s="208"/>
-      <c r="H2" s="209"/>
+      <c r="A2" s="205"/>
+      <c r="B2" s="206"/>
+      <c r="C2" s="206"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="206"/>
+      <c r="F2" s="206"/>
+      <c r="G2" s="206"/>
+      <c r="H2" s="207"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="198" t="s">
+      <c r="A3" s="196" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="199"/>
-      <c r="C3" s="199"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="198" t="s">
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="196" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="199"/>
-      <c r="G3" s="199"/>
-      <c r="H3" s="200"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="197"/>
+      <c r="H3" s="198"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="93">
@@ -10044,18 +10363,18 @@
       <c r="H21" s="85"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="201" t="s">
+      <c r="A22" s="199" t="s">
         <v>319</v>
       </c>
-      <c r="B22" s="202"/>
-      <c r="C22" s="202"/>
-      <c r="D22" s="203"/>
-      <c r="E22" s="201" t="s">
+      <c r="B22" s="200"/>
+      <c r="C22" s="200"/>
+      <c r="D22" s="201"/>
+      <c r="E22" s="199" t="s">
         <v>320</v>
       </c>
-      <c r="F22" s="202"/>
-      <c r="G22" s="202"/>
-      <c r="H22" s="203"/>
+      <c r="F22" s="200"/>
+      <c r="G22" s="200"/>
+      <c r="H22" s="201"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="78">
@@ -10332,40 +10651,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="152" t="s">
+      <c r="A1" s="150" t="s">
         <v>499</v>
       </c>
-      <c r="B1" s="153"/>
-      <c r="C1" s="153"/>
-      <c r="D1" s="153"/>
-      <c r="E1" s="153"/>
-      <c r="F1" s="153"/>
-      <c r="G1" s="153"/>
-      <c r="H1" s="154"/>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="152"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="155"/>
-      <c r="B2" s="156"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="157"/>
+      <c r="A2" s="153"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="155"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="158" t="s">
+      <c r="A3" s="156" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="159"/>
-      <c r="C3" s="159"/>
-      <c r="D3" s="159"/>
-      <c r="E3" s="159" t="s">
+      <c r="B3" s="157"/>
+      <c r="C3" s="157"/>
+      <c r="D3" s="157"/>
+      <c r="E3" s="157" t="s">
         <v>322</v>
       </c>
-      <c r="F3" s="159"/>
-      <c r="G3" s="159"/>
-      <c r="H3" s="160"/>
+      <c r="F3" s="157"/>
+      <c r="G3" s="157"/>
+      <c r="H3" s="158"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="20">

</xml_diff>

<commit_message>
chg: Updated Datalink preset onepager, updated Bullseye in CombatFlite
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -4,25 +4,26 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
     <sheet name="Aircraft" sheetId="2" r:id="rId2"/>
-    <sheet name="F-16 Presets" sheetId="12" r:id="rId3"/>
-    <sheet name="A10 presets" sheetId="5" r:id="rId4"/>
-    <sheet name="F-14 Presets" sheetId="13" r:id="rId5"/>
-    <sheet name="FA-18 Hornet Presets" sheetId="10" r:id="rId6"/>
-    <sheet name="AH64 Presets" sheetId="16" r:id="rId7"/>
-    <sheet name="OH-58 Presets" sheetId="18" r:id="rId8"/>
-    <sheet name="F-15 Presets " sheetId="17" r:id="rId9"/>
+    <sheet name="Datalink" sheetId="19" r:id="rId3"/>
+    <sheet name="F-16 Presets" sheetId="12" r:id="rId4"/>
+    <sheet name="A10 presets" sheetId="5" r:id="rId5"/>
+    <sheet name="F-14 Presets" sheetId="13" r:id="rId6"/>
+    <sheet name="FA-18 Hornet Presets" sheetId="10" r:id="rId7"/>
+    <sheet name="AH64 Presets" sheetId="16" r:id="rId8"/>
+    <sheet name="OH-58 Presets" sheetId="18" r:id="rId9"/>
+    <sheet name="F-15 Presets " sheetId="17" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="763">
   <si>
     <t>AWACS</t>
   </si>
@@ -2305,6 +2306,12 @@
   </si>
   <si>
     <t>WF91</t>
+  </si>
+  <si>
+    <t>RED F16</t>
+  </si>
+  <si>
+    <t>BLUE F-16</t>
   </si>
 </sst>
 </file>
@@ -2314,7 +2321,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2467,8 +2474,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2571,8 +2609,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="41">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -3094,11 +3138,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="216">
+  <cellXfs count="251">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3452,210 +3520,275 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="18" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="24" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="24" fillId="18" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="24" fillId="18" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4084,13 +4217,13 @@
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
       <c r="T2" s="12"/>
-      <c r="V2" s="148" t="s">
+      <c r="V2" s="153" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="148"/>
-      <c r="X2" s="148"/>
-      <c r="Y2" s="148"/>
-      <c r="Z2" s="148"/>
+      <c r="W2" s="153"/>
+      <c r="X2" s="153"/>
+      <c r="Y2" s="153"/>
+      <c r="Z2" s="153"/>
       <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
       <c r="AC2" s="12"/>
@@ -4145,9 +4278,9 @@
         <v>433</v>
       </c>
       <c r="Q3" s="12"/>
-      <c r="R3" s="147"/>
-      <c r="S3" s="147"/>
-      <c r="T3" s="147"/>
+      <c r="R3" s="152"/>
+      <c r="S3" s="152"/>
+      <c r="T3" s="152"/>
       <c r="V3" s="122" t="s">
         <v>335</v>
       </c>
@@ -4231,22 +4364,22 @@
       <c r="AA4" s="36"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="36"/>
-      <c r="AD4" s="148" t="s">
+      <c r="AD4" s="153" t="s">
         <v>436</v>
       </c>
-      <c r="AE4" s="148"/>
-      <c r="AF4" s="148"/>
-      <c r="AG4" s="148"/>
-      <c r="AH4" s="148"/>
-      <c r="AJ4" s="148" t="s">
+      <c r="AE4" s="153"/>
+      <c r="AF4" s="153"/>
+      <c r="AG4" s="153"/>
+      <c r="AH4" s="153"/>
+      <c r="AJ4" s="153" t="s">
         <v>1</v>
       </c>
-      <c r="AK4" s="148"/>
-      <c r="AL4" s="148"/>
-      <c r="AM4" s="148"/>
-      <c r="AN4" s="148"/>
-      <c r="AO4" s="148"/>
-      <c r="AP4" s="148"/>
+      <c r="AK4" s="153"/>
+      <c r="AL4" s="153"/>
+      <c r="AM4" s="153"/>
+      <c r="AN4" s="153"/>
+      <c r="AO4" s="153"/>
+      <c r="AP4" s="153"/>
     </row>
     <row r="5" spans="1:42" ht="15.75">
       <c r="A5" s="129" t="s">
@@ -5339,15 +5472,15 @@
       <c r="AH17" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="AJ17" s="148" t="s">
+      <c r="AJ17" s="153" t="s">
         <v>277</v>
       </c>
-      <c r="AK17" s="148"/>
-      <c r="AL17" s="148"/>
-      <c r="AM17" s="148"/>
-      <c r="AN17" s="148"/>
-      <c r="AO17" s="148"/>
-      <c r="AP17" s="148"/>
+      <c r="AK17" s="153"/>
+      <c r="AL17" s="153"/>
+      <c r="AM17" s="153"/>
+      <c r="AN17" s="153"/>
+      <c r="AO17" s="153"/>
+      <c r="AP17" s="153"/>
     </row>
     <row r="18" spans="1:42" ht="15.75">
       <c r="A18" s="129" t="s">
@@ -5564,9 +5697,9 @@
       <c r="O20" s="35"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="147"/>
-      <c r="S20" s="147"/>
-      <c r="T20" s="147"/>
+      <c r="R20" s="152"/>
+      <c r="S20" s="152"/>
+      <c r="T20" s="152"/>
       <c r="U20" s="2"/>
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
@@ -5906,13 +6039,13 @@
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
-      <c r="AD24" s="148" t="s">
+      <c r="AD24" s="153" t="s">
         <v>493</v>
       </c>
-      <c r="AE24" s="148"/>
-      <c r="AF24" s="148"/>
-      <c r="AG24" s="148"/>
-      <c r="AH24" s="148"/>
+      <c r="AE24" s="153"/>
+      <c r="AF24" s="153"/>
+      <c r="AG24" s="153"/>
+      <c r="AH24" s="153"/>
       <c r="AJ24" s="142" t="s">
         <v>570</v>
       </c>
@@ -6222,15 +6355,15 @@
       <c r="S29" s="35"/>
       <c r="T29" s="35"/>
       <c r="U29" s="35"/>
-      <c r="V29" s="148" t="s">
+      <c r="V29" s="153" t="s">
         <v>212</v>
       </c>
-      <c r="W29" s="148"/>
-      <c r="X29" s="148"/>
-      <c r="Y29" s="148"/>
-      <c r="Z29" s="148"/>
-      <c r="AA29" s="148"/>
-      <c r="AB29" s="148"/>
+      <c r="W29" s="153"/>
+      <c r="X29" s="153"/>
+      <c r="Y29" s="153"/>
+      <c r="Z29" s="153"/>
+      <c r="AA29" s="153"/>
+      <c r="AB29" s="153"/>
     </row>
     <row r="30" spans="1:42">
       <c r="A30" s="129"/>
@@ -6320,11 +6453,11 @@
       <c r="Y31" s="37"/>
       <c r="Z31" s="37"/>
       <c r="AA31" s="12"/>
-      <c r="AD31" s="149" t="s">
+      <c r="AD31" s="154" t="s">
         <v>263</v>
       </c>
-      <c r="AE31" s="150"/>
-      <c r="AF31" s="151"/>
+      <c r="AE31" s="155"/>
+      <c r="AF31" s="156"/>
     </row>
     <row r="32" spans="1:42">
       <c r="S32" s="12"/>
@@ -6429,15 +6562,15 @@
       <c r="S37" s="12"/>
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
-      <c r="V37" s="148" t="s">
+      <c r="V37" s="153" t="s">
         <v>9</v>
       </c>
-      <c r="W37" s="148"/>
-      <c r="X37" s="148"/>
-      <c r="Y37" s="148"/>
-      <c r="Z37" s="148"/>
-      <c r="AA37" s="148"/>
-      <c r="AB37" s="148"/>
+      <c r="W37" s="153"/>
+      <c r="X37" s="153"/>
+      <c r="Y37" s="153"/>
+      <c r="Z37" s="153"/>
+      <c r="AA37" s="153"/>
+      <c r="AB37" s="153"/>
       <c r="AD37" s="3" t="s">
         <v>259</v>
       </c>
@@ -6536,15 +6669,15 @@
       <c r="S42" s="12"/>
       <c r="T42" s="12"/>
       <c r="U42" s="12"/>
-      <c r="V42" s="148" t="s">
+      <c r="V42" s="153" t="s">
         <v>247</v>
       </c>
-      <c r="W42" s="148"/>
-      <c r="X42" s="148"/>
-      <c r="Y42" s="148"/>
-      <c r="Z42" s="148"/>
-      <c r="AA42" s="148"/>
-      <c r="AB42" s="148"/>
+      <c r="W42" s="153"/>
+      <c r="X42" s="153"/>
+      <c r="Y42" s="153"/>
+      <c r="Z42" s="153"/>
+      <c r="AA42" s="153"/>
+      <c r="AB42" s="153"/>
       <c r="AD42" s="3" t="s">
         <v>265</v>
       </c>
@@ -6649,15 +6782,15 @@
       <c r="S48" s="12"/>
       <c r="T48" s="12"/>
       <c r="U48" s="12"/>
-      <c r="V48" s="149" t="s">
+      <c r="V48" s="154" t="s">
         <v>480</v>
       </c>
-      <c r="W48" s="150"/>
-      <c r="X48" s="150"/>
-      <c r="Y48" s="150"/>
-      <c r="Z48" s="150"/>
-      <c r="AA48" s="150"/>
-      <c r="AB48" s="151"/>
+      <c r="W48" s="155"/>
+      <c r="X48" s="155"/>
+      <c r="Y48" s="155"/>
+      <c r="Z48" s="155"/>
+      <c r="AA48" s="155"/>
+      <c r="AB48" s="156"/>
     </row>
     <row r="49" spans="19:28">
       <c r="S49" s="12"/>
@@ -6765,12 +6898,644 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="20" max="20" width="19.7109375" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="161" t="s">
+        <v>495</v>
+      </c>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
+      <c r="H1" s="163"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A2" s="164"/>
+      <c r="B2" s="165"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="166"/>
+    </row>
+    <row r="3" spans="1:8" ht="19.5" customHeight="1">
+      <c r="A3" s="167" t="s">
+        <v>323</v>
+      </c>
+      <c r="B3" s="168"/>
+      <c r="C3" s="168"/>
+      <c r="D3" s="168"/>
+      <c r="E3" s="168" t="s">
+        <v>322</v>
+      </c>
+      <c r="F3" s="168"/>
+      <c r="G3" s="168"/>
+      <c r="H3" s="169"/>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A4" s="20">
+        <v>1</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="E4" s="21">
+        <v>1</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="22" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A5" s="20">
+        <v>2</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="21">
+        <v>2</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="22"/>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A6" s="20">
+        <v>3</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="21">
+        <v>3</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="22"/>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A7" s="20">
+        <v>4</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="21">
+        <v>4</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="22"/>
+    </row>
+    <row r="8" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A8" s="20">
+        <v>5</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="21">
+        <v>5</v>
+      </c>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="22"/>
+    </row>
+    <row r="9" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A9" s="20">
+        <v>6</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="21">
+        <v>6</v>
+      </c>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="22"/>
+    </row>
+    <row r="10" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A10" s="20">
+        <v>7</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="21">
+        <v>7</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="22"/>
+    </row>
+    <row r="11" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A11" s="20">
+        <v>8</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="21">
+        <v>8</v>
+      </c>
+      <c r="F11" s="22"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="22"/>
+    </row>
+    <row r="12" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A12" s="20">
+        <v>9</v>
+      </c>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="21">
+        <v>9</v>
+      </c>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="22"/>
+    </row>
+    <row r="13" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A13" s="20">
+        <v>10</v>
+      </c>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="21">
+        <v>10</v>
+      </c>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="22"/>
+    </row>
+    <row r="14" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A14" s="20">
+        <v>11</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="21">
+        <v>11</v>
+      </c>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="22"/>
+    </row>
+    <row r="15" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A15" s="20">
+        <v>12</v>
+      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="21">
+        <v>12</v>
+      </c>
+      <c r="F15" s="22"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="22"/>
+    </row>
+    <row r="16" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A16" s="20">
+        <v>13</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="21">
+        <v>13</v>
+      </c>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="22"/>
+    </row>
+    <row r="17" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A17" s="20">
+        <v>14</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="21">
+        <v>14</v>
+      </c>
+      <c r="F17" s="22"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="22"/>
+    </row>
+    <row r="18" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A18" s="20">
+        <v>15</v>
+      </c>
+      <c r="B18" s="22"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="21">
+        <v>15</v>
+      </c>
+      <c r="F18" s="22"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="22"/>
+    </row>
+    <row r="19" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A19" s="20">
+        <v>16</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="21">
+        <v>16</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="22"/>
+    </row>
+    <row r="20" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A20" s="20">
+        <v>17</v>
+      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="21">
+        <v>17</v>
+      </c>
+      <c r="F20" s="22"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="22"/>
+    </row>
+    <row r="21" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A21" s="20">
+        <v>18</v>
+      </c>
+      <c r="B21" s="22"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="21">
+        <v>18</v>
+      </c>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="22"/>
+    </row>
+    <row r="22" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A22" s="20">
+        <v>19</v>
+      </c>
+      <c r="B22" s="22"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="21">
+        <v>19</v>
+      </c>
+      <c r="F22" s="22"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="22"/>
+    </row>
+    <row r="23" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A23" s="20">
+        <v>20</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="108">
+        <v>20</v>
+      </c>
+      <c r="F23" s="111"/>
+      <c r="G23" s="112"/>
+      <c r="H23" s="111"/>
+    </row>
+    <row r="24" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="110">
+        <v>21</v>
+      </c>
+      <c r="F24" s="109"/>
+      <c r="G24" s="113"/>
+      <c r="H24" s="109"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="110">
+        <v>22</v>
+      </c>
+      <c r="F25" s="109"/>
+      <c r="G25" s="113"/>
+      <c r="H25" s="109"/>
+    </row>
+    <row r="26" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A26" s="24"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="110">
+        <v>23</v>
+      </c>
+      <c r="F26" s="109"/>
+      <c r="G26" s="113"/>
+      <c r="H26" s="109"/>
+    </row>
+    <row r="27" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A27" s="24"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="110">
+        <v>24</v>
+      </c>
+      <c r="F27" s="109"/>
+      <c r="G27" s="113"/>
+      <c r="H27" s="109"/>
+    </row>
+    <row r="28" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A28" s="24"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="110">
+        <v>25</v>
+      </c>
+      <c r="F28" s="109"/>
+      <c r="G28" s="113"/>
+      <c r="H28" s="109"/>
+    </row>
+    <row r="29" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A29" s="24"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="110">
+        <v>26</v>
+      </c>
+      <c r="F29" s="109"/>
+      <c r="G29" s="113"/>
+      <c r="H29" s="109"/>
+    </row>
+    <row r="30" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A30" s="24"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="110">
+        <v>27</v>
+      </c>
+      <c r="F30" s="109"/>
+      <c r="G30" s="113"/>
+      <c r="H30" s="109"/>
+    </row>
+    <row r="31" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A31" s="24"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="110">
+        <v>28</v>
+      </c>
+      <c r="F31" s="109"/>
+      <c r="G31" s="113"/>
+      <c r="H31" s="109"/>
+    </row>
+    <row r="32" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A32" s="24"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="110">
+        <v>29</v>
+      </c>
+      <c r="F32" s="109"/>
+      <c r="G32" s="113"/>
+      <c r="H32" s="109"/>
+    </row>
+    <row r="33" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A33" s="24"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="110">
+        <v>30</v>
+      </c>
+      <c r="F33" s="109"/>
+      <c r="G33" s="113"/>
+      <c r="H33" s="109"/>
+    </row>
+    <row r="34" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A34" s="24"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="110">
+        <v>31</v>
+      </c>
+      <c r="F34" s="109"/>
+      <c r="G34" s="113"/>
+      <c r="H34" s="109"/>
+    </row>
+    <row r="35" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A35" s="24"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="110">
+        <v>32</v>
+      </c>
+      <c r="F35" s="109"/>
+      <c r="G35" s="113"/>
+      <c r="H35" s="109"/>
+    </row>
+    <row r="36" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A36" s="24"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="110">
+        <v>33</v>
+      </c>
+      <c r="F36" s="109"/>
+      <c r="G36" s="113"/>
+      <c r="H36" s="109"/>
+    </row>
+    <row r="37" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A37" s="24"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="110">
+        <v>34</v>
+      </c>
+      <c r="F37" s="109"/>
+      <c r="G37" s="113"/>
+      <c r="H37" s="109"/>
+    </row>
+    <row r="38" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A38" s="24"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="110">
+        <v>35</v>
+      </c>
+      <c r="F38" s="109"/>
+      <c r="G38" s="113"/>
+      <c r="H38" s="109"/>
+    </row>
+    <row r="39" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A39" s="24"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="110">
+        <v>36</v>
+      </c>
+      <c r="F39" s="109"/>
+      <c r="G39" s="113"/>
+      <c r="H39" s="109"/>
+    </row>
+    <row r="40" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A40" s="24"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="110">
+        <v>37</v>
+      </c>
+      <c r="F40" s="109"/>
+      <c r="G40" s="113"/>
+      <c r="H40" s="109"/>
+    </row>
+    <row r="41" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A41" s="24"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="110">
+        <v>38</v>
+      </c>
+      <c r="F41" s="109"/>
+      <c r="G41" s="113"/>
+      <c r="H41" s="109"/>
+    </row>
+    <row r="42" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A42" s="24"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="20">
+        <v>39</v>
+      </c>
+      <c r="F42" s="22"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="22"/>
+    </row>
+    <row r="43" spans="1:8" ht="18.75" thickBot="1">
+      <c r="A43" s="24"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="110">
+        <v>40</v>
+      </c>
+      <c r="F43" s="109"/>
+      <c r="G43" s="113"/>
+      <c r="H43" s="109"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="24"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="26"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="24"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="26"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="24"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="26"/>
+    </row>
+    <row r="47" spans="1:8" ht="27.75" customHeight="1" thickBot="1">
+      <c r="A47" s="27"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+  </mergeCells>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AJ45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -6785,48 +7550,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:36">
-      <c r="B2" s="148" t="s">
+      <c r="B2" s="153" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
-      <c r="F2" s="148"/>
-      <c r="H2" s="148" t="s">
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="H2" s="153" t="s">
         <v>231</v>
       </c>
-      <c r="I2" s="148"/>
-      <c r="J2" s="148"/>
-      <c r="K2" s="148"/>
-      <c r="L2" s="148"/>
-      <c r="N2" s="148" t="s">
+      <c r="I2" s="153"/>
+      <c r="J2" s="153"/>
+      <c r="K2" s="153"/>
+      <c r="L2" s="153"/>
+      <c r="N2" s="153" t="s">
         <v>239</v>
       </c>
-      <c r="O2" s="148"/>
-      <c r="P2" s="148"/>
-      <c r="Q2" s="148"/>
-      <c r="R2" s="148"/>
-      <c r="T2" s="148" t="s">
+      <c r="O2" s="153"/>
+      <c r="P2" s="153"/>
+      <c r="Q2" s="153"/>
+      <c r="R2" s="153"/>
+      <c r="T2" s="153" t="s">
         <v>249</v>
       </c>
-      <c r="U2" s="148"/>
-      <c r="V2" s="148"/>
-      <c r="W2" s="148"/>
-      <c r="X2" s="148"/>
-      <c r="Z2" s="148" t="s">
+      <c r="U2" s="153"/>
+      <c r="V2" s="153"/>
+      <c r="W2" s="153"/>
+      <c r="X2" s="153"/>
+      <c r="Z2" s="153" t="s">
         <v>321</v>
       </c>
-      <c r="AA2" s="148"/>
-      <c r="AB2" s="148"/>
-      <c r="AC2" s="148"/>
-      <c r="AD2" s="148"/>
-      <c r="AF2" s="148" t="s">
+      <c r="AA2" s="153"/>
+      <c r="AB2" s="153"/>
+      <c r="AC2" s="153"/>
+      <c r="AD2" s="153"/>
+      <c r="AF2" s="153" t="s">
         <v>498</v>
       </c>
-      <c r="AG2" s="148"/>
-      <c r="AH2" s="148"/>
-      <c r="AI2" s="148"/>
-      <c r="AJ2" s="148"/>
+      <c r="AG2" s="153"/>
+      <c r="AH2" s="153"/>
+      <c r="AI2" s="153"/>
+      <c r="AJ2" s="153"/>
     </row>
     <row r="3" spans="2:36">
       <c r="B3" s="124" t="s">
@@ -7252,13 +8017,13 @@
       <c r="F24" s="140"/>
     </row>
     <row r="25" spans="2:20">
-      <c r="B25" s="148" t="s">
+      <c r="B25" s="153" t="s">
         <v>754</v>
       </c>
-      <c r="C25" s="148"/>
-      <c r="D25" s="148"/>
-      <c r="E25" s="148"/>
-      <c r="F25" s="148"/>
+      <c r="C25" s="153"/>
+      <c r="D25" s="153"/>
+      <c r="E25" s="153"/>
+      <c r="F25" s="153"/>
     </row>
     <row r="26" spans="2:20">
       <c r="B26" s="124" t="s">
@@ -7473,52 +8238,52 @@
       <c r="C42" s="3" t="s">
         <v>756</v>
       </c>
-      <c r="D42" s="214">
+      <c r="D42" s="147">
         <v>941</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>760</v>
       </c>
-      <c r="F42" s="215">
+      <c r="F42" s="148">
         <v>11341</v>
       </c>
     </row>
     <row r="43" spans="2:6">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="214">
+      <c r="D43" s="147">
         <v>942</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>757</v>
       </c>
-      <c r="F43" s="215">
+      <c r="F43" s="148">
         <v>11342</v>
       </c>
     </row>
     <row r="44" spans="2:6">
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="214">
+      <c r="D44" s="147">
         <v>943</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>758</v>
       </c>
-      <c r="F44" s="215">
+      <c r="F44" s="148">
         <v>11343</v>
       </c>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
-      <c r="D45" s="214">
+      <c r="D45" s="147">
         <v>945</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>759</v>
       </c>
-      <c r="F45" s="215">
+      <c r="F45" s="148">
         <v>11344</v>
       </c>
     </row>
@@ -7542,6 +8307,762 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:X46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" style="74" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="12" max="12" width="1.7109375" customWidth="1"/>
+    <col min="18" max="18" width="1.5703125" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="1.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A1" s="245" t="s">
+        <v>762</v>
+      </c>
+      <c r="B1" s="246"/>
+      <c r="C1" s="247"/>
+      <c r="D1" s="220"/>
+      <c r="E1" s="220"/>
+      <c r="F1" s="220"/>
+      <c r="G1" s="220"/>
+      <c r="H1" s="220"/>
+      <c r="I1" s="220"/>
+      <c r="J1" s="149"/>
+    </row>
+    <row r="2" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A2" s="234" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="234" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" s="235" t="s">
+        <v>325</v>
+      </c>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
+      <c r="F2" s="219"/>
+      <c r="G2" s="219"/>
+      <c r="H2" s="219"/>
+      <c r="I2" s="219"/>
+      <c r="J2" s="150"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75">
+      <c r="A3" s="248" t="s">
+        <v>329</v>
+      </c>
+      <c r="B3" s="229" t="s">
+        <v>324</v>
+      </c>
+      <c r="C3" s="230" t="s">
+        <v>677</v>
+      </c>
+      <c r="D3" s="219"/>
+      <c r="E3" s="219"/>
+      <c r="F3" s="219"/>
+      <c r="G3" s="219"/>
+      <c r="H3" s="219"/>
+      <c r="I3" s="219"/>
+      <c r="J3" s="150"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.75">
+      <c r="A4" s="249"/>
+      <c r="B4" s="228" t="s">
+        <v>326</v>
+      </c>
+      <c r="C4" s="231" t="s">
+        <v>678</v>
+      </c>
+      <c r="D4" s="219"/>
+      <c r="E4" s="219"/>
+      <c r="F4" s="219"/>
+      <c r="G4" s="219"/>
+      <c r="H4" s="219"/>
+      <c r="I4" s="219"/>
+      <c r="J4" s="150"/>
+    </row>
+    <row r="5" spans="1:10" ht="18.75">
+      <c r="A5" s="249"/>
+      <c r="B5" s="228" t="s">
+        <v>327</v>
+      </c>
+      <c r="C5" s="231" t="s">
+        <v>679</v>
+      </c>
+      <c r="D5" s="219"/>
+      <c r="E5" s="219"/>
+      <c r="F5" s="219"/>
+      <c r="G5" s="219"/>
+      <c r="H5" s="219"/>
+      <c r="I5" s="219"/>
+      <c r="J5" s="150"/>
+    </row>
+    <row r="6" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A6" s="250"/>
+      <c r="B6" s="232" t="s">
+        <v>328</v>
+      </c>
+      <c r="C6" s="233" t="s">
+        <v>680</v>
+      </c>
+      <c r="D6" s="219"/>
+      <c r="E6" s="219"/>
+      <c r="F6" s="219"/>
+      <c r="G6" s="219"/>
+      <c r="H6" s="219"/>
+      <c r="I6" s="219"/>
+      <c r="J6" s="150"/>
+    </row>
+    <row r="7" spans="1:10" ht="18.75">
+      <c r="A7" s="248" t="s">
+        <v>715</v>
+      </c>
+      <c r="B7" s="229" t="s">
+        <v>685</v>
+      </c>
+      <c r="C7" s="230" t="s">
+        <v>692</v>
+      </c>
+      <c r="D7" s="219"/>
+      <c r="E7" s="219"/>
+      <c r="F7" s="219"/>
+      <c r="G7" s="219"/>
+      <c r="H7" s="219"/>
+      <c r="I7" s="219"/>
+      <c r="J7" s="150"/>
+    </row>
+    <row r="8" spans="1:10" ht="18.75">
+      <c r="A8" s="249"/>
+      <c r="B8" s="228" t="s">
+        <v>686</v>
+      </c>
+      <c r="C8" s="231" t="s">
+        <v>689</v>
+      </c>
+      <c r="D8" s="219"/>
+      <c r="E8" s="219"/>
+      <c r="F8" s="219"/>
+      <c r="G8" s="219"/>
+      <c r="H8" s="219"/>
+      <c r="I8" s="219"/>
+      <c r="J8" s="150"/>
+    </row>
+    <row r="9" spans="1:10" ht="18.75">
+      <c r="A9" s="249"/>
+      <c r="B9" s="228" t="s">
+        <v>687</v>
+      </c>
+      <c r="C9" s="231" t="s">
+        <v>690</v>
+      </c>
+      <c r="D9" s="219"/>
+      <c r="E9" s="219"/>
+      <c r="F9" s="219"/>
+      <c r="G9" s="219"/>
+      <c r="H9" s="219"/>
+      <c r="I9" s="219"/>
+      <c r="J9" s="150"/>
+    </row>
+    <row r="10" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A10" s="250"/>
+      <c r="B10" s="232" t="s">
+        <v>688</v>
+      </c>
+      <c r="C10" s="233" t="s">
+        <v>691</v>
+      </c>
+      <c r="D10" s="219"/>
+      <c r="E10" s="219"/>
+      <c r="F10" s="219"/>
+      <c r="G10" s="219"/>
+      <c r="H10" s="219"/>
+      <c r="I10" s="219"/>
+      <c r="J10" s="150"/>
+    </row>
+    <row r="11" spans="1:10" ht="18.75">
+      <c r="A11" s="248" t="s">
+        <v>713</v>
+      </c>
+      <c r="B11" s="229" t="s">
+        <v>697</v>
+      </c>
+      <c r="C11" s="230" t="s">
+        <v>701</v>
+      </c>
+      <c r="D11" s="219"/>
+      <c r="E11" s="219"/>
+      <c r="F11" s="219"/>
+      <c r="G11" s="219"/>
+      <c r="H11" s="219"/>
+      <c r="I11" s="219"/>
+      <c r="J11" s="150"/>
+    </row>
+    <row r="12" spans="1:10" ht="18.75">
+      <c r="A12" s="249"/>
+      <c r="B12" s="228" t="s">
+        <v>698</v>
+      </c>
+      <c r="C12" s="231" t="s">
+        <v>702</v>
+      </c>
+      <c r="D12" s="219"/>
+      <c r="E12" s="219"/>
+      <c r="F12" s="219"/>
+      <c r="G12" s="219"/>
+      <c r="H12" s="219"/>
+      <c r="I12" s="219"/>
+      <c r="J12" s="150"/>
+    </row>
+    <row r="13" spans="1:10" ht="18.75">
+      <c r="A13" s="249"/>
+      <c r="B13" s="228" t="s">
+        <v>699</v>
+      </c>
+      <c r="C13" s="231" t="s">
+        <v>703</v>
+      </c>
+      <c r="D13" s="219"/>
+      <c r="E13" s="219"/>
+      <c r="F13" s="219"/>
+      <c r="G13" s="219"/>
+      <c r="H13" s="219"/>
+      <c r="I13" s="219"/>
+      <c r="J13" s="150"/>
+    </row>
+    <row r="14" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A14" s="250"/>
+      <c r="B14" s="232" t="s">
+        <v>700</v>
+      </c>
+      <c r="C14" s="233" t="s">
+        <v>704</v>
+      </c>
+      <c r="D14" s="219"/>
+      <c r="E14" s="219"/>
+      <c r="F14" s="219"/>
+      <c r="G14" s="219"/>
+      <c r="H14" s="219"/>
+      <c r="I14" s="219"/>
+      <c r="J14" s="150"/>
+    </row>
+    <row r="15" spans="1:10" ht="18.75">
+      <c r="A15" s="248" t="s">
+        <v>714</v>
+      </c>
+      <c r="B15" s="229" t="s">
+        <v>716</v>
+      </c>
+      <c r="C15" s="230" t="s">
+        <v>709</v>
+      </c>
+      <c r="D15" s="219"/>
+      <c r="E15" s="219"/>
+      <c r="F15" s="219"/>
+      <c r="G15" s="219"/>
+      <c r="H15" s="219"/>
+      <c r="I15" s="219"/>
+      <c r="J15" s="150"/>
+    </row>
+    <row r="16" spans="1:10" ht="18.75">
+      <c r="A16" s="249"/>
+      <c r="B16" s="228" t="s">
+        <v>717</v>
+      </c>
+      <c r="C16" s="231" t="s">
+        <v>710</v>
+      </c>
+      <c r="D16" s="219"/>
+      <c r="E16" s="219"/>
+      <c r="F16" s="219"/>
+      <c r="G16" s="219"/>
+      <c r="H16" s="219"/>
+      <c r="I16" s="219"/>
+      <c r="J16" s="150"/>
+    </row>
+    <row r="17" spans="1:10" ht="18.75">
+      <c r="A17" s="249"/>
+      <c r="B17" s="228" t="s">
+        <v>718</v>
+      </c>
+      <c r="C17" s="231" t="s">
+        <v>711</v>
+      </c>
+      <c r="D17" s="219"/>
+      <c r="E17" s="219"/>
+      <c r="F17" s="219"/>
+      <c r="G17" s="219"/>
+      <c r="H17" s="219"/>
+      <c r="I17" s="219"/>
+      <c r="J17" s="150"/>
+    </row>
+    <row r="18" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A18" s="250"/>
+      <c r="B18" s="232" t="s">
+        <v>719</v>
+      </c>
+      <c r="C18" s="233" t="s">
+        <v>712</v>
+      </c>
+      <c r="D18" s="219"/>
+      <c r="E18" s="219"/>
+      <c r="F18" s="219"/>
+      <c r="G18" s="219"/>
+      <c r="H18" s="219"/>
+      <c r="I18" s="219"/>
+      <c r="J18" s="150"/>
+    </row>
+    <row r="19" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A19" s="222"/>
+      <c r="B19" s="221"/>
+      <c r="C19" s="221"/>
+      <c r="D19" s="219"/>
+      <c r="E19" s="219"/>
+      <c r="F19" s="219"/>
+      <c r="G19" s="219"/>
+      <c r="H19" s="219"/>
+      <c r="I19" s="219"/>
+      <c r="J19" s="150"/>
+    </row>
+    <row r="20" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A20" s="236" t="s">
+        <v>761</v>
+      </c>
+      <c r="B20" s="237"/>
+      <c r="C20" s="238"/>
+      <c r="D20" s="219"/>
+      <c r="E20" s="219"/>
+      <c r="F20" s="219"/>
+      <c r="G20" s="219"/>
+      <c r="H20" s="219"/>
+      <c r="I20" s="219"/>
+      <c r="J20" s="150"/>
+    </row>
+    <row r="21" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A21" s="234" t="s">
+        <v>218</v>
+      </c>
+      <c r="B21" s="234" t="s">
+        <v>282</v>
+      </c>
+      <c r="C21" s="235" t="s">
+        <v>325</v>
+      </c>
+      <c r="D21" s="219"/>
+      <c r="E21" s="219"/>
+      <c r="F21" s="219"/>
+      <c r="G21" s="219"/>
+      <c r="H21" s="219"/>
+      <c r="I21" s="219"/>
+      <c r="J21" s="150"/>
+    </row>
+    <row r="22" spans="1:10" ht="18.75">
+      <c r="A22" s="239" t="s">
+        <v>507</v>
+      </c>
+      <c r="B22" s="229" t="s">
+        <v>723</v>
+      </c>
+      <c r="C22" s="230" t="s">
+        <v>724</v>
+      </c>
+      <c r="D22" s="219"/>
+      <c r="E22" s="223"/>
+      <c r="F22" s="219"/>
+      <c r="G22" s="219"/>
+      <c r="H22" s="219"/>
+      <c r="I22" s="219"/>
+      <c r="J22" s="150"/>
+    </row>
+    <row r="23" spans="1:10" ht="18.75">
+      <c r="A23" s="240"/>
+      <c r="B23" s="228" t="s">
+        <v>728</v>
+      </c>
+      <c r="C23" s="231" t="s">
+        <v>731</v>
+      </c>
+      <c r="D23" s="219"/>
+      <c r="E23" s="223"/>
+      <c r="F23" s="219"/>
+      <c r="G23" s="219"/>
+      <c r="H23" s="219"/>
+      <c r="I23" s="219"/>
+      <c r="J23" s="150"/>
+    </row>
+    <row r="24" spans="1:10" ht="18.75">
+      <c r="A24" s="240"/>
+      <c r="B24" s="228" t="s">
+        <v>729</v>
+      </c>
+      <c r="C24" s="231" t="s">
+        <v>732</v>
+      </c>
+      <c r="D24" s="219"/>
+      <c r="E24" s="219"/>
+      <c r="F24" s="219"/>
+      <c r="G24" s="219"/>
+      <c r="H24" s="219"/>
+      <c r="I24" s="219"/>
+      <c r="J24" s="150"/>
+    </row>
+    <row r="25" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A25" s="241"/>
+      <c r="B25" s="232" t="s">
+        <v>730</v>
+      </c>
+      <c r="C25" s="233" t="s">
+        <v>733</v>
+      </c>
+      <c r="D25" s="219"/>
+      <c r="E25" s="219"/>
+      <c r="F25" s="219"/>
+      <c r="G25" s="219"/>
+      <c r="H25" s="219"/>
+      <c r="I25" s="219"/>
+      <c r="J25" s="150"/>
+    </row>
+    <row r="26" spans="1:10" ht="18.75">
+      <c r="A26" s="239" t="s">
+        <v>740</v>
+      </c>
+      <c r="B26" s="229" t="s">
+        <v>735</v>
+      </c>
+      <c r="C26" s="230" t="s">
+        <v>739</v>
+      </c>
+      <c r="D26" s="219"/>
+      <c r="E26" s="219"/>
+      <c r="F26" s="219"/>
+      <c r="G26" s="219"/>
+      <c r="H26" s="219"/>
+      <c r="I26" s="219"/>
+      <c r="J26" s="150"/>
+    </row>
+    <row r="27" spans="1:10" ht="18.75">
+      <c r="A27" s="240"/>
+      <c r="B27" s="228" t="s">
+        <v>736</v>
+      </c>
+      <c r="C27" s="231">
+        <v>11322</v>
+      </c>
+      <c r="D27" s="219"/>
+      <c r="E27" s="219"/>
+      <c r="F27" s="219"/>
+      <c r="G27" s="219"/>
+      <c r="H27" s="219"/>
+      <c r="I27" s="219"/>
+      <c r="J27" s="150"/>
+    </row>
+    <row r="28" spans="1:10" ht="18.75">
+      <c r="A28" s="240"/>
+      <c r="B28" s="228" t="s">
+        <v>737</v>
+      </c>
+      <c r="C28" s="231">
+        <v>11323</v>
+      </c>
+      <c r="D28" s="219"/>
+      <c r="E28" s="219"/>
+      <c r="F28" s="219"/>
+      <c r="G28" s="219"/>
+      <c r="H28" s="219"/>
+      <c r="I28" s="219"/>
+      <c r="J28" s="150"/>
+    </row>
+    <row r="29" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A29" s="241"/>
+      <c r="B29" s="232" t="s">
+        <v>738</v>
+      </c>
+      <c r="C29" s="233">
+        <v>11324</v>
+      </c>
+      <c r="D29" s="219"/>
+      <c r="E29" s="219"/>
+      <c r="F29" s="219"/>
+      <c r="G29" s="219"/>
+      <c r="H29" s="219"/>
+      <c r="I29" s="219"/>
+      <c r="J29" s="150"/>
+    </row>
+    <row r="30" spans="1:10" ht="18.75">
+      <c r="A30" s="239" t="s">
+        <v>748</v>
+      </c>
+      <c r="B30" s="229" t="s">
+        <v>749</v>
+      </c>
+      <c r="C30" s="230" t="s">
+        <v>744</v>
+      </c>
+      <c r="D30" s="219"/>
+      <c r="E30" s="219"/>
+      <c r="F30" s="219"/>
+      <c r="G30" s="219"/>
+      <c r="H30" s="219"/>
+      <c r="I30" s="219"/>
+      <c r="J30" s="150"/>
+    </row>
+    <row r="31" spans="1:10" ht="18.75">
+      <c r="A31" s="240"/>
+      <c r="B31" s="228" t="s">
+        <v>750</v>
+      </c>
+      <c r="C31" s="231" t="s">
+        <v>745</v>
+      </c>
+      <c r="D31" s="219"/>
+      <c r="E31" s="219"/>
+      <c r="F31" s="219"/>
+      <c r="G31" s="219"/>
+      <c r="H31" s="219"/>
+      <c r="I31" s="219"/>
+      <c r="J31" s="150"/>
+    </row>
+    <row r="32" spans="1:10" ht="18.75">
+      <c r="A32" s="240"/>
+      <c r="B32" s="228" t="s">
+        <v>751</v>
+      </c>
+      <c r="C32" s="231" t="s">
+        <v>746</v>
+      </c>
+      <c r="D32" s="219"/>
+      <c r="E32" s="219"/>
+      <c r="F32" s="219"/>
+      <c r="G32" s="223"/>
+      <c r="H32" s="219"/>
+      <c r="I32" s="219"/>
+      <c r="J32" s="150"/>
+    </row>
+    <row r="33" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A33" s="241"/>
+      <c r="B33" s="232" t="s">
+        <v>752</v>
+      </c>
+      <c r="C33" s="233" t="s">
+        <v>747</v>
+      </c>
+      <c r="D33" s="219"/>
+      <c r="E33" s="219"/>
+      <c r="F33" s="219"/>
+      <c r="G33" s="223"/>
+      <c r="H33" s="219"/>
+      <c r="I33" s="219"/>
+      <c r="J33" s="150"/>
+    </row>
+    <row r="34" spans="1:10" ht="18.75">
+      <c r="A34" s="239" t="s">
+        <v>755</v>
+      </c>
+      <c r="B34" s="229" t="s">
+        <v>760</v>
+      </c>
+      <c r="C34" s="242">
+        <v>11341</v>
+      </c>
+      <c r="D34" s="219"/>
+      <c r="E34" s="219"/>
+      <c r="F34" s="219"/>
+      <c r="G34" s="223"/>
+      <c r="H34" s="219"/>
+      <c r="I34" s="219"/>
+      <c r="J34" s="150"/>
+    </row>
+    <row r="35" spans="1:10" ht="18.75">
+      <c r="A35" s="240"/>
+      <c r="B35" s="228" t="s">
+        <v>757</v>
+      </c>
+      <c r="C35" s="243">
+        <v>11342</v>
+      </c>
+      <c r="D35" s="219"/>
+      <c r="E35" s="219"/>
+      <c r="F35" s="219"/>
+      <c r="G35" s="223"/>
+      <c r="H35" s="219"/>
+      <c r="I35" s="219"/>
+      <c r="J35" s="150"/>
+    </row>
+    <row r="36" spans="1:10" ht="18.75">
+      <c r="A36" s="240"/>
+      <c r="B36" s="228" t="s">
+        <v>758</v>
+      </c>
+      <c r="C36" s="243">
+        <v>11343</v>
+      </c>
+      <c r="D36" s="219"/>
+      <c r="E36" s="219"/>
+      <c r="F36" s="219"/>
+      <c r="G36" s="223"/>
+      <c r="H36" s="219"/>
+      <c r="I36" s="219"/>
+      <c r="J36" s="150"/>
+    </row>
+    <row r="37" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A37" s="241"/>
+      <c r="B37" s="232" t="s">
+        <v>759</v>
+      </c>
+      <c r="C37" s="244">
+        <v>11344</v>
+      </c>
+      <c r="D37" s="219"/>
+      <c r="E37" s="219"/>
+      <c r="F37" s="219"/>
+      <c r="G37" s="223"/>
+      <c r="H37" s="219"/>
+      <c r="I37" s="219"/>
+      <c r="J37" s="150"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="224"/>
+      <c r="B38" s="219"/>
+      <c r="C38" s="219"/>
+      <c r="D38" s="219"/>
+      <c r="E38" s="219"/>
+      <c r="F38" s="219"/>
+      <c r="G38" s="223"/>
+      <c r="H38" s="219"/>
+      <c r="I38" s="219"/>
+      <c r="J38" s="150"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="224"/>
+      <c r="B39" s="219"/>
+      <c r="C39" s="219"/>
+      <c r="D39" s="219"/>
+      <c r="E39" s="219"/>
+      <c r="F39" s="219"/>
+      <c r="G39" s="223"/>
+      <c r="H39" s="219"/>
+      <c r="I39" s="219"/>
+      <c r="J39" s="150"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="224"/>
+      <c r="B40" s="219"/>
+      <c r="C40" s="219"/>
+      <c r="D40" s="219"/>
+      <c r="E40" s="219"/>
+      <c r="F40" s="219"/>
+      <c r="G40" s="223"/>
+      <c r="H40" s="219"/>
+      <c r="I40" s="219"/>
+      <c r="J40" s="150"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="224"/>
+      <c r="B41" s="219"/>
+      <c r="C41" s="219"/>
+      <c r="D41" s="219"/>
+      <c r="E41" s="219"/>
+      <c r="F41" s="219"/>
+      <c r="G41" s="223"/>
+      <c r="H41" s="219"/>
+      <c r="I41" s="219"/>
+      <c r="J41" s="150"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="224"/>
+      <c r="B42" s="219"/>
+      <c r="C42" s="219"/>
+      <c r="D42" s="219"/>
+      <c r="E42" s="219"/>
+      <c r="F42" s="219"/>
+      <c r="G42" s="223"/>
+      <c r="H42" s="219"/>
+      <c r="I42" s="219"/>
+      <c r="J42" s="150"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="224"/>
+      <c r="B43" s="219"/>
+      <c r="C43" s="219"/>
+      <c r="D43" s="219"/>
+      <c r="E43" s="219"/>
+      <c r="F43" s="219"/>
+      <c r="G43" s="223"/>
+      <c r="H43" s="219"/>
+      <c r="I43" s="219"/>
+      <c r="J43" s="150"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="224"/>
+      <c r="B44" s="219"/>
+      <c r="C44" s="219"/>
+      <c r="D44" s="219"/>
+      <c r="E44" s="219"/>
+      <c r="F44" s="219"/>
+      <c r="G44" s="223"/>
+      <c r="H44" s="219"/>
+      <c r="I44" s="219"/>
+      <c r="J44" s="150"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="224"/>
+      <c r="B45" s="219"/>
+      <c r="C45" s="219"/>
+      <c r="D45" s="219"/>
+      <c r="E45" s="219"/>
+      <c r="F45" s="219"/>
+      <c r="G45" s="219"/>
+      <c r="H45" s="219"/>
+      <c r="I45" s="223"/>
+      <c r="J45" s="150"/>
+    </row>
+    <row r="46" spans="1:10" ht="46.5" customHeight="1" thickBot="1">
+      <c r="A46" s="225"/>
+      <c r="B46" s="226"/>
+      <c r="C46" s="226"/>
+      <c r="D46" s="226"/>
+      <c r="E46" s="226"/>
+      <c r="F46" s="226"/>
+      <c r="G46" s="226"/>
+      <c r="H46" s="226"/>
+      <c r="I46" s="227"/>
+      <c r="J46" s="151"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+  </mergeCells>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C3:C6 C7:C10 C11:C14 C15:C19 C26:C29 C30:C33 C34:C36 C21:C25" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -7561,40 +9082,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="161" t="s">
         <v>330</v>
       </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157"/>
-      <c r="F1" s="157"/>
-      <c r="G1" s="157"/>
-      <c r="H1" s="158"/>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
+      <c r="H1" s="163"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="159"/>
-      <c r="B2" s="160"/>
-      <c r="C2" s="160"/>
-      <c r="D2" s="160"/>
-      <c r="E2" s="160"/>
-      <c r="F2" s="160"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="161"/>
+      <c r="A2" s="164"/>
+      <c r="B2" s="165"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="166"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="162" t="s">
+      <c r="A3" s="167" t="s">
         <v>253</v>
       </c>
-      <c r="B3" s="163"/>
-      <c r="C3" s="163"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163" t="s">
+      <c r="B3" s="168"/>
+      <c r="C3" s="168"/>
+      <c r="D3" s="168"/>
+      <c r="E3" s="168" t="s">
         <v>254</v>
       </c>
-      <c r="F3" s="163"/>
-      <c r="G3" s="163"/>
-      <c r="H3" s="164"/>
+      <c r="F3" s="168"/>
+      <c r="G3" s="168"/>
+      <c r="H3" s="169"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="20">
@@ -8128,11 +9649,11 @@
       <c r="C27" s="144" t="s">
         <v>609</v>
       </c>
-      <c r="D27" s="155" t="s">
+      <c r="D27" s="160" t="s">
         <v>585</v>
       </c>
-      <c r="E27" s="155"/>
-      <c r="F27" s="155"/>
+      <c r="E27" s="160"/>
+      <c r="F27" s="160"/>
       <c r="G27" s="25"/>
       <c r="H27" s="26"/>
     </row>
@@ -8144,11 +9665,11 @@
       <c r="C28" s="144" t="s">
         <v>613</v>
       </c>
-      <c r="D28" s="155" t="s">
+      <c r="D28" s="160" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="155"/>
-      <c r="F28" s="155"/>
+      <c r="E28" s="160"/>
+      <c r="F28" s="160"/>
       <c r="G28" s="25"/>
       <c r="H28" s="26"/>
     </row>
@@ -8160,11 +9681,11 @@
       <c r="C29" s="144" t="s">
         <v>614</v>
       </c>
-      <c r="D29" s="155" t="s">
+      <c r="D29" s="160" t="s">
         <v>586</v>
       </c>
-      <c r="E29" s="155"/>
-      <c r="F29" s="155"/>
+      <c r="E29" s="160"/>
+      <c r="F29" s="160"/>
       <c r="G29" s="25"/>
       <c r="H29" s="26"/>
     </row>
@@ -8176,11 +9697,11 @@
       <c r="C30" s="144" t="s">
         <v>615</v>
       </c>
-      <c r="D30" s="155" t="s">
+      <c r="D30" s="160" t="s">
         <v>587</v>
       </c>
-      <c r="E30" s="155"/>
-      <c r="F30" s="155"/>
+      <c r="E30" s="160"/>
+      <c r="F30" s="160"/>
       <c r="G30" s="25"/>
       <c r="H30" s="26"/>
     </row>
@@ -8192,11 +9713,11 @@
       <c r="C31" s="144" t="s">
         <v>616</v>
       </c>
-      <c r="D31" s="155" t="s">
+      <c r="D31" s="160" t="s">
         <v>588</v>
       </c>
-      <c r="E31" s="155"/>
-      <c r="F31" s="155"/>
+      <c r="E31" s="160"/>
+      <c r="F31" s="160"/>
       <c r="G31" s="25"/>
       <c r="H31" s="26"/>
     </row>
@@ -8208,11 +9729,11 @@
       <c r="C32" s="144" t="s">
         <v>617</v>
       </c>
-      <c r="D32" s="155" t="s">
+      <c r="D32" s="160" t="s">
         <v>589</v>
       </c>
-      <c r="E32" s="155"/>
-      <c r="F32" s="155"/>
+      <c r="E32" s="160"/>
+      <c r="F32" s="160"/>
       <c r="G32" s="25"/>
       <c r="H32" s="26"/>
     </row>
@@ -8224,11 +9745,11 @@
       <c r="C33" s="144" t="s">
         <v>630</v>
       </c>
-      <c r="D33" s="155" t="s">
+      <c r="D33" s="160" t="s">
         <v>489</v>
       </c>
-      <c r="E33" s="155"/>
-      <c r="F33" s="155"/>
+      <c r="E33" s="160"/>
+      <c r="F33" s="160"/>
       <c r="G33" s="25"/>
       <c r="H33" s="26"/>
     </row>
@@ -8240,11 +9761,11 @@
       <c r="C34" s="144" t="s">
         <v>631</v>
       </c>
-      <c r="D34" s="155" t="s">
+      <c r="D34" s="160" t="s">
         <v>590</v>
       </c>
-      <c r="E34" s="155"/>
-      <c r="F34" s="155"/>
+      <c r="E34" s="160"/>
+      <c r="F34" s="160"/>
       <c r="G34" s="25"/>
       <c r="H34" s="26"/>
     </row>
@@ -8256,11 +9777,11 @@
       <c r="C35" s="144" t="s">
         <v>632</v>
       </c>
-      <c r="D35" s="155" t="s">
+      <c r="D35" s="160" t="s">
         <v>591</v>
       </c>
-      <c r="E35" s="155"/>
-      <c r="F35" s="155"/>
+      <c r="E35" s="160"/>
+      <c r="F35" s="160"/>
       <c r="G35" s="25"/>
       <c r="H35" s="26"/>
     </row>
@@ -8270,11 +9791,11 @@
       <c r="C36" s="144" t="s">
         <v>667</v>
       </c>
-      <c r="D36" s="152" t="s">
+      <c r="D36" s="157" t="s">
         <v>606</v>
       </c>
-      <c r="E36" s="153"/>
-      <c r="F36" s="154"/>
+      <c r="E36" s="158"/>
+      <c r="F36" s="159"/>
       <c r="G36" s="25"/>
       <c r="H36" s="26"/>
     </row>
@@ -8284,11 +9805,11 @@
       <c r="C37" s="144" t="s">
         <v>670</v>
       </c>
-      <c r="D37" s="152" t="s">
+      <c r="D37" s="157" t="s">
         <v>668</v>
       </c>
-      <c r="E37" s="153"/>
-      <c r="F37" s="154"/>
+      <c r="E37" s="158"/>
+      <c r="F37" s="159"/>
       <c r="G37" s="25"/>
       <c r="H37" s="26"/>
     </row>
@@ -8298,11 +9819,11 @@
       <c r="C38" s="144" t="s">
         <v>669</v>
       </c>
-      <c r="D38" s="152" t="s">
+      <c r="D38" s="157" t="s">
         <v>671</v>
       </c>
-      <c r="E38" s="153"/>
-      <c r="F38" s="154"/>
+      <c r="E38" s="158"/>
+      <c r="F38" s="159"/>
       <c r="G38" s="25"/>
       <c r="H38" s="26"/>
     </row>
@@ -8310,9 +9831,9 @@
       <c r="A39" s="24"/>
       <c r="B39" s="146"/>
       <c r="C39" s="144"/>
-      <c r="D39" s="152"/>
-      <c r="E39" s="153"/>
-      <c r="F39" s="154"/>
+      <c r="D39" s="157"/>
+      <c r="E39" s="158"/>
+      <c r="F39" s="159"/>
       <c r="G39" s="25"/>
       <c r="H39" s="26"/>
     </row>
@@ -8432,7 +9953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K39"/>
   <sheetViews>
@@ -8449,28 +9970,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="168" t="s">
+      <c r="A1" s="173" t="s">
         <v>331</v>
       </c>
-      <c r="B1" s="168"/>
-      <c r="C1" s="168"/>
-      <c r="D1" s="168"/>
-      <c r="E1" s="168"/>
-      <c r="F1" s="168"/>
-      <c r="G1" s="168"/>
-      <c r="H1" s="168"/>
+      <c r="B1" s="173"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="173"/>
+      <c r="G1" s="173"/>
+      <c r="H1" s="173"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="165" t="s">
+      <c r="A2" s="170" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="166"/>
-      <c r="C2" s="166"/>
-      <c r="D2" s="166"/>
-      <c r="E2" s="166"/>
-      <c r="F2" s="166"/>
-      <c r="G2" s="166"/>
-      <c r="H2" s="167"/>
+      <c r="B2" s="171"/>
+      <c r="C2" s="171"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="171"/>
+      <c r="G2" s="171"/>
+      <c r="H2" s="172"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="5"/>
@@ -8649,16 +10170,16 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="165" t="s">
+      <c r="A15" s="170" t="s">
         <v>225</v>
       </c>
-      <c r="B15" s="166"/>
-      <c r="C15" s="166"/>
-      <c r="D15" s="166"/>
-      <c r="E15" s="166"/>
-      <c r="F15" s="166"/>
-      <c r="G15" s="166"/>
-      <c r="H15" s="167"/>
+      <c r="B15" s="171"/>
+      <c r="C15" s="171"/>
+      <c r="D15" s="171"/>
+      <c r="E15" s="171"/>
+      <c r="F15" s="171"/>
+      <c r="G15" s="171"/>
+      <c r="H15" s="172"/>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="9"/>
@@ -8834,16 +10355,16 @@
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:11" ht="15.75">
-      <c r="A28" s="165" t="s">
+      <c r="A28" s="170" t="s">
         <v>226</v>
       </c>
-      <c r="B28" s="166"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
-      <c r="H28" s="167"/>
+      <c r="B28" s="171"/>
+      <c r="C28" s="171"/>
+      <c r="D28" s="171"/>
+      <c r="E28" s="171"/>
+      <c r="F28" s="171"/>
+      <c r="G28" s="171"/>
+      <c r="H28" s="172"/>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="5"/>
@@ -9019,7 +10540,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H33"/>
   <sheetViews>
@@ -9043,40 +10564,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="174" t="s">
         <v>332</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="171"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
+      <c r="H1" s="176"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="172"/>
-      <c r="B2" s="173"/>
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="173"/>
-      <c r="G2" s="173"/>
-      <c r="H2" s="174"/>
+      <c r="A2" s="177"/>
+      <c r="B2" s="178"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="178"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="179"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="175" t="s">
+      <c r="A3" s="180" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="176"/>
-      <c r="C3" s="177"/>
-      <c r="D3" s="178"/>
-      <c r="E3" s="175" t="s">
+      <c r="B3" s="181"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="180" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="176"/>
-      <c r="G3" s="177"/>
-      <c r="H3" s="178"/>
+      <c r="F3" s="181"/>
+      <c r="G3" s="182"/>
+      <c r="H3" s="183"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="16">
@@ -9493,7 +11014,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H41"/>
   <sheetViews>
@@ -9515,40 +11036,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="196" t="s">
+      <c r="A1" s="201" t="s">
         <v>333</v>
       </c>
-      <c r="B1" s="196"/>
-      <c r="C1" s="196"/>
-      <c r="D1" s="196"/>
-      <c r="E1" s="196"/>
-      <c r="F1" s="196"/>
-      <c r="G1" s="196"/>
-      <c r="H1" s="196"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="197"/>
-      <c r="B2" s="197"/>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="197"/>
-      <c r="F2" s="197"/>
-      <c r="G2" s="197"/>
-      <c r="H2" s="197"/>
+      <c r="A2" s="202"/>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="202"/>
+      <c r="F2" s="202"/>
+      <c r="G2" s="202"/>
+      <c r="H2" s="202"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="198" t="s">
+      <c r="A3" s="203" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="199"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="201"/>
-      <c r="E3" s="198" t="s">
+      <c r="B3" s="204"/>
+      <c r="C3" s="205"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="203" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="199"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="201"/>
+      <c r="F3" s="204"/>
+      <c r="G3" s="205"/>
+      <c r="H3" s="206"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="46">
@@ -9841,114 +11362,114 @@
       <c r="H24" s="74"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="198" t="s">
+      <c r="A25" s="203" t="s">
         <v>293</v>
       </c>
-      <c r="B25" s="199"/>
-      <c r="C25" s="200"/>
-      <c r="D25" s="201"/>
-      <c r="E25" s="198" t="s">
+      <c r="B25" s="204"/>
+      <c r="C25" s="205"/>
+      <c r="D25" s="206"/>
+      <c r="E25" s="203" t="s">
         <v>294</v>
       </c>
-      <c r="F25" s="199"/>
-      <c r="G25" s="200"/>
-      <c r="H25" s="201"/>
+      <c r="F25" s="204"/>
+      <c r="G25" s="205"/>
+      <c r="H25" s="206"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="50" t="s">
         <v>295</v>
       </c>
-      <c r="B26" s="185"/>
-      <c r="C26" s="186"/>
-      <c r="D26" s="187"/>
+      <c r="B26" s="190"/>
+      <c r="C26" s="191"/>
+      <c r="D26" s="192"/>
       <c r="E26" s="46" t="s">
         <v>296</v>
       </c>
-      <c r="F26" s="193"/>
-      <c r="G26" s="194"/>
-      <c r="H26" s="195"/>
+      <c r="F26" s="198"/>
+      <c r="G26" s="199"/>
+      <c r="H26" s="200"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="B27" s="188"/>
-      <c r="C27" s="189"/>
-      <c r="D27" s="191"/>
+      <c r="B27" s="193"/>
+      <c r="C27" s="194"/>
+      <c r="D27" s="196"/>
       <c r="E27" s="50" t="s">
         <v>298</v>
       </c>
-      <c r="F27" s="185"/>
-      <c r="G27" s="186"/>
-      <c r="H27" s="192"/>
+      <c r="F27" s="190"/>
+      <c r="G27" s="191"/>
+      <c r="H27" s="197"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="50" t="s">
         <v>299</v>
       </c>
-      <c r="B28" s="185"/>
-      <c r="C28" s="186"/>
-      <c r="D28" s="187"/>
+      <c r="B28" s="190"/>
+      <c r="C28" s="191"/>
+      <c r="D28" s="192"/>
       <c r="E28" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="F28" s="188"/>
-      <c r="G28" s="189"/>
-      <c r="H28" s="190"/>
+      <c r="F28" s="193"/>
+      <c r="G28" s="194"/>
+      <c r="H28" s="195"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="58" t="s">
         <v>301</v>
       </c>
-      <c r="B29" s="188"/>
-      <c r="C29" s="189"/>
-      <c r="D29" s="191"/>
+      <c r="B29" s="193"/>
+      <c r="C29" s="194"/>
+      <c r="D29" s="196"/>
       <c r="E29" s="50" t="s">
         <v>302</v>
       </c>
-      <c r="F29" s="185"/>
-      <c r="G29" s="186"/>
-      <c r="H29" s="192"/>
+      <c r="F29" s="190"/>
+      <c r="G29" s="191"/>
+      <c r="H29" s="197"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="50" t="s">
         <v>303</v>
       </c>
-      <c r="B30" s="185"/>
-      <c r="C30" s="186"/>
-      <c r="D30" s="187"/>
+      <c r="B30" s="190"/>
+      <c r="C30" s="191"/>
+      <c r="D30" s="192"/>
       <c r="E30" s="58" t="s">
         <v>304</v>
       </c>
-      <c r="F30" s="188"/>
-      <c r="G30" s="189"/>
-      <c r="H30" s="190"/>
+      <c r="F30" s="193"/>
+      <c r="G30" s="194"/>
+      <c r="H30" s="195"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="B31" s="188"/>
-      <c r="C31" s="189"/>
-      <c r="D31" s="191"/>
+      <c r="B31" s="193"/>
+      <c r="C31" s="194"/>
+      <c r="D31" s="196"/>
       <c r="E31" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="F31" s="185"/>
-      <c r="G31" s="186"/>
-      <c r="H31" s="192"/>
+      <c r="F31" s="190"/>
+      <c r="G31" s="191"/>
+      <c r="H31" s="197"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="50" t="s">
         <v>307</v>
       </c>
-      <c r="B32" s="185"/>
-      <c r="C32" s="186"/>
-      <c r="D32" s="187"/>
+      <c r="B32" s="190"/>
+      <c r="C32" s="191"/>
+      <c r="D32" s="192"/>
       <c r="E32" s="58"/>
-      <c r="F32" s="188"/>
-      <c r="G32" s="189"/>
-      <c r="H32" s="190" t="s">
+      <c r="F32" s="193"/>
+      <c r="G32" s="194"/>
+      <c r="H32" s="195" t="s">
         <v>245</v>
       </c>
     </row>
@@ -9956,13 +11477,13 @@
       <c r="A33" s="58" t="s">
         <v>308</v>
       </c>
-      <c r="B33" s="188"/>
-      <c r="C33" s="189"/>
-      <c r="D33" s="191"/>
+      <c r="B33" s="193"/>
+      <c r="C33" s="194"/>
+      <c r="D33" s="196"/>
       <c r="E33" s="50"/>
-      <c r="F33" s="185"/>
-      <c r="G33" s="186"/>
-      <c r="H33" s="192" t="s">
+      <c r="F33" s="190"/>
+      <c r="G33" s="191"/>
+      <c r="H33" s="197" t="s">
         <v>288</v>
       </c>
     </row>
@@ -9970,13 +11491,13 @@
       <c r="A34" s="50" t="s">
         <v>309</v>
       </c>
-      <c r="B34" s="185"/>
-      <c r="C34" s="186"/>
-      <c r="D34" s="187"/>
+      <c r="B34" s="190"/>
+      <c r="C34" s="191"/>
+      <c r="D34" s="192"/>
       <c r="E34" s="58"/>
-      <c r="F34" s="188"/>
-      <c r="G34" s="189"/>
-      <c r="H34" s="190" t="s">
+      <c r="F34" s="193"/>
+      <c r="G34" s="194"/>
+      <c r="H34" s="195" t="s">
         <v>289</v>
       </c>
     </row>
@@ -9984,13 +11505,13 @@
       <c r="A35" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="B35" s="188"/>
-      <c r="C35" s="189"/>
-      <c r="D35" s="191"/>
+      <c r="B35" s="193"/>
+      <c r="C35" s="194"/>
+      <c r="D35" s="196"/>
       <c r="E35" s="50"/>
-      <c r="F35" s="185"/>
-      <c r="G35" s="186"/>
-      <c r="H35" s="192" t="s">
+      <c r="F35" s="190"/>
+      <c r="G35" s="191"/>
+      <c r="H35" s="197" t="s">
         <v>290</v>
       </c>
     </row>
@@ -9998,13 +11519,13 @@
       <c r="A36" s="50" t="s">
         <v>311</v>
       </c>
-      <c r="B36" s="185"/>
-      <c r="C36" s="186"/>
-      <c r="D36" s="187"/>
+      <c r="B36" s="190"/>
+      <c r="C36" s="191"/>
+      <c r="D36" s="192"/>
       <c r="E36" s="58"/>
-      <c r="F36" s="188"/>
-      <c r="G36" s="189"/>
-      <c r="H36" s="190" t="s">
+      <c r="F36" s="193"/>
+      <c r="G36" s="194"/>
+      <c r="H36" s="195" t="s">
         <v>291</v>
       </c>
     </row>
@@ -10012,13 +11533,13 @@
       <c r="A37" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="B37" s="188"/>
-      <c r="C37" s="189"/>
-      <c r="D37" s="191"/>
+      <c r="B37" s="193"/>
+      <c r="C37" s="194"/>
+      <c r="D37" s="196"/>
       <c r="E37" s="50"/>
-      <c r="F37" s="185"/>
-      <c r="G37" s="186"/>
-      <c r="H37" s="192" t="s">
+      <c r="F37" s="190"/>
+      <c r="G37" s="191"/>
+      <c r="H37" s="197" t="s">
         <v>292</v>
       </c>
     </row>
@@ -10026,13 +11547,13 @@
       <c r="A38" s="50" t="s">
         <v>313</v>
       </c>
-      <c r="B38" s="185"/>
-      <c r="C38" s="186"/>
-      <c r="D38" s="187"/>
+      <c r="B38" s="190"/>
+      <c r="C38" s="191"/>
+      <c r="D38" s="192"/>
       <c r="E38" s="58"/>
-      <c r="F38" s="188"/>
-      <c r="G38" s="189"/>
-      <c r="H38" s="190" t="s">
+      <c r="F38" s="193"/>
+      <c r="G38" s="194"/>
+      <c r="H38" s="195" t="s">
         <v>244</v>
       </c>
     </row>
@@ -10040,13 +11561,13 @@
       <c r="A39" s="58" t="s">
         <v>314</v>
       </c>
-      <c r="B39" s="188"/>
-      <c r="C39" s="189"/>
-      <c r="D39" s="191"/>
+      <c r="B39" s="193"/>
+      <c r="C39" s="194"/>
+      <c r="D39" s="196"/>
       <c r="E39" s="50"/>
-      <c r="F39" s="185"/>
-      <c r="G39" s="186"/>
-      <c r="H39" s="192" t="s">
+      <c r="F39" s="190"/>
+      <c r="G39" s="191"/>
+      <c r="H39" s="197" t="s">
         <v>245</v>
       </c>
     </row>
@@ -10054,25 +11575,25 @@
       <c r="A40" s="50" t="s">
         <v>315</v>
       </c>
-      <c r="B40" s="185"/>
-      <c r="C40" s="186"/>
-      <c r="D40" s="187"/>
+      <c r="B40" s="190"/>
+      <c r="C40" s="191"/>
+      <c r="D40" s="192"/>
       <c r="E40" s="58"/>
-      <c r="F40" s="188"/>
-      <c r="G40" s="189"/>
-      <c r="H40" s="190"/>
+      <c r="F40" s="193"/>
+      <c r="G40" s="194"/>
+      <c r="H40" s="195"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="70" t="s">
         <v>316</v>
       </c>
-      <c r="B41" s="179"/>
-      <c r="C41" s="180"/>
-      <c r="D41" s="181"/>
+      <c r="B41" s="184"/>
+      <c r="C41" s="185"/>
+      <c r="D41" s="186"/>
       <c r="E41" s="75"/>
-      <c r="F41" s="182"/>
-      <c r="G41" s="183"/>
-      <c r="H41" s="184"/>
+      <c r="F41" s="187"/>
+      <c r="G41" s="188"/>
+      <c r="H41" s="189"/>
     </row>
   </sheetData>
   <mergeCells count="37">
@@ -10119,7 +11640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H42"/>
   <sheetViews>
@@ -10141,40 +11662,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="208" t="s">
+      <c r="A1" s="213" t="s">
         <v>334</v>
       </c>
-      <c r="B1" s="209"/>
-      <c r="C1" s="209"/>
-      <c r="D1" s="209"/>
-      <c r="E1" s="209"/>
-      <c r="F1" s="209"/>
-      <c r="G1" s="209"/>
-      <c r="H1" s="210"/>
+      <c r="B1" s="214"/>
+      <c r="C1" s="214"/>
+      <c r="D1" s="214"/>
+      <c r="E1" s="214"/>
+      <c r="F1" s="214"/>
+      <c r="G1" s="214"/>
+      <c r="H1" s="215"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="211"/>
-      <c r="B2" s="212"/>
-      <c r="C2" s="212"/>
-      <c r="D2" s="212"/>
-      <c r="E2" s="212"/>
-      <c r="F2" s="212"/>
-      <c r="G2" s="212"/>
-      <c r="H2" s="213"/>
+      <c r="A2" s="216"/>
+      <c r="B2" s="217"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
+      <c r="G2" s="217"/>
+      <c r="H2" s="218"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="202" t="s">
+      <c r="A3" s="207" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="203"/>
-      <c r="C3" s="203"/>
-      <c r="D3" s="204"/>
-      <c r="E3" s="202" t="s">
+      <c r="B3" s="208"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="209"/>
+      <c r="E3" s="207" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="203"/>
-      <c r="G3" s="203"/>
-      <c r="H3" s="204"/>
+      <c r="F3" s="208"/>
+      <c r="G3" s="208"/>
+      <c r="H3" s="209"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="93">
@@ -10391,18 +11912,18 @@
       <c r="H21" s="85"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="205" t="s">
+      <c r="A22" s="210" t="s">
         <v>319</v>
       </c>
-      <c r="B22" s="206"/>
-      <c r="C22" s="206"/>
-      <c r="D22" s="207"/>
-      <c r="E22" s="205" t="s">
+      <c r="B22" s="211"/>
+      <c r="C22" s="211"/>
+      <c r="D22" s="212"/>
+      <c r="E22" s="210" t="s">
         <v>320</v>
       </c>
-      <c r="F22" s="206"/>
-      <c r="G22" s="206"/>
-      <c r="H22" s="207"/>
+      <c r="F22" s="211"/>
+      <c r="G22" s="211"/>
+      <c r="H22" s="212"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="78">
@@ -10657,7 +12178,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H42"/>
   <sheetViews>
@@ -10679,40 +12200,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="208" t="s">
+      <c r="A1" s="213" t="s">
         <v>494</v>
       </c>
-      <c r="B1" s="209"/>
-      <c r="C1" s="209"/>
-      <c r="D1" s="209"/>
-      <c r="E1" s="209"/>
-      <c r="F1" s="209"/>
-      <c r="G1" s="209"/>
-      <c r="H1" s="210"/>
+      <c r="B1" s="214"/>
+      <c r="C1" s="214"/>
+      <c r="D1" s="214"/>
+      <c r="E1" s="214"/>
+      <c r="F1" s="214"/>
+      <c r="G1" s="214"/>
+      <c r="H1" s="215"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="211"/>
-      <c r="B2" s="212"/>
-      <c r="C2" s="212"/>
-      <c r="D2" s="212"/>
-      <c r="E2" s="212"/>
-      <c r="F2" s="212"/>
-      <c r="G2" s="212"/>
-      <c r="H2" s="213"/>
+      <c r="A2" s="216"/>
+      <c r="B2" s="217"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
+      <c r="G2" s="217"/>
+      <c r="H2" s="218"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="202" t="s">
+      <c r="A3" s="207" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="203"/>
-      <c r="C3" s="203"/>
-      <c r="D3" s="204"/>
-      <c r="E3" s="202" t="s">
+      <c r="B3" s="208"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="209"/>
+      <c r="E3" s="207" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="203"/>
-      <c r="G3" s="203"/>
-      <c r="H3" s="204"/>
+      <c r="F3" s="208"/>
+      <c r="G3" s="208"/>
+      <c r="H3" s="209"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="93">
@@ -10929,18 +12450,18 @@
       <c r="H21" s="85"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="205" t="s">
+      <c r="A22" s="210" t="s">
         <v>319</v>
       </c>
-      <c r="B22" s="206"/>
-      <c r="C22" s="206"/>
-      <c r="D22" s="207"/>
-      <c r="E22" s="205" t="s">
+      <c r="B22" s="211"/>
+      <c r="C22" s="211"/>
+      <c r="D22" s="212"/>
+      <c r="E22" s="210" t="s">
         <v>320</v>
       </c>
-      <c r="F22" s="206"/>
-      <c r="G22" s="206"/>
-      <c r="H22" s="207"/>
+      <c r="F22" s="211"/>
+      <c r="G22" s="211"/>
+      <c r="H22" s="212"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="78">
@@ -11193,636 +12714,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H47"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="20" max="20" width="19.7109375" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="156" t="s">
-        <v>495</v>
-      </c>
-      <c r="B1" s="157"/>
-      <c r="C1" s="157"/>
-      <c r="D1" s="157"/>
-      <c r="E1" s="157"/>
-      <c r="F1" s="157"/>
-      <c r="G1" s="157"/>
-      <c r="H1" s="158"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="159"/>
-      <c r="B2" s="160"/>
-      <c r="C2" s="160"/>
-      <c r="D2" s="160"/>
-      <c r="E2" s="160"/>
-      <c r="F2" s="160"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="161"/>
-    </row>
-    <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="162" t="s">
-        <v>323</v>
-      </c>
-      <c r="B3" s="163"/>
-      <c r="C3" s="163"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163" t="s">
-        <v>322</v>
-      </c>
-      <c r="F3" s="163"/>
-      <c r="G3" s="163"/>
-      <c r="H3" s="164"/>
-    </row>
-    <row r="4" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A4" s="20">
-        <v>1</v>
-      </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="30" t="s">
-        <v>250</v>
-      </c>
-      <c r="E4" s="21">
-        <v>1</v>
-      </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="22" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A5" s="20">
-        <v>2</v>
-      </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="21">
-        <v>2</v>
-      </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="22"/>
-    </row>
-    <row r="6" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A6" s="20">
-        <v>3</v>
-      </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="21">
-        <v>3</v>
-      </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="22"/>
-    </row>
-    <row r="7" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A7" s="20">
-        <v>4</v>
-      </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="21">
-        <v>4</v>
-      </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="22"/>
-    </row>
-    <row r="8" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A8" s="20">
-        <v>5</v>
-      </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="21">
-        <v>5</v>
-      </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="22"/>
-    </row>
-    <row r="9" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A9" s="20">
-        <v>6</v>
-      </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="21">
-        <v>6</v>
-      </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="22"/>
-    </row>
-    <row r="10" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A10" s="20">
-        <v>7</v>
-      </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="21">
-        <v>7</v>
-      </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="22"/>
-    </row>
-    <row r="11" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A11" s="20">
-        <v>8</v>
-      </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="21">
-        <v>8</v>
-      </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="22"/>
-    </row>
-    <row r="12" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A12" s="20">
-        <v>9</v>
-      </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="21">
-        <v>9</v>
-      </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="22"/>
-    </row>
-    <row r="13" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A13" s="20">
-        <v>10</v>
-      </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="21">
-        <v>10</v>
-      </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="22"/>
-    </row>
-    <row r="14" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A14" s="20">
-        <v>11</v>
-      </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="21">
-        <v>11</v>
-      </c>
-      <c r="F14" s="22"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="22"/>
-    </row>
-    <row r="15" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A15" s="20">
-        <v>12</v>
-      </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="21">
-        <v>12</v>
-      </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="22"/>
-    </row>
-    <row r="16" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A16" s="20">
-        <v>13</v>
-      </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="21">
-        <v>13</v>
-      </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="22"/>
-    </row>
-    <row r="17" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A17" s="20">
-        <v>14</v>
-      </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="21">
-        <v>14</v>
-      </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="22"/>
-    </row>
-    <row r="18" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A18" s="20">
-        <v>15</v>
-      </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="21">
-        <v>15</v>
-      </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="22"/>
-    </row>
-    <row r="19" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A19" s="20">
-        <v>16</v>
-      </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="21">
-        <v>16</v>
-      </c>
-      <c r="F19" s="22"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="22"/>
-    </row>
-    <row r="20" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A20" s="20">
-        <v>17</v>
-      </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="21">
-        <v>17</v>
-      </c>
-      <c r="F20" s="22"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="22"/>
-    </row>
-    <row r="21" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A21" s="20">
-        <v>18</v>
-      </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="21">
-        <v>18</v>
-      </c>
-      <c r="F21" s="22"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="22"/>
-    </row>
-    <row r="22" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A22" s="20">
-        <v>19</v>
-      </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="21">
-        <v>19</v>
-      </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="22"/>
-    </row>
-    <row r="23" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A23" s="20">
-        <v>20</v>
-      </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="108">
-        <v>20</v>
-      </c>
-      <c r="F23" s="111"/>
-      <c r="G23" s="112"/>
-      <c r="H23" s="111"/>
-    </row>
-    <row r="24" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A24" s="24"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="110">
-        <v>21</v>
-      </c>
-      <c r="F24" s="109"/>
-      <c r="G24" s="113"/>
-      <c r="H24" s="109"/>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A25" s="24"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="110">
-        <v>22</v>
-      </c>
-      <c r="F25" s="109"/>
-      <c r="G25" s="113"/>
-      <c r="H25" s="109"/>
-    </row>
-    <row r="26" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A26" s="24"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="110">
-        <v>23</v>
-      </c>
-      <c r="F26" s="109"/>
-      <c r="G26" s="113"/>
-      <c r="H26" s="109"/>
-    </row>
-    <row r="27" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A27" s="24"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="110">
-        <v>24</v>
-      </c>
-      <c r="F27" s="109"/>
-      <c r="G27" s="113"/>
-      <c r="H27" s="109"/>
-    </row>
-    <row r="28" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A28" s="24"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="110">
-        <v>25</v>
-      </c>
-      <c r="F28" s="109"/>
-      <c r="G28" s="113"/>
-      <c r="H28" s="109"/>
-    </row>
-    <row r="29" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A29" s="24"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="110">
-        <v>26</v>
-      </c>
-      <c r="F29" s="109"/>
-      <c r="G29" s="113"/>
-      <c r="H29" s="109"/>
-    </row>
-    <row r="30" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A30" s="24"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="110">
-        <v>27</v>
-      </c>
-      <c r="F30" s="109"/>
-      <c r="G30" s="113"/>
-      <c r="H30" s="109"/>
-    </row>
-    <row r="31" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A31" s="24"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="110">
-        <v>28</v>
-      </c>
-      <c r="F31" s="109"/>
-      <c r="G31" s="113"/>
-      <c r="H31" s="109"/>
-    </row>
-    <row r="32" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A32" s="24"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="110">
-        <v>29</v>
-      </c>
-      <c r="F32" s="109"/>
-      <c r="G32" s="113"/>
-      <c r="H32" s="109"/>
-    </row>
-    <row r="33" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A33" s="24"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="110">
-        <v>30</v>
-      </c>
-      <c r="F33" s="109"/>
-      <c r="G33" s="113"/>
-      <c r="H33" s="109"/>
-    </row>
-    <row r="34" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A34" s="24"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="110">
-        <v>31</v>
-      </c>
-      <c r="F34" s="109"/>
-      <c r="G34" s="113"/>
-      <c r="H34" s="109"/>
-    </row>
-    <row r="35" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A35" s="24"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="110">
-        <v>32</v>
-      </c>
-      <c r="F35" s="109"/>
-      <c r="G35" s="113"/>
-      <c r="H35" s="109"/>
-    </row>
-    <row r="36" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A36" s="24"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="110">
-        <v>33</v>
-      </c>
-      <c r="F36" s="109"/>
-      <c r="G36" s="113"/>
-      <c r="H36" s="109"/>
-    </row>
-    <row r="37" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A37" s="24"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="110">
-        <v>34</v>
-      </c>
-      <c r="F37" s="109"/>
-      <c r="G37" s="113"/>
-      <c r="H37" s="109"/>
-    </row>
-    <row r="38" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A38" s="24"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="110">
-        <v>35</v>
-      </c>
-      <c r="F38" s="109"/>
-      <c r="G38" s="113"/>
-      <c r="H38" s="109"/>
-    </row>
-    <row r="39" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A39" s="24"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="110">
-        <v>36</v>
-      </c>
-      <c r="F39" s="109"/>
-      <c r="G39" s="113"/>
-      <c r="H39" s="109"/>
-    </row>
-    <row r="40" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A40" s="24"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="110">
-        <v>37</v>
-      </c>
-      <c r="F40" s="109"/>
-      <c r="G40" s="113"/>
-      <c r="H40" s="109"/>
-    </row>
-    <row r="41" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A41" s="24"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="110">
-        <v>38</v>
-      </c>
-      <c r="F41" s="109"/>
-      <c r="G41" s="113"/>
-      <c r="H41" s="109"/>
-    </row>
-    <row r="42" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A42" s="24"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="20">
-        <v>39</v>
-      </c>
-      <c r="F42" s="22"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="22"/>
-    </row>
-    <row r="43" spans="1:8" ht="18.75" thickBot="1">
-      <c r="A43" s="24"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="110">
-        <v>40</v>
-      </c>
-      <c r="F43" s="109"/>
-      <c r="G43" s="113"/>
-      <c r="H43" s="109"/>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="24"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="26"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="24"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="26"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="24"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="26"/>
-    </row>
-    <row r="47" spans="1:8" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A47" s="27"/>
-      <c r="B47" s="28"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="29"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-  </mergeCells>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
chg: corrected Datalink for F16 flights to 4xx series
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" activeTab="2"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="763">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="769">
   <si>
     <t>AWACS</t>
   </si>
@@ -2044,42 +2044,6 @@
     <t>225.75</t>
   </si>
   <si>
-    <t>311</t>
-  </si>
-  <si>
-    <t>312</t>
-  </si>
-  <si>
-    <t>313</t>
-  </si>
-  <si>
-    <t>314</t>
-  </si>
-  <si>
-    <t>00311</t>
-  </si>
-  <si>
-    <t>00312</t>
-  </si>
-  <si>
-    <t>00313</t>
-  </si>
-  <si>
-    <t>00314</t>
-  </si>
-  <si>
-    <t>321</t>
-  </si>
-  <si>
-    <t>322</t>
-  </si>
-  <si>
-    <t>323</t>
-  </si>
-  <si>
-    <t>324</t>
-  </si>
-  <si>
     <t>LO21</t>
   </si>
   <si>
@@ -2092,30 +2056,6 @@
     <t>LO24</t>
   </si>
   <si>
-    <t>00322</t>
-  </si>
-  <si>
-    <t>00323</t>
-  </si>
-  <si>
-    <t>00324</t>
-  </si>
-  <si>
-    <t>00321</t>
-  </si>
-  <si>
-    <t>331</t>
-  </si>
-  <si>
-    <t>332</t>
-  </si>
-  <si>
-    <t>333</t>
-  </si>
-  <si>
-    <t>334</t>
-  </si>
-  <si>
     <t>JI31</t>
   </si>
   <si>
@@ -2128,42 +2068,6 @@
     <t>JI34</t>
   </si>
   <si>
-    <t>00331</t>
-  </si>
-  <si>
-    <t>00332</t>
-  </si>
-  <si>
-    <t>00333</t>
-  </si>
-  <si>
-    <t>00334</t>
-  </si>
-  <si>
-    <t>341</t>
-  </si>
-  <si>
-    <t>342</t>
-  </si>
-  <si>
-    <t>343</t>
-  </si>
-  <si>
-    <t>344</t>
-  </si>
-  <si>
-    <t>00341</t>
-  </si>
-  <si>
-    <t>00342</t>
-  </si>
-  <si>
-    <t>00343</t>
-  </si>
-  <si>
-    <t>00344</t>
-  </si>
-  <si>
     <t>JEDI 3</t>
   </si>
   <si>
@@ -2197,9 +2101,6 @@
     <t>VM91</t>
   </si>
   <si>
-    <t>11311</t>
-  </si>
-  <si>
     <t>912</t>
   </si>
   <si>
@@ -2218,15 +2119,6 @@
     <t>VM94</t>
   </si>
   <si>
-    <t>11312</t>
-  </si>
-  <si>
-    <t>11313</t>
-  </si>
-  <si>
-    <t>11314</t>
-  </si>
-  <si>
     <t>921</t>
   </si>
   <si>
@@ -2242,9 +2134,6 @@
     <t>NA94</t>
   </si>
   <si>
-    <t>11321</t>
-  </si>
-  <si>
     <t>NINJA</t>
   </si>
   <si>
@@ -2257,18 +2146,6 @@
     <t>932</t>
   </si>
   <si>
-    <t>11331</t>
-  </si>
-  <si>
-    <t>11332</t>
-  </si>
-  <si>
-    <t>11333</t>
-  </si>
-  <si>
-    <t>11334</t>
-  </si>
-  <si>
     <t>RATTLER</t>
   </si>
   <si>
@@ -2312,6 +2189,147 @@
   </si>
   <si>
     <t>BLUE F-16</t>
+  </si>
+  <si>
+    <t>00411</t>
+  </si>
+  <si>
+    <t>00412</t>
+  </si>
+  <si>
+    <t>00413</t>
+  </si>
+  <si>
+    <t>00414</t>
+  </si>
+  <si>
+    <t>00421</t>
+  </si>
+  <si>
+    <t>00422</t>
+  </si>
+  <si>
+    <t>00423</t>
+  </si>
+  <si>
+    <t>00424</t>
+  </si>
+  <si>
+    <t>00431</t>
+  </si>
+  <si>
+    <t>00432</t>
+  </si>
+  <si>
+    <t>00433</t>
+  </si>
+  <si>
+    <t>00434</t>
+  </si>
+  <si>
+    <t>00441</t>
+  </si>
+  <si>
+    <t>00442</t>
+  </si>
+  <si>
+    <t>00443</t>
+  </si>
+  <si>
+    <t>00444</t>
+  </si>
+  <si>
+    <t>11411</t>
+  </si>
+  <si>
+    <t>11412</t>
+  </si>
+  <si>
+    <t>11413</t>
+  </si>
+  <si>
+    <t>11414</t>
+  </si>
+  <si>
+    <t>11421</t>
+  </si>
+  <si>
+    <t>11422</t>
+  </si>
+  <si>
+    <t>11423</t>
+  </si>
+  <si>
+    <t>11424</t>
+  </si>
+  <si>
+    <t>11431</t>
+  </si>
+  <si>
+    <t>11432</t>
+  </si>
+  <si>
+    <t>11433</t>
+  </si>
+  <si>
+    <t>11434</t>
+  </si>
+  <si>
+    <t>411</t>
+  </si>
+  <si>
+    <t>412</t>
+  </si>
+  <si>
+    <t>413</t>
+  </si>
+  <si>
+    <t>414</t>
+  </si>
+  <si>
+    <t>421</t>
+  </si>
+  <si>
+    <t>422</t>
+  </si>
+  <si>
+    <t>423</t>
+  </si>
+  <si>
+    <t>424</t>
+  </si>
+  <si>
+    <t>431</t>
+  </si>
+  <si>
+    <t>432</t>
+  </si>
+  <si>
+    <t>433</t>
+  </si>
+  <si>
+    <t>434</t>
+  </si>
+  <si>
+    <t>441</t>
+  </si>
+  <si>
+    <t>442</t>
+  </si>
+  <si>
+    <t>443</t>
+  </si>
+  <si>
+    <t>444</t>
+  </si>
+  <si>
+    <t>DATALINK TRMA v0.1</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>AGGRESSOR F/A-18 (RED AIRCRAFT)</t>
   </si>
 </sst>
 </file>
@@ -2321,7 +2339,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2505,6 +2523,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="19">
     <fill>
@@ -2616,7 +2642,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -3162,11 +3188,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="251">
+  <cellXfs count="252">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3524,212 +3600,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -3745,6 +3618,39 @@
     <xf numFmtId="49" fontId="24" fillId="18" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="23" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3754,33 +3660,6 @@
     <xf numFmtId="0" fontId="25" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3789,6 +3668,210 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4217,13 +4300,13 @@
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
       <c r="T2" s="12"/>
-      <c r="V2" s="153" t="s">
+      <c r="V2" s="170" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="153"/>
-      <c r="X2" s="153"/>
-      <c r="Y2" s="153"/>
-      <c r="Z2" s="153"/>
+      <c r="W2" s="170"/>
+      <c r="X2" s="170"/>
+      <c r="Y2" s="170"/>
+      <c r="Z2" s="170"/>
       <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
       <c r="AC2" s="12"/>
@@ -4278,9 +4361,9 @@
         <v>433</v>
       </c>
       <c r="Q3" s="12"/>
-      <c r="R3" s="152"/>
-      <c r="S3" s="152"/>
-      <c r="T3" s="152"/>
+      <c r="R3" s="174"/>
+      <c r="S3" s="174"/>
+      <c r="T3" s="174"/>
       <c r="V3" s="122" t="s">
         <v>335</v>
       </c>
@@ -4364,22 +4447,22 @@
       <c r="AA4" s="36"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="36"/>
-      <c r="AD4" s="153" t="s">
+      <c r="AD4" s="170" t="s">
         <v>436</v>
       </c>
-      <c r="AE4" s="153"/>
-      <c r="AF4" s="153"/>
-      <c r="AG4" s="153"/>
-      <c r="AH4" s="153"/>
-      <c r="AJ4" s="153" t="s">
+      <c r="AE4" s="170"/>
+      <c r="AF4" s="170"/>
+      <c r="AG4" s="170"/>
+      <c r="AH4" s="170"/>
+      <c r="AJ4" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="AK4" s="153"/>
-      <c r="AL4" s="153"/>
-      <c r="AM4" s="153"/>
-      <c r="AN4" s="153"/>
-      <c r="AO4" s="153"/>
-      <c r="AP4" s="153"/>
+      <c r="AK4" s="170"/>
+      <c r="AL4" s="170"/>
+      <c r="AM4" s="170"/>
+      <c r="AN4" s="170"/>
+      <c r="AO4" s="170"/>
+      <c r="AP4" s="170"/>
     </row>
     <row r="5" spans="1:42" ht="15.75">
       <c r="A5" s="129" t="s">
@@ -5472,15 +5555,15 @@
       <c r="AH17" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="AJ17" s="153" t="s">
+      <c r="AJ17" s="170" t="s">
         <v>277</v>
       </c>
-      <c r="AK17" s="153"/>
-      <c r="AL17" s="153"/>
-      <c r="AM17" s="153"/>
-      <c r="AN17" s="153"/>
-      <c r="AO17" s="153"/>
-      <c r="AP17" s="153"/>
+      <c r="AK17" s="170"/>
+      <c r="AL17" s="170"/>
+      <c r="AM17" s="170"/>
+      <c r="AN17" s="170"/>
+      <c r="AO17" s="170"/>
+      <c r="AP17" s="170"/>
     </row>
     <row r="18" spans="1:42" ht="15.75">
       <c r="A18" s="129" t="s">
@@ -5697,9 +5780,9 @@
       <c r="O20" s="35"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="152"/>
-      <c r="S20" s="152"/>
-      <c r="T20" s="152"/>
+      <c r="R20" s="174"/>
+      <c r="S20" s="174"/>
+      <c r="T20" s="174"/>
       <c r="U20" s="2"/>
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
@@ -6039,13 +6122,13 @@
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
-      <c r="AD24" s="153" t="s">
+      <c r="AD24" s="170" t="s">
         <v>493</v>
       </c>
-      <c r="AE24" s="153"/>
-      <c r="AF24" s="153"/>
-      <c r="AG24" s="153"/>
-      <c r="AH24" s="153"/>
+      <c r="AE24" s="170"/>
+      <c r="AF24" s="170"/>
+      <c r="AG24" s="170"/>
+      <c r="AH24" s="170"/>
       <c r="AJ24" s="142" t="s">
         <v>570</v>
       </c>
@@ -6355,15 +6438,15 @@
       <c r="S29" s="35"/>
       <c r="T29" s="35"/>
       <c r="U29" s="35"/>
-      <c r="V29" s="153" t="s">
+      <c r="V29" s="170" t="s">
         <v>212</v>
       </c>
-      <c r="W29" s="153"/>
-      <c r="X29" s="153"/>
-      <c r="Y29" s="153"/>
-      <c r="Z29" s="153"/>
-      <c r="AA29" s="153"/>
-      <c r="AB29" s="153"/>
+      <c r="W29" s="170"/>
+      <c r="X29" s="170"/>
+      <c r="Y29" s="170"/>
+      <c r="Z29" s="170"/>
+      <c r="AA29" s="170"/>
+      <c r="AB29" s="170"/>
     </row>
     <row r="30" spans="1:42">
       <c r="A30" s="129"/>
@@ -6453,11 +6536,11 @@
       <c r="Y31" s="37"/>
       <c r="Z31" s="37"/>
       <c r="AA31" s="12"/>
-      <c r="AD31" s="154" t="s">
+      <c r="AD31" s="171" t="s">
         <v>263</v>
       </c>
-      <c r="AE31" s="155"/>
-      <c r="AF31" s="156"/>
+      <c r="AE31" s="172"/>
+      <c r="AF31" s="173"/>
     </row>
     <row r="32" spans="1:42">
       <c r="S32" s="12"/>
@@ -6562,15 +6645,15 @@
       <c r="S37" s="12"/>
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
-      <c r="V37" s="153" t="s">
+      <c r="V37" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="W37" s="153"/>
-      <c r="X37" s="153"/>
-      <c r="Y37" s="153"/>
-      <c r="Z37" s="153"/>
-      <c r="AA37" s="153"/>
-      <c r="AB37" s="153"/>
+      <c r="W37" s="170"/>
+      <c r="X37" s="170"/>
+      <c r="Y37" s="170"/>
+      <c r="Z37" s="170"/>
+      <c r="AA37" s="170"/>
+      <c r="AB37" s="170"/>
       <c r="AD37" s="3" t="s">
         <v>259</v>
       </c>
@@ -6669,15 +6752,15 @@
       <c r="S42" s="12"/>
       <c r="T42" s="12"/>
       <c r="U42" s="12"/>
-      <c r="V42" s="153" t="s">
+      <c r="V42" s="170" t="s">
         <v>247</v>
       </c>
-      <c r="W42" s="153"/>
-      <c r="X42" s="153"/>
-      <c r="Y42" s="153"/>
-      <c r="Z42" s="153"/>
-      <c r="AA42" s="153"/>
-      <c r="AB42" s="153"/>
+      <c r="W42" s="170"/>
+      <c r="X42" s="170"/>
+      <c r="Y42" s="170"/>
+      <c r="Z42" s="170"/>
+      <c r="AA42" s="170"/>
+      <c r="AB42" s="170"/>
       <c r="AD42" s="3" t="s">
         <v>265</v>
       </c>
@@ -6782,15 +6865,15 @@
       <c r="S48" s="12"/>
       <c r="T48" s="12"/>
       <c r="U48" s="12"/>
-      <c r="V48" s="154" t="s">
+      <c r="V48" s="171" t="s">
         <v>480</v>
       </c>
-      <c r="W48" s="155"/>
-      <c r="X48" s="155"/>
-      <c r="Y48" s="155"/>
-      <c r="Z48" s="155"/>
-      <c r="AA48" s="155"/>
-      <c r="AB48" s="156"/>
+      <c r="W48" s="172"/>
+      <c r="X48" s="172"/>
+      <c r="Y48" s="172"/>
+      <c r="Z48" s="172"/>
+      <c r="AA48" s="172"/>
+      <c r="AB48" s="173"/>
     </row>
     <row r="49" spans="19:28">
       <c r="S49" s="12"/>
@@ -6880,11 +6963,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="V42:AB42"/>
-    <mergeCell ref="AD4:AH4"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="V48:AB48"/>
-    <mergeCell ref="V37:AB37"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="AJ4:AP4"/>
@@ -6892,6 +6970,11 @@
     <mergeCell ref="AD31:AF31"/>
     <mergeCell ref="V29:AB29"/>
     <mergeCell ref="AD24:AH24"/>
+    <mergeCell ref="V42:AB42"/>
+    <mergeCell ref="AD4:AH4"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="V48:AB48"/>
+    <mergeCell ref="V37:AB37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6920,40 +7003,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="184" t="s">
         <v>495</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
-      <c r="G1" s="162"/>
-      <c r="H1" s="163"/>
+      <c r="B1" s="185"/>
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="186"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="164"/>
-      <c r="B2" s="165"/>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="166"/>
+      <c r="A2" s="187"/>
+      <c r="B2" s="188"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="188"/>
+      <c r="G2" s="188"/>
+      <c r="H2" s="189"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="167" t="s">
+      <c r="A3" s="190" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="168"/>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168" t="s">
+      <c r="B3" s="191"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="191"/>
+      <c r="E3" s="191" t="s">
         <v>322</v>
       </c>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="169"/>
+      <c r="F3" s="191"/>
+      <c r="G3" s="191"/>
+      <c r="H3" s="192"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="20">
@@ -7534,13 +7617,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AJ45"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="1.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="7" max="7" width="2.5703125" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" style="74"/>
     <col min="13" max="13" width="1.7109375" customWidth="1"/>
@@ -7550,48 +7634,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:36">
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="170" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
-      <c r="H2" s="153" t="s">
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="H2" s="170" t="s">
         <v>231</v>
       </c>
-      <c r="I2" s="153"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
-      <c r="L2" s="153"/>
-      <c r="N2" s="153" t="s">
+      <c r="I2" s="170"/>
+      <c r="J2" s="170"/>
+      <c r="K2" s="170"/>
+      <c r="L2" s="170"/>
+      <c r="N2" s="170" t="s">
         <v>239</v>
       </c>
-      <c r="O2" s="153"/>
-      <c r="P2" s="153"/>
-      <c r="Q2" s="153"/>
-      <c r="R2" s="153"/>
-      <c r="T2" s="153" t="s">
+      <c r="O2" s="170"/>
+      <c r="P2" s="170"/>
+      <c r="Q2" s="170"/>
+      <c r="R2" s="170"/>
+      <c r="T2" s="170" t="s">
         <v>249</v>
       </c>
-      <c r="U2" s="153"/>
-      <c r="V2" s="153"/>
-      <c r="W2" s="153"/>
-      <c r="X2" s="153"/>
-      <c r="Z2" s="153" t="s">
+      <c r="U2" s="170"/>
+      <c r="V2" s="170"/>
+      <c r="W2" s="170"/>
+      <c r="X2" s="170"/>
+      <c r="Z2" s="170" t="s">
         <v>321</v>
       </c>
-      <c r="AA2" s="153"/>
-      <c r="AB2" s="153"/>
-      <c r="AC2" s="153"/>
-      <c r="AD2" s="153"/>
-      <c r="AF2" s="153" t="s">
+      <c r="AA2" s="170"/>
+      <c r="AB2" s="170"/>
+      <c r="AC2" s="170"/>
+      <c r="AD2" s="170"/>
+      <c r="AF2" s="170" t="s">
         <v>498</v>
       </c>
-      <c r="AG2" s="153"/>
-      <c r="AH2" s="153"/>
-      <c r="AI2" s="153"/>
-      <c r="AJ2" s="153"/>
+      <c r="AG2" s="170"/>
+      <c r="AH2" s="170"/>
+      <c r="AI2" s="170"/>
+      <c r="AJ2" s="170"/>
     </row>
     <row r="3" spans="2:36">
       <c r="B3" s="124" t="s">
@@ -7693,13 +7777,13 @@
         <v>482</v>
       </c>
       <c r="D4" s="126" t="s">
-        <v>673</v>
+        <v>750</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>324</v>
       </c>
       <c r="F4" s="126" t="s">
-        <v>677</v>
+        <v>722</v>
       </c>
       <c r="H4" t="s">
         <v>501</v>
@@ -7725,30 +7809,30 @@
     </row>
     <row r="5" spans="2:36">
       <c r="B5" s="3" t="s">
-        <v>720</v>
+        <v>688</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="126" t="s">
-        <v>674</v>
+        <v>751</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>326</v>
       </c>
       <c r="F5" s="126" t="s">
-        <v>678</v>
+        <v>723</v>
       </c>
     </row>
     <row r="6" spans="2:36">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="126" t="s">
-        <v>675</v>
+        <v>752</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>327</v>
       </c>
       <c r="F6" s="126" t="s">
-        <v>679</v>
+        <v>724</v>
       </c>
       <c r="H6" t="s">
         <v>503</v>
@@ -7761,13 +7845,13 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="126" t="s">
-        <v>676</v>
+        <v>753</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>328</v>
       </c>
       <c r="F7" s="126" t="s">
-        <v>680</v>
+        <v>725</v>
       </c>
     </row>
     <row r="8" spans="2:36">
@@ -7791,19 +7875,19 @@
     </row>
     <row r="9" spans="2:36">
       <c r="B9" s="3" t="s">
-        <v>715</v>
+        <v>683</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>482</v>
       </c>
       <c r="D9" s="126" t="s">
-        <v>681</v>
+        <v>754</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>685</v>
+        <v>673</v>
       </c>
       <c r="F9" s="126" t="s">
-        <v>692</v>
+        <v>726</v>
       </c>
       <c r="H9" t="s">
         <v>506</v>
@@ -7815,43 +7899,43 @@
     </row>
     <row r="10" spans="2:36">
       <c r="B10" s="3" t="s">
-        <v>720</v>
+        <v>688</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="126" t="s">
-        <v>682</v>
+        <v>755</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>686</v>
+        <v>674</v>
       </c>
       <c r="F10" s="126" t="s">
-        <v>689</v>
+        <v>727</v>
       </c>
     </row>
     <row r="11" spans="2:36">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="126" t="s">
-        <v>683</v>
+        <v>756</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>687</v>
+        <v>675</v>
       </c>
       <c r="F11" s="126" t="s">
-        <v>690</v>
+        <v>728</v>
       </c>
     </row>
     <row r="12" spans="2:36">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="126" t="s">
-        <v>684</v>
+        <v>757</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>688</v>
+        <v>676</v>
       </c>
       <c r="F12" s="126" t="s">
-        <v>691</v>
+        <v>729</v>
       </c>
     </row>
     <row r="13" spans="2:36">
@@ -7866,47 +7950,47 @@
     </row>
     <row r="14" spans="2:36">
       <c r="B14" s="3" t="s">
-        <v>713</v>
+        <v>681</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>482</v>
       </c>
       <c r="D14" s="126" t="s">
-        <v>693</v>
+        <v>758</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>697</v>
+        <v>677</v>
       </c>
       <c r="F14" s="126" t="s">
-        <v>701</v>
+        <v>730</v>
       </c>
     </row>
     <row r="15" spans="2:36">
       <c r="B15" s="3" t="s">
-        <v>721</v>
+        <v>689</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="126" t="s">
-        <v>694</v>
+        <v>759</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>698</v>
+        <v>678</v>
       </c>
       <c r="F15" s="126" t="s">
-        <v>702</v>
+        <v>731</v>
       </c>
     </row>
     <row r="16" spans="2:36">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="126" t="s">
-        <v>695</v>
+        <v>760</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>699</v>
+        <v>679</v>
       </c>
       <c r="F16" s="126" t="s">
-        <v>703</v>
+        <v>732</v>
       </c>
       <c r="H16" t="s">
         <v>577</v>
@@ -7916,13 +8000,13 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="126" t="s">
-        <v>696</v>
+        <v>761</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>700</v>
+        <v>680</v>
       </c>
       <c r="F17" s="126" t="s">
-        <v>704</v>
+        <v>733</v>
       </c>
     </row>
     <row r="18" spans="2:20">
@@ -7931,25 +8015,25 @@
       <c r="D18" s="126"/>
       <c r="E18" s="3"/>
       <c r="F18" s="126"/>
+      <c r="H18" t="s">
+        <v>767</v>
+      </c>
     </row>
     <row r="19" spans="2:20">
       <c r="B19" s="3" t="s">
-        <v>714</v>
+        <v>682</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>482</v>
       </c>
       <c r="D19" s="126" t="s">
-        <v>705</v>
+        <v>762</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>716</v>
+        <v>684</v>
       </c>
       <c r="F19" s="126" t="s">
-        <v>709</v>
-      </c>
-      <c r="H19" t="s">
-        <v>358</v>
+        <v>734</v>
       </c>
       <c r="T19" t="s">
         <v>358</v>
@@ -7957,20 +8041,17 @@
     </row>
     <row r="20" spans="2:20">
       <c r="B20" s="3" t="s">
-        <v>721</v>
+        <v>689</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="126" t="s">
-        <v>706</v>
+        <v>763</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>717</v>
+        <v>685</v>
       </c>
       <c r="F20" s="126" t="s">
-        <v>710</v>
-      </c>
-      <c r="H20" t="s">
-        <v>508</v>
+        <v>735</v>
       </c>
       <c r="T20" t="s">
         <v>509</v>
@@ -7980,26 +8061,26 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="126" t="s">
-        <v>707</v>
+        <v>764</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>718</v>
+        <v>686</v>
       </c>
       <c r="F21" s="126" t="s">
-        <v>711</v>
+        <v>736</v>
       </c>
     </row>
     <row r="22" spans="2:20">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="126" t="s">
-        <v>708</v>
+        <v>765</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>719</v>
+        <v>687</v>
       </c>
       <c r="F22" s="126" t="s">
-        <v>712</v>
+        <v>737</v>
       </c>
     </row>
     <row r="23" spans="2:20">
@@ -8017,13 +8098,20 @@
       <c r="F24" s="140"/>
     </row>
     <row r="25" spans="2:20">
-      <c r="B25" s="153" t="s">
-        <v>754</v>
-      </c>
-      <c r="C25" s="153"/>
-      <c r="D25" s="153"/>
-      <c r="E25" s="153"/>
-      <c r="F25" s="153"/>
+      <c r="B25" s="170" t="s">
+        <v>713</v>
+      </c>
+      <c r="C25" s="170"/>
+      <c r="D25" s="170"/>
+      <c r="E25" s="170"/>
+      <c r="F25" s="170"/>
+      <c r="H25" s="170" t="s">
+        <v>768</v>
+      </c>
+      <c r="I25" s="170"/>
+      <c r="J25" s="170"/>
+      <c r="K25" s="170"/>
+      <c r="L25" s="170"/>
     </row>
     <row r="26" spans="2:20">
       <c r="B26" s="124" t="s">
@@ -8041,6 +8129,21 @@
       <c r="F26" s="125" t="s">
         <v>325</v>
       </c>
+      <c r="H26" s="124" t="s">
+        <v>218</v>
+      </c>
+      <c r="I26" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="J26" s="125" t="s">
+        <v>452</v>
+      </c>
+      <c r="K26" s="124" t="s">
+        <v>282</v>
+      </c>
+      <c r="L26" s="125" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="27" spans="2:20">
       <c r="B27" s="3" t="s">
@@ -8050,52 +8153,55 @@
         <v>482</v>
       </c>
       <c r="D27" s="126" t="s">
-        <v>722</v>
+        <v>690</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>723</v>
+        <v>691</v>
       </c>
       <c r="F27" s="126" t="s">
-        <v>724</v>
+        <v>738</v>
+      </c>
+      <c r="H27" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="28" spans="2:20">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="126" t="s">
-        <v>725</v>
+        <v>692</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>728</v>
+        <v>695</v>
       </c>
       <c r="F28" s="126" t="s">
-        <v>731</v>
+        <v>739</v>
       </c>
     </row>
     <row r="29" spans="2:20">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="126" t="s">
-        <v>726</v>
+        <v>693</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>729</v>
+        <v>696</v>
       </c>
       <c r="F29" s="126" t="s">
-        <v>732</v>
+        <v>740</v>
       </c>
     </row>
     <row r="30" spans="2:20">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="126" t="s">
-        <v>727</v>
+        <v>694</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>730</v>
+        <v>697</v>
       </c>
       <c r="F30" s="126" t="s">
-        <v>733</v>
+        <v>741</v>
       </c>
     </row>
     <row r="31" spans="2:20">
@@ -8107,19 +8213,19 @@
     </row>
     <row r="32" spans="2:20">
       <c r="B32" s="3" t="s">
-        <v>740</v>
+        <v>703</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>741</v>
+        <v>704</v>
       </c>
       <c r="D32" s="126" t="s">
-        <v>734</v>
+        <v>698</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>735</v>
+        <v>699</v>
       </c>
       <c r="F32" s="126" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
     </row>
     <row r="33" spans="2:6">
@@ -8129,10 +8235,10 @@
         <v>922</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>736</v>
-      </c>
-      <c r="F33" s="126">
-        <v>11322</v>
+        <v>700</v>
+      </c>
+      <c r="F33" s="126" t="s">
+        <v>743</v>
       </c>
     </row>
     <row r="34" spans="2:6">
@@ -8142,10 +8248,10 @@
         <v>923</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>737</v>
-      </c>
-      <c r="F34" s="126">
-        <v>11323</v>
+        <v>701</v>
+      </c>
+      <c r="F34" s="126" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="35" spans="2:6">
@@ -8155,10 +8261,10 @@
         <v>924</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>738</v>
-      </c>
-      <c r="F35" s="126">
-        <v>11324</v>
+        <v>702</v>
+      </c>
+      <c r="F35" s="126" t="s">
+        <v>745</v>
       </c>
     </row>
     <row r="36" spans="2:6">
@@ -8170,32 +8276,32 @@
     </row>
     <row r="37" spans="2:6">
       <c r="B37" s="3" t="s">
-        <v>748</v>
+        <v>707</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>753</v>
+        <v>712</v>
       </c>
       <c r="D37" s="126" t="s">
-        <v>742</v>
+        <v>705</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>749</v>
+        <v>708</v>
       </c>
       <c r="F37" s="126" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
     </row>
     <row r="38" spans="2:6">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="126" t="s">
-        <v>743</v>
+        <v>706</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>750</v>
+        <v>709</v>
       </c>
       <c r="F38" s="126" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
     </row>
     <row r="39" spans="2:6">
@@ -8205,10 +8311,10 @@
         <v>933</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>751</v>
+        <v>710</v>
       </c>
       <c r="F39" s="126" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
     </row>
     <row r="40" spans="2:6">
@@ -8218,10 +8324,10 @@
         <v>934</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>752</v>
+        <v>711</v>
       </c>
       <c r="F40" s="126" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
     </row>
     <row r="41" spans="2:6">
@@ -8233,19 +8339,19 @@
     </row>
     <row r="42" spans="2:6">
       <c r="B42" s="3" t="s">
-        <v>755</v>
+        <v>714</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>756</v>
+        <v>715</v>
       </c>
       <c r="D42" s="147">
         <v>941</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>760</v>
+        <v>719</v>
       </c>
       <c r="F42" s="148">
-        <v>11341</v>
+        <v>11441</v>
       </c>
     </row>
     <row r="43" spans="2:6">
@@ -8255,10 +8361,10 @@
         <v>942</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>757</v>
+        <v>716</v>
       </c>
       <c r="F43" s="148">
-        <v>11342</v>
+        <v>11442</v>
       </c>
     </row>
     <row r="44" spans="2:6">
@@ -8268,10 +8374,10 @@
         <v>943</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>758</v>
+        <v>717</v>
       </c>
       <c r="F44" s="148">
-        <v>11343</v>
+        <v>11443</v>
       </c>
     </row>
     <row r="45" spans="2:6">
@@ -8281,14 +8387,14 @@
         <v>945</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>759</v>
+        <v>718</v>
       </c>
       <c r="F45" s="148">
-        <v>11344</v>
+        <v>11444</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="B25:F25"/>
     <mergeCell ref="AF2:AJ2"/>
     <mergeCell ref="Z2:AD2"/>
@@ -8296,21 +8402,22 @@
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="N2:R2"/>
     <mergeCell ref="T2:X2"/>
+    <mergeCell ref="H25:L25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D4 D5:D7 D9:D12 D14:D17 D19:D22 D27:D30 D32:D35 D37:D40 F27:F40 F4:F22" numberStoredAsText="1"/>
+    <ignoredError sqref="D27:D30 D32:D35 D37:D40 F13 F18 F8 F4:F7 F9:F12 F19:F22 F14:F17 F36 F31 F27:F30 F32:F35 F37:F40 D4:D22" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X46"/>
+  <dimension ref="A1:W47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -8321,742 +8428,757 @@
     <col min="6" max="6" width="2.5703125" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" style="74" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
     <col min="12" max="12" width="1.7109375" customWidth="1"/>
     <col min="18" max="18" width="1.5703125" customWidth="1"/>
     <col min="23" max="23" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="1.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A1" s="245" t="s">
-        <v>762</v>
-      </c>
-      <c r="B1" s="246"/>
-      <c r="C1" s="247"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="220"/>
-      <c r="I1" s="220"/>
-      <c r="J1" s="149"/>
+    <row r="1" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
+      <c r="A1" s="249" t="s">
+        <v>766</v>
+      </c>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="250"/>
+      <c r="I1" s="250"/>
+      <c r="J1" s="251"/>
     </row>
     <row r="2" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A2" s="234" t="s">
+      <c r="A2" s="246" t="s">
+        <v>721</v>
+      </c>
+      <c r="B2" s="247"/>
+      <c r="C2" s="248"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="151"/>
+      <c r="H2" s="151"/>
+      <c r="I2" s="151"/>
+      <c r="J2" s="149"/>
+    </row>
+    <row r="3" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A3" s="165" t="s">
         <v>218</v>
       </c>
-      <c r="B2" s="234" t="s">
+      <c r="B3" s="165" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="235" t="s">
+      <c r="C3" s="166" t="s">
         <v>325</v>
       </c>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
-      <c r="G2" s="219"/>
-      <c r="H2" s="219"/>
-      <c r="I2" s="219"/>
-      <c r="J2" s="150"/>
-    </row>
-    <row r="3" spans="1:10" ht="18.75">
-      <c r="A3" s="248" t="s">
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="149"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.75">
+      <c r="A4" s="181" t="s">
         <v>329</v>
       </c>
-      <c r="B3" s="229" t="s">
+      <c r="B4" s="160" t="s">
         <v>324</v>
       </c>
-      <c r="C3" s="230" t="s">
+      <c r="C4" s="161" t="s">
+        <v>722</v>
+      </c>
+      <c r="D4" s="151"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="151"/>
+      <c r="G4" s="151"/>
+      <c r="H4" s="151"/>
+      <c r="I4" s="151"/>
+      <c r="J4" s="149"/>
+    </row>
+    <row r="5" spans="1:10" ht="18.75">
+      <c r="A5" s="182"/>
+      <c r="B5" s="159" t="s">
+        <v>326</v>
+      </c>
+      <c r="C5" s="162" t="s">
+        <v>723</v>
+      </c>
+      <c r="D5" s="151"/>
+      <c r="E5" s="151"/>
+      <c r="F5" s="151"/>
+      <c r="G5" s="151"/>
+      <c r="H5" s="151"/>
+      <c r="I5" s="151"/>
+      <c r="J5" s="149"/>
+    </row>
+    <row r="6" spans="1:10" ht="18.75">
+      <c r="A6" s="182"/>
+      <c r="B6" s="159" t="s">
+        <v>327</v>
+      </c>
+      <c r="C6" s="162" t="s">
+        <v>724</v>
+      </c>
+      <c r="D6" s="151"/>
+      <c r="E6" s="151"/>
+      <c r="F6" s="151"/>
+      <c r="G6" s="151"/>
+      <c r="H6" s="151"/>
+      <c r="I6" s="151"/>
+      <c r="J6" s="149"/>
+    </row>
+    <row r="7" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A7" s="183"/>
+      <c r="B7" s="163" t="s">
+        <v>328</v>
+      </c>
+      <c r="C7" s="164" t="s">
+        <v>725</v>
+      </c>
+      <c r="D7" s="151"/>
+      <c r="E7" s="151"/>
+      <c r="F7" s="151"/>
+      <c r="G7" s="151"/>
+      <c r="H7" s="151"/>
+      <c r="I7" s="151"/>
+      <c r="J7" s="149"/>
+    </row>
+    <row r="8" spans="1:10" ht="18.75">
+      <c r="A8" s="181" t="s">
+        <v>683</v>
+      </c>
+      <c r="B8" s="160" t="s">
+        <v>673</v>
+      </c>
+      <c r="C8" s="161" t="s">
+        <v>726</v>
+      </c>
+      <c r="D8" s="151"/>
+      <c r="E8" s="151"/>
+      <c r="F8" s="151"/>
+      <c r="G8" s="151"/>
+      <c r="H8" s="151"/>
+      <c r="I8" s="151"/>
+      <c r="J8" s="149"/>
+    </row>
+    <row r="9" spans="1:10" ht="18.75">
+      <c r="A9" s="182"/>
+      <c r="B9" s="159" t="s">
+        <v>674</v>
+      </c>
+      <c r="C9" s="162" t="s">
+        <v>727</v>
+      </c>
+      <c r="D9" s="151"/>
+      <c r="E9" s="151"/>
+      <c r="F9" s="151"/>
+      <c r="G9" s="151"/>
+      <c r="H9" s="151"/>
+      <c r="I9" s="151"/>
+      <c r="J9" s="149"/>
+    </row>
+    <row r="10" spans="1:10" ht="18.75">
+      <c r="A10" s="182"/>
+      <c r="B10" s="159" t="s">
+        <v>675</v>
+      </c>
+      <c r="C10" s="162" t="s">
+        <v>728</v>
+      </c>
+      <c r="D10" s="151"/>
+      <c r="E10" s="151"/>
+      <c r="F10" s="151"/>
+      <c r="G10" s="151"/>
+      <c r="H10" s="151"/>
+      <c r="I10" s="151"/>
+      <c r="J10" s="149"/>
+    </row>
+    <row r="11" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A11" s="183"/>
+      <c r="B11" s="163" t="s">
+        <v>676</v>
+      </c>
+      <c r="C11" s="164" t="s">
+        <v>729</v>
+      </c>
+      <c r="D11" s="151"/>
+      <c r="E11" s="151"/>
+      <c r="F11" s="151"/>
+      <c r="G11" s="151"/>
+      <c r="H11" s="151"/>
+      <c r="I11" s="151"/>
+      <c r="J11" s="149"/>
+    </row>
+    <row r="12" spans="1:10" ht="18.75">
+      <c r="A12" s="181" t="s">
+        <v>681</v>
+      </c>
+      <c r="B12" s="160" t="s">
         <v>677</v>
       </c>
-      <c r="D3" s="219"/>
-      <c r="E3" s="219"/>
-      <c r="F3" s="219"/>
-      <c r="G3" s="219"/>
-      <c r="H3" s="219"/>
-      <c r="I3" s="219"/>
-      <c r="J3" s="150"/>
-    </row>
-    <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="249"/>
-      <c r="B4" s="228" t="s">
-        <v>326</v>
-      </c>
-      <c r="C4" s="231" t="s">
+      <c r="C12" s="161" t="s">
+        <v>730</v>
+      </c>
+      <c r="D12" s="151"/>
+      <c r="E12" s="151"/>
+      <c r="F12" s="151"/>
+      <c r="G12" s="151"/>
+      <c r="H12" s="151"/>
+      <c r="I12" s="151"/>
+      <c r="J12" s="149"/>
+    </row>
+    <row r="13" spans="1:10" ht="18.75">
+      <c r="A13" s="182"/>
+      <c r="B13" s="159" t="s">
         <v>678</v>
       </c>
-      <c r="D4" s="219"/>
-      <c r="E4" s="219"/>
-      <c r="F4" s="219"/>
-      <c r="G4" s="219"/>
-      <c r="H4" s="219"/>
-      <c r="I4" s="219"/>
-      <c r="J4" s="150"/>
-    </row>
-    <row r="5" spans="1:10" ht="18.75">
-      <c r="A5" s="249"/>
-      <c r="B5" s="228" t="s">
-        <v>327</v>
-      </c>
-      <c r="C5" s="231" t="s">
+      <c r="C13" s="162" t="s">
+        <v>731</v>
+      </c>
+      <c r="D13" s="151"/>
+      <c r="E13" s="151"/>
+      <c r="F13" s="151"/>
+      <c r="G13" s="151"/>
+      <c r="H13" s="151"/>
+      <c r="I13" s="151"/>
+      <c r="J13" s="149"/>
+    </row>
+    <row r="14" spans="1:10" ht="18.75">
+      <c r="A14" s="182"/>
+      <c r="B14" s="159" t="s">
         <v>679</v>
       </c>
-      <c r="D5" s="219"/>
-      <c r="E5" s="219"/>
-      <c r="F5" s="219"/>
-      <c r="G5" s="219"/>
-      <c r="H5" s="219"/>
-      <c r="I5" s="219"/>
-      <c r="J5" s="150"/>
-    </row>
-    <row r="6" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A6" s="250"/>
-      <c r="B6" s="232" t="s">
-        <v>328</v>
-      </c>
-      <c r="C6" s="233" t="s">
+      <c r="C14" s="162" t="s">
+        <v>732</v>
+      </c>
+      <c r="D14" s="151"/>
+      <c r="E14" s="151"/>
+      <c r="F14" s="151"/>
+      <c r="G14" s="151"/>
+      <c r="H14" s="151"/>
+      <c r="I14" s="151"/>
+      <c r="J14" s="149"/>
+    </row>
+    <row r="15" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A15" s="183"/>
+      <c r="B15" s="163" t="s">
         <v>680</v>
       </c>
-      <c r="D6" s="219"/>
-      <c r="E6" s="219"/>
-      <c r="F6" s="219"/>
-      <c r="G6" s="219"/>
-      <c r="H6" s="219"/>
-      <c r="I6" s="219"/>
-      <c r="J6" s="150"/>
-    </row>
-    <row r="7" spans="1:10" ht="18.75">
-      <c r="A7" s="248" t="s">
-        <v>715</v>
-      </c>
-      <c r="B7" s="229" t="s">
+      <c r="C15" s="164" t="s">
+        <v>733</v>
+      </c>
+      <c r="D15" s="151"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="151"/>
+      <c r="G15" s="151"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="151"/>
+      <c r="J15" s="149"/>
+    </row>
+    <row r="16" spans="1:10" ht="18.75">
+      <c r="A16" s="181" t="s">
+        <v>682</v>
+      </c>
+      <c r="B16" s="160" t="s">
+        <v>684</v>
+      </c>
+      <c r="C16" s="161" t="s">
+        <v>734</v>
+      </c>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="149"/>
+    </row>
+    <row r="17" spans="1:10" ht="18.75">
+      <c r="A17" s="182"/>
+      <c r="B17" s="159" t="s">
         <v>685</v>
       </c>
-      <c r="C7" s="230" t="s">
-        <v>692</v>
-      </c>
-      <c r="D7" s="219"/>
-      <c r="E7" s="219"/>
-      <c r="F7" s="219"/>
-      <c r="G7" s="219"/>
-      <c r="H7" s="219"/>
-      <c r="I7" s="219"/>
-      <c r="J7" s="150"/>
-    </row>
-    <row r="8" spans="1:10" ht="18.75">
-      <c r="A8" s="249"/>
-      <c r="B8" s="228" t="s">
+      <c r="C17" s="162" t="s">
+        <v>735</v>
+      </c>
+      <c r="D17" s="151"/>
+      <c r="E17" s="151"/>
+      <c r="F17" s="151"/>
+      <c r="G17" s="151"/>
+      <c r="H17" s="151"/>
+      <c r="I17" s="151"/>
+      <c r="J17" s="149"/>
+    </row>
+    <row r="18" spans="1:10" ht="18.75">
+      <c r="A18" s="182"/>
+      <c r="B18" s="159" t="s">
         <v>686</v>
       </c>
-      <c r="C8" s="231" t="s">
-        <v>689</v>
-      </c>
-      <c r="D8" s="219"/>
-      <c r="E8" s="219"/>
-      <c r="F8" s="219"/>
-      <c r="G8" s="219"/>
-      <c r="H8" s="219"/>
-      <c r="I8" s="219"/>
-      <c r="J8" s="150"/>
-    </row>
-    <row r="9" spans="1:10" ht="18.75">
-      <c r="A9" s="249"/>
-      <c r="B9" s="228" t="s">
+      <c r="C18" s="162" t="s">
+        <v>736</v>
+      </c>
+      <c r="D18" s="151"/>
+      <c r="E18" s="151"/>
+      <c r="F18" s="151"/>
+      <c r="G18" s="151"/>
+      <c r="H18" s="151"/>
+      <c r="I18" s="151"/>
+      <c r="J18" s="149"/>
+    </row>
+    <row r="19" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A19" s="183"/>
+      <c r="B19" s="163" t="s">
         <v>687</v>
       </c>
-      <c r="C9" s="231" t="s">
-        <v>690</v>
-      </c>
-      <c r="D9" s="219"/>
-      <c r="E9" s="219"/>
-      <c r="F9" s="219"/>
-      <c r="G9" s="219"/>
-      <c r="H9" s="219"/>
-      <c r="I9" s="219"/>
-      <c r="J9" s="150"/>
-    </row>
-    <row r="10" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A10" s="250"/>
-      <c r="B10" s="232" t="s">
-        <v>688</v>
-      </c>
-      <c r="C10" s="233" t="s">
+      <c r="C19" s="164" t="s">
+        <v>737</v>
+      </c>
+      <c r="D19" s="151"/>
+      <c r="E19" s="151"/>
+      <c r="F19" s="151"/>
+      <c r="G19" s="151"/>
+      <c r="H19" s="151"/>
+      <c r="I19" s="151"/>
+      <c r="J19" s="149"/>
+    </row>
+    <row r="20" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A20" s="153"/>
+      <c r="B20" s="152"/>
+      <c r="C20" s="152"/>
+      <c r="D20" s="151"/>
+      <c r="E20" s="151"/>
+      <c r="F20" s="151"/>
+      <c r="G20" s="151"/>
+      <c r="H20" s="151"/>
+      <c r="I20" s="151"/>
+      <c r="J20" s="149"/>
+    </row>
+    <row r="21" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A21" s="178" t="s">
+        <v>720</v>
+      </c>
+      <c r="B21" s="179"/>
+      <c r="C21" s="180"/>
+      <c r="D21" s="151"/>
+      <c r="E21" s="151"/>
+      <c r="F21" s="151"/>
+      <c r="G21" s="151"/>
+      <c r="H21" s="151"/>
+      <c r="I21" s="151"/>
+      <c r="J21" s="149"/>
+    </row>
+    <row r="22" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A22" s="165" t="s">
+        <v>218</v>
+      </c>
+      <c r="B22" s="165" t="s">
+        <v>282</v>
+      </c>
+      <c r="C22" s="166" t="s">
+        <v>325</v>
+      </c>
+      <c r="D22" s="151"/>
+      <c r="E22" s="151"/>
+      <c r="F22" s="151"/>
+      <c r="G22" s="151"/>
+      <c r="H22" s="151"/>
+      <c r="I22" s="151"/>
+      <c r="J22" s="149"/>
+    </row>
+    <row r="23" spans="1:10" ht="18.75">
+      <c r="A23" s="175" t="s">
+        <v>507</v>
+      </c>
+      <c r="B23" s="160" t="s">
         <v>691</v>
       </c>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="219"/>
-      <c r="H10" s="219"/>
-      <c r="I10" s="219"/>
-      <c r="J10" s="150"/>
-    </row>
-    <row r="11" spans="1:10" ht="18.75">
-      <c r="A11" s="248" t="s">
-        <v>713</v>
-      </c>
-      <c r="B11" s="229" t="s">
+      <c r="C23" s="161" t="s">
+        <v>738</v>
+      </c>
+      <c r="D23" s="151"/>
+      <c r="E23" s="154"/>
+      <c r="F23" s="151"/>
+      <c r="G23" s="151"/>
+      <c r="H23" s="151"/>
+      <c r="I23" s="151"/>
+      <c r="J23" s="149"/>
+    </row>
+    <row r="24" spans="1:10" ht="18.75">
+      <c r="A24" s="176"/>
+      <c r="B24" s="159" t="s">
+        <v>695</v>
+      </c>
+      <c r="C24" s="162" t="s">
+        <v>739</v>
+      </c>
+      <c r="D24" s="151"/>
+      <c r="E24" s="154"/>
+      <c r="F24" s="151"/>
+      <c r="G24" s="151"/>
+      <c r="H24" s="151"/>
+      <c r="I24" s="151"/>
+      <c r="J24" s="149"/>
+    </row>
+    <row r="25" spans="1:10" ht="18.75">
+      <c r="A25" s="176"/>
+      <c r="B25" s="159" t="s">
+        <v>696</v>
+      </c>
+      <c r="C25" s="162" t="s">
+        <v>740</v>
+      </c>
+      <c r="D25" s="151"/>
+      <c r="E25" s="151"/>
+      <c r="F25" s="151"/>
+      <c r="G25" s="151"/>
+      <c r="H25" s="151"/>
+      <c r="I25" s="151"/>
+      <c r="J25" s="149"/>
+    </row>
+    <row r="26" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A26" s="177"/>
+      <c r="B26" s="163" t="s">
         <v>697</v>
       </c>
-      <c r="C11" s="230" t="s">
+      <c r="C26" s="164" t="s">
+        <v>741</v>
+      </c>
+      <c r="D26" s="151"/>
+      <c r="E26" s="151"/>
+      <c r="F26" s="151"/>
+      <c r="G26" s="151"/>
+      <c r="H26" s="151"/>
+      <c r="I26" s="151"/>
+      <c r="J26" s="149"/>
+    </row>
+    <row r="27" spans="1:10" ht="18.75">
+      <c r="A27" s="175" t="s">
+        <v>703</v>
+      </c>
+      <c r="B27" s="160" t="s">
+        <v>699</v>
+      </c>
+      <c r="C27" s="161" t="s">
+        <v>742</v>
+      </c>
+      <c r="D27" s="151"/>
+      <c r="E27" s="151"/>
+      <c r="F27" s="151"/>
+      <c r="G27" s="151"/>
+      <c r="H27" s="151"/>
+      <c r="I27" s="151"/>
+      <c r="J27" s="149"/>
+    </row>
+    <row r="28" spans="1:10" ht="18.75">
+      <c r="A28" s="176"/>
+      <c r="B28" s="159" t="s">
+        <v>700</v>
+      </c>
+      <c r="C28" s="162" t="s">
+        <v>743</v>
+      </c>
+      <c r="D28" s="151"/>
+      <c r="E28" s="151"/>
+      <c r="F28" s="151"/>
+      <c r="G28" s="151"/>
+      <c r="H28" s="151"/>
+      <c r="I28" s="151"/>
+      <c r="J28" s="149"/>
+    </row>
+    <row r="29" spans="1:10" ht="18.75">
+      <c r="A29" s="176"/>
+      <c r="B29" s="159" t="s">
         <v>701</v>
       </c>
-      <c r="D11" s="219"/>
-      <c r="E11" s="219"/>
-      <c r="F11" s="219"/>
-      <c r="G11" s="219"/>
-      <c r="H11" s="219"/>
-      <c r="I11" s="219"/>
-      <c r="J11" s="150"/>
-    </row>
-    <row r="12" spans="1:10" ht="18.75">
-      <c r="A12" s="249"/>
-      <c r="B12" s="228" t="s">
-        <v>698</v>
-      </c>
-      <c r="C12" s="231" t="s">
+      <c r="C29" s="162" t="s">
+        <v>744</v>
+      </c>
+      <c r="D29" s="151"/>
+      <c r="E29" s="151"/>
+      <c r="F29" s="151"/>
+      <c r="G29" s="151"/>
+      <c r="H29" s="151"/>
+      <c r="I29" s="151"/>
+      <c r="J29" s="149"/>
+    </row>
+    <row r="30" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A30" s="177"/>
+      <c r="B30" s="163" t="s">
         <v>702</v>
       </c>
-      <c r="D12" s="219"/>
-      <c r="E12" s="219"/>
-      <c r="F12" s="219"/>
-      <c r="G12" s="219"/>
-      <c r="H12" s="219"/>
-      <c r="I12" s="219"/>
-      <c r="J12" s="150"/>
-    </row>
-    <row r="13" spans="1:10" ht="18.75">
-      <c r="A13" s="249"/>
-      <c r="B13" s="228" t="s">
-        <v>699</v>
-      </c>
-      <c r="C13" s="231" t="s">
-        <v>703</v>
-      </c>
-      <c r="D13" s="219"/>
-      <c r="E13" s="219"/>
-      <c r="F13" s="219"/>
-      <c r="G13" s="219"/>
-      <c r="H13" s="219"/>
-      <c r="I13" s="219"/>
-      <c r="J13" s="150"/>
-    </row>
-    <row r="14" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A14" s="250"/>
-      <c r="B14" s="232" t="s">
-        <v>700</v>
-      </c>
-      <c r="C14" s="233" t="s">
-        <v>704</v>
-      </c>
-      <c r="D14" s="219"/>
-      <c r="E14" s="219"/>
-      <c r="F14" s="219"/>
-      <c r="G14" s="219"/>
-      <c r="H14" s="219"/>
-      <c r="I14" s="219"/>
-      <c r="J14" s="150"/>
-    </row>
-    <row r="15" spans="1:10" ht="18.75">
-      <c r="A15" s="248" t="s">
+      <c r="C30" s="164" t="s">
+        <v>745</v>
+      </c>
+      <c r="D30" s="151"/>
+      <c r="E30" s="151"/>
+      <c r="F30" s="151"/>
+      <c r="G30" s="151"/>
+      <c r="H30" s="151"/>
+      <c r="I30" s="151"/>
+      <c r="J30" s="149"/>
+    </row>
+    <row r="31" spans="1:10" ht="18.75">
+      <c r="A31" s="175" t="s">
+        <v>707</v>
+      </c>
+      <c r="B31" s="160" t="s">
+        <v>708</v>
+      </c>
+      <c r="C31" s="161" t="s">
+        <v>746</v>
+      </c>
+      <c r="D31" s="151"/>
+      <c r="E31" s="151"/>
+      <c r="F31" s="151"/>
+      <c r="G31" s="151"/>
+      <c r="H31" s="151"/>
+      <c r="I31" s="151"/>
+      <c r="J31" s="149"/>
+    </row>
+    <row r="32" spans="1:10" ht="18.75">
+      <c r="A32" s="176"/>
+      <c r="B32" s="159" t="s">
+        <v>709</v>
+      </c>
+      <c r="C32" s="162" t="s">
+        <v>747</v>
+      </c>
+      <c r="D32" s="151"/>
+      <c r="E32" s="151"/>
+      <c r="F32" s="151"/>
+      <c r="G32" s="151"/>
+      <c r="H32" s="151"/>
+      <c r="I32" s="151"/>
+      <c r="J32" s="149"/>
+    </row>
+    <row r="33" spans="1:10" ht="18.75">
+      <c r="A33" s="176"/>
+      <c r="B33" s="159" t="s">
+        <v>710</v>
+      </c>
+      <c r="C33" s="162" t="s">
+        <v>748</v>
+      </c>
+      <c r="D33" s="151"/>
+      <c r="E33" s="151"/>
+      <c r="F33" s="151"/>
+      <c r="G33" s="154"/>
+      <c r="H33" s="151"/>
+      <c r="I33" s="151"/>
+      <c r="J33" s="149"/>
+    </row>
+    <row r="34" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A34" s="177"/>
+      <c r="B34" s="163" t="s">
+        <v>711</v>
+      </c>
+      <c r="C34" s="164" t="s">
+        <v>749</v>
+      </c>
+      <c r="D34" s="151"/>
+      <c r="E34" s="151"/>
+      <c r="F34" s="151"/>
+      <c r="G34" s="154"/>
+      <c r="H34" s="151"/>
+      <c r="I34" s="151"/>
+      <c r="J34" s="149"/>
+    </row>
+    <row r="35" spans="1:10" ht="18.75">
+      <c r="A35" s="175" t="s">
         <v>714</v>
       </c>
-      <c r="B15" s="229" t="s">
+      <c r="B35" s="160" t="s">
+        <v>719</v>
+      </c>
+      <c r="C35" s="167">
+        <v>11441</v>
+      </c>
+      <c r="D35" s="151"/>
+      <c r="E35" s="151"/>
+      <c r="F35" s="151"/>
+      <c r="G35" s="154"/>
+      <c r="H35" s="151"/>
+      <c r="I35" s="151"/>
+      <c r="J35" s="149"/>
+    </row>
+    <row r="36" spans="1:10" ht="18.75">
+      <c r="A36" s="176"/>
+      <c r="B36" s="159" t="s">
         <v>716</v>
       </c>
-      <c r="C15" s="230" t="s">
-        <v>709</v>
-      </c>
-      <c r="D15" s="219"/>
-      <c r="E15" s="219"/>
-      <c r="F15" s="219"/>
-      <c r="G15" s="219"/>
-      <c r="H15" s="219"/>
-      <c r="I15" s="219"/>
-      <c r="J15" s="150"/>
-    </row>
-    <row r="16" spans="1:10" ht="18.75">
-      <c r="A16" s="249"/>
-      <c r="B16" s="228" t="s">
+      <c r="C36" s="168">
+        <v>11442</v>
+      </c>
+      <c r="D36" s="151"/>
+      <c r="E36" s="151"/>
+      <c r="F36" s="151"/>
+      <c r="G36" s="154"/>
+      <c r="H36" s="151"/>
+      <c r="I36" s="151"/>
+      <c r="J36" s="149"/>
+    </row>
+    <row r="37" spans="1:10" ht="18.75">
+      <c r="A37" s="176"/>
+      <c r="B37" s="159" t="s">
         <v>717</v>
       </c>
-      <c r="C16" s="231" t="s">
-        <v>710</v>
-      </c>
-      <c r="D16" s="219"/>
-      <c r="E16" s="219"/>
-      <c r="F16" s="219"/>
-      <c r="G16" s="219"/>
-      <c r="H16" s="219"/>
-      <c r="I16" s="219"/>
-      <c r="J16" s="150"/>
-    </row>
-    <row r="17" spans="1:10" ht="18.75">
-      <c r="A17" s="249"/>
-      <c r="B17" s="228" t="s">
+      <c r="C37" s="168">
+        <v>11443</v>
+      </c>
+      <c r="D37" s="151"/>
+      <c r="E37" s="151"/>
+      <c r="F37" s="151"/>
+      <c r="G37" s="154"/>
+      <c r="H37" s="151"/>
+      <c r="I37" s="151"/>
+      <c r="J37" s="149"/>
+    </row>
+    <row r="38" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A38" s="177"/>
+      <c r="B38" s="163" t="s">
         <v>718</v>
       </c>
-      <c r="C17" s="231" t="s">
-        <v>711</v>
-      </c>
-      <c r="D17" s="219"/>
-      <c r="E17" s="219"/>
-      <c r="F17" s="219"/>
-      <c r="G17" s="219"/>
-      <c r="H17" s="219"/>
-      <c r="I17" s="219"/>
-      <c r="J17" s="150"/>
-    </row>
-    <row r="18" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A18" s="250"/>
-      <c r="B18" s="232" t="s">
-        <v>719</v>
-      </c>
-      <c r="C18" s="233" t="s">
-        <v>712</v>
-      </c>
-      <c r="D18" s="219"/>
-      <c r="E18" s="219"/>
-      <c r="F18" s="219"/>
-      <c r="G18" s="219"/>
-      <c r="H18" s="219"/>
-      <c r="I18" s="219"/>
-      <c r="J18" s="150"/>
-    </row>
-    <row r="19" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A19" s="222"/>
-      <c r="B19" s="221"/>
-      <c r="C19" s="221"/>
-      <c r="D19" s="219"/>
-      <c r="E19" s="219"/>
-      <c r="F19" s="219"/>
-      <c r="G19" s="219"/>
-      <c r="H19" s="219"/>
-      <c r="I19" s="219"/>
-      <c r="J19" s="150"/>
-    </row>
-    <row r="20" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A20" s="236" t="s">
-        <v>761</v>
-      </c>
-      <c r="B20" s="237"/>
-      <c r="C20" s="238"/>
-      <c r="D20" s="219"/>
-      <c r="E20" s="219"/>
-      <c r="F20" s="219"/>
-      <c r="G20" s="219"/>
-      <c r="H20" s="219"/>
-      <c r="I20" s="219"/>
-      <c r="J20" s="150"/>
-    </row>
-    <row r="21" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A21" s="234" t="s">
-        <v>218</v>
-      </c>
-      <c r="B21" s="234" t="s">
-        <v>282</v>
-      </c>
-      <c r="C21" s="235" t="s">
-        <v>325</v>
-      </c>
-      <c r="D21" s="219"/>
-      <c r="E21" s="219"/>
-      <c r="F21" s="219"/>
-      <c r="G21" s="219"/>
-      <c r="H21" s="219"/>
-      <c r="I21" s="219"/>
-      <c r="J21" s="150"/>
-    </row>
-    <row r="22" spans="1:10" ht="18.75">
-      <c r="A22" s="239" t="s">
-        <v>507</v>
-      </c>
-      <c r="B22" s="229" t="s">
-        <v>723</v>
-      </c>
-      <c r="C22" s="230" t="s">
-        <v>724</v>
-      </c>
-      <c r="D22" s="219"/>
-      <c r="E22" s="223"/>
-      <c r="F22" s="219"/>
-      <c r="G22" s="219"/>
-      <c r="H22" s="219"/>
-      <c r="I22" s="219"/>
-      <c r="J22" s="150"/>
-    </row>
-    <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="240"/>
-      <c r="B23" s="228" t="s">
-        <v>728</v>
-      </c>
-      <c r="C23" s="231" t="s">
-        <v>731</v>
-      </c>
-      <c r="D23" s="219"/>
-      <c r="E23" s="223"/>
-      <c r="F23" s="219"/>
-      <c r="G23" s="219"/>
-      <c r="H23" s="219"/>
-      <c r="I23" s="219"/>
-      <c r="J23" s="150"/>
-    </row>
-    <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="240"/>
-      <c r="B24" s="228" t="s">
-        <v>729</v>
-      </c>
-      <c r="C24" s="231" t="s">
-        <v>732</v>
-      </c>
-      <c r="D24" s="219"/>
-      <c r="E24" s="219"/>
-      <c r="F24" s="219"/>
-      <c r="G24" s="219"/>
-      <c r="H24" s="219"/>
-      <c r="I24" s="219"/>
-      <c r="J24" s="150"/>
-    </row>
-    <row r="25" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A25" s="241"/>
-      <c r="B25" s="232" t="s">
-        <v>730</v>
-      </c>
-      <c r="C25" s="233" t="s">
-        <v>733</v>
-      </c>
-      <c r="D25" s="219"/>
-      <c r="E25" s="219"/>
-      <c r="F25" s="219"/>
-      <c r="G25" s="219"/>
-      <c r="H25" s="219"/>
-      <c r="I25" s="219"/>
-      <c r="J25" s="150"/>
-    </row>
-    <row r="26" spans="1:10" ht="18.75">
-      <c r="A26" s="239" t="s">
-        <v>740</v>
-      </c>
-      <c r="B26" s="229" t="s">
-        <v>735</v>
-      </c>
-      <c r="C26" s="230" t="s">
-        <v>739</v>
-      </c>
-      <c r="D26" s="219"/>
-      <c r="E26" s="219"/>
-      <c r="F26" s="219"/>
-      <c r="G26" s="219"/>
-      <c r="H26" s="219"/>
-      <c r="I26" s="219"/>
-      <c r="J26" s="150"/>
-    </row>
-    <row r="27" spans="1:10" ht="18.75">
-      <c r="A27" s="240"/>
-      <c r="B27" s="228" t="s">
-        <v>736</v>
-      </c>
-      <c r="C27" s="231">
-        <v>11322</v>
-      </c>
-      <c r="D27" s="219"/>
-      <c r="E27" s="219"/>
-      <c r="F27" s="219"/>
-      <c r="G27" s="219"/>
-      <c r="H27" s="219"/>
-      <c r="I27" s="219"/>
-      <c r="J27" s="150"/>
-    </row>
-    <row r="28" spans="1:10" ht="18.75">
-      <c r="A28" s="240"/>
-      <c r="B28" s="228" t="s">
-        <v>737</v>
-      </c>
-      <c r="C28" s="231">
-        <v>11323</v>
-      </c>
-      <c r="D28" s="219"/>
-      <c r="E28" s="219"/>
-      <c r="F28" s="219"/>
-      <c r="G28" s="219"/>
-      <c r="H28" s="219"/>
-      <c r="I28" s="219"/>
-      <c r="J28" s="150"/>
-    </row>
-    <row r="29" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A29" s="241"/>
-      <c r="B29" s="232" t="s">
-        <v>738</v>
-      </c>
-      <c r="C29" s="233">
-        <v>11324</v>
-      </c>
-      <c r="D29" s="219"/>
-      <c r="E29" s="219"/>
-      <c r="F29" s="219"/>
-      <c r="G29" s="219"/>
-      <c r="H29" s="219"/>
-      <c r="I29" s="219"/>
-      <c r="J29" s="150"/>
-    </row>
-    <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="239" t="s">
-        <v>748</v>
-      </c>
-      <c r="B30" s="229" t="s">
-        <v>749</v>
-      </c>
-      <c r="C30" s="230" t="s">
-        <v>744</v>
-      </c>
-      <c r="D30" s="219"/>
-      <c r="E30" s="219"/>
-      <c r="F30" s="219"/>
-      <c r="G30" s="219"/>
-      <c r="H30" s="219"/>
-      <c r="I30" s="219"/>
-      <c r="J30" s="150"/>
-    </row>
-    <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="240"/>
-      <c r="B31" s="228" t="s">
-        <v>750</v>
-      </c>
-      <c r="C31" s="231" t="s">
-        <v>745</v>
-      </c>
-      <c r="D31" s="219"/>
-      <c r="E31" s="219"/>
-      <c r="F31" s="219"/>
-      <c r="G31" s="219"/>
-      <c r="H31" s="219"/>
-      <c r="I31" s="219"/>
-      <c r="J31" s="150"/>
-    </row>
-    <row r="32" spans="1:10" ht="18.75">
-      <c r="A32" s="240"/>
-      <c r="B32" s="228" t="s">
-        <v>751</v>
-      </c>
-      <c r="C32" s="231" t="s">
-        <v>746</v>
-      </c>
-      <c r="D32" s="219"/>
-      <c r="E32" s="219"/>
-      <c r="F32" s="219"/>
-      <c r="G32" s="223"/>
-      <c r="H32" s="219"/>
-      <c r="I32" s="219"/>
-      <c r="J32" s="150"/>
-    </row>
-    <row r="33" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A33" s="241"/>
-      <c r="B33" s="232" t="s">
-        <v>752</v>
-      </c>
-      <c r="C33" s="233" t="s">
-        <v>747</v>
-      </c>
-      <c r="D33" s="219"/>
-      <c r="E33" s="219"/>
-      <c r="F33" s="219"/>
-      <c r="G33" s="223"/>
-      <c r="H33" s="219"/>
-      <c r="I33" s="219"/>
-      <c r="J33" s="150"/>
-    </row>
-    <row r="34" spans="1:10" ht="18.75">
-      <c r="A34" s="239" t="s">
-        <v>755</v>
-      </c>
-      <c r="B34" s="229" t="s">
-        <v>760</v>
-      </c>
-      <c r="C34" s="242">
-        <v>11341</v>
-      </c>
-      <c r="D34" s="219"/>
-      <c r="E34" s="219"/>
-      <c r="F34" s="219"/>
-      <c r="G34" s="223"/>
-      <c r="H34" s="219"/>
-      <c r="I34" s="219"/>
-      <c r="J34" s="150"/>
-    </row>
-    <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="240"/>
-      <c r="B35" s="228" t="s">
-        <v>757</v>
-      </c>
-      <c r="C35" s="243">
-        <v>11342</v>
-      </c>
-      <c r="D35" s="219"/>
-      <c r="E35" s="219"/>
-      <c r="F35" s="219"/>
-      <c r="G35" s="223"/>
-      <c r="H35" s="219"/>
-      <c r="I35" s="219"/>
-      <c r="J35" s="150"/>
-    </row>
-    <row r="36" spans="1:10" ht="18.75">
-      <c r="A36" s="240"/>
-      <c r="B36" s="228" t="s">
-        <v>758</v>
-      </c>
-      <c r="C36" s="243">
-        <v>11343</v>
-      </c>
-      <c r="D36" s="219"/>
-      <c r="E36" s="219"/>
-      <c r="F36" s="219"/>
-      <c r="G36" s="223"/>
-      <c r="H36" s="219"/>
-      <c r="I36" s="219"/>
-      <c r="J36" s="150"/>
-    </row>
-    <row r="37" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A37" s="241"/>
-      <c r="B37" s="232" t="s">
-        <v>759</v>
-      </c>
-      <c r="C37" s="244">
-        <v>11344</v>
-      </c>
-      <c r="D37" s="219"/>
-      <c r="E37" s="219"/>
-      <c r="F37" s="219"/>
-      <c r="G37" s="223"/>
-      <c r="H37" s="219"/>
-      <c r="I37" s="219"/>
-      <c r="J37" s="150"/>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="224"/>
-      <c r="B38" s="219"/>
-      <c r="C38" s="219"/>
-      <c r="D38" s="219"/>
-      <c r="E38" s="219"/>
-      <c r="F38" s="219"/>
-      <c r="G38" s="223"/>
-      <c r="H38" s="219"/>
-      <c r="I38" s="219"/>
-      <c r="J38" s="150"/>
+      <c r="C38" s="169">
+        <v>11444</v>
+      </c>
+      <c r="D38" s="151"/>
+      <c r="E38" s="151"/>
+      <c r="F38" s="151"/>
+      <c r="G38" s="154"/>
+      <c r="H38" s="151"/>
+      <c r="I38" s="151"/>
+      <c r="J38" s="149"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="224"/>
-      <c r="B39" s="219"/>
-      <c r="C39" s="219"/>
-      <c r="D39" s="219"/>
-      <c r="E39" s="219"/>
-      <c r="F39" s="219"/>
-      <c r="G39" s="223"/>
-      <c r="H39" s="219"/>
-      <c r="I39" s="219"/>
-      <c r="J39" s="150"/>
+      <c r="A39" s="155"/>
+      <c r="B39" s="151"/>
+      <c r="C39" s="151"/>
+      <c r="D39" s="151"/>
+      <c r="E39" s="151"/>
+      <c r="F39" s="151"/>
+      <c r="G39" s="154"/>
+      <c r="H39" s="151"/>
+      <c r="I39" s="151"/>
+      <c r="J39" s="149"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="224"/>
-      <c r="B40" s="219"/>
-      <c r="C40" s="219"/>
-      <c r="D40" s="219"/>
-      <c r="E40" s="219"/>
-      <c r="F40" s="219"/>
-      <c r="G40" s="223"/>
-      <c r="H40" s="219"/>
-      <c r="I40" s="219"/>
-      <c r="J40" s="150"/>
+      <c r="A40" s="155"/>
+      <c r="B40" s="151"/>
+      <c r="C40" s="151"/>
+      <c r="D40" s="151"/>
+      <c r="E40" s="151"/>
+      <c r="F40" s="151"/>
+      <c r="G40" s="154"/>
+      <c r="H40" s="151"/>
+      <c r="I40" s="151"/>
+      <c r="J40" s="149"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="224"/>
-      <c r="B41" s="219"/>
-      <c r="C41" s="219"/>
-      <c r="D41" s="219"/>
-      <c r="E41" s="219"/>
-      <c r="F41" s="219"/>
-      <c r="G41" s="223"/>
-      <c r="H41" s="219"/>
-      <c r="I41" s="219"/>
-      <c r="J41" s="150"/>
+      <c r="A41" s="155"/>
+      <c r="B41" s="151"/>
+      <c r="C41" s="151"/>
+      <c r="D41" s="151"/>
+      <c r="E41" s="151"/>
+      <c r="F41" s="151"/>
+      <c r="G41" s="154"/>
+      <c r="H41" s="151"/>
+      <c r="I41" s="151"/>
+      <c r="J41" s="149"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="224"/>
-      <c r="B42" s="219"/>
-      <c r="C42" s="219"/>
-      <c r="D42" s="219"/>
-      <c r="E42" s="219"/>
-      <c r="F42" s="219"/>
-      <c r="G42" s="223"/>
-      <c r="H42" s="219"/>
-      <c r="I42" s="219"/>
-      <c r="J42" s="150"/>
+      <c r="A42" s="155"/>
+      <c r="B42" s="151"/>
+      <c r="C42" s="151"/>
+      <c r="D42" s="151"/>
+      <c r="E42" s="151"/>
+      <c r="F42" s="151"/>
+      <c r="G42" s="154"/>
+      <c r="H42" s="151"/>
+      <c r="I42" s="151"/>
+      <c r="J42" s="149"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="224"/>
-      <c r="B43" s="219"/>
-      <c r="C43" s="219"/>
-      <c r="D43" s="219"/>
-      <c r="E43" s="219"/>
-      <c r="F43" s="219"/>
-      <c r="G43" s="223"/>
-      <c r="H43" s="219"/>
-      <c r="I43" s="219"/>
-      <c r="J43" s="150"/>
+      <c r="A43" s="155"/>
+      <c r="B43" s="151"/>
+      <c r="C43" s="151"/>
+      <c r="D43" s="151"/>
+      <c r="E43" s="151"/>
+      <c r="F43" s="151"/>
+      <c r="G43" s="154"/>
+      <c r="H43" s="151"/>
+      <c r="I43" s="151"/>
+      <c r="J43" s="149"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="224"/>
-      <c r="B44" s="219"/>
-      <c r="C44" s="219"/>
-      <c r="D44" s="219"/>
-      <c r="E44" s="219"/>
-      <c r="F44" s="219"/>
-      <c r="G44" s="223"/>
-      <c r="H44" s="219"/>
-      <c r="I44" s="219"/>
-      <c r="J44" s="150"/>
+      <c r="A44" s="155"/>
+      <c r="B44" s="151"/>
+      <c r="C44" s="151"/>
+      <c r="D44" s="151"/>
+      <c r="E44" s="151"/>
+      <c r="F44" s="151"/>
+      <c r="G44" s="154"/>
+      <c r="H44" s="151"/>
+      <c r="I44" s="151"/>
+      <c r="J44" s="149"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="224"/>
-      <c r="B45" s="219"/>
-      <c r="C45" s="219"/>
-      <c r="D45" s="219"/>
-      <c r="E45" s="219"/>
-      <c r="F45" s="219"/>
-      <c r="G45" s="219"/>
-      <c r="H45" s="219"/>
-      <c r="I45" s="223"/>
-      <c r="J45" s="150"/>
-    </row>
-    <row r="46" spans="1:10" ht="46.5" customHeight="1" thickBot="1">
-      <c r="A46" s="225"/>
-      <c r="B46" s="226"/>
-      <c r="C46" s="226"/>
-      <c r="D46" s="226"/>
-      <c r="E46" s="226"/>
-      <c r="F46" s="226"/>
-      <c r="G46" s="226"/>
-      <c r="H46" s="226"/>
-      <c r="I46" s="227"/>
-      <c r="J46" s="151"/>
+      <c r="A45" s="155"/>
+      <c r="B45" s="151"/>
+      <c r="C45" s="151"/>
+      <c r="D45" s="151"/>
+      <c r="E45" s="151"/>
+      <c r="F45" s="151"/>
+      <c r="G45" s="154"/>
+      <c r="H45" s="151"/>
+      <c r="I45" s="151"/>
+      <c r="J45" s="149"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="155"/>
+      <c r="B46" s="151"/>
+      <c r="C46" s="151"/>
+      <c r="D46" s="151"/>
+      <c r="E46" s="151"/>
+      <c r="F46" s="151"/>
+      <c r="G46" s="151"/>
+      <c r="H46" s="151"/>
+      <c r="I46" s="154"/>
+      <c r="J46" s="149"/>
+    </row>
+    <row r="47" spans="1:10" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A47" s="156"/>
+      <c r="B47" s="157"/>
+      <c r="C47" s="157"/>
+      <c r="D47" s="157"/>
+      <c r="E47" s="157"/>
+      <c r="F47" s="157"/>
+      <c r="G47" s="157"/>
+      <c r="H47" s="157"/>
+      <c r="I47" s="158"/>
+      <c r="J47" s="150"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
+  <mergeCells count="11">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C3:C6 C7:C10 C11:C14 C15:C19 C26:C29 C30:C33 C34:C36 C21:C25" numberStoredAsText="1"/>
+    <ignoredError sqref="C20 C22 C4:C19 C23:C38" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -9082,40 +9204,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="184" t="s">
         <v>330</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
-      <c r="G1" s="162"/>
-      <c r="H1" s="163"/>
+      <c r="B1" s="185"/>
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="186"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="164"/>
-      <c r="B2" s="165"/>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="166"/>
+      <c r="A2" s="187"/>
+      <c r="B2" s="188"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="188"/>
+      <c r="G2" s="188"/>
+      <c r="H2" s="189"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="167" t="s">
+      <c r="A3" s="190" t="s">
         <v>253</v>
       </c>
-      <c r="B3" s="168"/>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168" t="s">
+      <c r="B3" s="191"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="191"/>
+      <c r="E3" s="191" t="s">
         <v>254</v>
       </c>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="169"/>
+      <c r="F3" s="191"/>
+      <c r="G3" s="191"/>
+      <c r="H3" s="192"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="20">
@@ -9649,11 +9771,11 @@
       <c r="C27" s="144" t="s">
         <v>609</v>
       </c>
-      <c r="D27" s="160" t="s">
+      <c r="D27" s="193" t="s">
         <v>585</v>
       </c>
-      <c r="E27" s="160"/>
-      <c r="F27" s="160"/>
+      <c r="E27" s="193"/>
+      <c r="F27" s="193"/>
       <c r="G27" s="25"/>
       <c r="H27" s="26"/>
     </row>
@@ -9665,11 +9787,11 @@
       <c r="C28" s="144" t="s">
         <v>613</v>
       </c>
-      <c r="D28" s="160" t="s">
+      <c r="D28" s="193" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="160"/>
-      <c r="F28" s="160"/>
+      <c r="E28" s="193"/>
+      <c r="F28" s="193"/>
       <c r="G28" s="25"/>
       <c r="H28" s="26"/>
     </row>
@@ -9681,11 +9803,11 @@
       <c r="C29" s="144" t="s">
         <v>614</v>
       </c>
-      <c r="D29" s="160" t="s">
+      <c r="D29" s="193" t="s">
         <v>586</v>
       </c>
-      <c r="E29" s="160"/>
-      <c r="F29" s="160"/>
+      <c r="E29" s="193"/>
+      <c r="F29" s="193"/>
       <c r="G29" s="25"/>
       <c r="H29" s="26"/>
     </row>
@@ -9697,11 +9819,11 @@
       <c r="C30" s="144" t="s">
         <v>615</v>
       </c>
-      <c r="D30" s="160" t="s">
+      <c r="D30" s="193" t="s">
         <v>587</v>
       </c>
-      <c r="E30" s="160"/>
-      <c r="F30" s="160"/>
+      <c r="E30" s="193"/>
+      <c r="F30" s="193"/>
       <c r="G30" s="25"/>
       <c r="H30" s="26"/>
     </row>
@@ -9713,11 +9835,11 @@
       <c r="C31" s="144" t="s">
         <v>616</v>
       </c>
-      <c r="D31" s="160" t="s">
+      <c r="D31" s="193" t="s">
         <v>588</v>
       </c>
-      <c r="E31" s="160"/>
-      <c r="F31" s="160"/>
+      <c r="E31" s="193"/>
+      <c r="F31" s="193"/>
       <c r="G31" s="25"/>
       <c r="H31" s="26"/>
     </row>
@@ -9729,11 +9851,11 @@
       <c r="C32" s="144" t="s">
         <v>617</v>
       </c>
-      <c r="D32" s="160" t="s">
+      <c r="D32" s="193" t="s">
         <v>589</v>
       </c>
-      <c r="E32" s="160"/>
-      <c r="F32" s="160"/>
+      <c r="E32" s="193"/>
+      <c r="F32" s="193"/>
       <c r="G32" s="25"/>
       <c r="H32" s="26"/>
     </row>
@@ -9745,11 +9867,11 @@
       <c r="C33" s="144" t="s">
         <v>630</v>
       </c>
-      <c r="D33" s="160" t="s">
+      <c r="D33" s="193" t="s">
         <v>489</v>
       </c>
-      <c r="E33" s="160"/>
-      <c r="F33" s="160"/>
+      <c r="E33" s="193"/>
+      <c r="F33" s="193"/>
       <c r="G33" s="25"/>
       <c r="H33" s="26"/>
     </row>
@@ -9761,11 +9883,11 @@
       <c r="C34" s="144" t="s">
         <v>631</v>
       </c>
-      <c r="D34" s="160" t="s">
+      <c r="D34" s="193" t="s">
         <v>590</v>
       </c>
-      <c r="E34" s="160"/>
-      <c r="F34" s="160"/>
+      <c r="E34" s="193"/>
+      <c r="F34" s="193"/>
       <c r="G34" s="25"/>
       <c r="H34" s="26"/>
     </row>
@@ -9777,11 +9899,11 @@
       <c r="C35" s="144" t="s">
         <v>632</v>
       </c>
-      <c r="D35" s="160" t="s">
+      <c r="D35" s="193" t="s">
         <v>591</v>
       </c>
-      <c r="E35" s="160"/>
-      <c r="F35" s="160"/>
+      <c r="E35" s="193"/>
+      <c r="F35" s="193"/>
       <c r="G35" s="25"/>
       <c r="H35" s="26"/>
     </row>
@@ -9791,11 +9913,11 @@
       <c r="C36" s="144" t="s">
         <v>667</v>
       </c>
-      <c r="D36" s="157" t="s">
+      <c r="D36" s="194" t="s">
         <v>606</v>
       </c>
-      <c r="E36" s="158"/>
-      <c r="F36" s="159"/>
+      <c r="E36" s="195"/>
+      <c r="F36" s="196"/>
       <c r="G36" s="25"/>
       <c r="H36" s="26"/>
     </row>
@@ -9805,11 +9927,11 @@
       <c r="C37" s="144" t="s">
         <v>670</v>
       </c>
-      <c r="D37" s="157" t="s">
+      <c r="D37" s="194" t="s">
         <v>668</v>
       </c>
-      <c r="E37" s="158"/>
-      <c r="F37" s="159"/>
+      <c r="E37" s="195"/>
+      <c r="F37" s="196"/>
       <c r="G37" s="25"/>
       <c r="H37" s="26"/>
     </row>
@@ -9819,11 +9941,11 @@
       <c r="C38" s="144" t="s">
         <v>669</v>
       </c>
-      <c r="D38" s="157" t="s">
+      <c r="D38" s="194" t="s">
         <v>671</v>
       </c>
-      <c r="E38" s="158"/>
-      <c r="F38" s="159"/>
+      <c r="E38" s="195"/>
+      <c r="F38" s="196"/>
       <c r="G38" s="25"/>
       <c r="H38" s="26"/>
     </row>
@@ -9831,9 +9953,9 @@
       <c r="A39" s="24"/>
       <c r="B39" s="146"/>
       <c r="C39" s="144"/>
-      <c r="D39" s="157"/>
-      <c r="E39" s="158"/>
-      <c r="F39" s="159"/>
+      <c r="D39" s="194"/>
+      <c r="E39" s="195"/>
+      <c r="F39" s="196"/>
       <c r="G39" s="25"/>
       <c r="H39" s="26"/>
     </row>
@@ -9931,6 +10053,13 @@
     <row r="52" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:H3"/>
@@ -9940,13 +10069,6 @@
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9970,28 +10092,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="200" t="s">
         <v>331</v>
       </c>
-      <c r="B1" s="173"/>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
+      <c r="B1" s="200"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="200"/>
+      <c r="E1" s="200"/>
+      <c r="F1" s="200"/>
+      <c r="G1" s="200"/>
+      <c r="H1" s="200"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="170" t="s">
+      <c r="A2" s="197" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="171"/>
-      <c r="C2" s="171"/>
-      <c r="D2" s="171"/>
-      <c r="E2" s="171"/>
-      <c r="F2" s="171"/>
-      <c r="G2" s="171"/>
-      <c r="H2" s="172"/>
+      <c r="B2" s="198"/>
+      <c r="C2" s="198"/>
+      <c r="D2" s="198"/>
+      <c r="E2" s="198"/>
+      <c r="F2" s="198"/>
+      <c r="G2" s="198"/>
+      <c r="H2" s="199"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="5"/>
@@ -10170,16 +10292,16 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="170" t="s">
+      <c r="A15" s="197" t="s">
         <v>225</v>
       </c>
-      <c r="B15" s="171"/>
-      <c r="C15" s="171"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="171"/>
-      <c r="F15" s="171"/>
-      <c r="G15" s="171"/>
-      <c r="H15" s="172"/>
+      <c r="B15" s="198"/>
+      <c r="C15" s="198"/>
+      <c r="D15" s="198"/>
+      <c r="E15" s="198"/>
+      <c r="F15" s="198"/>
+      <c r="G15" s="198"/>
+      <c r="H15" s="199"/>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="9"/>
@@ -10355,16 +10477,16 @@
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:11" ht="15.75">
-      <c r="A28" s="170" t="s">
+      <c r="A28" s="197" t="s">
         <v>226</v>
       </c>
-      <c r="B28" s="171"/>
-      <c r="C28" s="171"/>
-      <c r="D28" s="171"/>
-      <c r="E28" s="171"/>
-      <c r="F28" s="171"/>
-      <c r="G28" s="171"/>
-      <c r="H28" s="172"/>
+      <c r="B28" s="198"/>
+      <c r="C28" s="198"/>
+      <c r="D28" s="198"/>
+      <c r="E28" s="198"/>
+      <c r="F28" s="198"/>
+      <c r="G28" s="198"/>
+      <c r="H28" s="199"/>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="5"/>
@@ -10564,40 +10686,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="201" t="s">
         <v>332</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="176"/>
+      <c r="B1" s="202"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="202"/>
+      <c r="E1" s="202"/>
+      <c r="F1" s="202"/>
+      <c r="G1" s="202"/>
+      <c r="H1" s="203"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="177"/>
-      <c r="B2" s="178"/>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="179"/>
+      <c r="A2" s="204"/>
+      <c r="B2" s="205"/>
+      <c r="C2" s="205"/>
+      <c r="D2" s="205"/>
+      <c r="E2" s="205"/>
+      <c r="F2" s="205"/>
+      <c r="G2" s="205"/>
+      <c r="H2" s="206"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="180" t="s">
+      <c r="A3" s="207" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="181"/>
-      <c r="C3" s="182"/>
-      <c r="D3" s="183"/>
-      <c r="E3" s="180" t="s">
+      <c r="B3" s="208"/>
+      <c r="C3" s="209"/>
+      <c r="D3" s="210"/>
+      <c r="E3" s="207" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="181"/>
-      <c r="G3" s="182"/>
-      <c r="H3" s="183"/>
+      <c r="F3" s="208"/>
+      <c r="G3" s="209"/>
+      <c r="H3" s="210"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="16">
@@ -11036,40 +11158,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="201" t="s">
+      <c r="A1" s="211" t="s">
         <v>333</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="202"/>
-      <c r="B2" s="202"/>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="202"/>
+      <c r="A2" s="212"/>
+      <c r="B2" s="212"/>
+      <c r="C2" s="212"/>
+      <c r="D2" s="212"/>
+      <c r="E2" s="212"/>
+      <c r="F2" s="212"/>
+      <c r="G2" s="212"/>
+      <c r="H2" s="212"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="203" t="s">
+      <c r="A3" s="213" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="204"/>
-      <c r="C3" s="205"/>
-      <c r="D3" s="206"/>
-      <c r="E3" s="203" t="s">
+      <c r="B3" s="214"/>
+      <c r="C3" s="215"/>
+      <c r="D3" s="216"/>
+      <c r="E3" s="213" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="204"/>
-      <c r="G3" s="205"/>
-      <c r="H3" s="206"/>
+      <c r="F3" s="214"/>
+      <c r="G3" s="215"/>
+      <c r="H3" s="216"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="46">
@@ -11362,114 +11484,114 @@
       <c r="H24" s="74"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="203" t="s">
+      <c r="A25" s="213" t="s">
         <v>293</v>
       </c>
-      <c r="B25" s="204"/>
-      <c r="C25" s="205"/>
-      <c r="D25" s="206"/>
-      <c r="E25" s="203" t="s">
+      <c r="B25" s="214"/>
+      <c r="C25" s="215"/>
+      <c r="D25" s="216"/>
+      <c r="E25" s="213" t="s">
         <v>294</v>
       </c>
-      <c r="F25" s="204"/>
-      <c r="G25" s="205"/>
-      <c r="H25" s="206"/>
+      <c r="F25" s="214"/>
+      <c r="G25" s="215"/>
+      <c r="H25" s="216"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="50" t="s">
         <v>295</v>
       </c>
-      <c r="B26" s="190"/>
-      <c r="C26" s="191"/>
-      <c r="D26" s="192"/>
+      <c r="B26" s="217"/>
+      <c r="C26" s="218"/>
+      <c r="D26" s="219"/>
       <c r="E26" s="46" t="s">
         <v>296</v>
       </c>
-      <c r="F26" s="198"/>
-      <c r="G26" s="199"/>
-      <c r="H26" s="200"/>
+      <c r="F26" s="220"/>
+      <c r="G26" s="221"/>
+      <c r="H26" s="222"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="B27" s="193"/>
-      <c r="C27" s="194"/>
-      <c r="D27" s="196"/>
+      <c r="B27" s="223"/>
+      <c r="C27" s="224"/>
+      <c r="D27" s="225"/>
       <c r="E27" s="50" t="s">
         <v>298</v>
       </c>
-      <c r="F27" s="190"/>
-      <c r="G27" s="191"/>
-      <c r="H27" s="197"/>
+      <c r="F27" s="217"/>
+      <c r="G27" s="218"/>
+      <c r="H27" s="226"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="50" t="s">
         <v>299</v>
       </c>
-      <c r="B28" s="190"/>
-      <c r="C28" s="191"/>
-      <c r="D28" s="192"/>
+      <c r="B28" s="217"/>
+      <c r="C28" s="218"/>
+      <c r="D28" s="219"/>
       <c r="E28" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="F28" s="193"/>
-      <c r="G28" s="194"/>
-      <c r="H28" s="195"/>
+      <c r="F28" s="223"/>
+      <c r="G28" s="224"/>
+      <c r="H28" s="227"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="58" t="s">
         <v>301</v>
       </c>
-      <c r="B29" s="193"/>
-      <c r="C29" s="194"/>
-      <c r="D29" s="196"/>
+      <c r="B29" s="223"/>
+      <c r="C29" s="224"/>
+      <c r="D29" s="225"/>
       <c r="E29" s="50" t="s">
         <v>302</v>
       </c>
-      <c r="F29" s="190"/>
-      <c r="G29" s="191"/>
-      <c r="H29" s="197"/>
+      <c r="F29" s="217"/>
+      <c r="G29" s="218"/>
+      <c r="H29" s="226"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="50" t="s">
         <v>303</v>
       </c>
-      <c r="B30" s="190"/>
-      <c r="C30" s="191"/>
-      <c r="D30" s="192"/>
+      <c r="B30" s="217"/>
+      <c r="C30" s="218"/>
+      <c r="D30" s="219"/>
       <c r="E30" s="58" t="s">
         <v>304</v>
       </c>
-      <c r="F30" s="193"/>
-      <c r="G30" s="194"/>
-      <c r="H30" s="195"/>
+      <c r="F30" s="223"/>
+      <c r="G30" s="224"/>
+      <c r="H30" s="227"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="B31" s="193"/>
-      <c r="C31" s="194"/>
-      <c r="D31" s="196"/>
+      <c r="B31" s="223"/>
+      <c r="C31" s="224"/>
+      <c r="D31" s="225"/>
       <c r="E31" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="F31" s="190"/>
-      <c r="G31" s="191"/>
-      <c r="H31" s="197"/>
+      <c r="F31" s="217"/>
+      <c r="G31" s="218"/>
+      <c r="H31" s="226"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="50" t="s">
         <v>307</v>
       </c>
-      <c r="B32" s="190"/>
-      <c r="C32" s="191"/>
-      <c r="D32" s="192"/>
+      <c r="B32" s="217"/>
+      <c r="C32" s="218"/>
+      <c r="D32" s="219"/>
       <c r="E32" s="58"/>
-      <c r="F32" s="193"/>
-      <c r="G32" s="194"/>
-      <c r="H32" s="195" t="s">
+      <c r="F32" s="223"/>
+      <c r="G32" s="224"/>
+      <c r="H32" s="227" t="s">
         <v>245</v>
       </c>
     </row>
@@ -11477,13 +11599,13 @@
       <c r="A33" s="58" t="s">
         <v>308</v>
       </c>
-      <c r="B33" s="193"/>
-      <c r="C33" s="194"/>
-      <c r="D33" s="196"/>
+      <c r="B33" s="223"/>
+      <c r="C33" s="224"/>
+      <c r="D33" s="225"/>
       <c r="E33" s="50"/>
-      <c r="F33" s="190"/>
-      <c r="G33" s="191"/>
-      <c r="H33" s="197" t="s">
+      <c r="F33" s="217"/>
+      <c r="G33" s="218"/>
+      <c r="H33" s="226" t="s">
         <v>288</v>
       </c>
     </row>
@@ -11491,13 +11613,13 @@
       <c r="A34" s="50" t="s">
         <v>309</v>
       </c>
-      <c r="B34" s="190"/>
-      <c r="C34" s="191"/>
-      <c r="D34" s="192"/>
+      <c r="B34" s="217"/>
+      <c r="C34" s="218"/>
+      <c r="D34" s="219"/>
       <c r="E34" s="58"/>
-      <c r="F34" s="193"/>
-      <c r="G34" s="194"/>
-      <c r="H34" s="195" t="s">
+      <c r="F34" s="223"/>
+      <c r="G34" s="224"/>
+      <c r="H34" s="227" t="s">
         <v>289</v>
       </c>
     </row>
@@ -11505,13 +11627,13 @@
       <c r="A35" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="B35" s="193"/>
-      <c r="C35" s="194"/>
-      <c r="D35" s="196"/>
+      <c r="B35" s="223"/>
+      <c r="C35" s="224"/>
+      <c r="D35" s="225"/>
       <c r="E35" s="50"/>
-      <c r="F35" s="190"/>
-      <c r="G35" s="191"/>
-      <c r="H35" s="197" t="s">
+      <c r="F35" s="217"/>
+      <c r="G35" s="218"/>
+      <c r="H35" s="226" t="s">
         <v>290</v>
       </c>
     </row>
@@ -11519,13 +11641,13 @@
       <c r="A36" s="50" t="s">
         <v>311</v>
       </c>
-      <c r="B36" s="190"/>
-      <c r="C36" s="191"/>
-      <c r="D36" s="192"/>
+      <c r="B36" s="217"/>
+      <c r="C36" s="218"/>
+      <c r="D36" s="219"/>
       <c r="E36" s="58"/>
-      <c r="F36" s="193"/>
-      <c r="G36" s="194"/>
-      <c r="H36" s="195" t="s">
+      <c r="F36" s="223"/>
+      <c r="G36" s="224"/>
+      <c r="H36" s="227" t="s">
         <v>291</v>
       </c>
     </row>
@@ -11533,13 +11655,13 @@
       <c r="A37" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="B37" s="193"/>
-      <c r="C37" s="194"/>
-      <c r="D37" s="196"/>
+      <c r="B37" s="223"/>
+      <c r="C37" s="224"/>
+      <c r="D37" s="225"/>
       <c r="E37" s="50"/>
-      <c r="F37" s="190"/>
-      <c r="G37" s="191"/>
-      <c r="H37" s="197" t="s">
+      <c r="F37" s="217"/>
+      <c r="G37" s="218"/>
+      <c r="H37" s="226" t="s">
         <v>292</v>
       </c>
     </row>
@@ -11547,13 +11669,13 @@
       <c r="A38" s="50" t="s">
         <v>313</v>
       </c>
-      <c r="B38" s="190"/>
-      <c r="C38" s="191"/>
-      <c r="D38" s="192"/>
+      <c r="B38" s="217"/>
+      <c r="C38" s="218"/>
+      <c r="D38" s="219"/>
       <c r="E38" s="58"/>
-      <c r="F38" s="193"/>
-      <c r="G38" s="194"/>
-      <c r="H38" s="195" t="s">
+      <c r="F38" s="223"/>
+      <c r="G38" s="224"/>
+      <c r="H38" s="227" t="s">
         <v>244</v>
       </c>
     </row>
@@ -11561,13 +11683,13 @@
       <c r="A39" s="58" t="s">
         <v>314</v>
       </c>
-      <c r="B39" s="193"/>
-      <c r="C39" s="194"/>
-      <c r="D39" s="196"/>
+      <c r="B39" s="223"/>
+      <c r="C39" s="224"/>
+      <c r="D39" s="225"/>
       <c r="E39" s="50"/>
-      <c r="F39" s="190"/>
-      <c r="G39" s="191"/>
-      <c r="H39" s="197" t="s">
+      <c r="F39" s="217"/>
+      <c r="G39" s="218"/>
+      <c r="H39" s="226" t="s">
         <v>245</v>
       </c>
     </row>
@@ -11575,57 +11697,28 @@
       <c r="A40" s="50" t="s">
         <v>315</v>
       </c>
-      <c r="B40" s="190"/>
-      <c r="C40" s="191"/>
-      <c r="D40" s="192"/>
+      <c r="B40" s="217"/>
+      <c r="C40" s="218"/>
+      <c r="D40" s="219"/>
       <c r="E40" s="58"/>
-      <c r="F40" s="193"/>
-      <c r="G40" s="194"/>
-      <c r="H40" s="195"/>
+      <c r="F40" s="223"/>
+      <c r="G40" s="224"/>
+      <c r="H40" s="227"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="70" t="s">
         <v>316</v>
       </c>
-      <c r="B41" s="184"/>
-      <c r="C41" s="185"/>
-      <c r="D41" s="186"/>
+      <c r="B41" s="228"/>
+      <c r="C41" s="229"/>
+      <c r="D41" s="230"/>
       <c r="E41" s="75"/>
-      <c r="F41" s="187"/>
-      <c r="G41" s="188"/>
-      <c r="H41" s="189"/>
+      <c r="F41" s="231"/>
+      <c r="G41" s="232"/>
+      <c r="H41" s="233"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -11634,6 +11727,35 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11662,40 +11784,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="213" t="s">
+      <c r="A1" s="240" t="s">
         <v>334</v>
       </c>
-      <c r="B1" s="214"/>
-      <c r="C1" s="214"/>
-      <c r="D1" s="214"/>
-      <c r="E1" s="214"/>
-      <c r="F1" s="214"/>
-      <c r="G1" s="214"/>
-      <c r="H1" s="215"/>
+      <c r="B1" s="241"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="241"/>
+      <c r="E1" s="241"/>
+      <c r="F1" s="241"/>
+      <c r="G1" s="241"/>
+      <c r="H1" s="242"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="216"/>
-      <c r="B2" s="217"/>
-      <c r="C2" s="217"/>
-      <c r="D2" s="217"/>
-      <c r="E2" s="217"/>
-      <c r="F2" s="217"/>
-      <c r="G2" s="217"/>
-      <c r="H2" s="218"/>
+      <c r="A2" s="243"/>
+      <c r="B2" s="244"/>
+      <c r="C2" s="244"/>
+      <c r="D2" s="244"/>
+      <c r="E2" s="244"/>
+      <c r="F2" s="244"/>
+      <c r="G2" s="244"/>
+      <c r="H2" s="245"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="207" t="s">
+      <c r="A3" s="234" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="208"/>
-      <c r="C3" s="208"/>
-      <c r="D3" s="209"/>
-      <c r="E3" s="207" t="s">
+      <c r="B3" s="235"/>
+      <c r="C3" s="235"/>
+      <c r="D3" s="236"/>
+      <c r="E3" s="234" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="208"/>
-      <c r="G3" s="208"/>
-      <c r="H3" s="209"/>
+      <c r="F3" s="235"/>
+      <c r="G3" s="235"/>
+      <c r="H3" s="236"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="93">
@@ -11912,18 +12034,18 @@
       <c r="H21" s="85"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="210" t="s">
+      <c r="A22" s="237" t="s">
         <v>319</v>
       </c>
-      <c r="B22" s="211"/>
-      <c r="C22" s="211"/>
-      <c r="D22" s="212"/>
-      <c r="E22" s="210" t="s">
+      <c r="B22" s="238"/>
+      <c r="C22" s="238"/>
+      <c r="D22" s="239"/>
+      <c r="E22" s="237" t="s">
         <v>320</v>
       </c>
-      <c r="F22" s="211"/>
-      <c r="G22" s="211"/>
-      <c r="H22" s="212"/>
+      <c r="F22" s="238"/>
+      <c r="G22" s="238"/>
+      <c r="H22" s="239"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="78">
@@ -12200,40 +12322,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="213" t="s">
+      <c r="A1" s="240" t="s">
         <v>494</v>
       </c>
-      <c r="B1" s="214"/>
-      <c r="C1" s="214"/>
-      <c r="D1" s="214"/>
-      <c r="E1" s="214"/>
-      <c r="F1" s="214"/>
-      <c r="G1" s="214"/>
-      <c r="H1" s="215"/>
+      <c r="B1" s="241"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="241"/>
+      <c r="E1" s="241"/>
+      <c r="F1" s="241"/>
+      <c r="G1" s="241"/>
+      <c r="H1" s="242"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="216"/>
-      <c r="B2" s="217"/>
-      <c r="C2" s="217"/>
-      <c r="D2" s="217"/>
-      <c r="E2" s="217"/>
-      <c r="F2" s="217"/>
-      <c r="G2" s="217"/>
-      <c r="H2" s="218"/>
+      <c r="A2" s="243"/>
+      <c r="B2" s="244"/>
+      <c r="C2" s="244"/>
+      <c r="D2" s="244"/>
+      <c r="E2" s="244"/>
+      <c r="F2" s="244"/>
+      <c r="G2" s="244"/>
+      <c r="H2" s="245"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="207" t="s">
+      <c r="A3" s="234" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="208"/>
-      <c r="C3" s="208"/>
-      <c r="D3" s="209"/>
-      <c r="E3" s="207" t="s">
+      <c r="B3" s="235"/>
+      <c r="C3" s="235"/>
+      <c r="D3" s="236"/>
+      <c r="E3" s="234" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="208"/>
-      <c r="G3" s="208"/>
-      <c r="H3" s="209"/>
+      <c r="F3" s="235"/>
+      <c r="G3" s="235"/>
+      <c r="H3" s="236"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="93">
@@ -12450,18 +12572,18 @@
       <c r="H21" s="85"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="210" t="s">
+      <c r="A22" s="237" t="s">
         <v>319</v>
       </c>
-      <c r="B22" s="211"/>
-      <c r="C22" s="211"/>
-      <c r="D22" s="212"/>
-      <c r="E22" s="210" t="s">
+      <c r="B22" s="238"/>
+      <c r="C22" s="238"/>
+      <c r="D22" s="239"/>
+      <c r="E22" s="237" t="s">
         <v>320</v>
       </c>
-      <c r="F22" s="211"/>
-      <c r="G22" s="211"/>
-      <c r="H22" s="212"/>
+      <c r="F22" s="238"/>
+      <c r="G22" s="238"/>
+      <c r="H22" s="239"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="78">

</xml_diff>

<commit_message>
AR305 added (low level KC-130)
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="852">
   <si>
     <t>AWACS</t>
   </si>
@@ -2564,6 +2564,21 @@
   </si>
   <si>
     <t>MUSTANG</t>
+  </si>
+  <si>
+    <t>TANKER KC-130</t>
+  </si>
+  <si>
+    <t>AR305</t>
+  </si>
+  <si>
+    <t>SHELL 7</t>
+  </si>
+  <si>
+    <t>RED 12</t>
+  </si>
+  <si>
+    <t>46X</t>
   </si>
 </sst>
 </file>
@@ -3698,7 +3713,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="298">
+  <cellXfs count="299">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4188,6 +4203,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4197,9 +4218,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4245,6 +4263,18 @@
     <xf numFmtId="0" fontId="26" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4272,18 +4302,6 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4326,6 +4344,57 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4343,57 +4412,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4777,8 +4795,8 @@
   <sheetPr codeName="Ark1"/>
   <dimension ref="A1:AP53"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V50" sqref="V50:X52"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AJ41" sqref="AJ41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -4894,13 +4912,13 @@
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
       <c r="T2" s="12"/>
-      <c r="V2" s="204" t="s">
+      <c r="V2" s="206" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="204"/>
-      <c r="X2" s="204"/>
-      <c r="Y2" s="204"/>
-      <c r="Z2" s="204"/>
+      <c r="W2" s="206"/>
+      <c r="X2" s="206"/>
+      <c r="Y2" s="206"/>
+      <c r="Z2" s="206"/>
       <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
       <c r="AC2" s="12"/>
@@ -4955,9 +4973,9 @@
         <v>433</v>
       </c>
       <c r="Q3" s="12"/>
-      <c r="R3" s="208"/>
-      <c r="S3" s="208"/>
-      <c r="T3" s="208"/>
+      <c r="R3" s="205"/>
+      <c r="S3" s="205"/>
+      <c r="T3" s="205"/>
       <c r="V3" s="122" t="s">
         <v>335</v>
       </c>
@@ -5041,22 +5059,22 @@
       <c r="AA4" s="36"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="36"/>
-      <c r="AD4" s="204" t="s">
+      <c r="AD4" s="206" t="s">
         <v>436</v>
       </c>
-      <c r="AE4" s="204"/>
-      <c r="AF4" s="204"/>
-      <c r="AG4" s="204"/>
-      <c r="AH4" s="204"/>
-      <c r="AJ4" s="204" t="s">
+      <c r="AE4" s="206"/>
+      <c r="AF4" s="206"/>
+      <c r="AG4" s="206"/>
+      <c r="AH4" s="206"/>
+      <c r="AJ4" s="206" t="s">
         <v>1</v>
       </c>
-      <c r="AK4" s="204"/>
-      <c r="AL4" s="204"/>
-      <c r="AM4" s="204"/>
-      <c r="AN4" s="204"/>
-      <c r="AO4" s="204"/>
-      <c r="AP4" s="204"/>
+      <c r="AK4" s="206"/>
+      <c r="AL4" s="206"/>
+      <c r="AM4" s="206"/>
+      <c r="AN4" s="206"/>
+      <c r="AO4" s="206"/>
+      <c r="AP4" s="206"/>
     </row>
     <row r="5" spans="1:42" ht="15.75">
       <c r="A5" s="129" t="s">
@@ -6149,15 +6167,15 @@
       <c r="AH17" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="AJ17" s="204" t="s">
+      <c r="AJ17" s="206" t="s">
         <v>277</v>
       </c>
-      <c r="AK17" s="204"/>
-      <c r="AL17" s="204"/>
-      <c r="AM17" s="204"/>
-      <c r="AN17" s="204"/>
-      <c r="AO17" s="204"/>
-      <c r="AP17" s="204"/>
+      <c r="AK17" s="206"/>
+      <c r="AL17" s="206"/>
+      <c r="AM17" s="206"/>
+      <c r="AN17" s="206"/>
+      <c r="AO17" s="206"/>
+      <c r="AP17" s="206"/>
     </row>
     <row r="18" spans="1:42" ht="15.75">
       <c r="A18" s="129" t="s">
@@ -6374,9 +6392,9 @@
       <c r="O20" s="35"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="208"/>
-      <c r="S20" s="208"/>
-      <c r="T20" s="208"/>
+      <c r="R20" s="205"/>
+      <c r="S20" s="205"/>
+      <c r="T20" s="205"/>
       <c r="U20" s="2"/>
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
@@ -6716,13 +6734,13 @@
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
-      <c r="AD24" s="204" t="s">
+      <c r="AD24" s="206" t="s">
         <v>493</v>
       </c>
-      <c r="AE24" s="204"/>
-      <c r="AF24" s="204"/>
-      <c r="AG24" s="204"/>
-      <c r="AH24" s="204"/>
+      <c r="AE24" s="206"/>
+      <c r="AF24" s="206"/>
+      <c r="AG24" s="206"/>
+      <c r="AH24" s="206"/>
       <c r="AJ24" s="142" t="s">
         <v>568</v>
       </c>
@@ -6782,7 +6800,7 @@
       <c r="L25" s="130" t="s">
         <v>33</v>
       </c>
-      <c r="M25" s="130" t="s">
+      <c r="M25" s="135" t="s">
         <v>521</v>
       </c>
       <c r="N25" s="129" t="s">
@@ -6878,6 +6896,15 @@
       <c r="AH26" s="3" t="s">
         <v>492</v>
       </c>
+      <c r="AJ26" s="206" t="s">
+        <v>847</v>
+      </c>
+      <c r="AK26" s="206"/>
+      <c r="AL26" s="206"/>
+      <c r="AM26" s="206"/>
+      <c r="AN26" s="206"/>
+      <c r="AO26" s="206"/>
+      <c r="AP26" s="206"/>
     </row>
     <row r="27" spans="1:42">
       <c r="A27" s="129" t="s">
@@ -6934,6 +6961,27 @@
       <c r="Z27" s="12"/>
       <c r="AA27" s="12"/>
       <c r="AB27" s="12"/>
+      <c r="AJ27" s="204" t="s">
+        <v>218</v>
+      </c>
+      <c r="AK27" s="204" t="s">
+        <v>219</v>
+      </c>
+      <c r="AL27" s="204" t="s">
+        <v>224</v>
+      </c>
+      <c r="AM27" s="204" t="s">
+        <v>227</v>
+      </c>
+      <c r="AN27" s="204" t="s">
+        <v>220</v>
+      </c>
+      <c r="AO27" s="204" t="s">
+        <v>284</v>
+      </c>
+      <c r="AP27" s="204" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="28" spans="1:42">
       <c r="A28" s="129" t="s">
@@ -6982,6 +7030,27 @@
       <c r="S28" s="12"/>
       <c r="T28" s="12"/>
       <c r="U28" s="12"/>
+      <c r="AJ28" t="s">
+        <v>848</v>
+      </c>
+      <c r="AK28" t="s">
+        <v>849</v>
+      </c>
+      <c r="AL28" t="s">
+        <v>521</v>
+      </c>
+      <c r="AM28" t="s">
+        <v>850</v>
+      </c>
+      <c r="AN28" t="s">
+        <v>851</v>
+      </c>
+      <c r="AO28">
+        <v>5307</v>
+      </c>
+      <c r="AP28">
+        <v>307</v>
+      </c>
     </row>
     <row r="29" spans="1:42">
       <c r="A29" s="129" t="s">
@@ -7032,15 +7101,15 @@
       <c r="S29" s="35"/>
       <c r="T29" s="35"/>
       <c r="U29" s="35"/>
-      <c r="V29" s="204" t="s">
+      <c r="V29" s="206" t="s">
         <v>212</v>
       </c>
-      <c r="W29" s="204"/>
-      <c r="X29" s="204"/>
-      <c r="Y29" s="204"/>
-      <c r="Z29" s="204"/>
-      <c r="AA29" s="204"/>
-      <c r="AB29" s="204"/>
+      <c r="W29" s="206"/>
+      <c r="X29" s="206"/>
+      <c r="Y29" s="206"/>
+      <c r="Z29" s="206"/>
+      <c r="AA29" s="206"/>
+      <c r="AB29" s="206"/>
     </row>
     <row r="30" spans="1:42">
       <c r="A30" s="129"/>
@@ -7130,11 +7199,11 @@
       <c r="Y31" s="37"/>
       <c r="Z31" s="37"/>
       <c r="AA31" s="12"/>
-      <c r="AD31" s="205" t="s">
+      <c r="AD31" s="207" t="s">
         <v>263</v>
       </c>
-      <c r="AE31" s="206"/>
-      <c r="AF31" s="207"/>
+      <c r="AE31" s="208"/>
+      <c r="AF31" s="209"/>
     </row>
     <row r="32" spans="1:42">
       <c r="S32" s="12"/>
@@ -7239,15 +7308,15 @@
       <c r="S37" s="12"/>
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
-      <c r="V37" s="204" t="s">
+      <c r="V37" s="206" t="s">
         <v>9</v>
       </c>
-      <c r="W37" s="204"/>
-      <c r="X37" s="204"/>
-      <c r="Y37" s="204"/>
-      <c r="Z37" s="204"/>
-      <c r="AA37" s="204"/>
-      <c r="AB37" s="204"/>
+      <c r="W37" s="206"/>
+      <c r="X37" s="206"/>
+      <c r="Y37" s="206"/>
+      <c r="Z37" s="206"/>
+      <c r="AA37" s="206"/>
+      <c r="AB37" s="206"/>
       <c r="AD37" s="3" t="s">
         <v>259</v>
       </c>
@@ -7346,15 +7415,15 @@
       <c r="S42" s="12"/>
       <c r="T42" s="12"/>
       <c r="U42" s="12"/>
-      <c r="V42" s="204" t="s">
+      <c r="V42" s="206" t="s">
         <v>247</v>
       </c>
-      <c r="W42" s="204"/>
-      <c r="X42" s="204"/>
-      <c r="Y42" s="204"/>
-      <c r="Z42" s="204"/>
-      <c r="AA42" s="204"/>
-      <c r="AB42" s="204"/>
+      <c r="W42" s="206"/>
+      <c r="X42" s="206"/>
+      <c r="Y42" s="206"/>
+      <c r="Z42" s="206"/>
+      <c r="AA42" s="206"/>
+      <c r="AB42" s="206"/>
       <c r="AD42" s="3" t="s">
         <v>265</v>
       </c>
@@ -7459,15 +7528,15 @@
       <c r="S48" s="12"/>
       <c r="T48" s="12"/>
       <c r="U48" s="12"/>
-      <c r="V48" s="205" t="s">
+      <c r="V48" s="207" t="s">
         <v>480</v>
       </c>
-      <c r="W48" s="206"/>
-      <c r="X48" s="206"/>
-      <c r="Y48" s="206"/>
-      <c r="Z48" s="206"/>
-      <c r="AA48" s="206"/>
-      <c r="AB48" s="207"/>
+      <c r="W48" s="208"/>
+      <c r="X48" s="208"/>
+      <c r="Y48" s="208"/>
+      <c r="Z48" s="208"/>
+      <c r="AA48" s="208"/>
+      <c r="AB48" s="209"/>
     </row>
     <row r="49" spans="19:28">
       <c r="S49" s="12"/>
@@ -7556,7 +7625,12 @@
       <c r="AA53" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="V42:AB42"/>
+    <mergeCell ref="AD4:AH4"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="V48:AB48"/>
+    <mergeCell ref="V37:AB37"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="AJ4:AP4"/>
@@ -7564,11 +7638,7 @@
     <mergeCell ref="AD31:AF31"/>
     <mergeCell ref="V29:AB29"/>
     <mergeCell ref="AD24:AH24"/>
-    <mergeCell ref="V42:AB42"/>
-    <mergeCell ref="AD4:AH4"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="V48:AB48"/>
-    <mergeCell ref="V37:AB37"/>
+    <mergeCell ref="AJ26:AP26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7596,40 +7666,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="286" t="s">
+      <c r="A1" s="287" t="s">
         <v>494</v>
       </c>
-      <c r="B1" s="287"/>
-      <c r="C1" s="287"/>
-      <c r="D1" s="287"/>
-      <c r="E1" s="287"/>
-      <c r="F1" s="287"/>
-      <c r="G1" s="287"/>
-      <c r="H1" s="288"/>
+      <c r="B1" s="288"/>
+      <c r="C1" s="288"/>
+      <c r="D1" s="288"/>
+      <c r="E1" s="288"/>
+      <c r="F1" s="288"/>
+      <c r="G1" s="288"/>
+      <c r="H1" s="289"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="289"/>
-      <c r="B2" s="290"/>
-      <c r="C2" s="290"/>
-      <c r="D2" s="290"/>
-      <c r="E2" s="290"/>
-      <c r="F2" s="290"/>
-      <c r="G2" s="290"/>
-      <c r="H2" s="291"/>
+      <c r="A2" s="290"/>
+      <c r="B2" s="291"/>
+      <c r="C2" s="291"/>
+      <c r="D2" s="291"/>
+      <c r="E2" s="291"/>
+      <c r="F2" s="291"/>
+      <c r="G2" s="291"/>
+      <c r="H2" s="292"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="292" t="s">
+      <c r="A3" s="293" t="s">
         <v>767</v>
       </c>
-      <c r="B3" s="293"/>
-      <c r="C3" s="293"/>
-      <c r="D3" s="294"/>
-      <c r="E3" s="292" t="s">
+      <c r="B3" s="294"/>
+      <c r="C3" s="294"/>
+      <c r="D3" s="295"/>
+      <c r="E3" s="293" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="293"/>
-      <c r="G3" s="293"/>
-      <c r="H3" s="294"/>
+      <c r="F3" s="294"/>
+      <c r="G3" s="294"/>
+      <c r="H3" s="295"/>
     </row>
     <row r="4" spans="1:8" ht="16.5">
       <c r="A4" s="195">
@@ -8102,18 +8172,18 @@
       <c r="H24" s="175"/>
     </row>
     <row r="25" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A25" s="295" t="s">
+      <c r="A25" s="296" t="s">
         <v>318</v>
       </c>
-      <c r="B25" s="296"/>
-      <c r="C25" s="296"/>
-      <c r="D25" s="297"/>
-      <c r="E25" s="295" t="s">
+      <c r="B25" s="297"/>
+      <c r="C25" s="297"/>
+      <c r="D25" s="298"/>
+      <c r="E25" s="296" t="s">
         <v>817</v>
       </c>
-      <c r="F25" s="296"/>
-      <c r="G25" s="296"/>
-      <c r="H25" s="297"/>
+      <c r="F25" s="297"/>
+      <c r="G25" s="297"/>
+      <c r="H25" s="298"/>
     </row>
     <row r="26" spans="1:8" ht="16.5">
       <c r="A26" s="184">
@@ -8510,7 +8580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AJ45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AC19" sqref="AC19"/>
     </sheetView>
   </sheetViews>
@@ -8547,48 +8617,48 @@
       </c>
     </row>
     <row r="2" spans="2:36">
-      <c r="B2" s="204" t="s">
+      <c r="B2" s="206" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="204"/>
-      <c r="D2" s="204"/>
-      <c r="E2" s="204"/>
-      <c r="F2" s="204"/>
-      <c r="H2" s="204" t="s">
+      <c r="C2" s="206"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="206"/>
+      <c r="F2" s="206"/>
+      <c r="H2" s="206" t="s">
         <v>231</v>
       </c>
-      <c r="I2" s="204"/>
-      <c r="J2" s="204"/>
-      <c r="K2" s="204"/>
-      <c r="L2" s="204"/>
-      <c r="N2" s="204" t="s">
+      <c r="I2" s="206"/>
+      <c r="J2" s="206"/>
+      <c r="K2" s="206"/>
+      <c r="L2" s="206"/>
+      <c r="N2" s="206" t="s">
         <v>239</v>
       </c>
-      <c r="O2" s="204"/>
-      <c r="P2" s="204"/>
-      <c r="Q2" s="204"/>
-      <c r="R2" s="204"/>
-      <c r="T2" s="204" t="s">
+      <c r="O2" s="206"/>
+      <c r="P2" s="206"/>
+      <c r="Q2" s="206"/>
+      <c r="R2" s="206"/>
+      <c r="T2" s="206" t="s">
         <v>249</v>
       </c>
-      <c r="U2" s="204"/>
-      <c r="V2" s="204"/>
-      <c r="W2" s="204"/>
-      <c r="X2" s="204"/>
-      <c r="Z2" s="204" t="s">
+      <c r="U2" s="206"/>
+      <c r="V2" s="206"/>
+      <c r="W2" s="206"/>
+      <c r="X2" s="206"/>
+      <c r="Z2" s="206" t="s">
         <v>321</v>
       </c>
-      <c r="AA2" s="204"/>
-      <c r="AB2" s="204"/>
-      <c r="AC2" s="204"/>
-      <c r="AD2" s="204"/>
-      <c r="AF2" s="204" t="s">
+      <c r="AA2" s="206"/>
+      <c r="AB2" s="206"/>
+      <c r="AC2" s="206"/>
+      <c r="AD2" s="206"/>
+      <c r="AF2" s="206" t="s">
         <v>498</v>
       </c>
-      <c r="AG2" s="204"/>
-      <c r="AH2" s="204"/>
-      <c r="AI2" s="204"/>
-      <c r="AJ2" s="204"/>
+      <c r="AG2" s="206"/>
+      <c r="AH2" s="206"/>
+      <c r="AI2" s="206"/>
+      <c r="AJ2" s="206"/>
     </row>
     <row r="3" spans="2:36">
       <c r="B3" s="124" t="s">
@@ -9063,20 +9133,20 @@
       <c r="F24" s="140"/>
     </row>
     <row r="25" spans="2:20">
-      <c r="B25" s="204" t="s">
+      <c r="B25" s="206" t="s">
         <v>711</v>
       </c>
-      <c r="C25" s="204"/>
-      <c r="D25" s="204"/>
-      <c r="E25" s="204"/>
-      <c r="F25" s="204"/>
-      <c r="H25" s="204" t="s">
+      <c r="C25" s="206"/>
+      <c r="D25" s="206"/>
+      <c r="E25" s="206"/>
+      <c r="F25" s="206"/>
+      <c r="H25" s="206" t="s">
         <v>766</v>
       </c>
-      <c r="I25" s="204"/>
-      <c r="J25" s="204"/>
-      <c r="K25" s="204"/>
-      <c r="L25" s="204"/>
+      <c r="I25" s="206"/>
+      <c r="J25" s="206"/>
+      <c r="K25" s="206"/>
+      <c r="L25" s="206"/>
     </row>
     <row r="26" spans="2:20">
       <c r="B26" s="124" t="s">
@@ -9401,25 +9471,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>764</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="211"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
+      <c r="E1" s="211"/>
+      <c r="F1" s="211"/>
+      <c r="G1" s="211"/>
+      <c r="H1" s="211"/>
+      <c r="I1" s="211"/>
+      <c r="J1" s="212"/>
     </row>
     <row r="2" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A2" s="215" t="s">
+      <c r="A2" s="216" t="s">
         <v>719</v>
       </c>
-      <c r="B2" s="216"/>
-      <c r="C2" s="217"/>
+      <c r="B2" s="217"/>
+      <c r="C2" s="218"/>
       <c r="D2" s="151"/>
       <c r="E2" s="151"/>
       <c r="F2" s="151"/>
@@ -9447,7 +9517,7 @@
       <c r="J3" s="149"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="221" t="s">
+      <c r="A4" s="222" t="s">
         <v>329</v>
       </c>
       <c r="B4" s="160" t="s">
@@ -9465,7 +9535,7 @@
       <c r="J4" s="149"/>
     </row>
     <row r="5" spans="1:10" ht="18.75">
-      <c r="A5" s="222"/>
+      <c r="A5" s="223"/>
       <c r="B5" s="159" t="s">
         <v>326</v>
       </c>
@@ -9481,7 +9551,7 @@
       <c r="J5" s="149"/>
     </row>
     <row r="6" spans="1:10" ht="18.75">
-      <c r="A6" s="222"/>
+      <c r="A6" s="223"/>
       <c r="B6" s="159" t="s">
         <v>327</v>
       </c>
@@ -9497,7 +9567,7 @@
       <c r="J6" s="149"/>
     </row>
     <row r="7" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A7" s="223"/>
+      <c r="A7" s="224"/>
       <c r="B7" s="163" t="s">
         <v>328</v>
       </c>
@@ -9513,7 +9583,7 @@
       <c r="J7" s="149"/>
     </row>
     <row r="8" spans="1:10" ht="18.75">
-      <c r="A8" s="221" t="s">
+      <c r="A8" s="222" t="s">
         <v>681</v>
       </c>
       <c r="B8" s="160" t="s">
@@ -9531,7 +9601,7 @@
       <c r="J8" s="149"/>
     </row>
     <row r="9" spans="1:10" ht="18.75">
-      <c r="A9" s="222"/>
+      <c r="A9" s="223"/>
       <c r="B9" s="159" t="s">
         <v>672</v>
       </c>
@@ -9547,7 +9617,7 @@
       <c r="J9" s="149"/>
     </row>
     <row r="10" spans="1:10" ht="18.75">
-      <c r="A10" s="222"/>
+      <c r="A10" s="223"/>
       <c r="B10" s="159" t="s">
         <v>673</v>
       </c>
@@ -9563,7 +9633,7 @@
       <c r="J10" s="149"/>
     </row>
     <row r="11" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A11" s="223"/>
+      <c r="A11" s="224"/>
       <c r="B11" s="163" t="s">
         <v>674</v>
       </c>
@@ -9579,7 +9649,7 @@
       <c r="J11" s="149"/>
     </row>
     <row r="12" spans="1:10" ht="18.75">
-      <c r="A12" s="221" t="s">
+      <c r="A12" s="222" t="s">
         <v>679</v>
       </c>
       <c r="B12" s="160" t="s">
@@ -9597,7 +9667,7 @@
       <c r="J12" s="149"/>
     </row>
     <row r="13" spans="1:10" ht="18.75">
-      <c r="A13" s="222"/>
+      <c r="A13" s="223"/>
       <c r="B13" s="159" t="s">
         <v>676</v>
       </c>
@@ -9613,7 +9683,7 @@
       <c r="J13" s="149"/>
     </row>
     <row r="14" spans="1:10" ht="18.75">
-      <c r="A14" s="222"/>
+      <c r="A14" s="223"/>
       <c r="B14" s="159" t="s">
         <v>677</v>
       </c>
@@ -9629,7 +9699,7 @@
       <c r="J14" s="149"/>
     </row>
     <row r="15" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A15" s="223"/>
+      <c r="A15" s="224"/>
       <c r="B15" s="163" t="s">
         <v>678</v>
       </c>
@@ -9645,7 +9715,7 @@
       <c r="J15" s="149"/>
     </row>
     <row r="16" spans="1:10" ht="18.75">
-      <c r="A16" s="221" t="s">
+      <c r="A16" s="222" t="s">
         <v>680</v>
       </c>
       <c r="B16" s="160" t="s">
@@ -9663,7 +9733,7 @@
       <c r="J16" s="149"/>
     </row>
     <row r="17" spans="1:10" ht="18.75">
-      <c r="A17" s="222"/>
+      <c r="A17" s="223"/>
       <c r="B17" s="159" t="s">
         <v>683</v>
       </c>
@@ -9679,7 +9749,7 @@
       <c r="J17" s="149"/>
     </row>
     <row r="18" spans="1:10" ht="18.75">
-      <c r="A18" s="222"/>
+      <c r="A18" s="223"/>
       <c r="B18" s="159" t="s">
         <v>684</v>
       </c>
@@ -9695,7 +9765,7 @@
       <c r="J18" s="149"/>
     </row>
     <row r="19" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A19" s="223"/>
+      <c r="A19" s="224"/>
       <c r="B19" s="163" t="s">
         <v>685</v>
       </c>
@@ -9723,11 +9793,11 @@
       <c r="J20" s="149"/>
     </row>
     <row r="21" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A21" s="218" t="s">
+      <c r="A21" s="219" t="s">
         <v>718</v>
       </c>
-      <c r="B21" s="219"/>
-      <c r="C21" s="220"/>
+      <c r="B21" s="220"/>
+      <c r="C21" s="221"/>
       <c r="D21" s="151"/>
       <c r="E21" s="151"/>
       <c r="F21" s="151"/>
@@ -9755,7 +9825,7 @@
       <c r="J22" s="149"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="212" t="s">
+      <c r="A23" s="213" t="s">
         <v>505</v>
       </c>
       <c r="B23" s="160" t="s">
@@ -9773,7 +9843,7 @@
       <c r="J23" s="149"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="213"/>
+      <c r="A24" s="214"/>
       <c r="B24" s="159" t="s">
         <v>693</v>
       </c>
@@ -9789,7 +9859,7 @@
       <c r="J24" s="149"/>
     </row>
     <row r="25" spans="1:10" ht="18.75">
-      <c r="A25" s="213"/>
+      <c r="A25" s="214"/>
       <c r="B25" s="159" t="s">
         <v>694</v>
       </c>
@@ -9805,7 +9875,7 @@
       <c r="J25" s="149"/>
     </row>
     <row r="26" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A26" s="214"/>
+      <c r="A26" s="215"/>
       <c r="B26" s="163" t="s">
         <v>695</v>
       </c>
@@ -9821,7 +9891,7 @@
       <c r="J26" s="149"/>
     </row>
     <row r="27" spans="1:10" ht="18.75">
-      <c r="A27" s="212" t="s">
+      <c r="A27" s="213" t="s">
         <v>701</v>
       </c>
       <c r="B27" s="160" t="s">
@@ -9839,7 +9909,7 @@
       <c r="J27" s="149"/>
     </row>
     <row r="28" spans="1:10" ht="18.75">
-      <c r="A28" s="213"/>
+      <c r="A28" s="214"/>
       <c r="B28" s="159" t="s">
         <v>698</v>
       </c>
@@ -9855,7 +9925,7 @@
       <c r="J28" s="149"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="213"/>
+      <c r="A29" s="214"/>
       <c r="B29" s="159" t="s">
         <v>699</v>
       </c>
@@ -9871,7 +9941,7 @@
       <c r="J29" s="149"/>
     </row>
     <row r="30" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A30" s="214"/>
+      <c r="A30" s="215"/>
       <c r="B30" s="163" t="s">
         <v>700</v>
       </c>
@@ -9887,7 +9957,7 @@
       <c r="J30" s="149"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="212" t="s">
+      <c r="A31" s="213" t="s">
         <v>705</v>
       </c>
       <c r="B31" s="160" t="s">
@@ -9905,7 +9975,7 @@
       <c r="J31" s="149"/>
     </row>
     <row r="32" spans="1:10" ht="18.75">
-      <c r="A32" s="213"/>
+      <c r="A32" s="214"/>
       <c r="B32" s="159" t="s">
         <v>707</v>
       </c>
@@ -9921,7 +9991,7 @@
       <c r="J32" s="149"/>
     </row>
     <row r="33" spans="1:10" ht="18.75">
-      <c r="A33" s="213"/>
+      <c r="A33" s="214"/>
       <c r="B33" s="159" t="s">
         <v>708</v>
       </c>
@@ -9937,7 +10007,7 @@
       <c r="J33" s="149"/>
     </row>
     <row r="34" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A34" s="214"/>
+      <c r="A34" s="215"/>
       <c r="B34" s="163" t="s">
         <v>709</v>
       </c>
@@ -9953,7 +10023,7 @@
       <c r="J34" s="149"/>
     </row>
     <row r="35" spans="1:10" ht="18.75">
-      <c r="A35" s="212" t="s">
+      <c r="A35" s="213" t="s">
         <v>712</v>
       </c>
       <c r="B35" s="160" t="s">
@@ -9971,7 +10041,7 @@
       <c r="J35" s="149"/>
     </row>
     <row r="36" spans="1:10" ht="18.75">
-      <c r="A36" s="213"/>
+      <c r="A36" s="214"/>
       <c r="B36" s="159" t="s">
         <v>714</v>
       </c>
@@ -9987,7 +10057,7 @@
       <c r="J36" s="149"/>
     </row>
     <row r="37" spans="1:10" ht="18.75">
-      <c r="A37" s="213"/>
+      <c r="A37" s="214"/>
       <c r="B37" s="159" t="s">
         <v>715</v>
       </c>
@@ -10003,7 +10073,7 @@
       <c r="J37" s="149"/>
     </row>
     <row r="38" spans="1:10" ht="19.5" thickBot="1">
-      <c r="A38" s="214"/>
+      <c r="A38" s="215"/>
       <c r="B38" s="163" t="s">
         <v>716</v>
       </c>
@@ -10169,40 +10239,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="224" t="s">
+      <c r="A1" s="229" t="s">
         <v>330</v>
       </c>
-      <c r="B1" s="225"/>
-      <c r="C1" s="225"/>
-      <c r="D1" s="225"/>
-      <c r="E1" s="225"/>
-      <c r="F1" s="225"/>
-      <c r="G1" s="225"/>
-      <c r="H1" s="226"/>
+      <c r="B1" s="230"/>
+      <c r="C1" s="230"/>
+      <c r="D1" s="230"/>
+      <c r="E1" s="230"/>
+      <c r="F1" s="230"/>
+      <c r="G1" s="230"/>
+      <c r="H1" s="231"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="227"/>
-      <c r="B2" s="228"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="229"/>
+      <c r="A2" s="232"/>
+      <c r="B2" s="233"/>
+      <c r="C2" s="233"/>
+      <c r="D2" s="233"/>
+      <c r="E2" s="233"/>
+      <c r="F2" s="233"/>
+      <c r="G2" s="233"/>
+      <c r="H2" s="234"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="230" t="s">
+      <c r="A3" s="235" t="s">
         <v>253</v>
       </c>
-      <c r="B3" s="231"/>
-      <c r="C3" s="231"/>
-      <c r="D3" s="231"/>
-      <c r="E3" s="231" t="s">
+      <c r="B3" s="236"/>
+      <c r="C3" s="236"/>
+      <c r="D3" s="236"/>
+      <c r="E3" s="236" t="s">
         <v>254</v>
       </c>
-      <c r="F3" s="231"/>
-      <c r="G3" s="231"/>
-      <c r="H3" s="232"/>
+      <c r="F3" s="236"/>
+      <c r="G3" s="236"/>
+      <c r="H3" s="237"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="20">
@@ -10736,11 +10806,11 @@
       <c r="C27" s="144" t="s">
         <v>607</v>
       </c>
-      <c r="D27" s="233" t="s">
+      <c r="D27" s="228" t="s">
         <v>583</v>
       </c>
-      <c r="E27" s="233"/>
-      <c r="F27" s="233"/>
+      <c r="E27" s="228"/>
+      <c r="F27" s="228"/>
       <c r="G27" s="25"/>
       <c r="H27" s="26"/>
     </row>
@@ -10752,11 +10822,11 @@
       <c r="C28" s="144" t="s">
         <v>611</v>
       </c>
-      <c r="D28" s="233" t="s">
+      <c r="D28" s="228" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="233"/>
-      <c r="F28" s="233"/>
+      <c r="E28" s="228"/>
+      <c r="F28" s="228"/>
       <c r="G28" s="25"/>
       <c r="H28" s="26"/>
     </row>
@@ -10768,11 +10838,11 @@
       <c r="C29" s="144" t="s">
         <v>612</v>
       </c>
-      <c r="D29" s="233" t="s">
+      <c r="D29" s="228" t="s">
         <v>584</v>
       </c>
-      <c r="E29" s="233"/>
-      <c r="F29" s="233"/>
+      <c r="E29" s="228"/>
+      <c r="F29" s="228"/>
       <c r="G29" s="25"/>
       <c r="H29" s="26"/>
     </row>
@@ -10784,11 +10854,11 @@
       <c r="C30" s="144" t="s">
         <v>613</v>
       </c>
-      <c r="D30" s="233" t="s">
+      <c r="D30" s="228" t="s">
         <v>585</v>
       </c>
-      <c r="E30" s="233"/>
-      <c r="F30" s="233"/>
+      <c r="E30" s="228"/>
+      <c r="F30" s="228"/>
       <c r="G30" s="25"/>
       <c r="H30" s="26"/>
     </row>
@@ -10800,11 +10870,11 @@
       <c r="C31" s="144" t="s">
         <v>614</v>
       </c>
-      <c r="D31" s="233" t="s">
+      <c r="D31" s="228" t="s">
         <v>586</v>
       </c>
-      <c r="E31" s="233"/>
-      <c r="F31" s="233"/>
+      <c r="E31" s="228"/>
+      <c r="F31" s="228"/>
       <c r="G31" s="25"/>
       <c r="H31" s="26"/>
     </row>
@@ -10816,11 +10886,11 @@
       <c r="C32" s="144" t="s">
         <v>615</v>
       </c>
-      <c r="D32" s="233" t="s">
+      <c r="D32" s="228" t="s">
         <v>587</v>
       </c>
-      <c r="E32" s="233"/>
-      <c r="F32" s="233"/>
+      <c r="E32" s="228"/>
+      <c r="F32" s="228"/>
       <c r="G32" s="25"/>
       <c r="H32" s="26"/>
     </row>
@@ -10832,11 +10902,11 @@
       <c r="C33" s="144" t="s">
         <v>628</v>
       </c>
-      <c r="D33" s="233" t="s">
+      <c r="D33" s="228" t="s">
         <v>489</v>
       </c>
-      <c r="E33" s="233"/>
-      <c r="F33" s="233"/>
+      <c r="E33" s="228"/>
+      <c r="F33" s="228"/>
       <c r="G33" s="25"/>
       <c r="H33" s="26"/>
     </row>
@@ -10848,11 +10918,11 @@
       <c r="C34" s="144" t="s">
         <v>629</v>
       </c>
-      <c r="D34" s="233" t="s">
+      <c r="D34" s="228" t="s">
         <v>588</v>
       </c>
-      <c r="E34" s="233"/>
-      <c r="F34" s="233"/>
+      <c r="E34" s="228"/>
+      <c r="F34" s="228"/>
       <c r="G34" s="25"/>
       <c r="H34" s="26"/>
     </row>
@@ -10864,11 +10934,11 @@
       <c r="C35" s="144" t="s">
         <v>630</v>
       </c>
-      <c r="D35" s="233" t="s">
+      <c r="D35" s="228" t="s">
         <v>589</v>
       </c>
-      <c r="E35" s="233"/>
-      <c r="F35" s="233"/>
+      <c r="E35" s="228"/>
+      <c r="F35" s="228"/>
       <c r="G35" s="25"/>
       <c r="H35" s="26"/>
     </row>
@@ -10878,11 +10948,11 @@
       <c r="C36" s="144" t="s">
         <v>665</v>
       </c>
-      <c r="D36" s="234" t="s">
+      <c r="D36" s="225" t="s">
         <v>604</v>
       </c>
-      <c r="E36" s="235"/>
-      <c r="F36" s="236"/>
+      <c r="E36" s="226"/>
+      <c r="F36" s="227"/>
       <c r="G36" s="25"/>
       <c r="H36" s="26"/>
     </row>
@@ -10892,11 +10962,11 @@
       <c r="C37" s="144" t="s">
         <v>668</v>
       </c>
-      <c r="D37" s="234" t="s">
+      <c r="D37" s="225" t="s">
         <v>666</v>
       </c>
-      <c r="E37" s="235"/>
-      <c r="F37" s="236"/>
+      <c r="E37" s="226"/>
+      <c r="F37" s="227"/>
       <c r="G37" s="25"/>
       <c r="H37" s="26"/>
     </row>
@@ -10906,11 +10976,11 @@
       <c r="C38" s="144" t="s">
         <v>667</v>
       </c>
-      <c r="D38" s="234" t="s">
+      <c r="D38" s="225" t="s">
         <v>669</v>
       </c>
-      <c r="E38" s="235"/>
-      <c r="F38" s="236"/>
+      <c r="E38" s="226"/>
+      <c r="F38" s="227"/>
       <c r="G38" s="25"/>
       <c r="H38" s="26"/>
     </row>
@@ -10918,9 +10988,9 @@
       <c r="A39" s="24"/>
       <c r="B39" s="146"/>
       <c r="C39" s="144"/>
-      <c r="D39" s="234"/>
-      <c r="E39" s="235"/>
-      <c r="F39" s="236"/>
+      <c r="D39" s="225"/>
+      <c r="E39" s="226"/>
+      <c r="F39" s="227"/>
       <c r="G39" s="25"/>
       <c r="H39" s="26"/>
     </row>
@@ -11018,13 +11088,6 @@
     <row r="52" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:H3"/>
@@ -11034,6 +11097,13 @@
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11057,28 +11127,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="240" t="s">
+      <c r="A1" s="241" t="s">
         <v>331</v>
       </c>
-      <c r="B1" s="240"/>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
+      <c r="B1" s="241"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="241"/>
+      <c r="E1" s="241"/>
+      <c r="F1" s="241"/>
+      <c r="G1" s="241"/>
+      <c r="H1" s="241"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="237" t="s">
+      <c r="A2" s="238" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="238"/>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
-      <c r="G2" s="238"/>
-      <c r="H2" s="239"/>
+      <c r="B2" s="239"/>
+      <c r="C2" s="239"/>
+      <c r="D2" s="239"/>
+      <c r="E2" s="239"/>
+      <c r="F2" s="239"/>
+      <c r="G2" s="239"/>
+      <c r="H2" s="240"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="5"/>
@@ -11257,16 +11327,16 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="237" t="s">
+      <c r="A15" s="238" t="s">
         <v>225</v>
       </c>
-      <c r="B15" s="238"/>
-      <c r="C15" s="238"/>
-      <c r="D15" s="238"/>
-      <c r="E15" s="238"/>
-      <c r="F15" s="238"/>
-      <c r="G15" s="238"/>
-      <c r="H15" s="239"/>
+      <c r="B15" s="239"/>
+      <c r="C15" s="239"/>
+      <c r="D15" s="239"/>
+      <c r="E15" s="239"/>
+      <c r="F15" s="239"/>
+      <c r="G15" s="239"/>
+      <c r="H15" s="240"/>
     </row>
     <row r="16" spans="1:11" ht="15.75">
       <c r="A16" s="9"/>
@@ -11442,16 +11512,16 @@
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:11" ht="15.75">
-      <c r="A28" s="237" t="s">
+      <c r="A28" s="238" t="s">
         <v>226</v>
       </c>
-      <c r="B28" s="238"/>
-      <c r="C28" s="238"/>
-      <c r="D28" s="238"/>
-      <c r="E28" s="238"/>
-      <c r="F28" s="238"/>
-      <c r="G28" s="238"/>
-      <c r="H28" s="239"/>
+      <c r="B28" s="239"/>
+      <c r="C28" s="239"/>
+      <c r="D28" s="239"/>
+      <c r="E28" s="239"/>
+      <c r="F28" s="239"/>
+      <c r="G28" s="239"/>
+      <c r="H28" s="240"/>
     </row>
     <row r="29" spans="1:11" ht="15.75">
       <c r="A29" s="5"/>
@@ -11651,40 +11721,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="241" t="s">
+      <c r="A1" s="242" t="s">
         <v>332</v>
       </c>
-      <c r="B1" s="242"/>
-      <c r="C1" s="242"/>
-      <c r="D1" s="242"/>
-      <c r="E1" s="242"/>
-      <c r="F1" s="242"/>
-      <c r="G1" s="242"/>
-      <c r="H1" s="243"/>
+      <c r="B1" s="243"/>
+      <c r="C1" s="243"/>
+      <c r="D1" s="243"/>
+      <c r="E1" s="243"/>
+      <c r="F1" s="243"/>
+      <c r="G1" s="243"/>
+      <c r="H1" s="244"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="244"/>
-      <c r="B2" s="245"/>
-      <c r="C2" s="245"/>
-      <c r="D2" s="245"/>
-      <c r="E2" s="245"/>
-      <c r="F2" s="245"/>
-      <c r="G2" s="245"/>
-      <c r="H2" s="246"/>
+      <c r="A2" s="245"/>
+      <c r="B2" s="246"/>
+      <c r="C2" s="246"/>
+      <c r="D2" s="246"/>
+      <c r="E2" s="246"/>
+      <c r="F2" s="246"/>
+      <c r="G2" s="246"/>
+      <c r="H2" s="247"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="247" t="s">
+      <c r="A3" s="248" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="248"/>
-      <c r="C3" s="249"/>
-      <c r="D3" s="250"/>
-      <c r="E3" s="247" t="s">
+      <c r="B3" s="249"/>
+      <c r="C3" s="250"/>
+      <c r="D3" s="251"/>
+      <c r="E3" s="248" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="248"/>
-      <c r="G3" s="249"/>
-      <c r="H3" s="250"/>
+      <c r="F3" s="249"/>
+      <c r="G3" s="250"/>
+      <c r="H3" s="251"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="16">
@@ -12123,40 +12193,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="251" t="s">
+      <c r="A1" s="269" t="s">
         <v>333</v>
       </c>
-      <c r="B1" s="251"/>
-      <c r="C1" s="251"/>
-      <c r="D1" s="251"/>
-      <c r="E1" s="251"/>
-      <c r="F1" s="251"/>
-      <c r="G1" s="251"/>
-      <c r="H1" s="251"/>
+      <c r="B1" s="269"/>
+      <c r="C1" s="269"/>
+      <c r="D1" s="269"/>
+      <c r="E1" s="269"/>
+      <c r="F1" s="269"/>
+      <c r="G1" s="269"/>
+      <c r="H1" s="269"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="252"/>
-      <c r="B2" s="252"/>
-      <c r="C2" s="252"/>
-      <c r="D2" s="252"/>
-      <c r="E2" s="252"/>
-      <c r="F2" s="252"/>
-      <c r="G2" s="252"/>
-      <c r="H2" s="252"/>
+      <c r="A2" s="270"/>
+      <c r="B2" s="270"/>
+      <c r="C2" s="270"/>
+      <c r="D2" s="270"/>
+      <c r="E2" s="270"/>
+      <c r="F2" s="270"/>
+      <c r="G2" s="270"/>
+      <c r="H2" s="270"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="253" t="s">
+      <c r="A3" s="271" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="254"/>
-      <c r="C3" s="255"/>
-      <c r="D3" s="256"/>
-      <c r="E3" s="253" t="s">
+      <c r="B3" s="272"/>
+      <c r="C3" s="273"/>
+      <c r="D3" s="274"/>
+      <c r="E3" s="271" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="254"/>
-      <c r="G3" s="255"/>
-      <c r="H3" s="256"/>
+      <c r="F3" s="272"/>
+      <c r="G3" s="273"/>
+      <c r="H3" s="274"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="46">
@@ -12449,114 +12519,114 @@
       <c r="H24" s="74"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="253" t="s">
+      <c r="A25" s="271" t="s">
         <v>293</v>
       </c>
-      <c r="B25" s="254"/>
-      <c r="C25" s="255"/>
-      <c r="D25" s="256"/>
-      <c r="E25" s="253" t="s">
+      <c r="B25" s="272"/>
+      <c r="C25" s="273"/>
+      <c r="D25" s="274"/>
+      <c r="E25" s="271" t="s">
         <v>294</v>
       </c>
-      <c r="F25" s="254"/>
-      <c r="G25" s="255"/>
-      <c r="H25" s="256"/>
+      <c r="F25" s="272"/>
+      <c r="G25" s="273"/>
+      <c r="H25" s="274"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="50" t="s">
         <v>295</v>
       </c>
-      <c r="B26" s="257"/>
-      <c r="C26" s="258"/>
-      <c r="D26" s="259"/>
+      <c r="B26" s="258"/>
+      <c r="C26" s="259"/>
+      <c r="D26" s="260"/>
       <c r="E26" s="46" t="s">
         <v>296</v>
       </c>
-      <c r="F26" s="260"/>
-      <c r="G26" s="261"/>
-      <c r="H26" s="262"/>
+      <c r="F26" s="266"/>
+      <c r="G26" s="267"/>
+      <c r="H26" s="268"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="B27" s="263"/>
-      <c r="C27" s="264"/>
-      <c r="D27" s="265"/>
+      <c r="B27" s="261"/>
+      <c r="C27" s="262"/>
+      <c r="D27" s="264"/>
       <c r="E27" s="50" t="s">
         <v>298</v>
       </c>
-      <c r="F27" s="257"/>
-      <c r="G27" s="258"/>
-      <c r="H27" s="266"/>
+      <c r="F27" s="258"/>
+      <c r="G27" s="259"/>
+      <c r="H27" s="265"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="50" t="s">
         <v>299</v>
       </c>
-      <c r="B28" s="257"/>
-      <c r="C28" s="258"/>
-      <c r="D28" s="259"/>
+      <c r="B28" s="258"/>
+      <c r="C28" s="259"/>
+      <c r="D28" s="260"/>
       <c r="E28" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="F28" s="263"/>
-      <c r="G28" s="264"/>
-      <c r="H28" s="267"/>
+      <c r="F28" s="261"/>
+      <c r="G28" s="262"/>
+      <c r="H28" s="263"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="58" t="s">
         <v>301</v>
       </c>
-      <c r="B29" s="263"/>
-      <c r="C29" s="264"/>
-      <c r="D29" s="265"/>
+      <c r="B29" s="261"/>
+      <c r="C29" s="262"/>
+      <c r="D29" s="264"/>
       <c r="E29" s="50" t="s">
         <v>302</v>
       </c>
-      <c r="F29" s="257"/>
-      <c r="G29" s="258"/>
-      <c r="H29" s="266"/>
+      <c r="F29" s="258"/>
+      <c r="G29" s="259"/>
+      <c r="H29" s="265"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="50" t="s">
         <v>303</v>
       </c>
-      <c r="B30" s="257"/>
-      <c r="C30" s="258"/>
-      <c r="D30" s="259"/>
+      <c r="B30" s="258"/>
+      <c r="C30" s="259"/>
+      <c r="D30" s="260"/>
       <c r="E30" s="58" t="s">
         <v>304</v>
       </c>
-      <c r="F30" s="263"/>
-      <c r="G30" s="264"/>
-      <c r="H30" s="267"/>
+      <c r="F30" s="261"/>
+      <c r="G30" s="262"/>
+      <c r="H30" s="263"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="B31" s="263"/>
-      <c r="C31" s="264"/>
-      <c r="D31" s="265"/>
+      <c r="B31" s="261"/>
+      <c r="C31" s="262"/>
+      <c r="D31" s="264"/>
       <c r="E31" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="F31" s="257"/>
-      <c r="G31" s="258"/>
-      <c r="H31" s="266"/>
+      <c r="F31" s="258"/>
+      <c r="G31" s="259"/>
+      <c r="H31" s="265"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="50" t="s">
         <v>307</v>
       </c>
-      <c r="B32" s="257"/>
-      <c r="C32" s="258"/>
-      <c r="D32" s="259"/>
+      <c r="B32" s="258"/>
+      <c r="C32" s="259"/>
+      <c r="D32" s="260"/>
       <c r="E32" s="58"/>
-      <c r="F32" s="263"/>
-      <c r="G32" s="264"/>
-      <c r="H32" s="267" t="s">
+      <c r="F32" s="261"/>
+      <c r="G32" s="262"/>
+      <c r="H32" s="263" t="s">
         <v>245</v>
       </c>
     </row>
@@ -12564,13 +12634,13 @@
       <c r="A33" s="58" t="s">
         <v>308</v>
       </c>
-      <c r="B33" s="263"/>
-      <c r="C33" s="264"/>
-      <c r="D33" s="265"/>
+      <c r="B33" s="261"/>
+      <c r="C33" s="262"/>
+      <c r="D33" s="264"/>
       <c r="E33" s="50"/>
-      <c r="F33" s="257"/>
-      <c r="G33" s="258"/>
-      <c r="H33" s="266" t="s">
+      <c r="F33" s="258"/>
+      <c r="G33" s="259"/>
+      <c r="H33" s="265" t="s">
         <v>288</v>
       </c>
     </row>
@@ -12578,13 +12648,13 @@
       <c r="A34" s="50" t="s">
         <v>309</v>
       </c>
-      <c r="B34" s="257"/>
-      <c r="C34" s="258"/>
-      <c r="D34" s="259"/>
+      <c r="B34" s="258"/>
+      <c r="C34" s="259"/>
+      <c r="D34" s="260"/>
       <c r="E34" s="58"/>
-      <c r="F34" s="263"/>
-      <c r="G34" s="264"/>
-      <c r="H34" s="267" t="s">
+      <c r="F34" s="261"/>
+      <c r="G34" s="262"/>
+      <c r="H34" s="263" t="s">
         <v>289</v>
       </c>
     </row>
@@ -12592,13 +12662,13 @@
       <c r="A35" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="B35" s="263"/>
-      <c r="C35" s="264"/>
-      <c r="D35" s="265"/>
+      <c r="B35" s="261"/>
+      <c r="C35" s="262"/>
+      <c r="D35" s="264"/>
       <c r="E35" s="50"/>
-      <c r="F35" s="257"/>
-      <c r="G35" s="258"/>
-      <c r="H35" s="266" t="s">
+      <c r="F35" s="258"/>
+      <c r="G35" s="259"/>
+      <c r="H35" s="265" t="s">
         <v>290</v>
       </c>
     </row>
@@ -12606,13 +12676,13 @@
       <c r="A36" s="50" t="s">
         <v>311</v>
       </c>
-      <c r="B36" s="257"/>
-      <c r="C36" s="258"/>
-      <c r="D36" s="259"/>
+      <c r="B36" s="258"/>
+      <c r="C36" s="259"/>
+      <c r="D36" s="260"/>
       <c r="E36" s="58"/>
-      <c r="F36" s="263"/>
-      <c r="G36" s="264"/>
-      <c r="H36" s="267" t="s">
+      <c r="F36" s="261"/>
+      <c r="G36" s="262"/>
+      <c r="H36" s="263" t="s">
         <v>291</v>
       </c>
     </row>
@@ -12620,13 +12690,13 @@
       <c r="A37" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="B37" s="263"/>
-      <c r="C37" s="264"/>
-      <c r="D37" s="265"/>
+      <c r="B37" s="261"/>
+      <c r="C37" s="262"/>
+      <c r="D37" s="264"/>
       <c r="E37" s="50"/>
-      <c r="F37" s="257"/>
-      <c r="G37" s="258"/>
-      <c r="H37" s="266" t="s">
+      <c r="F37" s="258"/>
+      <c r="G37" s="259"/>
+      <c r="H37" s="265" t="s">
         <v>292</v>
       </c>
     </row>
@@ -12634,13 +12704,13 @@
       <c r="A38" s="50" t="s">
         <v>313</v>
       </c>
-      <c r="B38" s="257"/>
-      <c r="C38" s="258"/>
-      <c r="D38" s="259"/>
+      <c r="B38" s="258"/>
+      <c r="C38" s="259"/>
+      <c r="D38" s="260"/>
       <c r="E38" s="58"/>
-      <c r="F38" s="263"/>
-      <c r="G38" s="264"/>
-      <c r="H38" s="267" t="s">
+      <c r="F38" s="261"/>
+      <c r="G38" s="262"/>
+      <c r="H38" s="263" t="s">
         <v>244</v>
       </c>
     </row>
@@ -12648,13 +12718,13 @@
       <c r="A39" s="58" t="s">
         <v>314</v>
       </c>
-      <c r="B39" s="263"/>
-      <c r="C39" s="264"/>
-      <c r="D39" s="265"/>
+      <c r="B39" s="261"/>
+      <c r="C39" s="262"/>
+      <c r="D39" s="264"/>
       <c r="E39" s="50"/>
-      <c r="F39" s="257"/>
-      <c r="G39" s="258"/>
-      <c r="H39" s="266" t="s">
+      <c r="F39" s="258"/>
+      <c r="G39" s="259"/>
+      <c r="H39" s="265" t="s">
         <v>245</v>
       </c>
     </row>
@@ -12662,28 +12732,57 @@
       <c r="A40" s="50" t="s">
         <v>315</v>
       </c>
-      <c r="B40" s="257"/>
-      <c r="C40" s="258"/>
-      <c r="D40" s="259"/>
+      <c r="B40" s="258"/>
+      <c r="C40" s="259"/>
+      <c r="D40" s="260"/>
       <c r="E40" s="58"/>
-      <c r="F40" s="263"/>
-      <c r="G40" s="264"/>
-      <c r="H40" s="267"/>
+      <c r="F40" s="261"/>
+      <c r="G40" s="262"/>
+      <c r="H40" s="263"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="70" t="s">
         <v>316</v>
       </c>
-      <c r="B41" s="268"/>
-      <c r="C41" s="269"/>
-      <c r="D41" s="270"/>
+      <c r="B41" s="252"/>
+      <c r="C41" s="253"/>
+      <c r="D41" s="254"/>
       <c r="E41" s="75"/>
-      <c r="F41" s="271"/>
-      <c r="G41" s="272"/>
-      <c r="H41" s="273"/>
+      <c r="F41" s="255"/>
+      <c r="G41" s="256"/>
+      <c r="H41" s="257"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -12692,35 +12791,6 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12749,40 +12819,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="280" t="s">
+      <c r="A1" s="281" t="s">
         <v>334</v>
       </c>
-      <c r="B1" s="281"/>
-      <c r="C1" s="281"/>
-      <c r="D1" s="281"/>
-      <c r="E1" s="281"/>
-      <c r="F1" s="281"/>
-      <c r="G1" s="281"/>
-      <c r="H1" s="282"/>
+      <c r="B1" s="282"/>
+      <c r="C1" s="282"/>
+      <c r="D1" s="282"/>
+      <c r="E1" s="282"/>
+      <c r="F1" s="282"/>
+      <c r="G1" s="282"/>
+      <c r="H1" s="283"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="283"/>
-      <c r="B2" s="284"/>
-      <c r="C2" s="284"/>
-      <c r="D2" s="284"/>
-      <c r="E2" s="284"/>
-      <c r="F2" s="284"/>
-      <c r="G2" s="284"/>
-      <c r="H2" s="285"/>
+      <c r="A2" s="284"/>
+      <c r="B2" s="285"/>
+      <c r="C2" s="285"/>
+      <c r="D2" s="285"/>
+      <c r="E2" s="285"/>
+      <c r="F2" s="285"/>
+      <c r="G2" s="285"/>
+      <c r="H2" s="286"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="274" t="s">
+      <c r="A3" s="275" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="275"/>
-      <c r="C3" s="275"/>
-      <c r="D3" s="276"/>
-      <c r="E3" s="274" t="s">
+      <c r="B3" s="276"/>
+      <c r="C3" s="276"/>
+      <c r="D3" s="277"/>
+      <c r="E3" s="275" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="275"/>
-      <c r="G3" s="275"/>
-      <c r="H3" s="276"/>
+      <c r="F3" s="276"/>
+      <c r="G3" s="276"/>
+      <c r="H3" s="277"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="93">
@@ -12999,18 +13069,18 @@
       <c r="H21" s="85"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="277" t="s">
+      <c r="A22" s="278" t="s">
         <v>319</v>
       </c>
-      <c r="B22" s="278"/>
-      <c r="C22" s="278"/>
-      <c r="D22" s="279"/>
-      <c r="E22" s="277" t="s">
+      <c r="B22" s="279"/>
+      <c r="C22" s="279"/>
+      <c r="D22" s="280"/>
+      <c r="E22" s="278" t="s">
         <v>320</v>
       </c>
-      <c r="F22" s="278"/>
-      <c r="G22" s="278"/>
-      <c r="H22" s="279"/>
+      <c r="F22" s="279"/>
+      <c r="G22" s="279"/>
+      <c r="H22" s="280"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="78">
@@ -13287,40 +13357,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="224" t="s">
+      <c r="A1" s="229" t="s">
         <v>495</v>
       </c>
-      <c r="B1" s="225"/>
-      <c r="C1" s="225"/>
-      <c r="D1" s="225"/>
-      <c r="E1" s="225"/>
-      <c r="F1" s="225"/>
-      <c r="G1" s="225"/>
-      <c r="H1" s="226"/>
+      <c r="B1" s="230"/>
+      <c r="C1" s="230"/>
+      <c r="D1" s="230"/>
+      <c r="E1" s="230"/>
+      <c r="F1" s="230"/>
+      <c r="G1" s="230"/>
+      <c r="H1" s="231"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="227"/>
-      <c r="B2" s="228"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="229"/>
+      <c r="A2" s="232"/>
+      <c r="B2" s="233"/>
+      <c r="C2" s="233"/>
+      <c r="D2" s="233"/>
+      <c r="E2" s="233"/>
+      <c r="F2" s="233"/>
+      <c r="G2" s="233"/>
+      <c r="H2" s="234"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="230" t="s">
+      <c r="A3" s="235" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="231"/>
-      <c r="C3" s="231"/>
-      <c r="D3" s="231"/>
-      <c r="E3" s="231" t="s">
+      <c r="B3" s="236"/>
+      <c r="C3" s="236"/>
+      <c r="D3" s="236"/>
+      <c r="E3" s="236" t="s">
         <v>322</v>
       </c>
-      <c r="F3" s="231"/>
-      <c r="G3" s="231"/>
-      <c r="H3" s="232"/>
+      <c r="F3" s="236"/>
+      <c r="G3" s="236"/>
+      <c r="H3" s="237"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="20">

</xml_diff>

<commit_message>
chg: Added range 34: Anti surface warfare training (ASUW)
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="853">
   <si>
     <t>AWACS</t>
   </si>
@@ -2579,6 +2579,9 @@
   </si>
   <si>
     <t>46X</t>
+  </si>
+  <si>
+    <t>Apache</t>
   </si>
 </sst>
 </file>
@@ -4203,21 +4206,21 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4263,6 +4266,36 @@
     <xf numFmtId="0" fontId="26" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4272,36 +4305,6 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4344,6 +4347,57 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4361,57 +4415,6 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4795,7 +4798,7 @@
   <sheetPr codeName="Ark1"/>
   <dimension ref="A1:AP53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AJ41" sqref="AJ41"/>
     </sheetView>
   </sheetViews>
@@ -4912,13 +4915,13 @@
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
       <c r="T2" s="12"/>
-      <c r="V2" s="206" t="s">
+      <c r="V2" s="205" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="206"/>
-      <c r="X2" s="206"/>
-      <c r="Y2" s="206"/>
-      <c r="Z2" s="206"/>
+      <c r="W2" s="205"/>
+      <c r="X2" s="205"/>
+      <c r="Y2" s="205"/>
+      <c r="Z2" s="205"/>
       <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
       <c r="AC2" s="12"/>
@@ -4973,9 +4976,9 @@
         <v>433</v>
       </c>
       <c r="Q3" s="12"/>
-      <c r="R3" s="205"/>
-      <c r="S3" s="205"/>
-      <c r="T3" s="205"/>
+      <c r="R3" s="209"/>
+      <c r="S3" s="209"/>
+      <c r="T3" s="209"/>
       <c r="V3" s="122" t="s">
         <v>335</v>
       </c>
@@ -5059,22 +5062,22 @@
       <c r="AA4" s="36"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="36"/>
-      <c r="AD4" s="206" t="s">
+      <c r="AD4" s="205" t="s">
         <v>436</v>
       </c>
-      <c r="AE4" s="206"/>
-      <c r="AF4" s="206"/>
-      <c r="AG4" s="206"/>
-      <c r="AH4" s="206"/>
-      <c r="AJ4" s="206" t="s">
+      <c r="AE4" s="205"/>
+      <c r="AF4" s="205"/>
+      <c r="AG4" s="205"/>
+      <c r="AH4" s="205"/>
+      <c r="AJ4" s="205" t="s">
         <v>1</v>
       </c>
-      <c r="AK4" s="206"/>
-      <c r="AL4" s="206"/>
-      <c r="AM4" s="206"/>
-      <c r="AN4" s="206"/>
-      <c r="AO4" s="206"/>
-      <c r="AP4" s="206"/>
+      <c r="AK4" s="205"/>
+      <c r="AL4" s="205"/>
+      <c r="AM4" s="205"/>
+      <c r="AN4" s="205"/>
+      <c r="AO4" s="205"/>
+      <c r="AP4" s="205"/>
     </row>
     <row r="5" spans="1:42" ht="15.75">
       <c r="A5" s="129" t="s">
@@ -6167,15 +6170,15 @@
       <c r="AH17" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="AJ17" s="206" t="s">
+      <c r="AJ17" s="205" t="s">
         <v>277</v>
       </c>
-      <c r="AK17" s="206"/>
-      <c r="AL17" s="206"/>
-      <c r="AM17" s="206"/>
-      <c r="AN17" s="206"/>
-      <c r="AO17" s="206"/>
-      <c r="AP17" s="206"/>
+      <c r="AK17" s="205"/>
+      <c r="AL17" s="205"/>
+      <c r="AM17" s="205"/>
+      <c r="AN17" s="205"/>
+      <c r="AO17" s="205"/>
+      <c r="AP17" s="205"/>
     </row>
     <row r="18" spans="1:42" ht="15.75">
       <c r="A18" s="129" t="s">
@@ -6392,9 +6395,9 @@
       <c r="O20" s="35"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="205"/>
-      <c r="S20" s="205"/>
-      <c r="T20" s="205"/>
+      <c r="R20" s="209"/>
+      <c r="S20" s="209"/>
+      <c r="T20" s="209"/>
       <c r="U20" s="2"/>
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
@@ -6734,13 +6737,13 @@
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
-      <c r="AD24" s="206" t="s">
+      <c r="AD24" s="205" t="s">
         <v>493</v>
       </c>
-      <c r="AE24" s="206"/>
-      <c r="AF24" s="206"/>
-      <c r="AG24" s="206"/>
-      <c r="AH24" s="206"/>
+      <c r="AE24" s="205"/>
+      <c r="AF24" s="205"/>
+      <c r="AG24" s="205"/>
+      <c r="AH24" s="205"/>
       <c r="AJ24" s="142" t="s">
         <v>568</v>
       </c>
@@ -6896,15 +6899,15 @@
       <c r="AH26" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="AJ26" s="206" t="s">
+      <c r="AJ26" s="205" t="s">
         <v>847</v>
       </c>
-      <c r="AK26" s="206"/>
-      <c r="AL26" s="206"/>
-      <c r="AM26" s="206"/>
-      <c r="AN26" s="206"/>
-      <c r="AO26" s="206"/>
-      <c r="AP26" s="206"/>
+      <c r="AK26" s="205"/>
+      <c r="AL26" s="205"/>
+      <c r="AM26" s="205"/>
+      <c r="AN26" s="205"/>
+      <c r="AO26" s="205"/>
+      <c r="AP26" s="205"/>
     </row>
     <row r="27" spans="1:42">
       <c r="A27" s="129" t="s">
@@ -7101,15 +7104,15 @@
       <c r="S29" s="35"/>
       <c r="T29" s="35"/>
       <c r="U29" s="35"/>
-      <c r="V29" s="206" t="s">
+      <c r="V29" s="205" t="s">
         <v>212</v>
       </c>
-      <c r="W29" s="206"/>
-      <c r="X29" s="206"/>
-      <c r="Y29" s="206"/>
-      <c r="Z29" s="206"/>
-      <c r="AA29" s="206"/>
-      <c r="AB29" s="206"/>
+      <c r="W29" s="205"/>
+      <c r="X29" s="205"/>
+      <c r="Y29" s="205"/>
+      <c r="Z29" s="205"/>
+      <c r="AA29" s="205"/>
+      <c r="AB29" s="205"/>
     </row>
     <row r="30" spans="1:42">
       <c r="A30" s="129"/>
@@ -7199,11 +7202,11 @@
       <c r="Y31" s="37"/>
       <c r="Z31" s="37"/>
       <c r="AA31" s="12"/>
-      <c r="AD31" s="207" t="s">
+      <c r="AD31" s="206" t="s">
         <v>263</v>
       </c>
-      <c r="AE31" s="208"/>
-      <c r="AF31" s="209"/>
+      <c r="AE31" s="207"/>
+      <c r="AF31" s="208"/>
     </row>
     <row r="32" spans="1:42">
       <c r="S32" s="12"/>
@@ -7308,15 +7311,15 @@
       <c r="S37" s="12"/>
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
-      <c r="V37" s="206" t="s">
+      <c r="V37" s="205" t="s">
         <v>9</v>
       </c>
-      <c r="W37" s="206"/>
-      <c r="X37" s="206"/>
-      <c r="Y37" s="206"/>
-      <c r="Z37" s="206"/>
-      <c r="AA37" s="206"/>
-      <c r="AB37" s="206"/>
+      <c r="W37" s="205"/>
+      <c r="X37" s="205"/>
+      <c r="Y37" s="205"/>
+      <c r="Z37" s="205"/>
+      <c r="AA37" s="205"/>
+      <c r="AB37" s="205"/>
       <c r="AD37" s="3" t="s">
         <v>259</v>
       </c>
@@ -7415,15 +7418,15 @@
       <c r="S42" s="12"/>
       <c r="T42" s="12"/>
       <c r="U42" s="12"/>
-      <c r="V42" s="206" t="s">
+      <c r="V42" s="205" t="s">
         <v>247</v>
       </c>
-      <c r="W42" s="206"/>
-      <c r="X42" s="206"/>
-      <c r="Y42" s="206"/>
-      <c r="Z42" s="206"/>
-      <c r="AA42" s="206"/>
-      <c r="AB42" s="206"/>
+      <c r="W42" s="205"/>
+      <c r="X42" s="205"/>
+      <c r="Y42" s="205"/>
+      <c r="Z42" s="205"/>
+      <c r="AA42" s="205"/>
+      <c r="AB42" s="205"/>
       <c r="AD42" s="3" t="s">
         <v>265</v>
       </c>
@@ -7528,15 +7531,15 @@
       <c r="S48" s="12"/>
       <c r="T48" s="12"/>
       <c r="U48" s="12"/>
-      <c r="V48" s="207" t="s">
+      <c r="V48" s="206" t="s">
         <v>480</v>
       </c>
-      <c r="W48" s="208"/>
-      <c r="X48" s="208"/>
-      <c r="Y48" s="208"/>
-      <c r="Z48" s="208"/>
-      <c r="AA48" s="208"/>
-      <c r="AB48" s="209"/>
+      <c r="W48" s="207"/>
+      <c r="X48" s="207"/>
+      <c r="Y48" s="207"/>
+      <c r="Z48" s="207"/>
+      <c r="AA48" s="207"/>
+      <c r="AB48" s="208"/>
     </row>
     <row r="49" spans="19:28">
       <c r="S49" s="12"/>
@@ -7626,11 +7629,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="V42:AB42"/>
-    <mergeCell ref="AD4:AH4"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="V48:AB48"/>
-    <mergeCell ref="V37:AB37"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="AJ4:AP4"/>
@@ -7639,6 +7637,11 @@
     <mergeCell ref="V29:AB29"/>
     <mergeCell ref="AD24:AH24"/>
     <mergeCell ref="AJ26:AP26"/>
+    <mergeCell ref="V42:AB42"/>
+    <mergeCell ref="AD4:AH4"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="V48:AB48"/>
+    <mergeCell ref="V37:AB37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8580,8 +8583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AJ45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AC19" sqref="AC19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AB18" sqref="AB18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -8617,48 +8620,48 @@
       </c>
     </row>
     <row r="2" spans="2:36">
-      <c r="B2" s="206" t="s">
+      <c r="B2" s="205" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="206"/>
-      <c r="D2" s="206"/>
-      <c r="E2" s="206"/>
-      <c r="F2" s="206"/>
-      <c r="H2" s="206" t="s">
+      <c r="C2" s="205"/>
+      <c r="D2" s="205"/>
+      <c r="E2" s="205"/>
+      <c r="F2" s="205"/>
+      <c r="H2" s="205" t="s">
         <v>231</v>
       </c>
-      <c r="I2" s="206"/>
-      <c r="J2" s="206"/>
-      <c r="K2" s="206"/>
-      <c r="L2" s="206"/>
-      <c r="N2" s="206" t="s">
+      <c r="I2" s="205"/>
+      <c r="J2" s="205"/>
+      <c r="K2" s="205"/>
+      <c r="L2" s="205"/>
+      <c r="N2" s="205" t="s">
         <v>239</v>
       </c>
-      <c r="O2" s="206"/>
-      <c r="P2" s="206"/>
-      <c r="Q2" s="206"/>
-      <c r="R2" s="206"/>
-      <c r="T2" s="206" t="s">
+      <c r="O2" s="205"/>
+      <c r="P2" s="205"/>
+      <c r="Q2" s="205"/>
+      <c r="R2" s="205"/>
+      <c r="T2" s="205" t="s">
         <v>249</v>
       </c>
-      <c r="U2" s="206"/>
-      <c r="V2" s="206"/>
-      <c r="W2" s="206"/>
-      <c r="X2" s="206"/>
-      <c r="Z2" s="206" t="s">
+      <c r="U2" s="205"/>
+      <c r="V2" s="205"/>
+      <c r="W2" s="205"/>
+      <c r="X2" s="205"/>
+      <c r="Z2" s="205" t="s">
         <v>321</v>
       </c>
-      <c r="AA2" s="206"/>
-      <c r="AB2" s="206"/>
-      <c r="AC2" s="206"/>
-      <c r="AD2" s="206"/>
-      <c r="AF2" s="206" t="s">
+      <c r="AA2" s="205"/>
+      <c r="AB2" s="205"/>
+      <c r="AC2" s="205"/>
+      <c r="AD2" s="205"/>
+      <c r="AF2" s="205" t="s">
         <v>498</v>
       </c>
-      <c r="AG2" s="206"/>
-      <c r="AH2" s="206"/>
-      <c r="AI2" s="206"/>
-      <c r="AJ2" s="206"/>
+      <c r="AG2" s="205"/>
+      <c r="AH2" s="205"/>
+      <c r="AI2" s="205"/>
+      <c r="AJ2" s="205"/>
     </row>
     <row r="3" spans="2:36">
       <c r="B3" s="124" t="s">
@@ -8782,6 +8785,12 @@
       </c>
       <c r="AA4" t="s">
         <v>482</v>
+      </c>
+      <c r="AB4">
+        <v>511</v>
+      </c>
+      <c r="AC4">
+        <v>511</v>
       </c>
       <c r="AF4" s="3" t="s">
         <v>838</v>
@@ -8863,6 +8872,12 @@
       <c r="AA8" t="s">
         <v>482</v>
       </c>
+      <c r="AB8">
+        <v>521</v>
+      </c>
+      <c r="AC8">
+        <v>521</v>
+      </c>
       <c r="AF8" s="3" t="s">
         <v>839</v>
       </c>
@@ -8947,6 +8962,18 @@
       </c>
       <c r="F12" s="126" t="s">
         <v>727</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>852</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>482</v>
+      </c>
+      <c r="AB12">
+        <v>531</v>
+      </c>
+      <c r="AC12">
+        <v>531</v>
       </c>
       <c r="AF12" s="3" t="s">
         <v>846</v>
@@ -9133,20 +9160,20 @@
       <c r="F24" s="140"/>
     </row>
     <row r="25" spans="2:20">
-      <c r="B25" s="206" t="s">
+      <c r="B25" s="205" t="s">
         <v>711</v>
       </c>
-      <c r="C25" s="206"/>
-      <c r="D25" s="206"/>
-      <c r="E25" s="206"/>
-      <c r="F25" s="206"/>
-      <c r="H25" s="206" t="s">
+      <c r="C25" s="205"/>
+      <c r="D25" s="205"/>
+      <c r="E25" s="205"/>
+      <c r="F25" s="205"/>
+      <c r="H25" s="205" t="s">
         <v>766</v>
       </c>
-      <c r="I25" s="206"/>
-      <c r="J25" s="206"/>
-      <c r="K25" s="206"/>
-      <c r="L25" s="206"/>
+      <c r="I25" s="205"/>
+      <c r="J25" s="205"/>
+      <c r="K25" s="205"/>
+      <c r="L25" s="205"/>
     </row>
     <row r="26" spans="2:20">
       <c r="B26" s="124" t="s">
@@ -10239,40 +10266,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="229" t="s">
+      <c r="A1" s="225" t="s">
         <v>330</v>
       </c>
-      <c r="B1" s="230"/>
-      <c r="C1" s="230"/>
-      <c r="D1" s="230"/>
-      <c r="E1" s="230"/>
-      <c r="F1" s="230"/>
-      <c r="G1" s="230"/>
-      <c r="H1" s="231"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="227"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="232"/>
-      <c r="B2" s="233"/>
-      <c r="C2" s="233"/>
-      <c r="D2" s="233"/>
-      <c r="E2" s="233"/>
-      <c r="F2" s="233"/>
-      <c r="G2" s="233"/>
-      <c r="H2" s="234"/>
+      <c r="A2" s="228"/>
+      <c r="B2" s="229"/>
+      <c r="C2" s="229"/>
+      <c r="D2" s="229"/>
+      <c r="E2" s="229"/>
+      <c r="F2" s="229"/>
+      <c r="G2" s="229"/>
+      <c r="H2" s="230"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="235" t="s">
+      <c r="A3" s="231" t="s">
         <v>253</v>
       </c>
-      <c r="B3" s="236"/>
-      <c r="C3" s="236"/>
-      <c r="D3" s="236"/>
-      <c r="E3" s="236" t="s">
+      <c r="B3" s="232"/>
+      <c r="C3" s="232"/>
+      <c r="D3" s="232"/>
+      <c r="E3" s="232" t="s">
         <v>254</v>
       </c>
-      <c r="F3" s="236"/>
-      <c r="G3" s="236"/>
-      <c r="H3" s="237"/>
+      <c r="F3" s="232"/>
+      <c r="G3" s="232"/>
+      <c r="H3" s="233"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="20">
@@ -10806,11 +10833,11 @@
       <c r="C27" s="144" t="s">
         <v>607</v>
       </c>
-      <c r="D27" s="228" t="s">
+      <c r="D27" s="234" t="s">
         <v>583</v>
       </c>
-      <c r="E27" s="228"/>
-      <c r="F27" s="228"/>
+      <c r="E27" s="234"/>
+      <c r="F27" s="234"/>
       <c r="G27" s="25"/>
       <c r="H27" s="26"/>
     </row>
@@ -10822,11 +10849,11 @@
       <c r="C28" s="144" t="s">
         <v>611</v>
       </c>
-      <c r="D28" s="228" t="s">
+      <c r="D28" s="234" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="228"/>
-      <c r="F28" s="228"/>
+      <c r="E28" s="234"/>
+      <c r="F28" s="234"/>
       <c r="G28" s="25"/>
       <c r="H28" s="26"/>
     </row>
@@ -10838,11 +10865,11 @@
       <c r="C29" s="144" t="s">
         <v>612</v>
       </c>
-      <c r="D29" s="228" t="s">
+      <c r="D29" s="234" t="s">
         <v>584</v>
       </c>
-      <c r="E29" s="228"/>
-      <c r="F29" s="228"/>
+      <c r="E29" s="234"/>
+      <c r="F29" s="234"/>
       <c r="G29" s="25"/>
       <c r="H29" s="26"/>
     </row>
@@ -10854,11 +10881,11 @@
       <c r="C30" s="144" t="s">
         <v>613</v>
       </c>
-      <c r="D30" s="228" t="s">
+      <c r="D30" s="234" t="s">
         <v>585</v>
       </c>
-      <c r="E30" s="228"/>
-      <c r="F30" s="228"/>
+      <c r="E30" s="234"/>
+      <c r="F30" s="234"/>
       <c r="G30" s="25"/>
       <c r="H30" s="26"/>
     </row>
@@ -10870,11 +10897,11 @@
       <c r="C31" s="144" t="s">
         <v>614</v>
       </c>
-      <c r="D31" s="228" t="s">
+      <c r="D31" s="234" t="s">
         <v>586</v>
       </c>
-      <c r="E31" s="228"/>
-      <c r="F31" s="228"/>
+      <c r="E31" s="234"/>
+      <c r="F31" s="234"/>
       <c r="G31" s="25"/>
       <c r="H31" s="26"/>
     </row>
@@ -10886,11 +10913,11 @@
       <c r="C32" s="144" t="s">
         <v>615</v>
       </c>
-      <c r="D32" s="228" t="s">
+      <c r="D32" s="234" t="s">
         <v>587</v>
       </c>
-      <c r="E32" s="228"/>
-      <c r="F32" s="228"/>
+      <c r="E32" s="234"/>
+      <c r="F32" s="234"/>
       <c r="G32" s="25"/>
       <c r="H32" s="26"/>
     </row>
@@ -10902,11 +10929,11 @@
       <c r="C33" s="144" t="s">
         <v>628</v>
       </c>
-      <c r="D33" s="228" t="s">
+      <c r="D33" s="234" t="s">
         <v>489</v>
       </c>
-      <c r="E33" s="228"/>
-      <c r="F33" s="228"/>
+      <c r="E33" s="234"/>
+      <c r="F33" s="234"/>
       <c r="G33" s="25"/>
       <c r="H33" s="26"/>
     </row>
@@ -10918,11 +10945,11 @@
       <c r="C34" s="144" t="s">
         <v>629</v>
       </c>
-      <c r="D34" s="228" t="s">
+      <c r="D34" s="234" t="s">
         <v>588</v>
       </c>
-      <c r="E34" s="228"/>
-      <c r="F34" s="228"/>
+      <c r="E34" s="234"/>
+      <c r="F34" s="234"/>
       <c r="G34" s="25"/>
       <c r="H34" s="26"/>
     </row>
@@ -10934,11 +10961,11 @@
       <c r="C35" s="144" t="s">
         <v>630</v>
       </c>
-      <c r="D35" s="228" t="s">
+      <c r="D35" s="234" t="s">
         <v>589</v>
       </c>
-      <c r="E35" s="228"/>
-      <c r="F35" s="228"/>
+      <c r="E35" s="234"/>
+      <c r="F35" s="234"/>
       <c r="G35" s="25"/>
       <c r="H35" s="26"/>
     </row>
@@ -10948,11 +10975,11 @@
       <c r="C36" s="144" t="s">
         <v>665</v>
       </c>
-      <c r="D36" s="225" t="s">
+      <c r="D36" s="235" t="s">
         <v>604</v>
       </c>
-      <c r="E36" s="226"/>
-      <c r="F36" s="227"/>
+      <c r="E36" s="236"/>
+      <c r="F36" s="237"/>
       <c r="G36" s="25"/>
       <c r="H36" s="26"/>
     </row>
@@ -10962,11 +10989,11 @@
       <c r="C37" s="144" t="s">
         <v>668</v>
       </c>
-      <c r="D37" s="225" t="s">
+      <c r="D37" s="235" t="s">
         <v>666</v>
       </c>
-      <c r="E37" s="226"/>
-      <c r="F37" s="227"/>
+      <c r="E37" s="236"/>
+      <c r="F37" s="237"/>
       <c r="G37" s="25"/>
       <c r="H37" s="26"/>
     </row>
@@ -10976,11 +11003,11 @@
       <c r="C38" s="144" t="s">
         <v>667</v>
       </c>
-      <c r="D38" s="225" t="s">
+      <c r="D38" s="235" t="s">
         <v>669</v>
       </c>
-      <c r="E38" s="226"/>
-      <c r="F38" s="227"/>
+      <c r="E38" s="236"/>
+      <c r="F38" s="237"/>
       <c r="G38" s="25"/>
       <c r="H38" s="26"/>
     </row>
@@ -10988,9 +11015,9 @@
       <c r="A39" s="24"/>
       <c r="B39" s="146"/>
       <c r="C39" s="144"/>
-      <c r="D39" s="225"/>
-      <c r="E39" s="226"/>
-      <c r="F39" s="227"/>
+      <c r="D39" s="235"/>
+      <c r="E39" s="236"/>
+      <c r="F39" s="237"/>
       <c r="G39" s="25"/>
       <c r="H39" s="26"/>
     </row>
@@ -11088,6 +11115,13 @@
     <row r="52" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:H3"/>
@@ -11097,13 +11131,6 @@
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12193,40 +12220,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="269" t="s">
+      <c r="A1" s="252" t="s">
         <v>333</v>
       </c>
-      <c r="B1" s="269"/>
-      <c r="C1" s="269"/>
-      <c r="D1" s="269"/>
-      <c r="E1" s="269"/>
-      <c r="F1" s="269"/>
-      <c r="G1" s="269"/>
-      <c r="H1" s="269"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="252"/>
+      <c r="E1" s="252"/>
+      <c r="F1" s="252"/>
+      <c r="G1" s="252"/>
+      <c r="H1" s="252"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="270"/>
-      <c r="B2" s="270"/>
-      <c r="C2" s="270"/>
-      <c r="D2" s="270"/>
-      <c r="E2" s="270"/>
-      <c r="F2" s="270"/>
-      <c r="G2" s="270"/>
-      <c r="H2" s="270"/>
+      <c r="A2" s="253"/>
+      <c r="B2" s="253"/>
+      <c r="C2" s="253"/>
+      <c r="D2" s="253"/>
+      <c r="E2" s="253"/>
+      <c r="F2" s="253"/>
+      <c r="G2" s="253"/>
+      <c r="H2" s="253"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="271" t="s">
+      <c r="A3" s="254" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="272"/>
-      <c r="C3" s="273"/>
-      <c r="D3" s="274"/>
-      <c r="E3" s="271" t="s">
+      <c r="B3" s="255"/>
+      <c r="C3" s="256"/>
+      <c r="D3" s="257"/>
+      <c r="E3" s="254" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="272"/>
-      <c r="G3" s="273"/>
-      <c r="H3" s="274"/>
+      <c r="F3" s="255"/>
+      <c r="G3" s="256"/>
+      <c r="H3" s="257"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="46">
@@ -12519,18 +12546,18 @@
       <c r="H24" s="74"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="271" t="s">
+      <c r="A25" s="254" t="s">
         <v>293</v>
       </c>
-      <c r="B25" s="272"/>
-      <c r="C25" s="273"/>
-      <c r="D25" s="274"/>
-      <c r="E25" s="271" t="s">
+      <c r="B25" s="255"/>
+      <c r="C25" s="256"/>
+      <c r="D25" s="257"/>
+      <c r="E25" s="254" t="s">
         <v>294</v>
       </c>
-      <c r="F25" s="272"/>
-      <c r="G25" s="273"/>
-      <c r="H25" s="274"/>
+      <c r="F25" s="255"/>
+      <c r="G25" s="256"/>
+      <c r="H25" s="257"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="50" t="s">
@@ -12542,23 +12569,23 @@
       <c r="E26" s="46" t="s">
         <v>296</v>
       </c>
-      <c r="F26" s="266"/>
-      <c r="G26" s="267"/>
-      <c r="H26" s="268"/>
+      <c r="F26" s="261"/>
+      <c r="G26" s="262"/>
+      <c r="H26" s="263"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="B27" s="261"/>
-      <c r="C27" s="262"/>
-      <c r="D27" s="264"/>
+      <c r="B27" s="264"/>
+      <c r="C27" s="265"/>
+      <c r="D27" s="266"/>
       <c r="E27" s="50" t="s">
         <v>298</v>
       </c>
       <c r="F27" s="258"/>
       <c r="G27" s="259"/>
-      <c r="H27" s="265"/>
+      <c r="H27" s="267"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="50" t="s">
@@ -12570,23 +12597,23 @@
       <c r="E28" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="F28" s="261"/>
-      <c r="G28" s="262"/>
-      <c r="H28" s="263"/>
+      <c r="F28" s="264"/>
+      <c r="G28" s="265"/>
+      <c r="H28" s="268"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="58" t="s">
         <v>301</v>
       </c>
-      <c r="B29" s="261"/>
-      <c r="C29" s="262"/>
-      <c r="D29" s="264"/>
+      <c r="B29" s="264"/>
+      <c r="C29" s="265"/>
+      <c r="D29" s="266"/>
       <c r="E29" s="50" t="s">
         <v>302</v>
       </c>
       <c r="F29" s="258"/>
       <c r="G29" s="259"/>
-      <c r="H29" s="265"/>
+      <c r="H29" s="267"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="50" t="s">
@@ -12598,23 +12625,23 @@
       <c r="E30" s="58" t="s">
         <v>304</v>
       </c>
-      <c r="F30" s="261"/>
-      <c r="G30" s="262"/>
-      <c r="H30" s="263"/>
+      <c r="F30" s="264"/>
+      <c r="G30" s="265"/>
+      <c r="H30" s="268"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="B31" s="261"/>
-      <c r="C31" s="262"/>
-      <c r="D31" s="264"/>
+      <c r="B31" s="264"/>
+      <c r="C31" s="265"/>
+      <c r="D31" s="266"/>
       <c r="E31" s="50" t="s">
         <v>306</v>
       </c>
       <c r="F31" s="258"/>
       <c r="G31" s="259"/>
-      <c r="H31" s="265"/>
+      <c r="H31" s="267"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="50" t="s">
@@ -12624,9 +12651,9 @@
       <c r="C32" s="259"/>
       <c r="D32" s="260"/>
       <c r="E32" s="58"/>
-      <c r="F32" s="261"/>
-      <c r="G32" s="262"/>
-      <c r="H32" s="263" t="s">
+      <c r="F32" s="264"/>
+      <c r="G32" s="265"/>
+      <c r="H32" s="268" t="s">
         <v>245</v>
       </c>
     </row>
@@ -12634,13 +12661,13 @@
       <c r="A33" s="58" t="s">
         <v>308</v>
       </c>
-      <c r="B33" s="261"/>
-      <c r="C33" s="262"/>
-      <c r="D33" s="264"/>
+      <c r="B33" s="264"/>
+      <c r="C33" s="265"/>
+      <c r="D33" s="266"/>
       <c r="E33" s="50"/>
       <c r="F33" s="258"/>
       <c r="G33" s="259"/>
-      <c r="H33" s="265" t="s">
+      <c r="H33" s="267" t="s">
         <v>288</v>
       </c>
     </row>
@@ -12652,9 +12679,9 @@
       <c r="C34" s="259"/>
       <c r="D34" s="260"/>
       <c r="E34" s="58"/>
-      <c r="F34" s="261"/>
-      <c r="G34" s="262"/>
-      <c r="H34" s="263" t="s">
+      <c r="F34" s="264"/>
+      <c r="G34" s="265"/>
+      <c r="H34" s="268" t="s">
         <v>289</v>
       </c>
     </row>
@@ -12662,13 +12689,13 @@
       <c r="A35" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="B35" s="261"/>
-      <c r="C35" s="262"/>
-      <c r="D35" s="264"/>
+      <c r="B35" s="264"/>
+      <c r="C35" s="265"/>
+      <c r="D35" s="266"/>
       <c r="E35" s="50"/>
       <c r="F35" s="258"/>
       <c r="G35" s="259"/>
-      <c r="H35" s="265" t="s">
+      <c r="H35" s="267" t="s">
         <v>290</v>
       </c>
     </row>
@@ -12680,9 +12707,9 @@
       <c r="C36" s="259"/>
       <c r="D36" s="260"/>
       <c r="E36" s="58"/>
-      <c r="F36" s="261"/>
-      <c r="G36" s="262"/>
-      <c r="H36" s="263" t="s">
+      <c r="F36" s="264"/>
+      <c r="G36" s="265"/>
+      <c r="H36" s="268" t="s">
         <v>291</v>
       </c>
     </row>
@@ -12690,13 +12717,13 @@
       <c r="A37" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="B37" s="261"/>
-      <c r="C37" s="262"/>
-      <c r="D37" s="264"/>
+      <c r="B37" s="264"/>
+      <c r="C37" s="265"/>
+      <c r="D37" s="266"/>
       <c r="E37" s="50"/>
       <c r="F37" s="258"/>
       <c r="G37" s="259"/>
-      <c r="H37" s="265" t="s">
+      <c r="H37" s="267" t="s">
         <v>292</v>
       </c>
     </row>
@@ -12708,9 +12735,9 @@
       <c r="C38" s="259"/>
       <c r="D38" s="260"/>
       <c r="E38" s="58"/>
-      <c r="F38" s="261"/>
-      <c r="G38" s="262"/>
-      <c r="H38" s="263" t="s">
+      <c r="F38" s="264"/>
+      <c r="G38" s="265"/>
+      <c r="H38" s="268" t="s">
         <v>244</v>
       </c>
     </row>
@@ -12718,13 +12745,13 @@
       <c r="A39" s="58" t="s">
         <v>314</v>
       </c>
-      <c r="B39" s="261"/>
-      <c r="C39" s="262"/>
-      <c r="D39" s="264"/>
+      <c r="B39" s="264"/>
+      <c r="C39" s="265"/>
+      <c r="D39" s="266"/>
       <c r="E39" s="50"/>
       <c r="F39" s="258"/>
       <c r="G39" s="259"/>
-      <c r="H39" s="265" t="s">
+      <c r="H39" s="267" t="s">
         <v>245</v>
       </c>
     </row>
@@ -12736,53 +12763,24 @@
       <c r="C40" s="259"/>
       <c r="D40" s="260"/>
       <c r="E40" s="58"/>
-      <c r="F40" s="261"/>
-      <c r="G40" s="262"/>
-      <c r="H40" s="263"/>
+      <c r="F40" s="264"/>
+      <c r="G40" s="265"/>
+      <c r="H40" s="268"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="70" t="s">
         <v>316</v>
       </c>
-      <c r="B41" s="252"/>
-      <c r="C41" s="253"/>
-      <c r="D41" s="254"/>
+      <c r="B41" s="269"/>
+      <c r="C41" s="270"/>
+      <c r="D41" s="271"/>
       <c r="E41" s="75"/>
-      <c r="F41" s="255"/>
-      <c r="G41" s="256"/>
-      <c r="H41" s="257"/>
+      <c r="F41" s="272"/>
+      <c r="G41" s="273"/>
+      <c r="H41" s="274"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -12791,6 +12789,35 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -13357,40 +13384,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="229" t="s">
+      <c r="A1" s="225" t="s">
         <v>495</v>
       </c>
-      <c r="B1" s="230"/>
-      <c r="C1" s="230"/>
-      <c r="D1" s="230"/>
-      <c r="E1" s="230"/>
-      <c r="F1" s="230"/>
-      <c r="G1" s="230"/>
-      <c r="H1" s="231"/>
+      <c r="B1" s="226"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="226"/>
+      <c r="H1" s="227"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="232"/>
-      <c r="B2" s="233"/>
-      <c r="C2" s="233"/>
-      <c r="D2" s="233"/>
-      <c r="E2" s="233"/>
-      <c r="F2" s="233"/>
-      <c r="G2" s="233"/>
-      <c r="H2" s="234"/>
+      <c r="A2" s="228"/>
+      <c r="B2" s="229"/>
+      <c r="C2" s="229"/>
+      <c r="D2" s="229"/>
+      <c r="E2" s="229"/>
+      <c r="F2" s="229"/>
+      <c r="G2" s="229"/>
+      <c r="H2" s="230"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="235" t="s">
+      <c r="A3" s="231" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="236"/>
-      <c r="C3" s="236"/>
-      <c r="D3" s="236"/>
-      <c r="E3" s="236" t="s">
+      <c r="B3" s="232"/>
+      <c r="C3" s="232"/>
+      <c r="D3" s="232"/>
+      <c r="E3" s="232" t="s">
         <v>322</v>
       </c>
-      <c r="F3" s="236"/>
-      <c r="G3" s="236"/>
-      <c r="H3" s="237"/>
+      <c r="F3" s="232"/>
+      <c r="G3" s="232"/>
+      <c r="H3" s="233"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="20">

</xml_diff>

<commit_message>
chg: Added range 34 freq to SPINS
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="2340" yWindow="600" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="856">
   <si>
     <t>AWACS</t>
   </si>
@@ -2582,6 +2582,15 @@
   </si>
   <si>
     <t>Apache</t>
+  </si>
+  <si>
+    <t>Range 34</t>
+  </si>
+  <si>
+    <t>BRONZE 12</t>
+  </si>
+  <si>
+    <t>COPPER 4</t>
   </si>
 </sst>
 </file>
@@ -4796,10 +4805,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Ark1"/>
-  <dimension ref="A1:AP53"/>
+  <dimension ref="A1:AP54"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AJ41" sqref="AJ41"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4:AH27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -5209,7 +5218,7 @@
       <c r="J6" s="130"/>
       <c r="K6" s="130"/>
       <c r="L6" s="130"/>
-      <c r="M6" s="130" t="s">
+      <c r="M6" s="127" t="s">
         <v>378</v>
       </c>
       <c r="N6" s="129" t="s">
@@ -5442,7 +5451,7 @@
         <v>383</v>
       </c>
       <c r="D9" s="130"/>
-      <c r="E9" s="130" t="s">
+      <c r="E9" s="127" t="s">
         <v>384</v>
       </c>
       <c r="F9" s="131" t="s">
@@ -6667,6 +6676,21 @@
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
       <c r="T23" s="12"/>
+      <c r="AD23" s="10" t="s">
+        <v>853</v>
+      </c>
+      <c r="AE23" s="127" t="s">
+        <v>378</v>
+      </c>
+      <c r="AF23" s="10" t="s">
+        <v>854</v>
+      </c>
+      <c r="AG23" s="127" t="s">
+        <v>384</v>
+      </c>
+      <c r="AH23" s="10" t="s">
+        <v>855</v>
+      </c>
       <c r="AJ23" s="142" t="s">
         <v>565</v>
       </c>
@@ -6737,13 +6761,6 @@
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
-      <c r="AD24" s="205" t="s">
-        <v>493</v>
-      </c>
-      <c r="AE24" s="205"/>
-      <c r="AF24" s="205"/>
-      <c r="AG24" s="205"/>
-      <c r="AH24" s="205"/>
       <c r="AJ24" s="142" t="s">
         <v>568</v>
       </c>
@@ -6820,21 +6837,13 @@
       <c r="Z25" s="12"/>
       <c r="AA25" s="12"/>
       <c r="AB25" s="12"/>
-      <c r="AD25" s="115" t="s">
-        <v>218</v>
-      </c>
-      <c r="AE25" s="115" t="s">
-        <v>216</v>
-      </c>
-      <c r="AF25" s="115" t="s">
-        <v>227</v>
-      </c>
-      <c r="AG25" s="115" t="s">
-        <v>217</v>
-      </c>
-      <c r="AH25" s="115" t="s">
-        <v>227</v>
-      </c>
+      <c r="AD25" s="205" t="s">
+        <v>493</v>
+      </c>
+      <c r="AE25" s="205"/>
+      <c r="AF25" s="205"/>
+      <c r="AG25" s="205"/>
+      <c r="AH25" s="205"/>
     </row>
     <row r="26" spans="1:42">
       <c r="A26" s="129" t="s">
@@ -6884,20 +6893,20 @@
       <c r="Z26" s="12"/>
       <c r="AA26" s="12"/>
       <c r="AB26" s="12"/>
-      <c r="AD26" s="3" t="s">
-        <v>489</v>
-      </c>
-      <c r="AE26" s="128" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF26" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="AG26" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH26" s="3" t="s">
-        <v>492</v>
+      <c r="AD26" s="115" t="s">
+        <v>218</v>
+      </c>
+      <c r="AE26" s="115" t="s">
+        <v>216</v>
+      </c>
+      <c r="AF26" s="115" t="s">
+        <v>227</v>
+      </c>
+      <c r="AG26" s="115" t="s">
+        <v>217</v>
+      </c>
+      <c r="AH26" s="115" t="s">
+        <v>227</v>
       </c>
       <c r="AJ26" s="205" t="s">
         <v>847</v>
@@ -6964,6 +6973,21 @@
       <c r="Z27" s="12"/>
       <c r="AA27" s="12"/>
       <c r="AB27" s="12"/>
+      <c r="AD27" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="AE27" s="128" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF27" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="AG27" s="128" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH27" s="3" t="s">
+        <v>492</v>
+      </c>
       <c r="AJ27" s="204" t="s">
         <v>218</v>
       </c>
@@ -7202,11 +7226,6 @@
       <c r="Y31" s="37"/>
       <c r="Z31" s="37"/>
       <c r="AA31" s="12"/>
-      <c r="AD31" s="206" t="s">
-        <v>263</v>
-      </c>
-      <c r="AE31" s="207"/>
-      <c r="AF31" s="208"/>
     </row>
     <row r="32" spans="1:42">
       <c r="S32" s="12"/>
@@ -7218,15 +7237,6 @@
       <c r="Y32" s="117"/>
       <c r="Z32" s="117"/>
       <c r="AA32" s="12"/>
-      <c r="AD32" s="44" t="s">
-        <v>218</v>
-      </c>
-      <c r="AE32" s="44" t="s">
-        <v>224</v>
-      </c>
-      <c r="AF32" s="44" t="s">
-        <v>227</v>
-      </c>
     </row>
     <row r="33" spans="19:37">
       <c r="S33" s="12"/>
@@ -7238,11 +7248,6 @@
       <c r="Y33" s="12"/>
       <c r="Z33" s="12"/>
       <c r="AA33" s="12"/>
-      <c r="AD33" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="AE33" s="10"/>
-      <c r="AF33" s="10"/>
     </row>
     <row r="34" spans="19:37">
       <c r="S34" s="12"/>
@@ -7254,11 +7259,6 @@
       <c r="Y34" s="12"/>
       <c r="Z34" s="12"/>
       <c r="AA34" s="12"/>
-      <c r="AD34" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="AE34" s="10"/>
-      <c r="AF34" s="10"/>
       <c r="AG34" s="116"/>
       <c r="AH34" s="116"/>
       <c r="AI34" s="116"/>
@@ -7275,11 +7275,6 @@
       <c r="Y35" s="12"/>
       <c r="Z35" s="12"/>
       <c r="AA35" s="12"/>
-      <c r="AD35" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="AE35" s="11"/>
-      <c r="AF35" s="10"/>
       <c r="AG35" s="12"/>
       <c r="AH35" s="12"/>
       <c r="AI35" s="12"/>
@@ -7296,11 +7291,6 @@
       <c r="Y36" s="12"/>
       <c r="Z36" s="12"/>
       <c r="AA36" s="12"/>
-      <c r="AD36" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="AE36" s="10"/>
-      <c r="AF36" s="10"/>
       <c r="AG36" s="12"/>
       <c r="AH36" s="12"/>
       <c r="AI36" s="12"/>
@@ -7320,11 +7310,6 @@
       <c r="Z37" s="205"/>
       <c r="AA37" s="205"/>
       <c r="AB37" s="205"/>
-      <c r="AD37" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="AE37" s="10"/>
-      <c r="AF37" s="10"/>
       <c r="AG37" s="12"/>
       <c r="AH37" s="12"/>
       <c r="AI37" s="12"/>
@@ -7352,11 +7337,11 @@
       </c>
       <c r="AA38" s="114"/>
       <c r="AB38" s="114"/>
-      <c r="AD38" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="AE38" s="11"/>
-      <c r="AF38" s="10"/>
+      <c r="AD38" s="206" t="s">
+        <v>263</v>
+      </c>
+      <c r="AE38" s="207"/>
+      <c r="AF38" s="208"/>
       <c r="AG38" s="12"/>
       <c r="AH38" s="12"/>
       <c r="AI38" s="12"/>
@@ -7376,11 +7361,15 @@
       <c r="Z39" s="10"/>
       <c r="AA39" s="10"/>
       <c r="AB39" s="3"/>
-      <c r="AD39" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="AE39" s="11"/>
-      <c r="AF39" s="10"/>
+      <c r="AD39" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="AE39" s="44" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF39" s="44" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="40" spans="19:37">
       <c r="S40" s="12"/>
@@ -7393,9 +7382,9 @@
       <c r="Z40" s="12"/>
       <c r="AA40" s="12"/>
       <c r="AD40" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="AE40" s="11"/>
+        <v>255</v>
+      </c>
+      <c r="AE40" s="10"/>
       <c r="AF40" s="10"/>
     </row>
     <row r="41" spans="19:37">
@@ -7409,7 +7398,7 @@
       <c r="Z41" s="12"/>
       <c r="AA41" s="12"/>
       <c r="AD41" s="3" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="AE41" s="10"/>
       <c r="AF41" s="10"/>
@@ -7428,9 +7417,9 @@
       <c r="AA42" s="205"/>
       <c r="AB42" s="205"/>
       <c r="AD42" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="AE42" s="10"/>
+        <v>257</v>
+      </c>
+      <c r="AE42" s="11"/>
       <c r="AF42" s="10"/>
     </row>
     <row r="43" spans="19:37">
@@ -7457,7 +7446,7 @@
       </c>
       <c r="AB43" s="115"/>
       <c r="AD43" s="3" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="AE43" s="10"/>
       <c r="AF43" s="10"/>
@@ -7473,8 +7462,8 @@
       <c r="Z44" s="10"/>
       <c r="AA44" s="10"/>
       <c r="AB44" s="3"/>
-      <c r="AD44" s="10" t="s">
-        <v>267</v>
+      <c r="AD44" s="3" t="s">
+        <v>259</v>
       </c>
       <c r="AE44" s="10"/>
       <c r="AF44" s="10"/>
@@ -7489,8 +7478,8 @@
       <c r="Y45" s="12"/>
       <c r="Z45" s="12"/>
       <c r="AA45" s="12"/>
-      <c r="AD45" s="10" t="s">
-        <v>268</v>
+      <c r="AD45" s="3" t="s">
+        <v>260</v>
       </c>
       <c r="AE45" s="11"/>
       <c r="AF45" s="10"/>
@@ -7505,8 +7494,8 @@
       <c r="Y46" s="12"/>
       <c r="Z46" s="117"/>
       <c r="AA46" s="12"/>
-      <c r="AD46" s="10" t="s">
-        <v>269</v>
+      <c r="AD46" s="3" t="s">
+        <v>261</v>
       </c>
       <c r="AE46" s="11"/>
       <c r="AF46" s="10"/>
@@ -7521,10 +7510,10 @@
       <c r="Y47" s="12"/>
       <c r="Z47" s="12"/>
       <c r="AA47" s="12"/>
-      <c r="AD47" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="AE47" s="10"/>
+      <c r="AD47" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE47" s="11"/>
       <c r="AF47" s="10"/>
     </row>
     <row r="48" spans="19:37">
@@ -7540,8 +7529,13 @@
       <c r="Z48" s="207"/>
       <c r="AA48" s="207"/>
       <c r="AB48" s="208"/>
-    </row>
-    <row r="49" spans="19:28">
+      <c r="AD48" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="AE48" s="10"/>
+      <c r="AF48" s="10"/>
+    </row>
+    <row r="49" spans="19:32">
       <c r="S49" s="12"/>
       <c r="T49" s="12"/>
       <c r="U49" s="12"/>
@@ -7562,8 +7556,13 @@
         <v>220</v>
       </c>
       <c r="AB49" s="115"/>
-    </row>
-    <row r="50" spans="19:28">
+      <c r="AD49" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="AE49" s="10"/>
+      <c r="AF49" s="10"/>
+    </row>
+    <row r="50" spans="19:32">
       <c r="S50" s="12"/>
       <c r="T50" s="12"/>
       <c r="U50" s="12"/>
@@ -7581,8 +7580,13 @@
       <c r="AA50" s="12" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="51" spans="19:28">
+      <c r="AD50" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="AE50" s="10"/>
+      <c r="AF50" s="10"/>
+    </row>
+    <row r="51" spans="19:32">
       <c r="S51" s="12"/>
       <c r="T51" s="12"/>
       <c r="U51" s="12"/>
@@ -7598,8 +7602,13 @@
       <c r="Y51" s="12"/>
       <c r="Z51" s="12"/>
       <c r="AA51" s="12"/>
-    </row>
-    <row r="52" spans="19:28">
+      <c r="AD51" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="AE51" s="10"/>
+      <c r="AF51" s="10"/>
+    </row>
+    <row r="52" spans="19:32">
       <c r="S52" s="12"/>
       <c r="T52" s="12"/>
       <c r="U52" s="12"/>
@@ -7615,8 +7624,13 @@
       <c r="Y52" s="12"/>
       <c r="Z52" s="12"/>
       <c r="AA52" s="12"/>
-    </row>
-    <row r="53" spans="19:28">
+      <c r="AD52" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="AE52" s="11"/>
+      <c r="AF52" s="10"/>
+    </row>
+    <row r="53" spans="19:32">
       <c r="S53" s="12"/>
       <c r="T53" s="12"/>
       <c r="U53" s="12"/>
@@ -7626,6 +7640,18 @@
       <c r="Y53" s="12"/>
       <c r="Z53" s="12"/>
       <c r="AA53" s="12"/>
+      <c r="AD53" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE53" s="11"/>
+      <c r="AF53" s="10"/>
+    </row>
+    <row r="54" spans="19:32">
+      <c r="AD54" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="AE54" s="10"/>
+      <c r="AF54" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -7633,9 +7659,9 @@
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="AJ4:AP4"/>
     <mergeCell ref="AJ17:AP17"/>
-    <mergeCell ref="AD31:AF31"/>
+    <mergeCell ref="AD38:AF38"/>
     <mergeCell ref="V29:AB29"/>
-    <mergeCell ref="AD24:AH24"/>
+    <mergeCell ref="AD25:AH25"/>
     <mergeCell ref="AJ26:AP26"/>
     <mergeCell ref="V42:AB42"/>
     <mergeCell ref="AD4:AH4"/>
@@ -8583,7 +8609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AJ45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="AB18" sqref="AB18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
chg: Added Strike+OCA Escort tasking for range 23
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="1240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2057" uniqueCount="1243">
   <si>
     <t>AWACS</t>
   </si>
@@ -3744,6 +3744,15 @@
   </si>
   <si>
     <t>281.77</t>
+  </si>
+  <si>
+    <t>Tactical freq 1</t>
+  </si>
+  <si>
+    <t>Tactical freq 2</t>
+  </si>
+  <si>
+    <t>MAROON 10</t>
   </si>
 </sst>
 </file>
@@ -4227,7 +4236,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="89">
+  <borders count="90">
     <border>
       <left/>
       <right/>
@@ -5395,11 +5404,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="421">
+  <cellXfs count="422">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6112,12 +6132,22 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6127,13 +6157,49 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6145,50 +6211,35 @@
     <xf numFmtId="0" fontId="26" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6199,36 +6250,6 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6289,6 +6310,42 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="26" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="26" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="26" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6307,42 +6364,6 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="23" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="26" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="26" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="26" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6415,6 +6436,57 @@
     <xf numFmtId="0" fontId="33" fillId="20" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6433,58 +6505,7 @@
     <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6797,8 +6818,8 @@
   <sheetPr codeName="Ark1"/>
   <dimension ref="A1:AP83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -6975,9 +6996,9 @@
         <v>429</v>
       </c>
       <c r="Q3" s="11"/>
-      <c r="R3" s="296"/>
-      <c r="S3" s="296"/>
-      <c r="T3" s="296"/>
+      <c r="R3" s="301"/>
+      <c r="S3" s="301"/>
+      <c r="T3" s="301"/>
       <c r="V3" s="119" t="s">
         <v>331</v>
       </c>
@@ -7681,18 +7702,14 @@
       <c r="R11" s="116"/>
       <c r="S11" s="117"/>
       <c r="T11" s="2"/>
-      <c r="V11" s="113"/>
-      <c r="W11" s="113" t="s">
-        <v>223</v>
-      </c>
-      <c r="X11" s="113" t="s">
-        <v>226</v>
-      </c>
-      <c r="Y11" s="113" t="s">
-        <v>282</v>
-      </c>
-      <c r="Z11" s="113" t="s">
-        <v>285</v>
+      <c r="V11" s="421" t="s">
+        <v>1240</v>
+      </c>
+      <c r="W11" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="X11" s="421" t="s">
+        <v>1242</v>
       </c>
       <c r="AA11" s="36"/>
       <c r="AB11" s="35"/>
@@ -7781,18 +7798,8 @@
       <c r="R12" s="116"/>
       <c r="S12" s="117"/>
       <c r="T12" s="11"/>
-      <c r="V12" s="420" t="s">
-        <v>283</v>
-      </c>
-      <c r="W12" s="9" t="s">
-        <v>1238</v>
-      </c>
-      <c r="X12" s="3"/>
-      <c r="Y12" s="9" t="s">
-        <v>1236</v>
-      </c>
-      <c r="Z12" s="9">
-        <v>602</v>
+      <c r="V12" s="421" t="s">
+        <v>1241</v>
       </c>
       <c r="AA12" s="35"/>
       <c r="AD12" s="3" t="s">
@@ -7883,13 +7890,19 @@
       <c r="R13" s="116"/>
       <c r="S13" s="117"/>
       <c r="T13" s="11"/>
-      <c r="V13" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="W13" s="9"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="9"/>
+      <c r="V13" s="113"/>
+      <c r="W13" s="113" t="s">
+        <v>223</v>
+      </c>
+      <c r="X13" s="113" t="s">
+        <v>226</v>
+      </c>
+      <c r="Y13" s="113" t="s">
+        <v>282</v>
+      </c>
+      <c r="Z13" s="113" t="s">
+        <v>285</v>
+      </c>
       <c r="AA13" s="11"/>
       <c r="AD13" s="3" t="s">
         <v>439</v>
@@ -7979,13 +7992,19 @@
       <c r="R14" s="118"/>
       <c r="S14" s="117"/>
       <c r="T14" s="11"/>
-      <c r="V14" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="W14" s="3"/>
+      <c r="V14" s="296" t="s">
+        <v>283</v>
+      </c>
+      <c r="W14" s="9" t="s">
+        <v>1238</v>
+      </c>
       <c r="X14" s="3"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="9"/>
+      <c r="Y14" s="9" t="s">
+        <v>1236</v>
+      </c>
+      <c r="Z14" s="9">
+        <v>602</v>
+      </c>
       <c r="AA14" s="11"/>
       <c r="AD14" s="43"/>
       <c r="AE14" s="43"/>
@@ -8063,19 +8082,13 @@
       <c r="R15" s="118"/>
       <c r="S15" s="117"/>
       <c r="T15" s="11"/>
-      <c r="V15" s="420" t="s">
-        <v>1235</v>
-      </c>
-      <c r="W15" s="9" t="s">
-        <v>1239</v>
-      </c>
+      <c r="V15" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="W15" s="9"/>
       <c r="X15" s="3"/>
-      <c r="Y15" s="9" t="s">
-        <v>1237</v>
-      </c>
-      <c r="Z15" s="9">
-        <v>601</v>
-      </c>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
       <c r="AA15" s="11"/>
       <c r="AD15" s="3" t="s">
         <v>440</v>
@@ -8142,6 +8155,13 @@
       <c r="R16" s="118"/>
       <c r="S16" s="117"/>
       <c r="T16" s="11"/>
+      <c r="V16" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
       <c r="AD16" s="3" t="s">
         <v>441</v>
       </c>
@@ -8207,6 +8227,19 @@
       <c r="R17" s="11"/>
       <c r="S17" s="117"/>
       <c r="T17" s="11"/>
+      <c r="V17" s="296" t="s">
+        <v>1235</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>1239</v>
+      </c>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="9" t="s">
+        <v>1237</v>
+      </c>
+      <c r="Z17" s="9">
+        <v>601</v>
+      </c>
       <c r="AD17" s="9" t="s">
         <v>442</v>
       </c>
@@ -8254,7 +8287,7 @@
       <c r="J18" s="127" t="s">
         <v>405</v>
       </c>
-      <c r="K18" s="127" t="s">
+      <c r="K18" s="13" t="s">
         <v>188</v>
       </c>
       <c r="L18" s="13" t="s">
@@ -8426,9 +8459,9 @@
       <c r="O20" s="34"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="296"/>
-      <c r="S20" s="296"/>
-      <c r="T20" s="296"/>
+      <c r="R20" s="301"/>
+      <c r="S20" s="301"/>
+      <c r="T20" s="301"/>
       <c r="U20" s="2"/>
       <c r="V20" s="11"/>
       <c r="W20" s="11"/>
@@ -9401,11 +9434,11 @@
       </c>
       <c r="AA38" s="112"/>
       <c r="AB38" s="112"/>
-      <c r="AD38" s="298" t="s">
+      <c r="AD38" s="302" t="s">
         <v>261</v>
       </c>
-      <c r="AE38" s="299"/>
-      <c r="AF38" s="300"/>
+      <c r="AE38" s="303"/>
+      <c r="AF38" s="304"/>
       <c r="AG38" s="11"/>
       <c r="AH38" s="11"/>
       <c r="AI38" s="11"/>
@@ -9584,15 +9617,15 @@
       <c r="S48" s="11"/>
       <c r="T48" s="11"/>
       <c r="U48" s="11"/>
-      <c r="V48" s="301" t="s">
+      <c r="V48" s="298" t="s">
         <v>476</v>
       </c>
-      <c r="W48" s="302"/>
-      <c r="X48" s="302"/>
-      <c r="Y48" s="302"/>
-      <c r="Z48" s="302"/>
-      <c r="AA48" s="302"/>
-      <c r="AB48" s="303"/>
+      <c r="W48" s="299"/>
+      <c r="X48" s="299"/>
+      <c r="Y48" s="299"/>
+      <c r="Z48" s="299"/>
+      <c r="AA48" s="299"/>
+      <c r="AB48" s="300"/>
       <c r="AD48" s="3" t="s">
         <v>262</v>
       </c>
@@ -10217,11 +10250,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="V42:AB42"/>
-    <mergeCell ref="AD4:AH4"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="V48:AB48"/>
-    <mergeCell ref="V37:AB37"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="AJ4:AP4"/>
@@ -10230,6 +10258,11 @@
     <mergeCell ref="V29:AB29"/>
     <mergeCell ref="AD25:AH25"/>
     <mergeCell ref="AJ30:AP30"/>
+    <mergeCell ref="V42:AB42"/>
+    <mergeCell ref="AD4:AH4"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="V48:AB48"/>
+    <mergeCell ref="V37:AB37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10257,40 +10290,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="385" t="s">
+      <c r="A1" s="386" t="s">
         <v>490</v>
       </c>
-      <c r="B1" s="386"/>
-      <c r="C1" s="386"/>
-      <c r="D1" s="386"/>
-      <c r="E1" s="386"/>
-      <c r="F1" s="386"/>
-      <c r="G1" s="386"/>
-      <c r="H1" s="387"/>
+      <c r="B1" s="387"/>
+      <c r="C1" s="387"/>
+      <c r="D1" s="387"/>
+      <c r="E1" s="387"/>
+      <c r="F1" s="387"/>
+      <c r="G1" s="387"/>
+      <c r="H1" s="388"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="388"/>
-      <c r="B2" s="389"/>
-      <c r="C2" s="389"/>
-      <c r="D2" s="389"/>
-      <c r="E2" s="389"/>
-      <c r="F2" s="389"/>
-      <c r="G2" s="389"/>
-      <c r="H2" s="390"/>
+      <c r="A2" s="389"/>
+      <c r="B2" s="390"/>
+      <c r="C2" s="390"/>
+      <c r="D2" s="390"/>
+      <c r="E2" s="390"/>
+      <c r="F2" s="390"/>
+      <c r="G2" s="390"/>
+      <c r="H2" s="391"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="391" t="s">
+      <c r="A3" s="392" t="s">
         <v>754</v>
       </c>
-      <c r="B3" s="392"/>
-      <c r="C3" s="392"/>
-      <c r="D3" s="393"/>
-      <c r="E3" s="391" t="s">
+      <c r="B3" s="393"/>
+      <c r="C3" s="393"/>
+      <c r="D3" s="394"/>
+      <c r="E3" s="392" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="392"/>
-      <c r="G3" s="392"/>
-      <c r="H3" s="393"/>
+      <c r="F3" s="393"/>
+      <c r="G3" s="393"/>
+      <c r="H3" s="394"/>
     </row>
     <row r="4" spans="1:8" ht="16.5">
       <c r="A4" s="189">
@@ -10763,18 +10796,18 @@
       <c r="H24" s="169"/>
     </row>
     <row r="25" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A25" s="394" t="s">
+      <c r="A25" s="395" t="s">
         <v>316</v>
       </c>
-      <c r="B25" s="395"/>
-      <c r="C25" s="395"/>
-      <c r="D25" s="396"/>
-      <c r="E25" s="394" t="s">
+      <c r="B25" s="396"/>
+      <c r="C25" s="396"/>
+      <c r="D25" s="397"/>
+      <c r="E25" s="395" t="s">
         <v>804</v>
       </c>
-      <c r="F25" s="395"/>
-      <c r="G25" s="395"/>
-      <c r="H25" s="396"/>
+      <c r="F25" s="396"/>
+      <c r="G25" s="396"/>
+      <c r="H25" s="397"/>
     </row>
     <row r="26" spans="1:8" ht="16.5">
       <c r="A26" s="178">
@@ -11189,40 +11222,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="414" t="s">
+      <c r="A1" s="398" t="s">
         <v>329</v>
       </c>
-      <c r="B1" s="414"/>
-      <c r="C1" s="414"/>
-      <c r="D1" s="414"/>
-      <c r="E1" s="414"/>
-      <c r="F1" s="414"/>
-      <c r="G1" s="414"/>
-      <c r="H1" s="414"/>
+      <c r="B1" s="398"/>
+      <c r="C1" s="398"/>
+      <c r="D1" s="398"/>
+      <c r="E1" s="398"/>
+      <c r="F1" s="398"/>
+      <c r="G1" s="398"/>
+      <c r="H1" s="398"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="415"/>
-      <c r="B2" s="415"/>
-      <c r="C2" s="415"/>
-      <c r="D2" s="415"/>
-      <c r="E2" s="415"/>
-      <c r="F2" s="415"/>
-      <c r="G2" s="415"/>
-      <c r="H2" s="415"/>
+      <c r="A2" s="399"/>
+      <c r="B2" s="399"/>
+      <c r="C2" s="399"/>
+      <c r="D2" s="399"/>
+      <c r="E2" s="399"/>
+      <c r="F2" s="399"/>
+      <c r="G2" s="399"/>
+      <c r="H2" s="399"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="416" t="s">
+      <c r="A3" s="400" t="s">
         <v>227</v>
       </c>
-      <c r="B3" s="417"/>
-      <c r="C3" s="418"/>
-      <c r="D3" s="419"/>
-      <c r="E3" s="416" t="s">
+      <c r="B3" s="401"/>
+      <c r="C3" s="402"/>
+      <c r="D3" s="403"/>
+      <c r="E3" s="400" t="s">
         <v>228</v>
       </c>
-      <c r="F3" s="417"/>
-      <c r="G3" s="418"/>
-      <c r="H3" s="419"/>
+      <c r="F3" s="401"/>
+      <c r="G3" s="402"/>
+      <c r="H3" s="403"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="44">
@@ -11515,114 +11548,114 @@
       <c r="H24" s="72"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="416" t="s">
+      <c r="A25" s="400" t="s">
         <v>291</v>
       </c>
-      <c r="B25" s="417"/>
-      <c r="C25" s="418"/>
-      <c r="D25" s="419"/>
-      <c r="E25" s="416" t="s">
+      <c r="B25" s="401"/>
+      <c r="C25" s="402"/>
+      <c r="D25" s="403"/>
+      <c r="E25" s="400" t="s">
         <v>292</v>
       </c>
-      <c r="F25" s="417"/>
-      <c r="G25" s="418"/>
-      <c r="H25" s="419"/>
+      <c r="F25" s="401"/>
+      <c r="G25" s="402"/>
+      <c r="H25" s="403"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="B26" s="403"/>
-      <c r="C26" s="404"/>
-      <c r="D26" s="405"/>
+      <c r="B26" s="404"/>
+      <c r="C26" s="405"/>
+      <c r="D26" s="406"/>
       <c r="E26" s="44" t="s">
         <v>294</v>
       </c>
-      <c r="F26" s="411"/>
-      <c r="G26" s="412"/>
-      <c r="H26" s="413"/>
+      <c r="F26" s="407"/>
+      <c r="G26" s="408"/>
+      <c r="H26" s="409"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="56" t="s">
         <v>295</v>
       </c>
-      <c r="B27" s="406"/>
-      <c r="C27" s="407"/>
-      <c r="D27" s="409"/>
+      <c r="B27" s="410"/>
+      <c r="C27" s="411"/>
+      <c r="D27" s="412"/>
       <c r="E27" s="48" t="s">
         <v>296</v>
       </c>
-      <c r="F27" s="403"/>
-      <c r="G27" s="404"/>
-      <c r="H27" s="410"/>
+      <c r="F27" s="404"/>
+      <c r="G27" s="405"/>
+      <c r="H27" s="413"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="48" t="s">
         <v>297</v>
       </c>
-      <c r="B28" s="403"/>
-      <c r="C28" s="404"/>
-      <c r="D28" s="405"/>
+      <c r="B28" s="404"/>
+      <c r="C28" s="405"/>
+      <c r="D28" s="406"/>
       <c r="E28" s="56" t="s">
         <v>298</v>
       </c>
-      <c r="F28" s="406"/>
-      <c r="G28" s="407"/>
-      <c r="H28" s="408"/>
+      <c r="F28" s="410"/>
+      <c r="G28" s="411"/>
+      <c r="H28" s="414"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="56" t="s">
         <v>299</v>
       </c>
-      <c r="B29" s="406"/>
-      <c r="C29" s="407"/>
-      <c r="D29" s="409"/>
+      <c r="B29" s="410"/>
+      <c r="C29" s="411"/>
+      <c r="D29" s="412"/>
       <c r="E29" s="48" t="s">
         <v>300</v>
       </c>
-      <c r="F29" s="403"/>
-      <c r="G29" s="404"/>
-      <c r="H29" s="410"/>
+      <c r="F29" s="404"/>
+      <c r="G29" s="405"/>
+      <c r="H29" s="413"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="48" t="s">
         <v>301</v>
       </c>
-      <c r="B30" s="403"/>
-      <c r="C30" s="404"/>
-      <c r="D30" s="405"/>
+      <c r="B30" s="404"/>
+      <c r="C30" s="405"/>
+      <c r="D30" s="406"/>
       <c r="E30" s="56" t="s">
         <v>302</v>
       </c>
-      <c r="F30" s="406"/>
-      <c r="G30" s="407"/>
-      <c r="H30" s="408"/>
+      <c r="F30" s="410"/>
+      <c r="G30" s="411"/>
+      <c r="H30" s="414"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="56" t="s">
         <v>303</v>
       </c>
-      <c r="B31" s="406"/>
-      <c r="C31" s="407"/>
-      <c r="D31" s="409"/>
+      <c r="B31" s="410"/>
+      <c r="C31" s="411"/>
+      <c r="D31" s="412"/>
       <c r="E31" s="48" t="s">
         <v>304</v>
       </c>
-      <c r="F31" s="403"/>
-      <c r="G31" s="404"/>
-      <c r="H31" s="410"/>
+      <c r="F31" s="404"/>
+      <c r="G31" s="405"/>
+      <c r="H31" s="413"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="48" t="s">
         <v>305</v>
       </c>
-      <c r="B32" s="403"/>
-      <c r="C32" s="404"/>
-      <c r="D32" s="405"/>
+      <c r="B32" s="404"/>
+      <c r="C32" s="405"/>
+      <c r="D32" s="406"/>
       <c r="E32" s="56"/>
-      <c r="F32" s="406"/>
-      <c r="G32" s="407"/>
-      <c r="H32" s="408" t="s">
+      <c r="F32" s="410"/>
+      <c r="G32" s="411"/>
+      <c r="H32" s="414" t="s">
         <v>243</v>
       </c>
     </row>
@@ -11630,13 +11663,13 @@
       <c r="A33" s="56" t="s">
         <v>306</v>
       </c>
-      <c r="B33" s="406"/>
-      <c r="C33" s="407"/>
-      <c r="D33" s="409"/>
+      <c r="B33" s="410"/>
+      <c r="C33" s="411"/>
+      <c r="D33" s="412"/>
       <c r="E33" s="48"/>
-      <c r="F33" s="403"/>
-      <c r="G33" s="404"/>
-      <c r="H33" s="410" t="s">
+      <c r="F33" s="404"/>
+      <c r="G33" s="405"/>
+      <c r="H33" s="413" t="s">
         <v>286</v>
       </c>
     </row>
@@ -11644,13 +11677,13 @@
       <c r="A34" s="48" t="s">
         <v>307</v>
       </c>
-      <c r="B34" s="403"/>
-      <c r="C34" s="404"/>
-      <c r="D34" s="405"/>
+      <c r="B34" s="404"/>
+      <c r="C34" s="405"/>
+      <c r="D34" s="406"/>
       <c r="E34" s="56"/>
-      <c r="F34" s="406"/>
-      <c r="G34" s="407"/>
-      <c r="H34" s="408" t="s">
+      <c r="F34" s="410"/>
+      <c r="G34" s="411"/>
+      <c r="H34" s="414" t="s">
         <v>287</v>
       </c>
     </row>
@@ -11658,13 +11691,13 @@
       <c r="A35" s="56" t="s">
         <v>308</v>
       </c>
-      <c r="B35" s="406"/>
-      <c r="C35" s="407"/>
-      <c r="D35" s="409"/>
+      <c r="B35" s="410"/>
+      <c r="C35" s="411"/>
+      <c r="D35" s="412"/>
       <c r="E35" s="48"/>
-      <c r="F35" s="403"/>
-      <c r="G35" s="404"/>
-      <c r="H35" s="410" t="s">
+      <c r="F35" s="404"/>
+      <c r="G35" s="405"/>
+      <c r="H35" s="413" t="s">
         <v>288</v>
       </c>
     </row>
@@ -11672,13 +11705,13 @@
       <c r="A36" s="48" t="s">
         <v>309</v>
       </c>
-      <c r="B36" s="403"/>
-      <c r="C36" s="404"/>
-      <c r="D36" s="405"/>
+      <c r="B36" s="404"/>
+      <c r="C36" s="405"/>
+      <c r="D36" s="406"/>
       <c r="E36" s="56"/>
-      <c r="F36" s="406"/>
-      <c r="G36" s="407"/>
-      <c r="H36" s="408" t="s">
+      <c r="F36" s="410"/>
+      <c r="G36" s="411"/>
+      <c r="H36" s="414" t="s">
         <v>289</v>
       </c>
     </row>
@@ -11686,13 +11719,13 @@
       <c r="A37" s="56" t="s">
         <v>310</v>
       </c>
-      <c r="B37" s="406"/>
-      <c r="C37" s="407"/>
-      <c r="D37" s="409"/>
+      <c r="B37" s="410"/>
+      <c r="C37" s="411"/>
+      <c r="D37" s="412"/>
       <c r="E37" s="48"/>
-      <c r="F37" s="403"/>
-      <c r="G37" s="404"/>
-      <c r="H37" s="410" t="s">
+      <c r="F37" s="404"/>
+      <c r="G37" s="405"/>
+      <c r="H37" s="413" t="s">
         <v>290</v>
       </c>
     </row>
@@ -11700,13 +11733,13 @@
       <c r="A38" s="48" t="s">
         <v>311</v>
       </c>
-      <c r="B38" s="403"/>
-      <c r="C38" s="404"/>
-      <c r="D38" s="405"/>
+      <c r="B38" s="404"/>
+      <c r="C38" s="405"/>
+      <c r="D38" s="406"/>
       <c r="E38" s="56"/>
-      <c r="F38" s="406"/>
-      <c r="G38" s="407"/>
-      <c r="H38" s="408" t="s">
+      <c r="F38" s="410"/>
+      <c r="G38" s="411"/>
+      <c r="H38" s="414" t="s">
         <v>242</v>
       </c>
     </row>
@@ -11714,13 +11747,13 @@
       <c r="A39" s="56" t="s">
         <v>312</v>
       </c>
-      <c r="B39" s="406"/>
-      <c r="C39" s="407"/>
-      <c r="D39" s="409"/>
+      <c r="B39" s="410"/>
+      <c r="C39" s="411"/>
+      <c r="D39" s="412"/>
       <c r="E39" s="48"/>
-      <c r="F39" s="403"/>
-      <c r="G39" s="404"/>
-      <c r="H39" s="410" t="s">
+      <c r="F39" s="404"/>
+      <c r="G39" s="405"/>
+      <c r="H39" s="413" t="s">
         <v>243</v>
       </c>
     </row>
@@ -11728,57 +11761,28 @@
       <c r="A40" s="48" t="s">
         <v>313</v>
       </c>
-      <c r="B40" s="403"/>
-      <c r="C40" s="404"/>
-      <c r="D40" s="405"/>
+      <c r="B40" s="404"/>
+      <c r="C40" s="405"/>
+      <c r="D40" s="406"/>
       <c r="E40" s="56"/>
-      <c r="F40" s="406"/>
-      <c r="G40" s="407"/>
-      <c r="H40" s="408"/>
+      <c r="F40" s="410"/>
+      <c r="G40" s="411"/>
+      <c r="H40" s="414"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="68" t="s">
         <v>314</v>
       </c>
-      <c r="B41" s="397"/>
-      <c r="C41" s="398"/>
-      <c r="D41" s="399"/>
+      <c r="B41" s="415"/>
+      <c r="C41" s="416"/>
+      <c r="D41" s="417"/>
       <c r="E41" s="73"/>
-      <c r="F41" s="400"/>
-      <c r="G41" s="401"/>
-      <c r="H41" s="402"/>
+      <c r="F41" s="418"/>
+      <c r="G41" s="419"/>
+      <c r="H41" s="420"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -11787,6 +11791,35 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -13875,39 +13908,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27" customHeight="1" thickBot="1">
-      <c r="A1" s="313" t="s">
+      <c r="A1" s="317" t="s">
         <v>1149</v>
       </c>
-      <c r="B1" s="314"/>
-      <c r="C1" s="314"/>
-      <c r="D1" s="314"/>
-      <c r="E1" s="314"/>
-      <c r="F1" s="314"/>
-      <c r="G1" s="314"/>
-      <c r="H1" s="314"/>
-      <c r="I1" s="314"/>
-      <c r="J1" s="314"/>
-      <c r="K1" s="314"/>
-      <c r="L1" s="315"/>
+      <c r="B1" s="318"/>
+      <c r="C1" s="318"/>
+      <c r="D1" s="318"/>
+      <c r="E1" s="318"/>
+      <c r="F1" s="318"/>
+      <c r="G1" s="318"/>
+      <c r="H1" s="318"/>
+      <c r="I1" s="318"/>
+      <c r="J1" s="318"/>
+      <c r="K1" s="318"/>
+      <c r="L1" s="319"/>
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A2" s="310" t="s">
+      <c r="A2" s="314" t="s">
         <v>1150</v>
       </c>
-      <c r="B2" s="311"/>
-      <c r="C2" s="312"/>
+      <c r="B2" s="315"/>
+      <c r="C2" s="316"/>
       <c r="D2" s="285"/>
-      <c r="E2" s="310" t="s">
+      <c r="E2" s="314" t="s">
         <v>1058</v>
       </c>
-      <c r="F2" s="311"/>
-      <c r="G2" s="312"/>
+      <c r="F2" s="315"/>
+      <c r="G2" s="316"/>
       <c r="H2" s="285"/>
-      <c r="I2" s="310" t="s">
+      <c r="I2" s="314" t="s">
         <v>1057</v>
       </c>
-      <c r="J2" s="311"/>
-      <c r="K2" s="312"/>
+      <c r="J2" s="315"/>
+      <c r="K2" s="316"/>
       <c r="L2" s="145"/>
     </row>
     <row r="3" spans="1:12" ht="19.5" thickBot="1">
@@ -13943,7 +13976,7 @@
       <c r="L3" s="145"/>
     </row>
     <row r="4" spans="1:12" ht="18.75">
-      <c r="A4" s="304" t="s">
+      <c r="A4" s="320" t="s">
         <v>327</v>
       </c>
       <c r="B4" s="155" t="s">
@@ -13953,7 +13986,7 @@
         <v>708</v>
       </c>
       <c r="D4" s="279"/>
-      <c r="E4" s="307" t="s">
+      <c r="E4" s="311" t="s">
         <v>978</v>
       </c>
       <c r="F4" s="155" t="s">
@@ -13963,7 +13996,7 @@
         <v>1031</v>
       </c>
       <c r="H4" s="148"/>
-      <c r="I4" s="307" t="s">
+      <c r="I4" s="311" t="s">
         <v>1060</v>
       </c>
       <c r="J4" s="155" t="s">
@@ -13975,7 +14008,7 @@
       <c r="L4" s="145"/>
     </row>
     <row r="5" spans="1:12" ht="18.75">
-      <c r="A5" s="305"/>
+      <c r="A5" s="321"/>
       <c r="B5" s="154" t="s">
         <v>324</v>
       </c>
@@ -13983,7 +14016,7 @@
         <v>709</v>
       </c>
       <c r="D5" s="279"/>
-      <c r="E5" s="308"/>
+      <c r="E5" s="312"/>
       <c r="F5" s="154" t="s">
         <v>1005</v>
       </c>
@@ -13991,7 +14024,7 @@
         <v>1032</v>
       </c>
       <c r="H5" s="148"/>
-      <c r="I5" s="308"/>
+      <c r="I5" s="312"/>
       <c r="J5" s="154" t="s">
         <v>1095</v>
       </c>
@@ -14001,7 +14034,7 @@
       <c r="L5" s="145"/>
     </row>
     <row r="6" spans="1:12" ht="18.75">
-      <c r="A6" s="305"/>
+      <c r="A6" s="321"/>
       <c r="B6" s="154" t="s">
         <v>325</v>
       </c>
@@ -14009,7 +14042,7 @@
         <v>710</v>
       </c>
       <c r="D6" s="279"/>
-      <c r="E6" s="308"/>
+      <c r="E6" s="312"/>
       <c r="F6" s="154" t="s">
         <v>1006</v>
       </c>
@@ -14017,7 +14050,7 @@
         <v>1033</v>
       </c>
       <c r="H6" s="148"/>
-      <c r="I6" s="308"/>
+      <c r="I6" s="312"/>
       <c r="J6" s="154" t="s">
         <v>1096</v>
       </c>
@@ -14027,7 +14060,7 @@
       <c r="L6" s="145"/>
     </row>
     <row r="7" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A7" s="306"/>
+      <c r="A7" s="322"/>
       <c r="B7" s="158" t="s">
         <v>326</v>
       </c>
@@ -14035,7 +14068,7 @@
         <v>711</v>
       </c>
       <c r="D7" s="279"/>
-      <c r="E7" s="309"/>
+      <c r="E7" s="313"/>
       <c r="F7" s="158" t="s">
         <v>1007</v>
       </c>
@@ -14043,7 +14076,7 @@
         <v>1034</v>
       </c>
       <c r="H7" s="148"/>
-      <c r="I7" s="309"/>
+      <c r="I7" s="313"/>
       <c r="J7" s="158" t="s">
         <v>1097</v>
       </c>
@@ -14053,7 +14086,7 @@
       <c r="L7" s="145"/>
     </row>
     <row r="8" spans="1:12" ht="18.75">
-      <c r="A8" s="304" t="s">
+      <c r="A8" s="320" t="s">
         <v>670</v>
       </c>
       <c r="B8" s="155" t="s">
@@ -14063,7 +14096,7 @@
         <v>712</v>
       </c>
       <c r="D8" s="279"/>
-      <c r="E8" s="307" t="s">
+      <c r="E8" s="311" t="s">
         <v>977</v>
       </c>
       <c r="F8" s="155" t="s">
@@ -14073,7 +14106,7 @@
         <v>1035</v>
       </c>
       <c r="H8" s="148"/>
-      <c r="I8" s="307" t="s">
+      <c r="I8" s="311" t="s">
         <v>1061</v>
       </c>
       <c r="J8" s="155" t="s">
@@ -14085,7 +14118,7 @@
       <c r="L8" s="145"/>
     </row>
     <row r="9" spans="1:12" ht="18.75">
-      <c r="A9" s="305"/>
+      <c r="A9" s="321"/>
       <c r="B9" s="154" t="s">
         <v>661</v>
       </c>
@@ -14093,7 +14126,7 @@
         <v>713</v>
       </c>
       <c r="D9" s="279"/>
-      <c r="E9" s="308"/>
+      <c r="E9" s="312"/>
       <c r="F9" s="154" t="s">
         <v>1009</v>
       </c>
@@ -14101,7 +14134,7 @@
         <v>1036</v>
       </c>
       <c r="H9" s="148"/>
-      <c r="I9" s="308"/>
+      <c r="I9" s="312"/>
       <c r="J9" s="154" t="s">
         <v>1098</v>
       </c>
@@ -14111,7 +14144,7 @@
       <c r="L9" s="145"/>
     </row>
     <row r="10" spans="1:12" ht="18.75">
-      <c r="A10" s="305"/>
+      <c r="A10" s="321"/>
       <c r="B10" s="154" t="s">
         <v>662</v>
       </c>
@@ -14119,7 +14152,7 @@
         <v>714</v>
       </c>
       <c r="D10" s="279"/>
-      <c r="E10" s="308"/>
+      <c r="E10" s="312"/>
       <c r="F10" s="154" t="s">
         <v>1011</v>
       </c>
@@ -14127,7 +14160,7 @@
         <v>1037</v>
       </c>
       <c r="H10" s="148"/>
-      <c r="I10" s="308"/>
+      <c r="I10" s="312"/>
       <c r="J10" s="154" t="s">
         <v>1099</v>
       </c>
@@ -14137,7 +14170,7 @@
       <c r="L10" s="145"/>
     </row>
     <row r="11" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A11" s="306"/>
+      <c r="A11" s="322"/>
       <c r="B11" s="158" t="s">
         <v>663</v>
       </c>
@@ -14145,7 +14178,7 @@
         <v>715</v>
       </c>
       <c r="D11" s="279"/>
-      <c r="E11" s="309"/>
+      <c r="E11" s="313"/>
       <c r="F11" s="158" t="s">
         <v>1012</v>
       </c>
@@ -14153,7 +14186,7 @@
         <v>1038</v>
       </c>
       <c r="H11" s="148"/>
-      <c r="I11" s="309"/>
+      <c r="I11" s="313"/>
       <c r="J11" s="158" t="s">
         <v>1100</v>
       </c>
@@ -14163,7 +14196,7 @@
       <c r="L11" s="145"/>
     </row>
     <row r="12" spans="1:12" ht="18.75">
-      <c r="A12" s="304" t="s">
+      <c r="A12" s="320" t="s">
         <v>668</v>
       </c>
       <c r="B12" s="155" t="s">
@@ -14173,7 +14206,7 @@
         <v>716</v>
       </c>
       <c r="D12" s="279"/>
-      <c r="E12" s="307" t="s">
+      <c r="E12" s="311" t="s">
         <v>976</v>
       </c>
       <c r="F12" s="155" t="s">
@@ -14183,7 +14216,7 @@
         <v>1039</v>
       </c>
       <c r="H12" s="148"/>
-      <c r="I12" s="307" t="s">
+      <c r="I12" s="311" t="s">
         <v>1062</v>
       </c>
       <c r="J12" s="155" t="s">
@@ -14195,7 +14228,7 @@
       <c r="L12" s="145"/>
     </row>
     <row r="13" spans="1:12" ht="18.75">
-      <c r="A13" s="305"/>
+      <c r="A13" s="321"/>
       <c r="B13" s="154" t="s">
         <v>665</v>
       </c>
@@ -14203,7 +14236,7 @@
         <v>717</v>
       </c>
       <c r="D13" s="279"/>
-      <c r="E13" s="308"/>
+      <c r="E13" s="312"/>
       <c r="F13" s="154" t="s">
         <v>1014</v>
       </c>
@@ -14211,7 +14244,7 @@
         <v>1040</v>
       </c>
       <c r="H13" s="148"/>
-      <c r="I13" s="308"/>
+      <c r="I13" s="312"/>
       <c r="J13" s="154" t="s">
         <v>1102</v>
       </c>
@@ -14221,7 +14254,7 @@
       <c r="L13" s="145"/>
     </row>
     <row r="14" spans="1:12" ht="18.75">
-      <c r="A14" s="305"/>
+      <c r="A14" s="321"/>
       <c r="B14" s="154" t="s">
         <v>666</v>
       </c>
@@ -14229,7 +14262,7 @@
         <v>718</v>
       </c>
       <c r="D14" s="279"/>
-      <c r="E14" s="308"/>
+      <c r="E14" s="312"/>
       <c r="F14" s="154" t="s">
         <v>1015</v>
       </c>
@@ -14237,7 +14270,7 @@
         <v>1041</v>
       </c>
       <c r="H14" s="148"/>
-      <c r="I14" s="308"/>
+      <c r="I14" s="312"/>
       <c r="J14" s="154" t="s">
         <v>1103</v>
       </c>
@@ -14247,7 +14280,7 @@
       <c r="L14" s="145"/>
     </row>
     <row r="15" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A15" s="306"/>
+      <c r="A15" s="322"/>
       <c r="B15" s="158" t="s">
         <v>667</v>
       </c>
@@ -14255,7 +14288,7 @@
         <v>719</v>
       </c>
       <c r="D15" s="279"/>
-      <c r="E15" s="309"/>
+      <c r="E15" s="313"/>
       <c r="F15" s="158" t="s">
         <v>1016</v>
       </c>
@@ -14263,7 +14296,7 @@
         <v>1042</v>
       </c>
       <c r="H15" s="148"/>
-      <c r="I15" s="309"/>
+      <c r="I15" s="313"/>
       <c r="J15" s="158" t="s">
         <v>1104</v>
       </c>
@@ -14273,7 +14306,7 @@
       <c r="L15" s="145"/>
     </row>
     <row r="16" spans="1:12" ht="18.75">
-      <c r="A16" s="304" t="s">
+      <c r="A16" s="320" t="s">
         <v>669</v>
       </c>
       <c r="B16" s="155" t="s">
@@ -14283,7 +14316,7 @@
         <v>720</v>
       </c>
       <c r="D16" s="279"/>
-      <c r="E16" s="307" t="s">
+      <c r="E16" s="311" t="s">
         <v>975</v>
       </c>
       <c r="F16" s="155" t="s">
@@ -14293,7 +14326,7 @@
         <v>1043</v>
       </c>
       <c r="H16" s="148"/>
-      <c r="I16" s="307" t="s">
+      <c r="I16" s="311" t="s">
         <v>1063</v>
       </c>
       <c r="J16" s="155" t="s">
@@ -14305,7 +14338,7 @@
       <c r="L16" s="145"/>
     </row>
     <row r="17" spans="1:12" ht="18.75">
-      <c r="A17" s="305"/>
+      <c r="A17" s="321"/>
       <c r="B17" s="154" t="s">
         <v>672</v>
       </c>
@@ -14313,7 +14346,7 @@
         <v>721</v>
       </c>
       <c r="D17" s="279"/>
-      <c r="E17" s="308"/>
+      <c r="E17" s="312"/>
       <c r="F17" s="154" t="s">
         <v>1018</v>
       </c>
@@ -14321,7 +14354,7 @@
         <v>1044</v>
       </c>
       <c r="H17" s="148"/>
-      <c r="I17" s="308"/>
+      <c r="I17" s="312"/>
       <c r="J17" s="154" t="s">
         <v>1106</v>
       </c>
@@ -14331,7 +14364,7 @@
       <c r="L17" s="145"/>
     </row>
     <row r="18" spans="1:12" ht="18.75">
-      <c r="A18" s="305"/>
+      <c r="A18" s="321"/>
       <c r="B18" s="154" t="s">
         <v>673</v>
       </c>
@@ -14339,7 +14372,7 @@
         <v>722</v>
       </c>
       <c r="D18" s="279"/>
-      <c r="E18" s="308"/>
+      <c r="E18" s="312"/>
       <c r="F18" s="154" t="s">
         <v>1019</v>
       </c>
@@ -14347,7 +14380,7 @@
         <v>1045</v>
       </c>
       <c r="H18" s="148"/>
-      <c r="I18" s="308"/>
+      <c r="I18" s="312"/>
       <c r="J18" s="154" t="s">
         <v>1107</v>
       </c>
@@ -14357,7 +14390,7 @@
       <c r="L18" s="145"/>
     </row>
     <row r="19" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A19" s="306"/>
+      <c r="A19" s="322"/>
       <c r="B19" s="158" t="s">
         <v>674</v>
       </c>
@@ -14365,7 +14398,7 @@
         <v>723</v>
       </c>
       <c r="D19" s="279"/>
-      <c r="E19" s="309"/>
+      <c r="E19" s="313"/>
       <c r="F19" s="158" t="s">
         <v>1020</v>
       </c>
@@ -14373,7 +14406,7 @@
         <v>1046</v>
       </c>
       <c r="H19" s="148"/>
-      <c r="I19" s="309"/>
+      <c r="I19" s="313"/>
       <c r="J19" s="158" t="s">
         <v>1108</v>
       </c>
@@ -14387,7 +14420,7 @@
       <c r="B20" s="148"/>
       <c r="C20" s="148"/>
       <c r="D20" s="148"/>
-      <c r="E20" s="307" t="s">
+      <c r="E20" s="311" t="s">
         <v>563</v>
       </c>
       <c r="F20" s="155" t="s">
@@ -14397,7 +14430,7 @@
         <v>1047</v>
       </c>
       <c r="H20" s="148"/>
-      <c r="I20" s="307" t="s">
+      <c r="I20" s="311" t="s">
         <v>1064</v>
       </c>
       <c r="J20" s="155" t="s">
@@ -14413,7 +14446,7 @@
       <c r="B21" s="148"/>
       <c r="C21" s="148"/>
       <c r="D21" s="148"/>
-      <c r="E21" s="308"/>
+      <c r="E21" s="312"/>
       <c r="F21" s="154" t="s">
         <v>1022</v>
       </c>
@@ -14421,7 +14454,7 @@
         <v>1048</v>
       </c>
       <c r="H21" s="148"/>
-      <c r="I21" s="308"/>
+      <c r="I21" s="312"/>
       <c r="J21" s="154" t="s">
         <v>1110</v>
       </c>
@@ -14435,7 +14468,7 @@
       <c r="B22" s="148"/>
       <c r="C22" s="148"/>
       <c r="D22" s="148"/>
-      <c r="E22" s="308"/>
+      <c r="E22" s="312"/>
       <c r="F22" s="154" t="s">
         <v>1023</v>
       </c>
@@ -14443,7 +14476,7 @@
         <v>1049</v>
       </c>
       <c r="H22" s="148"/>
-      <c r="I22" s="308"/>
+      <c r="I22" s="312"/>
       <c r="J22" s="154" t="s">
         <v>1111</v>
       </c>
@@ -14459,7 +14492,7 @@
       <c r="B23" s="282"/>
       <c r="C23" s="283"/>
       <c r="D23" s="148"/>
-      <c r="E23" s="309"/>
+      <c r="E23" s="313"/>
       <c r="F23" s="158" t="s">
         <v>1024</v>
       </c>
@@ -14467,7 +14500,7 @@
         <v>1050</v>
       </c>
       <c r="H23" s="148"/>
-      <c r="I23" s="309"/>
+      <c r="I23" s="313"/>
       <c r="J23" s="158" t="s">
         <v>1112</v>
       </c>
@@ -14487,7 +14520,7 @@
         <v>323</v>
       </c>
       <c r="D24" s="148"/>
-      <c r="E24" s="307" t="s">
+      <c r="E24" s="311" t="s">
         <v>752</v>
       </c>
       <c r="F24" s="155" t="s">
@@ -14497,7 +14530,7 @@
         <v>1051</v>
       </c>
       <c r="H24" s="148"/>
-      <c r="I24" s="307" t="s">
+      <c r="I24" s="311" t="s">
         <v>1065</v>
       </c>
       <c r="J24" s="155" t="s">
@@ -14509,7 +14542,7 @@
       <c r="L24" s="145"/>
     </row>
     <row r="25" spans="1:12" ht="18.75">
-      <c r="A25" s="319" t="s">
+      <c r="A25" s="305" t="s">
         <v>496</v>
       </c>
       <c r="B25" s="155" t="s">
@@ -14519,7 +14552,7 @@
         <v>724</v>
       </c>
       <c r="D25" s="148"/>
-      <c r="E25" s="308"/>
+      <c r="E25" s="312"/>
       <c r="F25" s="154" t="s">
         <v>1026</v>
       </c>
@@ -14527,7 +14560,7 @@
         <v>1052</v>
       </c>
       <c r="H25" s="148"/>
-      <c r="I25" s="308"/>
+      <c r="I25" s="312"/>
       <c r="J25" s="154" t="s">
         <v>1114</v>
       </c>
@@ -14537,7 +14570,7 @@
       <c r="L25" s="145"/>
     </row>
     <row r="26" spans="1:12" ht="18.75">
-      <c r="A26" s="320"/>
+      <c r="A26" s="306"/>
       <c r="B26" s="154" t="s">
         <v>682</v>
       </c>
@@ -14545,7 +14578,7 @@
         <v>725</v>
       </c>
       <c r="D26" s="148"/>
-      <c r="E26" s="308"/>
+      <c r="E26" s="312"/>
       <c r="F26" s="154" t="s">
         <v>1027</v>
       </c>
@@ -14553,7 +14586,7 @@
         <v>1053</v>
       </c>
       <c r="H26" s="148"/>
-      <c r="I26" s="308"/>
+      <c r="I26" s="312"/>
       <c r="J26" s="154" t="s">
         <v>1115</v>
       </c>
@@ -14563,7 +14596,7 @@
       <c r="L26" s="145"/>
     </row>
     <row r="27" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A27" s="320"/>
+      <c r="A27" s="306"/>
       <c r="B27" s="154" t="s">
         <v>683</v>
       </c>
@@ -14571,7 +14604,7 @@
         <v>726</v>
       </c>
       <c r="D27" s="148"/>
-      <c r="E27" s="309"/>
+      <c r="E27" s="313"/>
       <c r="F27" s="158" t="s">
         <v>1028</v>
       </c>
@@ -14579,7 +14612,7 @@
         <v>1054</v>
       </c>
       <c r="H27" s="148"/>
-      <c r="I27" s="309"/>
+      <c r="I27" s="313"/>
       <c r="J27" s="158" t="s">
         <v>1116</v>
       </c>
@@ -14589,7 +14622,7 @@
       <c r="L27" s="145"/>
     </row>
     <row r="28" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A28" s="321"/>
+      <c r="A28" s="307"/>
       <c r="B28" s="158" t="s">
         <v>684</v>
       </c>
@@ -14597,7 +14630,7 @@
         <v>727</v>
       </c>
       <c r="D28" s="148"/>
-      <c r="E28" s="307" t="s">
+      <c r="E28" s="311" t="s">
         <v>565</v>
       </c>
       <c r="F28" s="155" t="s">
@@ -14607,7 +14640,7 @@
         <v>1055</v>
       </c>
       <c r="H28" s="148"/>
-      <c r="I28" s="307" t="s">
+      <c r="I28" s="311" t="s">
         <v>1066</v>
       </c>
       <c r="J28" s="155" t="s">
@@ -14619,7 +14652,7 @@
       <c r="L28" s="145"/>
     </row>
     <row r="29" spans="1:12" ht="18.75">
-      <c r="A29" s="319" t="s">
+      <c r="A29" s="305" t="s">
         <v>690</v>
       </c>
       <c r="B29" s="155" t="s">
@@ -14629,7 +14662,7 @@
         <v>728</v>
       </c>
       <c r="D29" s="279"/>
-      <c r="E29" s="308"/>
+      <c r="E29" s="312"/>
       <c r="F29" s="154" t="s">
         <v>1030</v>
       </c>
@@ -14637,7 +14670,7 @@
         <v>1056</v>
       </c>
       <c r="H29" s="148"/>
-      <c r="I29" s="308"/>
+      <c r="I29" s="312"/>
       <c r="J29" s="154" t="s">
         <v>1118</v>
       </c>
@@ -14647,7 +14680,7 @@
       <c r="L29" s="145"/>
     </row>
     <row r="30" spans="1:12" ht="18.75">
-      <c r="A30" s="320"/>
+      <c r="A30" s="306"/>
       <c r="B30" s="154" t="s">
         <v>687</v>
       </c>
@@ -14655,11 +14688,11 @@
         <v>729</v>
       </c>
       <c r="D30" s="279"/>
-      <c r="E30" s="308"/>
+      <c r="E30" s="312"/>
       <c r="F30" s="154"/>
       <c r="G30" s="276"/>
       <c r="H30" s="148"/>
-      <c r="I30" s="308"/>
+      <c r="I30" s="312"/>
       <c r="J30" s="154" t="s">
         <v>1119</v>
       </c>
@@ -14669,7 +14702,7 @@
       <c r="L30" s="145"/>
     </row>
     <row r="31" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A31" s="320"/>
+      <c r="A31" s="306"/>
       <c r="B31" s="154" t="s">
         <v>688</v>
       </c>
@@ -14677,11 +14710,11 @@
         <v>730</v>
       </c>
       <c r="D31" s="279"/>
-      <c r="E31" s="309"/>
+      <c r="E31" s="313"/>
       <c r="F31" s="158"/>
       <c r="G31" s="277"/>
       <c r="H31" s="148"/>
-      <c r="I31" s="309"/>
+      <c r="I31" s="313"/>
       <c r="J31" s="158" t="s">
         <v>1120</v>
       </c>
@@ -14691,7 +14724,7 @@
       <c r="L31" s="145"/>
     </row>
     <row r="32" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A32" s="321"/>
+      <c r="A32" s="307"/>
       <c r="B32" s="158" t="s">
         <v>689</v>
       </c>
@@ -14709,7 +14742,7 @@
       <c r="L32" s="145"/>
     </row>
     <row r="33" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A33" s="319" t="s">
+      <c r="A33" s="305" t="s">
         <v>694</v>
       </c>
       <c r="B33" s="155" t="s">
@@ -14719,21 +14752,21 @@
         <v>732</v>
       </c>
       <c r="D33" s="279"/>
-      <c r="E33" s="316" t="s">
+      <c r="E33" s="308" t="s">
         <v>1152</v>
       </c>
-      <c r="F33" s="317"/>
-      <c r="G33" s="318"/>
+      <c r="F33" s="309"/>
+      <c r="G33" s="310"/>
       <c r="H33" s="147"/>
-      <c r="I33" s="316" t="s">
+      <c r="I33" s="308" t="s">
         <v>1151</v>
       </c>
-      <c r="J33" s="317"/>
-      <c r="K33" s="318"/>
+      <c r="J33" s="309"/>
+      <c r="K33" s="310"/>
       <c r="L33" s="145"/>
     </row>
     <row r="34" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A34" s="320"/>
+      <c r="A34" s="306"/>
       <c r="B34" s="154" t="s">
         <v>696</v>
       </c>
@@ -14763,7 +14796,7 @@
       <c r="L34" s="145"/>
     </row>
     <row r="35" spans="1:12" ht="18.75">
-      <c r="A35" s="320"/>
+      <c r="A35" s="306"/>
       <c r="B35" s="154" t="s">
         <v>697</v>
       </c>
@@ -14771,7 +14804,7 @@
         <v>734</v>
       </c>
       <c r="D35" s="279"/>
-      <c r="E35" s="319" t="s">
+      <c r="E35" s="305" t="s">
         <v>497</v>
       </c>
       <c r="F35" s="155" t="s">
@@ -14781,7 +14814,7 @@
         <v>11311</v>
       </c>
       <c r="H35" s="147"/>
-      <c r="I35" s="319" t="s">
+      <c r="I35" s="305" t="s">
         <v>958</v>
       </c>
       <c r="J35" s="155" t="s">
@@ -14793,7 +14826,7 @@
       <c r="L35" s="145"/>
     </row>
     <row r="36" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A36" s="321"/>
+      <c r="A36" s="307"/>
       <c r="B36" s="158" t="s">
         <v>698</v>
       </c>
@@ -14801,7 +14834,7 @@
         <v>735</v>
       </c>
       <c r="D36" s="279"/>
-      <c r="E36" s="320"/>
+      <c r="E36" s="306"/>
       <c r="F36" s="154" t="s">
         <v>961</v>
       </c>
@@ -14809,7 +14842,7 @@
         <v>11312</v>
       </c>
       <c r="H36" s="147"/>
-      <c r="I36" s="320"/>
+      <c r="I36" s="306"/>
       <c r="J36" s="154" t="s">
         <v>968</v>
       </c>
@@ -14819,7 +14852,7 @@
       <c r="L36" s="145"/>
     </row>
     <row r="37" spans="1:12" ht="18.75">
-      <c r="A37" s="319" t="s">
+      <c r="A37" s="305" t="s">
         <v>701</v>
       </c>
       <c r="B37" s="155" t="s">
@@ -14829,7 +14862,7 @@
         <v>11441</v>
       </c>
       <c r="D37" s="279"/>
-      <c r="E37" s="320"/>
+      <c r="E37" s="306"/>
       <c r="F37" s="154" t="s">
         <v>962</v>
       </c>
@@ -14837,7 +14870,7 @@
         <v>11313</v>
       </c>
       <c r="H37" s="147"/>
-      <c r="I37" s="320"/>
+      <c r="I37" s="306"/>
       <c r="J37" s="154" t="s">
         <v>969</v>
       </c>
@@ -14847,7 +14880,7 @@
       <c r="L37" s="145"/>
     </row>
     <row r="38" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A38" s="320"/>
+      <c r="A38" s="306"/>
       <c r="B38" s="154" t="s">
         <v>703</v>
       </c>
@@ -14855,7 +14888,7 @@
         <v>11442</v>
       </c>
       <c r="D38" s="279"/>
-      <c r="E38" s="321"/>
+      <c r="E38" s="307"/>
       <c r="F38" s="158" t="s">
         <v>962</v>
       </c>
@@ -14863,7 +14896,7 @@
         <v>11314</v>
       </c>
       <c r="H38" s="147"/>
-      <c r="I38" s="321"/>
+      <c r="I38" s="307"/>
       <c r="J38" s="158" t="s">
         <v>970</v>
       </c>
@@ -14873,7 +14906,7 @@
       <c r="L38" s="145"/>
     </row>
     <row r="39" spans="1:12" ht="18.75">
-      <c r="A39" s="320"/>
+      <c r="A39" s="306"/>
       <c r="B39" s="154" t="s">
         <v>704</v>
       </c>
@@ -14881,7 +14914,7 @@
         <v>11443</v>
       </c>
       <c r="D39" s="279"/>
-      <c r="E39" s="319" t="s">
+      <c r="E39" s="305" t="s">
         <v>957</v>
       </c>
       <c r="F39" s="155" t="s">
@@ -14891,7 +14924,7 @@
         <v>11321</v>
       </c>
       <c r="H39" s="147"/>
-      <c r="I39" s="319" t="s">
+      <c r="I39" s="305" t="s">
         <v>959</v>
       </c>
       <c r="J39" s="155" t="s">
@@ -14903,7 +14936,7 @@
       <c r="L39" s="145"/>
     </row>
     <row r="40" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A40" s="321"/>
+      <c r="A40" s="307"/>
       <c r="B40" s="158" t="s">
         <v>705</v>
       </c>
@@ -14911,7 +14944,7 @@
         <v>11444</v>
       </c>
       <c r="D40" s="279"/>
-      <c r="E40" s="320"/>
+      <c r="E40" s="306"/>
       <c r="F40" s="154" t="s">
         <v>964</v>
       </c>
@@ -14919,7 +14952,7 @@
         <v>11322</v>
       </c>
       <c r="H40" s="147"/>
-      <c r="I40" s="320"/>
+      <c r="I40" s="306"/>
       <c r="J40" s="154" t="s">
         <v>972</v>
       </c>
@@ -14933,7 +14966,7 @@
       <c r="B41" s="148"/>
       <c r="C41" s="279"/>
       <c r="D41" s="279"/>
-      <c r="E41" s="320"/>
+      <c r="E41" s="306"/>
       <c r="F41" s="154" t="s">
         <v>965</v>
       </c>
@@ -14941,7 +14974,7 @@
         <v>11323</v>
       </c>
       <c r="H41" s="147"/>
-      <c r="I41" s="320"/>
+      <c r="I41" s="306"/>
       <c r="J41" s="154" t="s">
         <v>973</v>
       </c>
@@ -14955,7 +14988,7 @@
       <c r="B42" s="148"/>
       <c r="C42" s="279"/>
       <c r="D42" s="279"/>
-      <c r="E42" s="321"/>
+      <c r="E42" s="307"/>
       <c r="F42" s="158" t="s">
         <v>966</v>
       </c>
@@ -14963,7 +14996,7 @@
         <v>11324</v>
       </c>
       <c r="H42" s="147"/>
-      <c r="I42" s="321"/>
+      <c r="I42" s="307"/>
       <c r="J42" s="158" t="s">
         <v>974</v>
       </c>
@@ -15016,16 +15049,18 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="I35:I38"/>
-    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A7"/>
     <mergeCell ref="I16:I19"/>
     <mergeCell ref="I12:I15"/>
     <mergeCell ref="I8:I11"/>
@@ -15036,18 +15071,16 @@
     <mergeCell ref="I28:I31"/>
     <mergeCell ref="E20:E23"/>
     <mergeCell ref="E24:E27"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="I35:I38"/>
+    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="E33:G33"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15078,40 +15111,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="326" t="s">
+      <c r="A1" s="323" t="s">
         <v>1154</v>
       </c>
-      <c r="B1" s="327"/>
-      <c r="C1" s="327"/>
-      <c r="D1" s="327"/>
-      <c r="E1" s="327"/>
-      <c r="F1" s="327"/>
-      <c r="G1" s="327"/>
-      <c r="H1" s="328"/>
+      <c r="B1" s="324"/>
+      <c r="C1" s="324"/>
+      <c r="D1" s="324"/>
+      <c r="E1" s="324"/>
+      <c r="F1" s="324"/>
+      <c r="G1" s="324"/>
+      <c r="H1" s="325"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="329"/>
-      <c r="B2" s="330"/>
-      <c r="C2" s="330"/>
-      <c r="D2" s="330"/>
-      <c r="E2" s="330"/>
-      <c r="F2" s="330"/>
-      <c r="G2" s="330"/>
-      <c r="H2" s="331"/>
+      <c r="A2" s="326"/>
+      <c r="B2" s="327"/>
+      <c r="C2" s="327"/>
+      <c r="D2" s="327"/>
+      <c r="E2" s="327"/>
+      <c r="F2" s="327"/>
+      <c r="G2" s="327"/>
+      <c r="H2" s="328"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="332" t="s">
+      <c r="A3" s="329" t="s">
         <v>251</v>
       </c>
-      <c r="B3" s="333"/>
-      <c r="C3" s="333"/>
-      <c r="D3" s="333"/>
-      <c r="E3" s="333" t="s">
+      <c r="B3" s="330"/>
+      <c r="C3" s="330"/>
+      <c r="D3" s="330"/>
+      <c r="E3" s="330" t="s">
         <v>252</v>
       </c>
-      <c r="F3" s="333"/>
-      <c r="G3" s="333"/>
-      <c r="H3" s="334"/>
+      <c r="F3" s="330"/>
+      <c r="G3" s="330"/>
+      <c r="H3" s="331"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="19">
@@ -15645,11 +15678,11 @@
       <c r="C27" s="140" t="s">
         <v>597</v>
       </c>
-      <c r="D27" s="325" t="s">
+      <c r="D27" s="332" t="s">
         <v>573</v>
       </c>
-      <c r="E27" s="325"/>
-      <c r="F27" s="325"/>
+      <c r="E27" s="332"/>
+      <c r="F27" s="332"/>
       <c r="G27" s="24"/>
       <c r="H27" s="25"/>
     </row>
@@ -15661,11 +15694,11 @@
       <c r="C28" s="140" t="s">
         <v>601</v>
       </c>
-      <c r="D28" s="325" t="s">
+      <c r="D28" s="332" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="325"/>
-      <c r="F28" s="325"/>
+      <c r="E28" s="332"/>
+      <c r="F28" s="332"/>
       <c r="G28" s="24"/>
       <c r="H28" s="25"/>
     </row>
@@ -15677,11 +15710,11 @@
       <c r="C29" s="140" t="s">
         <v>602</v>
       </c>
-      <c r="D29" s="325" t="s">
+      <c r="D29" s="332" t="s">
         <v>574</v>
       </c>
-      <c r="E29" s="325"/>
-      <c r="F29" s="325"/>
+      <c r="E29" s="332"/>
+      <c r="F29" s="332"/>
       <c r="G29" s="24"/>
       <c r="H29" s="25"/>
     </row>
@@ -15693,11 +15726,11 @@
       <c r="C30" s="140" t="s">
         <v>603</v>
       </c>
-      <c r="D30" s="325" t="s">
+      <c r="D30" s="332" t="s">
         <v>575</v>
       </c>
-      <c r="E30" s="325"/>
-      <c r="F30" s="325"/>
+      <c r="E30" s="332"/>
+      <c r="F30" s="332"/>
       <c r="G30" s="24"/>
       <c r="H30" s="25"/>
     </row>
@@ -15709,11 +15742,11 @@
       <c r="C31" s="140" t="s">
         <v>604</v>
       </c>
-      <c r="D31" s="325" t="s">
+      <c r="D31" s="332" t="s">
         <v>576</v>
       </c>
-      <c r="E31" s="325"/>
-      <c r="F31" s="325"/>
+      <c r="E31" s="332"/>
+      <c r="F31" s="332"/>
       <c r="G31" s="24"/>
       <c r="H31" s="25"/>
     </row>
@@ -15725,11 +15758,11 @@
       <c r="C32" s="140" t="s">
         <v>605</v>
       </c>
-      <c r="D32" s="325" t="s">
+      <c r="D32" s="332" t="s">
         <v>577</v>
       </c>
-      <c r="E32" s="325"/>
-      <c r="F32" s="325"/>
+      <c r="E32" s="332"/>
+      <c r="F32" s="332"/>
       <c r="G32" s="24"/>
       <c r="H32" s="25"/>
     </row>
@@ -15741,11 +15774,11 @@
       <c r="C33" s="140" t="s">
         <v>617</v>
       </c>
-      <c r="D33" s="325" t="s">
+      <c r="D33" s="332" t="s">
         <v>485</v>
       </c>
-      <c r="E33" s="325"/>
-      <c r="F33" s="325"/>
+      <c r="E33" s="332"/>
+      <c r="F33" s="332"/>
       <c r="G33" s="24"/>
       <c r="H33" s="25"/>
     </row>
@@ -15757,11 +15790,11 @@
       <c r="C34" s="140" t="s">
         <v>618</v>
       </c>
-      <c r="D34" s="325" t="s">
+      <c r="D34" s="332" t="s">
         <v>578</v>
       </c>
-      <c r="E34" s="325"/>
-      <c r="F34" s="325"/>
+      <c r="E34" s="332"/>
+      <c r="F34" s="332"/>
       <c r="G34" s="24"/>
       <c r="H34" s="25"/>
     </row>
@@ -15773,11 +15806,11 @@
       <c r="C35" s="140" t="s">
         <v>619</v>
       </c>
-      <c r="D35" s="325" t="s">
+      <c r="D35" s="332" t="s">
         <v>579</v>
       </c>
-      <c r="E35" s="325"/>
-      <c r="F35" s="325"/>
+      <c r="E35" s="332"/>
+      <c r="F35" s="332"/>
       <c r="G35" s="24"/>
       <c r="H35" s="25"/>
     </row>
@@ -15787,11 +15820,11 @@
       <c r="C36" s="140" t="s">
         <v>654</v>
       </c>
-      <c r="D36" s="322" t="s">
+      <c r="D36" s="333" t="s">
         <v>594</v>
       </c>
-      <c r="E36" s="323"/>
-      <c r="F36" s="324"/>
+      <c r="E36" s="334"/>
+      <c r="F36" s="335"/>
       <c r="G36" s="24"/>
       <c r="H36" s="25"/>
     </row>
@@ -15801,11 +15834,11 @@
       <c r="C37" s="140" t="s">
         <v>657</v>
       </c>
-      <c r="D37" s="322" t="s">
+      <c r="D37" s="333" t="s">
         <v>655</v>
       </c>
-      <c r="E37" s="323"/>
-      <c r="F37" s="324"/>
+      <c r="E37" s="334"/>
+      <c r="F37" s="335"/>
       <c r="G37" s="24"/>
       <c r="H37" s="25"/>
     </row>
@@ -15815,11 +15848,11 @@
       <c r="C38" s="140" t="s">
         <v>656</v>
       </c>
-      <c r="D38" s="322" t="s">
+      <c r="D38" s="333" t="s">
         <v>658</v>
       </c>
-      <c r="E38" s="323"/>
-      <c r="F38" s="324"/>
+      <c r="E38" s="334"/>
+      <c r="F38" s="335"/>
       <c r="G38" s="24"/>
       <c r="H38" s="25"/>
     </row>
@@ -15827,9 +15860,9 @@
       <c r="A39" s="23"/>
       <c r="B39" s="142"/>
       <c r="C39" s="140"/>
-      <c r="D39" s="322"/>
-      <c r="E39" s="323"/>
-      <c r="F39" s="324"/>
+      <c r="D39" s="333"/>
+      <c r="E39" s="334"/>
+      <c r="F39" s="335"/>
       <c r="G39" s="24"/>
       <c r="H39" s="25"/>
     </row>
@@ -15927,6 +15960,13 @@
     <row r="52" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:H3"/>
@@ -15936,13 +15976,6 @@
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15970,28 +16003,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="344" t="s">
+      <c r="A1" s="345" t="s">
         <v>1187</v>
       </c>
-      <c r="B1" s="344"/>
-      <c r="C1" s="344"/>
-      <c r="D1" s="344"/>
-      <c r="E1" s="344"/>
-      <c r="F1" s="344"/>
-      <c r="G1" s="344"/>
-      <c r="H1" s="344"/>
+      <c r="B1" s="345"/>
+      <c r="C1" s="345"/>
+      <c r="D1" s="345"/>
+      <c r="E1" s="345"/>
+      <c r="F1" s="345"/>
+      <c r="G1" s="345"/>
+      <c r="H1" s="345"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="338" t="s">
+      <c r="A2" s="339" t="s">
         <v>1155</v>
       </c>
-      <c r="B2" s="339"/>
-      <c r="C2" s="339"/>
-      <c r="D2" s="339"/>
-      <c r="E2" s="339"/>
-      <c r="F2" s="339"/>
-      <c r="G2" s="339"/>
-      <c r="H2" s="340"/>
+      <c r="B2" s="340"/>
+      <c r="C2" s="340"/>
+      <c r="D2" s="340"/>
+      <c r="E2" s="340"/>
+      <c r="F2" s="340"/>
+      <c r="G2" s="340"/>
+      <c r="H2" s="341"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="5"/>
@@ -16310,16 +16343,16 @@
       <c r="H17" s="291"/>
     </row>
     <row r="18" spans="1:11" ht="15.75">
-      <c r="A18" s="341" t="s">
+      <c r="A18" s="342" t="s">
         <v>224</v>
       </c>
-      <c r="B18" s="342"/>
-      <c r="C18" s="342"/>
-      <c r="D18" s="342"/>
-      <c r="E18" s="342"/>
-      <c r="F18" s="342"/>
-      <c r="G18" s="342"/>
-      <c r="H18" s="343"/>
+      <c r="B18" s="343"/>
+      <c r="C18" s="343"/>
+      <c r="D18" s="343"/>
+      <c r="E18" s="343"/>
+      <c r="F18" s="343"/>
+      <c r="G18" s="343"/>
+      <c r="H18" s="344"/>
     </row>
     <row r="19" spans="1:11" ht="15.75">
       <c r="A19" s="292"/>
@@ -16575,16 +16608,16 @@
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:11" ht="15.75">
-      <c r="A31" s="338" t="s">
+      <c r="A31" s="339" t="s">
         <v>225</v>
       </c>
-      <c r="B31" s="339"/>
-      <c r="C31" s="339"/>
-      <c r="D31" s="339"/>
-      <c r="E31" s="339"/>
-      <c r="F31" s="339"/>
-      <c r="G31" s="339"/>
-      <c r="H31" s="340"/>
+      <c r="B31" s="340"/>
+      <c r="C31" s="340"/>
+      <c r="D31" s="340"/>
+      <c r="E31" s="340"/>
+      <c r="F31" s="340"/>
+      <c r="G31" s="340"/>
+      <c r="H31" s="341"/>
     </row>
     <row r="32" spans="1:11" ht="15.75">
       <c r="A32" s="5"/>
@@ -16810,18 +16843,18 @@
     </row>
     <row r="43" spans="1:8" ht="10.5" customHeight="1"/>
     <row r="44" spans="1:8" ht="15.75">
-      <c r="A44" s="335" t="s">
+      <c r="A44" s="336" t="s">
         <v>1178</v>
       </c>
-      <c r="B44" s="336"/>
-      <c r="C44" s="336"/>
-      <c r="D44" s="337"/>
-      <c r="E44" s="335" t="s">
+      <c r="B44" s="337"/>
+      <c r="C44" s="337"/>
+      <c r="D44" s="338"/>
+      <c r="E44" s="336" t="s">
         <v>1178</v>
       </c>
-      <c r="F44" s="336"/>
-      <c r="G44" s="336"/>
-      <c r="H44" s="337"/>
+      <c r="F44" s="337"/>
+      <c r="G44" s="337"/>
+      <c r="H44" s="338"/>
     </row>
     <row r="45" spans="1:8" ht="15.75">
       <c r="A45" s="3"/>
@@ -16939,40 +16972,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="345" t="s">
+      <c r="A1" s="346" t="s">
         <v>328</v>
       </c>
-      <c r="B1" s="346"/>
-      <c r="C1" s="346"/>
-      <c r="D1" s="346"/>
-      <c r="E1" s="346"/>
-      <c r="F1" s="346"/>
-      <c r="G1" s="346"/>
-      <c r="H1" s="347"/>
+      <c r="B1" s="347"/>
+      <c r="C1" s="347"/>
+      <c r="D1" s="347"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="347"/>
+      <c r="G1" s="347"/>
+      <c r="H1" s="348"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="348"/>
-      <c r="B2" s="349"/>
-      <c r="C2" s="349"/>
-      <c r="D2" s="349"/>
-      <c r="E2" s="349"/>
-      <c r="F2" s="349"/>
-      <c r="G2" s="349"/>
-      <c r="H2" s="350"/>
+      <c r="A2" s="349"/>
+      <c r="B2" s="350"/>
+      <c r="C2" s="350"/>
+      <c r="D2" s="350"/>
+      <c r="E2" s="350"/>
+      <c r="F2" s="350"/>
+      <c r="G2" s="350"/>
+      <c r="H2" s="351"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="351" t="s">
+      <c r="A3" s="352" t="s">
         <v>227</v>
       </c>
-      <c r="B3" s="352"/>
-      <c r="C3" s="353"/>
-      <c r="D3" s="354"/>
-      <c r="E3" s="351" t="s">
+      <c r="B3" s="353"/>
+      <c r="C3" s="354"/>
+      <c r="D3" s="355"/>
+      <c r="E3" s="352" t="s">
         <v>228</v>
       </c>
-      <c r="F3" s="352"/>
-      <c r="G3" s="353"/>
-      <c r="H3" s="354"/>
+      <c r="F3" s="353"/>
+      <c r="G3" s="354"/>
+      <c r="H3" s="355"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="15">
@@ -17409,28 +17442,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="355" t="s">
+      <c r="A1" s="368" t="s">
         <v>955</v>
       </c>
-      <c r="B1" s="356"/>
-      <c r="C1" s="356"/>
-      <c r="D1" s="356"/>
-      <c r="E1" s="356"/>
-      <c r="F1" s="357"/>
+      <c r="B1" s="369"/>
+      <c r="C1" s="369"/>
+      <c r="D1" s="369"/>
+      <c r="E1" s="369"/>
+      <c r="F1" s="370"/>
       <c r="G1" s="199"/>
       <c r="H1" s="199"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="358" t="s">
+      <c r="A2" s="371" t="s">
         <v>843</v>
       </c>
-      <c r="B2" s="359"/>
-      <c r="C2" s="360"/>
-      <c r="D2" s="358" t="s">
+      <c r="B2" s="372"/>
+      <c r="C2" s="373"/>
+      <c r="D2" s="371" t="s">
         <v>844</v>
       </c>
-      <c r="E2" s="359"/>
-      <c r="F2" s="360"/>
+      <c r="E2" s="372"/>
+      <c r="F2" s="373"/>
       <c r="G2" s="199"/>
       <c r="H2" s="199"/>
     </row>
@@ -17454,7 +17487,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="199"/>
-      <c r="H3" s="361" t="s">
+      <c r="H3" s="365" t="s">
         <v>847</v>
       </c>
     </row>
@@ -17478,7 +17511,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="199"/>
-      <c r="H4" s="362"/>
+      <c r="H4" s="366"/>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A5" s="200">
@@ -17500,7 +17533,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="199"/>
-      <c r="H5" s="362"/>
+      <c r="H5" s="366"/>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A6" s="203">
@@ -17522,7 +17555,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="199"/>
-      <c r="H6" s="362"/>
+      <c r="H6" s="366"/>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A7" s="203">
@@ -17544,7 +17577,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="199"/>
-      <c r="H7" s="362"/>
+      <c r="H7" s="366"/>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A8" s="206">
@@ -17566,7 +17599,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="199"/>
-      <c r="H8" s="362"/>
+      <c r="H8" s="366"/>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A9" s="206">
@@ -17588,7 +17621,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="199"/>
-      <c r="H9" s="362"/>
+      <c r="H9" s="366"/>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A10" s="209">
@@ -17610,7 +17643,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="199"/>
-      <c r="H10" s="363"/>
+      <c r="H10" s="367"/>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="212">
@@ -17632,7 +17665,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="199"/>
-      <c r="H11" s="364" t="s">
+      <c r="H11" s="356" t="s">
         <v>859</v>
       </c>
     </row>
@@ -17656,7 +17689,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="199"/>
-      <c r="H12" s="365"/>
+      <c r="H12" s="357"/>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A13" s="215">
@@ -17678,7 +17711,7 @@
         <v>11</v>
       </c>
       <c r="G13" s="199"/>
-      <c r="H13" s="365"/>
+      <c r="H13" s="357"/>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A14" s="215">
@@ -17700,7 +17733,7 @@
         <v>12</v>
       </c>
       <c r="G14" s="199"/>
-      <c r="H14" s="365"/>
+      <c r="H14" s="357"/>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A15" s="219">
@@ -17722,7 +17755,7 @@
         <v>13</v>
       </c>
       <c r="G15" s="199"/>
-      <c r="H15" s="365"/>
+      <c r="H15" s="357"/>
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A16" s="219">
@@ -17744,7 +17777,7 @@
         <v>14</v>
       </c>
       <c r="G16" s="199"/>
-      <c r="H16" s="365"/>
+      <c r="H16" s="357"/>
     </row>
     <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A17" s="219">
@@ -17766,7 +17799,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="199"/>
-      <c r="H17" s="365"/>
+      <c r="H17" s="357"/>
     </row>
     <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A18" s="219">
@@ -17788,7 +17821,7 @@
         <v>16</v>
       </c>
       <c r="G18" s="199"/>
-      <c r="H18" s="365"/>
+      <c r="H18" s="357"/>
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A19" s="219">
@@ -17810,7 +17843,7 @@
         <v>17</v>
       </c>
       <c r="G19" s="199"/>
-      <c r="H19" s="365"/>
+      <c r="H19" s="357"/>
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A20" s="222">
@@ -17832,7 +17865,7 @@
         <v>18</v>
       </c>
       <c r="G20" s="199"/>
-      <c r="H20" s="365"/>
+      <c r="H20" s="357"/>
     </row>
     <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A21" s="222">
@@ -17854,7 +17887,7 @@
         <v>19</v>
       </c>
       <c r="G21" s="199"/>
-      <c r="H21" s="365"/>
+      <c r="H21" s="357"/>
     </row>
     <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A22" s="225">
@@ -17876,7 +17909,7 @@
         <v>20</v>
       </c>
       <c r="G22" s="199"/>
-      <c r="H22" s="366"/>
+      <c r="H22" s="358"/>
     </row>
     <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1"/>
@@ -17894,28 +17927,28 @@
     <row r="36" spans="1:8" ht="20.100000000000001" customHeight="1"/>
     <row r="37" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1"/>
     <row r="38" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A38" s="367" t="s">
+      <c r="A38" s="359" t="s">
         <v>956</v>
       </c>
-      <c r="B38" s="368"/>
-      <c r="C38" s="368"/>
-      <c r="D38" s="368"/>
-      <c r="E38" s="368"/>
-      <c r="F38" s="369"/>
+      <c r="B38" s="360"/>
+      <c r="C38" s="360"/>
+      <c r="D38" s="360"/>
+      <c r="E38" s="360"/>
+      <c r="F38" s="361"/>
       <c r="G38" s="199"/>
       <c r="H38" s="199"/>
     </row>
     <row r="39" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A39" s="370" t="s">
+      <c r="A39" s="362" t="s">
         <v>843</v>
       </c>
-      <c r="B39" s="371"/>
-      <c r="C39" s="372"/>
-      <c r="D39" s="370" t="s">
+      <c r="B39" s="363"/>
+      <c r="C39" s="364"/>
+      <c r="D39" s="362" t="s">
         <v>844</v>
       </c>
-      <c r="E39" s="371"/>
-      <c r="F39" s="372"/>
+      <c r="E39" s="363"/>
+      <c r="F39" s="364"/>
       <c r="G39" s="199"/>
       <c r="H39" s="199"/>
     </row>
@@ -17939,7 +17972,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="199"/>
-      <c r="H40" s="361" t="s">
+      <c r="H40" s="365" t="s">
         <v>847</v>
       </c>
     </row>
@@ -17963,7 +17996,7 @@
         <v>2</v>
       </c>
       <c r="G41" s="199"/>
-      <c r="H41" s="362"/>
+      <c r="H41" s="366"/>
     </row>
     <row r="42" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A42" s="228">
@@ -17985,7 +18018,7 @@
         <v>3</v>
       </c>
       <c r="G42" s="199"/>
-      <c r="H42" s="362"/>
+      <c r="H42" s="366"/>
     </row>
     <row r="43" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A43" s="230">
@@ -18007,7 +18040,7 @@
         <v>4</v>
       </c>
       <c r="G43" s="199"/>
-      <c r="H43" s="362"/>
+      <c r="H43" s="366"/>
     </row>
     <row r="44" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A44" s="230">
@@ -18029,7 +18062,7 @@
         <v>5</v>
       </c>
       <c r="G44" s="199"/>
-      <c r="H44" s="362"/>
+      <c r="H44" s="366"/>
     </row>
     <row r="45" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A45" s="232">
@@ -18051,7 +18084,7 @@
         <v>6</v>
       </c>
       <c r="G45" s="199"/>
-      <c r="H45" s="362"/>
+      <c r="H45" s="366"/>
     </row>
     <row r="46" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A46" s="232">
@@ -18073,7 +18106,7 @@
         <v>7</v>
       </c>
       <c r="G46" s="199"/>
-      <c r="H46" s="362"/>
+      <c r="H46" s="366"/>
     </row>
     <row r="47" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A47" s="234">
@@ -18095,7 +18128,7 @@
         <v>8</v>
       </c>
       <c r="G47" s="199"/>
-      <c r="H47" s="363"/>
+      <c r="H47" s="367"/>
     </row>
     <row r="48" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="A48" s="237">
@@ -18117,7 +18150,7 @@
         <v>9</v>
       </c>
       <c r="G48" s="199"/>
-      <c r="H48" s="364" t="s">
+      <c r="H48" s="356" t="s">
         <v>859</v>
       </c>
     </row>
@@ -18141,7 +18174,7 @@
         <v>10</v>
       </c>
       <c r="G49" s="199"/>
-      <c r="H49" s="365"/>
+      <c r="H49" s="357"/>
     </row>
     <row r="50" spans="1:8" ht="16.5" thickBot="1">
       <c r="A50" s="239">
@@ -18163,7 +18196,7 @@
         <v>11</v>
       </c>
       <c r="G50" s="199"/>
-      <c r="H50" s="365"/>
+      <c r="H50" s="357"/>
     </row>
     <row r="51" spans="1:8" ht="16.5" thickBot="1">
       <c r="A51" s="242">
@@ -18185,7 +18218,7 @@
         <v>12</v>
       </c>
       <c r="G51" s="199"/>
-      <c r="H51" s="365"/>
+      <c r="H51" s="357"/>
     </row>
     <row r="52" spans="1:8" ht="16.5" thickBot="1">
       <c r="A52" s="242">
@@ -18207,7 +18240,7 @@
         <v>13</v>
       </c>
       <c r="G52" s="199"/>
-      <c r="H52" s="365"/>
+      <c r="H52" s="357"/>
     </row>
     <row r="53" spans="1:8" ht="16.5" thickBot="1">
       <c r="A53" s="242">
@@ -18229,7 +18262,7 @@
         <v>14</v>
       </c>
       <c r="G53" s="199"/>
-      <c r="H53" s="365"/>
+      <c r="H53" s="357"/>
     </row>
     <row r="54" spans="1:8" ht="16.5" thickBot="1">
       <c r="A54" s="242">
@@ -18251,7 +18284,7 @@
         <v>15</v>
       </c>
       <c r="G54" s="199"/>
-      <c r="H54" s="365"/>
+      <c r="H54" s="357"/>
     </row>
     <row r="55" spans="1:8" ht="16.5" thickBot="1">
       <c r="A55" s="242">
@@ -18273,7 +18306,7 @@
         <v>16</v>
       </c>
       <c r="G55" s="199"/>
-      <c r="H55" s="365"/>
+      <c r="H55" s="357"/>
     </row>
     <row r="56" spans="1:8" ht="16.5" thickBot="1">
       <c r="A56" s="242">
@@ -18295,7 +18328,7 @@
         <v>17</v>
       </c>
       <c r="G56" s="199"/>
-      <c r="H56" s="365"/>
+      <c r="H56" s="357"/>
     </row>
     <row r="57" spans="1:8" ht="16.5" thickBot="1">
       <c r="A57" s="244">
@@ -18317,7 +18350,7 @@
         <v>18</v>
       </c>
       <c r="G57" s="199"/>
-      <c r="H57" s="365"/>
+      <c r="H57" s="357"/>
     </row>
     <row r="58" spans="1:8" ht="16.5" thickBot="1">
       <c r="A58" s="244">
@@ -18339,7 +18372,7 @@
         <v>19</v>
       </c>
       <c r="G58" s="199"/>
-      <c r="H58" s="365"/>
+      <c r="H58" s="357"/>
     </row>
     <row r="59" spans="1:8" ht="16.5" thickBot="1">
       <c r="A59" s="246">
@@ -18361,21 +18394,21 @@
         <v>20</v>
       </c>
       <c r="G59" s="199"/>
-      <c r="H59" s="366"/>
+      <c r="H59" s="358"/>
     </row>
     <row r="60" spans="1:8" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="H3:H10"/>
+    <mergeCell ref="H11:H22"/>
     <mergeCell ref="H48:H59"/>
     <mergeCell ref="A38:F38"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="D39:F39"/>
     <mergeCell ref="H40:H47"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="H3:H10"/>
-    <mergeCell ref="H11:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -18404,40 +18437,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="379" t="s">
+      <c r="A1" s="380" t="s">
         <v>330</v>
       </c>
-      <c r="B1" s="380"/>
-      <c r="C1" s="380"/>
-      <c r="D1" s="380"/>
-      <c r="E1" s="380"/>
-      <c r="F1" s="380"/>
-      <c r="G1" s="380"/>
-      <c r="H1" s="381"/>
+      <c r="B1" s="381"/>
+      <c r="C1" s="381"/>
+      <c r="D1" s="381"/>
+      <c r="E1" s="381"/>
+      <c r="F1" s="381"/>
+      <c r="G1" s="381"/>
+      <c r="H1" s="382"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="382"/>
-      <c r="B2" s="383"/>
-      <c r="C2" s="383"/>
-      <c r="D2" s="383"/>
-      <c r="E2" s="383"/>
-      <c r="F2" s="383"/>
-      <c r="G2" s="383"/>
-      <c r="H2" s="384"/>
+      <c r="A2" s="383"/>
+      <c r="B2" s="384"/>
+      <c r="C2" s="384"/>
+      <c r="D2" s="384"/>
+      <c r="E2" s="384"/>
+      <c r="F2" s="384"/>
+      <c r="G2" s="384"/>
+      <c r="H2" s="385"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="373" t="s">
+      <c r="A3" s="374" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="374"/>
-      <c r="C3" s="374"/>
-      <c r="D3" s="375"/>
-      <c r="E3" s="373" t="s">
+      <c r="B3" s="375"/>
+      <c r="C3" s="375"/>
+      <c r="D3" s="376"/>
+      <c r="E3" s="374" t="s">
         <v>316</v>
       </c>
-      <c r="F3" s="374"/>
-      <c r="G3" s="374"/>
-      <c r="H3" s="375"/>
+      <c r="F3" s="375"/>
+      <c r="G3" s="375"/>
+      <c r="H3" s="376"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="91">
@@ -18654,18 +18687,18 @@
       <c r="H21" s="83"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="376" t="s">
+      <c r="A22" s="377" t="s">
         <v>317</v>
       </c>
-      <c r="B22" s="377"/>
-      <c r="C22" s="377"/>
-      <c r="D22" s="378"/>
-      <c r="E22" s="376" t="s">
+      <c r="B22" s="378"/>
+      <c r="C22" s="378"/>
+      <c r="D22" s="379"/>
+      <c r="E22" s="377" t="s">
         <v>318</v>
       </c>
-      <c r="F22" s="377"/>
-      <c r="G22" s="377"/>
-      <c r="H22" s="378"/>
+      <c r="F22" s="378"/>
+      <c r="G22" s="378"/>
+      <c r="H22" s="379"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="76">
@@ -18942,40 +18975,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="326" t="s">
+      <c r="A1" s="323" t="s">
         <v>491</v>
       </c>
-      <c r="B1" s="327"/>
-      <c r="C1" s="327"/>
-      <c r="D1" s="327"/>
-      <c r="E1" s="327"/>
-      <c r="F1" s="327"/>
-      <c r="G1" s="327"/>
-      <c r="H1" s="328"/>
+      <c r="B1" s="324"/>
+      <c r="C1" s="324"/>
+      <c r="D1" s="324"/>
+      <c r="E1" s="324"/>
+      <c r="F1" s="324"/>
+      <c r="G1" s="324"/>
+      <c r="H1" s="325"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="329"/>
-      <c r="B2" s="330"/>
-      <c r="C2" s="330"/>
-      <c r="D2" s="330"/>
-      <c r="E2" s="330"/>
-      <c r="F2" s="330"/>
-      <c r="G2" s="330"/>
-      <c r="H2" s="331"/>
+      <c r="A2" s="326"/>
+      <c r="B2" s="327"/>
+      <c r="C2" s="327"/>
+      <c r="D2" s="327"/>
+      <c r="E2" s="327"/>
+      <c r="F2" s="327"/>
+      <c r="G2" s="327"/>
+      <c r="H2" s="328"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="332" t="s">
+      <c r="A3" s="329" t="s">
         <v>321</v>
       </c>
-      <c r="B3" s="333"/>
-      <c r="C3" s="333"/>
-      <c r="D3" s="333"/>
-      <c r="E3" s="333" t="s">
+      <c r="B3" s="330"/>
+      <c r="C3" s="330"/>
+      <c r="D3" s="330"/>
+      <c r="E3" s="330" t="s">
         <v>320</v>
       </c>
-      <c r="F3" s="333"/>
-      <c r="G3" s="333"/>
-      <c r="H3" s="334"/>
+      <c r="F3" s="330"/>
+      <c r="G3" s="330"/>
+      <c r="H3" s="331"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="19">

</xml_diff>

<commit_message>
chg: Added A-10, AH-64 and OH-58 to FOB Jokkmokk roadbase. Added ATIS information for Jokkmokk.
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2215" uniqueCount="1316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2239" uniqueCount="1337">
   <si>
     <t>AWACS</t>
   </si>
@@ -3972,6 +3972,69 @@
   </si>
   <si>
     <t>149.75</t>
+  </si>
+  <si>
+    <t>UZI</t>
+  </si>
+  <si>
+    <t>UI51</t>
+  </si>
+  <si>
+    <t>UI52</t>
+  </si>
+  <si>
+    <t>UI53</t>
+  </si>
+  <si>
+    <t>UI54</t>
+  </si>
+  <si>
+    <t>0151</t>
+  </si>
+  <si>
+    <t>0152</t>
+  </si>
+  <si>
+    <t>0153</t>
+  </si>
+  <si>
+    <t>0154</t>
+  </si>
+  <si>
+    <t>SPRINGFIELD</t>
+  </si>
+  <si>
+    <t>SD61</t>
+  </si>
+  <si>
+    <t>SD62</t>
+  </si>
+  <si>
+    <t>SD63</t>
+  </si>
+  <si>
+    <t>SD64</t>
+  </si>
+  <si>
+    <t>0161</t>
+  </si>
+  <si>
+    <t>0162</t>
+  </si>
+  <si>
+    <t>0163</t>
+  </si>
+  <si>
+    <t>0164</t>
+  </si>
+  <si>
+    <t>Sioux</t>
+  </si>
+  <si>
+    <t>WRATH</t>
+  </si>
+  <si>
+    <t>JOKKMOKK</t>
   </si>
 </sst>
 </file>
@@ -5904,7 +5967,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="426">
+  <cellXfs count="427">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6624,12 +6687,21 @@
     <xf numFmtId="49" fontId="47" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6639,13 +6711,49 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6657,50 +6765,35 @@
     <xf numFmtId="0" fontId="25" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6711,36 +6804,6 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6828,6 +6891,42 @@
     <xf numFmtId="49" fontId="45" fillId="31" borderId="93" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="26" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="26" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="26" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6846,42 +6945,6 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="26" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="26" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="26" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6954,6 +7017,57 @@
     <xf numFmtId="0" fontId="32" fillId="20" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6972,57 +7086,7 @@
     <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7335,7 +7399,7 @@
   <sheetPr codeName="Ark1"/>
   <dimension ref="A1:AP83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N70" sqref="N70"/>
     </sheetView>
   </sheetViews>
@@ -7443,13 +7507,13 @@
       <c r="N2" s="107" t="s">
         <v>330</v>
       </c>
-      <c r="V2" s="294" t="s">
+      <c r="V2" s="293" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="294"/>
-      <c r="X2" s="294"/>
-      <c r="Y2" s="294"/>
-      <c r="Z2" s="294"/>
+      <c r="W2" s="293"/>
+      <c r="X2" s="293"/>
+      <c r="Y2" s="293"/>
+      <c r="Z2" s="293"/>
     </row>
     <row r="3" spans="1:42">
       <c r="A3" s="107" t="s">
@@ -7498,9 +7562,9 @@
       <c r="P3" t="s">
         <v>426</v>
       </c>
-      <c r="R3" s="293"/>
-      <c r="S3" s="293"/>
-      <c r="T3" s="293"/>
+      <c r="R3" s="297"/>
+      <c r="S3" s="297"/>
+      <c r="T3" s="297"/>
       <c r="V3" s="101" t="s">
         <v>328</v>
       </c>
@@ -7582,22 +7646,22 @@
       <c r="AA4" s="23"/>
       <c r="AB4" s="23"/>
       <c r="AC4" s="23"/>
-      <c r="AD4" s="294" t="s">
+      <c r="AD4" s="293" t="s">
         <v>429</v>
       </c>
-      <c r="AE4" s="294"/>
-      <c r="AF4" s="294"/>
-      <c r="AG4" s="294"/>
-      <c r="AH4" s="294"/>
-      <c r="AJ4" s="294" t="s">
+      <c r="AE4" s="293"/>
+      <c r="AF4" s="293"/>
+      <c r="AG4" s="293"/>
+      <c r="AH4" s="293"/>
+      <c r="AJ4" s="293" t="s">
         <v>1</v>
       </c>
-      <c r="AK4" s="294"/>
-      <c r="AL4" s="294"/>
-      <c r="AM4" s="294"/>
-      <c r="AN4" s="294"/>
-      <c r="AO4" s="294"/>
-      <c r="AP4" s="294"/>
+      <c r="AK4" s="293"/>
+      <c r="AL4" s="293"/>
+      <c r="AM4" s="293"/>
+      <c r="AN4" s="293"/>
+      <c r="AO4" s="293"/>
+      <c r="AP4" s="293"/>
     </row>
     <row r="5" spans="1:42" ht="15.75">
       <c r="A5" s="107" t="s">
@@ -8813,15 +8877,15 @@
       <c r="AH18" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="AJ18" s="294" t="s">
+      <c r="AJ18" s="293" t="s">
         <v>274</v>
       </c>
-      <c r="AK18" s="294"/>
-      <c r="AL18" s="294"/>
-      <c r="AM18" s="294"/>
-      <c r="AN18" s="294"/>
-      <c r="AO18" s="294"/>
-      <c r="AP18" s="294"/>
+      <c r="AK18" s="293"/>
+      <c r="AL18" s="293"/>
+      <c r="AM18" s="293"/>
+      <c r="AN18" s="293"/>
+      <c r="AO18" s="293"/>
+      <c r="AP18" s="293"/>
     </row>
     <row r="19" spans="1:42" ht="15.75">
       <c r="A19" s="107" t="s">
@@ -8954,9 +9018,9 @@
       </c>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="293"/>
-      <c r="S20" s="293"/>
-      <c r="T20" s="293"/>
+      <c r="R20" s="297"/>
+      <c r="S20" s="297"/>
+      <c r="T20" s="297"/>
       <c r="U20" s="2"/>
       <c r="V20" s="272" t="s">
         <v>1253</v>
@@ -9371,13 +9435,13 @@
       <c r="S25" s="24"/>
       <c r="T25" s="24"/>
       <c r="X25" s="2"/>
-      <c r="AD25" s="294" t="s">
+      <c r="AD25" s="293" t="s">
         <v>486</v>
       </c>
-      <c r="AE25" s="294"/>
-      <c r="AF25" s="294"/>
-      <c r="AG25" s="294"/>
-      <c r="AH25" s="294"/>
+      <c r="AE25" s="293"/>
+      <c r="AF25" s="293"/>
+      <c r="AG25" s="293"/>
+      <c r="AH25" s="293"/>
       <c r="AJ25" s="116" t="s">
         <v>555</v>
       </c>
@@ -9627,15 +9691,15 @@
       <c r="N29" s="107" t="s">
         <v>355</v>
       </c>
-      <c r="V29" s="294" t="s">
+      <c r="V29" s="293" t="s">
         <v>212</v>
       </c>
-      <c r="W29" s="294"/>
-      <c r="X29" s="294"/>
-      <c r="Y29" s="294"/>
-      <c r="Z29" s="294"/>
-      <c r="AA29" s="294"/>
-      <c r="AB29" s="294"/>
+      <c r="W29" s="293"/>
+      <c r="X29" s="293"/>
+      <c r="Y29" s="293"/>
+      <c r="Z29" s="293"/>
+      <c r="AA29" s="293"/>
+      <c r="AB29" s="293"/>
     </row>
     <row r="30" spans="1:42">
       <c r="A30" s="107"/>
@@ -9691,15 +9755,15 @@
       </c>
       <c r="AA30" s="29"/>
       <c r="AB30" s="29"/>
-      <c r="AJ30" s="294" t="s">
+      <c r="AJ30" s="293" t="s">
         <v>831</v>
       </c>
-      <c r="AK30" s="294"/>
-      <c r="AL30" s="294"/>
-      <c r="AM30" s="294"/>
-      <c r="AN30" s="294"/>
-      <c r="AO30" s="294"/>
-      <c r="AP30" s="294"/>
+      <c r="AK30" s="293"/>
+      <c r="AL30" s="293"/>
+      <c r="AM30" s="293"/>
+      <c r="AN30" s="293"/>
+      <c r="AO30" s="293"/>
+      <c r="AP30" s="293"/>
     </row>
     <row r="31" spans="1:42">
       <c r="B31" s="24"/>
@@ -9786,15 +9850,15 @@
       <c r="AJ34" s="23"/>
     </row>
     <row r="37" spans="22:36">
-      <c r="V37" s="294" t="s">
+      <c r="V37" s="293" t="s">
         <v>9</v>
       </c>
-      <c r="W37" s="294"/>
-      <c r="X37" s="294"/>
-      <c r="Y37" s="294"/>
-      <c r="Z37" s="294"/>
-      <c r="AA37" s="294"/>
-      <c r="AB37" s="294"/>
+      <c r="W37" s="293"/>
+      <c r="X37" s="293"/>
+      <c r="Y37" s="293"/>
+      <c r="Z37" s="293"/>
+      <c r="AA37" s="293"/>
+      <c r="AB37" s="293"/>
     </row>
     <row r="38" spans="22:36">
       <c r="V38" s="29" t="s">
@@ -9814,11 +9878,11 @@
       </c>
       <c r="AA38" s="29"/>
       <c r="AB38" s="29"/>
-      <c r="AD38" s="295" t="s">
+      <c r="AD38" s="298" t="s">
         <v>260</v>
       </c>
-      <c r="AE38" s="296"/>
-      <c r="AF38" s="297"/>
+      <c r="AE38" s="299"/>
+      <c r="AF38" s="300"/>
     </row>
     <row r="39" spans="22:36">
       <c r="V39" s="3" t="s">
@@ -9855,15 +9919,15 @@
       <c r="AF41" s="3"/>
     </row>
     <row r="42" spans="22:36">
-      <c r="V42" s="294" t="s">
+      <c r="V42" s="293" t="s">
         <v>244</v>
       </c>
-      <c r="W42" s="294"/>
-      <c r="X42" s="294"/>
-      <c r="Y42" s="294"/>
-      <c r="Z42" s="294"/>
-      <c r="AA42" s="294"/>
-      <c r="AB42" s="294"/>
+      <c r="W42" s="293"/>
+      <c r="X42" s="293"/>
+      <c r="Y42" s="293"/>
+      <c r="Z42" s="293"/>
+      <c r="AA42" s="293"/>
+      <c r="AB42" s="293"/>
       <c r="AD42" s="3" t="s">
         <v>254</v>
       </c>
@@ -9933,15 +9997,15 @@
       <c r="AF47" s="3"/>
     </row>
     <row r="48" spans="22:36">
-      <c r="V48" s="298" t="s">
+      <c r="V48" s="294" t="s">
         <v>473</v>
       </c>
-      <c r="W48" s="299"/>
-      <c r="X48" s="299"/>
-      <c r="Y48" s="299"/>
-      <c r="Z48" s="299"/>
-      <c r="AA48" s="299"/>
-      <c r="AB48" s="300"/>
+      <c r="W48" s="295"/>
+      <c r="X48" s="295"/>
+      <c r="Y48" s="295"/>
+      <c r="Z48" s="295"/>
+      <c r="AA48" s="295"/>
+      <c r="AB48" s="296"/>
       <c r="AD48" s="3" t="s">
         <v>261</v>
       </c>
@@ -10551,11 +10615,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="V42:AB42"/>
-    <mergeCell ref="AD4:AH4"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="V48:AB48"/>
-    <mergeCell ref="V37:AB37"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="AJ4:AP4"/>
@@ -10564,6 +10623,11 @@
     <mergeCell ref="V29:AB29"/>
     <mergeCell ref="AD25:AH25"/>
     <mergeCell ref="AJ30:AP30"/>
+    <mergeCell ref="V42:AB42"/>
+    <mergeCell ref="AD4:AH4"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="V48:AB48"/>
+    <mergeCell ref="V37:AB37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11523,40 +11587,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="420" t="s">
+      <c r="A1" s="403" t="s">
         <v>326</v>
       </c>
-      <c r="B1" s="420"/>
-      <c r="C1" s="420"/>
-      <c r="D1" s="420"/>
-      <c r="E1" s="420"/>
-      <c r="F1" s="420"/>
-      <c r="G1" s="420"/>
-      <c r="H1" s="420"/>
+      <c r="B1" s="403"/>
+      <c r="C1" s="403"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
+      <c r="G1" s="403"/>
+      <c r="H1" s="403"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="421"/>
-      <c r="B2" s="421"/>
-      <c r="C2" s="421"/>
-      <c r="D2" s="421"/>
-      <c r="E2" s="421"/>
-      <c r="F2" s="421"/>
-      <c r="G2" s="421"/>
-      <c r="H2" s="421"/>
+      <c r="A2" s="404"/>
+      <c r="B2" s="404"/>
+      <c r="C2" s="404"/>
+      <c r="D2" s="404"/>
+      <c r="E2" s="404"/>
+      <c r="F2" s="404"/>
+      <c r="G2" s="404"/>
+      <c r="H2" s="404"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="422" t="s">
+      <c r="A3" s="405" t="s">
         <v>227</v>
       </c>
-      <c r="B3" s="423"/>
-      <c r="C3" s="424"/>
-      <c r="D3" s="425"/>
-      <c r="E3" s="422" t="s">
+      <c r="B3" s="406"/>
+      <c r="C3" s="407"/>
+      <c r="D3" s="408"/>
+      <c r="E3" s="405" t="s">
         <v>228</v>
       </c>
-      <c r="F3" s="423"/>
-      <c r="G3" s="424"/>
-      <c r="H3" s="425"/>
+      <c r="F3" s="406"/>
+      <c r="G3" s="407"/>
+      <c r="H3" s="408"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="31">
@@ -11849,18 +11913,18 @@
       <c r="H24" s="59"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="422" t="s">
+      <c r="A25" s="405" t="s">
         <v>289</v>
       </c>
-      <c r="B25" s="423"/>
-      <c r="C25" s="424"/>
-      <c r="D25" s="425"/>
-      <c r="E25" s="422" t="s">
+      <c r="B25" s="406"/>
+      <c r="C25" s="407"/>
+      <c r="D25" s="408"/>
+      <c r="E25" s="405" t="s">
         <v>290</v>
       </c>
-      <c r="F25" s="423"/>
-      <c r="G25" s="424"/>
-      <c r="H25" s="425"/>
+      <c r="F25" s="406"/>
+      <c r="G25" s="407"/>
+      <c r="H25" s="408"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="35" t="s">
@@ -11872,23 +11936,23 @@
       <c r="E26" s="31" t="s">
         <v>292</v>
       </c>
-      <c r="F26" s="417"/>
-      <c r="G26" s="418"/>
-      <c r="H26" s="419"/>
+      <c r="F26" s="412"/>
+      <c r="G26" s="413"/>
+      <c r="H26" s="414"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="B27" s="412"/>
-      <c r="C27" s="413"/>
-      <c r="D27" s="415"/>
+      <c r="B27" s="415"/>
+      <c r="C27" s="416"/>
+      <c r="D27" s="417"/>
       <c r="E27" s="35" t="s">
         <v>294</v>
       </c>
       <c r="F27" s="409"/>
       <c r="G27" s="410"/>
-      <c r="H27" s="416"/>
+      <c r="H27" s="418"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="35" t="s">
@@ -11900,23 +11964,23 @@
       <c r="E28" s="43" t="s">
         <v>296</v>
       </c>
-      <c r="F28" s="412"/>
-      <c r="G28" s="413"/>
-      <c r="H28" s="414"/>
+      <c r="F28" s="415"/>
+      <c r="G28" s="416"/>
+      <c r="H28" s="419"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="43" t="s">
         <v>297</v>
       </c>
-      <c r="B29" s="412"/>
-      <c r="C29" s="413"/>
-      <c r="D29" s="415"/>
+      <c r="B29" s="415"/>
+      <c r="C29" s="416"/>
+      <c r="D29" s="417"/>
       <c r="E29" s="35" t="s">
         <v>298</v>
       </c>
       <c r="F29" s="409"/>
       <c r="G29" s="410"/>
-      <c r="H29" s="416"/>
+      <c r="H29" s="418"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="35" t="s">
@@ -11928,23 +11992,23 @@
       <c r="E30" s="43" t="s">
         <v>300</v>
       </c>
-      <c r="F30" s="412"/>
-      <c r="G30" s="413"/>
-      <c r="H30" s="414"/>
+      <c r="F30" s="415"/>
+      <c r="G30" s="416"/>
+      <c r="H30" s="419"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="43" t="s">
         <v>301</v>
       </c>
-      <c r="B31" s="412"/>
-      <c r="C31" s="413"/>
-      <c r="D31" s="415"/>
+      <c r="B31" s="415"/>
+      <c r="C31" s="416"/>
+      <c r="D31" s="417"/>
       <c r="E31" s="35" t="s">
         <v>302</v>
       </c>
       <c r="F31" s="409"/>
       <c r="G31" s="410"/>
-      <c r="H31" s="416"/>
+      <c r="H31" s="418"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="35" t="s">
@@ -11954,9 +12018,9 @@
       <c r="C32" s="410"/>
       <c r="D32" s="411"/>
       <c r="E32" s="43"/>
-      <c r="F32" s="412"/>
-      <c r="G32" s="413"/>
-      <c r="H32" s="414" t="s">
+      <c r="F32" s="415"/>
+      <c r="G32" s="416"/>
+      <c r="H32" s="419" t="s">
         <v>242</v>
       </c>
     </row>
@@ -11964,13 +12028,13 @@
       <c r="A33" s="43" t="s">
         <v>304</v>
       </c>
-      <c r="B33" s="412"/>
-      <c r="C33" s="413"/>
-      <c r="D33" s="415"/>
+      <c r="B33" s="415"/>
+      <c r="C33" s="416"/>
+      <c r="D33" s="417"/>
       <c r="E33" s="35"/>
       <c r="F33" s="409"/>
       <c r="G33" s="410"/>
-      <c r="H33" s="416" t="s">
+      <c r="H33" s="418" t="s">
         <v>284</v>
       </c>
     </row>
@@ -11982,9 +12046,9 @@
       <c r="C34" s="410"/>
       <c r="D34" s="411"/>
       <c r="E34" s="43"/>
-      <c r="F34" s="412"/>
-      <c r="G34" s="413"/>
-      <c r="H34" s="414" t="s">
+      <c r="F34" s="415"/>
+      <c r="G34" s="416"/>
+      <c r="H34" s="419" t="s">
         <v>285</v>
       </c>
     </row>
@@ -11992,13 +12056,13 @@
       <c r="A35" s="43" t="s">
         <v>306</v>
       </c>
-      <c r="B35" s="412"/>
-      <c r="C35" s="413"/>
-      <c r="D35" s="415"/>
+      <c r="B35" s="415"/>
+      <c r="C35" s="416"/>
+      <c r="D35" s="417"/>
       <c r="E35" s="35"/>
       <c r="F35" s="409"/>
       <c r="G35" s="410"/>
-      <c r="H35" s="416" t="s">
+      <c r="H35" s="418" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12010,9 +12074,9 @@
       <c r="C36" s="410"/>
       <c r="D36" s="411"/>
       <c r="E36" s="43"/>
-      <c r="F36" s="412"/>
-      <c r="G36" s="413"/>
-      <c r="H36" s="414" t="s">
+      <c r="F36" s="415"/>
+      <c r="G36" s="416"/>
+      <c r="H36" s="419" t="s">
         <v>287</v>
       </c>
     </row>
@@ -12020,13 +12084,13 @@
       <c r="A37" s="43" t="s">
         <v>308</v>
       </c>
-      <c r="B37" s="412"/>
-      <c r="C37" s="413"/>
-      <c r="D37" s="415"/>
+      <c r="B37" s="415"/>
+      <c r="C37" s="416"/>
+      <c r="D37" s="417"/>
       <c r="E37" s="35"/>
       <c r="F37" s="409"/>
       <c r="G37" s="410"/>
-      <c r="H37" s="416" t="s">
+      <c r="H37" s="418" t="s">
         <v>288</v>
       </c>
     </row>
@@ -12038,9 +12102,9 @@
       <c r="C38" s="410"/>
       <c r="D38" s="411"/>
       <c r="E38" s="43"/>
-      <c r="F38" s="412"/>
-      <c r="G38" s="413"/>
-      <c r="H38" s="414" t="s">
+      <c r="F38" s="415"/>
+      <c r="G38" s="416"/>
+      <c r="H38" s="419" t="s">
         <v>241</v>
       </c>
     </row>
@@ -12048,13 +12112,13 @@
       <c r="A39" s="43" t="s">
         <v>310</v>
       </c>
-      <c r="B39" s="412"/>
-      <c r="C39" s="413"/>
-      <c r="D39" s="415"/>
+      <c r="B39" s="415"/>
+      <c r="C39" s="416"/>
+      <c r="D39" s="417"/>
       <c r="E39" s="35"/>
       <c r="F39" s="409"/>
       <c r="G39" s="410"/>
-      <c r="H39" s="416" t="s">
+      <c r="H39" s="418" t="s">
         <v>242</v>
       </c>
     </row>
@@ -12066,53 +12130,24 @@
       <c r="C40" s="410"/>
       <c r="D40" s="411"/>
       <c r="E40" s="43"/>
-      <c r="F40" s="412"/>
-      <c r="G40" s="413"/>
-      <c r="H40" s="414"/>
+      <c r="F40" s="415"/>
+      <c r="G40" s="416"/>
+      <c r="H40" s="419"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="55" t="s">
         <v>312</v>
       </c>
-      <c r="B41" s="403"/>
-      <c r="C41" s="404"/>
-      <c r="D41" s="405"/>
+      <c r="B41" s="420"/>
+      <c r="C41" s="421"/>
+      <c r="D41" s="422"/>
       <c r="E41" s="60"/>
-      <c r="F41" s="406"/>
-      <c r="G41" s="407"/>
-      <c r="H41" s="408"/>
+      <c r="F41" s="423"/>
+      <c r="G41" s="424"/>
+      <c r="H41" s="425"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -12121,6 +12156,35 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12131,8 +12195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AP61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AB7" sqref="AB7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AL12" sqref="AL12:AN12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -12149,6 +12213,7 @@
     <col min="17" max="17" width="9.5703125" customWidth="1"/>
     <col min="18" max="18" width="11.85546875" customWidth="1"/>
     <col min="19" max="19" width="1.5703125" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" customWidth="1"/>
     <col min="25" max="25" width="1.5703125" customWidth="1"/>
     <col min="30" max="30" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="1.42578125" customWidth="1"/>
@@ -12175,55 +12240,55 @@
       </c>
     </row>
     <row r="2" spans="2:42">
-      <c r="B2" s="294" t="s">
+      <c r="B2" s="293" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="294"/>
-      <c r="D2" s="294"/>
-      <c r="E2" s="294"/>
-      <c r="F2" s="294"/>
-      <c r="H2" s="294" t="s">
+      <c r="C2" s="293"/>
+      <c r="D2" s="293"/>
+      <c r="E2" s="293"/>
+      <c r="F2" s="293"/>
+      <c r="H2" s="293" t="s">
         <v>1055</v>
       </c>
-      <c r="I2" s="294"/>
-      <c r="J2" s="294"/>
-      <c r="K2" s="294"/>
-      <c r="L2" s="294"/>
-      <c r="N2" s="294" t="s">
+      <c r="I2" s="293"/>
+      <c r="J2" s="293"/>
+      <c r="K2" s="293"/>
+      <c r="L2" s="293"/>
+      <c r="N2" s="293" t="s">
         <v>1054</v>
       </c>
-      <c r="O2" s="294"/>
-      <c r="P2" s="294"/>
-      <c r="Q2" s="294"/>
-      <c r="R2" s="294"/>
-      <c r="T2" s="294" t="s">
+      <c r="O2" s="293"/>
+      <c r="P2" s="293"/>
+      <c r="Q2" s="293"/>
+      <c r="R2" s="293"/>
+      <c r="T2" s="293" t="s">
         <v>236</v>
       </c>
-      <c r="U2" s="294"/>
-      <c r="V2" s="294"/>
-      <c r="W2" s="294"/>
-      <c r="X2" s="294"/>
-      <c r="Z2" s="294" t="s">
+      <c r="U2" s="293"/>
+      <c r="V2" s="293"/>
+      <c r="W2" s="293"/>
+      <c r="X2" s="293"/>
+      <c r="Z2" s="293" t="s">
         <v>246</v>
       </c>
-      <c r="AA2" s="294"/>
-      <c r="AB2" s="294"/>
-      <c r="AC2" s="294"/>
-      <c r="AD2" s="294"/>
-      <c r="AF2" s="294" t="s">
+      <c r="AA2" s="293"/>
+      <c r="AB2" s="293"/>
+      <c r="AC2" s="293"/>
+      <c r="AD2" s="293"/>
+      <c r="AF2" s="293" t="s">
         <v>317</v>
       </c>
-      <c r="AG2" s="294"/>
-      <c r="AH2" s="294"/>
-      <c r="AI2" s="294"/>
-      <c r="AJ2" s="294"/>
-      <c r="AL2" s="294" t="s">
+      <c r="AG2" s="293"/>
+      <c r="AH2" s="293"/>
+      <c r="AI2" s="293"/>
+      <c r="AJ2" s="293"/>
+      <c r="AL2" s="293" t="s">
         <v>491</v>
       </c>
-      <c r="AM2" s="294"/>
-      <c r="AN2" s="294"/>
-      <c r="AO2" s="294"/>
-      <c r="AP2" s="294"/>
+      <c r="AM2" s="293"/>
+      <c r="AN2" s="293"/>
+      <c r="AO2" s="293"/>
+      <c r="AP2" s="293"/>
     </row>
     <row r="3" spans="2:42">
       <c r="B3" s="101" t="s">
@@ -12396,18 +12461,19 @@
       <c r="Z4" t="s">
         <v>492</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AF4" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AG4" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="AH4">
+      <c r="AH4" s="3">
         <v>511</v>
       </c>
-      <c r="AI4">
+      <c r="AI4" s="3">
         <v>511</v>
       </c>
+      <c r="AJ4" s="3"/>
       <c r="AL4" s="3" t="s">
         <v>822</v>
       </c>
@@ -12465,6 +12531,11 @@
       <c r="X5" s="104" t="s">
         <v>1195</v>
       </c>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
       <c r="AL5" s="3"/>
       <c r="AM5" s="3"/>
       <c r="AN5" s="3">
@@ -12516,6 +12587,11 @@
       <c r="X6" s="104" t="s">
         <v>1196</v>
       </c>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
       <c r="AL6" s="3"/>
       <c r="AM6" s="3"/>
       <c r="AN6" s="3"/>
@@ -12565,6 +12641,11 @@
       <c r="X7" s="104" t="s">
         <v>1197</v>
       </c>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
       <c r="AL7" s="3"/>
       <c r="AM7" s="3"/>
       <c r="AN7" s="3"/>
@@ -12590,18 +12671,19 @@
       <c r="V8" s="246"/>
       <c r="W8" s="246"/>
       <c r="X8" s="246"/>
-      <c r="AF8" t="s">
+      <c r="AF8" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="AG8" t="s">
+      <c r="AG8" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="AH8">
+      <c r="AH8" s="3">
         <v>521</v>
       </c>
-      <c r="AI8">
+      <c r="AI8" s="3">
         <v>521</v>
       </c>
+      <c r="AJ8" s="3"/>
       <c r="AL8" s="3" t="s">
         <v>823</v>
       </c>
@@ -12673,6 +12755,11 @@
       <c r="X9" s="104" t="s">
         <v>1199</v>
       </c>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="3"/>
       <c r="AL9" s="3"/>
       <c r="AM9" s="3"/>
       <c r="AN9" s="3">
@@ -12726,6 +12813,11 @@
       <c r="X10" s="104" t="s">
         <v>1200</v>
       </c>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
       <c r="AL10" s="3"/>
       <c r="AM10" s="3"/>
       <c r="AN10" s="3"/>
@@ -12775,6 +12867,11 @@
       <c r="X11" s="104" t="s">
         <v>1201</v>
       </c>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="3"/>
+      <c r="AJ11" s="3"/>
       <c r="AL11" s="3"/>
       <c r="AM11" s="3"/>
       <c r="AN11" s="3"/>
@@ -12824,27 +12921,22 @@
       <c r="X12" s="104" t="s">
         <v>1202</v>
       </c>
-      <c r="AF12" t="s">
+      <c r="AF12" s="3" t="s">
         <v>836</v>
       </c>
-      <c r="AG12" t="s">
+      <c r="AG12" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="AH12">
+      <c r="AH12" s="3">
         <v>531</v>
       </c>
-      <c r="AI12">
+      <c r="AI12" s="3">
         <v>531</v>
       </c>
-      <c r="AL12" s="3" t="s">
-        <v>830</v>
-      </c>
-      <c r="AM12" s="3" t="s">
-        <v>475</v>
-      </c>
-      <c r="AN12" s="3">
-        <v>631</v>
-      </c>
+      <c r="AJ12" s="3"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="3"/>
+      <c r="AN12" s="3"/>
     </row>
     <row r="13" spans="2:42">
       <c r="B13" s="245"/>
@@ -12867,10 +12959,19 @@
       <c r="V13" s="246"/>
       <c r="W13" s="246"/>
       <c r="X13" s="246"/>
-      <c r="AL13" s="3"/>
-      <c r="AM13" s="3"/>
+      <c r="AF13" s="3"/>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="3"/>
+      <c r="AJ13" s="3"/>
+      <c r="AL13" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="AM13" s="3" t="s">
+        <v>475</v>
+      </c>
       <c r="AN13" s="3">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="14" spans="2:42">
@@ -12934,10 +13035,15 @@
       <c r="X14" s="104" t="s">
         <v>1215</v>
       </c>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="3"/>
       <c r="AL14" s="3"/>
       <c r="AM14" s="3"/>
       <c r="AN14" s="3">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="15" spans="2:42">
@@ -12987,10 +13093,15 @@
       <c r="X15" s="104" t="s">
         <v>1216</v>
       </c>
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="3"/>
+      <c r="AH15" s="3"/>
+      <c r="AI15" s="3"/>
+      <c r="AJ15" s="3"/>
       <c r="AL15" s="3"/>
       <c r="AM15" s="3"/>
       <c r="AN15" s="3">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="16" spans="2:42">
@@ -13038,8 +13149,26 @@
       <c r="X16" s="104" t="s">
         <v>1217</v>
       </c>
-    </row>
-    <row r="17" spans="1:26">
+      <c r="AF16" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="AG16" s="3" t="s">
+        <v>913</v>
+      </c>
+      <c r="AH16" s="3">
+        <v>541</v>
+      </c>
+      <c r="AI16" s="3">
+        <v>541</v>
+      </c>
+      <c r="AJ16" s="3"/>
+      <c r="AL16" s="3"/>
+      <c r="AM16" s="3"/>
+      <c r="AN16" s="3">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="104" t="s">
@@ -13084,8 +13213,22 @@
       <c r="X17" s="104" t="s">
         <v>1218</v>
       </c>
-    </row>
-    <row r="18" spans="1:26">
+      <c r="AF17" s="3"/>
+      <c r="AG17" s="3"/>
+      <c r="AH17" s="3"/>
+      <c r="AI17" s="3"/>
+      <c r="AJ17" s="3"/>
+      <c r="AL17" s="3" t="s">
+        <v>1335</v>
+      </c>
+      <c r="AM17" s="3" t="s">
+        <v>1336</v>
+      </c>
+      <c r="AN17" s="270">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40">
       <c r="A18" s="247"/>
       <c r="B18" s="245"/>
       <c r="C18" s="245"/>
@@ -13107,8 +13250,18 @@
       <c r="V18" s="246"/>
       <c r="W18" s="246"/>
       <c r="X18" s="246"/>
-    </row>
-    <row r="19" spans="1:26">
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="3"/>
+      <c r="AJ18" s="3"/>
+      <c r="AL18" s="3"/>
+      <c r="AM18" s="3"/>
+      <c r="AN18" s="270">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40">
       <c r="B19" s="3" t="s">
         <v>666</v>
       </c>
@@ -13172,8 +13325,18 @@
       <c r="Z19" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="20" spans="1:26">
+      <c r="AF19" s="3"/>
+      <c r="AG19" s="3"/>
+      <c r="AH19" s="3"/>
+      <c r="AI19" s="3"/>
+      <c r="AJ19" s="3"/>
+      <c r="AL19" s="3"/>
+      <c r="AM19" s="3"/>
+      <c r="AN19" s="270">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40">
       <c r="B20" s="3" t="s">
         <v>673</v>
       </c>
@@ -13223,8 +13386,18 @@
       <c r="Z20" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="21" spans="1:26">
+      <c r="AF20" s="3"/>
+      <c r="AG20" s="3"/>
+      <c r="AH20" s="3"/>
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="3"/>
+      <c r="AL20" s="3"/>
+      <c r="AM20" s="3"/>
+      <c r="AN20" s="270">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="104" t="s">
@@ -13258,9 +13431,13 @@
       <c r="R21" s="104" t="s">
         <v>1131</v>
       </c>
-      <c r="X21" s="59"/>
-    </row>
-    <row r="22" spans="1:26">
+      <c r="T21" s="246"/>
+      <c r="U21" s="246"/>
+      <c r="V21" s="246"/>
+      <c r="W21" s="246"/>
+      <c r="X21" s="246"/>
+    </row>
+    <row r="22" spans="1:40">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="104" t="s">
@@ -13294,9 +13471,23 @@
       <c r="R22" s="104" t="s">
         <v>1130</v>
       </c>
-      <c r="X22" s="59"/>
-    </row>
-    <row r="23" spans="1:26">
+      <c r="T22" s="426" t="s">
+        <v>1316</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>913</v>
+      </c>
+      <c r="V22" s="270">
+        <v>151</v>
+      </c>
+      <c r="W22" s="270" t="s">
+        <v>1317</v>
+      </c>
+      <c r="X22" s="104" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40">
       <c r="D23" s="59"/>
       <c r="F23" s="59"/>
       <c r="H23" s="245"/>
@@ -13309,9 +13500,19 @@
       <c r="P23" s="246"/>
       <c r="Q23" s="245"/>
       <c r="R23" s="246"/>
-      <c r="X23" s="59"/>
-    </row>
-    <row r="24" spans="1:26">
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="270">
+        <v>152</v>
+      </c>
+      <c r="W23" s="270" t="s">
+        <v>1318</v>
+      </c>
+      <c r="X23" s="104" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40">
       <c r="D24" s="59"/>
       <c r="F24" s="59"/>
       <c r="H24" s="3" t="s">
@@ -13344,9 +13545,19 @@
       <c r="R24" s="104" t="s">
         <v>1129</v>
       </c>
-      <c r="X24" s="59"/>
-    </row>
-    <row r="25" spans="1:26">
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="270">
+        <v>153</v>
+      </c>
+      <c r="W24" s="270" t="s">
+        <v>1319</v>
+      </c>
+      <c r="X24" s="104" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40">
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="104" t="s">
@@ -13369,9 +13580,19 @@
       <c r="R25" s="104" t="s">
         <v>1128</v>
       </c>
-      <c r="X25" s="59"/>
-    </row>
-    <row r="26" spans="1:26">
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="270">
+        <v>154</v>
+      </c>
+      <c r="W25" s="270" t="s">
+        <v>1320</v>
+      </c>
+      <c r="X25" s="104" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="26" spans="1:40">
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="104" t="s">
@@ -13394,9 +13615,13 @@
       <c r="R26" s="104" t="s">
         <v>1127</v>
       </c>
-      <c r="X26" s="59"/>
-    </row>
-    <row r="27" spans="1:26">
+      <c r="T26" s="246"/>
+      <c r="U26" s="246"/>
+      <c r="V26" s="246"/>
+      <c r="W26" s="246"/>
+      <c r="X26" s="246"/>
+    </row>
+    <row r="27" spans="1:40">
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="104" t="s">
@@ -13419,9 +13644,23 @@
       <c r="R27" s="104" t="s">
         <v>1126</v>
       </c>
-      <c r="X27" s="59"/>
-    </row>
-    <row r="28" spans="1:26">
+      <c r="T27" s="426" t="s">
+        <v>1325</v>
+      </c>
+      <c r="U27" s="3" t="s">
+        <v>913</v>
+      </c>
+      <c r="V27" s="270">
+        <v>161</v>
+      </c>
+      <c r="W27" s="270" t="s">
+        <v>1326</v>
+      </c>
+      <c r="X27" s="104" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40">
       <c r="H28" s="245"/>
       <c r="I28" s="245"/>
       <c r="J28" s="246"/>
@@ -13432,9 +13671,19 @@
       <c r="P28" s="246"/>
       <c r="Q28" s="245"/>
       <c r="R28" s="246"/>
-      <c r="X28" s="59"/>
-    </row>
-    <row r="29" spans="1:26">
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="270">
+        <v>162</v>
+      </c>
+      <c r="W28" s="270" t="s">
+        <v>1327</v>
+      </c>
+      <c r="X28" s="104" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="29" spans="1:40">
       <c r="H29" s="3" t="s">
         <v>749</v>
       </c>
@@ -13465,9 +13714,19 @@
       <c r="R29" s="104" t="s">
         <v>1125</v>
       </c>
-      <c r="X29" s="59"/>
-    </row>
-    <row r="30" spans="1:26">
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="270">
+        <v>163</v>
+      </c>
+      <c r="W29" s="270" t="s">
+        <v>1328</v>
+      </c>
+      <c r="X29" s="104" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="30" spans="1:40">
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="104" t="s">
@@ -13490,9 +13749,19 @@
       <c r="R30" s="104" t="s">
         <v>1124</v>
       </c>
-      <c r="X30" s="59"/>
-    </row>
-    <row r="31" spans="1:26">
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="270">
+        <v>164</v>
+      </c>
+      <c r="W30" s="270" t="s">
+        <v>1329</v>
+      </c>
+      <c r="X30" s="104" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="31" spans="1:40">
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="104" t="s">
@@ -13517,7 +13786,7 @@
       </c>
       <c r="X31" s="59"/>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="1:40">
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="104" t="s">
@@ -13653,20 +13922,20 @@
       <c r="X39" s="59"/>
     </row>
     <row r="41" spans="2:24">
-      <c r="B41" s="294" t="s">
+      <c r="B41" s="293" t="s">
         <v>697</v>
       </c>
-      <c r="C41" s="294"/>
-      <c r="D41" s="294"/>
-      <c r="E41" s="294"/>
-      <c r="F41" s="294"/>
-      <c r="H41" s="294" t="s">
+      <c r="C41" s="293"/>
+      <c r="D41" s="293"/>
+      <c r="E41" s="293"/>
+      <c r="F41" s="293"/>
+      <c r="H41" s="293" t="s">
         <v>750</v>
       </c>
-      <c r="I41" s="294"/>
-      <c r="J41" s="294"/>
-      <c r="K41" s="294"/>
-      <c r="L41" s="294"/>
+      <c r="I41" s="293"/>
+      <c r="J41" s="293"/>
+      <c r="K41" s="293"/>
+      <c r="L41" s="293"/>
     </row>
     <row r="42" spans="2:24">
       <c r="B42" s="101" t="s">
@@ -14203,39 +14472,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27" customHeight="1" thickBot="1">
-      <c r="A1" s="310" t="s">
+      <c r="A1" s="313" t="s">
         <v>1146</v>
       </c>
-      <c r="B1" s="311"/>
-      <c r="C1" s="311"/>
-      <c r="D1" s="311"/>
-      <c r="E1" s="311"/>
-      <c r="F1" s="311"/>
-      <c r="G1" s="311"/>
-      <c r="H1" s="311"/>
-      <c r="I1" s="311"/>
-      <c r="J1" s="311"/>
-      <c r="K1" s="311"/>
-      <c r="L1" s="312"/>
+      <c r="B1" s="314"/>
+      <c r="C1" s="314"/>
+      <c r="D1" s="314"/>
+      <c r="E1" s="314"/>
+      <c r="F1" s="314"/>
+      <c r="G1" s="314"/>
+      <c r="H1" s="314"/>
+      <c r="I1" s="314"/>
+      <c r="J1" s="314"/>
+      <c r="K1" s="314"/>
+      <c r="L1" s="315"/>
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A2" s="307" t="s">
+      <c r="A2" s="310" t="s">
         <v>1147</v>
       </c>
-      <c r="B2" s="308"/>
-      <c r="C2" s="309"/>
+      <c r="B2" s="311"/>
+      <c r="C2" s="312"/>
       <c r="D2" s="259"/>
-      <c r="E2" s="307" t="s">
+      <c r="E2" s="310" t="s">
         <v>1055</v>
       </c>
-      <c r="F2" s="308"/>
-      <c r="G2" s="309"/>
+      <c r="F2" s="311"/>
+      <c r="G2" s="312"/>
       <c r="H2" s="259"/>
-      <c r="I2" s="307" t="s">
+      <c r="I2" s="310" t="s">
         <v>1054</v>
       </c>
-      <c r="J2" s="308"/>
-      <c r="K2" s="309"/>
+      <c r="J2" s="311"/>
+      <c r="K2" s="312"/>
       <c r="L2" s="122"/>
     </row>
     <row r="3" spans="1:12" ht="19.5" thickBot="1">
@@ -14271,7 +14540,7 @@
       <c r="L3" s="122"/>
     </row>
     <row r="4" spans="1:12" ht="18.75">
-      <c r="A4" s="301" t="s">
+      <c r="A4" s="316" t="s">
         <v>325</v>
       </c>
       <c r="B4" s="132" t="s">
@@ -14281,7 +14550,7 @@
         <v>705</v>
       </c>
       <c r="D4" s="253"/>
-      <c r="E4" s="304" t="s">
+      <c r="E4" s="307" t="s">
         <v>975</v>
       </c>
       <c r="F4" s="132" t="s">
@@ -14291,7 +14560,7 @@
         <v>1028</v>
       </c>
       <c r="H4" s="125"/>
-      <c r="I4" s="304" t="s">
+      <c r="I4" s="307" t="s">
         <v>1057</v>
       </c>
       <c r="J4" s="132" t="s">
@@ -14303,7 +14572,7 @@
       <c r="L4" s="122"/>
     </row>
     <row r="5" spans="1:12" ht="18.75">
-      <c r="A5" s="302"/>
+      <c r="A5" s="317"/>
       <c r="B5" s="131" t="s">
         <v>322</v>
       </c>
@@ -14311,7 +14580,7 @@
         <v>706</v>
       </c>
       <c r="D5" s="253"/>
-      <c r="E5" s="305"/>
+      <c r="E5" s="308"/>
       <c r="F5" s="131" t="s">
         <v>1002</v>
       </c>
@@ -14319,7 +14588,7 @@
         <v>1029</v>
       </c>
       <c r="H5" s="125"/>
-      <c r="I5" s="305"/>
+      <c r="I5" s="308"/>
       <c r="J5" s="131" t="s">
         <v>1092</v>
       </c>
@@ -14329,7 +14598,7 @@
       <c r="L5" s="122"/>
     </row>
     <row r="6" spans="1:12" ht="18.75">
-      <c r="A6" s="302"/>
+      <c r="A6" s="317"/>
       <c r="B6" s="131" t="s">
         <v>323</v>
       </c>
@@ -14337,7 +14606,7 @@
         <v>707</v>
       </c>
       <c r="D6" s="253"/>
-      <c r="E6" s="305"/>
+      <c r="E6" s="308"/>
       <c r="F6" s="131" t="s">
         <v>1003</v>
       </c>
@@ -14345,7 +14614,7 @@
         <v>1030</v>
       </c>
       <c r="H6" s="125"/>
-      <c r="I6" s="305"/>
+      <c r="I6" s="308"/>
       <c r="J6" s="131" t="s">
         <v>1093</v>
       </c>
@@ -14355,7 +14624,7 @@
       <c r="L6" s="122"/>
     </row>
     <row r="7" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A7" s="303"/>
+      <c r="A7" s="318"/>
       <c r="B7" s="135" t="s">
         <v>324</v>
       </c>
@@ -14363,7 +14632,7 @@
         <v>708</v>
       </c>
       <c r="D7" s="253"/>
-      <c r="E7" s="306"/>
+      <c r="E7" s="309"/>
       <c r="F7" s="135" t="s">
         <v>1004</v>
       </c>
@@ -14371,7 +14640,7 @@
         <v>1031</v>
       </c>
       <c r="H7" s="125"/>
-      <c r="I7" s="306"/>
+      <c r="I7" s="309"/>
       <c r="J7" s="135" t="s">
         <v>1094</v>
       </c>
@@ -14381,7 +14650,7 @@
       <c r="L7" s="122"/>
     </row>
     <row r="8" spans="1:12" ht="18.75">
-      <c r="A8" s="301" t="s">
+      <c r="A8" s="316" t="s">
         <v>667</v>
       </c>
       <c r="B8" s="132" t="s">
@@ -14391,7 +14660,7 @@
         <v>709</v>
       </c>
       <c r="D8" s="253"/>
-      <c r="E8" s="304" t="s">
+      <c r="E8" s="307" t="s">
         <v>974</v>
       </c>
       <c r="F8" s="132" t="s">
@@ -14401,7 +14670,7 @@
         <v>1032</v>
       </c>
       <c r="H8" s="125"/>
-      <c r="I8" s="304" t="s">
+      <c r="I8" s="307" t="s">
         <v>1058</v>
       </c>
       <c r="J8" s="132" t="s">
@@ -14413,7 +14682,7 @@
       <c r="L8" s="122"/>
     </row>
     <row r="9" spans="1:12" ht="18.75">
-      <c r="A9" s="302"/>
+      <c r="A9" s="317"/>
       <c r="B9" s="131" t="s">
         <v>658</v>
       </c>
@@ -14421,7 +14690,7 @@
         <v>710</v>
       </c>
       <c r="D9" s="253"/>
-      <c r="E9" s="305"/>
+      <c r="E9" s="308"/>
       <c r="F9" s="131" t="s">
         <v>1006</v>
       </c>
@@ -14429,7 +14698,7 @@
         <v>1033</v>
       </c>
       <c r="H9" s="125"/>
-      <c r="I9" s="305"/>
+      <c r="I9" s="308"/>
       <c r="J9" s="131" t="s">
         <v>1095</v>
       </c>
@@ -14439,7 +14708,7 @@
       <c r="L9" s="122"/>
     </row>
     <row r="10" spans="1:12" ht="18.75">
-      <c r="A10" s="302"/>
+      <c r="A10" s="317"/>
       <c r="B10" s="131" t="s">
         <v>659</v>
       </c>
@@ -14447,7 +14716,7 @@
         <v>711</v>
       </c>
       <c r="D10" s="253"/>
-      <c r="E10" s="305"/>
+      <c r="E10" s="308"/>
       <c r="F10" s="131" t="s">
         <v>1008</v>
       </c>
@@ -14455,7 +14724,7 @@
         <v>1034</v>
       </c>
       <c r="H10" s="125"/>
-      <c r="I10" s="305"/>
+      <c r="I10" s="308"/>
       <c r="J10" s="131" t="s">
         <v>1096</v>
       </c>
@@ -14465,7 +14734,7 @@
       <c r="L10" s="122"/>
     </row>
     <row r="11" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A11" s="303"/>
+      <c r="A11" s="318"/>
       <c r="B11" s="135" t="s">
         <v>660</v>
       </c>
@@ -14473,7 +14742,7 @@
         <v>712</v>
       </c>
       <c r="D11" s="253"/>
-      <c r="E11" s="306"/>
+      <c r="E11" s="309"/>
       <c r="F11" s="135" t="s">
         <v>1009</v>
       </c>
@@ -14481,7 +14750,7 @@
         <v>1035</v>
       </c>
       <c r="H11" s="125"/>
-      <c r="I11" s="306"/>
+      <c r="I11" s="309"/>
       <c r="J11" s="135" t="s">
         <v>1097</v>
       </c>
@@ -14491,7 +14760,7 @@
       <c r="L11" s="122"/>
     </row>
     <row r="12" spans="1:12" ht="18.75">
-      <c r="A12" s="301" t="s">
+      <c r="A12" s="316" t="s">
         <v>665</v>
       </c>
       <c r="B12" s="132" t="s">
@@ -14501,7 +14770,7 @@
         <v>713</v>
       </c>
       <c r="D12" s="253"/>
-      <c r="E12" s="304" t="s">
+      <c r="E12" s="307" t="s">
         <v>973</v>
       </c>
       <c r="F12" s="132" t="s">
@@ -14511,7 +14780,7 @@
         <v>1036</v>
       </c>
       <c r="H12" s="125"/>
-      <c r="I12" s="304" t="s">
+      <c r="I12" s="307" t="s">
         <v>1059</v>
       </c>
       <c r="J12" s="132" t="s">
@@ -14523,7 +14792,7 @@
       <c r="L12" s="122"/>
     </row>
     <row r="13" spans="1:12" ht="18.75">
-      <c r="A13" s="302"/>
+      <c r="A13" s="317"/>
       <c r="B13" s="131" t="s">
         <v>662</v>
       </c>
@@ -14531,7 +14800,7 @@
         <v>714</v>
       </c>
       <c r="D13" s="253"/>
-      <c r="E13" s="305"/>
+      <c r="E13" s="308"/>
       <c r="F13" s="131" t="s">
         <v>1011</v>
       </c>
@@ -14539,7 +14808,7 @@
         <v>1037</v>
       </c>
       <c r="H13" s="125"/>
-      <c r="I13" s="305"/>
+      <c r="I13" s="308"/>
       <c r="J13" s="131" t="s">
         <v>1099</v>
       </c>
@@ -14549,7 +14818,7 @@
       <c r="L13" s="122"/>
     </row>
     <row r="14" spans="1:12" ht="18.75">
-      <c r="A14" s="302"/>
+      <c r="A14" s="317"/>
       <c r="B14" s="131" t="s">
         <v>663</v>
       </c>
@@ -14557,7 +14826,7 @@
         <v>715</v>
       </c>
       <c r="D14" s="253"/>
-      <c r="E14" s="305"/>
+      <c r="E14" s="308"/>
       <c r="F14" s="131" t="s">
         <v>1012</v>
       </c>
@@ -14565,7 +14834,7 @@
         <v>1038</v>
       </c>
       <c r="H14" s="125"/>
-      <c r="I14" s="305"/>
+      <c r="I14" s="308"/>
       <c r="J14" s="131" t="s">
         <v>1100</v>
       </c>
@@ -14575,7 +14844,7 @@
       <c r="L14" s="122"/>
     </row>
     <row r="15" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A15" s="303"/>
+      <c r="A15" s="318"/>
       <c r="B15" s="135" t="s">
         <v>664</v>
       </c>
@@ -14583,7 +14852,7 @@
         <v>716</v>
       </c>
       <c r="D15" s="253"/>
-      <c r="E15" s="306"/>
+      <c r="E15" s="309"/>
       <c r="F15" s="135" t="s">
         <v>1013</v>
       </c>
@@ -14591,7 +14860,7 @@
         <v>1039</v>
       </c>
       <c r="H15" s="125"/>
-      <c r="I15" s="306"/>
+      <c r="I15" s="309"/>
       <c r="J15" s="135" t="s">
         <v>1101</v>
       </c>
@@ -14601,7 +14870,7 @@
       <c r="L15" s="122"/>
     </row>
     <row r="16" spans="1:12" ht="18.75">
-      <c r="A16" s="301" t="s">
+      <c r="A16" s="316" t="s">
         <v>666</v>
       </c>
       <c r="B16" s="132" t="s">
@@ -14611,7 +14880,7 @@
         <v>717</v>
       </c>
       <c r="D16" s="253"/>
-      <c r="E16" s="304" t="s">
+      <c r="E16" s="307" t="s">
         <v>972</v>
       </c>
       <c r="F16" s="132" t="s">
@@ -14621,7 +14890,7 @@
         <v>1040</v>
       </c>
       <c r="H16" s="125"/>
-      <c r="I16" s="304" t="s">
+      <c r="I16" s="307" t="s">
         <v>1060</v>
       </c>
       <c r="J16" s="132" t="s">
@@ -14633,7 +14902,7 @@
       <c r="L16" s="122"/>
     </row>
     <row r="17" spans="1:12" ht="18.75">
-      <c r="A17" s="302"/>
+      <c r="A17" s="317"/>
       <c r="B17" s="131" t="s">
         <v>669</v>
       </c>
@@ -14641,7 +14910,7 @@
         <v>718</v>
       </c>
       <c r="D17" s="253"/>
-      <c r="E17" s="305"/>
+      <c r="E17" s="308"/>
       <c r="F17" s="131" t="s">
         <v>1015</v>
       </c>
@@ -14649,7 +14918,7 @@
         <v>1041</v>
       </c>
       <c r="H17" s="125"/>
-      <c r="I17" s="305"/>
+      <c r="I17" s="308"/>
       <c r="J17" s="131" t="s">
         <v>1103</v>
       </c>
@@ -14659,7 +14928,7 @@
       <c r="L17" s="122"/>
     </row>
     <row r="18" spans="1:12" ht="18.75">
-      <c r="A18" s="302"/>
+      <c r="A18" s="317"/>
       <c r="B18" s="131" t="s">
         <v>670</v>
       </c>
@@ -14667,7 +14936,7 @@
         <v>719</v>
       </c>
       <c r="D18" s="253"/>
-      <c r="E18" s="305"/>
+      <c r="E18" s="308"/>
       <c r="F18" s="131" t="s">
         <v>1016</v>
       </c>
@@ -14675,7 +14944,7 @@
         <v>1042</v>
       </c>
       <c r="H18" s="125"/>
-      <c r="I18" s="305"/>
+      <c r="I18" s="308"/>
       <c r="J18" s="131" t="s">
         <v>1104</v>
       </c>
@@ -14685,7 +14954,7 @@
       <c r="L18" s="122"/>
     </row>
     <row r="19" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A19" s="303"/>
+      <c r="A19" s="318"/>
       <c r="B19" s="135" t="s">
         <v>671</v>
       </c>
@@ -14693,7 +14962,7 @@
         <v>720</v>
       </c>
       <c r="D19" s="253"/>
-      <c r="E19" s="306"/>
+      <c r="E19" s="309"/>
       <c r="F19" s="135" t="s">
         <v>1017</v>
       </c>
@@ -14701,7 +14970,7 @@
         <v>1043</v>
       </c>
       <c r="H19" s="125"/>
-      <c r="I19" s="306"/>
+      <c r="I19" s="309"/>
       <c r="J19" s="135" t="s">
         <v>1105</v>
       </c>
@@ -14715,7 +14984,7 @@
       <c r="B20" s="125"/>
       <c r="C20" s="125"/>
       <c r="D20" s="125"/>
-      <c r="E20" s="304" t="s">
+      <c r="E20" s="307" t="s">
         <v>560</v>
       </c>
       <c r="F20" s="132" t="s">
@@ -14725,7 +14994,7 @@
         <v>1044</v>
       </c>
       <c r="H20" s="125"/>
-      <c r="I20" s="304" t="s">
+      <c r="I20" s="307" t="s">
         <v>1061</v>
       </c>
       <c r="J20" s="132" t="s">
@@ -14741,7 +15010,7 @@
       <c r="B21" s="125"/>
       <c r="C21" s="125"/>
       <c r="D21" s="125"/>
-      <c r="E21" s="305"/>
+      <c r="E21" s="308"/>
       <c r="F21" s="131" t="s">
         <v>1019</v>
       </c>
@@ -14749,7 +15018,7 @@
         <v>1045</v>
       </c>
       <c r="H21" s="125"/>
-      <c r="I21" s="305"/>
+      <c r="I21" s="308"/>
       <c r="J21" s="131" t="s">
         <v>1107</v>
       </c>
@@ -14763,7 +15032,7 @@
       <c r="B22" s="125"/>
       <c r="C22" s="125"/>
       <c r="D22" s="125"/>
-      <c r="E22" s="305"/>
+      <c r="E22" s="308"/>
       <c r="F22" s="131" t="s">
         <v>1020</v>
       </c>
@@ -14771,7 +15040,7 @@
         <v>1046</v>
       </c>
       <c r="H22" s="125"/>
-      <c r="I22" s="305"/>
+      <c r="I22" s="308"/>
       <c r="J22" s="131" t="s">
         <v>1108</v>
       </c>
@@ -14787,7 +15056,7 @@
       <c r="B23" s="256"/>
       <c r="C23" s="257"/>
       <c r="D23" s="125"/>
-      <c r="E23" s="306"/>
+      <c r="E23" s="309"/>
       <c r="F23" s="135" t="s">
         <v>1021</v>
       </c>
@@ -14795,7 +15064,7 @@
         <v>1047</v>
       </c>
       <c r="H23" s="125"/>
-      <c r="I23" s="306"/>
+      <c r="I23" s="309"/>
       <c r="J23" s="135" t="s">
         <v>1109</v>
       </c>
@@ -14815,7 +15084,7 @@
         <v>321</v>
       </c>
       <c r="D24" s="125"/>
-      <c r="E24" s="304" t="s">
+      <c r="E24" s="307" t="s">
         <v>749</v>
       </c>
       <c r="F24" s="132" t="s">
@@ -14825,7 +15094,7 @@
         <v>1048</v>
       </c>
       <c r="H24" s="125"/>
-      <c r="I24" s="304" t="s">
+      <c r="I24" s="307" t="s">
         <v>1062</v>
       </c>
       <c r="J24" s="132" t="s">
@@ -14837,7 +15106,7 @@
       <c r="L24" s="122"/>
     </row>
     <row r="25" spans="1:12" ht="18.75">
-      <c r="A25" s="316" t="s">
+      <c r="A25" s="301" t="s">
         <v>493</v>
       </c>
       <c r="B25" s="132" t="s">
@@ -14847,7 +15116,7 @@
         <v>721</v>
       </c>
       <c r="D25" s="125"/>
-      <c r="E25" s="305"/>
+      <c r="E25" s="308"/>
       <c r="F25" s="131" t="s">
         <v>1023</v>
       </c>
@@ -14855,7 +15124,7 @@
         <v>1049</v>
       </c>
       <c r="H25" s="125"/>
-      <c r="I25" s="305"/>
+      <c r="I25" s="308"/>
       <c r="J25" s="131" t="s">
         <v>1111</v>
       </c>
@@ -14865,7 +15134,7 @@
       <c r="L25" s="122"/>
     </row>
     <row r="26" spans="1:12" ht="18.75">
-      <c r="A26" s="317"/>
+      <c r="A26" s="302"/>
       <c r="B26" s="131" t="s">
         <v>679</v>
       </c>
@@ -14873,7 +15142,7 @@
         <v>722</v>
       </c>
       <c r="D26" s="125"/>
-      <c r="E26" s="305"/>
+      <c r="E26" s="308"/>
       <c r="F26" s="131" t="s">
         <v>1024</v>
       </c>
@@ -14881,7 +15150,7 @@
         <v>1050</v>
       </c>
       <c r="H26" s="125"/>
-      <c r="I26" s="305"/>
+      <c r="I26" s="308"/>
       <c r="J26" s="131" t="s">
         <v>1112</v>
       </c>
@@ -14891,7 +15160,7 @@
       <c r="L26" s="122"/>
     </row>
     <row r="27" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A27" s="317"/>
+      <c r="A27" s="302"/>
       <c r="B27" s="131" t="s">
         <v>680</v>
       </c>
@@ -14899,7 +15168,7 @@
         <v>723</v>
       </c>
       <c r="D27" s="125"/>
-      <c r="E27" s="306"/>
+      <c r="E27" s="309"/>
       <c r="F27" s="135" t="s">
         <v>1025</v>
       </c>
@@ -14907,7 +15176,7 @@
         <v>1051</v>
       </c>
       <c r="H27" s="125"/>
-      <c r="I27" s="306"/>
+      <c r="I27" s="309"/>
       <c r="J27" s="135" t="s">
         <v>1113</v>
       </c>
@@ -14917,7 +15186,7 @@
       <c r="L27" s="122"/>
     </row>
     <row r="28" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A28" s="318"/>
+      <c r="A28" s="303"/>
       <c r="B28" s="135" t="s">
         <v>681</v>
       </c>
@@ -14925,7 +15194,7 @@
         <v>724</v>
       </c>
       <c r="D28" s="125"/>
-      <c r="E28" s="304" t="s">
+      <c r="E28" s="307" t="s">
         <v>562</v>
       </c>
       <c r="F28" s="132" t="s">
@@ -14935,7 +15204,7 @@
         <v>1052</v>
       </c>
       <c r="H28" s="125"/>
-      <c r="I28" s="304" t="s">
+      <c r="I28" s="307" t="s">
         <v>1063</v>
       </c>
       <c r="J28" s="132" t="s">
@@ -14947,7 +15216,7 @@
       <c r="L28" s="122"/>
     </row>
     <row r="29" spans="1:12" ht="18.75">
-      <c r="A29" s="316" t="s">
+      <c r="A29" s="301" t="s">
         <v>687</v>
       </c>
       <c r="B29" s="132" t="s">
@@ -14957,7 +15226,7 @@
         <v>725</v>
       </c>
       <c r="D29" s="253"/>
-      <c r="E29" s="305"/>
+      <c r="E29" s="308"/>
       <c r="F29" s="131" t="s">
         <v>1027</v>
       </c>
@@ -14965,7 +15234,7 @@
         <v>1053</v>
       </c>
       <c r="H29" s="125"/>
-      <c r="I29" s="305"/>
+      <c r="I29" s="308"/>
       <c r="J29" s="131" t="s">
         <v>1115</v>
       </c>
@@ -14975,7 +15244,7 @@
       <c r="L29" s="122"/>
     </row>
     <row r="30" spans="1:12" ht="18.75">
-      <c r="A30" s="317"/>
+      <c r="A30" s="302"/>
       <c r="B30" s="131" t="s">
         <v>684</v>
       </c>
@@ -14983,11 +15252,11 @@
         <v>726</v>
       </c>
       <c r="D30" s="253"/>
-      <c r="E30" s="305"/>
+      <c r="E30" s="308"/>
       <c r="F30" s="131"/>
       <c r="G30" s="250"/>
       <c r="H30" s="125"/>
-      <c r="I30" s="305"/>
+      <c r="I30" s="308"/>
       <c r="J30" s="131" t="s">
         <v>1116</v>
       </c>
@@ -14997,7 +15266,7 @@
       <c r="L30" s="122"/>
     </row>
     <row r="31" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A31" s="317"/>
+      <c r="A31" s="302"/>
       <c r="B31" s="131" t="s">
         <v>685</v>
       </c>
@@ -15005,11 +15274,11 @@
         <v>727</v>
       </c>
       <c r="D31" s="253"/>
-      <c r="E31" s="306"/>
+      <c r="E31" s="309"/>
       <c r="F31" s="135"/>
       <c r="G31" s="251"/>
       <c r="H31" s="125"/>
-      <c r="I31" s="306"/>
+      <c r="I31" s="309"/>
       <c r="J31" s="135" t="s">
         <v>1117</v>
       </c>
@@ -15019,7 +15288,7 @@
       <c r="L31" s="122"/>
     </row>
     <row r="32" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A32" s="318"/>
+      <c r="A32" s="303"/>
       <c r="B32" s="135" t="s">
         <v>686</v>
       </c>
@@ -15037,7 +15306,7 @@
       <c r="L32" s="122"/>
     </row>
     <row r="33" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A33" s="316" t="s">
+      <c r="A33" s="301" t="s">
         <v>691</v>
       </c>
       <c r="B33" s="132" t="s">
@@ -15047,21 +15316,21 @@
         <v>729</v>
       </c>
       <c r="D33" s="253"/>
-      <c r="E33" s="313" t="s">
+      <c r="E33" s="304" t="s">
         <v>1149</v>
       </c>
-      <c r="F33" s="314"/>
-      <c r="G33" s="315"/>
+      <c r="F33" s="305"/>
+      <c r="G33" s="306"/>
       <c r="H33" s="124"/>
-      <c r="I33" s="313" t="s">
+      <c r="I33" s="304" t="s">
         <v>1148</v>
       </c>
-      <c r="J33" s="314"/>
-      <c r="K33" s="315"/>
+      <c r="J33" s="305"/>
+      <c r="K33" s="306"/>
       <c r="L33" s="122"/>
     </row>
     <row r="34" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A34" s="317"/>
+      <c r="A34" s="302"/>
       <c r="B34" s="131" t="s">
         <v>693</v>
       </c>
@@ -15091,7 +15360,7 @@
       <c r="L34" s="122"/>
     </row>
     <row r="35" spans="1:12" ht="18.75">
-      <c r="A35" s="317"/>
+      <c r="A35" s="302"/>
       <c r="B35" s="131" t="s">
         <v>694</v>
       </c>
@@ -15099,7 +15368,7 @@
         <v>731</v>
       </c>
       <c r="D35" s="253"/>
-      <c r="E35" s="316" t="s">
+      <c r="E35" s="301" t="s">
         <v>494</v>
       </c>
       <c r="F35" s="132" t="s">
@@ -15109,7 +15378,7 @@
         <v>11311</v>
       </c>
       <c r="H35" s="124"/>
-      <c r="I35" s="316" t="s">
+      <c r="I35" s="301" t="s">
         <v>955</v>
       </c>
       <c r="J35" s="132" t="s">
@@ -15121,7 +15390,7 @@
       <c r="L35" s="122"/>
     </row>
     <row r="36" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A36" s="318"/>
+      <c r="A36" s="303"/>
       <c r="B36" s="135" t="s">
         <v>695</v>
       </c>
@@ -15129,7 +15398,7 @@
         <v>732</v>
       </c>
       <c r="D36" s="253"/>
-      <c r="E36" s="317"/>
+      <c r="E36" s="302"/>
       <c r="F36" s="131" t="s">
         <v>958</v>
       </c>
@@ -15137,7 +15406,7 @@
         <v>11312</v>
       </c>
       <c r="H36" s="124"/>
-      <c r="I36" s="317"/>
+      <c r="I36" s="302"/>
       <c r="J36" s="131" t="s">
         <v>965</v>
       </c>
@@ -15147,7 +15416,7 @@
       <c r="L36" s="122"/>
     </row>
     <row r="37" spans="1:12" ht="18.75">
-      <c r="A37" s="316" t="s">
+      <c r="A37" s="301" t="s">
         <v>698</v>
       </c>
       <c r="B37" s="132" t="s">
@@ -15157,7 +15426,7 @@
         <v>11441</v>
       </c>
       <c r="D37" s="253"/>
-      <c r="E37" s="317"/>
+      <c r="E37" s="302"/>
       <c r="F37" s="131" t="s">
         <v>959</v>
       </c>
@@ -15165,7 +15434,7 @@
         <v>11313</v>
       </c>
       <c r="H37" s="124"/>
-      <c r="I37" s="317"/>
+      <c r="I37" s="302"/>
       <c r="J37" s="131" t="s">
         <v>966</v>
       </c>
@@ -15175,7 +15444,7 @@
       <c r="L37" s="122"/>
     </row>
     <row r="38" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A38" s="317"/>
+      <c r="A38" s="302"/>
       <c r="B38" s="131" t="s">
         <v>700</v>
       </c>
@@ -15183,7 +15452,7 @@
         <v>11442</v>
       </c>
       <c r="D38" s="253"/>
-      <c r="E38" s="318"/>
+      <c r="E38" s="303"/>
       <c r="F38" s="135" t="s">
         <v>959</v>
       </c>
@@ -15191,7 +15460,7 @@
         <v>11314</v>
       </c>
       <c r="H38" s="124"/>
-      <c r="I38" s="318"/>
+      <c r="I38" s="303"/>
       <c r="J38" s="135" t="s">
         <v>967</v>
       </c>
@@ -15201,7 +15470,7 @@
       <c r="L38" s="122"/>
     </row>
     <row r="39" spans="1:12" ht="18.75">
-      <c r="A39" s="317"/>
+      <c r="A39" s="302"/>
       <c r="B39" s="131" t="s">
         <v>701</v>
       </c>
@@ -15209,7 +15478,7 @@
         <v>11443</v>
       </c>
       <c r="D39" s="253"/>
-      <c r="E39" s="316" t="s">
+      <c r="E39" s="301" t="s">
         <v>954</v>
       </c>
       <c r="F39" s="132" t="s">
@@ -15219,7 +15488,7 @@
         <v>11321</v>
       </c>
       <c r="H39" s="124"/>
-      <c r="I39" s="316" t="s">
+      <c r="I39" s="301" t="s">
         <v>956</v>
       </c>
       <c r="J39" s="132" t="s">
@@ -15231,7 +15500,7 @@
       <c r="L39" s="122"/>
     </row>
     <row r="40" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A40" s="318"/>
+      <c r="A40" s="303"/>
       <c r="B40" s="135" t="s">
         <v>702</v>
       </c>
@@ -15239,7 +15508,7 @@
         <v>11444</v>
       </c>
       <c r="D40" s="253"/>
-      <c r="E40" s="317"/>
+      <c r="E40" s="302"/>
       <c r="F40" s="131" t="s">
         <v>961</v>
       </c>
@@ -15247,7 +15516,7 @@
         <v>11322</v>
       </c>
       <c r="H40" s="124"/>
-      <c r="I40" s="317"/>
+      <c r="I40" s="302"/>
       <c r="J40" s="131" t="s">
         <v>969</v>
       </c>
@@ -15261,7 +15530,7 @@
       <c r="B41" s="125"/>
       <c r="C41" s="253"/>
       <c r="D41" s="253"/>
-      <c r="E41" s="317"/>
+      <c r="E41" s="302"/>
       <c r="F41" s="131" t="s">
         <v>962</v>
       </c>
@@ -15269,7 +15538,7 @@
         <v>11323</v>
       </c>
       <c r="H41" s="124"/>
-      <c r="I41" s="317"/>
+      <c r="I41" s="302"/>
       <c r="J41" s="131" t="s">
         <v>970</v>
       </c>
@@ -15283,7 +15552,7 @@
       <c r="B42" s="125"/>
       <c r="C42" s="253"/>
       <c r="D42" s="253"/>
-      <c r="E42" s="318"/>
+      <c r="E42" s="303"/>
       <c r="F42" s="135" t="s">
         <v>963</v>
       </c>
@@ -15291,7 +15560,7 @@
         <v>11324</v>
       </c>
       <c r="H42" s="124"/>
-      <c r="I42" s="318"/>
+      <c r="I42" s="303"/>
       <c r="J42" s="135" t="s">
         <v>971</v>
       </c>
@@ -15344,16 +15613,18 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="I35:I38"/>
-    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A7"/>
     <mergeCell ref="I16:I19"/>
     <mergeCell ref="I12:I15"/>
     <mergeCell ref="I8:I11"/>
@@ -15364,18 +15635,16 @@
     <mergeCell ref="I28:I31"/>
     <mergeCell ref="E20:E23"/>
     <mergeCell ref="E24:E27"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="I35:I38"/>
+    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="E33:G33"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15406,40 +15675,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="323" t="s">
+      <c r="A1" s="319" t="s">
         <v>1151</v>
       </c>
-      <c r="B1" s="324"/>
-      <c r="C1" s="324"/>
-      <c r="D1" s="324"/>
-      <c r="E1" s="324"/>
-      <c r="F1" s="324"/>
-      <c r="G1" s="324"/>
-      <c r="H1" s="325"/>
+      <c r="B1" s="320"/>
+      <c r="C1" s="320"/>
+      <c r="D1" s="320"/>
+      <c r="E1" s="320"/>
+      <c r="F1" s="320"/>
+      <c r="G1" s="320"/>
+      <c r="H1" s="321"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="326"/>
-      <c r="B2" s="327"/>
-      <c r="C2" s="327"/>
-      <c r="D2" s="327"/>
-      <c r="E2" s="327"/>
-      <c r="F2" s="327"/>
-      <c r="G2" s="327"/>
-      <c r="H2" s="328"/>
+      <c r="A2" s="322"/>
+      <c r="B2" s="323"/>
+      <c r="C2" s="323"/>
+      <c r="D2" s="323"/>
+      <c r="E2" s="323"/>
+      <c r="F2" s="323"/>
+      <c r="G2" s="323"/>
+      <c r="H2" s="324"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="329" t="s">
+      <c r="A3" s="325" t="s">
         <v>250</v>
       </c>
-      <c r="B3" s="330"/>
-      <c r="C3" s="330"/>
-      <c r="D3" s="330"/>
-      <c r="E3" s="330" t="s">
+      <c r="B3" s="326"/>
+      <c r="C3" s="326"/>
+      <c r="D3" s="326"/>
+      <c r="E3" s="326" t="s">
         <v>251</v>
       </c>
-      <c r="F3" s="330"/>
-      <c r="G3" s="330"/>
-      <c r="H3" s="331"/>
+      <c r="F3" s="326"/>
+      <c r="G3" s="326"/>
+      <c r="H3" s="327"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="12">
@@ -15973,11 +16242,11 @@
       <c r="C27" s="118" t="s">
         <v>594</v>
       </c>
-      <c r="D27" s="322" t="s">
+      <c r="D27" s="328" t="s">
         <v>570</v>
       </c>
-      <c r="E27" s="322"/>
-      <c r="F27" s="322"/>
+      <c r="E27" s="328"/>
+      <c r="F27" s="328"/>
       <c r="G27" s="17"/>
       <c r="H27" s="18"/>
     </row>
@@ -15989,11 +16258,11 @@
       <c r="C28" s="118" t="s">
         <v>598</v>
       </c>
-      <c r="D28" s="322" t="s">
+      <c r="D28" s="328" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="322"/>
-      <c r="F28" s="322"/>
+      <c r="E28" s="328"/>
+      <c r="F28" s="328"/>
       <c r="G28" s="17"/>
       <c r="H28" s="18"/>
     </row>
@@ -16005,11 +16274,11 @@
       <c r="C29" s="118" t="s">
         <v>599</v>
       </c>
-      <c r="D29" s="322" t="s">
+      <c r="D29" s="328" t="s">
         <v>571</v>
       </c>
-      <c r="E29" s="322"/>
-      <c r="F29" s="322"/>
+      <c r="E29" s="328"/>
+      <c r="F29" s="328"/>
       <c r="G29" s="17"/>
       <c r="H29" s="18"/>
     </row>
@@ -16021,11 +16290,11 @@
       <c r="C30" s="118" t="s">
         <v>600</v>
       </c>
-      <c r="D30" s="322" t="s">
+      <c r="D30" s="328" t="s">
         <v>572</v>
       </c>
-      <c r="E30" s="322"/>
-      <c r="F30" s="322"/>
+      <c r="E30" s="328"/>
+      <c r="F30" s="328"/>
       <c r="G30" s="17"/>
       <c r="H30" s="18"/>
     </row>
@@ -16037,11 +16306,11 @@
       <c r="C31" s="118" t="s">
         <v>601</v>
       </c>
-      <c r="D31" s="322" t="s">
+      <c r="D31" s="328" t="s">
         <v>573</v>
       </c>
-      <c r="E31" s="322"/>
-      <c r="F31" s="322"/>
+      <c r="E31" s="328"/>
+      <c r="F31" s="328"/>
       <c r="G31" s="17"/>
       <c r="H31" s="18"/>
     </row>
@@ -16053,11 +16322,11 @@
       <c r="C32" s="118" t="s">
         <v>602</v>
       </c>
-      <c r="D32" s="322" t="s">
+      <c r="D32" s="328" t="s">
         <v>574</v>
       </c>
-      <c r="E32" s="322"/>
-      <c r="F32" s="322"/>
+      <c r="E32" s="328"/>
+      <c r="F32" s="328"/>
       <c r="G32" s="17"/>
       <c r="H32" s="18"/>
     </row>
@@ -16069,11 +16338,11 @@
       <c r="C33" s="118" t="s">
         <v>614</v>
       </c>
-      <c r="D33" s="322" t="s">
+      <c r="D33" s="328" t="s">
         <v>482</v>
       </c>
-      <c r="E33" s="322"/>
-      <c r="F33" s="322"/>
+      <c r="E33" s="328"/>
+      <c r="F33" s="328"/>
       <c r="G33" s="17"/>
       <c r="H33" s="18"/>
     </row>
@@ -16085,11 +16354,11 @@
       <c r="C34" s="118" t="s">
         <v>615</v>
       </c>
-      <c r="D34" s="322" t="s">
+      <c r="D34" s="328" t="s">
         <v>575</v>
       </c>
-      <c r="E34" s="322"/>
-      <c r="F34" s="322"/>
+      <c r="E34" s="328"/>
+      <c r="F34" s="328"/>
       <c r="G34" s="17"/>
       <c r="H34" s="18"/>
     </row>
@@ -16101,11 +16370,11 @@
       <c r="C35" s="118" t="s">
         <v>616</v>
       </c>
-      <c r="D35" s="322" t="s">
+      <c r="D35" s="328" t="s">
         <v>576</v>
       </c>
-      <c r="E35" s="322"/>
-      <c r="F35" s="322"/>
+      <c r="E35" s="328"/>
+      <c r="F35" s="328"/>
       <c r="G35" s="17"/>
       <c r="H35" s="18"/>
     </row>
@@ -16115,11 +16384,11 @@
       <c r="C36" s="118" t="s">
         <v>651</v>
       </c>
-      <c r="D36" s="319" t="s">
+      <c r="D36" s="329" t="s">
         <v>591</v>
       </c>
-      <c r="E36" s="320"/>
-      <c r="F36" s="321"/>
+      <c r="E36" s="330"/>
+      <c r="F36" s="331"/>
       <c r="G36" s="17"/>
       <c r="H36" s="18"/>
     </row>
@@ -16129,11 +16398,11 @@
       <c r="C37" s="118" t="s">
         <v>654</v>
       </c>
-      <c r="D37" s="319" t="s">
+      <c r="D37" s="329" t="s">
         <v>652</v>
       </c>
-      <c r="E37" s="320"/>
-      <c r="F37" s="321"/>
+      <c r="E37" s="330"/>
+      <c r="F37" s="331"/>
       <c r="G37" s="17"/>
       <c r="H37" s="18"/>
     </row>
@@ -16143,11 +16412,11 @@
       <c r="C38" s="118" t="s">
         <v>653</v>
       </c>
-      <c r="D38" s="319" t="s">
+      <c r="D38" s="329" t="s">
         <v>655</v>
       </c>
-      <c r="E38" s="320"/>
-      <c r="F38" s="321"/>
+      <c r="E38" s="330"/>
+      <c r="F38" s="331"/>
       <c r="G38" s="17"/>
       <c r="H38" s="18"/>
     </row>
@@ -16155,9 +16424,9 @@
       <c r="A39" s="16"/>
       <c r="B39" s="120"/>
       <c r="C39" s="118"/>
-      <c r="D39" s="319"/>
-      <c r="E39" s="320"/>
-      <c r="F39" s="321"/>
+      <c r="D39" s="329"/>
+      <c r="E39" s="330"/>
+      <c r="F39" s="331"/>
       <c r="G39" s="17"/>
       <c r="H39" s="18"/>
     </row>
@@ -16255,6 +16524,13 @@
     <row r="52" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:H3"/>
@@ -16264,13 +16540,6 @@
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -18033,28 +18302,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="361" t="s">
+      <c r="A1" s="373" t="s">
         <v>952</v>
       </c>
-      <c r="B1" s="362"/>
-      <c r="C1" s="362"/>
-      <c r="D1" s="362"/>
-      <c r="E1" s="362"/>
-      <c r="F1" s="363"/>
+      <c r="B1" s="374"/>
+      <c r="C1" s="374"/>
+      <c r="D1" s="374"/>
+      <c r="E1" s="374"/>
+      <c r="F1" s="375"/>
       <c r="G1" s="175"/>
       <c r="H1" s="175"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="364" t="s">
+      <c r="A2" s="376" t="s">
         <v>840</v>
       </c>
-      <c r="B2" s="365"/>
-      <c r="C2" s="366"/>
-      <c r="D2" s="364" t="s">
+      <c r="B2" s="377"/>
+      <c r="C2" s="378"/>
+      <c r="D2" s="376" t="s">
         <v>841</v>
       </c>
-      <c r="E2" s="365"/>
-      <c r="F2" s="366"/>
+      <c r="E2" s="377"/>
+      <c r="F2" s="378"/>
       <c r="G2" s="175"/>
       <c r="H2" s="175"/>
     </row>
@@ -18078,7 +18347,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="175"/>
-      <c r="H3" s="367" t="s">
+      <c r="H3" s="370" t="s">
         <v>844</v>
       </c>
     </row>
@@ -18102,7 +18371,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="175"/>
-      <c r="H4" s="368"/>
+      <c r="H4" s="371"/>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A5" s="176">
@@ -18124,7 +18393,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="175"/>
-      <c r="H5" s="368"/>
+      <c r="H5" s="371"/>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A6" s="179">
@@ -18146,7 +18415,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="175"/>
-      <c r="H6" s="368"/>
+      <c r="H6" s="371"/>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A7" s="179">
@@ -18168,7 +18437,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="175"/>
-      <c r="H7" s="368"/>
+      <c r="H7" s="371"/>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A8" s="182">
@@ -18190,7 +18459,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="175"/>
-      <c r="H8" s="368"/>
+      <c r="H8" s="371"/>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A9" s="182">
@@ -18212,7 +18481,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="175"/>
-      <c r="H9" s="368"/>
+      <c r="H9" s="371"/>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A10" s="185">
@@ -18234,7 +18503,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="175"/>
-      <c r="H10" s="369"/>
+      <c r="H10" s="372"/>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="188">
@@ -18256,7 +18525,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="175"/>
-      <c r="H11" s="370" t="s">
+      <c r="H11" s="361" t="s">
         <v>856</v>
       </c>
     </row>
@@ -18280,7 +18549,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="175"/>
-      <c r="H12" s="371"/>
+      <c r="H12" s="362"/>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A13" s="191">
@@ -18302,7 +18571,7 @@
         <v>11</v>
       </c>
       <c r="G13" s="175"/>
-      <c r="H13" s="371"/>
+      <c r="H13" s="362"/>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A14" s="191">
@@ -18324,7 +18593,7 @@
         <v>12</v>
       </c>
       <c r="G14" s="175"/>
-      <c r="H14" s="371"/>
+      <c r="H14" s="362"/>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A15" s="195">
@@ -18346,7 +18615,7 @@
         <v>13</v>
       </c>
       <c r="G15" s="175"/>
-      <c r="H15" s="371"/>
+      <c r="H15" s="362"/>
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A16" s="195">
@@ -18368,7 +18637,7 @@
         <v>14</v>
       </c>
       <c r="G16" s="175"/>
-      <c r="H16" s="371"/>
+      <c r="H16" s="362"/>
     </row>
     <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A17" s="195">
@@ -18390,7 +18659,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="175"/>
-      <c r="H17" s="371"/>
+      <c r="H17" s="362"/>
     </row>
     <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A18" s="195">
@@ -18412,7 +18681,7 @@
         <v>16</v>
       </c>
       <c r="G18" s="175"/>
-      <c r="H18" s="371"/>
+      <c r="H18" s="362"/>
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A19" s="195">
@@ -18434,7 +18703,7 @@
         <v>17</v>
       </c>
       <c r="G19" s="175"/>
-      <c r="H19" s="371"/>
+      <c r="H19" s="362"/>
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A20" s="198">
@@ -18456,7 +18725,7 @@
         <v>18</v>
       </c>
       <c r="G20" s="175"/>
-      <c r="H20" s="371"/>
+      <c r="H20" s="362"/>
     </row>
     <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A21" s="198">
@@ -18478,7 +18747,7 @@
         <v>19</v>
       </c>
       <c r="G21" s="175"/>
-      <c r="H21" s="371"/>
+      <c r="H21" s="362"/>
     </row>
     <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A22" s="201">
@@ -18500,7 +18769,7 @@
         <v>20</v>
       </c>
       <c r="G22" s="175"/>
-      <c r="H22" s="372"/>
+      <c r="H22" s="363"/>
     </row>
     <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1"/>
@@ -18518,28 +18787,28 @@
     <row r="36" spans="1:8" ht="20.100000000000001" customHeight="1"/>
     <row r="37" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1"/>
     <row r="38" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A38" s="373" t="s">
+      <c r="A38" s="364" t="s">
         <v>953</v>
       </c>
-      <c r="B38" s="374"/>
-      <c r="C38" s="374"/>
-      <c r="D38" s="374"/>
-      <c r="E38" s="374"/>
-      <c r="F38" s="375"/>
+      <c r="B38" s="365"/>
+      <c r="C38" s="365"/>
+      <c r="D38" s="365"/>
+      <c r="E38" s="365"/>
+      <c r="F38" s="366"/>
       <c r="G38" s="175"/>
       <c r="H38" s="175"/>
     </row>
     <row r="39" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A39" s="376" t="s">
+      <c r="A39" s="367" t="s">
         <v>840</v>
       </c>
-      <c r="B39" s="377"/>
-      <c r="C39" s="378"/>
-      <c r="D39" s="376" t="s">
+      <c r="B39" s="368"/>
+      <c r="C39" s="369"/>
+      <c r="D39" s="367" t="s">
         <v>841</v>
       </c>
-      <c r="E39" s="377"/>
-      <c r="F39" s="378"/>
+      <c r="E39" s="368"/>
+      <c r="F39" s="369"/>
       <c r="G39" s="175"/>
       <c r="H39" s="175"/>
     </row>
@@ -18563,7 +18832,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="175"/>
-      <c r="H40" s="367" t="s">
+      <c r="H40" s="370" t="s">
         <v>844</v>
       </c>
     </row>
@@ -18587,7 +18856,7 @@
         <v>2</v>
       </c>
       <c r="G41" s="175"/>
-      <c r="H41" s="368"/>
+      <c r="H41" s="371"/>
     </row>
     <row r="42" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A42" s="204">
@@ -18609,7 +18878,7 @@
         <v>3</v>
       </c>
       <c r="G42" s="175"/>
-      <c r="H42" s="368"/>
+      <c r="H42" s="371"/>
     </row>
     <row r="43" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A43" s="206">
@@ -18631,7 +18900,7 @@
         <v>4</v>
       </c>
       <c r="G43" s="175"/>
-      <c r="H43" s="368"/>
+      <c r="H43" s="371"/>
     </row>
     <row r="44" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A44" s="206">
@@ -18653,7 +18922,7 @@
         <v>5</v>
       </c>
       <c r="G44" s="175"/>
-      <c r="H44" s="368"/>
+      <c r="H44" s="371"/>
     </row>
     <row r="45" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A45" s="208">
@@ -18675,7 +18944,7 @@
         <v>6</v>
       </c>
       <c r="G45" s="175"/>
-      <c r="H45" s="368"/>
+      <c r="H45" s="371"/>
     </row>
     <row r="46" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A46" s="208">
@@ -18697,7 +18966,7 @@
         <v>7</v>
       </c>
       <c r="G46" s="175"/>
-      <c r="H46" s="368"/>
+      <c r="H46" s="371"/>
     </row>
     <row r="47" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A47" s="210">
@@ -18719,7 +18988,7 @@
         <v>8</v>
       </c>
       <c r="G47" s="175"/>
-      <c r="H47" s="369"/>
+      <c r="H47" s="372"/>
     </row>
     <row r="48" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="A48" s="213">
@@ -18741,7 +19010,7 @@
         <v>9</v>
       </c>
       <c r="G48" s="175"/>
-      <c r="H48" s="370" t="s">
+      <c r="H48" s="361" t="s">
         <v>856</v>
       </c>
     </row>
@@ -18765,7 +19034,7 @@
         <v>10</v>
       </c>
       <c r="G49" s="175"/>
-      <c r="H49" s="371"/>
+      <c r="H49" s="362"/>
     </row>
     <row r="50" spans="1:8" ht="16.5" thickBot="1">
       <c r="A50" s="215">
@@ -18787,7 +19056,7 @@
         <v>11</v>
       </c>
       <c r="G50" s="175"/>
-      <c r="H50" s="371"/>
+      <c r="H50" s="362"/>
     </row>
     <row r="51" spans="1:8" ht="16.5" thickBot="1">
       <c r="A51" s="218">
@@ -18809,7 +19078,7 @@
         <v>12</v>
       </c>
       <c r="G51" s="175"/>
-      <c r="H51" s="371"/>
+      <c r="H51" s="362"/>
     </row>
     <row r="52" spans="1:8" ht="16.5" thickBot="1">
       <c r="A52" s="218">
@@ -18831,7 +19100,7 @@
         <v>13</v>
       </c>
       <c r="G52" s="175"/>
-      <c r="H52" s="371"/>
+      <c r="H52" s="362"/>
     </row>
     <row r="53" spans="1:8" ht="16.5" thickBot="1">
       <c r="A53" s="218">
@@ -18853,7 +19122,7 @@
         <v>14</v>
       </c>
       <c r="G53" s="175"/>
-      <c r="H53" s="371"/>
+      <c r="H53" s="362"/>
     </row>
     <row r="54" spans="1:8" ht="16.5" thickBot="1">
       <c r="A54" s="218">
@@ -18875,7 +19144,7 @@
         <v>15</v>
       </c>
       <c r="G54" s="175"/>
-      <c r="H54" s="371"/>
+      <c r="H54" s="362"/>
     </row>
     <row r="55" spans="1:8" ht="16.5" thickBot="1">
       <c r="A55" s="218">
@@ -18897,7 +19166,7 @@
         <v>16</v>
       </c>
       <c r="G55" s="175"/>
-      <c r="H55" s="371"/>
+      <c r="H55" s="362"/>
     </row>
     <row r="56" spans="1:8" ht="16.5" thickBot="1">
       <c r="A56" s="218">
@@ -18919,7 +19188,7 @@
         <v>17</v>
       </c>
       <c r="G56" s="175"/>
-      <c r="H56" s="371"/>
+      <c r="H56" s="362"/>
     </row>
     <row r="57" spans="1:8" ht="16.5" thickBot="1">
       <c r="A57" s="220">
@@ -18941,7 +19210,7 @@
         <v>18</v>
       </c>
       <c r="G57" s="175"/>
-      <c r="H57" s="371"/>
+      <c r="H57" s="362"/>
     </row>
     <row r="58" spans="1:8" ht="16.5" thickBot="1">
       <c r="A58" s="220">
@@ -18963,7 +19232,7 @@
         <v>19</v>
       </c>
       <c r="G58" s="175"/>
-      <c r="H58" s="371"/>
+      <c r="H58" s="362"/>
     </row>
     <row r="59" spans="1:8" ht="16.5" thickBot="1">
       <c r="A59" s="222">
@@ -18985,21 +19254,21 @@
         <v>20</v>
       </c>
       <c r="G59" s="175"/>
-      <c r="H59" s="372"/>
+      <c r="H59" s="363"/>
     </row>
     <row r="60" spans="1:8" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="H3:H10"/>
+    <mergeCell ref="H11:H22"/>
     <mergeCell ref="H48:H59"/>
     <mergeCell ref="A38:F38"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="D39:F39"/>
     <mergeCell ref="H40:H47"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="H3:H10"/>
-    <mergeCell ref="H11:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -19566,40 +19835,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="323" t="s">
+      <c r="A1" s="319" t="s">
         <v>488</v>
       </c>
-      <c r="B1" s="324"/>
-      <c r="C1" s="324"/>
-      <c r="D1" s="324"/>
-      <c r="E1" s="324"/>
-      <c r="F1" s="324"/>
-      <c r="G1" s="324"/>
-      <c r="H1" s="325"/>
+      <c r="B1" s="320"/>
+      <c r="C1" s="320"/>
+      <c r="D1" s="320"/>
+      <c r="E1" s="320"/>
+      <c r="F1" s="320"/>
+      <c r="G1" s="320"/>
+      <c r="H1" s="321"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="326"/>
-      <c r="B2" s="327"/>
-      <c r="C2" s="327"/>
-      <c r="D2" s="327"/>
-      <c r="E2" s="327"/>
-      <c r="F2" s="327"/>
-      <c r="G2" s="327"/>
-      <c r="H2" s="328"/>
+      <c r="A2" s="322"/>
+      <c r="B2" s="323"/>
+      <c r="C2" s="323"/>
+      <c r="D2" s="323"/>
+      <c r="E2" s="323"/>
+      <c r="F2" s="323"/>
+      <c r="G2" s="323"/>
+      <c r="H2" s="324"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="329" t="s">
+      <c r="A3" s="325" t="s">
         <v>319</v>
       </c>
-      <c r="B3" s="330"/>
-      <c r="C3" s="330"/>
-      <c r="D3" s="330"/>
-      <c r="E3" s="330" t="s">
+      <c r="B3" s="326"/>
+      <c r="C3" s="326"/>
+      <c r="D3" s="326"/>
+      <c r="E3" s="326" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="330"/>
-      <c r="G3" s="330"/>
-      <c r="H3" s="331"/>
+      <c r="F3" s="326"/>
+      <c r="G3" s="326"/>
+      <c r="H3" s="327"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="12">

</xml_diff>

<commit_message>
chg: Adjusted Kallax TWR freq
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -3794,9 +3794,6 @@
     <t>#IFF:5613FR</t>
   </si>
   <si>
-    <t>128.22</t>
-  </si>
-  <si>
     <t>AN/ARC-159 PILOT</t>
   </si>
   <si>
@@ -4035,6 +4032,9 @@
   </si>
   <si>
     <t>JOKKMOKK</t>
+  </si>
+  <si>
+    <t>128.4</t>
   </si>
 </sst>
 </file>
@@ -6687,9 +6687,22 @@
     <xf numFmtId="49" fontId="47" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6699,16 +6712,49 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6720,50 +6766,17 @@
     <xf numFmtId="0" fontId="24" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6792,18 +6805,6 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6891,6 +6892,33 @@
     <xf numFmtId="49" fontId="45" fillId="31" borderId="93" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="26" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6918,33 +6946,6 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7017,6 +7018,57 @@
     <xf numFmtId="0" fontId="32" fillId="20" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7035,58 +7087,6 @@
     <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7399,8 +7399,8 @@
   <sheetPr codeName="Ark1"/>
   <dimension ref="A1:AP83"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N70" sqref="N70"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M67" sqref="M67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -7507,13 +7507,13 @@
       <c r="N2" s="107" t="s">
         <v>330</v>
       </c>
-      <c r="V2" s="293" t="s">
+      <c r="V2" s="295" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="293"/>
-      <c r="X2" s="293"/>
-      <c r="Y2" s="293"/>
-      <c r="Z2" s="293"/>
+      <c r="W2" s="295"/>
+      <c r="X2" s="295"/>
+      <c r="Y2" s="295"/>
+      <c r="Z2" s="295"/>
     </row>
     <row r="3" spans="1:42">
       <c r="A3" s="107" t="s">
@@ -7562,9 +7562,9 @@
       <c r="P3" t="s">
         <v>426</v>
       </c>
-      <c r="R3" s="297"/>
-      <c r="S3" s="297"/>
-      <c r="T3" s="297"/>
+      <c r="R3" s="294"/>
+      <c r="S3" s="294"/>
+      <c r="T3" s="294"/>
       <c r="V3" s="101" t="s">
         <v>328</v>
       </c>
@@ -7646,22 +7646,22 @@
       <c r="AA4" s="23"/>
       <c r="AB4" s="23"/>
       <c r="AC4" s="23"/>
-      <c r="AD4" s="293" t="s">
+      <c r="AD4" s="295" t="s">
         <v>429</v>
       </c>
-      <c r="AE4" s="293"/>
-      <c r="AF4" s="293"/>
-      <c r="AG4" s="293"/>
-      <c r="AH4" s="293"/>
-      <c r="AJ4" s="293" t="s">
+      <c r="AE4" s="295"/>
+      <c r="AF4" s="295"/>
+      <c r="AG4" s="295"/>
+      <c r="AH4" s="295"/>
+      <c r="AJ4" s="295" t="s">
         <v>1</v>
       </c>
-      <c r="AK4" s="293"/>
-      <c r="AL4" s="293"/>
-      <c r="AM4" s="293"/>
-      <c r="AN4" s="293"/>
-      <c r="AO4" s="293"/>
-      <c r="AP4" s="293"/>
+      <c r="AK4" s="295"/>
+      <c r="AL4" s="295"/>
+      <c r="AM4" s="295"/>
+      <c r="AN4" s="295"/>
+      <c r="AO4" s="295"/>
+      <c r="AP4" s="295"/>
     </row>
     <row r="5" spans="1:42" ht="15.75">
       <c r="A5" s="107" t="s">
@@ -8877,15 +8877,15 @@
       <c r="AH18" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="AJ18" s="293" t="s">
+      <c r="AJ18" s="295" t="s">
         <v>274</v>
       </c>
-      <c r="AK18" s="293"/>
-      <c r="AL18" s="293"/>
-      <c r="AM18" s="293"/>
-      <c r="AN18" s="293"/>
-      <c r="AO18" s="293"/>
-      <c r="AP18" s="293"/>
+      <c r="AK18" s="295"/>
+      <c r="AL18" s="295"/>
+      <c r="AM18" s="295"/>
+      <c r="AN18" s="295"/>
+      <c r="AO18" s="295"/>
+      <c r="AP18" s="295"/>
     </row>
     <row r="19" spans="1:42" ht="15.75">
       <c r="A19" s="107" t="s">
@@ -9018,9 +9018,9 @@
       </c>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="297"/>
-      <c r="S20" s="297"/>
-      <c r="T20" s="297"/>
+      <c r="R20" s="294"/>
+      <c r="S20" s="294"/>
+      <c r="T20" s="294"/>
       <c r="U20" s="2"/>
       <c r="V20" s="272" t="s">
         <v>1253</v>
@@ -9435,13 +9435,13 @@
       <c r="S25" s="24"/>
       <c r="T25" s="24"/>
       <c r="X25" s="2"/>
-      <c r="AD25" s="293" t="s">
+      <c r="AD25" s="295" t="s">
         <v>486</v>
       </c>
-      <c r="AE25" s="293"/>
-      <c r="AF25" s="293"/>
-      <c r="AG25" s="293"/>
-      <c r="AH25" s="293"/>
+      <c r="AE25" s="295"/>
+      <c r="AF25" s="295"/>
+      <c r="AG25" s="295"/>
+      <c r="AH25" s="295"/>
       <c r="AJ25" s="116" t="s">
         <v>555</v>
       </c>
@@ -9691,15 +9691,15 @@
       <c r="N29" s="107" t="s">
         <v>355</v>
       </c>
-      <c r="V29" s="293" t="s">
+      <c r="V29" s="295" t="s">
         <v>212</v>
       </c>
-      <c r="W29" s="293"/>
-      <c r="X29" s="293"/>
-      <c r="Y29" s="293"/>
-      <c r="Z29" s="293"/>
-      <c r="AA29" s="293"/>
-      <c r="AB29" s="293"/>
+      <c r="W29" s="295"/>
+      <c r="X29" s="295"/>
+      <c r="Y29" s="295"/>
+      <c r="Z29" s="295"/>
+      <c r="AA29" s="295"/>
+      <c r="AB29" s="295"/>
     </row>
     <row r="30" spans="1:42">
       <c r="A30" s="107"/>
@@ -9755,15 +9755,15 @@
       </c>
       <c r="AA30" s="29"/>
       <c r="AB30" s="29"/>
-      <c r="AJ30" s="293" t="s">
+      <c r="AJ30" s="295" t="s">
         <v>831</v>
       </c>
-      <c r="AK30" s="293"/>
-      <c r="AL30" s="293"/>
-      <c r="AM30" s="293"/>
-      <c r="AN30" s="293"/>
-      <c r="AO30" s="293"/>
-      <c r="AP30" s="293"/>
+      <c r="AK30" s="295"/>
+      <c r="AL30" s="295"/>
+      <c r="AM30" s="295"/>
+      <c r="AN30" s="295"/>
+      <c r="AO30" s="295"/>
+      <c r="AP30" s="295"/>
     </row>
     <row r="31" spans="1:42">
       <c r="B31" s="24"/>
@@ -9850,15 +9850,15 @@
       <c r="AJ34" s="23"/>
     </row>
     <row r="37" spans="22:36">
-      <c r="V37" s="293" t="s">
+      <c r="V37" s="295" t="s">
         <v>9</v>
       </c>
-      <c r="W37" s="293"/>
-      <c r="X37" s="293"/>
-      <c r="Y37" s="293"/>
-      <c r="Z37" s="293"/>
-      <c r="AA37" s="293"/>
-      <c r="AB37" s="293"/>
+      <c r="W37" s="295"/>
+      <c r="X37" s="295"/>
+      <c r="Y37" s="295"/>
+      <c r="Z37" s="295"/>
+      <c r="AA37" s="295"/>
+      <c r="AB37" s="295"/>
     </row>
     <row r="38" spans="22:36">
       <c r="V38" s="29" t="s">
@@ -9878,11 +9878,11 @@
       </c>
       <c r="AA38" s="29"/>
       <c r="AB38" s="29"/>
-      <c r="AD38" s="298" t="s">
+      <c r="AD38" s="296" t="s">
         <v>260</v>
       </c>
-      <c r="AE38" s="299"/>
-      <c r="AF38" s="300"/>
+      <c r="AE38" s="297"/>
+      <c r="AF38" s="298"/>
     </row>
     <row r="39" spans="22:36">
       <c r="V39" s="3" t="s">
@@ -9919,15 +9919,15 @@
       <c r="AF41" s="3"/>
     </row>
     <row r="42" spans="22:36">
-      <c r="V42" s="293" t="s">
+      <c r="V42" s="295" t="s">
         <v>244</v>
       </c>
-      <c r="W42" s="293"/>
-      <c r="X42" s="293"/>
-      <c r="Y42" s="293"/>
-      <c r="Z42" s="293"/>
-      <c r="AA42" s="293"/>
-      <c r="AB42" s="293"/>
+      <c r="W42" s="295"/>
+      <c r="X42" s="295"/>
+      <c r="Y42" s="295"/>
+      <c r="Z42" s="295"/>
+      <c r="AA42" s="295"/>
+      <c r="AB42" s="295"/>
       <c r="AD42" s="3" t="s">
         <v>254</v>
       </c>
@@ -9997,15 +9997,15 @@
       <c r="AF47" s="3"/>
     </row>
     <row r="48" spans="22:36">
-      <c r="V48" s="294" t="s">
+      <c r="V48" s="299" t="s">
         <v>473</v>
       </c>
-      <c r="W48" s="295"/>
-      <c r="X48" s="295"/>
-      <c r="Y48" s="295"/>
-      <c r="Z48" s="295"/>
-      <c r="AA48" s="295"/>
-      <c r="AB48" s="296"/>
+      <c r="W48" s="300"/>
+      <c r="X48" s="300"/>
+      <c r="Y48" s="300"/>
+      <c r="Z48" s="300"/>
+      <c r="AA48" s="300"/>
+      <c r="AB48" s="301"/>
       <c r="AD48" s="3" t="s">
         <v>261</v>
       </c>
@@ -10278,7 +10278,7 @@
         <v>906</v>
       </c>
       <c r="X63" s="226" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="Y63" s="226"/>
       <c r="Z63" s="226"/>
@@ -10295,7 +10295,7 @@
         <v>249</v>
       </c>
       <c r="X64" s="3" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="Y64" s="3"/>
       <c r="Z64" s="3"/>
@@ -10442,7 +10442,7 @@
         <v>249</v>
       </c>
       <c r="X73" s="3" t="s">
-        <v>1256</v>
+        <v>1336</v>
       </c>
       <c r="Y73" s="3"/>
       <c r="Z73" s="3"/>
@@ -10615,6 +10615,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="V42:AB42"/>
+    <mergeCell ref="AD4:AH4"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="V48:AB48"/>
+    <mergeCell ref="V37:AB37"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="AJ4:AP4"/>
@@ -10623,11 +10628,6 @@
     <mergeCell ref="V29:AB29"/>
     <mergeCell ref="AD25:AH25"/>
     <mergeCell ref="AJ30:AP30"/>
-    <mergeCell ref="V42:AB42"/>
-    <mergeCell ref="AD4:AH4"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="V48:AB48"/>
-    <mergeCell ref="V37:AB37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10655,40 +10655,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="391" t="s">
+      <c r="A1" s="392" t="s">
         <v>487</v>
       </c>
-      <c r="B1" s="392"/>
-      <c r="C1" s="392"/>
-      <c r="D1" s="392"/>
-      <c r="E1" s="392"/>
-      <c r="F1" s="392"/>
-      <c r="G1" s="392"/>
-      <c r="H1" s="393"/>
+      <c r="B1" s="393"/>
+      <c r="C1" s="393"/>
+      <c r="D1" s="393"/>
+      <c r="E1" s="393"/>
+      <c r="F1" s="393"/>
+      <c r="G1" s="393"/>
+      <c r="H1" s="394"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="394"/>
-      <c r="B2" s="395"/>
-      <c r="C2" s="395"/>
-      <c r="D2" s="395"/>
-      <c r="E2" s="395"/>
-      <c r="F2" s="395"/>
-      <c r="G2" s="395"/>
-      <c r="H2" s="396"/>
+      <c r="A2" s="395"/>
+      <c r="B2" s="396"/>
+      <c r="C2" s="396"/>
+      <c r="D2" s="396"/>
+      <c r="E2" s="396"/>
+      <c r="F2" s="396"/>
+      <c r="G2" s="396"/>
+      <c r="H2" s="397"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="397" t="s">
+      <c r="A3" s="398" t="s">
         <v>751</v>
       </c>
-      <c r="B3" s="398"/>
-      <c r="C3" s="398"/>
-      <c r="D3" s="399"/>
-      <c r="E3" s="397" t="s">
+      <c r="B3" s="399"/>
+      <c r="C3" s="399"/>
+      <c r="D3" s="400"/>
+      <c r="E3" s="398" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="398"/>
-      <c r="G3" s="398"/>
-      <c r="H3" s="399"/>
+      <c r="F3" s="399"/>
+      <c r="G3" s="399"/>
+      <c r="H3" s="400"/>
     </row>
     <row r="4" spans="1:8" ht="16.5">
       <c r="A4" s="166">
@@ -11161,18 +11161,18 @@
       <c r="H24" s="146"/>
     </row>
     <row r="25" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A25" s="400" t="s">
+      <c r="A25" s="401" t="s">
         <v>314</v>
       </c>
-      <c r="B25" s="401"/>
-      <c r="C25" s="401"/>
-      <c r="D25" s="402"/>
-      <c r="E25" s="400" t="s">
+      <c r="B25" s="402"/>
+      <c r="C25" s="402"/>
+      <c r="D25" s="403"/>
+      <c r="E25" s="401" t="s">
         <v>801</v>
       </c>
-      <c r="F25" s="401"/>
-      <c r="G25" s="401"/>
-      <c r="H25" s="402"/>
+      <c r="F25" s="402"/>
+      <c r="G25" s="402"/>
+      <c r="H25" s="403"/>
     </row>
     <row r="26" spans="1:8" ht="16.5">
       <c r="A26" s="155">
@@ -11587,40 +11587,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="403" t="s">
+      <c r="A1" s="421" t="s">
         <v>326</v>
       </c>
-      <c r="B1" s="403"/>
-      <c r="C1" s="403"/>
-      <c r="D1" s="403"/>
-      <c r="E1" s="403"/>
-      <c r="F1" s="403"/>
-      <c r="G1" s="403"/>
-      <c r="H1" s="403"/>
+      <c r="B1" s="421"/>
+      <c r="C1" s="421"/>
+      <c r="D1" s="421"/>
+      <c r="E1" s="421"/>
+      <c r="F1" s="421"/>
+      <c r="G1" s="421"/>
+      <c r="H1" s="421"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="404"/>
-      <c r="B2" s="404"/>
-      <c r="C2" s="404"/>
-      <c r="D2" s="404"/>
-      <c r="E2" s="404"/>
-      <c r="F2" s="404"/>
-      <c r="G2" s="404"/>
-      <c r="H2" s="404"/>
+      <c r="A2" s="422"/>
+      <c r="B2" s="422"/>
+      <c r="C2" s="422"/>
+      <c r="D2" s="422"/>
+      <c r="E2" s="422"/>
+      <c r="F2" s="422"/>
+      <c r="G2" s="422"/>
+      <c r="H2" s="422"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="405" t="s">
+      <c r="A3" s="423" t="s">
         <v>227</v>
       </c>
-      <c r="B3" s="406"/>
-      <c r="C3" s="407"/>
-      <c r="D3" s="408"/>
-      <c r="E3" s="405" t="s">
+      <c r="B3" s="424"/>
+      <c r="C3" s="425"/>
+      <c r="D3" s="426"/>
+      <c r="E3" s="423" t="s">
         <v>228</v>
       </c>
-      <c r="F3" s="406"/>
-      <c r="G3" s="407"/>
-      <c r="H3" s="408"/>
+      <c r="F3" s="424"/>
+      <c r="G3" s="425"/>
+      <c r="H3" s="426"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="31">
@@ -11913,114 +11913,114 @@
       <c r="H24" s="59"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="405" t="s">
+      <c r="A25" s="423" t="s">
         <v>289</v>
       </c>
-      <c r="B25" s="406"/>
-      <c r="C25" s="407"/>
-      <c r="D25" s="408"/>
-      <c r="E25" s="405" t="s">
+      <c r="B25" s="424"/>
+      <c r="C25" s="425"/>
+      <c r="D25" s="426"/>
+      <c r="E25" s="423" t="s">
         <v>290</v>
       </c>
-      <c r="F25" s="406"/>
-      <c r="G25" s="407"/>
-      <c r="H25" s="408"/>
+      <c r="F25" s="424"/>
+      <c r="G25" s="425"/>
+      <c r="H25" s="426"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="35" t="s">
         <v>291</v>
       </c>
-      <c r="B26" s="409"/>
-      <c r="C26" s="410"/>
-      <c r="D26" s="411"/>
+      <c r="B26" s="410"/>
+      <c r="C26" s="411"/>
+      <c r="D26" s="412"/>
       <c r="E26" s="31" t="s">
         <v>292</v>
       </c>
-      <c r="F26" s="412"/>
-      <c r="G26" s="413"/>
-      <c r="H26" s="414"/>
+      <c r="F26" s="418"/>
+      <c r="G26" s="419"/>
+      <c r="H26" s="420"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="B27" s="415"/>
-      <c r="C27" s="416"/>
-      <c r="D27" s="417"/>
+      <c r="B27" s="413"/>
+      <c r="C27" s="414"/>
+      <c r="D27" s="416"/>
       <c r="E27" s="35" t="s">
         <v>294</v>
       </c>
-      <c r="F27" s="409"/>
-      <c r="G27" s="410"/>
-      <c r="H27" s="418"/>
+      <c r="F27" s="410"/>
+      <c r="G27" s="411"/>
+      <c r="H27" s="417"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="35" t="s">
         <v>295</v>
       </c>
-      <c r="B28" s="409"/>
-      <c r="C28" s="410"/>
-      <c r="D28" s="411"/>
+      <c r="B28" s="410"/>
+      <c r="C28" s="411"/>
+      <c r="D28" s="412"/>
       <c r="E28" s="43" t="s">
         <v>296</v>
       </c>
-      <c r="F28" s="415"/>
-      <c r="G28" s="416"/>
-      <c r="H28" s="419"/>
+      <c r="F28" s="413"/>
+      <c r="G28" s="414"/>
+      <c r="H28" s="415"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="43" t="s">
         <v>297</v>
       </c>
-      <c r="B29" s="415"/>
-      <c r="C29" s="416"/>
-      <c r="D29" s="417"/>
+      <c r="B29" s="413"/>
+      <c r="C29" s="414"/>
+      <c r="D29" s="416"/>
       <c r="E29" s="35" t="s">
         <v>298</v>
       </c>
-      <c r="F29" s="409"/>
-      <c r="G29" s="410"/>
-      <c r="H29" s="418"/>
+      <c r="F29" s="410"/>
+      <c r="G29" s="411"/>
+      <c r="H29" s="417"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="35" t="s">
         <v>299</v>
       </c>
-      <c r="B30" s="409"/>
-      <c r="C30" s="410"/>
-      <c r="D30" s="411"/>
+      <c r="B30" s="410"/>
+      <c r="C30" s="411"/>
+      <c r="D30" s="412"/>
       <c r="E30" s="43" t="s">
         <v>300</v>
       </c>
-      <c r="F30" s="415"/>
-      <c r="G30" s="416"/>
-      <c r="H30" s="419"/>
+      <c r="F30" s="413"/>
+      <c r="G30" s="414"/>
+      <c r="H30" s="415"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="43" t="s">
         <v>301</v>
       </c>
-      <c r="B31" s="415"/>
-      <c r="C31" s="416"/>
-      <c r="D31" s="417"/>
+      <c r="B31" s="413"/>
+      <c r="C31" s="414"/>
+      <c r="D31" s="416"/>
       <c r="E31" s="35" t="s">
         <v>302</v>
       </c>
-      <c r="F31" s="409"/>
-      <c r="G31" s="410"/>
-      <c r="H31" s="418"/>
+      <c r="F31" s="410"/>
+      <c r="G31" s="411"/>
+      <c r="H31" s="417"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="35" t="s">
         <v>303</v>
       </c>
-      <c r="B32" s="409"/>
-      <c r="C32" s="410"/>
-      <c r="D32" s="411"/>
+      <c r="B32" s="410"/>
+      <c r="C32" s="411"/>
+      <c r="D32" s="412"/>
       <c r="E32" s="43"/>
-      <c r="F32" s="415"/>
-      <c r="G32" s="416"/>
-      <c r="H32" s="419" t="s">
+      <c r="F32" s="413"/>
+      <c r="G32" s="414"/>
+      <c r="H32" s="415" t="s">
         <v>242</v>
       </c>
     </row>
@@ -12028,13 +12028,13 @@
       <c r="A33" s="43" t="s">
         <v>304</v>
       </c>
-      <c r="B33" s="415"/>
-      <c r="C33" s="416"/>
-      <c r="D33" s="417"/>
+      <c r="B33" s="413"/>
+      <c r="C33" s="414"/>
+      <c r="D33" s="416"/>
       <c r="E33" s="35"/>
-      <c r="F33" s="409"/>
-      <c r="G33" s="410"/>
-      <c r="H33" s="418" t="s">
+      <c r="F33" s="410"/>
+      <c r="G33" s="411"/>
+      <c r="H33" s="417" t="s">
         <v>284</v>
       </c>
     </row>
@@ -12042,13 +12042,13 @@
       <c r="A34" s="35" t="s">
         <v>305</v>
       </c>
-      <c r="B34" s="409"/>
-      <c r="C34" s="410"/>
-      <c r="D34" s="411"/>
+      <c r="B34" s="410"/>
+      <c r="C34" s="411"/>
+      <c r="D34" s="412"/>
       <c r="E34" s="43"/>
-      <c r="F34" s="415"/>
-      <c r="G34" s="416"/>
-      <c r="H34" s="419" t="s">
+      <c r="F34" s="413"/>
+      <c r="G34" s="414"/>
+      <c r="H34" s="415" t="s">
         <v>285</v>
       </c>
     </row>
@@ -12056,13 +12056,13 @@
       <c r="A35" s="43" t="s">
         <v>306</v>
       </c>
-      <c r="B35" s="415"/>
-      <c r="C35" s="416"/>
-      <c r="D35" s="417"/>
+      <c r="B35" s="413"/>
+      <c r="C35" s="414"/>
+      <c r="D35" s="416"/>
       <c r="E35" s="35"/>
-      <c r="F35" s="409"/>
-      <c r="G35" s="410"/>
-      <c r="H35" s="418" t="s">
+      <c r="F35" s="410"/>
+      <c r="G35" s="411"/>
+      <c r="H35" s="417" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12070,13 +12070,13 @@
       <c r="A36" s="35" t="s">
         <v>307</v>
       </c>
-      <c r="B36" s="409"/>
-      <c r="C36" s="410"/>
-      <c r="D36" s="411"/>
+      <c r="B36" s="410"/>
+      <c r="C36" s="411"/>
+      <c r="D36" s="412"/>
       <c r="E36" s="43"/>
-      <c r="F36" s="415"/>
-      <c r="G36" s="416"/>
-      <c r="H36" s="419" t="s">
+      <c r="F36" s="413"/>
+      <c r="G36" s="414"/>
+      <c r="H36" s="415" t="s">
         <v>287</v>
       </c>
     </row>
@@ -12084,13 +12084,13 @@
       <c r="A37" s="43" t="s">
         <v>308</v>
       </c>
-      <c r="B37" s="415"/>
-      <c r="C37" s="416"/>
-      <c r="D37" s="417"/>
+      <c r="B37" s="413"/>
+      <c r="C37" s="414"/>
+      <c r="D37" s="416"/>
       <c r="E37" s="35"/>
-      <c r="F37" s="409"/>
-      <c r="G37" s="410"/>
-      <c r="H37" s="418" t="s">
+      <c r="F37" s="410"/>
+      <c r="G37" s="411"/>
+      <c r="H37" s="417" t="s">
         <v>288</v>
       </c>
     </row>
@@ -12098,13 +12098,13 @@
       <c r="A38" s="35" t="s">
         <v>309</v>
       </c>
-      <c r="B38" s="409"/>
-      <c r="C38" s="410"/>
-      <c r="D38" s="411"/>
+      <c r="B38" s="410"/>
+      <c r="C38" s="411"/>
+      <c r="D38" s="412"/>
       <c r="E38" s="43"/>
-      <c r="F38" s="415"/>
-      <c r="G38" s="416"/>
-      <c r="H38" s="419" t="s">
+      <c r="F38" s="413"/>
+      <c r="G38" s="414"/>
+      <c r="H38" s="415" t="s">
         <v>241</v>
       </c>
     </row>
@@ -12112,13 +12112,13 @@
       <c r="A39" s="43" t="s">
         <v>310</v>
       </c>
-      <c r="B39" s="415"/>
-      <c r="C39" s="416"/>
-      <c r="D39" s="417"/>
+      <c r="B39" s="413"/>
+      <c r="C39" s="414"/>
+      <c r="D39" s="416"/>
       <c r="E39" s="35"/>
-      <c r="F39" s="409"/>
-      <c r="G39" s="410"/>
-      <c r="H39" s="418" t="s">
+      <c r="F39" s="410"/>
+      <c r="G39" s="411"/>
+      <c r="H39" s="417" t="s">
         <v>242</v>
       </c>
     </row>
@@ -12126,28 +12126,57 @@
       <c r="A40" s="35" t="s">
         <v>311</v>
       </c>
-      <c r="B40" s="409"/>
-      <c r="C40" s="410"/>
-      <c r="D40" s="411"/>
+      <c r="B40" s="410"/>
+      <c r="C40" s="411"/>
+      <c r="D40" s="412"/>
       <c r="E40" s="43"/>
-      <c r="F40" s="415"/>
-      <c r="G40" s="416"/>
-      <c r="H40" s="419"/>
+      <c r="F40" s="413"/>
+      <c r="G40" s="414"/>
+      <c r="H40" s="415"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="55" t="s">
         <v>312</v>
       </c>
-      <c r="B41" s="420"/>
-      <c r="C41" s="421"/>
-      <c r="D41" s="422"/>
+      <c r="B41" s="404"/>
+      <c r="C41" s="405"/>
+      <c r="D41" s="406"/>
       <c r="E41" s="60"/>
-      <c r="F41" s="423"/>
-      <c r="G41" s="424"/>
-      <c r="H41" s="425"/>
+      <c r="F41" s="407"/>
+      <c r="G41" s="408"/>
+      <c r="H41" s="409"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -12156,35 +12185,6 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12195,7 +12195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AP61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AL12" sqref="AL12:AN12"/>
     </sheetView>
   </sheetViews>
@@ -12240,55 +12240,55 @@
       </c>
     </row>
     <row r="2" spans="2:42">
-      <c r="B2" s="293" t="s">
+      <c r="B2" s="295" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="293"/>
-      <c r="D2" s="293"/>
-      <c r="E2" s="293"/>
-      <c r="F2" s="293"/>
-      <c r="H2" s="293" t="s">
+      <c r="C2" s="295"/>
+      <c r="D2" s="295"/>
+      <c r="E2" s="295"/>
+      <c r="F2" s="295"/>
+      <c r="H2" s="295" t="s">
         <v>1055</v>
       </c>
-      <c r="I2" s="293"/>
-      <c r="J2" s="293"/>
-      <c r="K2" s="293"/>
-      <c r="L2" s="293"/>
-      <c r="N2" s="293" t="s">
+      <c r="I2" s="295"/>
+      <c r="J2" s="295"/>
+      <c r="K2" s="295"/>
+      <c r="L2" s="295"/>
+      <c r="N2" s="295" t="s">
         <v>1054</v>
       </c>
-      <c r="O2" s="293"/>
-      <c r="P2" s="293"/>
-      <c r="Q2" s="293"/>
-      <c r="R2" s="293"/>
-      <c r="T2" s="293" t="s">
+      <c r="O2" s="295"/>
+      <c r="P2" s="295"/>
+      <c r="Q2" s="295"/>
+      <c r="R2" s="295"/>
+      <c r="T2" s="295" t="s">
         <v>236</v>
       </c>
-      <c r="U2" s="293"/>
-      <c r="V2" s="293"/>
-      <c r="W2" s="293"/>
-      <c r="X2" s="293"/>
-      <c r="Z2" s="293" t="s">
+      <c r="U2" s="295"/>
+      <c r="V2" s="295"/>
+      <c r="W2" s="295"/>
+      <c r="X2" s="295"/>
+      <c r="Z2" s="295" t="s">
         <v>246</v>
       </c>
-      <c r="AA2" s="293"/>
-      <c r="AB2" s="293"/>
-      <c r="AC2" s="293"/>
-      <c r="AD2" s="293"/>
-      <c r="AF2" s="293" t="s">
+      <c r="AA2" s="295"/>
+      <c r="AB2" s="295"/>
+      <c r="AC2" s="295"/>
+      <c r="AD2" s="295"/>
+      <c r="AF2" s="295" t="s">
         <v>317</v>
       </c>
-      <c r="AG2" s="293"/>
-      <c r="AH2" s="293"/>
-      <c r="AI2" s="293"/>
-      <c r="AJ2" s="293"/>
-      <c r="AL2" s="293" t="s">
+      <c r="AG2" s="295"/>
+      <c r="AH2" s="295"/>
+      <c r="AI2" s="295"/>
+      <c r="AJ2" s="295"/>
+      <c r="AL2" s="295" t="s">
         <v>491</v>
       </c>
-      <c r="AM2" s="293"/>
-      <c r="AN2" s="293"/>
-      <c r="AO2" s="293"/>
-      <c r="AP2" s="293"/>
+      <c r="AM2" s="295"/>
+      <c r="AN2" s="295"/>
+      <c r="AO2" s="295"/>
+      <c r="AP2" s="295"/>
     </row>
     <row r="3" spans="2:42">
       <c r="B3" s="101" t="s">
@@ -13150,7 +13150,7 @@
         <v>1217</v>
       </c>
       <c r="AF16" s="3" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="AG16" s="3" t="s">
         <v>913</v>
@@ -13219,10 +13219,10 @@
       <c r="AI17" s="3"/>
       <c r="AJ17" s="3"/>
       <c r="AL17" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="AM17" s="3" t="s">
         <v>1335</v>
-      </c>
-      <c r="AM17" s="3" t="s">
-        <v>1336</v>
       </c>
       <c r="AN17" s="270">
         <v>641</v>
@@ -13471,8 +13471,8 @@
       <c r="R22" s="104" t="s">
         <v>1130</v>
       </c>
-      <c r="T22" s="426" t="s">
-        <v>1316</v>
+      <c r="T22" s="293" t="s">
+        <v>1315</v>
       </c>
       <c r="U22" s="3" t="s">
         <v>913</v>
@@ -13481,10 +13481,10 @@
         <v>151</v>
       </c>
       <c r="W22" s="270" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="X22" s="104" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="23" spans="1:40">
@@ -13506,10 +13506,10 @@
         <v>152</v>
       </c>
       <c r="W23" s="270" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="X23" s="104" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="24" spans="1:40">
@@ -13551,10 +13551,10 @@
         <v>153</v>
       </c>
       <c r="W24" s="270" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="X24" s="104" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="25" spans="1:40">
@@ -13586,10 +13586,10 @@
         <v>154</v>
       </c>
       <c r="W25" s="270" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="X25" s="104" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="26" spans="1:40">
@@ -13644,8 +13644,8 @@
       <c r="R27" s="104" t="s">
         <v>1126</v>
       </c>
-      <c r="T27" s="426" t="s">
-        <v>1325</v>
+      <c r="T27" s="293" t="s">
+        <v>1324</v>
       </c>
       <c r="U27" s="3" t="s">
         <v>913</v>
@@ -13654,10 +13654,10 @@
         <v>161</v>
       </c>
       <c r="W27" s="270" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="X27" s="104" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="28" spans="1:40">
@@ -13677,10 +13677,10 @@
         <v>162</v>
       </c>
       <c r="W28" s="270" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="X28" s="104" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="29" spans="1:40">
@@ -13720,10 +13720,10 @@
         <v>163</v>
       </c>
       <c r="W29" s="270" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="X29" s="104" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="30" spans="1:40">
@@ -13755,10 +13755,10 @@
         <v>164</v>
       </c>
       <c r="W30" s="270" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="X30" s="104" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="31" spans="1:40">
@@ -13922,20 +13922,20 @@
       <c r="X39" s="59"/>
     </row>
     <row r="41" spans="2:24">
-      <c r="B41" s="293" t="s">
+      <c r="B41" s="295" t="s">
         <v>697</v>
       </c>
-      <c r="C41" s="293"/>
-      <c r="D41" s="293"/>
-      <c r="E41" s="293"/>
-      <c r="F41" s="293"/>
-      <c r="H41" s="293" t="s">
+      <c r="C41" s="295"/>
+      <c r="D41" s="295"/>
+      <c r="E41" s="295"/>
+      <c r="F41" s="295"/>
+      <c r="H41" s="295" t="s">
         <v>750</v>
       </c>
-      <c r="I41" s="293"/>
-      <c r="J41" s="293"/>
-      <c r="K41" s="293"/>
-      <c r="L41" s="293"/>
+      <c r="I41" s="295"/>
+      <c r="J41" s="295"/>
+      <c r="K41" s="295"/>
+      <c r="L41" s="295"/>
     </row>
     <row r="42" spans="2:24">
       <c r="B42" s="101" t="s">
@@ -14472,39 +14472,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27" customHeight="1" thickBot="1">
-      <c r="A1" s="313" t="s">
+      <c r="A1" s="311" t="s">
         <v>1146</v>
       </c>
-      <c r="B1" s="314"/>
-      <c r="C1" s="314"/>
-      <c r="D1" s="314"/>
-      <c r="E1" s="314"/>
-      <c r="F1" s="314"/>
-      <c r="G1" s="314"/>
-      <c r="H1" s="314"/>
-      <c r="I1" s="314"/>
-      <c r="J1" s="314"/>
-      <c r="K1" s="314"/>
-      <c r="L1" s="315"/>
+      <c r="B1" s="312"/>
+      <c r="C1" s="312"/>
+      <c r="D1" s="312"/>
+      <c r="E1" s="312"/>
+      <c r="F1" s="312"/>
+      <c r="G1" s="312"/>
+      <c r="H1" s="312"/>
+      <c r="I1" s="312"/>
+      <c r="J1" s="312"/>
+      <c r="K1" s="312"/>
+      <c r="L1" s="313"/>
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A2" s="310" t="s">
+      <c r="A2" s="308" t="s">
         <v>1147</v>
       </c>
-      <c r="B2" s="311"/>
-      <c r="C2" s="312"/>
+      <c r="B2" s="309"/>
+      <c r="C2" s="310"/>
       <c r="D2" s="259"/>
-      <c r="E2" s="310" t="s">
+      <c r="E2" s="308" t="s">
         <v>1055</v>
       </c>
-      <c r="F2" s="311"/>
-      <c r="G2" s="312"/>
+      <c r="F2" s="309"/>
+      <c r="G2" s="310"/>
       <c r="H2" s="259"/>
-      <c r="I2" s="310" t="s">
+      <c r="I2" s="308" t="s">
         <v>1054</v>
       </c>
-      <c r="J2" s="311"/>
-      <c r="K2" s="312"/>
+      <c r="J2" s="309"/>
+      <c r="K2" s="310"/>
       <c r="L2" s="122"/>
     </row>
     <row r="3" spans="1:12" ht="19.5" thickBot="1">
@@ -14540,7 +14540,7 @@
       <c r="L3" s="122"/>
     </row>
     <row r="4" spans="1:12" ht="18.75">
-      <c r="A4" s="316" t="s">
+      <c r="A4" s="302" t="s">
         <v>325</v>
       </c>
       <c r="B4" s="132" t="s">
@@ -14550,7 +14550,7 @@
         <v>705</v>
       </c>
       <c r="D4" s="253"/>
-      <c r="E4" s="307" t="s">
+      <c r="E4" s="305" t="s">
         <v>975</v>
       </c>
       <c r="F4" s="132" t="s">
@@ -14560,7 +14560,7 @@
         <v>1028</v>
       </c>
       <c r="H4" s="125"/>
-      <c r="I4" s="307" t="s">
+      <c r="I4" s="305" t="s">
         <v>1057</v>
       </c>
       <c r="J4" s="132" t="s">
@@ -14572,7 +14572,7 @@
       <c r="L4" s="122"/>
     </row>
     <row r="5" spans="1:12" ht="18.75">
-      <c r="A5" s="317"/>
+      <c r="A5" s="303"/>
       <c r="B5" s="131" t="s">
         <v>322</v>
       </c>
@@ -14580,7 +14580,7 @@
         <v>706</v>
       </c>
       <c r="D5" s="253"/>
-      <c r="E5" s="308"/>
+      <c r="E5" s="306"/>
       <c r="F5" s="131" t="s">
         <v>1002</v>
       </c>
@@ -14588,7 +14588,7 @@
         <v>1029</v>
       </c>
       <c r="H5" s="125"/>
-      <c r="I5" s="308"/>
+      <c r="I5" s="306"/>
       <c r="J5" s="131" t="s">
         <v>1092</v>
       </c>
@@ -14598,7 +14598,7 @@
       <c r="L5" s="122"/>
     </row>
     <row r="6" spans="1:12" ht="18.75">
-      <c r="A6" s="317"/>
+      <c r="A6" s="303"/>
       <c r="B6" s="131" t="s">
         <v>323</v>
       </c>
@@ -14606,7 +14606,7 @@
         <v>707</v>
       </c>
       <c r="D6" s="253"/>
-      <c r="E6" s="308"/>
+      <c r="E6" s="306"/>
       <c r="F6" s="131" t="s">
         <v>1003</v>
       </c>
@@ -14614,7 +14614,7 @@
         <v>1030</v>
       </c>
       <c r="H6" s="125"/>
-      <c r="I6" s="308"/>
+      <c r="I6" s="306"/>
       <c r="J6" s="131" t="s">
         <v>1093</v>
       </c>
@@ -14624,7 +14624,7 @@
       <c r="L6" s="122"/>
     </row>
     <row r="7" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A7" s="318"/>
+      <c r="A7" s="304"/>
       <c r="B7" s="135" t="s">
         <v>324</v>
       </c>
@@ -14632,7 +14632,7 @@
         <v>708</v>
       </c>
       <c r="D7" s="253"/>
-      <c r="E7" s="309"/>
+      <c r="E7" s="307"/>
       <c r="F7" s="135" t="s">
         <v>1004</v>
       </c>
@@ -14640,7 +14640,7 @@
         <v>1031</v>
       </c>
       <c r="H7" s="125"/>
-      <c r="I7" s="309"/>
+      <c r="I7" s="307"/>
       <c r="J7" s="135" t="s">
         <v>1094</v>
       </c>
@@ -14650,7 +14650,7 @@
       <c r="L7" s="122"/>
     </row>
     <row r="8" spans="1:12" ht="18.75">
-      <c r="A8" s="316" t="s">
+      <c r="A8" s="302" t="s">
         <v>667</v>
       </c>
       <c r="B8" s="132" t="s">
@@ -14660,7 +14660,7 @@
         <v>709</v>
       </c>
       <c r="D8" s="253"/>
-      <c r="E8" s="307" t="s">
+      <c r="E8" s="305" t="s">
         <v>974</v>
       </c>
       <c r="F8" s="132" t="s">
@@ -14670,7 +14670,7 @@
         <v>1032</v>
       </c>
       <c r="H8" s="125"/>
-      <c r="I8" s="307" t="s">
+      <c r="I8" s="305" t="s">
         <v>1058</v>
       </c>
       <c r="J8" s="132" t="s">
@@ -14682,7 +14682,7 @@
       <c r="L8" s="122"/>
     </row>
     <row r="9" spans="1:12" ht="18.75">
-      <c r="A9" s="317"/>
+      <c r="A9" s="303"/>
       <c r="B9" s="131" t="s">
         <v>658</v>
       </c>
@@ -14690,7 +14690,7 @@
         <v>710</v>
       </c>
       <c r="D9" s="253"/>
-      <c r="E9" s="308"/>
+      <c r="E9" s="306"/>
       <c r="F9" s="131" t="s">
         <v>1006</v>
       </c>
@@ -14698,7 +14698,7 @@
         <v>1033</v>
       </c>
       <c r="H9" s="125"/>
-      <c r="I9" s="308"/>
+      <c r="I9" s="306"/>
       <c r="J9" s="131" t="s">
         <v>1095</v>
       </c>
@@ -14708,7 +14708,7 @@
       <c r="L9" s="122"/>
     </row>
     <row r="10" spans="1:12" ht="18.75">
-      <c r="A10" s="317"/>
+      <c r="A10" s="303"/>
       <c r="B10" s="131" t="s">
         <v>659</v>
       </c>
@@ -14716,7 +14716,7 @@
         <v>711</v>
       </c>
       <c r="D10" s="253"/>
-      <c r="E10" s="308"/>
+      <c r="E10" s="306"/>
       <c r="F10" s="131" t="s">
         <v>1008</v>
       </c>
@@ -14724,7 +14724,7 @@
         <v>1034</v>
       </c>
       <c r="H10" s="125"/>
-      <c r="I10" s="308"/>
+      <c r="I10" s="306"/>
       <c r="J10" s="131" t="s">
         <v>1096</v>
       </c>
@@ -14734,7 +14734,7 @@
       <c r="L10" s="122"/>
     </row>
     <row r="11" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A11" s="318"/>
+      <c r="A11" s="304"/>
       <c r="B11" s="135" t="s">
         <v>660</v>
       </c>
@@ -14742,7 +14742,7 @@
         <v>712</v>
       </c>
       <c r="D11" s="253"/>
-      <c r="E11" s="309"/>
+      <c r="E11" s="307"/>
       <c r="F11" s="135" t="s">
         <v>1009</v>
       </c>
@@ -14750,7 +14750,7 @@
         <v>1035</v>
       </c>
       <c r="H11" s="125"/>
-      <c r="I11" s="309"/>
+      <c r="I11" s="307"/>
       <c r="J11" s="135" t="s">
         <v>1097</v>
       </c>
@@ -14760,7 +14760,7 @@
       <c r="L11" s="122"/>
     </row>
     <row r="12" spans="1:12" ht="18.75">
-      <c r="A12" s="316" t="s">
+      <c r="A12" s="302" t="s">
         <v>665</v>
       </c>
       <c r="B12" s="132" t="s">
@@ -14770,7 +14770,7 @@
         <v>713</v>
       </c>
       <c r="D12" s="253"/>
-      <c r="E12" s="307" t="s">
+      <c r="E12" s="305" t="s">
         <v>973</v>
       </c>
       <c r="F12" s="132" t="s">
@@ -14780,7 +14780,7 @@
         <v>1036</v>
       </c>
       <c r="H12" s="125"/>
-      <c r="I12" s="307" t="s">
+      <c r="I12" s="305" t="s">
         <v>1059</v>
       </c>
       <c r="J12" s="132" t="s">
@@ -14792,7 +14792,7 @@
       <c r="L12" s="122"/>
     </row>
     <row r="13" spans="1:12" ht="18.75">
-      <c r="A13" s="317"/>
+      <c r="A13" s="303"/>
       <c r="B13" s="131" t="s">
         <v>662</v>
       </c>
@@ -14800,7 +14800,7 @@
         <v>714</v>
       </c>
       <c r="D13" s="253"/>
-      <c r="E13" s="308"/>
+      <c r="E13" s="306"/>
       <c r="F13" s="131" t="s">
         <v>1011</v>
       </c>
@@ -14808,7 +14808,7 @@
         <v>1037</v>
       </c>
       <c r="H13" s="125"/>
-      <c r="I13" s="308"/>
+      <c r="I13" s="306"/>
       <c r="J13" s="131" t="s">
         <v>1099</v>
       </c>
@@ -14818,7 +14818,7 @@
       <c r="L13" s="122"/>
     </row>
     <row r="14" spans="1:12" ht="18.75">
-      <c r="A14" s="317"/>
+      <c r="A14" s="303"/>
       <c r="B14" s="131" t="s">
         <v>663</v>
       </c>
@@ -14826,7 +14826,7 @@
         <v>715</v>
       </c>
       <c r="D14" s="253"/>
-      <c r="E14" s="308"/>
+      <c r="E14" s="306"/>
       <c r="F14" s="131" t="s">
         <v>1012</v>
       </c>
@@ -14834,7 +14834,7 @@
         <v>1038</v>
       </c>
       <c r="H14" s="125"/>
-      <c r="I14" s="308"/>
+      <c r="I14" s="306"/>
       <c r="J14" s="131" t="s">
         <v>1100</v>
       </c>
@@ -14844,7 +14844,7 @@
       <c r="L14" s="122"/>
     </row>
     <row r="15" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A15" s="318"/>
+      <c r="A15" s="304"/>
       <c r="B15" s="135" t="s">
         <v>664</v>
       </c>
@@ -14852,7 +14852,7 @@
         <v>716</v>
       </c>
       <c r="D15" s="253"/>
-      <c r="E15" s="309"/>
+      <c r="E15" s="307"/>
       <c r="F15" s="135" t="s">
         <v>1013</v>
       </c>
@@ -14860,7 +14860,7 @@
         <v>1039</v>
       </c>
       <c r="H15" s="125"/>
-      <c r="I15" s="309"/>
+      <c r="I15" s="307"/>
       <c r="J15" s="135" t="s">
         <v>1101</v>
       </c>
@@ -14870,7 +14870,7 @@
       <c r="L15" s="122"/>
     </row>
     <row r="16" spans="1:12" ht="18.75">
-      <c r="A16" s="316" t="s">
+      <c r="A16" s="302" t="s">
         <v>666</v>
       </c>
       <c r="B16" s="132" t="s">
@@ -14880,7 +14880,7 @@
         <v>717</v>
       </c>
       <c r="D16" s="253"/>
-      <c r="E16" s="307" t="s">
+      <c r="E16" s="305" t="s">
         <v>972</v>
       </c>
       <c r="F16" s="132" t="s">
@@ -14890,7 +14890,7 @@
         <v>1040</v>
       </c>
       <c r="H16" s="125"/>
-      <c r="I16" s="307" t="s">
+      <c r="I16" s="305" t="s">
         <v>1060</v>
       </c>
       <c r="J16" s="132" t="s">
@@ -14902,7 +14902,7 @@
       <c r="L16" s="122"/>
     </row>
     <row r="17" spans="1:12" ht="18.75">
-      <c r="A17" s="317"/>
+      <c r="A17" s="303"/>
       <c r="B17" s="131" t="s">
         <v>669</v>
       </c>
@@ -14910,7 +14910,7 @@
         <v>718</v>
       </c>
       <c r="D17" s="253"/>
-      <c r="E17" s="308"/>
+      <c r="E17" s="306"/>
       <c r="F17" s="131" t="s">
         <v>1015</v>
       </c>
@@ -14918,7 +14918,7 @@
         <v>1041</v>
       </c>
       <c r="H17" s="125"/>
-      <c r="I17" s="308"/>
+      <c r="I17" s="306"/>
       <c r="J17" s="131" t="s">
         <v>1103</v>
       </c>
@@ -14928,7 +14928,7 @@
       <c r="L17" s="122"/>
     </row>
     <row r="18" spans="1:12" ht="18.75">
-      <c r="A18" s="317"/>
+      <c r="A18" s="303"/>
       <c r="B18" s="131" t="s">
         <v>670</v>
       </c>
@@ -14936,7 +14936,7 @@
         <v>719</v>
       </c>
       <c r="D18" s="253"/>
-      <c r="E18" s="308"/>
+      <c r="E18" s="306"/>
       <c r="F18" s="131" t="s">
         <v>1016</v>
       </c>
@@ -14944,7 +14944,7 @@
         <v>1042</v>
       </c>
       <c r="H18" s="125"/>
-      <c r="I18" s="308"/>
+      <c r="I18" s="306"/>
       <c r="J18" s="131" t="s">
         <v>1104</v>
       </c>
@@ -14954,7 +14954,7 @@
       <c r="L18" s="122"/>
     </row>
     <row r="19" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A19" s="318"/>
+      <c r="A19" s="304"/>
       <c r="B19" s="135" t="s">
         <v>671</v>
       </c>
@@ -14962,7 +14962,7 @@
         <v>720</v>
       </c>
       <c r="D19" s="253"/>
-      <c r="E19" s="309"/>
+      <c r="E19" s="307"/>
       <c r="F19" s="135" t="s">
         <v>1017</v>
       </c>
@@ -14970,7 +14970,7 @@
         <v>1043</v>
       </c>
       <c r="H19" s="125"/>
-      <c r="I19" s="309"/>
+      <c r="I19" s="307"/>
       <c r="J19" s="135" t="s">
         <v>1105</v>
       </c>
@@ -14984,7 +14984,7 @@
       <c r="B20" s="125"/>
       <c r="C20" s="125"/>
       <c r="D20" s="125"/>
-      <c r="E20" s="307" t="s">
+      <c r="E20" s="305" t="s">
         <v>560</v>
       </c>
       <c r="F20" s="132" t="s">
@@ -14994,7 +14994,7 @@
         <v>1044</v>
       </c>
       <c r="H20" s="125"/>
-      <c r="I20" s="307" t="s">
+      <c r="I20" s="305" t="s">
         <v>1061</v>
       </c>
       <c r="J20" s="132" t="s">
@@ -15010,7 +15010,7 @@
       <c r="B21" s="125"/>
       <c r="C21" s="125"/>
       <c r="D21" s="125"/>
-      <c r="E21" s="308"/>
+      <c r="E21" s="306"/>
       <c r="F21" s="131" t="s">
         <v>1019</v>
       </c>
@@ -15018,7 +15018,7 @@
         <v>1045</v>
       </c>
       <c r="H21" s="125"/>
-      <c r="I21" s="308"/>
+      <c r="I21" s="306"/>
       <c r="J21" s="131" t="s">
         <v>1107</v>
       </c>
@@ -15032,7 +15032,7 @@
       <c r="B22" s="125"/>
       <c r="C22" s="125"/>
       <c r="D22" s="125"/>
-      <c r="E22" s="308"/>
+      <c r="E22" s="306"/>
       <c r="F22" s="131" t="s">
         <v>1020</v>
       </c>
@@ -15040,7 +15040,7 @@
         <v>1046</v>
       </c>
       <c r="H22" s="125"/>
-      <c r="I22" s="308"/>
+      <c r="I22" s="306"/>
       <c r="J22" s="131" t="s">
         <v>1108</v>
       </c>
@@ -15056,7 +15056,7 @@
       <c r="B23" s="256"/>
       <c r="C23" s="257"/>
       <c r="D23" s="125"/>
-      <c r="E23" s="309"/>
+      <c r="E23" s="307"/>
       <c r="F23" s="135" t="s">
         <v>1021</v>
       </c>
@@ -15064,7 +15064,7 @@
         <v>1047</v>
       </c>
       <c r="H23" s="125"/>
-      <c r="I23" s="309"/>
+      <c r="I23" s="307"/>
       <c r="J23" s="135" t="s">
         <v>1109</v>
       </c>
@@ -15084,7 +15084,7 @@
         <v>321</v>
       </c>
       <c r="D24" s="125"/>
-      <c r="E24" s="307" t="s">
+      <c r="E24" s="305" t="s">
         <v>749</v>
       </c>
       <c r="F24" s="132" t="s">
@@ -15094,7 +15094,7 @@
         <v>1048</v>
       </c>
       <c r="H24" s="125"/>
-      <c r="I24" s="307" t="s">
+      <c r="I24" s="305" t="s">
         <v>1062</v>
       </c>
       <c r="J24" s="132" t="s">
@@ -15106,7 +15106,7 @@
       <c r="L24" s="122"/>
     </row>
     <row r="25" spans="1:12" ht="18.75">
-      <c r="A25" s="301" t="s">
+      <c r="A25" s="317" t="s">
         <v>493</v>
       </c>
       <c r="B25" s="132" t="s">
@@ -15116,7 +15116,7 @@
         <v>721</v>
       </c>
       <c r="D25" s="125"/>
-      <c r="E25" s="308"/>
+      <c r="E25" s="306"/>
       <c r="F25" s="131" t="s">
         <v>1023</v>
       </c>
@@ -15124,7 +15124,7 @@
         <v>1049</v>
       </c>
       <c r="H25" s="125"/>
-      <c r="I25" s="308"/>
+      <c r="I25" s="306"/>
       <c r="J25" s="131" t="s">
         <v>1111</v>
       </c>
@@ -15134,7 +15134,7 @@
       <c r="L25" s="122"/>
     </row>
     <row r="26" spans="1:12" ht="18.75">
-      <c r="A26" s="302"/>
+      <c r="A26" s="318"/>
       <c r="B26" s="131" t="s">
         <v>679</v>
       </c>
@@ -15142,7 +15142,7 @@
         <v>722</v>
       </c>
       <c r="D26" s="125"/>
-      <c r="E26" s="308"/>
+      <c r="E26" s="306"/>
       <c r="F26" s="131" t="s">
         <v>1024</v>
       </c>
@@ -15150,7 +15150,7 @@
         <v>1050</v>
       </c>
       <c r="H26" s="125"/>
-      <c r="I26" s="308"/>
+      <c r="I26" s="306"/>
       <c r="J26" s="131" t="s">
         <v>1112</v>
       </c>
@@ -15160,7 +15160,7 @@
       <c r="L26" s="122"/>
     </row>
     <row r="27" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A27" s="302"/>
+      <c r="A27" s="318"/>
       <c r="B27" s="131" t="s">
         <v>680</v>
       </c>
@@ -15168,7 +15168,7 @@
         <v>723</v>
       </c>
       <c r="D27" s="125"/>
-      <c r="E27" s="309"/>
+      <c r="E27" s="307"/>
       <c r="F27" s="135" t="s">
         <v>1025</v>
       </c>
@@ -15176,7 +15176,7 @@
         <v>1051</v>
       </c>
       <c r="H27" s="125"/>
-      <c r="I27" s="309"/>
+      <c r="I27" s="307"/>
       <c r="J27" s="135" t="s">
         <v>1113</v>
       </c>
@@ -15186,7 +15186,7 @@
       <c r="L27" s="122"/>
     </row>
     <row r="28" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A28" s="303"/>
+      <c r="A28" s="319"/>
       <c r="B28" s="135" t="s">
         <v>681</v>
       </c>
@@ -15194,7 +15194,7 @@
         <v>724</v>
       </c>
       <c r="D28" s="125"/>
-      <c r="E28" s="307" t="s">
+      <c r="E28" s="305" t="s">
         <v>562</v>
       </c>
       <c r="F28" s="132" t="s">
@@ -15204,7 +15204,7 @@
         <v>1052</v>
       </c>
       <c r="H28" s="125"/>
-      <c r="I28" s="307" t="s">
+      <c r="I28" s="305" t="s">
         <v>1063</v>
       </c>
       <c r="J28" s="132" t="s">
@@ -15216,7 +15216,7 @@
       <c r="L28" s="122"/>
     </row>
     <row r="29" spans="1:12" ht="18.75">
-      <c r="A29" s="301" t="s">
+      <c r="A29" s="317" t="s">
         <v>687</v>
       </c>
       <c r="B29" s="132" t="s">
@@ -15226,7 +15226,7 @@
         <v>725</v>
       </c>
       <c r="D29" s="253"/>
-      <c r="E29" s="308"/>
+      <c r="E29" s="306"/>
       <c r="F29" s="131" t="s">
         <v>1027</v>
       </c>
@@ -15234,7 +15234,7 @@
         <v>1053</v>
       </c>
       <c r="H29" s="125"/>
-      <c r="I29" s="308"/>
+      <c r="I29" s="306"/>
       <c r="J29" s="131" t="s">
         <v>1115</v>
       </c>
@@ -15244,7 +15244,7 @@
       <c r="L29" s="122"/>
     </row>
     <row r="30" spans="1:12" ht="18.75">
-      <c r="A30" s="302"/>
+      <c r="A30" s="318"/>
       <c r="B30" s="131" t="s">
         <v>684</v>
       </c>
@@ -15252,11 +15252,11 @@
         <v>726</v>
       </c>
       <c r="D30" s="253"/>
-      <c r="E30" s="308"/>
+      <c r="E30" s="306"/>
       <c r="F30" s="131"/>
       <c r="G30" s="250"/>
       <c r="H30" s="125"/>
-      <c r="I30" s="308"/>
+      <c r="I30" s="306"/>
       <c r="J30" s="131" t="s">
         <v>1116</v>
       </c>
@@ -15266,7 +15266,7 @@
       <c r="L30" s="122"/>
     </row>
     <row r="31" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A31" s="302"/>
+      <c r="A31" s="318"/>
       <c r="B31" s="131" t="s">
         <v>685</v>
       </c>
@@ -15274,11 +15274,11 @@
         <v>727</v>
       </c>
       <c r="D31" s="253"/>
-      <c r="E31" s="309"/>
+      <c r="E31" s="307"/>
       <c r="F31" s="135"/>
       <c r="G31" s="251"/>
       <c r="H31" s="125"/>
-      <c r="I31" s="309"/>
+      <c r="I31" s="307"/>
       <c r="J31" s="135" t="s">
         <v>1117</v>
       </c>
@@ -15288,7 +15288,7 @@
       <c r="L31" s="122"/>
     </row>
     <row r="32" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A32" s="303"/>
+      <c r="A32" s="319"/>
       <c r="B32" s="135" t="s">
         <v>686</v>
       </c>
@@ -15306,7 +15306,7 @@
       <c r="L32" s="122"/>
     </row>
     <row r="33" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A33" s="301" t="s">
+      <c r="A33" s="317" t="s">
         <v>691</v>
       </c>
       <c r="B33" s="132" t="s">
@@ -15316,21 +15316,21 @@
         <v>729</v>
       </c>
       <c r="D33" s="253"/>
-      <c r="E33" s="304" t="s">
+      <c r="E33" s="314" t="s">
         <v>1149</v>
       </c>
-      <c r="F33" s="305"/>
-      <c r="G33" s="306"/>
+      <c r="F33" s="315"/>
+      <c r="G33" s="316"/>
       <c r="H33" s="124"/>
-      <c r="I33" s="304" t="s">
+      <c r="I33" s="314" t="s">
         <v>1148</v>
       </c>
-      <c r="J33" s="305"/>
-      <c r="K33" s="306"/>
+      <c r="J33" s="315"/>
+      <c r="K33" s="316"/>
       <c r="L33" s="122"/>
     </row>
     <row r="34" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A34" s="302"/>
+      <c r="A34" s="318"/>
       <c r="B34" s="131" t="s">
         <v>693</v>
       </c>
@@ -15360,7 +15360,7 @@
       <c r="L34" s="122"/>
     </row>
     <row r="35" spans="1:12" ht="18.75">
-      <c r="A35" s="302"/>
+      <c r="A35" s="318"/>
       <c r="B35" s="131" t="s">
         <v>694</v>
       </c>
@@ -15368,7 +15368,7 @@
         <v>731</v>
       </c>
       <c r="D35" s="253"/>
-      <c r="E35" s="301" t="s">
+      <c r="E35" s="317" t="s">
         <v>494</v>
       </c>
       <c r="F35" s="132" t="s">
@@ -15378,7 +15378,7 @@
         <v>11311</v>
       </c>
       <c r="H35" s="124"/>
-      <c r="I35" s="301" t="s">
+      <c r="I35" s="317" t="s">
         <v>955</v>
       </c>
       <c r="J35" s="132" t="s">
@@ -15390,7 +15390,7 @@
       <c r="L35" s="122"/>
     </row>
     <row r="36" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A36" s="303"/>
+      <c r="A36" s="319"/>
       <c r="B36" s="135" t="s">
         <v>695</v>
       </c>
@@ -15398,7 +15398,7 @@
         <v>732</v>
       </c>
       <c r="D36" s="253"/>
-      <c r="E36" s="302"/>
+      <c r="E36" s="318"/>
       <c r="F36" s="131" t="s">
         <v>958</v>
       </c>
@@ -15406,7 +15406,7 @@
         <v>11312</v>
       </c>
       <c r="H36" s="124"/>
-      <c r="I36" s="302"/>
+      <c r="I36" s="318"/>
       <c r="J36" s="131" t="s">
         <v>965</v>
       </c>
@@ -15416,7 +15416,7 @@
       <c r="L36" s="122"/>
     </row>
     <row r="37" spans="1:12" ht="18.75">
-      <c r="A37" s="301" t="s">
+      <c r="A37" s="317" t="s">
         <v>698</v>
       </c>
       <c r="B37" s="132" t="s">
@@ -15426,7 +15426,7 @@
         <v>11441</v>
       </c>
       <c r="D37" s="253"/>
-      <c r="E37" s="302"/>
+      <c r="E37" s="318"/>
       <c r="F37" s="131" t="s">
         <v>959</v>
       </c>
@@ -15434,7 +15434,7 @@
         <v>11313</v>
       </c>
       <c r="H37" s="124"/>
-      <c r="I37" s="302"/>
+      <c r="I37" s="318"/>
       <c r="J37" s="131" t="s">
         <v>966</v>
       </c>
@@ -15444,7 +15444,7 @@
       <c r="L37" s="122"/>
     </row>
     <row r="38" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A38" s="302"/>
+      <c r="A38" s="318"/>
       <c r="B38" s="131" t="s">
         <v>700</v>
       </c>
@@ -15452,7 +15452,7 @@
         <v>11442</v>
       </c>
       <c r="D38" s="253"/>
-      <c r="E38" s="303"/>
+      <c r="E38" s="319"/>
       <c r="F38" s="135" t="s">
         <v>959</v>
       </c>
@@ -15460,7 +15460,7 @@
         <v>11314</v>
       </c>
       <c r="H38" s="124"/>
-      <c r="I38" s="303"/>
+      <c r="I38" s="319"/>
       <c r="J38" s="135" t="s">
         <v>967</v>
       </c>
@@ -15470,7 +15470,7 @@
       <c r="L38" s="122"/>
     </row>
     <row r="39" spans="1:12" ht="18.75">
-      <c r="A39" s="302"/>
+      <c r="A39" s="318"/>
       <c r="B39" s="131" t="s">
         <v>701</v>
       </c>
@@ -15478,7 +15478,7 @@
         <v>11443</v>
       </c>
       <c r="D39" s="253"/>
-      <c r="E39" s="301" t="s">
+      <c r="E39" s="317" t="s">
         <v>954</v>
       </c>
       <c r="F39" s="132" t="s">
@@ -15488,7 +15488,7 @@
         <v>11321</v>
       </c>
       <c r="H39" s="124"/>
-      <c r="I39" s="301" t="s">
+      <c r="I39" s="317" t="s">
         <v>956</v>
       </c>
       <c r="J39" s="132" t="s">
@@ -15500,7 +15500,7 @@
       <c r="L39" s="122"/>
     </row>
     <row r="40" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A40" s="303"/>
+      <c r="A40" s="319"/>
       <c r="B40" s="135" t="s">
         <v>702</v>
       </c>
@@ -15508,7 +15508,7 @@
         <v>11444</v>
       </c>
       <c r="D40" s="253"/>
-      <c r="E40" s="302"/>
+      <c r="E40" s="318"/>
       <c r="F40" s="131" t="s">
         <v>961</v>
       </c>
@@ -15516,7 +15516,7 @@
         <v>11322</v>
       </c>
       <c r="H40" s="124"/>
-      <c r="I40" s="302"/>
+      <c r="I40" s="318"/>
       <c r="J40" s="131" t="s">
         <v>969</v>
       </c>
@@ -15530,7 +15530,7 @@
       <c r="B41" s="125"/>
       <c r="C41" s="253"/>
       <c r="D41" s="253"/>
-      <c r="E41" s="302"/>
+      <c r="E41" s="318"/>
       <c r="F41" s="131" t="s">
         <v>962</v>
       </c>
@@ -15538,7 +15538,7 @@
         <v>11323</v>
       </c>
       <c r="H41" s="124"/>
-      <c r="I41" s="302"/>
+      <c r="I41" s="318"/>
       <c r="J41" s="131" t="s">
         <v>970</v>
       </c>
@@ -15552,7 +15552,7 @@
       <c r="B42" s="125"/>
       <c r="C42" s="253"/>
       <c r="D42" s="253"/>
-      <c r="E42" s="303"/>
+      <c r="E42" s="319"/>
       <c r="F42" s="135" t="s">
         <v>963</v>
       </c>
@@ -15560,7 +15560,7 @@
         <v>11324</v>
       </c>
       <c r="H42" s="124"/>
-      <c r="I42" s="303"/>
+      <c r="I42" s="319"/>
       <c r="J42" s="135" t="s">
         <v>971</v>
       </c>
@@ -15613,18 +15613,16 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="I35:I38"/>
+    <mergeCell ref="I39:I42"/>
     <mergeCell ref="I16:I19"/>
     <mergeCell ref="I12:I15"/>
     <mergeCell ref="I8:I11"/>
@@ -15635,16 +15633,18 @@
     <mergeCell ref="I28:I31"/>
     <mergeCell ref="E20:E23"/>
     <mergeCell ref="E24:E27"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="I35:I38"/>
-    <mergeCell ref="I39:I42"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="E16:E19"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15675,40 +15675,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="319" t="s">
+      <c r="A1" s="324" t="s">
         <v>1151</v>
       </c>
-      <c r="B1" s="320"/>
-      <c r="C1" s="320"/>
-      <c r="D1" s="320"/>
-      <c r="E1" s="320"/>
-      <c r="F1" s="320"/>
-      <c r="G1" s="320"/>
-      <c r="H1" s="321"/>
+      <c r="B1" s="325"/>
+      <c r="C1" s="325"/>
+      <c r="D1" s="325"/>
+      <c r="E1" s="325"/>
+      <c r="F1" s="325"/>
+      <c r="G1" s="325"/>
+      <c r="H1" s="326"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="322"/>
-      <c r="B2" s="323"/>
-      <c r="C2" s="323"/>
-      <c r="D2" s="323"/>
-      <c r="E2" s="323"/>
-      <c r="F2" s="323"/>
-      <c r="G2" s="323"/>
-      <c r="H2" s="324"/>
+      <c r="A2" s="327"/>
+      <c r="B2" s="328"/>
+      <c r="C2" s="328"/>
+      <c r="D2" s="328"/>
+      <c r="E2" s="328"/>
+      <c r="F2" s="328"/>
+      <c r="G2" s="328"/>
+      <c r="H2" s="329"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="325" t="s">
+      <c r="A3" s="330" t="s">
         <v>250</v>
       </c>
-      <c r="B3" s="326"/>
-      <c r="C3" s="326"/>
-      <c r="D3" s="326"/>
-      <c r="E3" s="326" t="s">
+      <c r="B3" s="331"/>
+      <c r="C3" s="331"/>
+      <c r="D3" s="331"/>
+      <c r="E3" s="331" t="s">
         <v>251</v>
       </c>
-      <c r="F3" s="326"/>
-      <c r="G3" s="326"/>
-      <c r="H3" s="327"/>
+      <c r="F3" s="331"/>
+      <c r="G3" s="331"/>
+      <c r="H3" s="332"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="12">
@@ -16242,11 +16242,11 @@
       <c r="C27" s="118" t="s">
         <v>594</v>
       </c>
-      <c r="D27" s="328" t="s">
+      <c r="D27" s="323" t="s">
         <v>570</v>
       </c>
-      <c r="E27" s="328"/>
-      <c r="F27" s="328"/>
+      <c r="E27" s="323"/>
+      <c r="F27" s="323"/>
       <c r="G27" s="17"/>
       <c r="H27" s="18"/>
     </row>
@@ -16258,11 +16258,11 @@
       <c r="C28" s="118" t="s">
         <v>598</v>
       </c>
-      <c r="D28" s="328" t="s">
+      <c r="D28" s="323" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="328"/>
-      <c r="F28" s="328"/>
+      <c r="E28" s="323"/>
+      <c r="F28" s="323"/>
       <c r="G28" s="17"/>
       <c r="H28" s="18"/>
     </row>
@@ -16274,11 +16274,11 @@
       <c r="C29" s="118" t="s">
         <v>599</v>
       </c>
-      <c r="D29" s="328" t="s">
+      <c r="D29" s="323" t="s">
         <v>571</v>
       </c>
-      <c r="E29" s="328"/>
-      <c r="F29" s="328"/>
+      <c r="E29" s="323"/>
+      <c r="F29" s="323"/>
       <c r="G29" s="17"/>
       <c r="H29" s="18"/>
     </row>
@@ -16290,11 +16290,11 @@
       <c r="C30" s="118" t="s">
         <v>600</v>
       </c>
-      <c r="D30" s="328" t="s">
+      <c r="D30" s="323" t="s">
         <v>572</v>
       </c>
-      <c r="E30" s="328"/>
-      <c r="F30" s="328"/>
+      <c r="E30" s="323"/>
+      <c r="F30" s="323"/>
       <c r="G30" s="17"/>
       <c r="H30" s="18"/>
     </row>
@@ -16306,11 +16306,11 @@
       <c r="C31" s="118" t="s">
         <v>601</v>
       </c>
-      <c r="D31" s="328" t="s">
+      <c r="D31" s="323" t="s">
         <v>573</v>
       </c>
-      <c r="E31" s="328"/>
-      <c r="F31" s="328"/>
+      <c r="E31" s="323"/>
+      <c r="F31" s="323"/>
       <c r="G31" s="17"/>
       <c r="H31" s="18"/>
     </row>
@@ -16322,11 +16322,11 @@
       <c r="C32" s="118" t="s">
         <v>602</v>
       </c>
-      <c r="D32" s="328" t="s">
+      <c r="D32" s="323" t="s">
         <v>574</v>
       </c>
-      <c r="E32" s="328"/>
-      <c r="F32" s="328"/>
+      <c r="E32" s="323"/>
+      <c r="F32" s="323"/>
       <c r="G32" s="17"/>
       <c r="H32" s="18"/>
     </row>
@@ -16338,11 +16338,11 @@
       <c r="C33" s="118" t="s">
         <v>614</v>
       </c>
-      <c r="D33" s="328" t="s">
+      <c r="D33" s="323" t="s">
         <v>482</v>
       </c>
-      <c r="E33" s="328"/>
-      <c r="F33" s="328"/>
+      <c r="E33" s="323"/>
+      <c r="F33" s="323"/>
       <c r="G33" s="17"/>
       <c r="H33" s="18"/>
     </row>
@@ -16354,11 +16354,11 @@
       <c r="C34" s="118" t="s">
         <v>615</v>
       </c>
-      <c r="D34" s="328" t="s">
+      <c r="D34" s="323" t="s">
         <v>575</v>
       </c>
-      <c r="E34" s="328"/>
-      <c r="F34" s="328"/>
+      <c r="E34" s="323"/>
+      <c r="F34" s="323"/>
       <c r="G34" s="17"/>
       <c r="H34" s="18"/>
     </row>
@@ -16370,11 +16370,11 @@
       <c r="C35" s="118" t="s">
         <v>616</v>
       </c>
-      <c r="D35" s="328" t="s">
+      <c r="D35" s="323" t="s">
         <v>576</v>
       </c>
-      <c r="E35" s="328"/>
-      <c r="F35" s="328"/>
+      <c r="E35" s="323"/>
+      <c r="F35" s="323"/>
       <c r="G35" s="17"/>
       <c r="H35" s="18"/>
     </row>
@@ -16384,11 +16384,11 @@
       <c r="C36" s="118" t="s">
         <v>651</v>
       </c>
-      <c r="D36" s="329" t="s">
+      <c r="D36" s="320" t="s">
         <v>591</v>
       </c>
-      <c r="E36" s="330"/>
-      <c r="F36" s="331"/>
+      <c r="E36" s="321"/>
+      <c r="F36" s="322"/>
       <c r="G36" s="17"/>
       <c r="H36" s="18"/>
     </row>
@@ -16398,11 +16398,11 @@
       <c r="C37" s="118" t="s">
         <v>654</v>
       </c>
-      <c r="D37" s="329" t="s">
+      <c r="D37" s="320" t="s">
         <v>652</v>
       </c>
-      <c r="E37" s="330"/>
-      <c r="F37" s="331"/>
+      <c r="E37" s="321"/>
+      <c r="F37" s="322"/>
       <c r="G37" s="17"/>
       <c r="H37" s="18"/>
     </row>
@@ -16412,11 +16412,11 @@
       <c r="C38" s="118" t="s">
         <v>653</v>
       </c>
-      <c r="D38" s="329" t="s">
+      <c r="D38" s="320" t="s">
         <v>655</v>
       </c>
-      <c r="E38" s="330"/>
-      <c r="F38" s="331"/>
+      <c r="E38" s="321"/>
+      <c r="F38" s="322"/>
       <c r="G38" s="17"/>
       <c r="H38" s="18"/>
     </row>
@@ -16424,9 +16424,9 @@
       <c r="A39" s="16"/>
       <c r="B39" s="120"/>
       <c r="C39" s="118"/>
-      <c r="D39" s="329"/>
-      <c r="E39" s="330"/>
-      <c r="F39" s="331"/>
+      <c r="D39" s="320"/>
+      <c r="E39" s="321"/>
+      <c r="F39" s="322"/>
       <c r="G39" s="17"/>
       <c r="H39" s="18"/>
     </row>
@@ -16524,13 +16524,6 @@
     <row r="52" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:H3"/>
@@ -16540,6 +16533,13 @@
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -16567,28 +16567,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75">
-      <c r="A1" s="341" t="s">
+      <c r="A1" s="342" t="s">
         <v>1184</v>
       </c>
-      <c r="B1" s="341"/>
-      <c r="C1" s="341"/>
-      <c r="D1" s="341"/>
-      <c r="E1" s="341"/>
-      <c r="F1" s="341"/>
-      <c r="G1" s="341"/>
-      <c r="H1" s="341"/>
+      <c r="B1" s="342"/>
+      <c r="C1" s="342"/>
+      <c r="D1" s="342"/>
+      <c r="E1" s="342"/>
+      <c r="F1" s="342"/>
+      <c r="G1" s="342"/>
+      <c r="H1" s="342"/>
     </row>
     <row r="2" spans="1:10" ht="15.75">
-      <c r="A2" s="335" t="s">
+      <c r="A2" s="336" t="s">
         <v>1152</v>
       </c>
-      <c r="B2" s="336"/>
-      <c r="C2" s="336"/>
-      <c r="D2" s="336"/>
-      <c r="E2" s="336"/>
-      <c r="F2" s="336"/>
-      <c r="G2" s="336"/>
-      <c r="H2" s="337"/>
+      <c r="B2" s="337"/>
+      <c r="C2" s="337"/>
+      <c r="D2" s="337"/>
+      <c r="E2" s="337"/>
+      <c r="F2" s="337"/>
+      <c r="G2" s="337"/>
+      <c r="H2" s="338"/>
     </row>
     <row r="3" spans="1:10" ht="15.75">
       <c r="A3" s="5"/>
@@ -16904,16 +16904,16 @@
       <c r="H17" s="264"/>
     </row>
     <row r="18" spans="1:11" ht="15.75">
-      <c r="A18" s="338" t="s">
+      <c r="A18" s="339" t="s">
         <v>224</v>
       </c>
-      <c r="B18" s="339"/>
-      <c r="C18" s="339"/>
-      <c r="D18" s="339"/>
-      <c r="E18" s="339"/>
-      <c r="F18" s="339"/>
-      <c r="G18" s="339"/>
-      <c r="H18" s="340"/>
+      <c r="B18" s="340"/>
+      <c r="C18" s="340"/>
+      <c r="D18" s="340"/>
+      <c r="E18" s="340"/>
+      <c r="F18" s="340"/>
+      <c r="G18" s="340"/>
+      <c r="H18" s="341"/>
     </row>
     <row r="19" spans="1:11" ht="15.75">
       <c r="A19" s="265"/>
@@ -17169,16 +17169,16 @@
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:11" ht="15.75">
-      <c r="A31" s="335" t="s">
+      <c r="A31" s="336" t="s">
         <v>225</v>
       </c>
-      <c r="B31" s="336"/>
-      <c r="C31" s="336"/>
-      <c r="D31" s="336"/>
-      <c r="E31" s="336"/>
-      <c r="F31" s="336"/>
-      <c r="G31" s="336"/>
-      <c r="H31" s="337"/>
+      <c r="B31" s="337"/>
+      <c r="C31" s="337"/>
+      <c r="D31" s="337"/>
+      <c r="E31" s="337"/>
+      <c r="F31" s="337"/>
+      <c r="G31" s="337"/>
+      <c r="H31" s="338"/>
     </row>
     <row r="32" spans="1:11" ht="15.75">
       <c r="A32" s="5"/>
@@ -17404,18 +17404,18 @@
     </row>
     <row r="43" spans="1:8" ht="10.5" customHeight="1"/>
     <row r="44" spans="1:8" ht="15.75">
-      <c r="A44" s="332" t="s">
+      <c r="A44" s="333" t="s">
         <v>1175</v>
       </c>
-      <c r="B44" s="333"/>
-      <c r="C44" s="333"/>
-      <c r="D44" s="334"/>
-      <c r="E44" s="332" t="s">
+      <c r="B44" s="334"/>
+      <c r="C44" s="334"/>
+      <c r="D44" s="335"/>
+      <c r="E44" s="333" t="s">
         <v>1175</v>
       </c>
-      <c r="F44" s="333"/>
-      <c r="G44" s="333"/>
-      <c r="H44" s="334"/>
+      <c r="F44" s="334"/>
+      <c r="G44" s="334"/>
+      <c r="H44" s="335"/>
     </row>
     <row r="45" spans="1:8" ht="15.75">
       <c r="A45" s="3"/>
@@ -17533,54 +17533,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1">
-      <c r="A1" s="345" t="s">
-        <v>1297</v>
-      </c>
-      <c r="B1" s="346"/>
-      <c r="C1" s="346"/>
-      <c r="D1" s="346"/>
-      <c r="E1" s="346"/>
-      <c r="F1" s="346"/>
-      <c r="G1" s="346"/>
-      <c r="H1" s="347"/>
+      <c r="A1" s="346" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B1" s="347"/>
+      <c r="C1" s="347"/>
+      <c r="D1" s="347"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="347"/>
+      <c r="G1" s="347"/>
+      <c r="H1" s="348"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="348"/>
-      <c r="B2" s="349"/>
-      <c r="C2" s="349"/>
-      <c r="D2" s="349"/>
-      <c r="E2" s="349"/>
-      <c r="F2" s="349"/>
-      <c r="G2" s="349"/>
-      <c r="H2" s="350"/>
+      <c r="A2" s="349"/>
+      <c r="B2" s="350"/>
+      <c r="C2" s="350"/>
+      <c r="D2" s="350"/>
+      <c r="E2" s="350"/>
+      <c r="F2" s="350"/>
+      <c r="G2" s="350"/>
+      <c r="H2" s="351"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="351" t="s">
+      <c r="A3" s="352" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B3" s="353"/>
+      <c r="C3" s="353"/>
+      <c r="D3" s="354"/>
+      <c r="E3" s="355" t="s">
         <v>1257</v>
       </c>
-      <c r="B3" s="352"/>
-      <c r="C3" s="352"/>
-      <c r="D3" s="353"/>
-      <c r="E3" s="354" t="s">
+      <c r="F3" s="353"/>
+      <c r="G3" s="353"/>
+      <c r="H3" s="356"/>
+    </row>
+    <row r="4" spans="1:8" ht="16.149999999999999" customHeight="1" thickBot="1">
+      <c r="A4" s="357" t="s">
         <v>1258</v>
       </c>
-      <c r="F3" s="352"/>
-      <c r="G3" s="352"/>
-      <c r="H3" s="355"/>
-    </row>
-    <row r="4" spans="1:8" ht="16.149999999999999" customHeight="1" thickBot="1">
-      <c r="A4" s="356" t="s">
+      <c r="B4" s="358"/>
+      <c r="C4" s="358"/>
+      <c r="D4" s="359"/>
+      <c r="E4" s="360" t="s">
         <v>1259</v>
       </c>
-      <c r="B4" s="357"/>
-      <c r="C4" s="357"/>
-      <c r="D4" s="358"/>
-      <c r="E4" s="359" t="s">
-        <v>1260</v>
-      </c>
-      <c r="F4" s="357"/>
-      <c r="G4" s="357"/>
-      <c r="H4" s="360"/>
+      <c r="F4" s="358"/>
+      <c r="G4" s="358"/>
+      <c r="H4" s="361"/>
     </row>
     <row r="5" spans="1:8" ht="19.5" thickBot="1">
       <c r="A5" s="273">
@@ -17588,10 +17588,10 @@
       </c>
       <c r="B5" s="274"/>
       <c r="C5" s="275" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="D5" s="275" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="E5" s="273">
         <v>1</v>
@@ -17601,7 +17601,7 @@
         <v>843</v>
       </c>
       <c r="H5" s="277" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="19.5" thickBot="1">
@@ -17610,10 +17610,10 @@
       </c>
       <c r="B6" s="274"/>
       <c r="C6" s="275" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="D6" s="275" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="E6" s="273">
         <v>2</v>
@@ -17632,22 +17632,22 @@
       </c>
       <c r="B7" s="274"/>
       <c r="C7" s="275" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="D7" s="275" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="E7" s="273">
         <v>3</v>
       </c>
       <c r="F7" s="276" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="G7" s="275" t="s">
         <v>379</v>
       </c>
       <c r="H7" s="277" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="19.5" thickBot="1">
@@ -17656,22 +17656,22 @@
       </c>
       <c r="B8" s="274"/>
       <c r="C8" s="275" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="D8" s="275" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="E8" s="273">
         <v>4</v>
       </c>
       <c r="F8" s="276" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="G8" s="275" t="s">
         <v>510</v>
       </c>
       <c r="H8" s="278" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="19.5" thickBot="1">
@@ -17680,10 +17680,10 @@
       </c>
       <c r="B9" s="274"/>
       <c r="C9" s="275" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="D9" s="275" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="E9" s="273">
         <v>5</v>
@@ -17707,7 +17707,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="280" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="E10" s="273">
         <v>6</v>
@@ -17717,7 +17717,7 @@
         <v>477</v>
       </c>
       <c r="H10" s="279" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="19.5" thickBot="1">
@@ -17731,7 +17731,7 @@
         <v>188</v>
       </c>
       <c r="D11" s="280" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="E11" s="273">
         <v>7</v>
@@ -17741,7 +17741,7 @@
         <v>479</v>
       </c>
       <c r="H11" s="279" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="19.5" thickBot="1">
@@ -17750,10 +17750,10 @@
       </c>
       <c r="B12" s="274"/>
       <c r="C12" s="275" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="D12" s="280" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="E12" s="273">
         <v>8</v>
@@ -17774,20 +17774,20 @@
       </c>
       <c r="B13" s="274"/>
       <c r="C13" s="275" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="D13" s="282" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="E13" s="273">
         <v>9</v>
       </c>
       <c r="F13" s="276"/>
       <c r="G13" s="275" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="H13" s="282" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="19.5" thickBot="1">
@@ -17796,10 +17796,10 @@
       </c>
       <c r="B14" s="274"/>
       <c r="C14" s="275" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="D14" s="282" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="E14" s="273">
         <v>10</v>
@@ -17811,7 +17811,7 @@
         <v>12</v>
       </c>
       <c r="H14" s="280" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="19.5" thickBot="1">
@@ -17820,20 +17820,20 @@
       </c>
       <c r="B15" s="274"/>
       <c r="C15" s="275" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="D15" s="275" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="E15" s="273">
         <v>11</v>
       </c>
       <c r="F15" s="276"/>
       <c r="G15" s="275" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="H15" s="282" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.5" thickBot="1">
@@ -17842,10 +17842,10 @@
       </c>
       <c r="B16" s="274"/>
       <c r="C16" s="275" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="D16" s="275" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E16" s="273">
         <v>12</v>
@@ -17857,7 +17857,7 @@
         <v>20</v>
       </c>
       <c r="H16" s="280" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="19.5" thickBot="1">
@@ -17866,10 +17866,10 @@
       </c>
       <c r="B17" s="274"/>
       <c r="C17" s="275" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="D17" s="275" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E17" s="273">
         <v>13</v>
@@ -17881,7 +17881,7 @@
         <v>188</v>
       </c>
       <c r="H17" s="280" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="19.5" thickBot="1">
@@ -17890,20 +17890,20 @@
       </c>
       <c r="B18" s="274"/>
       <c r="C18" s="275" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="D18" s="275" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E18" s="273">
         <v>14</v>
       </c>
       <c r="F18" s="276"/>
       <c r="G18" s="275" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="H18" s="280" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="19.5" thickBot="1">
@@ -17912,16 +17912,16 @@
       </c>
       <c r="B19" s="274"/>
       <c r="C19" s="275" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="D19" s="275" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="E19" s="273">
         <v>15</v>
       </c>
       <c r="F19" s="276" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="G19" s="275" t="s">
         <v>74</v>
@@ -17935,7 +17935,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="276" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="C20" s="275" t="s">
         <v>74</v>
@@ -17953,7 +17953,7 @@
         <v>171</v>
       </c>
       <c r="H20" s="280" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="19.5" thickBot="1">
@@ -17967,7 +17967,7 @@
         <v>171</v>
       </c>
       <c r="D21" s="280" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="E21" s="273">
         <v>17</v>
@@ -17979,7 +17979,7 @@
         <v>53</v>
       </c>
       <c r="H21" s="280" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="19.5" thickBot="1">
@@ -17993,7 +17993,7 @@
         <v>53</v>
       </c>
       <c r="D22" s="280" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="E22" s="273">
         <v>18</v>
@@ -18005,7 +18005,7 @@
         <v>73</v>
       </c>
       <c r="H22" s="280" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="19.5" thickBot="1">
@@ -18019,7 +18019,7 @@
         <v>73</v>
       </c>
       <c r="D23" s="280" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="E23" s="273">
         <v>19</v>
@@ -18031,7 +18031,7 @@
         <v>507</v>
       </c>
       <c r="H23" s="276" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="19.5" thickBot="1">
@@ -18040,10 +18040,10 @@
       </c>
       <c r="B24" s="284"/>
       <c r="C24" s="292" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="D24" s="284" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="E24" s="273">
         <v>20</v>
@@ -18055,16 +18055,16 @@
         <v>506</v>
       </c>
       <c r="H24" s="276" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="19.5" thickBot="1">
+      <c r="A25" s="343" t="s">
         <v>1288</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="19.5" thickBot="1">
-      <c r="A25" s="342" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B25" s="343"/>
-      <c r="C25" s="343"/>
-      <c r="D25" s="344"/>
+      <c r="B25" s="344"/>
+      <c r="C25" s="344"/>
+      <c r="D25" s="345"/>
       <c r="E25" s="274">
         <v>21</v>
       </c>
@@ -18075,7 +18075,7 @@
         <v>505</v>
       </c>
       <c r="H25" s="276" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="19.5" thickBot="1">
@@ -18097,7 +18097,7 @@
         <v>504</v>
       </c>
       <c r="H26" s="278" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="19.5" thickBot="1">
@@ -18207,7 +18207,7 @@
         <v>371</v>
       </c>
       <c r="H31" s="276" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="19.5" thickBot="1">
@@ -18229,7 +18229,7 @@
         <v>503</v>
       </c>
       <c r="H32" s="289" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="19.5" thickBot="1">
@@ -18247,7 +18247,7 @@
         <v>888</v>
       </c>
       <c r="H33" s="289" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="19.5" thickBot="1">
@@ -18262,10 +18262,10 @@
         <v>1230</v>
       </c>
       <c r="G34" s="290" t="s">
+        <v>1294</v>
+      </c>
+      <c r="H34" s="289" t="s">
         <v>1295</v>
-      </c>
-      <c r="H34" s="289" t="s">
-        <v>1296</v>
       </c>
     </row>
   </sheetData>
@@ -18302,28 +18302,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="373" t="s">
+      <c r="A1" s="362" t="s">
         <v>952</v>
       </c>
-      <c r="B1" s="374"/>
-      <c r="C1" s="374"/>
-      <c r="D1" s="374"/>
-      <c r="E1" s="374"/>
-      <c r="F1" s="375"/>
+      <c r="B1" s="363"/>
+      <c r="C1" s="363"/>
+      <c r="D1" s="363"/>
+      <c r="E1" s="363"/>
+      <c r="F1" s="364"/>
       <c r="G1" s="175"/>
       <c r="H1" s="175"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="376" t="s">
+      <c r="A2" s="365" t="s">
         <v>840</v>
       </c>
-      <c r="B2" s="377"/>
-      <c r="C2" s="378"/>
-      <c r="D2" s="376" t="s">
+      <c r="B2" s="366"/>
+      <c r="C2" s="367"/>
+      <c r="D2" s="365" t="s">
         <v>841</v>
       </c>
-      <c r="E2" s="377"/>
-      <c r="F2" s="378"/>
+      <c r="E2" s="366"/>
+      <c r="F2" s="367"/>
       <c r="G2" s="175"/>
       <c r="H2" s="175"/>
     </row>
@@ -18347,7 +18347,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="175"/>
-      <c r="H3" s="370" t="s">
+      <c r="H3" s="368" t="s">
         <v>844</v>
       </c>
     </row>
@@ -18371,7 +18371,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="175"/>
-      <c r="H4" s="371"/>
+      <c r="H4" s="369"/>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A5" s="176">
@@ -18393,7 +18393,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="175"/>
-      <c r="H5" s="371"/>
+      <c r="H5" s="369"/>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A6" s="179">
@@ -18415,7 +18415,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="175"/>
-      <c r="H6" s="371"/>
+      <c r="H6" s="369"/>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A7" s="179">
@@ -18437,7 +18437,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="175"/>
-      <c r="H7" s="371"/>
+      <c r="H7" s="369"/>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A8" s="182">
@@ -18459,7 +18459,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="175"/>
-      <c r="H8" s="371"/>
+      <c r="H8" s="369"/>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A9" s="182">
@@ -18481,7 +18481,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="175"/>
-      <c r="H9" s="371"/>
+      <c r="H9" s="369"/>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A10" s="185">
@@ -18503,7 +18503,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="175"/>
-      <c r="H10" s="372"/>
+      <c r="H10" s="370"/>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="188">
@@ -18525,7 +18525,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="175"/>
-      <c r="H11" s="361" t="s">
+      <c r="H11" s="371" t="s">
         <v>856</v>
       </c>
     </row>
@@ -18549,7 +18549,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="175"/>
-      <c r="H12" s="362"/>
+      <c r="H12" s="372"/>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A13" s="191">
@@ -18571,7 +18571,7 @@
         <v>11</v>
       </c>
       <c r="G13" s="175"/>
-      <c r="H13" s="362"/>
+      <c r="H13" s="372"/>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A14" s="191">
@@ -18593,7 +18593,7 @@
         <v>12</v>
       </c>
       <c r="G14" s="175"/>
-      <c r="H14" s="362"/>
+      <c r="H14" s="372"/>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A15" s="195">
@@ -18615,7 +18615,7 @@
         <v>13</v>
       </c>
       <c r="G15" s="175"/>
-      <c r="H15" s="362"/>
+      <c r="H15" s="372"/>
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A16" s="195">
@@ -18637,7 +18637,7 @@
         <v>14</v>
       </c>
       <c r="G16" s="175"/>
-      <c r="H16" s="362"/>
+      <c r="H16" s="372"/>
     </row>
     <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A17" s="195">
@@ -18659,7 +18659,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="175"/>
-      <c r="H17" s="362"/>
+      <c r="H17" s="372"/>
     </row>
     <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A18" s="195">
@@ -18681,7 +18681,7 @@
         <v>16</v>
       </c>
       <c r="G18" s="175"/>
-      <c r="H18" s="362"/>
+      <c r="H18" s="372"/>
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A19" s="195">
@@ -18703,7 +18703,7 @@
         <v>17</v>
       </c>
       <c r="G19" s="175"/>
-      <c r="H19" s="362"/>
+      <c r="H19" s="372"/>
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A20" s="198">
@@ -18725,7 +18725,7 @@
         <v>18</v>
       </c>
       <c r="G20" s="175"/>
-      <c r="H20" s="362"/>
+      <c r="H20" s="372"/>
     </row>
     <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A21" s="198">
@@ -18747,7 +18747,7 @@
         <v>19</v>
       </c>
       <c r="G21" s="175"/>
-      <c r="H21" s="362"/>
+      <c r="H21" s="372"/>
     </row>
     <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A22" s="201">
@@ -18769,7 +18769,7 @@
         <v>20</v>
       </c>
       <c r="G22" s="175"/>
-      <c r="H22" s="363"/>
+      <c r="H22" s="373"/>
     </row>
     <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1"/>
@@ -18787,28 +18787,28 @@
     <row r="36" spans="1:8" ht="20.100000000000001" customHeight="1"/>
     <row r="37" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1"/>
     <row r="38" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A38" s="364" t="s">
+      <c r="A38" s="374" t="s">
         <v>953</v>
       </c>
-      <c r="B38" s="365"/>
-      <c r="C38" s="365"/>
-      <c r="D38" s="365"/>
-      <c r="E38" s="365"/>
-      <c r="F38" s="366"/>
+      <c r="B38" s="375"/>
+      <c r="C38" s="375"/>
+      <c r="D38" s="375"/>
+      <c r="E38" s="375"/>
+      <c r="F38" s="376"/>
       <c r="G38" s="175"/>
       <c r="H38" s="175"/>
     </row>
     <row r="39" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A39" s="367" t="s">
+      <c r="A39" s="377" t="s">
         <v>840</v>
       </c>
-      <c r="B39" s="368"/>
-      <c r="C39" s="369"/>
-      <c r="D39" s="367" t="s">
+      <c r="B39" s="378"/>
+      <c r="C39" s="379"/>
+      <c r="D39" s="377" t="s">
         <v>841</v>
       </c>
-      <c r="E39" s="368"/>
-      <c r="F39" s="369"/>
+      <c r="E39" s="378"/>
+      <c r="F39" s="379"/>
       <c r="G39" s="175"/>
       <c r="H39" s="175"/>
     </row>
@@ -18832,7 +18832,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="175"/>
-      <c r="H40" s="370" t="s">
+      <c r="H40" s="368" t="s">
         <v>844</v>
       </c>
     </row>
@@ -18856,7 +18856,7 @@
         <v>2</v>
       </c>
       <c r="G41" s="175"/>
-      <c r="H41" s="371"/>
+      <c r="H41" s="369"/>
     </row>
     <row r="42" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A42" s="204">
@@ -18878,7 +18878,7 @@
         <v>3</v>
       </c>
       <c r="G42" s="175"/>
-      <c r="H42" s="371"/>
+      <c r="H42" s="369"/>
     </row>
     <row r="43" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A43" s="206">
@@ -18900,7 +18900,7 @@
         <v>4</v>
       </c>
       <c r="G43" s="175"/>
-      <c r="H43" s="371"/>
+      <c r="H43" s="369"/>
     </row>
     <row r="44" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A44" s="206">
@@ -18922,7 +18922,7 @@
         <v>5</v>
       </c>
       <c r="G44" s="175"/>
-      <c r="H44" s="371"/>
+      <c r="H44" s="369"/>
     </row>
     <row r="45" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A45" s="208">
@@ -18944,7 +18944,7 @@
         <v>6</v>
       </c>
       <c r="G45" s="175"/>
-      <c r="H45" s="371"/>
+      <c r="H45" s="369"/>
     </row>
     <row r="46" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A46" s="208">
@@ -18966,7 +18966,7 @@
         <v>7</v>
       </c>
       <c r="G46" s="175"/>
-      <c r="H46" s="371"/>
+      <c r="H46" s="369"/>
     </row>
     <row r="47" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A47" s="210">
@@ -18988,7 +18988,7 @@
         <v>8</v>
       </c>
       <c r="G47" s="175"/>
-      <c r="H47" s="372"/>
+      <c r="H47" s="370"/>
     </row>
     <row r="48" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="A48" s="213">
@@ -19010,7 +19010,7 @@
         <v>9</v>
       </c>
       <c r="G48" s="175"/>
-      <c r="H48" s="361" t="s">
+      <c r="H48" s="371" t="s">
         <v>856</v>
       </c>
     </row>
@@ -19034,7 +19034,7 @@
         <v>10</v>
       </c>
       <c r="G49" s="175"/>
-      <c r="H49" s="362"/>
+      <c r="H49" s="372"/>
     </row>
     <row r="50" spans="1:8" ht="16.5" thickBot="1">
       <c r="A50" s="215">
@@ -19056,7 +19056,7 @@
         <v>11</v>
       </c>
       <c r="G50" s="175"/>
-      <c r="H50" s="362"/>
+      <c r="H50" s="372"/>
     </row>
     <row r="51" spans="1:8" ht="16.5" thickBot="1">
       <c r="A51" s="218">
@@ -19078,7 +19078,7 @@
         <v>12</v>
       </c>
       <c r="G51" s="175"/>
-      <c r="H51" s="362"/>
+      <c r="H51" s="372"/>
     </row>
     <row r="52" spans="1:8" ht="16.5" thickBot="1">
       <c r="A52" s="218">
@@ -19100,7 +19100,7 @@
         <v>13</v>
       </c>
       <c r="G52" s="175"/>
-      <c r="H52" s="362"/>
+      <c r="H52" s="372"/>
     </row>
     <row r="53" spans="1:8" ht="16.5" thickBot="1">
       <c r="A53" s="218">
@@ -19122,7 +19122,7 @@
         <v>14</v>
       </c>
       <c r="G53" s="175"/>
-      <c r="H53" s="362"/>
+      <c r="H53" s="372"/>
     </row>
     <row r="54" spans="1:8" ht="16.5" thickBot="1">
       <c r="A54" s="218">
@@ -19144,7 +19144,7 @@
         <v>15</v>
       </c>
       <c r="G54" s="175"/>
-      <c r="H54" s="362"/>
+      <c r="H54" s="372"/>
     </row>
     <row r="55" spans="1:8" ht="16.5" thickBot="1">
       <c r="A55" s="218">
@@ -19166,7 +19166,7 @@
         <v>16</v>
       </c>
       <c r="G55" s="175"/>
-      <c r="H55" s="362"/>
+      <c r="H55" s="372"/>
     </row>
     <row r="56" spans="1:8" ht="16.5" thickBot="1">
       <c r="A56" s="218">
@@ -19188,7 +19188,7 @@
         <v>17</v>
       </c>
       <c r="G56" s="175"/>
-      <c r="H56" s="362"/>
+      <c r="H56" s="372"/>
     </row>
     <row r="57" spans="1:8" ht="16.5" thickBot="1">
       <c r="A57" s="220">
@@ -19210,7 +19210,7 @@
         <v>18</v>
       </c>
       <c r="G57" s="175"/>
-      <c r="H57" s="362"/>
+      <c r="H57" s="372"/>
     </row>
     <row r="58" spans="1:8" ht="16.5" thickBot="1">
       <c r="A58" s="220">
@@ -19232,7 +19232,7 @@
         <v>19</v>
       </c>
       <c r="G58" s="175"/>
-      <c r="H58" s="362"/>
+      <c r="H58" s="372"/>
     </row>
     <row r="59" spans="1:8" ht="16.5" thickBot="1">
       <c r="A59" s="222">
@@ -19254,21 +19254,21 @@
         <v>20</v>
       </c>
       <c r="G59" s="175"/>
-      <c r="H59" s="363"/>
+      <c r="H59" s="373"/>
     </row>
     <row r="60" spans="1:8" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="H48:H59"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="H40:H47"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="H3:H10"/>
     <mergeCell ref="H11:H22"/>
-    <mergeCell ref="H48:H59"/>
-    <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="H40:H47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -19297,40 +19297,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="385" t="s">
+      <c r="A1" s="386" t="s">
         <v>327</v>
       </c>
-      <c r="B1" s="386"/>
-      <c r="C1" s="386"/>
-      <c r="D1" s="386"/>
-      <c r="E1" s="386"/>
-      <c r="F1" s="386"/>
-      <c r="G1" s="386"/>
-      <c r="H1" s="387"/>
+      <c r="B1" s="387"/>
+      <c r="C1" s="387"/>
+      <c r="D1" s="387"/>
+      <c r="E1" s="387"/>
+      <c r="F1" s="387"/>
+      <c r="G1" s="387"/>
+      <c r="H1" s="388"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="388"/>
-      <c r="B2" s="389"/>
-      <c r="C2" s="389"/>
-      <c r="D2" s="389"/>
-      <c r="E2" s="389"/>
-      <c r="F2" s="389"/>
-      <c r="G2" s="389"/>
-      <c r="H2" s="390"/>
+      <c r="A2" s="389"/>
+      <c r="B2" s="390"/>
+      <c r="C2" s="390"/>
+      <c r="D2" s="390"/>
+      <c r="E2" s="390"/>
+      <c r="F2" s="390"/>
+      <c r="G2" s="390"/>
+      <c r="H2" s="391"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="379" t="s">
+      <c r="A3" s="380" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="380"/>
-      <c r="C3" s="380"/>
-      <c r="D3" s="381"/>
-      <c r="E3" s="379" t="s">
+      <c r="B3" s="381"/>
+      <c r="C3" s="381"/>
+      <c r="D3" s="382"/>
+      <c r="E3" s="380" t="s">
         <v>314</v>
       </c>
-      <c r="F3" s="380"/>
-      <c r="G3" s="380"/>
-      <c r="H3" s="381"/>
+      <c r="F3" s="381"/>
+      <c r="G3" s="381"/>
+      <c r="H3" s="382"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="77">
@@ -19547,18 +19547,18 @@
       <c r="H21" s="69"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="382" t="s">
+      <c r="A22" s="383" t="s">
         <v>315</v>
       </c>
-      <c r="B22" s="383"/>
-      <c r="C22" s="383"/>
-      <c r="D22" s="384"/>
-      <c r="E22" s="382" t="s">
+      <c r="B22" s="384"/>
+      <c r="C22" s="384"/>
+      <c r="D22" s="385"/>
+      <c r="E22" s="383" t="s">
         <v>316</v>
       </c>
-      <c r="F22" s="383"/>
-      <c r="G22" s="383"/>
-      <c r="H22" s="384"/>
+      <c r="F22" s="384"/>
+      <c r="G22" s="384"/>
+      <c r="H22" s="385"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="62">
@@ -19835,40 +19835,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="319" t="s">
+      <c r="A1" s="324" t="s">
         <v>488</v>
       </c>
-      <c r="B1" s="320"/>
-      <c r="C1" s="320"/>
-      <c r="D1" s="320"/>
-      <c r="E1" s="320"/>
-      <c r="F1" s="320"/>
-      <c r="G1" s="320"/>
-      <c r="H1" s="321"/>
+      <c r="B1" s="325"/>
+      <c r="C1" s="325"/>
+      <c r="D1" s="325"/>
+      <c r="E1" s="325"/>
+      <c r="F1" s="325"/>
+      <c r="G1" s="325"/>
+      <c r="H1" s="326"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="322"/>
-      <c r="B2" s="323"/>
-      <c r="C2" s="323"/>
-      <c r="D2" s="323"/>
-      <c r="E2" s="323"/>
-      <c r="F2" s="323"/>
-      <c r="G2" s="323"/>
-      <c r="H2" s="324"/>
+      <c r="A2" s="327"/>
+      <c r="B2" s="328"/>
+      <c r="C2" s="328"/>
+      <c r="D2" s="328"/>
+      <c r="E2" s="328"/>
+      <c r="F2" s="328"/>
+      <c r="G2" s="328"/>
+      <c r="H2" s="329"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="325" t="s">
+      <c r="A3" s="330" t="s">
         <v>319</v>
       </c>
-      <c r="B3" s="326"/>
-      <c r="C3" s="326"/>
-      <c r="D3" s="326"/>
-      <c r="E3" s="326" t="s">
+      <c r="B3" s="331"/>
+      <c r="C3" s="331"/>
+      <c r="D3" s="331"/>
+      <c r="E3" s="331" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="326"/>
-      <c r="G3" s="326"/>
-      <c r="H3" s="327"/>
+      <c r="F3" s="331"/>
+      <c r="G3" s="331"/>
+      <c r="H3" s="332"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="12">

</xml_diff>

<commit_message>
chg: Added red tankers to SW corner of range 17. Expanded range 17. Master communication file updated with freqs, CombatFlite update with pattern, and range 17 expansion, Tanker brief page updated
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2239" uniqueCount="1337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2249" uniqueCount="1344">
   <si>
     <t>AWACS</t>
   </si>
@@ -4035,6 +4035,27 @@
   </si>
   <si>
     <t>128.4</t>
+  </si>
+  <si>
+    <t>AR404 #IFF:5404FR</t>
+  </si>
+  <si>
+    <t>ARCO 7</t>
+  </si>
+  <si>
+    <t>41X</t>
+  </si>
+  <si>
+    <t>AR504 #IFF:5504FR</t>
+  </si>
+  <si>
+    <t>SHELL 8</t>
+  </si>
+  <si>
+    <t>48X</t>
+  </si>
+  <si>
+    <t>GOLD 12</t>
   </si>
 </sst>
 </file>
@@ -6688,12 +6709,21 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6703,13 +6733,49 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6721,50 +6787,35 @@
     <xf numFmtId="0" fontId="25" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6775,36 +6826,6 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6892,6 +6913,42 @@
     <xf numFmtId="49" fontId="45" fillId="31" borderId="93" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="26" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="26" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="26" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6910,42 +6967,6 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="26" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="26" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="26" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7018,6 +7039,57 @@
     <xf numFmtId="0" fontId="32" fillId="20" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7035,57 +7107,6 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7399,8 +7420,8 @@
   <sheetPr codeName="Ark1"/>
   <dimension ref="A1:AP83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M67" sqref="M67"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AL41" sqref="AL41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -7507,13 +7528,13 @@
       <c r="N2" s="107" t="s">
         <v>330</v>
       </c>
-      <c r="V2" s="295" t="s">
+      <c r="V2" s="294" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="295"/>
-      <c r="X2" s="295"/>
-      <c r="Y2" s="295"/>
-      <c r="Z2" s="295"/>
+      <c r="W2" s="294"/>
+      <c r="X2" s="294"/>
+      <c r="Y2" s="294"/>
+      <c r="Z2" s="294"/>
     </row>
     <row r="3" spans="1:42">
       <c r="A3" s="107" t="s">
@@ -7562,9 +7583,9 @@
       <c r="P3" t="s">
         <v>426</v>
       </c>
-      <c r="R3" s="294"/>
-      <c r="S3" s="294"/>
-      <c r="T3" s="294"/>
+      <c r="R3" s="298"/>
+      <c r="S3" s="298"/>
+      <c r="T3" s="298"/>
       <c r="V3" s="101" t="s">
         <v>328</v>
       </c>
@@ -7646,22 +7667,22 @@
       <c r="AA4" s="23"/>
       <c r="AB4" s="23"/>
       <c r="AC4" s="23"/>
-      <c r="AD4" s="295" t="s">
+      <c r="AD4" s="294" t="s">
         <v>429</v>
       </c>
-      <c r="AE4" s="295"/>
-      <c r="AF4" s="295"/>
-      <c r="AG4" s="295"/>
-      <c r="AH4" s="295"/>
-      <c r="AJ4" s="295" t="s">
+      <c r="AE4" s="294"/>
+      <c r="AF4" s="294"/>
+      <c r="AG4" s="294"/>
+      <c r="AH4" s="294"/>
+      <c r="AJ4" s="294" t="s">
         <v>1</v>
       </c>
-      <c r="AK4" s="295"/>
-      <c r="AL4" s="295"/>
-      <c r="AM4" s="295"/>
-      <c r="AN4" s="295"/>
-      <c r="AO4" s="295"/>
-      <c r="AP4" s="295"/>
+      <c r="AK4" s="294"/>
+      <c r="AL4" s="294"/>
+      <c r="AM4" s="294"/>
+      <c r="AN4" s="294"/>
+      <c r="AO4" s="294"/>
+      <c r="AP4" s="294"/>
     </row>
     <row r="5" spans="1:42" ht="15.75">
       <c r="A5" s="107" t="s">
@@ -8234,7 +8255,7 @@
       <c r="L11" s="108" t="s">
         <v>147</v>
       </c>
-      <c r="M11" s="9" t="s">
+      <c r="M11" s="112" t="s">
         <v>1228</v>
       </c>
       <c r="N11" s="107" t="s">
@@ -8649,6 +8670,27 @@
       <c r="AH15" s="3" t="s">
         <v>463</v>
       </c>
+      <c r="AJ15" s="115" t="s">
+        <v>1337</v>
+      </c>
+      <c r="AK15" s="9" t="s">
+        <v>1338</v>
+      </c>
+      <c r="AL15" s="112" t="s">
+        <v>510</v>
+      </c>
+      <c r="AM15" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="AN15" s="3" t="s">
+        <v>1339</v>
+      </c>
+      <c r="AO15" s="3">
+        <v>5404</v>
+      </c>
+      <c r="AP15" s="3">
+        <v>207</v>
+      </c>
     </row>
     <row r="16" spans="1:42" ht="15.75">
       <c r="A16" s="107" t="s">
@@ -8877,15 +8919,15 @@
       <c r="AH18" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="AJ18" s="295" t="s">
+      <c r="AJ18" s="294" t="s">
         <v>274</v>
       </c>
-      <c r="AK18" s="295"/>
-      <c r="AL18" s="295"/>
-      <c r="AM18" s="295"/>
-      <c r="AN18" s="295"/>
-      <c r="AO18" s="295"/>
-      <c r="AP18" s="295"/>
+      <c r="AK18" s="294"/>
+      <c r="AL18" s="294"/>
+      <c r="AM18" s="294"/>
+      <c r="AN18" s="294"/>
+      <c r="AO18" s="294"/>
+      <c r="AP18" s="294"/>
     </row>
     <row r="19" spans="1:42" ht="15.75">
       <c r="A19" s="107" t="s">
@@ -9018,9 +9060,9 @@
       </c>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="294"/>
-      <c r="S20" s="294"/>
-      <c r="T20" s="294"/>
+      <c r="R20" s="298"/>
+      <c r="S20" s="298"/>
+      <c r="T20" s="298"/>
       <c r="U20" s="2"/>
       <c r="V20" s="272" t="s">
         <v>1253</v>
@@ -9435,13 +9477,13 @@
       <c r="S25" s="24"/>
       <c r="T25" s="24"/>
       <c r="X25" s="2"/>
-      <c r="AD25" s="295" t="s">
+      <c r="AD25" s="294" t="s">
         <v>486</v>
       </c>
-      <c r="AE25" s="295"/>
-      <c r="AF25" s="295"/>
-      <c r="AG25" s="295"/>
-      <c r="AH25" s="295"/>
+      <c r="AE25" s="294"/>
+      <c r="AF25" s="294"/>
+      <c r="AG25" s="294"/>
+      <c r="AH25" s="294"/>
       <c r="AJ25" s="116" t="s">
         <v>555</v>
       </c>
@@ -9493,7 +9535,7 @@
         <v>420</v>
       </c>
       <c r="L26" s="9"/>
-      <c r="M26" s="9" t="s">
+      <c r="M26" s="112" t="s">
         <v>510</v>
       </c>
       <c r="N26" s="107" t="s">
@@ -9603,6 +9645,27 @@
       <c r="AH27" s="3" t="s">
         <v>485</v>
       </c>
+      <c r="AJ27" s="116" t="s">
+        <v>1340</v>
+      </c>
+      <c r="AK27" s="3" t="s">
+        <v>1341</v>
+      </c>
+      <c r="AL27" s="112" t="s">
+        <v>1228</v>
+      </c>
+      <c r="AM27" s="3" t="s">
+        <v>1343</v>
+      </c>
+      <c r="AN27" s="3" t="s">
+        <v>1342</v>
+      </c>
+      <c r="AO27" s="3">
+        <v>5504</v>
+      </c>
+      <c r="AP27" s="3">
+        <v>308</v>
+      </c>
     </row>
     <row r="28" spans="1:42">
       <c r="A28" s="107" t="s">
@@ -9691,15 +9754,15 @@
       <c r="N29" s="107" t="s">
         <v>355</v>
       </c>
-      <c r="V29" s="295" t="s">
+      <c r="V29" s="294" t="s">
         <v>212</v>
       </c>
-      <c r="W29" s="295"/>
-      <c r="X29" s="295"/>
-      <c r="Y29" s="295"/>
-      <c r="Z29" s="295"/>
-      <c r="AA29" s="295"/>
-      <c r="AB29" s="295"/>
+      <c r="W29" s="294"/>
+      <c r="X29" s="294"/>
+      <c r="Y29" s="294"/>
+      <c r="Z29" s="294"/>
+      <c r="AA29" s="294"/>
+      <c r="AB29" s="294"/>
     </row>
     <row r="30" spans="1:42">
       <c r="A30" s="107"/>
@@ -9755,15 +9818,15 @@
       </c>
       <c r="AA30" s="29"/>
       <c r="AB30" s="29"/>
-      <c r="AJ30" s="295" t="s">
+      <c r="AJ30" s="294" t="s">
         <v>831</v>
       </c>
-      <c r="AK30" s="295"/>
-      <c r="AL30" s="295"/>
-      <c r="AM30" s="295"/>
-      <c r="AN30" s="295"/>
-      <c r="AO30" s="295"/>
-      <c r="AP30" s="295"/>
+      <c r="AK30" s="294"/>
+      <c r="AL30" s="294"/>
+      <c r="AM30" s="294"/>
+      <c r="AN30" s="294"/>
+      <c r="AO30" s="294"/>
+      <c r="AP30" s="294"/>
     </row>
     <row r="31" spans="1:42">
       <c r="B31" s="24"/>
@@ -9850,15 +9913,15 @@
       <c r="AJ34" s="23"/>
     </row>
     <row r="37" spans="22:36">
-      <c r="V37" s="295" t="s">
+      <c r="V37" s="294" t="s">
         <v>9</v>
       </c>
-      <c r="W37" s="295"/>
-      <c r="X37" s="295"/>
-      <c r="Y37" s="295"/>
-      <c r="Z37" s="295"/>
-      <c r="AA37" s="295"/>
-      <c r="AB37" s="295"/>
+      <c r="W37" s="294"/>
+      <c r="X37" s="294"/>
+      <c r="Y37" s="294"/>
+      <c r="Z37" s="294"/>
+      <c r="AA37" s="294"/>
+      <c r="AB37" s="294"/>
     </row>
     <row r="38" spans="22:36">
       <c r="V38" s="29" t="s">
@@ -9878,11 +9941,11 @@
       </c>
       <c r="AA38" s="29"/>
       <c r="AB38" s="29"/>
-      <c r="AD38" s="296" t="s">
+      <c r="AD38" s="299" t="s">
         <v>260</v>
       </c>
-      <c r="AE38" s="297"/>
-      <c r="AF38" s="298"/>
+      <c r="AE38" s="300"/>
+      <c r="AF38" s="301"/>
     </row>
     <row r="39" spans="22:36">
       <c r="V39" s="3" t="s">
@@ -9919,15 +9982,15 @@
       <c r="AF41" s="3"/>
     </row>
     <row r="42" spans="22:36">
-      <c r="V42" s="295" t="s">
+      <c r="V42" s="294" t="s">
         <v>244</v>
       </c>
-      <c r="W42" s="295"/>
-      <c r="X42" s="295"/>
-      <c r="Y42" s="295"/>
-      <c r="Z42" s="295"/>
-      <c r="AA42" s="295"/>
-      <c r="AB42" s="295"/>
+      <c r="W42" s="294"/>
+      <c r="X42" s="294"/>
+      <c r="Y42" s="294"/>
+      <c r="Z42" s="294"/>
+      <c r="AA42" s="294"/>
+      <c r="AB42" s="294"/>
       <c r="AD42" s="3" t="s">
         <v>254</v>
       </c>
@@ -9997,15 +10060,15 @@
       <c r="AF47" s="3"/>
     </row>
     <row r="48" spans="22:36">
-      <c r="V48" s="299" t="s">
+      <c r="V48" s="295" t="s">
         <v>473</v>
       </c>
-      <c r="W48" s="300"/>
-      <c r="X48" s="300"/>
-      <c r="Y48" s="300"/>
-      <c r="Z48" s="300"/>
-      <c r="AA48" s="300"/>
-      <c r="AB48" s="301"/>
+      <c r="W48" s="296"/>
+      <c r="X48" s="296"/>
+      <c r="Y48" s="296"/>
+      <c r="Z48" s="296"/>
+      <c r="AA48" s="296"/>
+      <c r="AB48" s="297"/>
       <c r="AD48" s="3" t="s">
         <v>261</v>
       </c>
@@ -10615,11 +10678,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="V42:AB42"/>
-    <mergeCell ref="AD4:AH4"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="V48:AB48"/>
-    <mergeCell ref="V37:AB37"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="AJ4:AP4"/>
@@ -10628,6 +10686,11 @@
     <mergeCell ref="V29:AB29"/>
     <mergeCell ref="AD25:AH25"/>
     <mergeCell ref="AJ30:AP30"/>
+    <mergeCell ref="V42:AB42"/>
+    <mergeCell ref="AD4:AH4"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="V48:AB48"/>
+    <mergeCell ref="V37:AB37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11587,40 +11650,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="421" t="s">
+      <c r="A1" s="404" t="s">
         <v>326</v>
       </c>
-      <c r="B1" s="421"/>
-      <c r="C1" s="421"/>
-      <c r="D1" s="421"/>
-      <c r="E1" s="421"/>
-      <c r="F1" s="421"/>
-      <c r="G1" s="421"/>
-      <c r="H1" s="421"/>
+      <c r="B1" s="404"/>
+      <c r="C1" s="404"/>
+      <c r="D1" s="404"/>
+      <c r="E1" s="404"/>
+      <c r="F1" s="404"/>
+      <c r="G1" s="404"/>
+      <c r="H1" s="404"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="422"/>
-      <c r="B2" s="422"/>
-      <c r="C2" s="422"/>
-      <c r="D2" s="422"/>
-      <c r="E2" s="422"/>
-      <c r="F2" s="422"/>
-      <c r="G2" s="422"/>
-      <c r="H2" s="422"/>
+      <c r="A2" s="405"/>
+      <c r="B2" s="405"/>
+      <c r="C2" s="405"/>
+      <c r="D2" s="405"/>
+      <c r="E2" s="405"/>
+      <c r="F2" s="405"/>
+      <c r="G2" s="405"/>
+      <c r="H2" s="405"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="423" t="s">
+      <c r="A3" s="406" t="s">
         <v>227</v>
       </c>
-      <c r="B3" s="424"/>
-      <c r="C3" s="425"/>
-      <c r="D3" s="426"/>
-      <c r="E3" s="423" t="s">
+      <c r="B3" s="407"/>
+      <c r="C3" s="408"/>
+      <c r="D3" s="409"/>
+      <c r="E3" s="406" t="s">
         <v>228</v>
       </c>
-      <c r="F3" s="424"/>
-      <c r="G3" s="425"/>
-      <c r="H3" s="426"/>
+      <c r="F3" s="407"/>
+      <c r="G3" s="408"/>
+      <c r="H3" s="409"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="31">
@@ -11913,18 +11976,18 @@
       <c r="H24" s="59"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="423" t="s">
+      <c r="A25" s="406" t="s">
         <v>289</v>
       </c>
-      <c r="B25" s="424"/>
-      <c r="C25" s="425"/>
-      <c r="D25" s="426"/>
-      <c r="E25" s="423" t="s">
+      <c r="B25" s="407"/>
+      <c r="C25" s="408"/>
+      <c r="D25" s="409"/>
+      <c r="E25" s="406" t="s">
         <v>290</v>
       </c>
-      <c r="F25" s="424"/>
-      <c r="G25" s="425"/>
-      <c r="H25" s="426"/>
+      <c r="F25" s="407"/>
+      <c r="G25" s="408"/>
+      <c r="H25" s="409"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="35" t="s">
@@ -11936,23 +11999,23 @@
       <c r="E26" s="31" t="s">
         <v>292</v>
       </c>
-      <c r="F26" s="418"/>
-      <c r="G26" s="419"/>
-      <c r="H26" s="420"/>
+      <c r="F26" s="413"/>
+      <c r="G26" s="414"/>
+      <c r="H26" s="415"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="B27" s="413"/>
-      <c r="C27" s="414"/>
-      <c r="D27" s="416"/>
+      <c r="B27" s="416"/>
+      <c r="C27" s="417"/>
+      <c r="D27" s="418"/>
       <c r="E27" s="35" t="s">
         <v>294</v>
       </c>
       <c r="F27" s="410"/>
       <c r="G27" s="411"/>
-      <c r="H27" s="417"/>
+      <c r="H27" s="419"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="35" t="s">
@@ -11964,23 +12027,23 @@
       <c r="E28" s="43" t="s">
         <v>296</v>
       </c>
-      <c r="F28" s="413"/>
-      <c r="G28" s="414"/>
-      <c r="H28" s="415"/>
+      <c r="F28" s="416"/>
+      <c r="G28" s="417"/>
+      <c r="H28" s="420"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="43" t="s">
         <v>297</v>
       </c>
-      <c r="B29" s="413"/>
-      <c r="C29" s="414"/>
-      <c r="D29" s="416"/>
+      <c r="B29" s="416"/>
+      <c r="C29" s="417"/>
+      <c r="D29" s="418"/>
       <c r="E29" s="35" t="s">
         <v>298</v>
       </c>
       <c r="F29" s="410"/>
       <c r="G29" s="411"/>
-      <c r="H29" s="417"/>
+      <c r="H29" s="419"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="35" t="s">
@@ -11992,23 +12055,23 @@
       <c r="E30" s="43" t="s">
         <v>300</v>
       </c>
-      <c r="F30" s="413"/>
-      <c r="G30" s="414"/>
-      <c r="H30" s="415"/>
+      <c r="F30" s="416"/>
+      <c r="G30" s="417"/>
+      <c r="H30" s="420"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="43" t="s">
         <v>301</v>
       </c>
-      <c r="B31" s="413"/>
-      <c r="C31" s="414"/>
-      <c r="D31" s="416"/>
+      <c r="B31" s="416"/>
+      <c r="C31" s="417"/>
+      <c r="D31" s="418"/>
       <c r="E31" s="35" t="s">
         <v>302</v>
       </c>
       <c r="F31" s="410"/>
       <c r="G31" s="411"/>
-      <c r="H31" s="417"/>
+      <c r="H31" s="419"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="35" t="s">
@@ -12018,9 +12081,9 @@
       <c r="C32" s="411"/>
       <c r="D32" s="412"/>
       <c r="E32" s="43"/>
-      <c r="F32" s="413"/>
-      <c r="G32" s="414"/>
-      <c r="H32" s="415" t="s">
+      <c r="F32" s="416"/>
+      <c r="G32" s="417"/>
+      <c r="H32" s="420" t="s">
         <v>242</v>
       </c>
     </row>
@@ -12028,13 +12091,13 @@
       <c r="A33" s="43" t="s">
         <v>304</v>
       </c>
-      <c r="B33" s="413"/>
-      <c r="C33" s="414"/>
-      <c r="D33" s="416"/>
+      <c r="B33" s="416"/>
+      <c r="C33" s="417"/>
+      <c r="D33" s="418"/>
       <c r="E33" s="35"/>
       <c r="F33" s="410"/>
       <c r="G33" s="411"/>
-      <c r="H33" s="417" t="s">
+      <c r="H33" s="419" t="s">
         <v>284</v>
       </c>
     </row>
@@ -12046,9 +12109,9 @@
       <c r="C34" s="411"/>
       <c r="D34" s="412"/>
       <c r="E34" s="43"/>
-      <c r="F34" s="413"/>
-      <c r="G34" s="414"/>
-      <c r="H34" s="415" t="s">
+      <c r="F34" s="416"/>
+      <c r="G34" s="417"/>
+      <c r="H34" s="420" t="s">
         <v>285</v>
       </c>
     </row>
@@ -12056,13 +12119,13 @@
       <c r="A35" s="43" t="s">
         <v>306</v>
       </c>
-      <c r="B35" s="413"/>
-      <c r="C35" s="414"/>
-      <c r="D35" s="416"/>
+      <c r="B35" s="416"/>
+      <c r="C35" s="417"/>
+      <c r="D35" s="418"/>
       <c r="E35" s="35"/>
       <c r="F35" s="410"/>
       <c r="G35" s="411"/>
-      <c r="H35" s="417" t="s">
+      <c r="H35" s="419" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12074,9 +12137,9 @@
       <c r="C36" s="411"/>
       <c r="D36" s="412"/>
       <c r="E36" s="43"/>
-      <c r="F36" s="413"/>
-      <c r="G36" s="414"/>
-      <c r="H36" s="415" t="s">
+      <c r="F36" s="416"/>
+      <c r="G36" s="417"/>
+      <c r="H36" s="420" t="s">
         <v>287</v>
       </c>
     </row>
@@ -12084,13 +12147,13 @@
       <c r="A37" s="43" t="s">
         <v>308</v>
       </c>
-      <c r="B37" s="413"/>
-      <c r="C37" s="414"/>
-      <c r="D37" s="416"/>
+      <c r="B37" s="416"/>
+      <c r="C37" s="417"/>
+      <c r="D37" s="418"/>
       <c r="E37" s="35"/>
       <c r="F37" s="410"/>
       <c r="G37" s="411"/>
-      <c r="H37" s="417" t="s">
+      <c r="H37" s="419" t="s">
         <v>288</v>
       </c>
     </row>
@@ -12102,9 +12165,9 @@
       <c r="C38" s="411"/>
       <c r="D38" s="412"/>
       <c r="E38" s="43"/>
-      <c r="F38" s="413"/>
-      <c r="G38" s="414"/>
-      <c r="H38" s="415" t="s">
+      <c r="F38" s="416"/>
+      <c r="G38" s="417"/>
+      <c r="H38" s="420" t="s">
         <v>241</v>
       </c>
     </row>
@@ -12112,13 +12175,13 @@
       <c r="A39" s="43" t="s">
         <v>310</v>
       </c>
-      <c r="B39" s="413"/>
-      <c r="C39" s="414"/>
-      <c r="D39" s="416"/>
+      <c r="B39" s="416"/>
+      <c r="C39" s="417"/>
+      <c r="D39" s="418"/>
       <c r="E39" s="35"/>
       <c r="F39" s="410"/>
       <c r="G39" s="411"/>
-      <c r="H39" s="417" t="s">
+      <c r="H39" s="419" t="s">
         <v>242</v>
       </c>
     </row>
@@ -12130,53 +12193,24 @@
       <c r="C40" s="411"/>
       <c r="D40" s="412"/>
       <c r="E40" s="43"/>
-      <c r="F40" s="413"/>
-      <c r="G40" s="414"/>
-      <c r="H40" s="415"/>
+      <c r="F40" s="416"/>
+      <c r="G40" s="417"/>
+      <c r="H40" s="420"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="55" t="s">
         <v>312</v>
       </c>
-      <c r="B41" s="404"/>
-      <c r="C41" s="405"/>
-      <c r="D41" s="406"/>
+      <c r="B41" s="421"/>
+      <c r="C41" s="422"/>
+      <c r="D41" s="423"/>
       <c r="E41" s="60"/>
-      <c r="F41" s="407"/>
-      <c r="G41" s="408"/>
-      <c r="H41" s="409"/>
+      <c r="F41" s="424"/>
+      <c r="G41" s="425"/>
+      <c r="H41" s="426"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -12185,6 +12219,35 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12240,55 +12303,55 @@
       </c>
     </row>
     <row r="2" spans="2:42">
-      <c r="B2" s="295" t="s">
+      <c r="B2" s="294" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="295"/>
-      <c r="D2" s="295"/>
-      <c r="E2" s="295"/>
-      <c r="F2" s="295"/>
-      <c r="H2" s="295" t="s">
+      <c r="C2" s="294"/>
+      <c r="D2" s="294"/>
+      <c r="E2" s="294"/>
+      <c r="F2" s="294"/>
+      <c r="H2" s="294" t="s">
         <v>1055</v>
       </c>
-      <c r="I2" s="295"/>
-      <c r="J2" s="295"/>
-      <c r="K2" s="295"/>
-      <c r="L2" s="295"/>
-      <c r="N2" s="295" t="s">
+      <c r="I2" s="294"/>
+      <c r="J2" s="294"/>
+      <c r="K2" s="294"/>
+      <c r="L2" s="294"/>
+      <c r="N2" s="294" t="s">
         <v>1054</v>
       </c>
-      <c r="O2" s="295"/>
-      <c r="P2" s="295"/>
-      <c r="Q2" s="295"/>
-      <c r="R2" s="295"/>
-      <c r="T2" s="295" t="s">
+      <c r="O2" s="294"/>
+      <c r="P2" s="294"/>
+      <c r="Q2" s="294"/>
+      <c r="R2" s="294"/>
+      <c r="T2" s="294" t="s">
         <v>236</v>
       </c>
-      <c r="U2" s="295"/>
-      <c r="V2" s="295"/>
-      <c r="W2" s="295"/>
-      <c r="X2" s="295"/>
-      <c r="Z2" s="295" t="s">
+      <c r="U2" s="294"/>
+      <c r="V2" s="294"/>
+      <c r="W2" s="294"/>
+      <c r="X2" s="294"/>
+      <c r="Z2" s="294" t="s">
         <v>246</v>
       </c>
-      <c r="AA2" s="295"/>
-      <c r="AB2" s="295"/>
-      <c r="AC2" s="295"/>
-      <c r="AD2" s="295"/>
-      <c r="AF2" s="295" t="s">
+      <c r="AA2" s="294"/>
+      <c r="AB2" s="294"/>
+      <c r="AC2" s="294"/>
+      <c r="AD2" s="294"/>
+      <c r="AF2" s="294" t="s">
         <v>317</v>
       </c>
-      <c r="AG2" s="295"/>
-      <c r="AH2" s="295"/>
-      <c r="AI2" s="295"/>
-      <c r="AJ2" s="295"/>
-      <c r="AL2" s="295" t="s">
+      <c r="AG2" s="294"/>
+      <c r="AH2" s="294"/>
+      <c r="AI2" s="294"/>
+      <c r="AJ2" s="294"/>
+      <c r="AL2" s="294" t="s">
         <v>491</v>
       </c>
-      <c r="AM2" s="295"/>
-      <c r="AN2" s="295"/>
-      <c r="AO2" s="295"/>
-      <c r="AP2" s="295"/>
+      <c r="AM2" s="294"/>
+      <c r="AN2" s="294"/>
+      <c r="AO2" s="294"/>
+      <c r="AP2" s="294"/>
     </row>
     <row r="3" spans="2:42">
       <c r="B3" s="101" t="s">
@@ -13922,20 +13985,20 @@
       <c r="X39" s="59"/>
     </row>
     <row r="41" spans="2:24">
-      <c r="B41" s="295" t="s">
+      <c r="B41" s="294" t="s">
         <v>697</v>
       </c>
-      <c r="C41" s="295"/>
-      <c r="D41" s="295"/>
-      <c r="E41" s="295"/>
-      <c r="F41" s="295"/>
-      <c r="H41" s="295" t="s">
+      <c r="C41" s="294"/>
+      <c r="D41" s="294"/>
+      <c r="E41" s="294"/>
+      <c r="F41" s="294"/>
+      <c r="H41" s="294" t="s">
         <v>750</v>
       </c>
-      <c r="I41" s="295"/>
-      <c r="J41" s="295"/>
-      <c r="K41" s="295"/>
-      <c r="L41" s="295"/>
+      <c r="I41" s="294"/>
+      <c r="J41" s="294"/>
+      <c r="K41" s="294"/>
+      <c r="L41" s="294"/>
     </row>
     <row r="42" spans="2:24">
       <c r="B42" s="101" t="s">
@@ -14472,39 +14535,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27" customHeight="1" thickBot="1">
-      <c r="A1" s="311" t="s">
+      <c r="A1" s="314" t="s">
         <v>1146</v>
       </c>
-      <c r="B1" s="312"/>
-      <c r="C1" s="312"/>
-      <c r="D1" s="312"/>
-      <c r="E1" s="312"/>
-      <c r="F1" s="312"/>
-      <c r="G1" s="312"/>
-      <c r="H1" s="312"/>
-      <c r="I1" s="312"/>
-      <c r="J1" s="312"/>
-      <c r="K1" s="312"/>
-      <c r="L1" s="313"/>
+      <c r="B1" s="315"/>
+      <c r="C1" s="315"/>
+      <c r="D1" s="315"/>
+      <c r="E1" s="315"/>
+      <c r="F1" s="315"/>
+      <c r="G1" s="315"/>
+      <c r="H1" s="315"/>
+      <c r="I1" s="315"/>
+      <c r="J1" s="315"/>
+      <c r="K1" s="315"/>
+      <c r="L1" s="316"/>
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A2" s="308" t="s">
+      <c r="A2" s="311" t="s">
         <v>1147</v>
       </c>
-      <c r="B2" s="309"/>
-      <c r="C2" s="310"/>
+      <c r="B2" s="312"/>
+      <c r="C2" s="313"/>
       <c r="D2" s="259"/>
-      <c r="E2" s="308" t="s">
+      <c r="E2" s="311" t="s">
         <v>1055</v>
       </c>
-      <c r="F2" s="309"/>
-      <c r="G2" s="310"/>
+      <c r="F2" s="312"/>
+      <c r="G2" s="313"/>
       <c r="H2" s="259"/>
-      <c r="I2" s="308" t="s">
+      <c r="I2" s="311" t="s">
         <v>1054</v>
       </c>
-      <c r="J2" s="309"/>
-      <c r="K2" s="310"/>
+      <c r="J2" s="312"/>
+      <c r="K2" s="313"/>
       <c r="L2" s="122"/>
     </row>
     <row r="3" spans="1:12" ht="19.5" thickBot="1">
@@ -14540,7 +14603,7 @@
       <c r="L3" s="122"/>
     </row>
     <row r="4" spans="1:12" ht="18.75">
-      <c r="A4" s="302" t="s">
+      <c r="A4" s="317" t="s">
         <v>325</v>
       </c>
       <c r="B4" s="132" t="s">
@@ -14550,7 +14613,7 @@
         <v>705</v>
       </c>
       <c r="D4" s="253"/>
-      <c r="E4" s="305" t="s">
+      <c r="E4" s="308" t="s">
         <v>975</v>
       </c>
       <c r="F4" s="132" t="s">
@@ -14560,7 +14623,7 @@
         <v>1028</v>
       </c>
       <c r="H4" s="125"/>
-      <c r="I4" s="305" t="s">
+      <c r="I4" s="308" t="s">
         <v>1057</v>
       </c>
       <c r="J4" s="132" t="s">
@@ -14572,7 +14635,7 @@
       <c r="L4" s="122"/>
     </row>
     <row r="5" spans="1:12" ht="18.75">
-      <c r="A5" s="303"/>
+      <c r="A5" s="318"/>
       <c r="B5" s="131" t="s">
         <v>322</v>
       </c>
@@ -14580,7 +14643,7 @@
         <v>706</v>
       </c>
       <c r="D5" s="253"/>
-      <c r="E5" s="306"/>
+      <c r="E5" s="309"/>
       <c r="F5" s="131" t="s">
         <v>1002</v>
       </c>
@@ -14588,7 +14651,7 @@
         <v>1029</v>
       </c>
       <c r="H5" s="125"/>
-      <c r="I5" s="306"/>
+      <c r="I5" s="309"/>
       <c r="J5" s="131" t="s">
         <v>1092</v>
       </c>
@@ -14598,7 +14661,7 @@
       <c r="L5" s="122"/>
     </row>
     <row r="6" spans="1:12" ht="18.75">
-      <c r="A6" s="303"/>
+      <c r="A6" s="318"/>
       <c r="B6" s="131" t="s">
         <v>323</v>
       </c>
@@ -14606,7 +14669,7 @@
         <v>707</v>
       </c>
       <c r="D6" s="253"/>
-      <c r="E6" s="306"/>
+      <c r="E6" s="309"/>
       <c r="F6" s="131" t="s">
         <v>1003</v>
       </c>
@@ -14614,7 +14677,7 @@
         <v>1030</v>
       </c>
       <c r="H6" s="125"/>
-      <c r="I6" s="306"/>
+      <c r="I6" s="309"/>
       <c r="J6" s="131" t="s">
         <v>1093</v>
       </c>
@@ -14624,7 +14687,7 @@
       <c r="L6" s="122"/>
     </row>
     <row r="7" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A7" s="304"/>
+      <c r="A7" s="319"/>
       <c r="B7" s="135" t="s">
         <v>324</v>
       </c>
@@ -14632,7 +14695,7 @@
         <v>708</v>
       </c>
       <c r="D7" s="253"/>
-      <c r="E7" s="307"/>
+      <c r="E7" s="310"/>
       <c r="F7" s="135" t="s">
         <v>1004</v>
       </c>
@@ -14640,7 +14703,7 @@
         <v>1031</v>
       </c>
       <c r="H7" s="125"/>
-      <c r="I7" s="307"/>
+      <c r="I7" s="310"/>
       <c r="J7" s="135" t="s">
         <v>1094</v>
       </c>
@@ -14650,7 +14713,7 @@
       <c r="L7" s="122"/>
     </row>
     <row r="8" spans="1:12" ht="18.75">
-      <c r="A8" s="302" t="s">
+      <c r="A8" s="317" t="s">
         <v>667</v>
       </c>
       <c r="B8" s="132" t="s">
@@ -14660,7 +14723,7 @@
         <v>709</v>
       </c>
       <c r="D8" s="253"/>
-      <c r="E8" s="305" t="s">
+      <c r="E8" s="308" t="s">
         <v>974</v>
       </c>
       <c r="F8" s="132" t="s">
@@ -14670,7 +14733,7 @@
         <v>1032</v>
       </c>
       <c r="H8" s="125"/>
-      <c r="I8" s="305" t="s">
+      <c r="I8" s="308" t="s">
         <v>1058</v>
       </c>
       <c r="J8" s="132" t="s">
@@ -14682,7 +14745,7 @@
       <c r="L8" s="122"/>
     </row>
     <row r="9" spans="1:12" ht="18.75">
-      <c r="A9" s="303"/>
+      <c r="A9" s="318"/>
       <c r="B9" s="131" t="s">
         <v>658</v>
       </c>
@@ -14690,7 +14753,7 @@
         <v>710</v>
       </c>
       <c r="D9" s="253"/>
-      <c r="E9" s="306"/>
+      <c r="E9" s="309"/>
       <c r="F9" s="131" t="s">
         <v>1006</v>
       </c>
@@ -14698,7 +14761,7 @@
         <v>1033</v>
       </c>
       <c r="H9" s="125"/>
-      <c r="I9" s="306"/>
+      <c r="I9" s="309"/>
       <c r="J9" s="131" t="s">
         <v>1095</v>
       </c>
@@ -14708,7 +14771,7 @@
       <c r="L9" s="122"/>
     </row>
     <row r="10" spans="1:12" ht="18.75">
-      <c r="A10" s="303"/>
+      <c r="A10" s="318"/>
       <c r="B10" s="131" t="s">
         <v>659</v>
       </c>
@@ -14716,7 +14779,7 @@
         <v>711</v>
       </c>
       <c r="D10" s="253"/>
-      <c r="E10" s="306"/>
+      <c r="E10" s="309"/>
       <c r="F10" s="131" t="s">
         <v>1008</v>
       </c>
@@ -14724,7 +14787,7 @@
         <v>1034</v>
       </c>
       <c r="H10" s="125"/>
-      <c r="I10" s="306"/>
+      <c r="I10" s="309"/>
       <c r="J10" s="131" t="s">
         <v>1096</v>
       </c>
@@ -14734,7 +14797,7 @@
       <c r="L10" s="122"/>
     </row>
     <row r="11" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A11" s="304"/>
+      <c r="A11" s="319"/>
       <c r="B11" s="135" t="s">
         <v>660</v>
       </c>
@@ -14742,7 +14805,7 @@
         <v>712</v>
       </c>
       <c r="D11" s="253"/>
-      <c r="E11" s="307"/>
+      <c r="E11" s="310"/>
       <c r="F11" s="135" t="s">
         <v>1009</v>
       </c>
@@ -14750,7 +14813,7 @@
         <v>1035</v>
       </c>
       <c r="H11" s="125"/>
-      <c r="I11" s="307"/>
+      <c r="I11" s="310"/>
       <c r="J11" s="135" t="s">
         <v>1097</v>
       </c>
@@ -14760,7 +14823,7 @@
       <c r="L11" s="122"/>
     </row>
     <row r="12" spans="1:12" ht="18.75">
-      <c r="A12" s="302" t="s">
+      <c r="A12" s="317" t="s">
         <v>665</v>
       </c>
       <c r="B12" s="132" t="s">
@@ -14770,7 +14833,7 @@
         <v>713</v>
       </c>
       <c r="D12" s="253"/>
-      <c r="E12" s="305" t="s">
+      <c r="E12" s="308" t="s">
         <v>973</v>
       </c>
       <c r="F12" s="132" t="s">
@@ -14780,7 +14843,7 @@
         <v>1036</v>
       </c>
       <c r="H12" s="125"/>
-      <c r="I12" s="305" t="s">
+      <c r="I12" s="308" t="s">
         <v>1059</v>
       </c>
       <c r="J12" s="132" t="s">
@@ -14792,7 +14855,7 @@
       <c r="L12" s="122"/>
     </row>
     <row r="13" spans="1:12" ht="18.75">
-      <c r="A13" s="303"/>
+      <c r="A13" s="318"/>
       <c r="B13" s="131" t="s">
         <v>662</v>
       </c>
@@ -14800,7 +14863,7 @@
         <v>714</v>
       </c>
       <c r="D13" s="253"/>
-      <c r="E13" s="306"/>
+      <c r="E13" s="309"/>
       <c r="F13" s="131" t="s">
         <v>1011</v>
       </c>
@@ -14808,7 +14871,7 @@
         <v>1037</v>
       </c>
       <c r="H13" s="125"/>
-      <c r="I13" s="306"/>
+      <c r="I13" s="309"/>
       <c r="J13" s="131" t="s">
         <v>1099</v>
       </c>
@@ -14818,7 +14881,7 @@
       <c r="L13" s="122"/>
     </row>
     <row r="14" spans="1:12" ht="18.75">
-      <c r="A14" s="303"/>
+      <c r="A14" s="318"/>
       <c r="B14" s="131" t="s">
         <v>663</v>
       </c>
@@ -14826,7 +14889,7 @@
         <v>715</v>
       </c>
       <c r="D14" s="253"/>
-      <c r="E14" s="306"/>
+      <c r="E14" s="309"/>
       <c r="F14" s="131" t="s">
         <v>1012</v>
       </c>
@@ -14834,7 +14897,7 @@
         <v>1038</v>
       </c>
       <c r="H14" s="125"/>
-      <c r="I14" s="306"/>
+      <c r="I14" s="309"/>
       <c r="J14" s="131" t="s">
         <v>1100</v>
       </c>
@@ -14844,7 +14907,7 @@
       <c r="L14" s="122"/>
     </row>
     <row r="15" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A15" s="304"/>
+      <c r="A15" s="319"/>
       <c r="B15" s="135" t="s">
         <v>664</v>
       </c>
@@ -14852,7 +14915,7 @@
         <v>716</v>
       </c>
       <c r="D15" s="253"/>
-      <c r="E15" s="307"/>
+      <c r="E15" s="310"/>
       <c r="F15" s="135" t="s">
         <v>1013</v>
       </c>
@@ -14860,7 +14923,7 @@
         <v>1039</v>
       </c>
       <c r="H15" s="125"/>
-      <c r="I15" s="307"/>
+      <c r="I15" s="310"/>
       <c r="J15" s="135" t="s">
         <v>1101</v>
       </c>
@@ -14870,7 +14933,7 @@
       <c r="L15" s="122"/>
     </row>
     <row r="16" spans="1:12" ht="18.75">
-      <c r="A16" s="302" t="s">
+      <c r="A16" s="317" t="s">
         <v>666</v>
       </c>
       <c r="B16" s="132" t="s">
@@ -14880,7 +14943,7 @@
         <v>717</v>
       </c>
       <c r="D16" s="253"/>
-      <c r="E16" s="305" t="s">
+      <c r="E16" s="308" t="s">
         <v>972</v>
       </c>
       <c r="F16" s="132" t="s">
@@ -14890,7 +14953,7 @@
         <v>1040</v>
       </c>
       <c r="H16" s="125"/>
-      <c r="I16" s="305" t="s">
+      <c r="I16" s="308" t="s">
         <v>1060</v>
       </c>
       <c r="J16" s="132" t="s">
@@ -14902,7 +14965,7 @@
       <c r="L16" s="122"/>
     </row>
     <row r="17" spans="1:12" ht="18.75">
-      <c r="A17" s="303"/>
+      <c r="A17" s="318"/>
       <c r="B17" s="131" t="s">
         <v>669</v>
       </c>
@@ -14910,7 +14973,7 @@
         <v>718</v>
       </c>
       <c r="D17" s="253"/>
-      <c r="E17" s="306"/>
+      <c r="E17" s="309"/>
       <c r="F17" s="131" t="s">
         <v>1015</v>
       </c>
@@ -14918,7 +14981,7 @@
         <v>1041</v>
       </c>
       <c r="H17" s="125"/>
-      <c r="I17" s="306"/>
+      <c r="I17" s="309"/>
       <c r="J17" s="131" t="s">
         <v>1103</v>
       </c>
@@ -14928,7 +14991,7 @@
       <c r="L17" s="122"/>
     </row>
     <row r="18" spans="1:12" ht="18.75">
-      <c r="A18" s="303"/>
+      <c r="A18" s="318"/>
       <c r="B18" s="131" t="s">
         <v>670</v>
       </c>
@@ -14936,7 +14999,7 @@
         <v>719</v>
       </c>
       <c r="D18" s="253"/>
-      <c r="E18" s="306"/>
+      <c r="E18" s="309"/>
       <c r="F18" s="131" t="s">
         <v>1016</v>
       </c>
@@ -14944,7 +15007,7 @@
         <v>1042</v>
       </c>
       <c r="H18" s="125"/>
-      <c r="I18" s="306"/>
+      <c r="I18" s="309"/>
       <c r="J18" s="131" t="s">
         <v>1104</v>
       </c>
@@ -14954,7 +15017,7 @@
       <c r="L18" s="122"/>
     </row>
     <row r="19" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A19" s="304"/>
+      <c r="A19" s="319"/>
       <c r="B19" s="135" t="s">
         <v>671</v>
       </c>
@@ -14962,7 +15025,7 @@
         <v>720</v>
       </c>
       <c r="D19" s="253"/>
-      <c r="E19" s="307"/>
+      <c r="E19" s="310"/>
       <c r="F19" s="135" t="s">
         <v>1017</v>
       </c>
@@ -14970,7 +15033,7 @@
         <v>1043</v>
       </c>
       <c r="H19" s="125"/>
-      <c r="I19" s="307"/>
+      <c r="I19" s="310"/>
       <c r="J19" s="135" t="s">
         <v>1105</v>
       </c>
@@ -14984,7 +15047,7 @@
       <c r="B20" s="125"/>
       <c r="C20" s="125"/>
       <c r="D20" s="125"/>
-      <c r="E20" s="305" t="s">
+      <c r="E20" s="308" t="s">
         <v>560</v>
       </c>
       <c r="F20" s="132" t="s">
@@ -14994,7 +15057,7 @@
         <v>1044</v>
       </c>
       <c r="H20" s="125"/>
-      <c r="I20" s="305" t="s">
+      <c r="I20" s="308" t="s">
         <v>1061</v>
       </c>
       <c r="J20" s="132" t="s">
@@ -15010,7 +15073,7 @@
       <c r="B21" s="125"/>
       <c r="C21" s="125"/>
       <c r="D21" s="125"/>
-      <c r="E21" s="306"/>
+      <c r="E21" s="309"/>
       <c r="F21" s="131" t="s">
         <v>1019</v>
       </c>
@@ -15018,7 +15081,7 @@
         <v>1045</v>
       </c>
       <c r="H21" s="125"/>
-      <c r="I21" s="306"/>
+      <c r="I21" s="309"/>
       <c r="J21" s="131" t="s">
         <v>1107</v>
       </c>
@@ -15032,7 +15095,7 @@
       <c r="B22" s="125"/>
       <c r="C22" s="125"/>
       <c r="D22" s="125"/>
-      <c r="E22" s="306"/>
+      <c r="E22" s="309"/>
       <c r="F22" s="131" t="s">
         <v>1020</v>
       </c>
@@ -15040,7 +15103,7 @@
         <v>1046</v>
       </c>
       <c r="H22" s="125"/>
-      <c r="I22" s="306"/>
+      <c r="I22" s="309"/>
       <c r="J22" s="131" t="s">
         <v>1108</v>
       </c>
@@ -15056,7 +15119,7 @@
       <c r="B23" s="256"/>
       <c r="C23" s="257"/>
       <c r="D23" s="125"/>
-      <c r="E23" s="307"/>
+      <c r="E23" s="310"/>
       <c r="F23" s="135" t="s">
         <v>1021</v>
       </c>
@@ -15064,7 +15127,7 @@
         <v>1047</v>
       </c>
       <c r="H23" s="125"/>
-      <c r="I23" s="307"/>
+      <c r="I23" s="310"/>
       <c r="J23" s="135" t="s">
         <v>1109</v>
       </c>
@@ -15084,7 +15147,7 @@
         <v>321</v>
       </c>
       <c r="D24" s="125"/>
-      <c r="E24" s="305" t="s">
+      <c r="E24" s="308" t="s">
         <v>749</v>
       </c>
       <c r="F24" s="132" t="s">
@@ -15094,7 +15157,7 @@
         <v>1048</v>
       </c>
       <c r="H24" s="125"/>
-      <c r="I24" s="305" t="s">
+      <c r="I24" s="308" t="s">
         <v>1062</v>
       </c>
       <c r="J24" s="132" t="s">
@@ -15106,7 +15169,7 @@
       <c r="L24" s="122"/>
     </row>
     <row r="25" spans="1:12" ht="18.75">
-      <c r="A25" s="317" t="s">
+      <c r="A25" s="302" t="s">
         <v>493</v>
       </c>
       <c r="B25" s="132" t="s">
@@ -15116,7 +15179,7 @@
         <v>721</v>
       </c>
       <c r="D25" s="125"/>
-      <c r="E25" s="306"/>
+      <c r="E25" s="309"/>
       <c r="F25" s="131" t="s">
         <v>1023</v>
       </c>
@@ -15124,7 +15187,7 @@
         <v>1049</v>
       </c>
       <c r="H25" s="125"/>
-      <c r="I25" s="306"/>
+      <c r="I25" s="309"/>
       <c r="J25" s="131" t="s">
         <v>1111</v>
       </c>
@@ -15134,7 +15197,7 @@
       <c r="L25" s="122"/>
     </row>
     <row r="26" spans="1:12" ht="18.75">
-      <c r="A26" s="318"/>
+      <c r="A26" s="303"/>
       <c r="B26" s="131" t="s">
         <v>679</v>
       </c>
@@ -15142,7 +15205,7 @@
         <v>722</v>
       </c>
       <c r="D26" s="125"/>
-      <c r="E26" s="306"/>
+      <c r="E26" s="309"/>
       <c r="F26" s="131" t="s">
         <v>1024</v>
       </c>
@@ -15150,7 +15213,7 @@
         <v>1050</v>
       </c>
       <c r="H26" s="125"/>
-      <c r="I26" s="306"/>
+      <c r="I26" s="309"/>
       <c r="J26" s="131" t="s">
         <v>1112</v>
       </c>
@@ -15160,7 +15223,7 @@
       <c r="L26" s="122"/>
     </row>
     <row r="27" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A27" s="318"/>
+      <c r="A27" s="303"/>
       <c r="B27" s="131" t="s">
         <v>680</v>
       </c>
@@ -15168,7 +15231,7 @@
         <v>723</v>
       </c>
       <c r="D27" s="125"/>
-      <c r="E27" s="307"/>
+      <c r="E27" s="310"/>
       <c r="F27" s="135" t="s">
         <v>1025</v>
       </c>
@@ -15176,7 +15239,7 @@
         <v>1051</v>
       </c>
       <c r="H27" s="125"/>
-      <c r="I27" s="307"/>
+      <c r="I27" s="310"/>
       <c r="J27" s="135" t="s">
         <v>1113</v>
       </c>
@@ -15186,7 +15249,7 @@
       <c r="L27" s="122"/>
     </row>
     <row r="28" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A28" s="319"/>
+      <c r="A28" s="304"/>
       <c r="B28" s="135" t="s">
         <v>681</v>
       </c>
@@ -15194,7 +15257,7 @@
         <v>724</v>
       </c>
       <c r="D28" s="125"/>
-      <c r="E28" s="305" t="s">
+      <c r="E28" s="308" t="s">
         <v>562</v>
       </c>
       <c r="F28" s="132" t="s">
@@ -15204,7 +15267,7 @@
         <v>1052</v>
       </c>
       <c r="H28" s="125"/>
-      <c r="I28" s="305" t="s">
+      <c r="I28" s="308" t="s">
         <v>1063</v>
       </c>
       <c r="J28" s="132" t="s">
@@ -15216,7 +15279,7 @@
       <c r="L28" s="122"/>
     </row>
     <row r="29" spans="1:12" ht="18.75">
-      <c r="A29" s="317" t="s">
+      <c r="A29" s="302" t="s">
         <v>687</v>
       </c>
       <c r="B29" s="132" t="s">
@@ -15226,7 +15289,7 @@
         <v>725</v>
       </c>
       <c r="D29" s="253"/>
-      <c r="E29" s="306"/>
+      <c r="E29" s="309"/>
       <c r="F29" s="131" t="s">
         <v>1027</v>
       </c>
@@ -15234,7 +15297,7 @@
         <v>1053</v>
       </c>
       <c r="H29" s="125"/>
-      <c r="I29" s="306"/>
+      <c r="I29" s="309"/>
       <c r="J29" s="131" t="s">
         <v>1115</v>
       </c>
@@ -15244,7 +15307,7 @@
       <c r="L29" s="122"/>
     </row>
     <row r="30" spans="1:12" ht="18.75">
-      <c r="A30" s="318"/>
+      <c r="A30" s="303"/>
       <c r="B30" s="131" t="s">
         <v>684</v>
       </c>
@@ -15252,11 +15315,11 @@
         <v>726</v>
       </c>
       <c r="D30" s="253"/>
-      <c r="E30" s="306"/>
+      <c r="E30" s="309"/>
       <c r="F30" s="131"/>
       <c r="G30" s="250"/>
       <c r="H30" s="125"/>
-      <c r="I30" s="306"/>
+      <c r="I30" s="309"/>
       <c r="J30" s="131" t="s">
         <v>1116</v>
       </c>
@@ -15266,7 +15329,7 @@
       <c r="L30" s="122"/>
     </row>
     <row r="31" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A31" s="318"/>
+      <c r="A31" s="303"/>
       <c r="B31" s="131" t="s">
         <v>685</v>
       </c>
@@ -15274,11 +15337,11 @@
         <v>727</v>
       </c>
       <c r="D31" s="253"/>
-      <c r="E31" s="307"/>
+      <c r="E31" s="310"/>
       <c r="F31" s="135"/>
       <c r="G31" s="251"/>
       <c r="H31" s="125"/>
-      <c r="I31" s="307"/>
+      <c r="I31" s="310"/>
       <c r="J31" s="135" t="s">
         <v>1117</v>
       </c>
@@ -15288,7 +15351,7 @@
       <c r="L31" s="122"/>
     </row>
     <row r="32" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A32" s="319"/>
+      <c r="A32" s="304"/>
       <c r="B32" s="135" t="s">
         <v>686</v>
       </c>
@@ -15306,7 +15369,7 @@
       <c r="L32" s="122"/>
     </row>
     <row r="33" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A33" s="317" t="s">
+      <c r="A33" s="302" t="s">
         <v>691</v>
       </c>
       <c r="B33" s="132" t="s">
@@ -15316,21 +15379,21 @@
         <v>729</v>
       </c>
       <c r="D33" s="253"/>
-      <c r="E33" s="314" t="s">
+      <c r="E33" s="305" t="s">
         <v>1149</v>
       </c>
-      <c r="F33" s="315"/>
-      <c r="G33" s="316"/>
+      <c r="F33" s="306"/>
+      <c r="G33" s="307"/>
       <c r="H33" s="124"/>
-      <c r="I33" s="314" t="s">
+      <c r="I33" s="305" t="s">
         <v>1148</v>
       </c>
-      <c r="J33" s="315"/>
-      <c r="K33" s="316"/>
+      <c r="J33" s="306"/>
+      <c r="K33" s="307"/>
       <c r="L33" s="122"/>
     </row>
     <row r="34" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A34" s="318"/>
+      <c r="A34" s="303"/>
       <c r="B34" s="131" t="s">
         <v>693</v>
       </c>
@@ -15360,7 +15423,7 @@
       <c r="L34" s="122"/>
     </row>
     <row r="35" spans="1:12" ht="18.75">
-      <c r="A35" s="318"/>
+      <c r="A35" s="303"/>
       <c r="B35" s="131" t="s">
         <v>694</v>
       </c>
@@ -15368,7 +15431,7 @@
         <v>731</v>
       </c>
       <c r="D35" s="253"/>
-      <c r="E35" s="317" t="s">
+      <c r="E35" s="302" t="s">
         <v>494</v>
       </c>
       <c r="F35" s="132" t="s">
@@ -15378,7 +15441,7 @@
         <v>11311</v>
       </c>
       <c r="H35" s="124"/>
-      <c r="I35" s="317" t="s">
+      <c r="I35" s="302" t="s">
         <v>955</v>
       </c>
       <c r="J35" s="132" t="s">
@@ -15390,7 +15453,7 @@
       <c r="L35" s="122"/>
     </row>
     <row r="36" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A36" s="319"/>
+      <c r="A36" s="304"/>
       <c r="B36" s="135" t="s">
         <v>695</v>
       </c>
@@ -15398,7 +15461,7 @@
         <v>732</v>
       </c>
       <c r="D36" s="253"/>
-      <c r="E36" s="318"/>
+      <c r="E36" s="303"/>
       <c r="F36" s="131" t="s">
         <v>958</v>
       </c>
@@ -15406,7 +15469,7 @@
         <v>11312</v>
       </c>
       <c r="H36" s="124"/>
-      <c r="I36" s="318"/>
+      <c r="I36" s="303"/>
       <c r="J36" s="131" t="s">
         <v>965</v>
       </c>
@@ -15416,7 +15479,7 @@
       <c r="L36" s="122"/>
     </row>
     <row r="37" spans="1:12" ht="18.75">
-      <c r="A37" s="317" t="s">
+      <c r="A37" s="302" t="s">
         <v>698</v>
       </c>
       <c r="B37" s="132" t="s">
@@ -15426,7 +15489,7 @@
         <v>11441</v>
       </c>
       <c r="D37" s="253"/>
-      <c r="E37" s="318"/>
+      <c r="E37" s="303"/>
       <c r="F37" s="131" t="s">
         <v>959</v>
       </c>
@@ -15434,7 +15497,7 @@
         <v>11313</v>
       </c>
       <c r="H37" s="124"/>
-      <c r="I37" s="318"/>
+      <c r="I37" s="303"/>
       <c r="J37" s="131" t="s">
         <v>966</v>
       </c>
@@ -15444,7 +15507,7 @@
       <c r="L37" s="122"/>
     </row>
     <row r="38" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A38" s="318"/>
+      <c r="A38" s="303"/>
       <c r="B38" s="131" t="s">
         <v>700</v>
       </c>
@@ -15452,7 +15515,7 @@
         <v>11442</v>
       </c>
       <c r="D38" s="253"/>
-      <c r="E38" s="319"/>
+      <c r="E38" s="304"/>
       <c r="F38" s="135" t="s">
         <v>959</v>
       </c>
@@ -15460,7 +15523,7 @@
         <v>11314</v>
       </c>
       <c r="H38" s="124"/>
-      <c r="I38" s="319"/>
+      <c r="I38" s="304"/>
       <c r="J38" s="135" t="s">
         <v>967</v>
       </c>
@@ -15470,7 +15533,7 @@
       <c r="L38" s="122"/>
     </row>
     <row r="39" spans="1:12" ht="18.75">
-      <c r="A39" s="318"/>
+      <c r="A39" s="303"/>
       <c r="B39" s="131" t="s">
         <v>701</v>
       </c>
@@ -15478,7 +15541,7 @@
         <v>11443</v>
       </c>
       <c r="D39" s="253"/>
-      <c r="E39" s="317" t="s">
+      <c r="E39" s="302" t="s">
         <v>954</v>
       </c>
       <c r="F39" s="132" t="s">
@@ -15488,7 +15551,7 @@
         <v>11321</v>
       </c>
       <c r="H39" s="124"/>
-      <c r="I39" s="317" t="s">
+      <c r="I39" s="302" t="s">
         <v>956</v>
       </c>
       <c r="J39" s="132" t="s">
@@ -15500,7 +15563,7 @@
       <c r="L39" s="122"/>
     </row>
     <row r="40" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A40" s="319"/>
+      <c r="A40" s="304"/>
       <c r="B40" s="135" t="s">
         <v>702</v>
       </c>
@@ -15508,7 +15571,7 @@
         <v>11444</v>
       </c>
       <c r="D40" s="253"/>
-      <c r="E40" s="318"/>
+      <c r="E40" s="303"/>
       <c r="F40" s="131" t="s">
         <v>961</v>
       </c>
@@ -15516,7 +15579,7 @@
         <v>11322</v>
       </c>
       <c r="H40" s="124"/>
-      <c r="I40" s="318"/>
+      <c r="I40" s="303"/>
       <c r="J40" s="131" t="s">
         <v>969</v>
       </c>
@@ -15530,7 +15593,7 @@
       <c r="B41" s="125"/>
       <c r="C41" s="253"/>
       <c r="D41" s="253"/>
-      <c r="E41" s="318"/>
+      <c r="E41" s="303"/>
       <c r="F41" s="131" t="s">
         <v>962</v>
       </c>
@@ -15538,7 +15601,7 @@
         <v>11323</v>
       </c>
       <c r="H41" s="124"/>
-      <c r="I41" s="318"/>
+      <c r="I41" s="303"/>
       <c r="J41" s="131" t="s">
         <v>970</v>
       </c>
@@ -15552,7 +15615,7 @@
       <c r="B42" s="125"/>
       <c r="C42" s="253"/>
       <c r="D42" s="253"/>
-      <c r="E42" s="319"/>
+      <c r="E42" s="304"/>
       <c r="F42" s="135" t="s">
         <v>963</v>
       </c>
@@ -15560,7 +15623,7 @@
         <v>11324</v>
       </c>
       <c r="H42" s="124"/>
-      <c r="I42" s="319"/>
+      <c r="I42" s="304"/>
       <c r="J42" s="135" t="s">
         <v>971</v>
       </c>
@@ -15613,16 +15676,18 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="I35:I38"/>
-    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A7"/>
     <mergeCell ref="I16:I19"/>
     <mergeCell ref="I12:I15"/>
     <mergeCell ref="I8:I11"/>
@@ -15633,18 +15698,16 @@
     <mergeCell ref="I28:I31"/>
     <mergeCell ref="E20:E23"/>
     <mergeCell ref="E24:E27"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="I35:I38"/>
+    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="E33:G33"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15658,7 +15721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
@@ -15675,40 +15738,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="324" t="s">
+      <c r="A1" s="320" t="s">
         <v>1151</v>
       </c>
-      <c r="B1" s="325"/>
-      <c r="C1" s="325"/>
-      <c r="D1" s="325"/>
-      <c r="E1" s="325"/>
-      <c r="F1" s="325"/>
-      <c r="G1" s="325"/>
-      <c r="H1" s="326"/>
+      <c r="B1" s="321"/>
+      <c r="C1" s="321"/>
+      <c r="D1" s="321"/>
+      <c r="E1" s="321"/>
+      <c r="F1" s="321"/>
+      <c r="G1" s="321"/>
+      <c r="H1" s="322"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="327"/>
-      <c r="B2" s="328"/>
-      <c r="C2" s="328"/>
-      <c r="D2" s="328"/>
-      <c r="E2" s="328"/>
-      <c r="F2" s="328"/>
-      <c r="G2" s="328"/>
-      <c r="H2" s="329"/>
+      <c r="A2" s="323"/>
+      <c r="B2" s="324"/>
+      <c r="C2" s="324"/>
+      <c r="D2" s="324"/>
+      <c r="E2" s="324"/>
+      <c r="F2" s="324"/>
+      <c r="G2" s="324"/>
+      <c r="H2" s="325"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="330" t="s">
+      <c r="A3" s="326" t="s">
         <v>250</v>
       </c>
-      <c r="B3" s="331"/>
-      <c r="C3" s="331"/>
-      <c r="D3" s="331"/>
-      <c r="E3" s="331" t="s">
+      <c r="B3" s="327"/>
+      <c r="C3" s="327"/>
+      <c r="D3" s="327"/>
+      <c r="E3" s="327" t="s">
         <v>251</v>
       </c>
-      <c r="F3" s="331"/>
-      <c r="G3" s="331"/>
-      <c r="H3" s="332"/>
+      <c r="F3" s="327"/>
+      <c r="G3" s="327"/>
+      <c r="H3" s="328"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="12">
@@ -16242,11 +16305,11 @@
       <c r="C27" s="118" t="s">
         <v>594</v>
       </c>
-      <c r="D27" s="323" t="s">
+      <c r="D27" s="329" t="s">
         <v>570</v>
       </c>
-      <c r="E27" s="323"/>
-      <c r="F27" s="323"/>
+      <c r="E27" s="329"/>
+      <c r="F27" s="329"/>
       <c r="G27" s="17"/>
       <c r="H27" s="18"/>
     </row>
@@ -16258,11 +16321,11 @@
       <c r="C28" s="118" t="s">
         <v>598</v>
       </c>
-      <c r="D28" s="323" t="s">
+      <c r="D28" s="329" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="323"/>
-      <c r="F28" s="323"/>
+      <c r="E28" s="329"/>
+      <c r="F28" s="329"/>
       <c r="G28" s="17"/>
       <c r="H28" s="18"/>
     </row>
@@ -16274,11 +16337,11 @@
       <c r="C29" s="118" t="s">
         <v>599</v>
       </c>
-      <c r="D29" s="323" t="s">
+      <c r="D29" s="329" t="s">
         <v>571</v>
       </c>
-      <c r="E29" s="323"/>
-      <c r="F29" s="323"/>
+      <c r="E29" s="329"/>
+      <c r="F29" s="329"/>
       <c r="G29" s="17"/>
       <c r="H29" s="18"/>
     </row>
@@ -16290,11 +16353,11 @@
       <c r="C30" s="118" t="s">
         <v>600</v>
       </c>
-      <c r="D30" s="323" t="s">
+      <c r="D30" s="329" t="s">
         <v>572</v>
       </c>
-      <c r="E30" s="323"/>
-      <c r="F30" s="323"/>
+      <c r="E30" s="329"/>
+      <c r="F30" s="329"/>
       <c r="G30" s="17"/>
       <c r="H30" s="18"/>
     </row>
@@ -16306,11 +16369,11 @@
       <c r="C31" s="118" t="s">
         <v>601</v>
       </c>
-      <c r="D31" s="323" t="s">
+      <c r="D31" s="329" t="s">
         <v>573</v>
       </c>
-      <c r="E31" s="323"/>
-      <c r="F31" s="323"/>
+      <c r="E31" s="329"/>
+      <c r="F31" s="329"/>
       <c r="G31" s="17"/>
       <c r="H31" s="18"/>
     </row>
@@ -16322,11 +16385,11 @@
       <c r="C32" s="118" t="s">
         <v>602</v>
       </c>
-      <c r="D32" s="323" t="s">
+      <c r="D32" s="329" t="s">
         <v>574</v>
       </c>
-      <c r="E32" s="323"/>
-      <c r="F32" s="323"/>
+      <c r="E32" s="329"/>
+      <c r="F32" s="329"/>
       <c r="G32" s="17"/>
       <c r="H32" s="18"/>
     </row>
@@ -16338,11 +16401,11 @@
       <c r="C33" s="118" t="s">
         <v>614</v>
       </c>
-      <c r="D33" s="323" t="s">
+      <c r="D33" s="329" t="s">
         <v>482</v>
       </c>
-      <c r="E33" s="323"/>
-      <c r="F33" s="323"/>
+      <c r="E33" s="329"/>
+      <c r="F33" s="329"/>
       <c r="G33" s="17"/>
       <c r="H33" s="18"/>
     </row>
@@ -16354,11 +16417,11 @@
       <c r="C34" s="118" t="s">
         <v>615</v>
       </c>
-      <c r="D34" s="323" t="s">
+      <c r="D34" s="329" t="s">
         <v>575</v>
       </c>
-      <c r="E34" s="323"/>
-      <c r="F34" s="323"/>
+      <c r="E34" s="329"/>
+      <c r="F34" s="329"/>
       <c r="G34" s="17"/>
       <c r="H34" s="18"/>
     </row>
@@ -16370,11 +16433,11 @@
       <c r="C35" s="118" t="s">
         <v>616</v>
       </c>
-      <c r="D35" s="323" t="s">
+      <c r="D35" s="329" t="s">
         <v>576</v>
       </c>
-      <c r="E35" s="323"/>
-      <c r="F35" s="323"/>
+      <c r="E35" s="329"/>
+      <c r="F35" s="329"/>
       <c r="G35" s="17"/>
       <c r="H35" s="18"/>
     </row>
@@ -16384,11 +16447,11 @@
       <c r="C36" s="118" t="s">
         <v>651</v>
       </c>
-      <c r="D36" s="320" t="s">
+      <c r="D36" s="330" t="s">
         <v>591</v>
       </c>
-      <c r="E36" s="321"/>
-      <c r="F36" s="322"/>
+      <c r="E36" s="331"/>
+      <c r="F36" s="332"/>
       <c r="G36" s="17"/>
       <c r="H36" s="18"/>
     </row>
@@ -16398,11 +16461,11 @@
       <c r="C37" s="118" t="s">
         <v>654</v>
       </c>
-      <c r="D37" s="320" t="s">
+      <c r="D37" s="330" t="s">
         <v>652</v>
       </c>
-      <c r="E37" s="321"/>
-      <c r="F37" s="322"/>
+      <c r="E37" s="331"/>
+      <c r="F37" s="332"/>
       <c r="G37" s="17"/>
       <c r="H37" s="18"/>
     </row>
@@ -16412,11 +16475,11 @@
       <c r="C38" s="118" t="s">
         <v>653</v>
       </c>
-      <c r="D38" s="320" t="s">
+      <c r="D38" s="330" t="s">
         <v>655</v>
       </c>
-      <c r="E38" s="321"/>
-      <c r="F38" s="322"/>
+      <c r="E38" s="331"/>
+      <c r="F38" s="332"/>
       <c r="G38" s="17"/>
       <c r="H38" s="18"/>
     </row>
@@ -16424,9 +16487,9 @@
       <c r="A39" s="16"/>
       <c r="B39" s="120"/>
       <c r="C39" s="118"/>
-      <c r="D39" s="320"/>
-      <c r="E39" s="321"/>
-      <c r="F39" s="322"/>
+      <c r="D39" s="330"/>
+      <c r="E39" s="331"/>
+      <c r="F39" s="332"/>
       <c r="G39" s="17"/>
       <c r="H39" s="18"/>
     </row>
@@ -16524,6 +16587,13 @@
     <row r="52" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:H3"/>
@@ -16533,13 +16603,6 @@
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -18302,28 +18365,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="362" t="s">
+      <c r="A1" s="374" t="s">
         <v>952</v>
       </c>
-      <c r="B1" s="363"/>
-      <c r="C1" s="363"/>
-      <c r="D1" s="363"/>
-      <c r="E1" s="363"/>
-      <c r="F1" s="364"/>
+      <c r="B1" s="375"/>
+      <c r="C1" s="375"/>
+      <c r="D1" s="375"/>
+      <c r="E1" s="375"/>
+      <c r="F1" s="376"/>
       <c r="G1" s="175"/>
       <c r="H1" s="175"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="365" t="s">
+      <c r="A2" s="377" t="s">
         <v>840</v>
       </c>
-      <c r="B2" s="366"/>
-      <c r="C2" s="367"/>
-      <c r="D2" s="365" t="s">
+      <c r="B2" s="378"/>
+      <c r="C2" s="379"/>
+      <c r="D2" s="377" t="s">
         <v>841</v>
       </c>
-      <c r="E2" s="366"/>
-      <c r="F2" s="367"/>
+      <c r="E2" s="378"/>
+      <c r="F2" s="379"/>
       <c r="G2" s="175"/>
       <c r="H2" s="175"/>
     </row>
@@ -18347,7 +18410,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="175"/>
-      <c r="H3" s="368" t="s">
+      <c r="H3" s="371" t="s">
         <v>844</v>
       </c>
     </row>
@@ -18371,7 +18434,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="175"/>
-      <c r="H4" s="369"/>
+      <c r="H4" s="372"/>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A5" s="176">
@@ -18393,7 +18456,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="175"/>
-      <c r="H5" s="369"/>
+      <c r="H5" s="372"/>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A6" s="179">
@@ -18415,7 +18478,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="175"/>
-      <c r="H6" s="369"/>
+      <c r="H6" s="372"/>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A7" s="179">
@@ -18437,7 +18500,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="175"/>
-      <c r="H7" s="369"/>
+      <c r="H7" s="372"/>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A8" s="182">
@@ -18459,7 +18522,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="175"/>
-      <c r="H8" s="369"/>
+      <c r="H8" s="372"/>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A9" s="182">
@@ -18481,7 +18544,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="175"/>
-      <c r="H9" s="369"/>
+      <c r="H9" s="372"/>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A10" s="185">
@@ -18503,7 +18566,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="175"/>
-      <c r="H10" s="370"/>
+      <c r="H10" s="373"/>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="188">
@@ -18525,7 +18588,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="175"/>
-      <c r="H11" s="371" t="s">
+      <c r="H11" s="362" t="s">
         <v>856</v>
       </c>
     </row>
@@ -18549,7 +18612,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="175"/>
-      <c r="H12" s="372"/>
+      <c r="H12" s="363"/>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A13" s="191">
@@ -18571,7 +18634,7 @@
         <v>11</v>
       </c>
       <c r="G13" s="175"/>
-      <c r="H13" s="372"/>
+      <c r="H13" s="363"/>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A14" s="191">
@@ -18593,7 +18656,7 @@
         <v>12</v>
       </c>
       <c r="G14" s="175"/>
-      <c r="H14" s="372"/>
+      <c r="H14" s="363"/>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A15" s="195">
@@ -18615,7 +18678,7 @@
         <v>13</v>
       </c>
       <c r="G15" s="175"/>
-      <c r="H15" s="372"/>
+      <c r="H15" s="363"/>
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A16" s="195">
@@ -18637,7 +18700,7 @@
         <v>14</v>
       </c>
       <c r="G16" s="175"/>
-      <c r="H16" s="372"/>
+      <c r="H16" s="363"/>
     </row>
     <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A17" s="195">
@@ -18659,7 +18722,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="175"/>
-      <c r="H17" s="372"/>
+      <c r="H17" s="363"/>
     </row>
     <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A18" s="195">
@@ -18681,7 +18744,7 @@
         <v>16</v>
       </c>
       <c r="G18" s="175"/>
-      <c r="H18" s="372"/>
+      <c r="H18" s="363"/>
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A19" s="195">
@@ -18703,7 +18766,7 @@
         <v>17</v>
       </c>
       <c r="G19" s="175"/>
-      <c r="H19" s="372"/>
+      <c r="H19" s="363"/>
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A20" s="198">
@@ -18725,7 +18788,7 @@
         <v>18</v>
       </c>
       <c r="G20" s="175"/>
-      <c r="H20" s="372"/>
+      <c r="H20" s="363"/>
     </row>
     <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A21" s="198">
@@ -18747,7 +18810,7 @@
         <v>19</v>
       </c>
       <c r="G21" s="175"/>
-      <c r="H21" s="372"/>
+      <c r="H21" s="363"/>
     </row>
     <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A22" s="201">
@@ -18769,7 +18832,7 @@
         <v>20</v>
       </c>
       <c r="G22" s="175"/>
-      <c r="H22" s="373"/>
+      <c r="H22" s="364"/>
     </row>
     <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1"/>
@@ -18787,28 +18850,28 @@
     <row r="36" spans="1:8" ht="20.100000000000001" customHeight="1"/>
     <row r="37" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1"/>
     <row r="38" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A38" s="374" t="s">
+      <c r="A38" s="365" t="s">
         <v>953</v>
       </c>
-      <c r="B38" s="375"/>
-      <c r="C38" s="375"/>
-      <c r="D38" s="375"/>
-      <c r="E38" s="375"/>
-      <c r="F38" s="376"/>
+      <c r="B38" s="366"/>
+      <c r="C38" s="366"/>
+      <c r="D38" s="366"/>
+      <c r="E38" s="366"/>
+      <c r="F38" s="367"/>
       <c r="G38" s="175"/>
       <c r="H38" s="175"/>
     </row>
     <row r="39" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A39" s="377" t="s">
+      <c r="A39" s="368" t="s">
         <v>840</v>
       </c>
-      <c r="B39" s="378"/>
-      <c r="C39" s="379"/>
-      <c r="D39" s="377" t="s">
+      <c r="B39" s="369"/>
+      <c r="C39" s="370"/>
+      <c r="D39" s="368" t="s">
         <v>841</v>
       </c>
-      <c r="E39" s="378"/>
-      <c r="F39" s="379"/>
+      <c r="E39" s="369"/>
+      <c r="F39" s="370"/>
       <c r="G39" s="175"/>
       <c r="H39" s="175"/>
     </row>
@@ -18832,7 +18895,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="175"/>
-      <c r="H40" s="368" t="s">
+      <c r="H40" s="371" t="s">
         <v>844</v>
       </c>
     </row>
@@ -18856,7 +18919,7 @@
         <v>2</v>
       </c>
       <c r="G41" s="175"/>
-      <c r="H41" s="369"/>
+      <c r="H41" s="372"/>
     </row>
     <row r="42" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A42" s="204">
@@ -18878,7 +18941,7 @@
         <v>3</v>
       </c>
       <c r="G42" s="175"/>
-      <c r="H42" s="369"/>
+      <c r="H42" s="372"/>
     </row>
     <row r="43" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A43" s="206">
@@ -18900,7 +18963,7 @@
         <v>4</v>
       </c>
       <c r="G43" s="175"/>
-      <c r="H43" s="369"/>
+      <c r="H43" s="372"/>
     </row>
     <row r="44" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A44" s="206">
@@ -18922,7 +18985,7 @@
         <v>5</v>
       </c>
       <c r="G44" s="175"/>
-      <c r="H44" s="369"/>
+      <c r="H44" s="372"/>
     </row>
     <row r="45" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A45" s="208">
@@ -18944,7 +19007,7 @@
         <v>6</v>
       </c>
       <c r="G45" s="175"/>
-      <c r="H45" s="369"/>
+      <c r="H45" s="372"/>
     </row>
     <row r="46" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A46" s="208">
@@ -18966,7 +19029,7 @@
         <v>7</v>
       </c>
       <c r="G46" s="175"/>
-      <c r="H46" s="369"/>
+      <c r="H46" s="372"/>
     </row>
     <row r="47" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A47" s="210">
@@ -18988,7 +19051,7 @@
         <v>8</v>
       </c>
       <c r="G47" s="175"/>
-      <c r="H47" s="370"/>
+      <c r="H47" s="373"/>
     </row>
     <row r="48" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="A48" s="213">
@@ -19010,7 +19073,7 @@
         <v>9</v>
       </c>
       <c r="G48" s="175"/>
-      <c r="H48" s="371" t="s">
+      <c r="H48" s="362" t="s">
         <v>856</v>
       </c>
     </row>
@@ -19034,7 +19097,7 @@
         <v>10</v>
       </c>
       <c r="G49" s="175"/>
-      <c r="H49" s="372"/>
+      <c r="H49" s="363"/>
     </row>
     <row r="50" spans="1:8" ht="16.5" thickBot="1">
       <c r="A50" s="215">
@@ -19056,7 +19119,7 @@
         <v>11</v>
       </c>
       <c r="G50" s="175"/>
-      <c r="H50" s="372"/>
+      <c r="H50" s="363"/>
     </row>
     <row r="51" spans="1:8" ht="16.5" thickBot="1">
       <c r="A51" s="218">
@@ -19078,7 +19141,7 @@
         <v>12</v>
       </c>
       <c r="G51" s="175"/>
-      <c r="H51" s="372"/>
+      <c r="H51" s="363"/>
     </row>
     <row r="52" spans="1:8" ht="16.5" thickBot="1">
       <c r="A52" s="218">
@@ -19100,7 +19163,7 @@
         <v>13</v>
       </c>
       <c r="G52" s="175"/>
-      <c r="H52" s="372"/>
+      <c r="H52" s="363"/>
     </row>
     <row r="53" spans="1:8" ht="16.5" thickBot="1">
       <c r="A53" s="218">
@@ -19122,7 +19185,7 @@
         <v>14</v>
       </c>
       <c r="G53" s="175"/>
-      <c r="H53" s="372"/>
+      <c r="H53" s="363"/>
     </row>
     <row r="54" spans="1:8" ht="16.5" thickBot="1">
       <c r="A54" s="218">
@@ -19144,7 +19207,7 @@
         <v>15</v>
       </c>
       <c r="G54" s="175"/>
-      <c r="H54" s="372"/>
+      <c r="H54" s="363"/>
     </row>
     <row r="55" spans="1:8" ht="16.5" thickBot="1">
       <c r="A55" s="218">
@@ -19166,7 +19229,7 @@
         <v>16</v>
       </c>
       <c r="G55" s="175"/>
-      <c r="H55" s="372"/>
+      <c r="H55" s="363"/>
     </row>
     <row r="56" spans="1:8" ht="16.5" thickBot="1">
       <c r="A56" s="218">
@@ -19188,7 +19251,7 @@
         <v>17</v>
       </c>
       <c r="G56" s="175"/>
-      <c r="H56" s="372"/>
+      <c r="H56" s="363"/>
     </row>
     <row r="57" spans="1:8" ht="16.5" thickBot="1">
       <c r="A57" s="220">
@@ -19210,7 +19273,7 @@
         <v>18</v>
       </c>
       <c r="G57" s="175"/>
-      <c r="H57" s="372"/>
+      <c r="H57" s="363"/>
     </row>
     <row r="58" spans="1:8" ht="16.5" thickBot="1">
       <c r="A58" s="220">
@@ -19232,7 +19295,7 @@
         <v>19</v>
       </c>
       <c r="G58" s="175"/>
-      <c r="H58" s="372"/>
+      <c r="H58" s="363"/>
     </row>
     <row r="59" spans="1:8" ht="16.5" thickBot="1">
       <c r="A59" s="222">
@@ -19254,21 +19317,21 @@
         <v>20</v>
       </c>
       <c r="G59" s="175"/>
-      <c r="H59" s="373"/>
+      <c r="H59" s="364"/>
     </row>
     <row r="60" spans="1:8" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="H3:H10"/>
+    <mergeCell ref="H11:H22"/>
     <mergeCell ref="H48:H59"/>
     <mergeCell ref="A38:F38"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="D39:F39"/>
     <mergeCell ref="H40:H47"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="H3:H10"/>
-    <mergeCell ref="H11:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -19835,40 +19898,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="324" t="s">
+      <c r="A1" s="320" t="s">
         <v>488</v>
       </c>
-      <c r="B1" s="325"/>
-      <c r="C1" s="325"/>
-      <c r="D1" s="325"/>
-      <c r="E1" s="325"/>
-      <c r="F1" s="325"/>
-      <c r="G1" s="325"/>
-      <c r="H1" s="326"/>
+      <c r="B1" s="321"/>
+      <c r="C1" s="321"/>
+      <c r="D1" s="321"/>
+      <c r="E1" s="321"/>
+      <c r="F1" s="321"/>
+      <c r="G1" s="321"/>
+      <c r="H1" s="322"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="327"/>
-      <c r="B2" s="328"/>
-      <c r="C2" s="328"/>
-      <c r="D2" s="328"/>
-      <c r="E2" s="328"/>
-      <c r="F2" s="328"/>
-      <c r="G2" s="328"/>
-      <c r="H2" s="329"/>
+      <c r="A2" s="323"/>
+      <c r="B2" s="324"/>
+      <c r="C2" s="324"/>
+      <c r="D2" s="324"/>
+      <c r="E2" s="324"/>
+      <c r="F2" s="324"/>
+      <c r="G2" s="324"/>
+      <c r="H2" s="325"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="330" t="s">
+      <c r="A3" s="326" t="s">
         <v>319</v>
       </c>
-      <c r="B3" s="331"/>
-      <c r="C3" s="331"/>
-      <c r="D3" s="331"/>
-      <c r="E3" s="331" t="s">
+      <c r="B3" s="327"/>
+      <c r="C3" s="327"/>
+      <c r="D3" s="327"/>
+      <c r="E3" s="327" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="331"/>
-      <c r="G3" s="331"/>
-      <c r="H3" s="332"/>
+      <c r="F3" s="327"/>
+      <c r="G3" s="327"/>
+      <c r="H3" s="328"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="12">

</xml_diff>

<commit_message>
chg: Added red focus 3 to comms masterfile and combatflite file
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2249" uniqueCount="1344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="1347">
   <si>
     <t>AWACS</t>
   </si>
@@ -4056,6 +4056,15 @@
   </si>
   <si>
     <t>GOLD 12</t>
+  </si>
+  <si>
+    <t>FOCUS 3 (AI)</t>
+  </si>
+  <si>
+    <t>284.77</t>
+  </si>
+  <si>
+    <t>#IFF:5605FR</t>
   </si>
 </sst>
 </file>
@@ -6709,9 +6718,21 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6721,16 +6742,49 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6742,50 +6796,17 @@
     <xf numFmtId="0" fontId="24" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6814,18 +6835,6 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6913,6 +6922,33 @@
     <xf numFmtId="49" fontId="45" fillId="31" borderId="93" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="26" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6940,33 +6976,6 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7039,6 +7048,57 @@
     <xf numFmtId="0" fontId="32" fillId="20" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7056,57 +7116,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7421,7 +7430,7 @@
   <dimension ref="A1:AP83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AL41" sqref="AL41"/>
+      <selection activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -7528,13 +7537,13 @@
       <c r="N2" s="107" t="s">
         <v>330</v>
       </c>
-      <c r="V2" s="294" t="s">
+      <c r="V2" s="295" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="294"/>
-      <c r="X2" s="294"/>
-      <c r="Y2" s="294"/>
-      <c r="Z2" s="294"/>
+      <c r="W2" s="295"/>
+      <c r="X2" s="295"/>
+      <c r="Y2" s="295"/>
+      <c r="Z2" s="295"/>
     </row>
     <row r="3" spans="1:42">
       <c r="A3" s="107" t="s">
@@ -7583,9 +7592,9 @@
       <c r="P3" t="s">
         <v>426</v>
       </c>
-      <c r="R3" s="298"/>
-      <c r="S3" s="298"/>
-      <c r="T3" s="298"/>
+      <c r="R3" s="294"/>
+      <c r="S3" s="294"/>
+      <c r="T3" s="294"/>
       <c r="V3" s="101" t="s">
         <v>328</v>
       </c>
@@ -7667,22 +7676,22 @@
       <c r="AA4" s="23"/>
       <c r="AB4" s="23"/>
       <c r="AC4" s="23"/>
-      <c r="AD4" s="294" t="s">
+      <c r="AD4" s="295" t="s">
         <v>429</v>
       </c>
-      <c r="AE4" s="294"/>
-      <c r="AF4" s="294"/>
-      <c r="AG4" s="294"/>
-      <c r="AH4" s="294"/>
-      <c r="AJ4" s="294" t="s">
+      <c r="AE4" s="295"/>
+      <c r="AF4" s="295"/>
+      <c r="AG4" s="295"/>
+      <c r="AH4" s="295"/>
+      <c r="AJ4" s="295" t="s">
         <v>1</v>
       </c>
-      <c r="AK4" s="294"/>
-      <c r="AL4" s="294"/>
-      <c r="AM4" s="294"/>
-      <c r="AN4" s="294"/>
-      <c r="AO4" s="294"/>
-      <c r="AP4" s="294"/>
+      <c r="AK4" s="295"/>
+      <c r="AL4" s="295"/>
+      <c r="AM4" s="295"/>
+      <c r="AN4" s="295"/>
+      <c r="AO4" s="295"/>
+      <c r="AP4" s="295"/>
     </row>
     <row r="5" spans="1:42" ht="15.75">
       <c r="A5" s="107" t="s">
@@ -8642,18 +8651,18 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="100"/>
       <c r="S15" s="99"/>
-      <c r="V15" s="271" t="s">
-        <v>1248</v>
+      <c r="V15" s="116" t="s">
+        <v>1232</v>
       </c>
       <c r="W15" s="3" t="s">
-        <v>1249</v>
+        <v>1236</v>
       </c>
       <c r="X15" s="3"/>
       <c r="Y15" s="3" t="s">
-        <v>1250</v>
+        <v>1234</v>
       </c>
       <c r="Z15" s="3">
-        <v>611</v>
+        <v>601</v>
       </c>
       <c r="AD15" s="3" t="s">
         <v>437</v>
@@ -8739,18 +8748,18 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="100"/>
       <c r="S16" s="99"/>
-      <c r="V16" s="271" t="s">
-        <v>282</v>
-      </c>
-      <c r="W16" s="3" t="s">
-        <v>1251</v>
-      </c>
-      <c r="X16" s="3"/>
+      <c r="V16" s="116" t="s">
+        <v>1245</v>
+      </c>
+      <c r="W16" s="9" t="s">
+        <v>1244</v>
+      </c>
+      <c r="X16" s="9"/>
       <c r="Y16" s="3" t="s">
-        <v>1252</v>
-      </c>
-      <c r="Z16" s="3">
-        <v>612</v>
+        <v>1246</v>
+      </c>
+      <c r="Z16" s="270">
+        <v>604</v>
       </c>
       <c r="AD16" s="3" t="s">
         <v>438</v>
@@ -8815,17 +8824,17 @@
       <c r="Q17" s="2"/>
       <c r="S17" s="99"/>
       <c r="V17" s="116" t="s">
-        <v>1232</v>
-      </c>
-      <c r="W17" s="3" t="s">
-        <v>1236</v>
-      </c>
-      <c r="X17" s="3"/>
+        <v>1344</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>1345</v>
+      </c>
+      <c r="X17" s="9"/>
       <c r="Y17" s="3" t="s">
-        <v>1234</v>
-      </c>
-      <c r="Z17" s="3">
-        <v>601</v>
+        <v>1346</v>
+      </c>
+      <c r="Z17" s="270">
+        <v>605</v>
       </c>
       <c r="AD17" s="3" t="s">
         <v>439</v>
@@ -8892,17 +8901,17 @@
       <c r="S18" s="99"/>
       <c r="T18" s="24"/>
       <c r="V18" s="271" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="W18" s="3" t="s">
-        <v>1242</v>
+        <v>1249</v>
       </c>
       <c r="X18" s="3"/>
       <c r="Y18" s="3" t="s">
-        <v>1240</v>
+        <v>1250</v>
       </c>
       <c r="Z18" s="3">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="AD18" s="3" t="s">
         <v>440</v>
@@ -8919,15 +8928,15 @@
       <c r="AH18" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="AJ18" s="294" t="s">
+      <c r="AJ18" s="295" t="s">
         <v>274</v>
       </c>
-      <c r="AK18" s="294"/>
-      <c r="AL18" s="294"/>
-      <c r="AM18" s="294"/>
-      <c r="AN18" s="294"/>
-      <c r="AO18" s="294"/>
-      <c r="AP18" s="294"/>
+      <c r="AK18" s="295"/>
+      <c r="AL18" s="295"/>
+      <c r="AM18" s="295"/>
+      <c r="AN18" s="295"/>
+      <c r="AO18" s="295"/>
+      <c r="AP18" s="295"/>
     </row>
     <row r="19" spans="1:42" ht="15.75">
       <c r="A19" s="107" t="s">
@@ -8977,18 +8986,18 @@
       <c r="R19" s="23"/>
       <c r="S19" s="99"/>
       <c r="T19" s="23"/>
-      <c r="V19" s="116" t="s">
-        <v>1245</v>
-      </c>
-      <c r="W19" s="9" t="s">
-        <v>1244</v>
-      </c>
-      <c r="X19" s="9"/>
+      <c r="V19" s="271" t="s">
+        <v>282</v>
+      </c>
+      <c r="W19" s="3" t="s">
+        <v>1251</v>
+      </c>
+      <c r="X19" s="3"/>
       <c r="Y19" s="3" t="s">
-        <v>1246</v>
-      </c>
-      <c r="Z19" s="270">
-        <v>604</v>
+        <v>1252</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>612</v>
       </c>
       <c r="AD19" s="30"/>
       <c r="AE19" s="102"/>
@@ -9060,9 +9069,9 @@
       </c>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="298"/>
-      <c r="S20" s="298"/>
-      <c r="T20" s="298"/>
+      <c r="R20" s="294"/>
+      <c r="S20" s="294"/>
+      <c r="T20" s="294"/>
       <c r="U20" s="2"/>
       <c r="V20" s="272" t="s">
         <v>1253</v>
@@ -9162,10 +9171,19 @@
       <c r="R21" s="23"/>
       <c r="S21" s="23"/>
       <c r="T21" s="23"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
-      <c r="X21" s="2"/>
-      <c r="Y21" s="2"/>
+      <c r="V21" s="271" t="s">
+        <v>1247</v>
+      </c>
+      <c r="W21" s="3" t="s">
+        <v>1242</v>
+      </c>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>603</v>
+      </c>
       <c r="AD21" s="3" t="s">
         <v>442</v>
       </c>
@@ -9476,14 +9494,13 @@
       <c r="R25" s="24"/>
       <c r="S25" s="24"/>
       <c r="T25" s="24"/>
-      <c r="X25" s="2"/>
-      <c r="AD25" s="294" t="s">
+      <c r="AD25" s="295" t="s">
         <v>486</v>
       </c>
-      <c r="AE25" s="294"/>
-      <c r="AF25" s="294"/>
-      <c r="AG25" s="294"/>
-      <c r="AH25" s="294"/>
+      <c r="AE25" s="295"/>
+      <c r="AF25" s="295"/>
+      <c r="AG25" s="295"/>
+      <c r="AH25" s="295"/>
       <c r="AJ25" s="116" t="s">
         <v>555</v>
       </c>
@@ -9547,7 +9564,6 @@
       <c r="S26" s="23"/>
       <c r="T26" s="23"/>
       <c r="U26" s="23"/>
-      <c r="X26" s="2"/>
       <c r="AD26" s="29" t="s">
         <v>218</v>
       </c>
@@ -9754,15 +9770,15 @@
       <c r="N29" s="107" t="s">
         <v>355</v>
       </c>
-      <c r="V29" s="294" t="s">
+      <c r="V29" s="295" t="s">
         <v>212</v>
       </c>
-      <c r="W29" s="294"/>
-      <c r="X29" s="294"/>
-      <c r="Y29" s="294"/>
-      <c r="Z29" s="294"/>
-      <c r="AA29" s="294"/>
-      <c r="AB29" s="294"/>
+      <c r="W29" s="295"/>
+      <c r="X29" s="295"/>
+      <c r="Y29" s="295"/>
+      <c r="Z29" s="295"/>
+      <c r="AA29" s="295"/>
+      <c r="AB29" s="295"/>
     </row>
     <row r="30" spans="1:42">
       <c r="A30" s="107"/>
@@ -9818,15 +9834,15 @@
       </c>
       <c r="AA30" s="29"/>
       <c r="AB30" s="29"/>
-      <c r="AJ30" s="294" t="s">
+      <c r="AJ30" s="295" t="s">
         <v>831</v>
       </c>
-      <c r="AK30" s="294"/>
-      <c r="AL30" s="294"/>
-      <c r="AM30" s="294"/>
-      <c r="AN30" s="294"/>
-      <c r="AO30" s="294"/>
-      <c r="AP30" s="294"/>
+      <c r="AK30" s="295"/>
+      <c r="AL30" s="295"/>
+      <c r="AM30" s="295"/>
+      <c r="AN30" s="295"/>
+      <c r="AO30" s="295"/>
+      <c r="AP30" s="295"/>
     </row>
     <row r="31" spans="1:42">
       <c r="B31" s="24"/>
@@ -9913,15 +9929,15 @@
       <c r="AJ34" s="23"/>
     </row>
     <row r="37" spans="22:36">
-      <c r="V37" s="294" t="s">
+      <c r="V37" s="295" t="s">
         <v>9</v>
       </c>
-      <c r="W37" s="294"/>
-      <c r="X37" s="294"/>
-      <c r="Y37" s="294"/>
-      <c r="Z37" s="294"/>
-      <c r="AA37" s="294"/>
-      <c r="AB37" s="294"/>
+      <c r="W37" s="295"/>
+      <c r="X37" s="295"/>
+      <c r="Y37" s="295"/>
+      <c r="Z37" s="295"/>
+      <c r="AA37" s="295"/>
+      <c r="AB37" s="295"/>
     </row>
     <row r="38" spans="22:36">
       <c r="V38" s="29" t="s">
@@ -9941,11 +9957,11 @@
       </c>
       <c r="AA38" s="29"/>
       <c r="AB38" s="29"/>
-      <c r="AD38" s="299" t="s">
+      <c r="AD38" s="296" t="s">
         <v>260</v>
       </c>
-      <c r="AE38" s="300"/>
-      <c r="AF38" s="301"/>
+      <c r="AE38" s="297"/>
+      <c r="AF38" s="298"/>
     </row>
     <row r="39" spans="22:36">
       <c r="V39" s="3" t="s">
@@ -9982,15 +9998,15 @@
       <c r="AF41" s="3"/>
     </row>
     <row r="42" spans="22:36">
-      <c r="V42" s="294" t="s">
+      <c r="V42" s="295" t="s">
         <v>244</v>
       </c>
-      <c r="W42" s="294"/>
-      <c r="X42" s="294"/>
-      <c r="Y42" s="294"/>
-      <c r="Z42" s="294"/>
-      <c r="AA42" s="294"/>
-      <c r="AB42" s="294"/>
+      <c r="W42" s="295"/>
+      <c r="X42" s="295"/>
+      <c r="Y42" s="295"/>
+      <c r="Z42" s="295"/>
+      <c r="AA42" s="295"/>
+      <c r="AB42" s="295"/>
       <c r="AD42" s="3" t="s">
         <v>254</v>
       </c>
@@ -10060,15 +10076,15 @@
       <c r="AF47" s="3"/>
     </row>
     <row r="48" spans="22:36">
-      <c r="V48" s="295" t="s">
+      <c r="V48" s="299" t="s">
         <v>473</v>
       </c>
-      <c r="W48" s="296"/>
-      <c r="X48" s="296"/>
-      <c r="Y48" s="296"/>
-      <c r="Z48" s="296"/>
-      <c r="AA48" s="296"/>
-      <c r="AB48" s="297"/>
+      <c r="W48" s="300"/>
+      <c r="X48" s="300"/>
+      <c r="Y48" s="300"/>
+      <c r="Z48" s="300"/>
+      <c r="AA48" s="300"/>
+      <c r="AB48" s="301"/>
       <c r="AD48" s="3" t="s">
         <v>261</v>
       </c>
@@ -10678,6 +10694,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="V42:AB42"/>
+    <mergeCell ref="AD4:AH4"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="V48:AB48"/>
+    <mergeCell ref="V37:AB37"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="AJ4:AP4"/>
@@ -10686,11 +10707,6 @@
     <mergeCell ref="V29:AB29"/>
     <mergeCell ref="AD25:AH25"/>
     <mergeCell ref="AJ30:AP30"/>
-    <mergeCell ref="V42:AB42"/>
-    <mergeCell ref="AD4:AH4"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="V48:AB48"/>
-    <mergeCell ref="V37:AB37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11650,40 +11666,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="404" t="s">
+      <c r="A1" s="421" t="s">
         <v>326</v>
       </c>
-      <c r="B1" s="404"/>
-      <c r="C1" s="404"/>
-      <c r="D1" s="404"/>
-      <c r="E1" s="404"/>
-      <c r="F1" s="404"/>
-      <c r="G1" s="404"/>
-      <c r="H1" s="404"/>
+      <c r="B1" s="421"/>
+      <c r="C1" s="421"/>
+      <c r="D1" s="421"/>
+      <c r="E1" s="421"/>
+      <c r="F1" s="421"/>
+      <c r="G1" s="421"/>
+      <c r="H1" s="421"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="405"/>
-      <c r="B2" s="405"/>
-      <c r="C2" s="405"/>
-      <c r="D2" s="405"/>
-      <c r="E2" s="405"/>
-      <c r="F2" s="405"/>
-      <c r="G2" s="405"/>
-      <c r="H2" s="405"/>
+      <c r="A2" s="422"/>
+      <c r="B2" s="422"/>
+      <c r="C2" s="422"/>
+      <c r="D2" s="422"/>
+      <c r="E2" s="422"/>
+      <c r="F2" s="422"/>
+      <c r="G2" s="422"/>
+      <c r="H2" s="422"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="406" t="s">
+      <c r="A3" s="423" t="s">
         <v>227</v>
       </c>
-      <c r="B3" s="407"/>
-      <c r="C3" s="408"/>
-      <c r="D3" s="409"/>
-      <c r="E3" s="406" t="s">
+      <c r="B3" s="424"/>
+      <c r="C3" s="425"/>
+      <c r="D3" s="426"/>
+      <c r="E3" s="423" t="s">
         <v>228</v>
       </c>
-      <c r="F3" s="407"/>
-      <c r="G3" s="408"/>
-      <c r="H3" s="409"/>
+      <c r="F3" s="424"/>
+      <c r="G3" s="425"/>
+      <c r="H3" s="426"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="31">
@@ -11976,18 +11992,18 @@
       <c r="H24" s="59"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="406" t="s">
+      <c r="A25" s="423" t="s">
         <v>289</v>
       </c>
-      <c r="B25" s="407"/>
-      <c r="C25" s="408"/>
-      <c r="D25" s="409"/>
-      <c r="E25" s="406" t="s">
+      <c r="B25" s="424"/>
+      <c r="C25" s="425"/>
+      <c r="D25" s="426"/>
+      <c r="E25" s="423" t="s">
         <v>290</v>
       </c>
-      <c r="F25" s="407"/>
-      <c r="G25" s="408"/>
-      <c r="H25" s="409"/>
+      <c r="F25" s="424"/>
+      <c r="G25" s="425"/>
+      <c r="H25" s="426"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="35" t="s">
@@ -11999,23 +12015,23 @@
       <c r="E26" s="31" t="s">
         <v>292</v>
       </c>
-      <c r="F26" s="413"/>
-      <c r="G26" s="414"/>
-      <c r="H26" s="415"/>
+      <c r="F26" s="418"/>
+      <c r="G26" s="419"/>
+      <c r="H26" s="420"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="B27" s="416"/>
-      <c r="C27" s="417"/>
-      <c r="D27" s="418"/>
+      <c r="B27" s="413"/>
+      <c r="C27" s="414"/>
+      <c r="D27" s="416"/>
       <c r="E27" s="35" t="s">
         <v>294</v>
       </c>
       <c r="F27" s="410"/>
       <c r="G27" s="411"/>
-      <c r="H27" s="419"/>
+      <c r="H27" s="417"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="35" t="s">
@@ -12027,23 +12043,23 @@
       <c r="E28" s="43" t="s">
         <v>296</v>
       </c>
-      <c r="F28" s="416"/>
-      <c r="G28" s="417"/>
-      <c r="H28" s="420"/>
+      <c r="F28" s="413"/>
+      <c r="G28" s="414"/>
+      <c r="H28" s="415"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="43" t="s">
         <v>297</v>
       </c>
-      <c r="B29" s="416"/>
-      <c r="C29" s="417"/>
-      <c r="D29" s="418"/>
+      <c r="B29" s="413"/>
+      <c r="C29" s="414"/>
+      <c r="D29" s="416"/>
       <c r="E29" s="35" t="s">
         <v>298</v>
       </c>
       <c r="F29" s="410"/>
       <c r="G29" s="411"/>
-      <c r="H29" s="419"/>
+      <c r="H29" s="417"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="35" t="s">
@@ -12055,23 +12071,23 @@
       <c r="E30" s="43" t="s">
         <v>300</v>
       </c>
-      <c r="F30" s="416"/>
-      <c r="G30" s="417"/>
-      <c r="H30" s="420"/>
+      <c r="F30" s="413"/>
+      <c r="G30" s="414"/>
+      <c r="H30" s="415"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="43" t="s">
         <v>301</v>
       </c>
-      <c r="B31" s="416"/>
-      <c r="C31" s="417"/>
-      <c r="D31" s="418"/>
+      <c r="B31" s="413"/>
+      <c r="C31" s="414"/>
+      <c r="D31" s="416"/>
       <c r="E31" s="35" t="s">
         <v>302</v>
       </c>
       <c r="F31" s="410"/>
       <c r="G31" s="411"/>
-      <c r="H31" s="419"/>
+      <c r="H31" s="417"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="35" t="s">
@@ -12081,9 +12097,9 @@
       <c r="C32" s="411"/>
       <c r="D32" s="412"/>
       <c r="E32" s="43"/>
-      <c r="F32" s="416"/>
-      <c r="G32" s="417"/>
-      <c r="H32" s="420" t="s">
+      <c r="F32" s="413"/>
+      <c r="G32" s="414"/>
+      <c r="H32" s="415" t="s">
         <v>242</v>
       </c>
     </row>
@@ -12091,13 +12107,13 @@
       <c r="A33" s="43" t="s">
         <v>304</v>
       </c>
-      <c r="B33" s="416"/>
-      <c r="C33" s="417"/>
-      <c r="D33" s="418"/>
+      <c r="B33" s="413"/>
+      <c r="C33" s="414"/>
+      <c r="D33" s="416"/>
       <c r="E33" s="35"/>
       <c r="F33" s="410"/>
       <c r="G33" s="411"/>
-      <c r="H33" s="419" t="s">
+      <c r="H33" s="417" t="s">
         <v>284</v>
       </c>
     </row>
@@ -12109,9 +12125,9 @@
       <c r="C34" s="411"/>
       <c r="D34" s="412"/>
       <c r="E34" s="43"/>
-      <c r="F34" s="416"/>
-      <c r="G34" s="417"/>
-      <c r="H34" s="420" t="s">
+      <c r="F34" s="413"/>
+      <c r="G34" s="414"/>
+      <c r="H34" s="415" t="s">
         <v>285</v>
       </c>
     </row>
@@ -12119,13 +12135,13 @@
       <c r="A35" s="43" t="s">
         <v>306</v>
       </c>
-      <c r="B35" s="416"/>
-      <c r="C35" s="417"/>
-      <c r="D35" s="418"/>
+      <c r="B35" s="413"/>
+      <c r="C35" s="414"/>
+      <c r="D35" s="416"/>
       <c r="E35" s="35"/>
       <c r="F35" s="410"/>
       <c r="G35" s="411"/>
-      <c r="H35" s="419" t="s">
+      <c r="H35" s="417" t="s">
         <v>286</v>
       </c>
     </row>
@@ -12137,9 +12153,9 @@
       <c r="C36" s="411"/>
       <c r="D36" s="412"/>
       <c r="E36" s="43"/>
-      <c r="F36" s="416"/>
-      <c r="G36" s="417"/>
-      <c r="H36" s="420" t="s">
+      <c r="F36" s="413"/>
+      <c r="G36" s="414"/>
+      <c r="H36" s="415" t="s">
         <v>287</v>
       </c>
     </row>
@@ -12147,13 +12163,13 @@
       <c r="A37" s="43" t="s">
         <v>308</v>
       </c>
-      <c r="B37" s="416"/>
-      <c r="C37" s="417"/>
-      <c r="D37" s="418"/>
+      <c r="B37" s="413"/>
+      <c r="C37" s="414"/>
+      <c r="D37" s="416"/>
       <c r="E37" s="35"/>
       <c r="F37" s="410"/>
       <c r="G37" s="411"/>
-      <c r="H37" s="419" t="s">
+      <c r="H37" s="417" t="s">
         <v>288</v>
       </c>
     </row>
@@ -12165,9 +12181,9 @@
       <c r="C38" s="411"/>
       <c r="D38" s="412"/>
       <c r="E38" s="43"/>
-      <c r="F38" s="416"/>
-      <c r="G38" s="417"/>
-      <c r="H38" s="420" t="s">
+      <c r="F38" s="413"/>
+      <c r="G38" s="414"/>
+      <c r="H38" s="415" t="s">
         <v>241</v>
       </c>
     </row>
@@ -12175,13 +12191,13 @@
       <c r="A39" s="43" t="s">
         <v>310</v>
       </c>
-      <c r="B39" s="416"/>
-      <c r="C39" s="417"/>
-      <c r="D39" s="418"/>
+      <c r="B39" s="413"/>
+      <c r="C39" s="414"/>
+      <c r="D39" s="416"/>
       <c r="E39" s="35"/>
       <c r="F39" s="410"/>
       <c r="G39" s="411"/>
-      <c r="H39" s="419" t="s">
+      <c r="H39" s="417" t="s">
         <v>242</v>
       </c>
     </row>
@@ -12193,24 +12209,53 @@
       <c r="C40" s="411"/>
       <c r="D40" s="412"/>
       <c r="E40" s="43"/>
-      <c r="F40" s="416"/>
-      <c r="G40" s="417"/>
-      <c r="H40" s="420"/>
+      <c r="F40" s="413"/>
+      <c r="G40" s="414"/>
+      <c r="H40" s="415"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="55" t="s">
         <v>312</v>
       </c>
-      <c r="B41" s="421"/>
-      <c r="C41" s="422"/>
-      <c r="D41" s="423"/>
+      <c r="B41" s="404"/>
+      <c r="C41" s="405"/>
+      <c r="D41" s="406"/>
       <c r="E41" s="60"/>
-      <c r="F41" s="424"/>
-      <c r="G41" s="425"/>
-      <c r="H41" s="426"/>
+      <c r="F41" s="407"/>
+      <c r="G41" s="408"/>
+      <c r="H41" s="409"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -12219,35 +12264,6 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12303,55 +12319,55 @@
       </c>
     </row>
     <row r="2" spans="2:42">
-      <c r="B2" s="294" t="s">
+      <c r="B2" s="295" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="294"/>
-      <c r="D2" s="294"/>
-      <c r="E2" s="294"/>
-      <c r="F2" s="294"/>
-      <c r="H2" s="294" t="s">
+      <c r="C2" s="295"/>
+      <c r="D2" s="295"/>
+      <c r="E2" s="295"/>
+      <c r="F2" s="295"/>
+      <c r="H2" s="295" t="s">
         <v>1055</v>
       </c>
-      <c r="I2" s="294"/>
-      <c r="J2" s="294"/>
-      <c r="K2" s="294"/>
-      <c r="L2" s="294"/>
-      <c r="N2" s="294" t="s">
+      <c r="I2" s="295"/>
+      <c r="J2" s="295"/>
+      <c r="K2" s="295"/>
+      <c r="L2" s="295"/>
+      <c r="N2" s="295" t="s">
         <v>1054</v>
       </c>
-      <c r="O2" s="294"/>
-      <c r="P2" s="294"/>
-      <c r="Q2" s="294"/>
-      <c r="R2" s="294"/>
-      <c r="T2" s="294" t="s">
+      <c r="O2" s="295"/>
+      <c r="P2" s="295"/>
+      <c r="Q2" s="295"/>
+      <c r="R2" s="295"/>
+      <c r="T2" s="295" t="s">
         <v>236</v>
       </c>
-      <c r="U2" s="294"/>
-      <c r="V2" s="294"/>
-      <c r="W2" s="294"/>
-      <c r="X2" s="294"/>
-      <c r="Z2" s="294" t="s">
+      <c r="U2" s="295"/>
+      <c r="V2" s="295"/>
+      <c r="W2" s="295"/>
+      <c r="X2" s="295"/>
+      <c r="Z2" s="295" t="s">
         <v>246</v>
       </c>
-      <c r="AA2" s="294"/>
-      <c r="AB2" s="294"/>
-      <c r="AC2" s="294"/>
-      <c r="AD2" s="294"/>
-      <c r="AF2" s="294" t="s">
+      <c r="AA2" s="295"/>
+      <c r="AB2" s="295"/>
+      <c r="AC2" s="295"/>
+      <c r="AD2" s="295"/>
+      <c r="AF2" s="295" t="s">
         <v>317</v>
       </c>
-      <c r="AG2" s="294"/>
-      <c r="AH2" s="294"/>
-      <c r="AI2" s="294"/>
-      <c r="AJ2" s="294"/>
-      <c r="AL2" s="294" t="s">
+      <c r="AG2" s="295"/>
+      <c r="AH2" s="295"/>
+      <c r="AI2" s="295"/>
+      <c r="AJ2" s="295"/>
+      <c r="AL2" s="295" t="s">
         <v>491</v>
       </c>
-      <c r="AM2" s="294"/>
-      <c r="AN2" s="294"/>
-      <c r="AO2" s="294"/>
-      <c r="AP2" s="294"/>
+      <c r="AM2" s="295"/>
+      <c r="AN2" s="295"/>
+      <c r="AO2" s="295"/>
+      <c r="AP2" s="295"/>
     </row>
     <row r="3" spans="2:42">
       <c r="B3" s="101" t="s">
@@ -13985,20 +14001,20 @@
       <c r="X39" s="59"/>
     </row>
     <row r="41" spans="2:24">
-      <c r="B41" s="294" t="s">
+      <c r="B41" s="295" t="s">
         <v>697</v>
       </c>
-      <c r="C41" s="294"/>
-      <c r="D41" s="294"/>
-      <c r="E41" s="294"/>
-      <c r="F41" s="294"/>
-      <c r="H41" s="294" t="s">
+      <c r="C41" s="295"/>
+      <c r="D41" s="295"/>
+      <c r="E41" s="295"/>
+      <c r="F41" s="295"/>
+      <c r="H41" s="295" t="s">
         <v>750</v>
       </c>
-      <c r="I41" s="294"/>
-      <c r="J41" s="294"/>
-      <c r="K41" s="294"/>
-      <c r="L41" s="294"/>
+      <c r="I41" s="295"/>
+      <c r="J41" s="295"/>
+      <c r="K41" s="295"/>
+      <c r="L41" s="295"/>
     </row>
     <row r="42" spans="2:24">
       <c r="B42" s="101" t="s">
@@ -14535,39 +14551,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27" customHeight="1" thickBot="1">
-      <c r="A1" s="314" t="s">
+      <c r="A1" s="311" t="s">
         <v>1146</v>
       </c>
-      <c r="B1" s="315"/>
-      <c r="C1" s="315"/>
-      <c r="D1" s="315"/>
-      <c r="E1" s="315"/>
-      <c r="F1" s="315"/>
-      <c r="G1" s="315"/>
-      <c r="H1" s="315"/>
-      <c r="I1" s="315"/>
-      <c r="J1" s="315"/>
-      <c r="K1" s="315"/>
-      <c r="L1" s="316"/>
+      <c r="B1" s="312"/>
+      <c r="C1" s="312"/>
+      <c r="D1" s="312"/>
+      <c r="E1" s="312"/>
+      <c r="F1" s="312"/>
+      <c r="G1" s="312"/>
+      <c r="H1" s="312"/>
+      <c r="I1" s="312"/>
+      <c r="J1" s="312"/>
+      <c r="K1" s="312"/>
+      <c r="L1" s="313"/>
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A2" s="311" t="s">
+      <c r="A2" s="308" t="s">
         <v>1147</v>
       </c>
-      <c r="B2" s="312"/>
-      <c r="C2" s="313"/>
+      <c r="B2" s="309"/>
+      <c r="C2" s="310"/>
       <c r="D2" s="259"/>
-      <c r="E2" s="311" t="s">
+      <c r="E2" s="308" t="s">
         <v>1055</v>
       </c>
-      <c r="F2" s="312"/>
-      <c r="G2" s="313"/>
+      <c r="F2" s="309"/>
+      <c r="G2" s="310"/>
       <c r="H2" s="259"/>
-      <c r="I2" s="311" t="s">
+      <c r="I2" s="308" t="s">
         <v>1054</v>
       </c>
-      <c r="J2" s="312"/>
-      <c r="K2" s="313"/>
+      <c r="J2" s="309"/>
+      <c r="K2" s="310"/>
       <c r="L2" s="122"/>
     </row>
     <row r="3" spans="1:12" ht="19.5" thickBot="1">
@@ -14603,7 +14619,7 @@
       <c r="L3" s="122"/>
     </row>
     <row r="4" spans="1:12" ht="18.75">
-      <c r="A4" s="317" t="s">
+      <c r="A4" s="302" t="s">
         <v>325</v>
       </c>
       <c r="B4" s="132" t="s">
@@ -14613,7 +14629,7 @@
         <v>705</v>
       </c>
       <c r="D4" s="253"/>
-      <c r="E4" s="308" t="s">
+      <c r="E4" s="305" t="s">
         <v>975</v>
       </c>
       <c r="F4" s="132" t="s">
@@ -14623,7 +14639,7 @@
         <v>1028</v>
       </c>
       <c r="H4" s="125"/>
-      <c r="I4" s="308" t="s">
+      <c r="I4" s="305" t="s">
         <v>1057</v>
       </c>
       <c r="J4" s="132" t="s">
@@ -14635,7 +14651,7 @@
       <c r="L4" s="122"/>
     </row>
     <row r="5" spans="1:12" ht="18.75">
-      <c r="A5" s="318"/>
+      <c r="A5" s="303"/>
       <c r="B5" s="131" t="s">
         <v>322</v>
       </c>
@@ -14643,7 +14659,7 @@
         <v>706</v>
       </c>
       <c r="D5" s="253"/>
-      <c r="E5" s="309"/>
+      <c r="E5" s="306"/>
       <c r="F5" s="131" t="s">
         <v>1002</v>
       </c>
@@ -14651,7 +14667,7 @@
         <v>1029</v>
       </c>
       <c r="H5" s="125"/>
-      <c r="I5" s="309"/>
+      <c r="I5" s="306"/>
       <c r="J5" s="131" t="s">
         <v>1092</v>
       </c>
@@ -14661,7 +14677,7 @@
       <c r="L5" s="122"/>
     </row>
     <row r="6" spans="1:12" ht="18.75">
-      <c r="A6" s="318"/>
+      <c r="A6" s="303"/>
       <c r="B6" s="131" t="s">
         <v>323</v>
       </c>
@@ -14669,7 +14685,7 @@
         <v>707</v>
       </c>
       <c r="D6" s="253"/>
-      <c r="E6" s="309"/>
+      <c r="E6" s="306"/>
       <c r="F6" s="131" t="s">
         <v>1003</v>
       </c>
@@ -14677,7 +14693,7 @@
         <v>1030</v>
       </c>
       <c r="H6" s="125"/>
-      <c r="I6" s="309"/>
+      <c r="I6" s="306"/>
       <c r="J6" s="131" t="s">
         <v>1093</v>
       </c>
@@ -14687,7 +14703,7 @@
       <c r="L6" s="122"/>
     </row>
     <row r="7" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A7" s="319"/>
+      <c r="A7" s="304"/>
       <c r="B7" s="135" t="s">
         <v>324</v>
       </c>
@@ -14695,7 +14711,7 @@
         <v>708</v>
       </c>
       <c r="D7" s="253"/>
-      <c r="E7" s="310"/>
+      <c r="E7" s="307"/>
       <c r="F7" s="135" t="s">
         <v>1004</v>
       </c>
@@ -14703,7 +14719,7 @@
         <v>1031</v>
       </c>
       <c r="H7" s="125"/>
-      <c r="I7" s="310"/>
+      <c r="I7" s="307"/>
       <c r="J7" s="135" t="s">
         <v>1094</v>
       </c>
@@ -14713,7 +14729,7 @@
       <c r="L7" s="122"/>
     </row>
     <row r="8" spans="1:12" ht="18.75">
-      <c r="A8" s="317" t="s">
+      <c r="A8" s="302" t="s">
         <v>667</v>
       </c>
       <c r="B8" s="132" t="s">
@@ -14723,7 +14739,7 @@
         <v>709</v>
       </c>
       <c r="D8" s="253"/>
-      <c r="E8" s="308" t="s">
+      <c r="E8" s="305" t="s">
         <v>974</v>
       </c>
       <c r="F8" s="132" t="s">
@@ -14733,7 +14749,7 @@
         <v>1032</v>
       </c>
       <c r="H8" s="125"/>
-      <c r="I8" s="308" t="s">
+      <c r="I8" s="305" t="s">
         <v>1058</v>
       </c>
       <c r="J8" s="132" t="s">
@@ -14745,7 +14761,7 @@
       <c r="L8" s="122"/>
     </row>
     <row r="9" spans="1:12" ht="18.75">
-      <c r="A9" s="318"/>
+      <c r="A9" s="303"/>
       <c r="B9" s="131" t="s">
         <v>658</v>
       </c>
@@ -14753,7 +14769,7 @@
         <v>710</v>
       </c>
       <c r="D9" s="253"/>
-      <c r="E9" s="309"/>
+      <c r="E9" s="306"/>
       <c r="F9" s="131" t="s">
         <v>1006</v>
       </c>
@@ -14761,7 +14777,7 @@
         <v>1033</v>
       </c>
       <c r="H9" s="125"/>
-      <c r="I9" s="309"/>
+      <c r="I9" s="306"/>
       <c r="J9" s="131" t="s">
         <v>1095</v>
       </c>
@@ -14771,7 +14787,7 @@
       <c r="L9" s="122"/>
     </row>
     <row r="10" spans="1:12" ht="18.75">
-      <c r="A10" s="318"/>
+      <c r="A10" s="303"/>
       <c r="B10" s="131" t="s">
         <v>659</v>
       </c>
@@ -14779,7 +14795,7 @@
         <v>711</v>
       </c>
       <c r="D10" s="253"/>
-      <c r="E10" s="309"/>
+      <c r="E10" s="306"/>
       <c r="F10" s="131" t="s">
         <v>1008</v>
       </c>
@@ -14787,7 +14803,7 @@
         <v>1034</v>
       </c>
       <c r="H10" s="125"/>
-      <c r="I10" s="309"/>
+      <c r="I10" s="306"/>
       <c r="J10" s="131" t="s">
         <v>1096</v>
       </c>
@@ -14797,7 +14813,7 @@
       <c r="L10" s="122"/>
     </row>
     <row r="11" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A11" s="319"/>
+      <c r="A11" s="304"/>
       <c r="B11" s="135" t="s">
         <v>660</v>
       </c>
@@ -14805,7 +14821,7 @@
         <v>712</v>
       </c>
       <c r="D11" s="253"/>
-      <c r="E11" s="310"/>
+      <c r="E11" s="307"/>
       <c r="F11" s="135" t="s">
         <v>1009</v>
       </c>
@@ -14813,7 +14829,7 @@
         <v>1035</v>
       </c>
       <c r="H11" s="125"/>
-      <c r="I11" s="310"/>
+      <c r="I11" s="307"/>
       <c r="J11" s="135" t="s">
         <v>1097</v>
       </c>
@@ -14823,7 +14839,7 @@
       <c r="L11" s="122"/>
     </row>
     <row r="12" spans="1:12" ht="18.75">
-      <c r="A12" s="317" t="s">
+      <c r="A12" s="302" t="s">
         <v>665</v>
       </c>
       <c r="B12" s="132" t="s">
@@ -14833,7 +14849,7 @@
         <v>713</v>
       </c>
       <c r="D12" s="253"/>
-      <c r="E12" s="308" t="s">
+      <c r="E12" s="305" t="s">
         <v>973</v>
       </c>
       <c r="F12" s="132" t="s">
@@ -14843,7 +14859,7 @@
         <v>1036</v>
       </c>
       <c r="H12" s="125"/>
-      <c r="I12" s="308" t="s">
+      <c r="I12" s="305" t="s">
         <v>1059</v>
       </c>
       <c r="J12" s="132" t="s">
@@ -14855,7 +14871,7 @@
       <c r="L12" s="122"/>
     </row>
     <row r="13" spans="1:12" ht="18.75">
-      <c r="A13" s="318"/>
+      <c r="A13" s="303"/>
       <c r="B13" s="131" t="s">
         <v>662</v>
       </c>
@@ -14863,7 +14879,7 @@
         <v>714</v>
       </c>
       <c r="D13" s="253"/>
-      <c r="E13" s="309"/>
+      <c r="E13" s="306"/>
       <c r="F13" s="131" t="s">
         <v>1011</v>
       </c>
@@ -14871,7 +14887,7 @@
         <v>1037</v>
       </c>
       <c r="H13" s="125"/>
-      <c r="I13" s="309"/>
+      <c r="I13" s="306"/>
       <c r="J13" s="131" t="s">
         <v>1099</v>
       </c>
@@ -14881,7 +14897,7 @@
       <c r="L13" s="122"/>
     </row>
     <row r="14" spans="1:12" ht="18.75">
-      <c r="A14" s="318"/>
+      <c r="A14" s="303"/>
       <c r="B14" s="131" t="s">
         <v>663</v>
       </c>
@@ -14889,7 +14905,7 @@
         <v>715</v>
       </c>
       <c r="D14" s="253"/>
-      <c r="E14" s="309"/>
+      <c r="E14" s="306"/>
       <c r="F14" s="131" t="s">
         <v>1012</v>
       </c>
@@ -14897,7 +14913,7 @@
         <v>1038</v>
       </c>
       <c r="H14" s="125"/>
-      <c r="I14" s="309"/>
+      <c r="I14" s="306"/>
       <c r="J14" s="131" t="s">
         <v>1100</v>
       </c>
@@ -14907,7 +14923,7 @@
       <c r="L14" s="122"/>
     </row>
     <row r="15" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A15" s="319"/>
+      <c r="A15" s="304"/>
       <c r="B15" s="135" t="s">
         <v>664</v>
       </c>
@@ -14915,7 +14931,7 @@
         <v>716</v>
       </c>
       <c r="D15" s="253"/>
-      <c r="E15" s="310"/>
+      <c r="E15" s="307"/>
       <c r="F15" s="135" t="s">
         <v>1013</v>
       </c>
@@ -14923,7 +14939,7 @@
         <v>1039</v>
       </c>
       <c r="H15" s="125"/>
-      <c r="I15" s="310"/>
+      <c r="I15" s="307"/>
       <c r="J15" s="135" t="s">
         <v>1101</v>
       </c>
@@ -14933,7 +14949,7 @@
       <c r="L15" s="122"/>
     </row>
     <row r="16" spans="1:12" ht="18.75">
-      <c r="A16" s="317" t="s">
+      <c r="A16" s="302" t="s">
         <v>666</v>
       </c>
       <c r="B16" s="132" t="s">
@@ -14943,7 +14959,7 @@
         <v>717</v>
       </c>
       <c r="D16" s="253"/>
-      <c r="E16" s="308" t="s">
+      <c r="E16" s="305" t="s">
         <v>972</v>
       </c>
       <c r="F16" s="132" t="s">
@@ -14953,7 +14969,7 @@
         <v>1040</v>
       </c>
       <c r="H16" s="125"/>
-      <c r="I16" s="308" t="s">
+      <c r="I16" s="305" t="s">
         <v>1060</v>
       </c>
       <c r="J16" s="132" t="s">
@@ -14965,7 +14981,7 @@
       <c r="L16" s="122"/>
     </row>
     <row r="17" spans="1:12" ht="18.75">
-      <c r="A17" s="318"/>
+      <c r="A17" s="303"/>
       <c r="B17" s="131" t="s">
         <v>669</v>
       </c>
@@ -14973,7 +14989,7 @@
         <v>718</v>
       </c>
       <c r="D17" s="253"/>
-      <c r="E17" s="309"/>
+      <c r="E17" s="306"/>
       <c r="F17" s="131" t="s">
         <v>1015</v>
       </c>
@@ -14981,7 +14997,7 @@
         <v>1041</v>
       </c>
       <c r="H17" s="125"/>
-      <c r="I17" s="309"/>
+      <c r="I17" s="306"/>
       <c r="J17" s="131" t="s">
         <v>1103</v>
       </c>
@@ -14991,7 +15007,7 @@
       <c r="L17" s="122"/>
     </row>
     <row r="18" spans="1:12" ht="18.75">
-      <c r="A18" s="318"/>
+      <c r="A18" s="303"/>
       <c r="B18" s="131" t="s">
         <v>670</v>
       </c>
@@ -14999,7 +15015,7 @@
         <v>719</v>
       </c>
       <c r="D18" s="253"/>
-      <c r="E18" s="309"/>
+      <c r="E18" s="306"/>
       <c r="F18" s="131" t="s">
         <v>1016</v>
       </c>
@@ -15007,7 +15023,7 @@
         <v>1042</v>
       </c>
       <c r="H18" s="125"/>
-      <c r="I18" s="309"/>
+      <c r="I18" s="306"/>
       <c r="J18" s="131" t="s">
         <v>1104</v>
       </c>
@@ -15017,7 +15033,7 @@
       <c r="L18" s="122"/>
     </row>
     <row r="19" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A19" s="319"/>
+      <c r="A19" s="304"/>
       <c r="B19" s="135" t="s">
         <v>671</v>
       </c>
@@ -15025,7 +15041,7 @@
         <v>720</v>
       </c>
       <c r="D19" s="253"/>
-      <c r="E19" s="310"/>
+      <c r="E19" s="307"/>
       <c r="F19" s="135" t="s">
         <v>1017</v>
       </c>
@@ -15033,7 +15049,7 @@
         <v>1043</v>
       </c>
       <c r="H19" s="125"/>
-      <c r="I19" s="310"/>
+      <c r="I19" s="307"/>
       <c r="J19" s="135" t="s">
         <v>1105</v>
       </c>
@@ -15047,7 +15063,7 @@
       <c r="B20" s="125"/>
       <c r="C20" s="125"/>
       <c r="D20" s="125"/>
-      <c r="E20" s="308" t="s">
+      <c r="E20" s="305" t="s">
         <v>560</v>
       </c>
       <c r="F20" s="132" t="s">
@@ -15057,7 +15073,7 @@
         <v>1044</v>
       </c>
       <c r="H20" s="125"/>
-      <c r="I20" s="308" t="s">
+      <c r="I20" s="305" t="s">
         <v>1061</v>
       </c>
       <c r="J20" s="132" t="s">
@@ -15073,7 +15089,7 @@
       <c r="B21" s="125"/>
       <c r="C21" s="125"/>
       <c r="D21" s="125"/>
-      <c r="E21" s="309"/>
+      <c r="E21" s="306"/>
       <c r="F21" s="131" t="s">
         <v>1019</v>
       </c>
@@ -15081,7 +15097,7 @@
         <v>1045</v>
       </c>
       <c r="H21" s="125"/>
-      <c r="I21" s="309"/>
+      <c r="I21" s="306"/>
       <c r="J21" s="131" t="s">
         <v>1107</v>
       </c>
@@ -15095,7 +15111,7 @@
       <c r="B22" s="125"/>
       <c r="C22" s="125"/>
       <c r="D22" s="125"/>
-      <c r="E22" s="309"/>
+      <c r="E22" s="306"/>
       <c r="F22" s="131" t="s">
         <v>1020</v>
       </c>
@@ -15103,7 +15119,7 @@
         <v>1046</v>
       </c>
       <c r="H22" s="125"/>
-      <c r="I22" s="309"/>
+      <c r="I22" s="306"/>
       <c r="J22" s="131" t="s">
         <v>1108</v>
       </c>
@@ -15119,7 +15135,7 @@
       <c r="B23" s="256"/>
       <c r="C23" s="257"/>
       <c r="D23" s="125"/>
-      <c r="E23" s="310"/>
+      <c r="E23" s="307"/>
       <c r="F23" s="135" t="s">
         <v>1021</v>
       </c>
@@ -15127,7 +15143,7 @@
         <v>1047</v>
       </c>
       <c r="H23" s="125"/>
-      <c r="I23" s="310"/>
+      <c r="I23" s="307"/>
       <c r="J23" s="135" t="s">
         <v>1109</v>
       </c>
@@ -15147,7 +15163,7 @@
         <v>321</v>
       </c>
       <c r="D24" s="125"/>
-      <c r="E24" s="308" t="s">
+      <c r="E24" s="305" t="s">
         <v>749</v>
       </c>
       <c r="F24" s="132" t="s">
@@ -15157,7 +15173,7 @@
         <v>1048</v>
       </c>
       <c r="H24" s="125"/>
-      <c r="I24" s="308" t="s">
+      <c r="I24" s="305" t="s">
         <v>1062</v>
       </c>
       <c r="J24" s="132" t="s">
@@ -15169,7 +15185,7 @@
       <c r="L24" s="122"/>
     </row>
     <row r="25" spans="1:12" ht="18.75">
-      <c r="A25" s="302" t="s">
+      <c r="A25" s="317" t="s">
         <v>493</v>
       </c>
       <c r="B25" s="132" t="s">
@@ -15179,7 +15195,7 @@
         <v>721</v>
       </c>
       <c r="D25" s="125"/>
-      <c r="E25" s="309"/>
+      <c r="E25" s="306"/>
       <c r="F25" s="131" t="s">
         <v>1023</v>
       </c>
@@ -15187,7 +15203,7 @@
         <v>1049</v>
       </c>
       <c r="H25" s="125"/>
-      <c r="I25" s="309"/>
+      <c r="I25" s="306"/>
       <c r="J25" s="131" t="s">
         <v>1111</v>
       </c>
@@ -15197,7 +15213,7 @@
       <c r="L25" s="122"/>
     </row>
     <row r="26" spans="1:12" ht="18.75">
-      <c r="A26" s="303"/>
+      <c r="A26" s="318"/>
       <c r="B26" s="131" t="s">
         <v>679</v>
       </c>
@@ -15205,7 +15221,7 @@
         <v>722</v>
       </c>
       <c r="D26" s="125"/>
-      <c r="E26" s="309"/>
+      <c r="E26" s="306"/>
       <c r="F26" s="131" t="s">
         <v>1024</v>
       </c>
@@ -15213,7 +15229,7 @@
         <v>1050</v>
       </c>
       <c r="H26" s="125"/>
-      <c r="I26" s="309"/>
+      <c r="I26" s="306"/>
       <c r="J26" s="131" t="s">
         <v>1112</v>
       </c>
@@ -15223,7 +15239,7 @@
       <c r="L26" s="122"/>
     </row>
     <row r="27" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A27" s="303"/>
+      <c r="A27" s="318"/>
       <c r="B27" s="131" t="s">
         <v>680</v>
       </c>
@@ -15231,7 +15247,7 @@
         <v>723</v>
       </c>
       <c r="D27" s="125"/>
-      <c r="E27" s="310"/>
+      <c r="E27" s="307"/>
       <c r="F27" s="135" t="s">
         <v>1025</v>
       </c>
@@ -15239,7 +15255,7 @@
         <v>1051</v>
       </c>
       <c r="H27" s="125"/>
-      <c r="I27" s="310"/>
+      <c r="I27" s="307"/>
       <c r="J27" s="135" t="s">
         <v>1113</v>
       </c>
@@ -15249,7 +15265,7 @@
       <c r="L27" s="122"/>
     </row>
     <row r="28" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A28" s="304"/>
+      <c r="A28" s="319"/>
       <c r="B28" s="135" t="s">
         <v>681</v>
       </c>
@@ -15257,7 +15273,7 @@
         <v>724</v>
       </c>
       <c r="D28" s="125"/>
-      <c r="E28" s="308" t="s">
+      <c r="E28" s="305" t="s">
         <v>562</v>
       </c>
       <c r="F28" s="132" t="s">
@@ -15267,7 +15283,7 @@
         <v>1052</v>
       </c>
       <c r="H28" s="125"/>
-      <c r="I28" s="308" t="s">
+      <c r="I28" s="305" t="s">
         <v>1063</v>
       </c>
       <c r="J28" s="132" t="s">
@@ -15279,7 +15295,7 @@
       <c r="L28" s="122"/>
     </row>
     <row r="29" spans="1:12" ht="18.75">
-      <c r="A29" s="302" t="s">
+      <c r="A29" s="317" t="s">
         <v>687</v>
       </c>
       <c r="B29" s="132" t="s">
@@ -15289,7 +15305,7 @@
         <v>725</v>
       </c>
       <c r="D29" s="253"/>
-      <c r="E29" s="309"/>
+      <c r="E29" s="306"/>
       <c r="F29" s="131" t="s">
         <v>1027</v>
       </c>
@@ -15297,7 +15313,7 @@
         <v>1053</v>
       </c>
       <c r="H29" s="125"/>
-      <c r="I29" s="309"/>
+      <c r="I29" s="306"/>
       <c r="J29" s="131" t="s">
         <v>1115</v>
       </c>
@@ -15307,7 +15323,7 @@
       <c r="L29" s="122"/>
     </row>
     <row r="30" spans="1:12" ht="18.75">
-      <c r="A30" s="303"/>
+      <c r="A30" s="318"/>
       <c r="B30" s="131" t="s">
         <v>684</v>
       </c>
@@ -15315,11 +15331,11 @@
         <v>726</v>
       </c>
       <c r="D30" s="253"/>
-      <c r="E30" s="309"/>
+      <c r="E30" s="306"/>
       <c r="F30" s="131"/>
       <c r="G30" s="250"/>
       <c r="H30" s="125"/>
-      <c r="I30" s="309"/>
+      <c r="I30" s="306"/>
       <c r="J30" s="131" t="s">
         <v>1116</v>
       </c>
@@ -15329,7 +15345,7 @@
       <c r="L30" s="122"/>
     </row>
     <row r="31" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A31" s="303"/>
+      <c r="A31" s="318"/>
       <c r="B31" s="131" t="s">
         <v>685</v>
       </c>
@@ -15337,11 +15353,11 @@
         <v>727</v>
       </c>
       <c r="D31" s="253"/>
-      <c r="E31" s="310"/>
+      <c r="E31" s="307"/>
       <c r="F31" s="135"/>
       <c r="G31" s="251"/>
       <c r="H31" s="125"/>
-      <c r="I31" s="310"/>
+      <c r="I31" s="307"/>
       <c r="J31" s="135" t="s">
         <v>1117</v>
       </c>
@@ -15351,7 +15367,7 @@
       <c r="L31" s="122"/>
     </row>
     <row r="32" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A32" s="304"/>
+      <c r="A32" s="319"/>
       <c r="B32" s="135" t="s">
         <v>686</v>
       </c>
@@ -15369,7 +15385,7 @@
       <c r="L32" s="122"/>
     </row>
     <row r="33" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A33" s="302" t="s">
+      <c r="A33" s="317" t="s">
         <v>691</v>
       </c>
       <c r="B33" s="132" t="s">
@@ -15379,21 +15395,21 @@
         <v>729</v>
       </c>
       <c r="D33" s="253"/>
-      <c r="E33" s="305" t="s">
+      <c r="E33" s="314" t="s">
         <v>1149</v>
       </c>
-      <c r="F33" s="306"/>
-      <c r="G33" s="307"/>
+      <c r="F33" s="315"/>
+      <c r="G33" s="316"/>
       <c r="H33" s="124"/>
-      <c r="I33" s="305" t="s">
+      <c r="I33" s="314" t="s">
         <v>1148</v>
       </c>
-      <c r="J33" s="306"/>
-      <c r="K33" s="307"/>
+      <c r="J33" s="315"/>
+      <c r="K33" s="316"/>
       <c r="L33" s="122"/>
     </row>
     <row r="34" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A34" s="303"/>
+      <c r="A34" s="318"/>
       <c r="B34" s="131" t="s">
         <v>693</v>
       </c>
@@ -15423,7 +15439,7 @@
       <c r="L34" s="122"/>
     </row>
     <row r="35" spans="1:12" ht="18.75">
-      <c r="A35" s="303"/>
+      <c r="A35" s="318"/>
       <c r="B35" s="131" t="s">
         <v>694</v>
       </c>
@@ -15431,7 +15447,7 @@
         <v>731</v>
       </c>
       <c r="D35" s="253"/>
-      <c r="E35" s="302" t="s">
+      <c r="E35" s="317" t="s">
         <v>494</v>
       </c>
       <c r="F35" s="132" t="s">
@@ -15441,7 +15457,7 @@
         <v>11311</v>
       </c>
       <c r="H35" s="124"/>
-      <c r="I35" s="302" t="s">
+      <c r="I35" s="317" t="s">
         <v>955</v>
       </c>
       <c r="J35" s="132" t="s">
@@ -15453,7 +15469,7 @@
       <c r="L35" s="122"/>
     </row>
     <row r="36" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A36" s="304"/>
+      <c r="A36" s="319"/>
       <c r="B36" s="135" t="s">
         <v>695</v>
       </c>
@@ -15461,7 +15477,7 @@
         <v>732</v>
       </c>
       <c r="D36" s="253"/>
-      <c r="E36" s="303"/>
+      <c r="E36" s="318"/>
       <c r="F36" s="131" t="s">
         <v>958</v>
       </c>
@@ -15469,7 +15485,7 @@
         <v>11312</v>
       </c>
       <c r="H36" s="124"/>
-      <c r="I36" s="303"/>
+      <c r="I36" s="318"/>
       <c r="J36" s="131" t="s">
         <v>965</v>
       </c>
@@ -15479,7 +15495,7 @@
       <c r="L36" s="122"/>
     </row>
     <row r="37" spans="1:12" ht="18.75">
-      <c r="A37" s="302" t="s">
+      <c r="A37" s="317" t="s">
         <v>698</v>
       </c>
       <c r="B37" s="132" t="s">
@@ -15489,7 +15505,7 @@
         <v>11441</v>
       </c>
       <c r="D37" s="253"/>
-      <c r="E37" s="303"/>
+      <c r="E37" s="318"/>
       <c r="F37" s="131" t="s">
         <v>959</v>
       </c>
@@ -15497,7 +15513,7 @@
         <v>11313</v>
       </c>
       <c r="H37" s="124"/>
-      <c r="I37" s="303"/>
+      <c r="I37" s="318"/>
       <c r="J37" s="131" t="s">
         <v>966</v>
       </c>
@@ -15507,7 +15523,7 @@
       <c r="L37" s="122"/>
     </row>
     <row r="38" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A38" s="303"/>
+      <c r="A38" s="318"/>
       <c r="B38" s="131" t="s">
         <v>700</v>
       </c>
@@ -15515,7 +15531,7 @@
         <v>11442</v>
       </c>
       <c r="D38" s="253"/>
-      <c r="E38" s="304"/>
+      <c r="E38" s="319"/>
       <c r="F38" s="135" t="s">
         <v>959</v>
       </c>
@@ -15523,7 +15539,7 @@
         <v>11314</v>
       </c>
       <c r="H38" s="124"/>
-      <c r="I38" s="304"/>
+      <c r="I38" s="319"/>
       <c r="J38" s="135" t="s">
         <v>967</v>
       </c>
@@ -15533,7 +15549,7 @@
       <c r="L38" s="122"/>
     </row>
     <row r="39" spans="1:12" ht="18.75">
-      <c r="A39" s="303"/>
+      <c r="A39" s="318"/>
       <c r="B39" s="131" t="s">
         <v>701</v>
       </c>
@@ -15541,7 +15557,7 @@
         <v>11443</v>
       </c>
       <c r="D39" s="253"/>
-      <c r="E39" s="302" t="s">
+      <c r="E39" s="317" t="s">
         <v>954</v>
       </c>
       <c r="F39" s="132" t="s">
@@ -15551,7 +15567,7 @@
         <v>11321</v>
       </c>
       <c r="H39" s="124"/>
-      <c r="I39" s="302" t="s">
+      <c r="I39" s="317" t="s">
         <v>956</v>
       </c>
       <c r="J39" s="132" t="s">
@@ -15563,7 +15579,7 @@
       <c r="L39" s="122"/>
     </row>
     <row r="40" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A40" s="304"/>
+      <c r="A40" s="319"/>
       <c r="B40" s="135" t="s">
         <v>702</v>
       </c>
@@ -15571,7 +15587,7 @@
         <v>11444</v>
       </c>
       <c r="D40" s="253"/>
-      <c r="E40" s="303"/>
+      <c r="E40" s="318"/>
       <c r="F40" s="131" t="s">
         <v>961</v>
       </c>
@@ -15579,7 +15595,7 @@
         <v>11322</v>
       </c>
       <c r="H40" s="124"/>
-      <c r="I40" s="303"/>
+      <c r="I40" s="318"/>
       <c r="J40" s="131" t="s">
         <v>969</v>
       </c>
@@ -15593,7 +15609,7 @@
       <c r="B41" s="125"/>
       <c r="C41" s="253"/>
       <c r="D41" s="253"/>
-      <c r="E41" s="303"/>
+      <c r="E41" s="318"/>
       <c r="F41" s="131" t="s">
         <v>962</v>
       </c>
@@ -15601,7 +15617,7 @@
         <v>11323</v>
       </c>
       <c r="H41" s="124"/>
-      <c r="I41" s="303"/>
+      <c r="I41" s="318"/>
       <c r="J41" s="131" t="s">
         <v>970</v>
       </c>
@@ -15615,7 +15631,7 @@
       <c r="B42" s="125"/>
       <c r="C42" s="253"/>
       <c r="D42" s="253"/>
-      <c r="E42" s="304"/>
+      <c r="E42" s="319"/>
       <c r="F42" s="135" t="s">
         <v>963</v>
       </c>
@@ -15623,7 +15639,7 @@
         <v>11324</v>
       </c>
       <c r="H42" s="124"/>
-      <c r="I42" s="304"/>
+      <c r="I42" s="319"/>
       <c r="J42" s="135" t="s">
         <v>971</v>
       </c>
@@ -15676,18 +15692,16 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="I35:I38"/>
+    <mergeCell ref="I39:I42"/>
     <mergeCell ref="I16:I19"/>
     <mergeCell ref="I12:I15"/>
     <mergeCell ref="I8:I11"/>
@@ -15698,16 +15712,18 @@
     <mergeCell ref="I28:I31"/>
     <mergeCell ref="E20:E23"/>
     <mergeCell ref="E24:E27"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="I35:I38"/>
-    <mergeCell ref="I39:I42"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="E16:E19"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15738,40 +15754,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="320" t="s">
+      <c r="A1" s="324" t="s">
         <v>1151</v>
       </c>
-      <c r="B1" s="321"/>
-      <c r="C1" s="321"/>
-      <c r="D1" s="321"/>
-      <c r="E1" s="321"/>
-      <c r="F1" s="321"/>
-      <c r="G1" s="321"/>
-      <c r="H1" s="322"/>
+      <c r="B1" s="325"/>
+      <c r="C1" s="325"/>
+      <c r="D1" s="325"/>
+      <c r="E1" s="325"/>
+      <c r="F1" s="325"/>
+      <c r="G1" s="325"/>
+      <c r="H1" s="326"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="323"/>
-      <c r="B2" s="324"/>
-      <c r="C2" s="324"/>
-      <c r="D2" s="324"/>
-      <c r="E2" s="324"/>
-      <c r="F2" s="324"/>
-      <c r="G2" s="324"/>
-      <c r="H2" s="325"/>
+      <c r="A2" s="327"/>
+      <c r="B2" s="328"/>
+      <c r="C2" s="328"/>
+      <c r="D2" s="328"/>
+      <c r="E2" s="328"/>
+      <c r="F2" s="328"/>
+      <c r="G2" s="328"/>
+      <c r="H2" s="329"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="326" t="s">
+      <c r="A3" s="330" t="s">
         <v>250</v>
       </c>
-      <c r="B3" s="327"/>
-      <c r="C3" s="327"/>
-      <c r="D3" s="327"/>
-      <c r="E3" s="327" t="s">
+      <c r="B3" s="331"/>
+      <c r="C3" s="331"/>
+      <c r="D3" s="331"/>
+      <c r="E3" s="331" t="s">
         <v>251</v>
       </c>
-      <c r="F3" s="327"/>
-      <c r="G3" s="327"/>
-      <c r="H3" s="328"/>
+      <c r="F3" s="331"/>
+      <c r="G3" s="331"/>
+      <c r="H3" s="332"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="12">
@@ -16305,11 +16321,11 @@
       <c r="C27" s="118" t="s">
         <v>594</v>
       </c>
-      <c r="D27" s="329" t="s">
+      <c r="D27" s="323" t="s">
         <v>570</v>
       </c>
-      <c r="E27" s="329"/>
-      <c r="F27" s="329"/>
+      <c r="E27" s="323"/>
+      <c r="F27" s="323"/>
       <c r="G27" s="17"/>
       <c r="H27" s="18"/>
     </row>
@@ -16321,11 +16337,11 @@
       <c r="C28" s="118" t="s">
         <v>598</v>
       </c>
-      <c r="D28" s="329" t="s">
+      <c r="D28" s="323" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="329"/>
-      <c r="F28" s="329"/>
+      <c r="E28" s="323"/>
+      <c r="F28" s="323"/>
       <c r="G28" s="17"/>
       <c r="H28" s="18"/>
     </row>
@@ -16337,11 +16353,11 @@
       <c r="C29" s="118" t="s">
         <v>599</v>
       </c>
-      <c r="D29" s="329" t="s">
+      <c r="D29" s="323" t="s">
         <v>571</v>
       </c>
-      <c r="E29" s="329"/>
-      <c r="F29" s="329"/>
+      <c r="E29" s="323"/>
+      <c r="F29" s="323"/>
       <c r="G29" s="17"/>
       <c r="H29" s="18"/>
     </row>
@@ -16353,11 +16369,11 @@
       <c r="C30" s="118" t="s">
         <v>600</v>
       </c>
-      <c r="D30" s="329" t="s">
+      <c r="D30" s="323" t="s">
         <v>572</v>
       </c>
-      <c r="E30" s="329"/>
-      <c r="F30" s="329"/>
+      <c r="E30" s="323"/>
+      <c r="F30" s="323"/>
       <c r="G30" s="17"/>
       <c r="H30" s="18"/>
     </row>
@@ -16369,11 +16385,11 @@
       <c r="C31" s="118" t="s">
         <v>601</v>
       </c>
-      <c r="D31" s="329" t="s">
+      <c r="D31" s="323" t="s">
         <v>573</v>
       </c>
-      <c r="E31" s="329"/>
-      <c r="F31" s="329"/>
+      <c r="E31" s="323"/>
+      <c r="F31" s="323"/>
       <c r="G31" s="17"/>
       <c r="H31" s="18"/>
     </row>
@@ -16385,11 +16401,11 @@
       <c r="C32" s="118" t="s">
         <v>602</v>
       </c>
-      <c r="D32" s="329" t="s">
+      <c r="D32" s="323" t="s">
         <v>574</v>
       </c>
-      <c r="E32" s="329"/>
-      <c r="F32" s="329"/>
+      <c r="E32" s="323"/>
+      <c r="F32" s="323"/>
       <c r="G32" s="17"/>
       <c r="H32" s="18"/>
     </row>
@@ -16401,11 +16417,11 @@
       <c r="C33" s="118" t="s">
         <v>614</v>
       </c>
-      <c r="D33" s="329" t="s">
+      <c r="D33" s="323" t="s">
         <v>482</v>
       </c>
-      <c r="E33" s="329"/>
-      <c r="F33" s="329"/>
+      <c r="E33" s="323"/>
+      <c r="F33" s="323"/>
       <c r="G33" s="17"/>
       <c r="H33" s="18"/>
     </row>
@@ -16417,11 +16433,11 @@
       <c r="C34" s="118" t="s">
         <v>615</v>
       </c>
-      <c r="D34" s="329" t="s">
+      <c r="D34" s="323" t="s">
         <v>575</v>
       </c>
-      <c r="E34" s="329"/>
-      <c r="F34" s="329"/>
+      <c r="E34" s="323"/>
+      <c r="F34" s="323"/>
       <c r="G34" s="17"/>
       <c r="H34" s="18"/>
     </row>
@@ -16433,11 +16449,11 @@
       <c r="C35" s="118" t="s">
         <v>616</v>
       </c>
-      <c r="D35" s="329" t="s">
+      <c r="D35" s="323" t="s">
         <v>576</v>
       </c>
-      <c r="E35" s="329"/>
-      <c r="F35" s="329"/>
+      <c r="E35" s="323"/>
+      <c r="F35" s="323"/>
       <c r="G35" s="17"/>
       <c r="H35" s="18"/>
     </row>
@@ -16447,11 +16463,11 @@
       <c r="C36" s="118" t="s">
         <v>651</v>
       </c>
-      <c r="D36" s="330" t="s">
+      <c r="D36" s="320" t="s">
         <v>591</v>
       </c>
-      <c r="E36" s="331"/>
-      <c r="F36" s="332"/>
+      <c r="E36" s="321"/>
+      <c r="F36" s="322"/>
       <c r="G36" s="17"/>
       <c r="H36" s="18"/>
     </row>
@@ -16461,11 +16477,11 @@
       <c r="C37" s="118" t="s">
         <v>654</v>
       </c>
-      <c r="D37" s="330" t="s">
+      <c r="D37" s="320" t="s">
         <v>652</v>
       </c>
-      <c r="E37" s="331"/>
-      <c r="F37" s="332"/>
+      <c r="E37" s="321"/>
+      <c r="F37" s="322"/>
       <c r="G37" s="17"/>
       <c r="H37" s="18"/>
     </row>
@@ -16475,11 +16491,11 @@
       <c r="C38" s="118" t="s">
         <v>653</v>
       </c>
-      <c r="D38" s="330" t="s">
+      <c r="D38" s="320" t="s">
         <v>655</v>
       </c>
-      <c r="E38" s="331"/>
-      <c r="F38" s="332"/>
+      <c r="E38" s="321"/>
+      <c r="F38" s="322"/>
       <c r="G38" s="17"/>
       <c r="H38" s="18"/>
     </row>
@@ -16487,9 +16503,9 @@
       <c r="A39" s="16"/>
       <c r="B39" s="120"/>
       <c r="C39" s="118"/>
-      <c r="D39" s="330"/>
-      <c r="E39" s="331"/>
-      <c r="F39" s="332"/>
+      <c r="D39" s="320"/>
+      <c r="E39" s="321"/>
+      <c r="F39" s="322"/>
       <c r="G39" s="17"/>
       <c r="H39" s="18"/>
     </row>
@@ -16587,13 +16603,6 @@
     <row r="52" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:H3"/>
@@ -16603,6 +16612,13 @@
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -18365,28 +18381,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="374" t="s">
+      <c r="A1" s="362" t="s">
         <v>952</v>
       </c>
-      <c r="B1" s="375"/>
-      <c r="C1" s="375"/>
-      <c r="D1" s="375"/>
-      <c r="E1" s="375"/>
-      <c r="F1" s="376"/>
+      <c r="B1" s="363"/>
+      <c r="C1" s="363"/>
+      <c r="D1" s="363"/>
+      <c r="E1" s="363"/>
+      <c r="F1" s="364"/>
       <c r="G1" s="175"/>
       <c r="H1" s="175"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="377" t="s">
+      <c r="A2" s="365" t="s">
         <v>840</v>
       </c>
-      <c r="B2" s="378"/>
-      <c r="C2" s="379"/>
-      <c r="D2" s="377" t="s">
+      <c r="B2" s="366"/>
+      <c r="C2" s="367"/>
+      <c r="D2" s="365" t="s">
         <v>841</v>
       </c>
-      <c r="E2" s="378"/>
-      <c r="F2" s="379"/>
+      <c r="E2" s="366"/>
+      <c r="F2" s="367"/>
       <c r="G2" s="175"/>
       <c r="H2" s="175"/>
     </row>
@@ -18410,7 +18426,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="175"/>
-      <c r="H3" s="371" t="s">
+      <c r="H3" s="368" t="s">
         <v>844</v>
       </c>
     </row>
@@ -18434,7 +18450,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="175"/>
-      <c r="H4" s="372"/>
+      <c r="H4" s="369"/>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A5" s="176">
@@ -18456,7 +18472,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="175"/>
-      <c r="H5" s="372"/>
+      <c r="H5" s="369"/>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A6" s="179">
@@ -18478,7 +18494,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="175"/>
-      <c r="H6" s="372"/>
+      <c r="H6" s="369"/>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A7" s="179">
@@ -18500,7 +18516,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="175"/>
-      <c r="H7" s="372"/>
+      <c r="H7" s="369"/>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A8" s="182">
@@ -18522,7 +18538,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="175"/>
-      <c r="H8" s="372"/>
+      <c r="H8" s="369"/>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A9" s="182">
@@ -18544,7 +18560,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="175"/>
-      <c r="H9" s="372"/>
+      <c r="H9" s="369"/>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A10" s="185">
@@ -18566,7 +18582,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="175"/>
-      <c r="H10" s="373"/>
+      <c r="H10" s="370"/>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="188">
@@ -18588,7 +18604,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="175"/>
-      <c r="H11" s="362" t="s">
+      <c r="H11" s="371" t="s">
         <v>856</v>
       </c>
     </row>
@@ -18612,7 +18628,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="175"/>
-      <c r="H12" s="363"/>
+      <c r="H12" s="372"/>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A13" s="191">
@@ -18634,7 +18650,7 @@
         <v>11</v>
       </c>
       <c r="G13" s="175"/>
-      <c r="H13" s="363"/>
+      <c r="H13" s="372"/>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A14" s="191">
@@ -18656,7 +18672,7 @@
         <v>12</v>
       </c>
       <c r="G14" s="175"/>
-      <c r="H14" s="363"/>
+      <c r="H14" s="372"/>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A15" s="195">
@@ -18678,7 +18694,7 @@
         <v>13</v>
       </c>
       <c r="G15" s="175"/>
-      <c r="H15" s="363"/>
+      <c r="H15" s="372"/>
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A16" s="195">
@@ -18700,7 +18716,7 @@
         <v>14</v>
       </c>
       <c r="G16" s="175"/>
-      <c r="H16" s="363"/>
+      <c r="H16" s="372"/>
     </row>
     <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A17" s="195">
@@ -18722,7 +18738,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="175"/>
-      <c r="H17" s="363"/>
+      <c r="H17" s="372"/>
     </row>
     <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A18" s="195">
@@ -18744,7 +18760,7 @@
         <v>16</v>
       </c>
       <c r="G18" s="175"/>
-      <c r="H18" s="363"/>
+      <c r="H18" s="372"/>
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A19" s="195">
@@ -18766,7 +18782,7 @@
         <v>17</v>
       </c>
       <c r="G19" s="175"/>
-      <c r="H19" s="363"/>
+      <c r="H19" s="372"/>
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A20" s="198">
@@ -18788,7 +18804,7 @@
         <v>18</v>
       </c>
       <c r="G20" s="175"/>
-      <c r="H20" s="363"/>
+      <c r="H20" s="372"/>
     </row>
     <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A21" s="198">
@@ -18810,7 +18826,7 @@
         <v>19</v>
       </c>
       <c r="G21" s="175"/>
-      <c r="H21" s="363"/>
+      <c r="H21" s="372"/>
     </row>
     <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A22" s="201">
@@ -18832,7 +18848,7 @@
         <v>20</v>
       </c>
       <c r="G22" s="175"/>
-      <c r="H22" s="364"/>
+      <c r="H22" s="373"/>
     </row>
     <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1"/>
@@ -18850,28 +18866,28 @@
     <row r="36" spans="1:8" ht="20.100000000000001" customHeight="1"/>
     <row r="37" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1"/>
     <row r="38" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A38" s="365" t="s">
+      <c r="A38" s="374" t="s">
         <v>953</v>
       </c>
-      <c r="B38" s="366"/>
-      <c r="C38" s="366"/>
-      <c r="D38" s="366"/>
-      <c r="E38" s="366"/>
-      <c r="F38" s="367"/>
+      <c r="B38" s="375"/>
+      <c r="C38" s="375"/>
+      <c r="D38" s="375"/>
+      <c r="E38" s="375"/>
+      <c r="F38" s="376"/>
       <c r="G38" s="175"/>
       <c r="H38" s="175"/>
     </row>
     <row r="39" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A39" s="368" t="s">
+      <c r="A39" s="377" t="s">
         <v>840</v>
       </c>
-      <c r="B39" s="369"/>
-      <c r="C39" s="370"/>
-      <c r="D39" s="368" t="s">
+      <c r="B39" s="378"/>
+      <c r="C39" s="379"/>
+      <c r="D39" s="377" t="s">
         <v>841</v>
       </c>
-      <c r="E39" s="369"/>
-      <c r="F39" s="370"/>
+      <c r="E39" s="378"/>
+      <c r="F39" s="379"/>
       <c r="G39" s="175"/>
       <c r="H39" s="175"/>
     </row>
@@ -18895,7 +18911,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="175"/>
-      <c r="H40" s="371" t="s">
+      <c r="H40" s="368" t="s">
         <v>844</v>
       </c>
     </row>
@@ -18919,7 +18935,7 @@
         <v>2</v>
       </c>
       <c r="G41" s="175"/>
-      <c r="H41" s="372"/>
+      <c r="H41" s="369"/>
     </row>
     <row r="42" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A42" s="204">
@@ -18941,7 +18957,7 @@
         <v>3</v>
       </c>
       <c r="G42" s="175"/>
-      <c r="H42" s="372"/>
+      <c r="H42" s="369"/>
     </row>
     <row r="43" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A43" s="206">
@@ -18963,7 +18979,7 @@
         <v>4</v>
       </c>
       <c r="G43" s="175"/>
-      <c r="H43" s="372"/>
+      <c r="H43" s="369"/>
     </row>
     <row r="44" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A44" s="206">
@@ -18985,7 +19001,7 @@
         <v>5</v>
       </c>
       <c r="G44" s="175"/>
-      <c r="H44" s="372"/>
+      <c r="H44" s="369"/>
     </row>
     <row r="45" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A45" s="208">
@@ -19007,7 +19023,7 @@
         <v>6</v>
       </c>
       <c r="G45" s="175"/>
-      <c r="H45" s="372"/>
+      <c r="H45" s="369"/>
     </row>
     <row r="46" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A46" s="208">
@@ -19029,7 +19045,7 @@
         <v>7</v>
       </c>
       <c r="G46" s="175"/>
-      <c r="H46" s="372"/>
+      <c r="H46" s="369"/>
     </row>
     <row r="47" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A47" s="210">
@@ -19051,7 +19067,7 @@
         <v>8</v>
       </c>
       <c r="G47" s="175"/>
-      <c r="H47" s="373"/>
+      <c r="H47" s="370"/>
     </row>
     <row r="48" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="A48" s="213">
@@ -19073,7 +19089,7 @@
         <v>9</v>
       </c>
       <c r="G48" s="175"/>
-      <c r="H48" s="362" t="s">
+      <c r="H48" s="371" t="s">
         <v>856</v>
       </c>
     </row>
@@ -19097,7 +19113,7 @@
         <v>10</v>
       </c>
       <c r="G49" s="175"/>
-      <c r="H49" s="363"/>
+      <c r="H49" s="372"/>
     </row>
     <row r="50" spans="1:8" ht="16.5" thickBot="1">
       <c r="A50" s="215">
@@ -19119,7 +19135,7 @@
         <v>11</v>
       </c>
       <c r="G50" s="175"/>
-      <c r="H50" s="363"/>
+      <c r="H50" s="372"/>
     </row>
     <row r="51" spans="1:8" ht="16.5" thickBot="1">
       <c r="A51" s="218">
@@ -19141,7 +19157,7 @@
         <v>12</v>
       </c>
       <c r="G51" s="175"/>
-      <c r="H51" s="363"/>
+      <c r="H51" s="372"/>
     </row>
     <row r="52" spans="1:8" ht="16.5" thickBot="1">
       <c r="A52" s="218">
@@ -19163,7 +19179,7 @@
         <v>13</v>
       </c>
       <c r="G52" s="175"/>
-      <c r="H52" s="363"/>
+      <c r="H52" s="372"/>
     </row>
     <row r="53" spans="1:8" ht="16.5" thickBot="1">
       <c r="A53" s="218">
@@ -19185,7 +19201,7 @@
         <v>14</v>
       </c>
       <c r="G53" s="175"/>
-      <c r="H53" s="363"/>
+      <c r="H53" s="372"/>
     </row>
     <row r="54" spans="1:8" ht="16.5" thickBot="1">
       <c r="A54" s="218">
@@ -19207,7 +19223,7 @@
         <v>15</v>
       </c>
       <c r="G54" s="175"/>
-      <c r="H54" s="363"/>
+      <c r="H54" s="372"/>
     </row>
     <row r="55" spans="1:8" ht="16.5" thickBot="1">
       <c r="A55" s="218">
@@ -19229,7 +19245,7 @@
         <v>16</v>
       </c>
       <c r="G55" s="175"/>
-      <c r="H55" s="363"/>
+      <c r="H55" s="372"/>
     </row>
     <row r="56" spans="1:8" ht="16.5" thickBot="1">
       <c r="A56" s="218">
@@ -19251,7 +19267,7 @@
         <v>17</v>
       </c>
       <c r="G56" s="175"/>
-      <c r="H56" s="363"/>
+      <c r="H56" s="372"/>
     </row>
     <row r="57" spans="1:8" ht="16.5" thickBot="1">
       <c r="A57" s="220">
@@ -19273,7 +19289,7 @@
         <v>18</v>
       </c>
       <c r="G57" s="175"/>
-      <c r="H57" s="363"/>
+      <c r="H57" s="372"/>
     </row>
     <row r="58" spans="1:8" ht="16.5" thickBot="1">
       <c r="A58" s="220">
@@ -19295,7 +19311,7 @@
         <v>19</v>
       </c>
       <c r="G58" s="175"/>
-      <c r="H58" s="363"/>
+      <c r="H58" s="372"/>
     </row>
     <row r="59" spans="1:8" ht="16.5" thickBot="1">
       <c r="A59" s="222">
@@ -19317,21 +19333,21 @@
         <v>20</v>
       </c>
       <c r="G59" s="175"/>
-      <c r="H59" s="364"/>
+      <c r="H59" s="373"/>
     </row>
     <row r="60" spans="1:8" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="H48:H59"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="H40:H47"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="H3:H10"/>
     <mergeCell ref="H11:H22"/>
-    <mergeCell ref="H48:H59"/>
-    <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="H40:H47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -19898,40 +19914,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="320" t="s">
+      <c r="A1" s="324" t="s">
         <v>488</v>
       </c>
-      <c r="B1" s="321"/>
-      <c r="C1" s="321"/>
-      <c r="D1" s="321"/>
-      <c r="E1" s="321"/>
-      <c r="F1" s="321"/>
-      <c r="G1" s="321"/>
-      <c r="H1" s="322"/>
+      <c r="B1" s="325"/>
+      <c r="C1" s="325"/>
+      <c r="D1" s="325"/>
+      <c r="E1" s="325"/>
+      <c r="F1" s="325"/>
+      <c r="G1" s="325"/>
+      <c r="H1" s="326"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="323"/>
-      <c r="B2" s="324"/>
-      <c r="C2" s="324"/>
-      <c r="D2" s="324"/>
-      <c r="E2" s="324"/>
-      <c r="F2" s="324"/>
-      <c r="G2" s="324"/>
-      <c r="H2" s="325"/>
+      <c r="A2" s="327"/>
+      <c r="B2" s="328"/>
+      <c r="C2" s="328"/>
+      <c r="D2" s="328"/>
+      <c r="E2" s="328"/>
+      <c r="F2" s="328"/>
+      <c r="G2" s="328"/>
+      <c r="H2" s="329"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="326" t="s">
+      <c r="A3" s="330" t="s">
         <v>319</v>
       </c>
-      <c r="B3" s="327"/>
-      <c r="C3" s="327"/>
-      <c r="D3" s="327"/>
-      <c r="E3" s="327" t="s">
+      <c r="B3" s="331"/>
+      <c r="C3" s="331"/>
+      <c r="D3" s="331"/>
+      <c r="E3" s="331" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="327"/>
-      <c r="G3" s="327"/>
-      <c r="H3" s="328"/>
+      <c r="F3" s="331"/>
+      <c r="G3" s="331"/>
+      <c r="H3" s="332"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="12">

</xml_diff>

<commit_message>
chg: Added A-10 and AH-64 flight to Evenes airbase (In TRMA Comms & freq masterfile)
</commit_message>
<xml_diff>
--- a/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
+++ b/COMMUNICATIONS/TRMA Frequency and callsign master list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2263" uniqueCount="1352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2275" uniqueCount="1361">
   <si>
     <t>AWACS</t>
   </si>
@@ -4080,6 +4080,33 @@
   </si>
   <si>
     <t>DATALINK TRMA v1.1</t>
+  </si>
+  <si>
+    <t>PC71</t>
+  </si>
+  <si>
+    <t>PC72</t>
+  </si>
+  <si>
+    <t>PC73</t>
+  </si>
+  <si>
+    <t>PC74</t>
+  </si>
+  <si>
+    <t>0171</t>
+  </si>
+  <si>
+    <t>0172</t>
+  </si>
+  <si>
+    <t>0173</t>
+  </si>
+  <si>
+    <t>0174</t>
+  </si>
+  <si>
+    <t>Saber</t>
   </si>
 </sst>
 </file>
@@ -6730,9 +6757,25 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6742,18 +6785,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6763,6 +6794,42 @@
     <xf numFmtId="0" fontId="24" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6772,41 +6839,17 @@
     <xf numFmtId="0" fontId="24" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6835,18 +6878,6 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6934,6 +6965,33 @@
     <xf numFmtId="49" fontId="45" fillId="31" borderId="93" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="26" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6961,33 +7019,6 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7060,6 +7091,57 @@
     <xf numFmtId="0" fontId="32" fillId="20" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7078,61 +7160,6 @@
     <xf numFmtId="49" fontId="2" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7445,7 +7472,7 @@
   <sheetPr codeName="Ark1"/>
   <dimension ref="A1:AP83"/>
   <sheetViews>
-    <sheetView topLeftCell="G16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
@@ -7553,13 +7580,13 @@
       <c r="N2" s="107" t="s">
         <v>330</v>
       </c>
-      <c r="V2" s="293" t="s">
+      <c r="V2" s="296" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="293"/>
-      <c r="X2" s="293"/>
-      <c r="Y2" s="293"/>
-      <c r="Z2" s="293"/>
+      <c r="W2" s="296"/>
+      <c r="X2" s="296"/>
+      <c r="Y2" s="296"/>
+      <c r="Z2" s="296"/>
     </row>
     <row r="3" spans="1:42">
       <c r="A3" s="107" t="s">
@@ -7608,9 +7635,9 @@
       <c r="P3" t="s">
         <v>426</v>
       </c>
-      <c r="R3" s="297"/>
-      <c r="S3" s="297"/>
-      <c r="T3" s="297"/>
+      <c r="R3" s="295"/>
+      <c r="S3" s="295"/>
+      <c r="T3" s="295"/>
       <c r="V3" s="101" t="s">
         <v>328</v>
       </c>
@@ -7692,22 +7719,22 @@
       <c r="AA4" s="23"/>
       <c r="AB4" s="23"/>
       <c r="AC4" s="23"/>
-      <c r="AD4" s="293" t="s">
+      <c r="AD4" s="296" t="s">
         <v>429</v>
       </c>
-      <c r="AE4" s="293"/>
-      <c r="AF4" s="293"/>
-      <c r="AG4" s="293"/>
-      <c r="AH4" s="293"/>
-      <c r="AJ4" s="293" t="s">
+      <c r="AE4" s="296"/>
+      <c r="AF4" s="296"/>
+      <c r="AG4" s="296"/>
+      <c r="AH4" s="296"/>
+      <c r="AJ4" s="296" t="s">
         <v>1</v>
       </c>
-      <c r="AK4" s="293"/>
-      <c r="AL4" s="293"/>
-      <c r="AM4" s="293"/>
-      <c r="AN4" s="293"/>
-      <c r="AO4" s="293"/>
-      <c r="AP4" s="293"/>
+      <c r="AK4" s="296"/>
+      <c r="AL4" s="296"/>
+      <c r="AM4" s="296"/>
+      <c r="AN4" s="296"/>
+      <c r="AO4" s="296"/>
+      <c r="AP4" s="296"/>
     </row>
     <row r="5" spans="1:42" ht="15.75">
       <c r="A5" s="107" t="s">
@@ -8944,15 +8971,15 @@
       <c r="AH18" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="AJ18" s="293" t="s">
+      <c r="AJ18" s="296" t="s">
         <v>274</v>
       </c>
-      <c r="AK18" s="293"/>
-      <c r="AL18" s="293"/>
-      <c r="AM18" s="293"/>
-      <c r="AN18" s="293"/>
-      <c r="AO18" s="293"/>
-      <c r="AP18" s="293"/>
+      <c r="AK18" s="296"/>
+      <c r="AL18" s="296"/>
+      <c r="AM18" s="296"/>
+      <c r="AN18" s="296"/>
+      <c r="AO18" s="296"/>
+      <c r="AP18" s="296"/>
     </row>
     <row r="19" spans="1:42" ht="15.75">
       <c r="A19" s="107" t="s">
@@ -9085,9 +9112,9 @@
       </c>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="297"/>
-      <c r="S20" s="297"/>
-      <c r="T20" s="297"/>
+      <c r="R20" s="295"/>
+      <c r="S20" s="295"/>
+      <c r="T20" s="295"/>
       <c r="U20" s="2"/>
       <c r="V20" s="271" t="s">
         <v>1252</v>
@@ -9510,13 +9537,13 @@
       <c r="R25" s="24"/>
       <c r="S25" s="24"/>
       <c r="T25" s="24"/>
-      <c r="AD25" s="293" t="s">
+      <c r="AD25" s="296" t="s">
         <v>486</v>
       </c>
-      <c r="AE25" s="293"/>
-      <c r="AF25" s="293"/>
-      <c r="AG25" s="293"/>
-      <c r="AH25" s="293"/>
+      <c r="AE25" s="296"/>
+      <c r="AF25" s="296"/>
+      <c r="AG25" s="296"/>
+      <c r="AH25" s="296"/>
       <c r="AJ25" s="116" t="s">
         <v>555</v>
       </c>
@@ -9786,15 +9813,15 @@
       <c r="N29" s="107" t="s">
         <v>355</v>
       </c>
-      <c r="V29" s="293" t="s">
+      <c r="V29" s="296" t="s">
         <v>212</v>
       </c>
-      <c r="W29" s="293"/>
-      <c r="X29" s="293"/>
-      <c r="Y29" s="293"/>
-      <c r="Z29" s="293"/>
-      <c r="AA29" s="293"/>
-      <c r="AB29" s="293"/>
+      <c r="W29" s="296"/>
+      <c r="X29" s="296"/>
+      <c r="Y29" s="296"/>
+      <c r="Z29" s="296"/>
+      <c r="AA29" s="296"/>
+      <c r="AB29" s="296"/>
     </row>
     <row r="30" spans="1:42">
       <c r="A30" s="107"/>
@@ -9850,15 +9877,15 @@
       </c>
       <c r="AA30" s="29"/>
       <c r="AB30" s="29"/>
-      <c r="AJ30" s="293" t="s">
+      <c r="AJ30" s="296" t="s">
         <v>831</v>
       </c>
-      <c r="AK30" s="293"/>
-      <c r="AL30" s="293"/>
-      <c r="AM30" s="293"/>
-      <c r="AN30" s="293"/>
-      <c r="AO30" s="293"/>
-      <c r="AP30" s="293"/>
+      <c r="AK30" s="296"/>
+      <c r="AL30" s="296"/>
+      <c r="AM30" s="296"/>
+      <c r="AN30" s="296"/>
+      <c r="AO30" s="296"/>
+      <c r="AP30" s="296"/>
     </row>
     <row r="31" spans="1:42">
       <c r="B31" s="24"/>
@@ -9945,15 +9972,15 @@
       <c r="AJ34" s="23"/>
     </row>
     <row r="37" spans="22:36">
-      <c r="V37" s="293" t="s">
+      <c r="V37" s="296" t="s">
         <v>9</v>
       </c>
-      <c r="W37" s="293"/>
-      <c r="X37" s="293"/>
-      <c r="Y37" s="293"/>
-      <c r="Z37" s="293"/>
-      <c r="AA37" s="293"/>
-      <c r="AB37" s="293"/>
+      <c r="W37" s="296"/>
+      <c r="X37" s="296"/>
+      <c r="Y37" s="296"/>
+      <c r="Z37" s="296"/>
+      <c r="AA37" s="296"/>
+      <c r="AB37" s="296"/>
     </row>
     <row r="38" spans="22:36">
       <c r="V38" s="29" t="s">
@@ -9973,11 +10000,11 @@
       </c>
       <c r="AA38" s="29"/>
       <c r="AB38" s="29"/>
-      <c r="AD38" s="298" t="s">
+      <c r="AD38" s="297" t="s">
         <v>260</v>
       </c>
-      <c r="AE38" s="299"/>
-      <c r="AF38" s="300"/>
+      <c r="AE38" s="298"/>
+      <c r="AF38" s="299"/>
     </row>
     <row r="39" spans="22:36">
       <c r="V39" s="3" t="s">
@@ -10014,15 +10041,15 @@
       <c r="AF41" s="3"/>
     </row>
     <row r="42" spans="22:36">
-      <c r="V42" s="293" t="s">
+      <c r="V42" s="296" t="s">
         <v>244</v>
       </c>
-      <c r="W42" s="293"/>
-      <c r="X42" s="293"/>
-      <c r="Y42" s="293"/>
-      <c r="Z42" s="293"/>
-      <c r="AA42" s="293"/>
-      <c r="AB42" s="293"/>
+      <c r="W42" s="296"/>
+      <c r="X42" s="296"/>
+      <c r="Y42" s="296"/>
+      <c r="Z42" s="296"/>
+      <c r="AA42" s="296"/>
+      <c r="AB42" s="296"/>
       <c r="AD42" s="3" t="s">
         <v>254</v>
       </c>
@@ -10092,15 +10119,15 @@
       <c r="AF47" s="3"/>
     </row>
     <row r="48" spans="22:36">
-      <c r="V48" s="294" t="s">
+      <c r="V48" s="300" t="s">
         <v>473</v>
       </c>
-      <c r="W48" s="295"/>
-      <c r="X48" s="295"/>
-      <c r="Y48" s="295"/>
-      <c r="Z48" s="295"/>
-      <c r="AA48" s="295"/>
-      <c r="AB48" s="296"/>
+      <c r="W48" s="301"/>
+      <c r="X48" s="301"/>
+      <c r="Y48" s="301"/>
+      <c r="Z48" s="301"/>
+      <c r="AA48" s="301"/>
+      <c r="AB48" s="302"/>
       <c r="AD48" s="3" t="s">
         <v>261</v>
       </c>
@@ -10710,6 +10737,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="V42:AB42"/>
+    <mergeCell ref="AD4:AH4"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="V48:AB48"/>
+    <mergeCell ref="V37:AB37"/>
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="AJ4:AP4"/>
@@ -10718,11 +10750,6 @@
     <mergeCell ref="V29:AB29"/>
     <mergeCell ref="AD25:AH25"/>
     <mergeCell ref="AJ30:AP30"/>
-    <mergeCell ref="V42:AB42"/>
-    <mergeCell ref="AD4:AH4"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="V48:AB48"/>
-    <mergeCell ref="V37:AB37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10750,40 +10777,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="391" t="s">
+      <c r="A1" s="393" t="s">
         <v>487</v>
       </c>
-      <c r="B1" s="392"/>
-      <c r="C1" s="392"/>
-      <c r="D1" s="392"/>
-      <c r="E1" s="392"/>
-      <c r="F1" s="392"/>
-      <c r="G1" s="392"/>
-      <c r="H1" s="393"/>
+      <c r="B1" s="394"/>
+      <c r="C1" s="394"/>
+      <c r="D1" s="394"/>
+      <c r="E1" s="394"/>
+      <c r="F1" s="394"/>
+      <c r="G1" s="394"/>
+      <c r="H1" s="395"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A2" s="394"/>
-      <c r="B2" s="395"/>
-      <c r="C2" s="395"/>
-      <c r="D2" s="395"/>
-      <c r="E2" s="395"/>
-      <c r="F2" s="395"/>
-      <c r="G2" s="395"/>
-      <c r="H2" s="396"/>
+      <c r="A2" s="396"/>
+      <c r="B2" s="397"/>
+      <c r="C2" s="397"/>
+      <c r="D2" s="397"/>
+      <c r="E2" s="397"/>
+      <c r="F2" s="397"/>
+      <c r="G2" s="397"/>
+      <c r="H2" s="398"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="397" t="s">
+      <c r="A3" s="399" t="s">
         <v>751</v>
       </c>
-      <c r="B3" s="398"/>
-      <c r="C3" s="398"/>
-      <c r="D3" s="399"/>
-      <c r="E3" s="397" t="s">
+      <c r="B3" s="400"/>
+      <c r="C3" s="400"/>
+      <c r="D3" s="401"/>
+      <c r="E3" s="399" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="398"/>
-      <c r="G3" s="398"/>
-      <c r="H3" s="399"/>
+      <c r="F3" s="400"/>
+      <c r="G3" s="400"/>
+      <c r="H3" s="401"/>
     </row>
     <row r="4" spans="1:8" ht="16.5">
       <c r="A4" s="166">
@@ -11256,18 +11283,18 @@
       <c r="H24" s="146"/>
     </row>
     <row r="25" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A25" s="400" t="s">
+      <c r="A25" s="402" t="s">
         <v>314</v>
       </c>
-      <c r="B25" s="401"/>
-      <c r="C25" s="401"/>
-      <c r="D25" s="402"/>
-      <c r="E25" s="400" t="s">
+      <c r="B25" s="403"/>
+      <c r="C25" s="403"/>
+      <c r="D25" s="404"/>
+      <c r="E25" s="402" t="s">
         <v>801</v>
       </c>
-      <c r="F25" s="401"/>
-      <c r="G25" s="401"/>
-      <c r="H25" s="402"/>
+      <c r="F25" s="403"/>
+      <c r="G25" s="403"/>
+      <c r="H25" s="404"/>
     </row>
     <row r="26" spans="1:8" ht="16.5">
       <c r="A26" s="155">
@@ -11682,40 +11709,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="403" t="s">
+      <c r="A1" s="422" t="s">
         <v>326</v>
       </c>
-      <c r="B1" s="403"/>
-      <c r="C1" s="403"/>
-      <c r="D1" s="403"/>
-      <c r="E1" s="403"/>
-      <c r="F1" s="403"/>
-      <c r="G1" s="403"/>
-      <c r="H1" s="403"/>
+      <c r="B1" s="422"/>
+      <c r="C1" s="422"/>
+      <c r="D1" s="422"/>
+      <c r="E1" s="422"/>
+      <c r="F1" s="422"/>
+      <c r="G1" s="422"/>
+      <c r="H1" s="422"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="404"/>
-      <c r="B2" s="404"/>
-      <c r="C2" s="404"/>
-      <c r="D2" s="404"/>
-      <c r="E2" s="404"/>
-      <c r="F2" s="404"/>
-      <c r="G2" s="404"/>
-      <c r="H2" s="404"/>
+      <c r="A2" s="423"/>
+      <c r="B2" s="423"/>
+      <c r="C2" s="423"/>
+      <c r="D2" s="423"/>
+      <c r="E2" s="423"/>
+      <c r="F2" s="423"/>
+      <c r="G2" s="423"/>
+      <c r="H2" s="423"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1">
-      <c r="A3" s="405" t="s">
+      <c r="A3" s="424" t="s">
         <v>227</v>
       </c>
-      <c r="B3" s="406"/>
-      <c r="C3" s="407"/>
-      <c r="D3" s="408"/>
-      <c r="E3" s="405" t="s">
+      <c r="B3" s="425"/>
+      <c r="C3" s="426"/>
+      <c r="D3" s="427"/>
+      <c r="E3" s="424" t="s">
         <v>228</v>
       </c>
-      <c r="F3" s="406"/>
-      <c r="G3" s="407"/>
-      <c r="H3" s="408"/>
+      <c r="F3" s="425"/>
+      <c r="G3" s="426"/>
+      <c r="H3" s="427"/>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="31">
@@ -12008,114 +12035,114 @@
       <c r="H24" s="59"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1">
-      <c r="A25" s="405" t="s">
+      <c r="A25" s="424" t="s">
         <v>289</v>
       </c>
-      <c r="B25" s="406"/>
-      <c r="C25" s="407"/>
-      <c r="D25" s="408"/>
-      <c r="E25" s="405" t="s">
+      <c r="B25" s="425"/>
+      <c r="C25" s="426"/>
+      <c r="D25" s="427"/>
+      <c r="E25" s="424" t="s">
         <v>290</v>
       </c>
-      <c r="F25" s="406"/>
-      <c r="G25" s="407"/>
-      <c r="H25" s="408"/>
+      <c r="F25" s="425"/>
+      <c r="G25" s="426"/>
+      <c r="H25" s="427"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1">
       <c r="A26" s="35" t="s">
         <v>291</v>
       </c>
-      <c r="B26" s="409"/>
-      <c r="C26" s="410"/>
-      <c r="D26" s="411"/>
+      <c r="B26" s="411"/>
+      <c r="C26" s="412"/>
+      <c r="D26" s="413"/>
       <c r="E26" s="31" t="s">
         <v>292</v>
       </c>
-      <c r="F26" s="412"/>
-      <c r="G26" s="413"/>
-      <c r="H26" s="414"/>
+      <c r="F26" s="419"/>
+      <c r="G26" s="420"/>
+      <c r="H26" s="421"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" thickBot="1">
       <c r="A27" s="43" t="s">
         <v>293</v>
       </c>
-      <c r="B27" s="415"/>
-      <c r="C27" s="416"/>
+      <c r="B27" s="414"/>
+      <c r="C27" s="415"/>
       <c r="D27" s="417"/>
       <c r="E27" s="35" t="s">
         <v>294</v>
       </c>
-      <c r="F27" s="409"/>
-      <c r="G27" s="410"/>
+      <c r="F27" s="411"/>
+      <c r="G27" s="412"/>
       <c r="H27" s="418"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" thickBot="1">
       <c r="A28" s="35" t="s">
         <v>295</v>
       </c>
-      <c r="B28" s="409"/>
-      <c r="C28" s="410"/>
-      <c r="D28" s="411"/>
+      <c r="B28" s="411"/>
+      <c r="C28" s="412"/>
+      <c r="D28" s="413"/>
       <c r="E28" s="43" t="s">
         <v>296</v>
       </c>
-      <c r="F28" s="415"/>
-      <c r="G28" s="416"/>
-      <c r="H28" s="419"/>
+      <c r="F28" s="414"/>
+      <c r="G28" s="415"/>
+      <c r="H28" s="416"/>
     </row>
     <row r="29" spans="1:8" ht="18.75" thickBot="1">
       <c r="A29" s="43" t="s">
         <v>297</v>
       </c>
-      <c r="B29" s="415"/>
-      <c r="C29" s="416"/>
+      <c r="B29" s="414"/>
+      <c r="C29" s="415"/>
       <c r="D29" s="417"/>
       <c r="E29" s="35" t="s">
         <v>298</v>
       </c>
-      <c r="F29" s="409"/>
-      <c r="G29" s="410"/>
+      <c r="F29" s="411"/>
+      <c r="G29" s="412"/>
       <c r="H29" s="418"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1">
       <c r="A30" s="35" t="s">
         <v>299</v>
       </c>
-      <c r="B30" s="409"/>
-      <c r="C30" s="410"/>
-      <c r="D30" s="411"/>
+      <c r="B30" s="411"/>
+      <c r="C30" s="412"/>
+      <c r="D30" s="413"/>
       <c r="E30" s="43" t="s">
         <v>300</v>
       </c>
-      <c r="F30" s="415"/>
-      <c r="G30" s="416"/>
-      <c r="H30" s="419"/>
+      <c r="F30" s="414"/>
+      <c r="G30" s="415"/>
+      <c r="H30" s="416"/>
     </row>
     <row r="31" spans="1:8" ht="18.75" thickBot="1">
       <c r="A31" s="43" t="s">
         <v>301</v>
       </c>
-      <c r="B31" s="415"/>
-      <c r="C31" s="416"/>
+      <c r="B31" s="414"/>
+      <c r="C31" s="415"/>
       <c r="D31" s="417"/>
       <c r="E31" s="35" t="s">
         <v>302</v>
       </c>
-      <c r="F31" s="409"/>
-      <c r="G31" s="410"/>
+      <c r="F31" s="411"/>
+      <c r="G31" s="412"/>
       <c r="H31" s="418"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" thickBot="1">
       <c r="A32" s="35" t="s">
         <v>303</v>
       </c>
-      <c r="B32" s="409"/>
-      <c r="C32" s="410"/>
-      <c r="D32" s="411"/>
+      <c r="B32" s="411"/>
+      <c r="C32" s="412"/>
+      <c r="D32" s="413"/>
       <c r="E32" s="43"/>
-      <c r="F32" s="415"/>
-      <c r="G32" s="416"/>
-      <c r="H32" s="419" t="s">
+      <c r="F32" s="414"/>
+      <c r="G32" s="415"/>
+      <c r="H32" s="416" t="s">
         <v>242</v>
       </c>
     </row>
@@ -12123,12 +12150,12 @@
       <c r="A33" s="43" t="s">
         <v>304</v>
       </c>
-      <c r="B33" s="415"/>
-      <c r="C33" s="416"/>
+      <c r="B33" s="414"/>
+      <c r="C33" s="415"/>
       <c r="D33" s="417"/>
       <c r="E33" s="35"/>
-      <c r="F33" s="409"/>
-      <c r="G33" s="410"/>
+      <c r="F33" s="411"/>
+      <c r="G33" s="412"/>
       <c r="H33" s="418" t="s">
         <v>284</v>
       </c>
@@ -12137,13 +12164,13 @@
       <c r="A34" s="35" t="s">
         <v>305</v>
       </c>
-      <c r="B34" s="409"/>
-      <c r="C34" s="410"/>
-      <c r="D34" s="411"/>
+      <c r="B34" s="411"/>
+      <c r="C34" s="412"/>
+      <c r="D34" s="413"/>
       <c r="E34" s="43"/>
-      <c r="F34" s="415"/>
-      <c r="G34" s="416"/>
-      <c r="H34" s="419" t="s">
+      <c r="F34" s="414"/>
+      <c r="G34" s="415"/>
+      <c r="H34" s="416" t="s">
         <v>285</v>
       </c>
     </row>
@@ -12151,12 +12178,12 @@
       <c r="A35" s="43" t="s">
         <v>306</v>
       </c>
-      <c r="B35" s="415"/>
-      <c r="C35" s="416"/>
+      <c r="B35" s="414"/>
+      <c r="C35" s="415"/>
       <c r="D35" s="417"/>
       <c r="E35" s="35"/>
-      <c r="F35" s="409"/>
-      <c r="G35" s="410"/>
+      <c r="F35" s="411"/>
+      <c r="G35" s="412"/>
       <c r="H35" s="418" t="s">
         <v>286</v>
       </c>
@@ -12165,13 +12192,13 @@
       <c r="A36" s="35" t="s">
         <v>307</v>
       </c>
-      <c r="B36" s="409"/>
-      <c r="C36" s="410"/>
-      <c r="D36" s="411"/>
+      <c r="B36" s="411"/>
+      <c r="C36" s="412"/>
+      <c r="D36" s="413"/>
       <c r="E36" s="43"/>
-      <c r="F36" s="415"/>
-      <c r="G36" s="416"/>
-      <c r="H36" s="419" t="s">
+      <c r="F36" s="414"/>
+      <c r="G36" s="415"/>
+      <c r="H36" s="416" t="s">
         <v>287</v>
       </c>
     </row>
@@ -12179,12 +12206,12 @@
       <c r="A37" s="43" t="s">
         <v>308</v>
       </c>
-      <c r="B37" s="415"/>
-      <c r="C37" s="416"/>
+      <c r="B37" s="414"/>
+      <c r="C37" s="415"/>
       <c r="D37" s="417"/>
       <c r="E37" s="35"/>
-      <c r="F37" s="409"/>
-      <c r="G37" s="410"/>
+      <c r="F37" s="411"/>
+      <c r="G37" s="412"/>
       <c r="H37" s="418" t="s">
         <v>288</v>
       </c>
@@ -12193,13 +12220,13 @@
       <c r="A38" s="35" t="s">
         <v>309</v>
       </c>
-      <c r="B38" s="409"/>
-      <c r="C38" s="410"/>
-      <c r="D38" s="411"/>
+      <c r="B38" s="411"/>
+      <c r="C38" s="412"/>
+      <c r="D38" s="413"/>
       <c r="E38" s="43"/>
-      <c r="F38" s="415"/>
-      <c r="G38" s="416"/>
-      <c r="H38" s="419" t="s">
+      <c r="F38" s="414"/>
+      <c r="G38" s="415"/>
+      <c r="H38" s="416" t="s">
         <v>241</v>
       </c>
     </row>
@@ -12207,12 +12234,12 @@
       <c r="A39" s="43" t="s">
         <v>310</v>
       </c>
-      <c r="B39" s="415"/>
-      <c r="C39" s="416"/>
+      <c r="B39" s="414"/>
+      <c r="C39" s="415"/>
       <c r="D39" s="417"/>
       <c r="E39" s="35"/>
-      <c r="F39" s="409"/>
-      <c r="G39" s="410"/>
+      <c r="F39" s="411"/>
+      <c r="G39" s="412"/>
       <c r="H39" s="418" t="s">
         <v>242</v>
       </c>
@@ -12221,28 +12248,57 @@
       <c r="A40" s="35" t="s">
         <v>311</v>
       </c>
-      <c r="B40" s="409"/>
-      <c r="C40" s="410"/>
-      <c r="D40" s="411"/>
+      <c r="B40" s="411"/>
+      <c r="C40" s="412"/>
+      <c r="D40" s="413"/>
       <c r="E40" s="43"/>
-      <c r="F40" s="415"/>
-      <c r="G40" s="416"/>
-      <c r="H40" s="419"/>
+      <c r="F40" s="414"/>
+      <c r="G40" s="415"/>
+      <c r="H40" s="416"/>
     </row>
     <row r="41" spans="1:8" ht="18.75" thickBot="1">
       <c r="A41" s="55" t="s">
         <v>312</v>
       </c>
-      <c r="B41" s="420"/>
-      <c r="C41" s="421"/>
-      <c r="D41" s="422"/>
+      <c r="B41" s="405"/>
+      <c r="C41" s="406"/>
+      <c r="D41" s="407"/>
       <c r="E41" s="60"/>
-      <c r="F41" s="423"/>
-      <c r="G41" s="424"/>
-      <c r="H41" s="425"/>
+      <c r="F41" s="408"/>
+      <c r="G41" s="409"/>
+      <c r="H41" s="410"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:H37"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="F41:H41"/>
     <mergeCell ref="B38:D38"/>
@@ -12251,35 +12307,6 @@
     <mergeCell ref="F39:H39"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="F40:H40"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12290,8 +12317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AP66"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AA38" sqref="AA38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -12335,55 +12362,55 @@
       </c>
     </row>
     <row r="2" spans="2:42">
-      <c r="B2" s="293" t="s">
+      <c r="B2" s="296" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="293"/>
-      <c r="D2" s="293"/>
-      <c r="E2" s="293"/>
-      <c r="F2" s="293"/>
-      <c r="H2" s="293" t="s">
+      <c r="C2" s="296"/>
+      <c r="D2" s="296"/>
+      <c r="E2" s="296"/>
+      <c r="F2" s="296"/>
+      <c r="H2" s="296" t="s">
         <v>1055</v>
       </c>
-      <c r="I2" s="293"/>
-      <c r="J2" s="293"/>
-      <c r="K2" s="293"/>
-      <c r="L2" s="293"/>
-      <c r="N2" s="293" t="s">
+      <c r="I2" s="296"/>
+      <c r="J2" s="296"/>
+      <c r="K2" s="296"/>
+      <c r="L2" s="296"/>
+      <c r="N2" s="296" t="s">
         <v>1054</v>
       </c>
-      <c r="O2" s="293"/>
-      <c r="P2" s="293"/>
-      <c r="Q2" s="293"/>
-      <c r="R2" s="293"/>
-      <c r="T2" s="293" t="s">
+      <c r="O2" s="296"/>
+      <c r="P2" s="296"/>
+      <c r="Q2" s="296"/>
+      <c r="R2" s="296"/>
+      <c r="T2" s="296" t="s">
         <v>236</v>
       </c>
-      <c r="U2" s="293"/>
-      <c r="V2" s="293"/>
-      <c r="W2" s="293"/>
-      <c r="X2" s="293"/>
-      <c r="Z2" s="293" t="s">
+      <c r="U2" s="296"/>
+      <c r="V2" s="296"/>
+      <c r="W2" s="296"/>
+      <c r="X2" s="296"/>
+      <c r="Z2" s="296" t="s">
         <v>246</v>
       </c>
-      <c r="AA2" s="293"/>
-      <c r="AB2" s="293"/>
-      <c r="AC2" s="293"/>
-      <c r="AD2" s="293"/>
-      <c r="AF2" s="293" t="s">
+      <c r="AA2" s="296"/>
+      <c r="AB2" s="296"/>
+      <c r="AC2" s="296"/>
+      <c r="AD2" s="296"/>
+      <c r="AF2" s="296" t="s">
         <v>317</v>
       </c>
-      <c r="AG2" s="293"/>
-      <c r="AH2" s="293"/>
-      <c r="AI2" s="293"/>
-      <c r="AJ2" s="293"/>
-      <c r="AL2" s="293" t="s">
+      <c r="AG2" s="296"/>
+      <c r="AH2" s="296"/>
+      <c r="AI2" s="296"/>
+      <c r="AJ2" s="296"/>
+      <c r="AL2" s="296" t="s">
         <v>491</v>
       </c>
-      <c r="AM2" s="293"/>
-      <c r="AN2" s="293"/>
-      <c r="AO2" s="293"/>
-      <c r="AP2" s="293"/>
+      <c r="AM2" s="296"/>
+      <c r="AN2" s="296"/>
+      <c r="AO2" s="296"/>
+      <c r="AP2" s="296"/>
     </row>
     <row r="3" spans="2:42">
       <c r="B3" s="101" t="s">
@@ -13531,6 +13558,19 @@
       <c r="V21" s="246"/>
       <c r="W21" s="246"/>
       <c r="X21" s="246"/>
+      <c r="AF21" s="3" t="s">
+        <v>1360</v>
+      </c>
+      <c r="AG21" s="3" t="s">
+        <v>905</v>
+      </c>
+      <c r="AH21" s="3">
+        <v>551</v>
+      </c>
+      <c r="AI21" s="3">
+        <v>551</v>
+      </c>
+      <c r="AJ21" s="3"/>
     </row>
     <row r="22" spans="1:40">
       <c r="B22" s="3"/>
@@ -13581,6 +13621,11 @@
       <c r="X22" s="104" t="s">
         <v>1319</v>
       </c>
+      <c r="AF22" s="3"/>
+      <c r="AG22" s="3"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="3"/>
     </row>
     <row r="23" spans="1:40">
       <c r="D23" s="59"/>
@@ -13606,6 +13651,11 @@
       <c r="X23" s="104" t="s">
         <v>1320</v>
       </c>
+      <c r="AF23" s="3"/>
+      <c r="AG23" s="3"/>
+      <c r="AH23" s="3"/>
+      <c r="AI23" s="3"/>
+      <c r="AJ23" s="3"/>
     </row>
     <row r="24" spans="1:40">
       <c r="D24" s="59"/>
@@ -13651,6 +13701,11 @@
       <c r="X24" s="104" t="s">
         <v>1321</v>
       </c>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="3"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
     </row>
     <row r="25" spans="1:40">
       <c r="H25" s="3"/>
@@ -13686,6 +13741,11 @@
       <c r="X25" s="104" t="s">
         <v>1322</v>
       </c>
+      <c r="AF25" s="3"/>
+      <c r="AG25" s="3"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="3"/>
+      <c r="AJ25" s="3"/>
     </row>
     <row r="26" spans="1:40">
       <c r="H26" s="3"/>
@@ -13879,7 +13939,11 @@
       <c r="R31" s="104" t="s">
         <v>1123</v>
       </c>
-      <c r="X31" s="59"/>
+      <c r="T31" s="246"/>
+      <c r="U31" s="246"/>
+      <c r="V31" s="246"/>
+      <c r="W31" s="246"/>
+      <c r="X31" s="246"/>
     </row>
     <row r="32" spans="1:40">
       <c r="H32" s="3"/>
@@ -13904,7 +13968,21 @@
       <c r="R32" s="104" t="s">
         <v>1122</v>
       </c>
-      <c r="X32" s="59"/>
+      <c r="T32" s="292" t="s">
+        <v>495</v>
+      </c>
+      <c r="U32" s="3" t="s">
+        <v>905</v>
+      </c>
+      <c r="V32" s="269">
+        <v>171</v>
+      </c>
+      <c r="W32" s="269" t="s">
+        <v>1352</v>
+      </c>
+      <c r="X32" s="104" t="s">
+        <v>1356</v>
+      </c>
     </row>
     <row r="33" spans="2:24">
       <c r="H33" s="245"/>
@@ -13917,7 +13995,17 @@
       <c r="P33" s="246"/>
       <c r="Q33" s="245"/>
       <c r="R33" s="246"/>
-      <c r="X33" s="59"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="269">
+        <v>172</v>
+      </c>
+      <c r="W33" s="269" t="s">
+        <v>1353</v>
+      </c>
+      <c r="X33" s="104" t="s">
+        <v>1357</v>
+      </c>
     </row>
     <row r="34" spans="2:24">
       <c r="H34" s="3" t="s">
@@ -13950,7 +14038,17 @@
       <c r="R34" s="104" t="s">
         <v>1121</v>
       </c>
-      <c r="X34" s="59"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="269">
+        <v>173</v>
+      </c>
+      <c r="W34" s="269" t="s">
+        <v>1354</v>
+      </c>
+      <c r="X34" s="104" t="s">
+        <v>1358</v>
+      </c>
     </row>
     <row r="35" spans="2:24">
       <c r="H35" s="3"/>
@@ -13975,7 +14073,17 @@
       <c r="R35" s="104" t="s">
         <v>1120</v>
       </c>
-      <c r="X35" s="59"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+      <c r="V35" s="269">
+        <v>174</v>
+      </c>
+      <c r="W35" s="269" t="s">
+        <v>1355</v>
+      </c>
+      <c r="X35" s="104" t="s">
+        <v>1359</v>
+      </c>
     </row>
     <row r="36" spans="2:24">
       <c r="H36" s="3"/>
@@ -14017,20 +14125,20 @@
       <c r="X39" s="59"/>
     </row>
     <row r="41" spans="2:24">
-      <c r="B41" s="293" t="s">
+      <c r="B41" s="296" t="s">
         <v>697</v>
       </c>
-      <c r="C41" s="293"/>
-      <c r="D41" s="293"/>
-      <c r="E41" s="293"/>
-      <c r="F41" s="293"/>
-      <c r="H41" s="293" t="s">
+      <c r="C41" s="296"/>
+      <c r="D41" s="296"/>
+      <c r="E41" s="296"/>
+      <c r="F41" s="296"/>
+      <c r="H41" s="296" t="s">
         <v>750</v>
       </c>
-      <c r="I41" s="293"/>
-      <c r="J41" s="293"/>
-      <c r="K41" s="293"/>
-      <c r="L41" s="293"/>
+      <c r="I41" s="296"/>
+      <c r="J41" s="296"/>
+      <c r="K41" s="296"/>
+      <c r="L41" s="296"/>
     </row>
     <row r="42" spans="2:24">
       <c r="B42" s="101" t="s">
@@ -14523,46 +14631,46 @@
       <c r="C63" t="s">
         <v>929</v>
       </c>
-      <c r="D63" s="427">
+      <c r="D63" s="294">
         <v>951</v>
       </c>
       <c r="E63" t="s">
         <v>1347</v>
       </c>
-      <c r="F63" s="426">
+      <c r="F63" s="293">
         <v>11451</v>
       </c>
     </row>
     <row r="64" spans="2:12">
-      <c r="D64" s="427">
+      <c r="D64" s="294">
         <v>952</v>
       </c>
       <c r="E64" t="s">
         <v>1348</v>
       </c>
-      <c r="F64" s="426">
+      <c r="F64" s="293">
         <v>11452</v>
       </c>
     </row>
     <row r="65" spans="4:6">
-      <c r="D65" s="427">
+      <c r="D65" s="294">
         <v>953</v>
       </c>
       <c r="E65" t="s">
         <v>1349</v>
       </c>
-      <c r="F65" s="426">
+      <c r="F65" s="293">
         <v>11453</v>
       </c>
     </row>
     <row r="66" spans="4:6">
-      <c r="D66" s="427">
+      <c r="D66" s="294">
         <v>954</v>
       </c>
       <c r="E66" t="s">
         <v>1350</v>
       </c>
-      <c r="F66" s="426">
+      <c r="F66" s="293">
         <v>11454</v>
       </c>
     </row>
@@ -14590,7 +14698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
@@ -14617,39 +14725,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27" customHeight="1" thickBot="1">
-      <c r="A1" s="313" t="s">
+      <c r="A1" s="315" t="s">
         <v>1351</v>
       </c>
-      <c r="B1" s="314"/>
-      <c r="C1" s="314"/>
-      <c r="D1" s="314"/>
-      <c r="E1" s="314"/>
-      <c r="F1" s="314"/>
-      <c r="G1" s="314"/>
-      <c r="H1" s="314"/>
-      <c r="I1" s="314"/>
-      <c r="J1" s="314"/>
-      <c r="K1" s="314"/>
-      <c r="L1" s="315"/>
+      <c r="B1" s="316"/>
+      <c r="C1" s="316"/>
+      <c r="D1" s="316"/>
+      <c r="E1" s="316"/>
+      <c r="F1" s="316"/>
+      <c r="G1" s="316"/>
+      <c r="H1" s="316"/>
+      <c r="I1" s="316"/>
+      <c r="J1" s="316"/>
+      <c r="K1" s="316"/>
+      <c r="L1" s="317"/>
     </row>
     <row r="2" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A2" s="310" t="s">
+      <c r="A2" s="312" t="s">
         <v>1146</v>
       </c>
-      <c r="B2" s="311"/>
-      <c r="C2" s="312"/>
+      <c r="B2" s="313"/>
+      <c r="C2" s="314"/>
       <c r="D2" s="258"/>
-      <c r="E2" s="310" t="s">
+      <c r="E2" s="312" t="s">
         <v>1055</v>
       </c>
-      <c r="F2" s="311"/>
-      <c r="G2" s="312"/>
+      <c r="F2" s="313"/>
+      <c r="G2" s="314"/>
       <c r="H2" s="258"/>
-      <c r="I2" s="310" t="s">
+      <c r="I2" s="312" t="s">
         <v>1054</v>
       </c>
-      <c r="J2" s="311"/>
-      <c r="K2" s="312"/>
+      <c r="J2" s="313"/>
+      <c r="K2" s="314"/>
       <c r="L2" s="122"/>
     </row>
     <row r="3" spans="1:12" ht="19.5" thickBot="1">
@@ -14685,7 +14793,7 @@
       <c r="L3" s="122"/>
     </row>
     <row r="4" spans="1:12" ht="18.75">
-      <c r="A4" s="316" t="s">
+      <c r="A4" s="306" t="s">
         <v>325</v>
       </c>
       <c r="B4" s="132" t="s">
@@ -14695,7 +14803,7 @@
         <v>705</v>
       </c>
       <c r="D4" s="253"/>
-      <c r="E4" s="307" t="s">
+      <c r="E4" s="309" t="s">
         <v>975</v>
       </c>
       <c r="F4" s="132" t="s">
@@ -14705,7 +14813,7 @@
         <v>1028</v>
       </c>
       <c r="H4" s="125"/>
-      <c r="I4" s="307" t="s">
+      <c r="I4" s="309" t="s">
         <v>1057</v>
       </c>
       <c r="J4" s="132" t="s">
@@ -14717,7 +14825,7 @@
       <c r="L4" s="122"/>
     </row>
     <row r="5" spans="1:12" ht="18.75">
-      <c r="A5" s="317"/>
+      <c r="A5" s="307"/>
       <c r="B5" s="131" t="s">
         <v>322</v>
       </c>
@@ -14725,7 +14833,7 @@
         <v>706</v>
       </c>
       <c r="D5" s="253"/>
-      <c r="E5" s="308"/>
+      <c r="E5" s="310"/>
       <c r="F5" s="131" t="s">
         <v>1002</v>
       </c>
@@ -14733,7 +14841,7 @@
         <v>1029</v>
       </c>
       <c r="H5" s="125"/>
-      <c r="I5" s="308"/>
+      <c r="I5" s="310"/>
       <c r="J5" s="131" t="s">
         <v>1092</v>
       </c>
@@ -14743,7 +14851,7 @@
       <c r="L5" s="122"/>
     </row>
     <row r="6" spans="1:12" ht="18.75">
-      <c r="A6" s="317"/>
+      <c r="A6" s="307"/>
       <c r="B6" s="131" t="s">
         <v>323</v>
       </c>
@@ -14751,7 +14859,7 @@
         <v>707</v>
       </c>
       <c r="D6" s="253"/>
-      <c r="E6" s="308"/>
+      <c r="E6" s="310"/>
       <c r="F6" s="131" t="s">
         <v>1003</v>
       </c>
@@ -14759,7 +14867,7 @@
         <v>1030</v>
       </c>
       <c r="H6" s="125"/>
-      <c r="I6" s="308"/>
+      <c r="I6" s="310"/>
       <c r="J6" s="131" t="s">
         <v>1093</v>
       </c>
@@ -14769,7 +14877,7 @@
       <c r="L6" s="122"/>
     </row>
     <row r="7" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A7" s="318"/>
+      <c r="A7" s="308"/>
       <c r="B7" s="135" t="s">
         <v>324</v>
       </c>
@@ -14777,7 +14885,7 @@
         <v>708</v>
       </c>
       <c r="D7" s="253"/>
-      <c r="E7" s="309"/>
+      <c r="E7" s="311"/>
       <c r="F7" s="135" t="s">
         <v>1004</v>
       </c>
@@ -14785,7 +14893,7 @@
         <v>1031</v>
       </c>
       <c r="H7" s="125"/>
-      <c r="I7" s="309"/>
+      <c r="I7" s="311"/>
       <c r="J7" s="135" t="s">
         <v>1094</v>
       </c>
@@ -14795,7 +14903,7 @@
       <c r="L7" s="122"/>
     </row>
     <row r="8" spans="1:12" ht="18.75">
-      <c r="A8" s="316" t="s">
+      <c r="A8" s="306" t="s">
         <v>667</v>
       </c>
       <c r="B8" s="132" t="s">
@@ -14805,7 +14913,7 @@
         <v>709</v>
       </c>
       <c r="D8" s="253"/>
-      <c r="E8" s="307" t="s">
+      <c r="E8" s="309" t="s">
         <v>974</v>
       </c>
       <c r="F8" s="132" t="s">
@@ -14815,7 +14923,7 @@
         <v>1032</v>
       </c>
       <c r="H8" s="125"/>
-      <c r="I8" s="307" t="s">
+      <c r="I8" s="309" t="s">
         <v>1058</v>
       </c>
       <c r="J8" s="132" t="s">
@@ -14827,7 +14935,7 @@
       <c r="L8" s="122"/>
     </row>
     <row r="9" spans="1:12" ht="18.75">
-      <c r="A9" s="317"/>
+      <c r="A9" s="307"/>
       <c r="B9" s="131" t="s">
         <v>658</v>
       </c>
@@ -14835,7 +14943,7 @@
         <v>710</v>
       </c>
       <c r="D9" s="253"/>
-      <c r="E9" s="308"/>
+      <c r="E9" s="310"/>
       <c r="F9" s="131" t="s">
         <v>1006</v>
       </c>
@@ -14843,7 +14951,7 @@
         <v>1033</v>
       </c>
       <c r="H9" s="125"/>
-      <c r="I9" s="308"/>
+      <c r="I9" s="310"/>
       <c r="J9" s="131" t="s">
         <v>1095</v>
       </c>
@@ -14853,7 +14961,7 @@
       <c r="L9" s="122"/>
     </row>
     <row r="10" spans="1:12" ht="18.75">
-      <c r="A10" s="317"/>
+      <c r="A10" s="307"/>
       <c r="B10" s="131" t="s">
         <v>659</v>
       </c>
@@ -14861,7 +14969,7 @@
         <v>711</v>
       </c>
       <c r="D10" s="253"/>
-      <c r="E10" s="308"/>
+      <c r="E10" s="310"/>
       <c r="F10" s="131" t="s">
         <v>1008</v>
       </c>
@@ -14869,7 +14977,7 @@
         <v>1034</v>
       </c>
       <c r="H10" s="125"/>
-      <c r="I10" s="308"/>
+      <c r="I10" s="310"/>
       <c r="J10" s="131" t="s">
         <v>1096</v>
       </c>
@@ -14879,7 +14987,7 @@
       <c r="L10" s="122"/>
     </row>
     <row r="11" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A11" s="318"/>
+      <c r="A11" s="308"/>
       <c r="B11" s="135" t="s">
         <v>660</v>
       </c>
@@ -14887,7 +14995,7 @@
         <v>712</v>
       </c>
       <c r="D11" s="253"/>
-      <c r="E11" s="309"/>
+      <c r="E11" s="311"/>
       <c r="F11" s="135" t="s">
         <v>1009</v>
       </c>
@@ -14895,7 +15003,7 @@
         <v>1035</v>
       </c>
       <c r="H11" s="125"/>
-      <c r="I11" s="309"/>
+      <c r="I11" s="311"/>
       <c r="J11" s="135" t="s">
         <v>1097</v>
       </c>
@@ -14905,7 +15013,7 @@
       <c r="L11" s="122"/>
     </row>
     <row r="12" spans="1:12" ht="18.75">
-      <c r="A12" s="316" t="s">
+      <c r="A12" s="306" t="s">
         <v>665</v>
       </c>
       <c r="B12" s="132" t="s">
@@ -14915,7 +15023,7 @@
         <v>713</v>
       </c>
       <c r="D12" s="253"/>
-      <c r="E12" s="307" t="s">
+      <c r="E12" s="309" t="s">
         <v>973</v>
       </c>
       <c r="F12" s="132" t="s">
@@ -14925,7 +15033,7 @@
         <v>1036</v>
       </c>
       <c r="H12" s="125"/>
-      <c r="I12" s="307" t="s">
+      <c r="I12" s="309" t="s">
         <v>1059</v>
       </c>
       <c r="J12" s="132" t="s">
@@ -14937,7 +15045,7 @@
       <c r="L12" s="122"/>
     </row>
     <row r="13" spans="1:12" ht="18.75">
-      <c r="A13" s="317"/>
+      <c r="A13" s="307"/>
       <c r="B13" s="131" t="s">
         <v>662</v>
       </c>
@@ -14945,7 +15053,7 @@
         <v>714</v>
       </c>
       <c r="D13" s="253"/>
-      <c r="E13" s="308"/>
+      <c r="E13" s="310"/>
       <c r="F13" s="131" t="s">
         <v>1011</v>
       </c>
@@ -14953,7 +15061,7 @@
         <v>1037</v>
       </c>
       <c r="H13" s="125"/>
-      <c r="I13" s="308"/>
+      <c r="I13" s="310"/>
       <c r="J13" s="131" t="s">
         <v>1099</v>
       </c>
@@ -14963,7 +15071,7 @@
       <c r="L13" s="122"/>
     </row>
     <row r="14" spans="1:12" ht="18.75">
-      <c r="A14" s="317"/>
+      <c r="A14" s="307"/>
       <c r="B14" s="131" t="s">
         <v>663</v>
       </c>
@@ -14971,7 +15079,7 @@
         <v>715</v>
       </c>
       <c r="D14" s="253"/>
-      <c r="E14" s="308"/>
+      <c r="E14" s="310"/>
       <c r="F14" s="131" t="s">
         <v>1012</v>
       </c>
@@ -14979,7 +15087,7 @@
         <v>1038</v>
       </c>
       <c r="H14" s="125"/>
-      <c r="I14" s="308"/>
+      <c r="I14" s="310"/>
       <c r="J14" s="131" t="s">
         <v>1100</v>
       </c>
@@ -14989,7 +15097,7 @@
       <c r="L14" s="122"/>
     </row>
     <row r="15" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A15" s="318"/>
+      <c r="A15" s="308"/>
       <c r="B15" s="135" t="s">
         <v>664</v>
       </c>
@@ -14997,7 +15105,7 @@
         <v>716</v>
       </c>
       <c r="D15" s="253"/>
-      <c r="E15" s="309"/>
+      <c r="E15" s="311"/>
       <c r="F15" s="135" t="s">
         <v>1013</v>
       </c>
@@ -15005,7 +15113,7 @@
         <v>1039</v>
       </c>
       <c r="H15" s="125"/>
-      <c r="I15" s="309"/>
+      <c r="I15" s="311"/>
       <c r="J15" s="135" t="s">
         <v>1101</v>
       </c>
@@ -15015,7 +15123,7 @@
       <c r="L15" s="122"/>
     </row>
     <row r="16" spans="1:12" ht="18.75">
-      <c r="A16" s="316" t="s">
+      <c r="A16" s="306" t="s">
         <v>666</v>
       </c>
       <c r="B16" s="132" t="s">
@@ -15025,7 +15133,7 @@
         <v>717</v>
       </c>
       <c r="D16" s="253"/>
-      <c r="E16" s="307" t="s">
+      <c r="E16" s="309" t="s">
         <v>972</v>
       </c>
       <c r="F16" s="132" t="s">
@@ -15035,7 +15143,7 @@
         <v>1040</v>
       </c>
       <c r="H16" s="125"/>
-      <c r="I16" s="307" t="s">
+      <c r="I16" s="309" t="s">
         <v>1060</v>
       </c>
       <c r="J16" s="132" t="s">
@@ -15047,7 +15155,7 @@
       <c r="L16" s="122"/>
     </row>
     <row r="17" spans="1:12" ht="18.75">
-      <c r="A17" s="317"/>
+      <c r="A17" s="307"/>
       <c r="B17" s="131" t="s">
         <v>669</v>
       </c>
@@ -15055,7 +15163,7 @@
         <v>718</v>
       </c>
       <c r="D17" s="253"/>
-      <c r="E17" s="308"/>
+      <c r="E17" s="310"/>
       <c r="F17" s="131" t="s">
         <v>1015</v>
       </c>
@@ -15063,7 +15171,7 @@
         <v>1041</v>
       </c>
       <c r="H17" s="125"/>
-      <c r="I17" s="308"/>
+      <c r="I17" s="310"/>
       <c r="J17" s="131" t="s">
         <v>1103</v>
       </c>
@@ -15073,7 +15181,7 @@
       <c r="L17" s="122"/>
     </row>
     <row r="18" spans="1:12" ht="18.75">
-      <c r="A18" s="317"/>
+      <c r="A18" s="307"/>
       <c r="B18" s="131" t="s">
         <v>670</v>
       </c>
@@ -15081,7 +15189,7 @@
         <v>719</v>
       </c>
       <c r="D18" s="253"/>
-      <c r="E18" s="308"/>
+      <c r="E18" s="310"/>
       <c r="F18" s="131" t="s">
         <v>1016</v>
       </c>
@@ -15089,7 +15197,7 @@
         <v>1042</v>
       </c>
       <c r="H18" s="125"/>
-      <c r="I18" s="308"/>
+      <c r="I18" s="310"/>
       <c r="J18" s="131" t="s">
         <v>1104</v>
       </c>
@@ -15099,7 +15207,7 @@
       <c r="L18" s="122"/>
     </row>
     <row r="19" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A19" s="318"/>
+      <c r="A19" s="308"/>
       <c r="B19" s="135" t="s">
         <v>671</v>
       </c>
@@ -15107,7 +15215,7 @@
         <v>720</v>
       </c>
       <c r="D19" s="253"/>
-      <c r="E19" s="309"/>
+      <c r="E19" s="311"/>
       <c r="F19" s="135" t="s">
         <v>1017</v>
       </c>
@@ -15115,7 +15223,7 @@
         <v>1043</v>
       </c>
       <c r="H19" s="125"/>
-      <c r="I19" s="309"/>
+      <c r="I19" s="311"/>
       <c r="J19" s="135" t="s">
         <v>1105</v>
       </c>
@@ -15129,7 +15237,7 @@
       <c r="B20" s="125"/>
       <c r="C20" s="125"/>
       <c r="D20" s="125"/>
-      <c r="E20" s="307" t="s">
+      <c r="E20" s="309" t="s">
         <v>560</v>
       </c>
       <c r="F20" s="132" t="s">
@@ -15139,7 +15247,7 @@
         <v>1044</v>
       </c>
       <c r="H20" s="125"/>
-      <c r="I20" s="307" t="s">
+      <c r="I20" s="309" t="s">
         <v>1061</v>
       </c>
       <c r="J20" s="132" t="s">
@@ -15155,7 +15263,7 @@
       <c r="B21" s="125"/>
       <c r="C21" s="125"/>
       <c r="D21" s="125"/>
-      <c r="E21" s="308"/>
+      <c r="E21" s="310"/>
       <c r="F21" s="131" t="s">
         <v>1019</v>
       </c>
@@ -15163,7 +15271,7 @@
         <v>1045</v>
       </c>
       <c r="H21" s="125"/>
-      <c r="I21" s="308"/>
+      <c r="I21" s="310"/>
       <c r="J21" s="131" t="s">
         <v>1107</v>
       </c>
@@ -15177,7 +15285,7 @@
       <c r="B22" s="125"/>
       <c r="C22" s="125"/>
       <c r="D22" s="125"/>
-      <c r="E22" s="308"/>
+      <c r="E22" s="310"/>
       <c r="F22" s="131" t="s">
         <v>1020</v>
       </c>
@@ -15185,7 +15293,7 @@
         <v>1046</v>
       </c>
       <c r="H22" s="125"/>
-      <c r="I22" s="308"/>
+      <c r="I22" s="310"/>
       <c r="J22" s="131" t="s">
         <v>1108</v>
       </c>
@@ -15201,7 +15309,7 @@
       <c r="B23" s="256"/>
       <c r="C23" s="257"/>
       <c r="D23" s="125"/>
-      <c r="E23" s="309"/>
+      <c r="E23" s="311"/>
       <c r="F23" s="135" t="s">
         <v>1021</v>
       </c>
@@ -15209,7 +15317,7 @@
         <v>1047</v>
       </c>
       <c r="H23" s="125"/>
-      <c r="I23" s="309"/>
+      <c r="I23" s="311"/>
       <c r="J23" s="135" t="s">
         <v>1109</v>
       </c>
@@ -15229,7 +15337,7 @@
         <v>321</v>
       </c>
       <c r="D24" s="125"/>
-      <c r="E24" s="307" t="s">
+      <c r="E24" s="309" t="s">
         <v>749</v>
       </c>
       <c r="F24" s="132" t="s">
@@ -15239,7 +15347,7 @@
         <v>1048</v>
       </c>
       <c r="H24" s="125"/>
-      <c r="I24" s="307" t="s">
+      <c r="I24" s="309" t="s">
         <v>1062</v>
       </c>
       <c r="J24" s="132" t="s">
@@ -15251,7 +15359,7 @@
       <c r="L24" s="122"/>
     </row>
     <row r="25" spans="1:12" ht="18.75">
-      <c r="A25" s="301" t="s">
+      <c r="A25" s="303" t="s">
         <v>493</v>
       </c>
       <c r="B25" s="132" t="s">
@@ -15261,7 +15369,7 @@
         <v>721</v>
       </c>
       <c r="D25" s="125"/>
-      <c r="E25" s="308"/>
+      <c r="E25" s="310"/>
       <c r="F25" s="131" t="s">
         <v>1023</v>
       </c>
@@ -15269,7 +15377,7 @@
         <v>1049</v>
       </c>
       <c r="H25" s="125"/>
-      <c r="I25" s="308"/>
+      <c r="I25" s="310"/>
       <c r="J25" s="131" t="s">
         <v>1111</v>
       </c>
@@ -15279,7 +15387,7 @@
       <c r="L25" s="122"/>
     </row>
     <row r="26" spans="1:12" ht="18.75">
-      <c r="A26" s="302"/>
+      <c r="A26" s="304"/>
       <c r="B26" s="131" t="s">
         <v>679</v>
       </c>
@@ -15287,7 +15395,7 @@
         <v>722</v>
       </c>
       <c r="D26" s="125"/>
-      <c r="E26" s="308"/>
+      <c r="E26" s="310"/>
       <c r="F26" s="131" t="s">
         <v>1024</v>
       </c>
@@ -15295,7 +15403,7 @@
         <v>1050</v>
       </c>
       <c r="H26" s="125"/>
-      <c r="I26" s="308"/>
+      <c r="I26" s="310"/>
       <c r="J26" s="131" t="s">
         <v>1112</v>
       </c>
@@ -15305,7 +15413,7 @@
       <c r="L26" s="122"/>
     </row>
     <row r="27" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A27" s="302"/>
+      <c r="A27" s="304"/>
       <c r="B27" s="131" t="s">
         <v>680</v>
       </c>
@@ -15313,7 +15421,7 @@
         <v>723</v>
       </c>
       <c r="D27" s="125"/>
-      <c r="E27" s="309"/>
+      <c r="E27" s="311"/>
       <c r="F27" s="135" t="s">
         <v>1025</v>
       </c>
@@ -15321,7 +15429,7 @@
         <v>1051</v>
       </c>
       <c r="H27" s="125"/>
-      <c r="I27" s="309"/>
+      <c r="I27" s="311"/>
       <c r="J27" s="135" t="s">
         <v>1113</v>
       </c>
@@ -15331,7 +15439,7 @@
       <c r="L27" s="122"/>
     </row>
     <row r="28" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A28" s="303"/>
+      <c r="A28" s="305"/>
       <c r="B28" s="135" t="s">
         <v>681</v>
       </c>
@@ -15339,7 +15447,7 @@
         <v>724</v>
       </c>
       <c r="D28" s="125"/>
-      <c r="E28" s="307" t="s">
+      <c r="E28" s="309" t="s">
         <v>562</v>
       </c>
       <c r="F28" s="132" t="s">
@@ -15349,7 +15457,7 @@
         <v>1052</v>
       </c>
       <c r="H28" s="125"/>
-      <c r="I28" s="307" t="s">
+      <c r="I28" s="309" t="s">
         <v>1063</v>
       </c>
       <c r="J28" s="132" t="s">
@@ -15361,7 +15469,7 @@
       <c r="L28" s="122"/>
     </row>
     <row r="29" spans="1:12" ht="18.75">
-      <c r="A29" s="301" t="s">
+      <c r="A29" s="303" t="s">
         <v>687</v>
       </c>
       <c r="B29" s="132" t="s">
@@ -15371,7 +15479,7 @@
         <v>725</v>
       </c>
       <c r="D29" s="253"/>
-      <c r="E29" s="308"/>
+      <c r="E29" s="310"/>
       <c r="F29" s="131" t="s">
         <v>1027</v>
       </c>
@@ -15379,7 +15487,7 @@
         <v>1053</v>
       </c>
       <c r="H29" s="125"/>
-      <c r="I29" s="308"/>
+      <c r="I29" s="310"/>
       <c r="J29" s="131" t="s">
         <v>1115</v>
       </c>
@@ -15389,7 +15497,7 @@
       <c r="L29" s="122"/>
     </row>
     <row r="30" spans="1:12" ht="18.75">
-      <c r="A30" s="302"/>
+      <c r="A30" s="304"/>
       <c r="B30" s="131" t="s">
         <v>684</v>
       </c>
@@ -15397,11 +15505,11 @@
         <v>726</v>
       </c>
       <c r="D30" s="253"/>
-      <c r="E30" s="308"/>
+      <c r="E30" s="310"/>
       <c r="F30" s="131"/>
       <c r="G30" s="250"/>
       <c r="H30" s="125"/>
-      <c r="I30" s="308"/>
+      <c r="I30" s="310"/>
       <c r="J30" s="131" t="s">
         <v>1116</v>
       </c>
@@ -15411,7 +15519,7 @@
       <c r="L30" s="122"/>
     </row>
     <row r="31" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A31" s="302"/>
+      <c r="A31" s="304"/>
       <c r="B31" s="131" t="s">
         <v>685</v>
       </c>
@@ -15419,11 +15527,11 @@
         <v>727</v>
       </c>
       <c r="D31" s="253"/>
-      <c r="E31" s="309"/>
+      <c r="E31" s="311"/>
       <c r="F31" s="135"/>
       <c r="G31" s="251"/>
       <c r="H31" s="125"/>
-      <c r="I31" s="309"/>
+      <c r="I31" s="311"/>
       <c r="J31" s="135" t="s">
         <v>1117</v>
       </c>
@@ -15433,7 +15541,7 @@
       <c r="L31" s="122"/>
     </row>
     <row r="32" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A32" s="303"/>
+      <c r="A32" s="305"/>
       <c r="B32" s="135" t="s">
         <v>686</v>
       </c>
@@ -15451,7 +15559,7 @@
       <c r="L32" s="122"/>
     </row>
     <row r="33" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A33" s="301" t="s">
+      <c r="A33" s="303" t="s">
         <v>691</v>
       </c>
       <c r="B33" s="132" t="s">
@@ -15461,21 +15569,21 @@
         <v>729</v>
       </c>
       <c r="D33" s="253"/>
-      <c r="E33" s="304" t="s">
+      <c r="E33" s="318" t="s">
         <v>1148</v>
       </c>
-      <c r="F33" s="305"/>
-      <c r="G33" s="306"/>
+      <c r="F33" s="319"/>
+      <c r="G33" s="320"/>
       <c r="H33" s="124"/>
-      <c r="I33" s="304" t="s">
+      <c r="I33" s="318" t="s">
         <v>1147</v>
       </c>
-      <c r="J33" s="305"/>
-      <c r="K33" s="306"/>
+      <c r="J33" s="319"/>
+      <c r="K33" s="320"/>
       <c r="L33" s="122"/>
     </row>
     <row r="34" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A34" s="302"/>
+      <c r="A34" s="304"/>
       <c r="B34" s="131" t="s">
         <v>693</v>
       </c>
@@ -15505,7 +15613,7 @@
       <c r="L34" s="122"/>
     </row>
     <row r="35" spans="1:12" ht="18.75">
-      <c r="A35" s="302"/>
+      <c r="A35" s="304"/>
       <c r="B35" s="131" t="s">
         <v>694</v>
       </c>
@@ -15513,7 +15621,7 @@
         <v>731</v>
       </c>
       <c r="D35" s="253"/>
-      <c r="E35" s="301" t="s">
+      <c r="E35" s="303" t="s">
         <v>494</v>
       </c>
       <c r="F35" s="132" t="s">
@@ -15523,7 +15631,7 @@
         <v>11311</v>
       </c>
       <c r="H35" s="124"/>
-      <c r="I35" s="301" t="s">
+      <c r="I35" s="303" t="s">
         <v>955</v>
       </c>
       <c r="J35" s="132" t="s">
@@ -15535,7 +15643,7 @@
       <c r="L35" s="122"/>
     </row>
     <row r="36" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A36" s="303"/>
+      <c r="A36" s="305"/>
       <c r="B36" s="135" t="s">
         <v>695</v>
       </c>
@@ -15543,7 +15651,7 @@
         <v>732</v>
       </c>
       <c r="D36" s="253"/>
-      <c r="E36" s="302"/>
+      <c r="E36" s="304"/>
       <c r="F36" s="131" t="s">
         <v>958</v>
       </c>
@@ -15551,7 +15659,7 @@
         <v>11312</v>
       </c>
       <c r="H36" s="124"/>
-      <c r="I36" s="302"/>
+      <c r="I36" s="304"/>
       <c r="J36" s="131" t="s">
         <v>965</v>
       </c>
@@ -15561,7 +15669,7 @@
       <c r="L36" s="122"/>
     </row>
     <row r="37" spans="1:12" ht="18.75">
-      <c r="A37" s="301" t="s">
+      <c r="A37" s="303" t="s">
         <v>698</v>
       </c>
       <c r="B37" s="132" t="s">
@@ -15571,7 +15679,7 @@
         <v>11441</v>
       </c>
       <c r="D37" s="253"/>
-      <c r="E37" s="302"/>
+      <c r="E37" s="304"/>
       <c r="F37" s="131" t="s">
         <v>959</v>
       </c>
@@ -15579,7 +15687,7 @@
         <v>11313</v>
       </c>
       <c r="H37" s="124"/>
-      <c r="I37" s="302"/>
+      <c r="I37" s="304"/>
       <c r="J37" s="131" t="s">
         <v>966</v>
       </c>
@@ -15589,7 +15697,7 @@
       <c r="L37" s="122"/>
     </row>
     <row r="38" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A38" s="302"/>
+      <c r="A38" s="304"/>
       <c r="B38" s="131" t="s">
         <v>700</v>
       </c>
@@ -15597,7 +15705,7 @@
         <v>11442</v>
       </c>
       <c r="D38" s="253"/>
-      <c r="E38" s="303"/>
+      <c r="E38" s="305"/>
       <c r="F38" s="135" t="s">
         <v>959</v>
       </c>
@@ -15605,7 +15713,7 @@
         <v>11314</v>
       </c>
       <c r="H38" s="124"/>
-      <c r="I38" s="303"/>
+      <c r="I38" s="305"/>
       <c r="J38" s="135" t="s">
         <v>967</v>
       </c>
@@ -15615,7 +15723,7 @@
       <c r="L38" s="122"/>
     </row>
     <row r="39" spans="1:12" ht="18.75">
-      <c r="A39" s="302"/>
+      <c r="A39" s="304"/>
       <c r="B39" s="131" t="s">
         <v>701</v>
       </c>
@@ -15623,7 +15731,7 @@
         <v>11443</v>
       </c>
       <c r="D39" s="253"/>
-      <c r="E39" s="301" t="s">
+      <c r="E39" s="303" t="s">
         <v>954</v>
       </c>
       <c r="F39" s="132" t="s">
@@ -15633,7 +15741,7 @@
         <v>11321</v>
       </c>
       <c r="H39" s="124"/>
-      <c r="I39" s="301" t="s">
+      <c r="I39" s="303" t="s">
         <v>956</v>
       </c>
       <c r="J39" s="132" t="s">
@@ -15645,7 +15753,7 @@
       <c r="L39" s="122"/>
     </row>
     <row r="40" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A40" s="303"/>
+      <c r="A40" s="305"/>
       <c r="B40" s="135" t="s">
         <v>702</v>
       </c>
@@ -15653,7 +15761,7 @@
         <v>11444</v>
       </c>
       <c r="D40" s="253"/>
-      <c r="E40" s="302"/>
+      <c r="E40" s="304"/>
       <c r="F40" s="131" t="s">
         <v>961</v>
       </c>
@@ -15661,7 +15769,7 @@
         <v>11322</v>
       </c>
       <c r="H40" s="124"/>
-      <c r="I40" s="302"/>
+      <c r="I40" s="304"/>
       <c r="J40" s="131" t="s">
         <v>969</v>
       </c>
@@ -15671,7 +15779,7 @@
       <c r="L40" s="122"/>
     </row>
     <row r="41" spans="1:12" ht="18.75">
-      <c r="A41" s="301" t="s">
+      <c r="A41" s="303" t="s">
         <v>1346</v>
       </c>
       <c r="B41" s="132" t="s">
@@ -15681,7 +15789,7 @@
         <v>11451</v>
       </c>
       <c r="D41" s="253"/>
-      <c r="E41" s="302"/>
+      <c r="E41" s="304"/>
       <c r="F41" s="131" t="s">
         <v>962</v>
       </c>
@@ -15689,7 +15797,7 @@
         <v>11323</v>
       </c>
       <c r="H41" s="124"/>
-      <c r="I41" s="302"/>
+      <c r="I41" s="304"/>
       <c r="J41" s="131" t="s">
         <v>970</v>
       </c>
@@ -15699,7 +15807,7 @@
       <c r="L41" s="122"/>
     </row>
     <row r="42" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A42" s="302"/>
+      <c r="A42" s="304"/>
       <c r="B42" s="131" t="s">
         <v>1348</v>
       </c>
@@ -15707,7 +15815,7 @@
         <v>11452</v>
       </c>
       <c r="D42" s="253"/>
-      <c r="E42" s="303"/>
+      <c r="E42" s="305"/>
       <c r="F42" s="135" t="s">
         <v>963</v>
       </c>
@@ -15715,7 +15823,7 @@
         <v>11324</v>
       </c>
       <c r="H42" s="124"/>
-      <c r="I42" s="303"/>
+      <c r="I42" s="305"/>
       <c r="J42" s="135" t="s">
         <v>971</v>
       </c>
@@ -15725,7 +15833,7 @@
       <c r="L42" s="122"/>
     </row>
     <row r="43" spans="1:12" ht="18.75">
-      <c r="A43" s="302"/>
+      <c r="A43" s="304"/>
       <c r="B43" s="131" t="s">
         <v>1349</v>
       </c>
@@ -15743,7 +15851,7 @@
       <c r="L43" s="122"/>
     </row>
     <row r="44" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A44" s="303"/>
+      <c r="A44" s="305"/>
       <c r="B44" s="135" t="s">
         <v>1350</v>
       </c>
@@ -15776,19 +15884,12 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="I35:I38"/>
+    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="E33:G33"/>
     <mergeCell ref="I16:I19"/>
     <mergeCell ref="I12:I15"/>
     <mergeCell ref="I8:I11"/>
@@ -15799,16 +15900,23 @@
     <mergeCell ref="I28:I31"/>
     <mergeCell ref="E20:E23"/>
     <mergeCell ref="E24:E27"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="I35:I38"/>
-    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="E16:E19"/>
     <mergeCell ref="A25:A28"/>
     <mergeCell ref="A29:A32"/>
     <mergeCell ref="A33:A36"/>
     <mergeCell ref="A37:A40"/>
-    <mergeCell ref="E33:G33"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15839,40 +15947,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="319" t="s">
+      <c r="A1" s="325" t="s">
         <v>1150</v>
       </c>
-      <c r="B1" s="320"/>
-      <c r="C1" s="320"/>
-      <c r="D1" s="320"/>
-      <c r="E1" s="320"/>
-      <c r="F1" s="320"/>
-      <c r="G1" s="320"/>
-      <c r="H1" s="321"/>
+      <c r="B1" s="326"/>
+      <c r="C1" s="326"/>
+      <c r="D1" s="326"/>
+      <c r="E1" s="326"/>
+      <c r="F1" s="326"/>
+      <c r="G1" s="326"/>
+      <c r="H1" s="327"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="322"/>
-      <c r="B2" s="323"/>
-      <c r="C2" s="323"/>
-      <c r="D2" s="323"/>
-      <c r="E2" s="323"/>
-      <c r="F2" s="323"/>
-      <c r="G2" s="323"/>
-      <c r="H2" s="324"/>
+      <c r="A2" s="328"/>
+      <c r="B2" s="329"/>
+      <c r="C2" s="329"/>
+      <c r="D2" s="329"/>
+      <c r="E2" s="329"/>
+      <c r="F2" s="329"/>
+      <c r="G2" s="329"/>
+      <c r="H2" s="330"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="325" t="s">
+      <c r="A3" s="331" t="s">
         <v>250</v>
       </c>
-      <c r="B3" s="326"/>
-      <c r="C3" s="326"/>
-      <c r="D3" s="326"/>
-      <c r="E3" s="326" t="s">
+      <c r="B3" s="332"/>
+      <c r="C3" s="332"/>
+      <c r="D3" s="332"/>
+      <c r="E3" s="332" t="s">
         <v>251</v>
       </c>
-      <c r="F3" s="326"/>
-      <c r="G3" s="326"/>
-      <c r="H3" s="327"/>
+      <c r="F3" s="332"/>
+      <c r="G3" s="332"/>
+      <c r="H3" s="333"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="12">
@@ -16406,11 +16514,11 @@
       <c r="C27" s="118" t="s">
         <v>594</v>
       </c>
-      <c r="D27" s="328" t="s">
+      <c r="D27" s="324" t="s">
         <v>570</v>
       </c>
-      <c r="E27" s="328"/>
-      <c r="F27" s="328"/>
+      <c r="E27" s="324"/>
+      <c r="F27" s="324"/>
       <c r="G27" s="17"/>
       <c r="H27" s="18"/>
     </row>
@@ -16422,11 +16530,11 @@
       <c r="C28" s="118" t="s">
         <v>598</v>
       </c>
-      <c r="D28" s="328" t="s">
+      <c r="D28" s="324" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="328"/>
-      <c r="F28" s="328"/>
+      <c r="E28" s="324"/>
+      <c r="F28" s="324"/>
       <c r="G28" s="17"/>
       <c r="H28" s="18"/>
     </row>
@@ -16438,11 +16546,11 @@
       <c r="C29" s="118" t="s">
         <v>599</v>
       </c>
-      <c r="D29" s="328" t="s">
+      <c r="D29" s="324" t="s">
         <v>571</v>
       </c>
-      <c r="E29" s="328"/>
-      <c r="F29" s="328"/>
+      <c r="E29" s="324"/>
+      <c r="F29" s="324"/>
       <c r="G29" s="17"/>
       <c r="H29" s="18"/>
     </row>
@@ -16454,11 +16562,11 @@
       <c r="C30" s="118" t="s">
         <v>600</v>
       </c>
-      <c r="D30" s="328" t="s">
+      <c r="D30" s="324" t="s">
         <v>572</v>
       </c>
-      <c r="E30" s="328"/>
-      <c r="F30" s="328"/>
+      <c r="E30" s="324"/>
+      <c r="F30" s="324"/>
       <c r="G30" s="17"/>
       <c r="H30" s="18"/>
     </row>
@@ -16470,11 +16578,11 @@
       <c r="C31" s="118" t="s">
         <v>601</v>
       </c>
-      <c r="D31" s="328" t="s">
+      <c r="D31" s="324" t="s">
         <v>573</v>
       </c>
-      <c r="E31" s="328"/>
-      <c r="F31" s="328"/>
+      <c r="E31" s="324"/>
+      <c r="F31" s="324"/>
       <c r="G31" s="17"/>
       <c r="H31" s="18"/>
     </row>
@@ -16486,11 +16594,11 @@
       <c r="C32" s="118" t="s">
         <v>602</v>
       </c>
-      <c r="D32" s="328" t="s">
+      <c r="D32" s="324" t="s">
         <v>574</v>
       </c>
-      <c r="E32" s="328"/>
-      <c r="F32" s="328"/>
+      <c r="E32" s="324"/>
+      <c r="F32" s="324"/>
       <c r="G32" s="17"/>
       <c r="H32" s="18"/>
     </row>
@@ -16502,11 +16610,11 @@
       <c r="C33" s="118" t="s">
         <v>614</v>
       </c>
-      <c r="D33" s="328" t="s">
+      <c r="D33" s="324" t="s">
         <v>482</v>
       </c>
-      <c r="E33" s="328"/>
-      <c r="F33" s="328"/>
+      <c r="E33" s="324"/>
+      <c r="F33" s="324"/>
       <c r="G33" s="17"/>
       <c r="H33" s="18"/>
     </row>
@@ -16518,11 +16626,11 @@
       <c r="C34" s="118" t="s">
         <v>615</v>
       </c>
-      <c r="D34" s="328" t="s">
+      <c r="D34" s="324" t="s">
         <v>575</v>
       </c>
-      <c r="E34" s="328"/>
-      <c r="F34" s="328"/>
+      <c r="E34" s="324"/>
+      <c r="F34" s="324"/>
       <c r="G34" s="17"/>
       <c r="H34" s="18"/>
     </row>
@@ -16534,11 +16642,11 @@
       <c r="C35" s="118" t="s">
         <v>616</v>
       </c>
-      <c r="D35" s="328" t="s">
+      <c r="D35" s="324" t="s">
         <v>576</v>
       </c>
-      <c r="E35" s="328"/>
-      <c r="F35" s="328"/>
+      <c r="E35" s="324"/>
+      <c r="F35" s="324"/>
       <c r="G35" s="17"/>
       <c r="H35" s="18"/>
     </row>
@@ -16548,11 +16656,11 @@
       <c r="C36" s="118" t="s">
         <v>651</v>
       </c>
-      <c r="D36" s="329" t="s">
+      <c r="D36" s="321" t="s">
         <v>591</v>
       </c>
-      <c r="E36" s="330"/>
-      <c r="F36" s="331"/>
+      <c r="E36" s="322"/>
+      <c r="F36" s="323"/>
       <c r="G36" s="17"/>
       <c r="H36" s="18"/>
     </row>
@@ -16562,11 +16670,11 @@
       <c r="C37" s="118" t="s">
         <v>654</v>
       </c>
-      <c r="D37" s="329" t="s">
+      <c r="D37" s="321" t="s">
         <v>652</v>
       </c>
-      <c r="E37" s="330"/>
-      <c r="F37" s="331"/>
+      <c r="E37" s="322"/>
+      <c r="F37" s="323"/>
       <c r="G37" s="17"/>
       <c r="H37" s="18"/>
     </row>
@@ -16576,11 +16684,11 @@
       <c r="C38" s="118" t="s">
         <v>653</v>
       </c>
-      <c r="D38" s="329" t="s">
+      <c r="D38" s="321" t="s">
         <v>655</v>
       </c>
-      <c r="E38" s="330"/>
-      <c r="F38" s="331"/>
+      <c r="E38" s="322"/>
+      <c r="F38" s="323"/>
       <c r="G38" s="17"/>
       <c r="H38" s="18"/>
     </row>
@@ -16588,9 +16696,9 @@
       <c r="A39" s="16"/>
       <c r="B39" s="120"/>
       <c r="C39" s="118"/>
-      <c r="D39" s="329"/>
-      <c r="E39" s="330"/>
-      <c r="F39" s="331"/>
+      <c r="D39" s="321"/>
+      <c r="E39" s="322"/>
+      <c r="F39" s="323"/>
       <c r="G39" s="17"/>
       <c r="H39" s="18"/>
     </row>
@@ -16688,13 +16796,6 @@
     <row r="52" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:H3"/>
@@ -16704,6 +16805,13 @@
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -16731,28 +16839,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75">
-      <c r="A1" s="341" t="s">
+      <c r="A1" s="343" t="s">
         <v>1183</v>
       </c>
-      <c r="B1" s="341"/>
-      <c r="C1" s="341"/>
-      <c r="D1" s="341"/>
-      <c r="E1" s="341"/>
-      <c r="F1" s="341"/>
-      <c r="G1" s="341"/>
-      <c r="H1" s="341"/>
+      <c r="B1" s="343"/>
+      <c r="C1" s="343"/>
+      <c r="D1" s="343"/>
+      <c r="E1" s="343"/>
+      <c r="F1" s="343"/>
+      <c r="G1" s="343"/>
+      <c r="H1" s="343"/>
     </row>
     <row r="2" spans="1:10" ht="15.75">
-      <c r="A2" s="335" t="s">
+      <c r="A2" s="337" t="s">
         <v>1151</v>
       </c>
-      <c r="B2" s="336"/>
-      <c r="C2" s="336"/>
-      <c r="D2" s="336"/>
-      <c r="E2" s="336"/>
-      <c r="F2" s="336"/>
-      <c r="G2" s="336"/>
-      <c r="H2" s="337"/>
+      <c r="B2" s="338"/>
+      <c r="C2" s="338"/>
+      <c r="D2" s="338"/>
+      <c r="E2" s="338"/>
+      <c r="F2" s="338"/>
+      <c r="G2" s="338"/>
+      <c r="H2" s="339"/>
     </row>
     <row r="3" spans="1:10" ht="15.75">
       <c r="A3" s="5"/>
@@ -17068,16 +17176,16 @@
       <c r="H17" s="263"/>
     </row>
     <row r="18" spans="1:11" ht="15.75">
-      <c r="A18" s="338" t="s">
+      <c r="A18" s="340" t="s">
         <v>224</v>
       </c>
-      <c r="B18" s="339"/>
-      <c r="C18" s="339"/>
-      <c r="D18" s="339"/>
-      <c r="E18" s="339"/>
-      <c r="F18" s="339"/>
-      <c r="G18" s="339"/>
-      <c r="H18" s="340"/>
+      <c r="B18" s="341"/>
+      <c r="C18" s="341"/>
+      <c r="D18" s="341"/>
+      <c r="E18" s="341"/>
+      <c r="F18" s="341"/>
+      <c r="G18" s="341"/>
+      <c r="H18" s="342"/>
     </row>
     <row r="19" spans="1:11" ht="15.75">
       <c r="A19" s="264"/>
@@ -17333,16 +17441,16 @@
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:11" ht="15.75">
-      <c r="A31" s="335" t="s">
+      <c r="A31" s="337" t="s">
         <v>225</v>
       </c>
-      <c r="B31" s="336"/>
-      <c r="C31" s="336"/>
-      <c r="D31" s="336"/>
-      <c r="E31" s="336"/>
-      <c r="F31" s="336"/>
-      <c r="G31" s="336"/>
-      <c r="H31" s="337"/>
+      <c r="B31" s="338"/>
+      <c r="C31" s="338"/>
+      <c r="D31" s="338"/>
+      <c r="E31" s="338"/>
+      <c r="F31" s="338"/>
+      <c r="G31" s="338"/>
+      <c r="H31" s="339"/>
     </row>
     <row r="32" spans="1:11" ht="15.75">
       <c r="A32" s="5"/>
@@ -17568,18 +17676,18 @@
     </row>
     <row r="43" spans="1:8" ht="10.5" customHeight="1"/>
     <row r="44" spans="1:8" ht="15.75">
-      <c r="A44" s="332" t="s">
+      <c r="A44" s="334" t="s">
         <v>1174</v>
       </c>
-      <c r="B44" s="333"/>
-      <c r="C44" s="333"/>
-      <c r="D44" s="334"/>
-      <c r="E44" s="332" t="s">
+      <c r="B44" s="335"/>
+      <c r="C44" s="335"/>
+      <c r="D44" s="336"/>
+      <c r="E44" s="334" t="s">
         <v>1174</v>
       </c>
-      <c r="F44" s="333"/>
-      <c r="G44" s="333"/>
-      <c r="H44" s="334"/>
+      <c r="F44" s="335"/>
+      <c r="G44" s="335"/>
+      <c r="H44" s="336"/>
     </row>
     <row r="45" spans="1:8" ht="15.75">
       <c r="A45" s="3"/>
@@ -17697,54 +17805,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1">
-      <c r="A1" s="345" t="s">
+      <c r="A1" s="347" t="s">
         <v>1295</v>
       </c>
-      <c r="B1" s="346"/>
-      <c r="C1" s="346"/>
-      <c r="D1" s="346"/>
-      <c r="E1" s="346"/>
-      <c r="F1" s="346"/>
-      <c r="G1" s="346"/>
-      <c r="H1" s="347"/>
+      <c r="B1" s="348"/>
+      <c r="C1" s="348"/>
+      <c r="D1" s="348"/>
+      <c r="E1" s="348"/>
+      <c r="F1" s="348"/>
+      <c r="G1" s="348"/>
+      <c r="H1" s="349"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="348"/>
-      <c r="B2" s="349"/>
-      <c r="C2" s="349"/>
-      <c r="D2" s="349"/>
-      <c r="E2" s="349"/>
-      <c r="F2" s="349"/>
-      <c r="G2" s="349"/>
-      <c r="H2" s="350"/>
+      <c r="A2" s="350"/>
+      <c r="B2" s="351"/>
+      <c r="C2" s="351"/>
+      <c r="D2" s="351"/>
+      <c r="E2" s="351"/>
+      <c r="F2" s="351"/>
+      <c r="G2" s="351"/>
+      <c r="H2" s="352"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="351" t="s">
+      <c r="A3" s="353" t="s">
         <v>1255</v>
       </c>
-      <c r="B3" s="352"/>
-      <c r="C3" s="352"/>
-      <c r="D3" s="353"/>
-      <c r="E3" s="354" t="s">
+      <c r="B3" s="354"/>
+      <c r="C3" s="354"/>
+      <c r="D3" s="355"/>
+      <c r="E3" s="356" t="s">
         <v>1256</v>
       </c>
-      <c r="F3" s="352"/>
-      <c r="G3" s="352"/>
-      <c r="H3" s="355"/>
+      <c r="F3" s="354"/>
+      <c r="G3" s="354"/>
+      <c r="H3" s="357"/>
     </row>
     <row r="4" spans="1:8" ht="16.149999999999999" customHeight="1" thickBot="1">
-      <c r="A4" s="356" t="s">
+      <c r="A4" s="358" t="s">
         <v>1257</v>
       </c>
-      <c r="B4" s="357"/>
-      <c r="C4" s="357"/>
-      <c r="D4" s="358"/>
-      <c r="E4" s="359" t="s">
+      <c r="B4" s="359"/>
+      <c r="C4" s="359"/>
+      <c r="D4" s="360"/>
+      <c r="E4" s="361" t="s">
         <v>1258</v>
       </c>
-      <c r="F4" s="357"/>
-      <c r="G4" s="357"/>
-      <c r="H4" s="360"/>
+      <c r="F4" s="359"/>
+      <c r="G4" s="359"/>
+      <c r="H4" s="362"/>
     </row>
     <row r="5" spans="1:8" ht="19.5" thickBot="1">
       <c r="A5" s="272">
@@ -18223,12 +18331,12 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="19.5" thickBot="1">
-      <c r="A25" s="342" t="s">
+      <c r="A25" s="344" t="s">
         <v>1287</v>
       </c>
-      <c r="B25" s="343"/>
-      <c r="C25" s="343"/>
-      <c r="D25" s="344"/>
+      <c r="B25" s="345"/>
+      <c r="C25" s="345"/>
+      <c r="D25" s="346"/>
       <c r="E25" s="273">
         <v>21</v>
       </c>
@@ -18466,28 +18574,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="373" t="s">
+      <c r="A1" s="363" t="s">
         <v>952</v>
       </c>
-      <c r="B1" s="374"/>
-      <c r="C1" s="374"/>
-      <c r="D1" s="374"/>
-      <c r="E1" s="374"/>
-      <c r="F1" s="375"/>
+      <c r="B1" s="364"/>
+      <c r="C1" s="364"/>
+      <c r="D1" s="364"/>
+      <c r="E1" s="364"/>
+      <c r="F1" s="365"/>
       <c r="G1" s="175"/>
       <c r="H1" s="175"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="376" t="s">
+      <c r="A2" s="366" t="s">
         <v>840</v>
       </c>
-      <c r="B2" s="377"/>
-      <c r="C2" s="378"/>
-      <c r="D2" s="376" t="s">
+      <c r="B2" s="367"/>
+      <c r="C2" s="368"/>
+      <c r="D2" s="366" t="s">
         <v>841</v>
       </c>
-      <c r="E2" s="377"/>
-      <c r="F2" s="378"/>
+      <c r="E2" s="367"/>
+      <c r="F2" s="368"/>
       <c r="G2" s="175"/>
       <c r="H2" s="175"/>
     </row>
@@ -18511,7 +18619,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="175"/>
-      <c r="H3" s="370" t="s">
+      <c r="H3" s="369" t="s">
         <v>844</v>
       </c>
     </row>
@@ -18535,7 +18643,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="175"/>
-      <c r="H4" s="371"/>
+      <c r="H4" s="370"/>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A5" s="176">
@@ -18557,7 +18665,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="175"/>
-      <c r="H5" s="371"/>
+      <c r="H5" s="370"/>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A6" s="179">
@@ -18579,7 +18687,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="175"/>
-      <c r="H6" s="371"/>
+      <c r="H6" s="370"/>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A7" s="179">
@@ -18601,7 +18709,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="175"/>
-      <c r="H7" s="371"/>
+      <c r="H7" s="370"/>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A8" s="182">
@@ -18623,7 +18731,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="175"/>
-      <c r="H8" s="371"/>
+      <c r="H8" s="370"/>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A9" s="182">
@@ -18645,7 +18753,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="175"/>
-      <c r="H9" s="371"/>
+      <c r="H9" s="370"/>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A10" s="185">
@@ -18667,7 +18775,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="175"/>
-      <c r="H10" s="372"/>
+      <c r="H10" s="371"/>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="188">
@@ -18689,7 +18797,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="175"/>
-      <c r="H11" s="361" t="s">
+      <c r="H11" s="372" t="s">
         <v>856</v>
       </c>
     </row>
@@ -18713,7 +18821,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="175"/>
-      <c r="H12" s="362"/>
+      <c r="H12" s="373"/>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A13" s="191">
@@ -18735,7 +18843,7 @@
         <v>11</v>
       </c>
       <c r="G13" s="175"/>
-      <c r="H13" s="362"/>
+      <c r="H13" s="373"/>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A14" s="191">
@@ -18757,7 +18865,7 @@
         <v>12</v>
       </c>
       <c r="G14" s="175"/>
-      <c r="H14" s="362"/>
+      <c r="H14" s="373"/>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A15" s="195">
@@ -18779,7 +18887,7 @@
         <v>13</v>
       </c>
       <c r="G15" s="175"/>
-      <c r="H15" s="362"/>
+      <c r="H15" s="373"/>
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A16" s="195">
@@ -18801,7 +18909,7 @@
         <v>14</v>
       </c>
       <c r="G16" s="175"/>
-      <c r="H16" s="362"/>
+      <c r="H16" s="373"/>
     </row>
     <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A17" s="195">
@@ -18823,7 +18931,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="175"/>
-      <c r="H17" s="362"/>
+      <c r="H17" s="373"/>
     </row>
     <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A18" s="195">
@@ -18845,7 +18953,7 @@
         <v>16</v>
       </c>
       <c r="G18" s="175"/>
-      <c r="H18" s="362"/>
+      <c r="H18" s="373"/>
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A19" s="195">
@@ -18867,7 +18975,7 @@
         <v>17</v>
       </c>
       <c r="G19" s="175"/>
-      <c r="H19" s="362"/>
+      <c r="H19" s="373"/>
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A20" s="198">
@@ -18889,7 +18997,7 @@
         <v>18</v>
       </c>
       <c r="G20" s="175"/>
-      <c r="H20" s="362"/>
+      <c r="H20" s="373"/>
     </row>
     <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A21" s="198">
@@ -18911,7 +19019,7 @@
         <v>19</v>
       </c>
       <c r="G21" s="175"/>
-      <c r="H21" s="362"/>
+      <c r="H21" s="373"/>
     </row>
     <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A22" s="201">
@@ -18933,7 +19041,7 @@
         <v>20</v>
       </c>
       <c r="G22" s="175"/>
-      <c r="H22" s="363"/>
+      <c r="H22" s="374"/>
     </row>
     <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1"/>
     <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1"/>
@@ -18951,28 +19059,28 @@
     <row r="36" spans="1:8" ht="20.100000000000001" customHeight="1"/>
     <row r="37" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1"/>
     <row r="38" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A38" s="364" t="s">
+      <c r="A38" s="375" t="s">
         <v>953</v>
       </c>
-      <c r="B38" s="365"/>
-      <c r="C38" s="365"/>
-      <c r="D38" s="365"/>
-      <c r="E38" s="365"/>
-      <c r="F38" s="366"/>
+      <c r="B38" s="376"/>
+      <c r="C38" s="376"/>
+      <c r="D38" s="376"/>
+      <c r="E38" s="376"/>
+      <c r="F38" s="377"/>
       <c r="G38" s="175"/>
       <c r="H38" s="175"/>
     </row>
     <row r="39" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A39" s="367" t="s">
+      <c r="A39" s="378" t="s">
         <v>840</v>
       </c>
-      <c r="B39" s="368"/>
-      <c r="C39" s="369"/>
-      <c r="D39" s="367" t="s">
+      <c r="B39" s="379"/>
+      <c r="C39" s="380"/>
+      <c r="D39" s="378" t="s">
         <v>841</v>
       </c>
-      <c r="E39" s="368"/>
-      <c r="F39" s="369"/>
+      <c r="E39" s="379"/>
+      <c r="F39" s="380"/>
       <c r="G39" s="175"/>
       <c r="H39" s="175"/>
     </row>
@@ -18996,7 +19104,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="175"/>
-      <c r="H40" s="370" t="s">
+      <c r="H40" s="369" t="s">
         <v>844</v>
       </c>
     </row>
@@ -19020,7 +19128,7 @@
         <v>2</v>
       </c>
       <c r="G41" s="175"/>
-      <c r="H41" s="371"/>
+      <c r="H41" s="370"/>
     </row>
     <row r="42" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A42" s="204">
@@ -19042,7 +19150,7 @@
         <v>3</v>
       </c>
       <c r="G42" s="175"/>
-      <c r="H42" s="371"/>
+      <c r="H42" s="370"/>
     </row>
     <row r="43" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A43" s="206">
@@ -19064,7 +19172,7 @@
         <v>4</v>
       </c>
       <c r="G43" s="175"/>
-      <c r="H43" s="371"/>
+      <c r="H43" s="370"/>
     </row>
     <row r="44" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A44" s="206">
@@ -19086,7 +19194,7 @@
         <v>5</v>
       </c>
       <c r="G44" s="175"/>
-      <c r="H44" s="371"/>
+      <c r="H44" s="370"/>
     </row>
     <row r="45" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A45" s="208">
@@ -19108,7 +19216,7 @@
         <v>6</v>
       </c>
       <c r="G45" s="175"/>
-      <c r="H45" s="371"/>
+      <c r="H45" s="370"/>
     </row>
     <row r="46" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A46" s="208">
@@ -19130,7 +19238,7 @@
         <v>7</v>
       </c>
       <c r="G46" s="175"/>
-      <c r="H46" s="371"/>
+      <c r="H46" s="370"/>
     </row>
     <row r="47" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A47" s="210">
@@ -19152,7 +19260,7 @@
         <v>8</v>
       </c>
       <c r="G47" s="175"/>
-      <c r="H47" s="372"/>
+      <c r="H47" s="371"/>
     </row>
     <row r="48" spans="1:8" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="A48" s="213">
@@ -19174,7 +19282,7 @@
         <v>9</v>
       </c>
       <c r="G48" s="175"/>
-      <c r="H48" s="361" t="s">
+      <c r="H48" s="372" t="s">
         <v>856</v>
       </c>
     </row>
@@ -19198,7 +19306,7 @@
         <v>10</v>
       </c>
       <c r="G49" s="175"/>
-      <c r="H49" s="362"/>
+      <c r="H49" s="373"/>
     </row>
     <row r="50" spans="1:8" ht="16.5" thickBot="1">
       <c r="A50" s="215">
@@ -19220,7 +19328,7 @@
         <v>11</v>
       </c>
       <c r="G50" s="175"/>
-      <c r="H50" s="362"/>
+      <c r="H50" s="373"/>
     </row>
     <row r="51" spans="1:8" ht="16.5" thickBot="1">
       <c r="A51" s="218">
@@ -19242,7 +19350,7 @@
         <v>12</v>
       </c>
       <c r="G51" s="175"/>
-      <c r="H51" s="362"/>
+      <c r="H51" s="373"/>
     </row>
     <row r="52" spans="1:8" ht="16.5" thickBot="1">
       <c r="A52" s="218">
@@ -19264,7 +19372,7 @@
         <v>13</v>
       </c>
       <c r="G52" s="175"/>
-      <c r="H52" s="362"/>
+      <c r="H52" s="373"/>
     </row>
     <row r="53" spans="1:8" ht="16.5" thickBot="1">
       <c r="A53" s="218">
@@ -19286,7 +19394,7 @@
         <v>14</v>
       </c>
       <c r="G53" s="175"/>
-      <c r="H53" s="362"/>
+      <c r="H53" s="373"/>
     </row>
     <row r="54" spans="1:8" ht="16.5" thickBot="1">
       <c r="A54" s="218">
@@ -19308,7 +19416,7 @@
         <v>15</v>
       </c>
       <c r="G54" s="175"/>
-      <c r="H54" s="362"/>
+      <c r="H54" s="373"/>
     </row>
     <row r="55" spans="1:8" ht="16.5" thickBot="1">
       <c r="A55" s="218">
@@ -19330,7 +19438,7 @@
         <v>16</v>
       </c>
       <c r="G55" s="175"/>
-      <c r="H55" s="362"/>
+      <c r="H55" s="373"/>
     </row>
     <row r="56" spans="1:8" ht="16.5" thickBot="1">
       <c r="A56" s="218">
@@ -19352,7 +19460,7 @@
         <v>17</v>
       </c>
       <c r="G56" s="175"/>
-      <c r="H56" s="362"/>
+      <c r="H56" s="373"/>
     </row>
     <row r="57" spans="1:8" ht="16.5" thickBot="1">
       <c r="A57" s="220">
@@ -19374,7 +19482,7 @@
         <v>18</v>
       </c>
       <c r="G57" s="175"/>
-      <c r="H57" s="362"/>
+      <c r="H57" s="373"/>
     </row>
     <row r="58" spans="1:8" ht="16.5" thickBot="1">
       <c r="A58" s="220">
@@ -19396,7 +19504,7 @@
         <v>19</v>
       </c>
       <c r="G58" s="175"/>
-      <c r="H58" s="362"/>
+      <c r="H58" s="373"/>
     </row>
     <row r="59" spans="1:8" ht="16.5" thickBot="1">
       <c r="A59" s="222">
@@ -19418,21 +19526,21 @@
         <v>20</v>
       </c>
       <c r="G59" s="175"/>
-      <c r="H59" s="363"/>
+      <c r="H59" s="374"/>
     </row>
     <row r="60" spans="1:8" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="H48:H59"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="H40:H47"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="H3:H10"/>
     <mergeCell ref="H11:H22"/>
-    <mergeCell ref="H48:H59"/>
-    <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="H40:H47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -19461,40 +19569,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="385" t="s">
+      <c r="A1" s="387" t="s">
         <v>327</v>
       </c>
-      <c r="B1" s="386"/>
-      <c r="C1" s="386"/>
-      <c r="D1" s="386"/>
-      <c r="E1" s="386"/>
-      <c r="F1" s="386"/>
-      <c r="G1" s="386"/>
-      <c r="H1" s="387"/>
+      <c r="B1" s="388"/>
+      <c r="C1" s="388"/>
+      <c r="D1" s="388"/>
+      <c r="E1" s="388"/>
+      <c r="F1" s="388"/>
+      <c r="G1" s="388"/>
+      <c r="H1" s="389"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="388"/>
-      <c r="B2" s="389"/>
-      <c r="C2" s="389"/>
-      <c r="D2" s="389"/>
-      <c r="E2" s="389"/>
-      <c r="F2" s="389"/>
-      <c r="G2" s="389"/>
-      <c r="H2" s="390"/>
+      <c r="A2" s="390"/>
+      <c r="B2" s="391"/>
+      <c r="C2" s="391"/>
+      <c r="D2" s="391"/>
+      <c r="E2" s="391"/>
+      <c r="F2" s="391"/>
+      <c r="G2" s="391"/>
+      <c r="H2" s="392"/>
     </row>
     <row r="3" spans="1:8" ht="21" thickBot="1">
-      <c r="A3" s="379" t="s">
+      <c r="A3" s="381" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="380"/>
-      <c r="C3" s="380"/>
-      <c r="D3" s="381"/>
-      <c r="E3" s="379" t="s">
+      <c r="B3" s="382"/>
+      <c r="C3" s="382"/>
+      <c r="D3" s="383"/>
+      <c r="E3" s="381" t="s">
         <v>314</v>
       </c>
-      <c r="F3" s="380"/>
-      <c r="G3" s="380"/>
-      <c r="H3" s="381"/>
+      <c r="F3" s="382"/>
+      <c r="G3" s="382"/>
+      <c r="H3" s="383"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" thickBot="1">
       <c r="A4" s="77">
@@ -19711,18 +19819,18 @@
       <c r="H21" s="69"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A22" s="382" t="s">
+      <c r="A22" s="384" t="s">
         <v>315</v>
       </c>
-      <c r="B22" s="383"/>
-      <c r="C22" s="383"/>
-      <c r="D22" s="384"/>
-      <c r="E22" s="382" t="s">
+      <c r="B22" s="385"/>
+      <c r="C22" s="385"/>
+      <c r="D22" s="386"/>
+      <c r="E22" s="384" t="s">
         <v>316</v>
       </c>
-      <c r="F22" s="383"/>
-      <c r="G22" s="383"/>
-      <c r="H22" s="384"/>
+      <c r="F22" s="385"/>
+      <c r="G22" s="385"/>
+      <c r="H22" s="386"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1">
       <c r="A23" s="62">
@@ -19999,40 +20107,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="319" t="s">
+      <c r="A1" s="325" t="s">
         <v>488</v>
       </c>
-      <c r="B1" s="320"/>
-      <c r="C1" s="320"/>
-      <c r="D1" s="320"/>
-      <c r="E1" s="320"/>
-      <c r="F1" s="320"/>
-      <c r="G1" s="320"/>
-      <c r="H1" s="321"/>
+      <c r="B1" s="326"/>
+      <c r="C1" s="326"/>
+      <c r="D1" s="326"/>
+      <c r="E1" s="326"/>
+      <c r="F1" s="326"/>
+      <c r="G1" s="326"/>
+      <c r="H1" s="327"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="322"/>
-      <c r="B2" s="323"/>
-      <c r="C2" s="323"/>
-      <c r="D2" s="323"/>
-      <c r="E2" s="323"/>
-      <c r="F2" s="323"/>
-      <c r="G2" s="323"/>
-      <c r="H2" s="324"/>
+      <c r="A2" s="328"/>
+      <c r="B2" s="329"/>
+      <c r="C2" s="329"/>
+      <c r="D2" s="329"/>
+      <c r="E2" s="329"/>
+      <c r="F2" s="329"/>
+      <c r="G2" s="329"/>
+      <c r="H2" s="330"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A3" s="325" t="s">
+      <c r="A3" s="331" t="s">
         <v>319</v>
       </c>
-      <c r="B3" s="326"/>
-      <c r="C3" s="326"/>
-      <c r="D3" s="326"/>
-      <c r="E3" s="326" t="s">
+      <c r="B3" s="332"/>
+      <c r="C3" s="332"/>
+      <c r="D3" s="332"/>
+      <c r="E3" s="332" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="326"/>
-      <c r="G3" s="326"/>
-      <c r="H3" s="327"/>
+      <c r="F3" s="332"/>
+      <c r="G3" s="332"/>
+      <c r="H3" s="333"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1">
       <c r="A4" s="12">

</xml_diff>